<commit_message>
update papers for lane detection, 20181012
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="13140"/>
+    <workbookView windowWidth="15120" windowHeight="25890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83">
   <si>
     <t>Scope</t>
   </si>
@@ -246,6 +246,24 @@
   <si>
     <t>1. spatial path和context path分开, 同时满足速度和语义信息的提取
 2. context path 有用auxiliary loss</t>
+  </si>
+  <si>
+    <t>deep neural network for structural prediction and lane detection in traffic scene</t>
+  </si>
+  <si>
+    <t>an empirical evaluation of deep learning on highway driving</t>
+  </si>
+  <si>
+    <t>Efficient Deep Models for Monocular Road Segmentation</t>
+  </si>
+  <si>
+    <t>Embedding Structured Contour and Location Prior in Siamesed Fully Convolutional Networks for Road Detection</t>
+  </si>
+  <si>
+    <t>Find Your Own Way: Weakly-Supervised Segmentation of Path Proposals for Urban Autonomy</t>
+  </si>
+  <si>
+    <t>end to end ego lane estimation based on sequential transfer learning for self driving cars</t>
   </si>
   <si>
     <t>ICNet for Real-Time Semantic Segmentation on Hight-Resolution Images</t>
@@ -275,10 +293,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -323,6 +341,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -331,6 +357,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -338,8 +379,91 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -360,112 +484,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -488,13 +506,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -506,37 +608,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -548,127 +632,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,74 +752,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -831,153 +781,221 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1069,8 +1087,8 @@
     <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
     <cellStyle name="Accent2" xfId="17" builtinId="33"/>
     <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
     <cellStyle name="Neutral" xfId="21" builtinId="28"/>
     <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
@@ -1086,19 +1104,19 @@
     <cellStyle name="Good" xfId="33" builtinId="26"/>
     <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
     <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
+    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
+    <cellStyle name="Comma" xfId="46" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -1143,11 +1161,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1403,18 +1416,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -1441,7 +1455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="13.5" spans="1:4">
+    <row r="2" ht="14.25" spans="1:4">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1453,7 +1467,7 @@
       </c>
       <c r="D2" s="8"/>
     </row>
-    <row r="3" ht="13.5" spans="1:4">
+    <row r="3" ht="14.25" spans="1:4">
       <c r="A3" s="9"/>
       <c r="B3" s="7">
         <v>5</v>
@@ -1475,7 +1489,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" ht="39" spans="1:4">
+    <row r="5" ht="39.75" spans="1:4">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -1489,7 +1503,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" ht="13.5" spans="1:4">
+    <row r="6" ht="14.25" spans="1:4">
       <c r="A6" s="10"/>
       <c r="B6" s="11">
         <v>5</v>
@@ -1531,7 +1545,7 @@
       </c>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" ht="52.5" spans="1:4">
+    <row r="10" ht="54" spans="1:4">
       <c r="A10" s="10"/>
       <c r="B10" s="12">
         <v>2</v>
@@ -1651,7 +1665,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" ht="51.75" spans="1:7">
+    <row r="21" ht="52.5" spans="1:7">
       <c r="A21" s="10"/>
       <c r="B21" s="12">
         <v>2</v>
@@ -1755,7 +1769,7 @@
       </c>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" ht="80.25" spans="1:4">
+    <row r="29" ht="84" spans="1:4">
       <c r="A29" s="10"/>
       <c r="B29" s="7">
         <v>5</v>
@@ -1839,7 +1853,7 @@
       </c>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" ht="39.75" spans="1:4">
+    <row r="37" ht="41.25" spans="1:4">
       <c r="A37" s="16"/>
       <c r="B37" s="7">
         <v>5</v>
@@ -1849,7 +1863,7 @@
       </c>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" ht="52.5" spans="1:4">
+    <row r="38" ht="54" spans="1:4">
       <c r="A38" s="16"/>
       <c r="B38" s="7">
         <v>6</v>
@@ -1861,7 +1875,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" ht="13.5" spans="1:4">
+    <row r="39" ht="14.25" spans="1:4">
       <c r="A39" s="16"/>
       <c r="B39" s="17">
         <v>5</v>
@@ -1873,7 +1887,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" ht="27" spans="1:4">
+    <row r="40" ht="28.5" spans="1:4">
       <c r="A40" s="16"/>
       <c r="B40" s="17">
         <v>5</v>
@@ -1893,7 +1907,7 @@
       </c>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" ht="93" spans="1:4">
+    <row r="42" ht="96.75" spans="1:4">
       <c r="A42" s="16"/>
       <c r="B42" s="17">
         <v>5</v>
@@ -1905,7 +1919,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" ht="53.25" spans="1:4">
+    <row r="43" ht="55.5" spans="1:4">
       <c r="A43" s="16"/>
       <c r="B43" s="17">
         <v>5</v>
@@ -1917,7 +1931,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" ht="106.5" spans="1:4">
+    <row r="44" ht="111" spans="1:4">
       <c r="A44" s="16"/>
       <c r="B44" s="17">
         <v>5</v>
@@ -1939,7 +1953,7 @@
       </c>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" ht="26.25" spans="1:4">
+    <row r="46" ht="27" spans="1:4">
       <c r="A46" s="16"/>
       <c r="B46" s="17">
         <v>5</v>
@@ -1949,7 +1963,7 @@
       </c>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" ht="39.75" spans="1:4">
+    <row r="47" ht="41.25" spans="1:4">
       <c r="A47" s="16"/>
       <c r="B47" s="17">
         <v>5</v>
@@ -1963,53 +1977,105 @@
     </row>
     <row r="48" ht="25.5" spans="1:4">
       <c r="A48" s="16"/>
-      <c r="B48" s="17">
-        <v>2</v>
-      </c>
+      <c r="B48" s="17"/>
       <c r="C48" s="15" t="s">
         <v>71</v>
       </c>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" ht="53.25" spans="1:4">
+    <row r="49" ht="25.5" spans="1:4">
       <c r="A49" s="16"/>
-      <c r="B49" s="17">
+      <c r="B49" s="17"/>
+      <c r="C49" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" s="8"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="16"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51" ht="38.25" spans="1:4">
+      <c r="A51" s="16"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51" s="8"/>
+    </row>
+    <row r="52" ht="25.5" spans="1:4">
+      <c r="A52" s="16"/>
+      <c r="B52" s="17">
+        <v>1</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" ht="25.5" spans="1:4">
+      <c r="A53" s="16"/>
+      <c r="B53" s="17">
+        <v>2</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="8"/>
+    </row>
+    <row r="54" ht="25.5" spans="1:4">
+      <c r="A54" s="16"/>
+      <c r="B54" s="17">
+        <v>2</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D54" s="8"/>
+    </row>
+    <row r="55" ht="55.5" spans="1:4">
+      <c r="A55" s="16"/>
+      <c r="B55" s="17">
         <v>5</v>
       </c>
-      <c r="C49" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="50" ht="28.5" spans="1:4">
-      <c r="A50" s="16"/>
-      <c r="B50" s="17">
+      <c r="C55" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" ht="27" spans="1:4">
+      <c r="A56" s="16"/>
+      <c r="B56" s="17">
         <v>2</v>
       </c>
-      <c r="C50" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D50" s="8"/>
-    </row>
-    <row r="51" ht="119.25" spans="1:4">
-      <c r="A51" s="19"/>
-      <c r="B51" s="17">
+      <c r="C56" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D56" s="8"/>
+    </row>
+    <row r="57" ht="123.75" spans="1:4">
+      <c r="A57" s="19"/>
+      <c r="B57" s="17">
         <v>5</v>
       </c>
-      <c r="C51" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="20"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
+      <c r="C57" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="20"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2017,9 +2083,9 @@
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="A11:A18"/>
     <mergeCell ref="A19:A35"/>
-    <mergeCell ref="A36:A51"/>
+    <mergeCell ref="A36:A57"/>
   </mergeCells>
-  <conditionalFormatting sqref="B$1:B$1048576">
+  <conditionalFormatting sqref="B49:B1048576 B1:B47 B48">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
add reading note for paper_1012
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15120" windowHeight="25890"/>
+    <workbookView windowWidth="27720" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89">
   <si>
     <t>Scope</t>
   </si>
@@ -148,6 +148,10 @@
     <t>R-FCN-3000 at 30fps: Decoupling Detection and Classification(poster)</t>
   </si>
   <si>
+    <t>每一类一个Positino-Sensitive Filter不是必须的,
+ objectiveness和class解耦, objectiveness说明了是否框正了(用消耗资源的PS-score + PSRoIPooling), class直接RoIPooling后avereage</t>
+  </si>
+  <si>
     <t>Dynamic Zoom-In Network for Fast Object Detection in Large Images</t>
   </si>
   <si>
@@ -206,7 +210,15 @@
     <t>1. 提出（集成）了很多想法和新模块，在当年是很跨时代的: PRelu, spatial-dropout以及在各个模块的设计上</t>
   </si>
   <si>
+    <t>Learning deconvolution network for semantic segmentation</t>
+  </si>
+  <si>
     <t>Understanding Convolution for Semantic Segmentation</t>
+  </si>
+  <si>
+    <t>着眼于级联的dilated conv和up-conv的改进:
+1. 提出HDC(hybrid dilated conv): 指出了对于级联的dilated conv如何设置dilated-rate可以避免gridding-effect
+2. DUC(dense up-conv): 借鉴sub-pixel的概念, 先把channle扩展到C*d^2, 再resize到(Hxd)*(Wxd)*C, 相对于传统的deconv, 对小物体效果比较好</t>
   </si>
   <si>
     <t>DeepLab(v1~v3)
@@ -248,6 +260,9 @@
 2. context path 有用auxiliary loss</t>
   </si>
   <si>
+    <t>Real-time single image and video super-resolution using an efficient sub-pixel convolutional neural network</t>
+  </si>
+  <si>
     <t>deep neural network for structural prediction and lane detection in traffic scene</t>
   </si>
   <si>
@@ -260,7 +275,14 @@
     <t>Embedding Structured Contour and Location Prior in Siamesed Fully Convolutional Networks for Road Detection</t>
   </si>
   <si>
+    <t>1. 提出采用轮廓作为feature, 和RGB图同时作为输入的连体FCN, 能将F1 score提高2%, 同时加快training的速度
+2. 在featureMap后加入location prior(也就是每个activation点的坐标), 可以有效去除诸如把天空分类为道路的情况</t>
+  </si>
+  <si>
     <t>Find Your Own Way: Weakly-Supervised Segmentation of Path Proposals for Urban Autonomy</t>
+  </si>
+  <si>
+    <t>对于没有车道线的场景, 用weakly supervised的方法产生label进行分割</t>
   </si>
   <si>
     <t>end to end ego lane estimation based on sequential transfer learning for self driving cars</t>
@@ -294,9 +316,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -349,6 +371,59 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -359,19 +434,27 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -379,26 +462,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -410,31 +485,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -446,46 +506,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,25 +528,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,49 +684,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -590,103 +708,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -767,60 +795,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -849,157 +827,207 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1052,6 +1080,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1087,8 +1118,8 @@
     <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
     <cellStyle name="Accent2" xfId="17" builtinId="33"/>
     <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
-    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
     <cellStyle name="Neutral" xfId="21" builtinId="28"/>
     <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
@@ -1104,19 +1135,19 @@
     <cellStyle name="Good" xfId="33" builtinId="26"/>
     <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
     <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
-    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
-    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
-    <cellStyle name="Comma" xfId="46" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
-    <cellStyle name="Percent" xfId="48" builtinId="5"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -1161,6 +1192,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1416,19 +1452,18 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -1455,7 +1490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="14.25" spans="1:4">
+    <row r="2" ht="13.5" spans="1:4">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1467,7 +1502,7 @@
       </c>
       <c r="D2" s="8"/>
     </row>
-    <row r="3" ht="14.25" spans="1:4">
+    <row r="3" ht="13.5" spans="1:4">
       <c r="A3" s="9"/>
       <c r="B3" s="7">
         <v>5</v>
@@ -1489,7 +1524,7 @@
       </c>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" ht="39.75" spans="1:4">
+    <row r="5" ht="39" spans="1:4">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -1503,7 +1538,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" ht="14.25" spans="1:4">
+    <row r="6" ht="13.5" spans="1:4">
       <c r="A6" s="10"/>
       <c r="B6" s="11">
         <v>5</v>
@@ -1545,7 +1580,7 @@
       </c>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" ht="54" spans="1:4">
+    <row r="10" ht="52.5" spans="1:4">
       <c r="A10" s="10"/>
       <c r="B10" s="12">
         <v>2</v>
@@ -1658,14 +1693,14 @@
         <v>29</v>
       </c>
       <c r="D20" s="8"/>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" ht="52.5" spans="1:7">
+    <row r="21" ht="51.75" spans="1:7">
       <c r="A21" s="10"/>
       <c r="B21" s="12">
         <v>2</v>
@@ -1749,15 +1784,17 @@
       </c>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" ht="25.5" spans="1:4">
+    <row r="27" ht="40.5" spans="1:4">
       <c r="A27" s="10"/>
-      <c r="B27" s="12">
-        <v>1</v>
+      <c r="B27" s="7">
+        <v>5</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="8"/>
+      <c r="D27" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="28" ht="25.5" spans="1:4">
       <c r="A28" s="10"/>
@@ -1765,20 +1802,20 @@
         <v>3</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" ht="84" spans="1:4">
+    <row r="29" ht="80.25" spans="1:4">
       <c r="A29" s="10"/>
       <c r="B29" s="7">
         <v>5</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" ht="25.5" spans="1:4">
@@ -1787,7 +1824,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D30" s="8"/>
     </row>
@@ -1797,7 +1834,7 @@
         <v>2</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D31" s="8"/>
     </row>
@@ -1807,7 +1844,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D32" s="8"/>
     </row>
@@ -1817,7 +1854,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D33" s="8"/>
     </row>
@@ -1827,7 +1864,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D34" s="8"/>
     </row>
@@ -1837,245 +1874,281 @@
         <v>1</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D35" s="8"/>
     </row>
     <row r="36" ht="25.5" spans="1:4">
       <c r="A36" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B36" s="12">
         <v>2</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" ht="41.25" spans="1:4">
+    <row r="37" ht="39.75" spans="1:4">
       <c r="A37" s="16"/>
       <c r="B37" s="7">
         <v>5</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" ht="54" spans="1:4">
+    <row r="38" ht="52.5" spans="1:4">
       <c r="A38" s="16"/>
       <c r="B38" s="7">
         <v>6</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" ht="14.25" spans="1:4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" ht="13.5" spans="1:4">
       <c r="A39" s="16"/>
       <c r="B39" s="17">
         <v>5</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" ht="28.5" spans="1:4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" ht="27" spans="1:4">
       <c r="A40" s="16"/>
       <c r="B40" s="17">
         <v>5</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" ht="25.5" spans="1:4">
       <c r="A41" s="16"/>
-      <c r="B41" s="17"/>
+      <c r="B41" s="17">
+        <v>1</v>
+      </c>
       <c r="C41" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" ht="96.75" spans="1:4">
+    <row r="42" ht="93" spans="1:4">
       <c r="A42" s="16"/>
       <c r="B42" s="17">
         <v>5</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="43" ht="55.5" spans="1:4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" ht="93" spans="1:4">
       <c r="A43" s="16"/>
       <c r="B43" s="17">
         <v>5</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" ht="111" spans="1:4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" ht="53.25" spans="1:4">
       <c r="A44" s="16"/>
       <c r="B44" s="17">
         <v>5</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" ht="106.5" spans="1:4">
       <c r="A45" s="16"/>
       <c r="B45" s="17">
         <v>5</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D45" s="8"/>
-    </row>
-    <row r="46" ht="27" spans="1:4">
+        <v>68</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="16"/>
       <c r="B46" s="17">
         <v>5</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" ht="41.25" spans="1:4">
+    <row r="47" ht="26.25" spans="1:4">
       <c r="A47" s="16"/>
       <c r="B47" s="17">
         <v>5</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="48" ht="25.5" spans="1:4">
+        <v>71</v>
+      </c>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" ht="39.75" spans="1:4">
       <c r="A48" s="16"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D48" s="8"/>
+      <c r="B48" s="17">
+        <v>5</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="49" ht="25.5" spans="1:4">
       <c r="A49" s="16"/>
-      <c r="B49" s="17"/>
+      <c r="B49" s="17">
+        <v>2</v>
+      </c>
       <c r="C49" s="15" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" ht="25.5" spans="1:4">
       <c r="A50" s="16"/>
-      <c r="B50" s="17"/>
+      <c r="B50" s="17">
+        <v>1</v>
+      </c>
       <c r="C50" s="15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" ht="38.25" spans="1:4">
+    <row r="51" ht="25.5" spans="1:4">
       <c r="A51" s="16"/>
-      <c r="B51" s="17"/>
+      <c r="B51" s="17">
+        <v>1</v>
+      </c>
       <c r="C51" s="15" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" ht="25.5" spans="1:4">
+    <row r="52" spans="1:4">
       <c r="A52" s="16"/>
       <c r="B52" s="17">
         <v>1</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" ht="25.5" spans="1:4">
+    <row r="53" ht="66.75" spans="1:4">
       <c r="A53" s="16"/>
       <c r="B53" s="17">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D53" s="8"/>
+        <v>78</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="54" ht="25.5" spans="1:4">
       <c r="A54" s="16"/>
-      <c r="B54" s="17">
-        <v>2</v>
+      <c r="B54" s="18">
+        <v>3</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D54" s="8"/>
-    </row>
-    <row r="55" ht="55.5" spans="1:4">
+        <v>80</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" ht="25.5" spans="1:4">
       <c r="A55" s="16"/>
       <c r="B55" s="17">
-        <v>5</v>
-      </c>
-      <c r="C55" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="56" ht="27" spans="1:4">
+        <v>2</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D55" s="8"/>
+    </row>
+    <row r="56" ht="25.5" spans="1:4">
       <c r="A56" s="16"/>
       <c r="B56" s="17">
         <v>2</v>
       </c>
-      <c r="C56" s="18" t="s">
-        <v>80</v>
+      <c r="C56" s="15" t="s">
+        <v>83</v>
       </c>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" ht="123.75" spans="1:4">
-      <c r="A57" s="19"/>
+    <row r="57" ht="53.25" spans="1:4">
+      <c r="A57" s="16"/>
       <c r="B57" s="17">
         <v>5</v>
       </c>
-      <c r="C57" s="8" t="s">
-        <v>81</v>
+      <c r="C57" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="20"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" ht="28.5" spans="1:4">
+      <c r="A58" s="16"/>
+      <c r="B58" s="17">
+        <v>2</v>
+      </c>
+      <c r="C58" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D58" s="8"/>
+    </row>
+    <row r="59" ht="119.25" spans="1:4">
+      <c r="A59" s="20"/>
+      <c r="B59" s="17">
+        <v>5</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="21"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2083,9 +2156,9 @@
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="A11:A18"/>
     <mergeCell ref="A19:A35"/>
-    <mergeCell ref="A36:A57"/>
+    <mergeCell ref="A36:A59"/>
   </mergeCells>
-  <conditionalFormatting sqref="B49:B1048576 B1:B47 B48">
+  <conditionalFormatting sqref="B$1:B$1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
add comments for paper_1102
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15120" windowHeight="9810"/>
+    <workbookView windowWidth="27720" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124">
   <si>
     <t>Scope</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>orthognotic</t>
-  </si>
-  <si>
-    <t>Learning Efficient Object Detection Models with Knowledge Distillation</t>
   </si>
   <si>
     <t>Focal Loss for Dense Object Detection</t>
@@ -95,21 +92,43 @@
     <t>MnasNet: Platform-Aware Neural Architecture Search for Mobile</t>
   </si>
   <si>
+    <t>Rectified Linear Units Improve Restricted Boltzmann Machines</t>
+  </si>
+  <si>
+    <t>Understanding the difficulty of training deep feedforward neural networks</t>
+  </si>
+  <si>
+    <t>Deep Sparse Rectifier Neural Networks(提出ReLU)</t>
+  </si>
+  <si>
     <t>Non-local Neural Networks</t>
   </si>
   <si>
+    <t>Wide Residual Networks</t>
+  </si>
+  <si>
     <t>Wider or Deeper: Revisiting the ResNet Model for Visual Recognition</t>
   </si>
   <si>
+    <t>resnet 是有有效深度的, 超过有效深度的branch, 其实并没有end to end 训练到, 因此对于resnet unit要求为: 1. strong enough to converge even if it is reused in many sub-networks, 2. shollow enough to enable an large effective depth</t>
+  </si>
+  <si>
     <t>learning transferable architectures for scable image recognition(NASNet)</t>
   </si>
   <si>
     <t>Delving Deep into Rectifiers: Surpassing Human-Level Performance on ImageNet Classification</t>
   </si>
   <si>
+    <t>1. 提出PReLU: 模型在浅层更倾向于保留信息而在深层更加任务驱动: the learned model tends to keep more information in earlier stages and becomes more discriminative in deeper stages
+2. 提出了在考虑rectifier的情况下初始化weights的方法, 对于rulu, weights的标准差应该为: sqrt(1/nl), nl=k*k*c, k为kernel_size, c为channel数</t>
+  </si>
+  <si>
     <t>Aggregated Residual Transformations for Deep Neural Networks</t>
   </si>
   <si>
+    <t>模型容量不变的前提下, 增加gropu数量能够提高性能(representing power), 但group太大后, 提升就不明显了</t>
+  </si>
+  <si>
     <t>Deformable Convolutional Networks</t>
   </si>
   <si>
@@ -123,6 +142,9 @@
   </si>
   <si>
     <t>object detection</t>
+  </si>
+  <si>
+    <t>Learning Efficient Object Detection Models with Knowledge Distillation</t>
   </si>
   <si>
     <t>RON-Reverse Connection with Objectness Prior Networks for Object Detection</t>
@@ -401,11 +423,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,22 +464,45 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF31424E"/>
       <name val="microsoft yahei"/>
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -471,6 +516,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -479,8 +531,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -496,24 +549,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -525,9 +563,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -535,6 +572,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -549,36 +600,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -591,13 +613,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -626,37 +641,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -668,13 +725,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -686,7 +749,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -698,13 +779,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -716,31 +809,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -752,61 +821,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -887,6 +902,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -898,6 +924,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -917,37 +967,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -960,166 +984,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1156,18 +1171,15 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1183,7 +1195,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1213,8 +1225,8 @@
     <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
     <cellStyle name="Accent2" xfId="17" builtinId="33"/>
     <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
-    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
     <cellStyle name="Neutral" xfId="21" builtinId="28"/>
     <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
@@ -1230,19 +1242,19 @@
     <cellStyle name="Good" xfId="33" builtinId="26"/>
     <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
     <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
-    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
-    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
-    <cellStyle name="Comma" xfId="46" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
-    <cellStyle name="Percent" xfId="48" builtinId="5"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -1287,6 +1299,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1542,19 +1559,18 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -1581,7 +1597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="14.25" spans="1:4">
+    <row r="2" ht="13.5" spans="1:4">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1593,7 +1609,7 @@
       </c>
       <c r="D2" s="8"/>
     </row>
-    <row r="3" ht="14.25" spans="1:4">
+    <row r="3" ht="13.5" spans="1:4">
       <c r="A3" s="9"/>
       <c r="B3" s="7">
         <v>5</v>
@@ -1603,7 +1619,7 @@
       </c>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" ht="14.25" spans="1:4">
+    <row r="4" ht="13.5" spans="1:4">
       <c r="A4" s="9"/>
       <c r="B4" s="7"/>
       <c r="C4" s="10" t="s">
@@ -1623,7 +1639,7 @@
       </c>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" ht="39.75" spans="1:4">
+    <row r="6" ht="39" spans="1:4">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -1637,7 +1653,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" ht="14.25" spans="1:4">
+    <row r="7" ht="13.5" spans="1:4">
       <c r="A7" s="9"/>
       <c r="B7" s="11">
         <v>5</v>
@@ -1649,83 +1665,83 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" ht="25.5" spans="1:4">
+    <row r="8" spans="1:4">
       <c r="A8" s="9"/>
       <c r="B8" s="12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" ht="25.5" spans="1:4">
       <c r="A9" s="9"/>
       <c r="B9" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" ht="25.5" spans="1:4">
+    <row r="10" ht="52.5" spans="1:4">
       <c r="A10" s="9"/>
-      <c r="B10" s="12">
-        <v>3</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="14">
+        <v>2</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" ht="54" spans="1:4">
-      <c r="A11" s="9"/>
+    <row r="11" spans="1:4">
+      <c r="A11" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="B11" s="12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="14">
+    <row r="12" ht="27" spans="1:4">
+      <c r="A12" s="9"/>
+      <c r="B12" s="12">
         <v>5</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" ht="28.5" spans="1:4">
+      <c r="D12" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" ht="25.5" spans="1:4">
       <c r="A13" s="9"/>
       <c r="B13" s="14">
-        <v>5</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>22</v>
       </c>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" ht="25.5" spans="1:4">
       <c r="A14" s="9"/>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>3</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="8"/>
     </row>
     <row r="15" ht="25.5" spans="1:4">
       <c r="A15" s="9"/>
-      <c r="B15" s="12">
+      <c r="B15" s="14">
         <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1733,506 +1749,506 @@
       </c>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" ht="25.5" spans="1:4">
       <c r="A16" s="9"/>
-      <c r="B16" s="12">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" s="14">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" ht="25.5" spans="1:4">
+    <row r="17" ht="13.5" spans="1:4">
       <c r="A17" s="9"/>
-      <c r="B17" s="12">
-        <v>1</v>
+      <c r="B17" s="14">
+        <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" ht="25.5" spans="1:4">
+    <row r="18" spans="1:4">
       <c r="A18" s="9"/>
-      <c r="B18" s="12">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="14">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" ht="25.5" spans="1:4">
+    <row r="19" spans="1:4">
       <c r="A19" s="9"/>
-      <c r="B19" s="12">
-        <v>1</v>
-      </c>
-      <c r="C19" s="8" t="s">
+      <c r="B19" s="14">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" ht="25.5" spans="1:4">
+    <row r="20" ht="39.75" spans="1:4">
       <c r="A20" s="9"/>
       <c r="B20" s="12">
-        <v>1</v>
-      </c>
-      <c r="C20" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="D20" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" ht="25.5" spans="1:4">
       <c r="A21" s="9"/>
-      <c r="B21" s="12">
-        <v>1</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>30</v>
+      <c r="B21" s="14">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" ht="78.75" spans="1:4">
       <c r="A22" s="9"/>
       <c r="B22" s="12">
-        <v>2</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" ht="25.5" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" ht="27" spans="1:4">
       <c r="A23" s="9"/>
       <c r="B23" s="12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" ht="25.5" spans="1:4">
+        <v>34</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="9"/>
       <c r="B24" s="14">
         <v>1</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>33</v>
+      <c r="C24" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" ht="25.5" spans="1:4">
-      <c r="A25" s="9" t="s">
-        <v>34</v>
-      </c>
+    <row r="25" spans="1:4">
+      <c r="A25" s="9"/>
       <c r="B25" s="14">
         <v>2</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>35</v>
+      <c r="C25" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" ht="25.5" spans="1:4">
       <c r="A26" s="9"/>
       <c r="B26" s="14">
-        <v>2</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>36</v>
+        <v>1</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="D26" s="8"/>
     </row>
     <row r="27" ht="25.5" spans="1:4">
       <c r="A27" s="9"/>
-      <c r="B27" s="14">
-        <v>2</v>
+      <c r="B27" s="12">
+        <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D27" s="8"/>
     </row>
     <row r="28" ht="25.5" spans="1:4">
-      <c r="A28" s="9"/>
-      <c r="B28" s="14">
+      <c r="A28" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="12">
         <v>2</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" ht="25.5" spans="1:4">
       <c r="A29" s="9"/>
-      <c r="B29" s="14">
-        <v>5</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>39</v>
+      <c r="B29" s="12">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="D29" s="8"/>
-      <c r="F29" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="9"/>
-      <c r="B30" s="14">
-        <v>2</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>41</v>
+      <c r="B30" s="12">
+        <v>2</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="D30" s="8"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-    </row>
-    <row r="31" ht="52.5" spans="1:7">
+    </row>
+    <row r="31" ht="25.5" spans="1:4">
       <c r="A31" s="9"/>
       <c r="B31" s="12">
         <v>2</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>42</v>
+      <c r="C31" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="D31" s="8"/>
-      <c r="F31" s="1">
-        <v>0</v>
-      </c>
-      <c r="G31" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" ht="25.5" spans="1:7">
+    </row>
+    <row r="32" ht="25.5" spans="1:4">
       <c r="A32" s="9"/>
       <c r="B32" s="12">
-        <v>3</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>44</v>
+        <v>2</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="D32" s="8"/>
-      <c r="F32" s="1">
-        <v>1</v>
-      </c>
-      <c r="G32" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="9"/>
       <c r="B33" s="12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D33" s="8"/>
-      <c r="F33" s="1">
-        <v>2</v>
-      </c>
-      <c r="G33" t="s">
+      <c r="F33" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G33" s="17" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="9"/>
       <c r="B34" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D34" s="8"/>
-      <c r="F34" s="1">
-        <v>3</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+    </row>
+    <row r="35" ht="51.75" spans="1:7">
+      <c r="A35" s="9"/>
+      <c r="B35" s="14">
+        <v>2</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="9"/>
-      <c r="B35" s="12">
-        <v>3</v>
-      </c>
-      <c r="C35" s="8" t="s">
+      <c r="D35" s="8"/>
+      <c r="F35" s="1">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" ht="25.5" spans="1:4">
+    </row>
+    <row r="36" ht="25.5" spans="1:7">
       <c r="A36" s="9"/>
-      <c r="B36" s="12">
+      <c r="B36" s="14">
         <v>3</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>51</v>
       </c>
       <c r="D36" s="8"/>
-    </row>
-    <row r="37" ht="42.75" spans="1:4">
+      <c r="F36" s="1">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="9"/>
-      <c r="B37" s="7">
-        <v>5</v>
+      <c r="B37" s="14">
+        <v>3</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="38" ht="25.5" spans="1:4">
+      <c r="D37" s="8"/>
+      <c r="F37" s="1">
+        <v>2</v>
+      </c>
+      <c r="G37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="9"/>
-      <c r="B38" s="12">
+      <c r="B38" s="14">
         <v>3</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D38" s="8"/>
-    </row>
-    <row r="39" ht="25.5" spans="1:4">
+      <c r="F38" s="1">
+        <v>3</v>
+      </c>
+      <c r="G38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="9"/>
-      <c r="B39" s="12">
+      <c r="B39" s="14">
         <v>3</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" ht="84" spans="1:4">
+    <row r="40" ht="25.5" spans="1:4">
       <c r="A40" s="9"/>
-      <c r="B40" s="7">
-        <v>5</v>
+      <c r="B40" s="14">
+        <v>3</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" ht="25.5" spans="1:4">
+        <v>58</v>
+      </c>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" ht="40.5" spans="1:4">
       <c r="A41" s="9"/>
-      <c r="B41" s="12">
-        <v>2</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D41" s="8"/>
+      <c r="B41" s="7">
+        <v>5</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="42" ht="25.5" spans="1:4">
       <c r="A42" s="9"/>
-      <c r="B42" s="12">
-        <v>2</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>59</v>
+      <c r="B42" s="14">
+        <v>3</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" ht="25.5" spans="1:4">
       <c r="A43" s="9"/>
-      <c r="B43" s="12">
-        <v>2</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>60</v>
+      <c r="B43" s="14">
+        <v>3</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" ht="80.25" spans="1:4">
       <c r="A44" s="9"/>
-      <c r="B44" s="12">
-        <v>2</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D44" s="8"/>
+      <c r="B44" s="7">
+        <v>5</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="45" ht="25.5" spans="1:4">
       <c r="A45" s="9"/>
-      <c r="B45" s="12">
+      <c r="B45" s="14">
         <v>2</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" ht="25.5" spans="1:4">
       <c r="A46" s="9"/>
-      <c r="B46" s="12">
+      <c r="B46" s="14">
         <v>2</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" ht="25.5" spans="1:4">
+    <row r="47" spans="1:4">
       <c r="A47" s="9"/>
-      <c r="B47" s="12">
+      <c r="B47" s="14">
         <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" ht="25.5" spans="1:4">
+    <row r="48" spans="1:4">
       <c r="A48" s="9"/>
-      <c r="B48" s="12">
+      <c r="B48" s="14">
         <v>2</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" ht="25.5" spans="1:4">
       <c r="A49" s="9"/>
-      <c r="B49" s="12">
-        <v>1</v>
+      <c r="B49" s="14">
+        <v>2</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" ht="38.25" spans="1:4">
+    <row r="50" spans="1:4">
       <c r="A50" s="9"/>
-      <c r="B50" s="12">
-        <v>1</v>
+      <c r="B50" s="14">
+        <v>2</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D50" s="8"/>
     </row>
     <row r="51" ht="25.5" spans="1:4">
       <c r="A51" s="9"/>
-      <c r="B51" s="12">
-        <v>1</v>
+      <c r="B51" s="14">
+        <v>2</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D51" s="8"/>
     </row>
     <row r="52" ht="25.5" spans="1:4">
       <c r="A52" s="9"/>
-      <c r="B52" s="12">
+      <c r="B52" s="14">
+        <v>2</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="9"/>
+      <c r="B53" s="14">
         <v>1</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D52" s="8"/>
-    </row>
-    <row r="53" ht="25.5" spans="1:4">
-      <c r="A53" s="9"/>
-      <c r="B53" s="12">
+      <c r="C53" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D53" s="8"/>
+    </row>
+    <row r="54" ht="38.25" spans="1:4">
+      <c r="A54" s="9"/>
+      <c r="B54" s="14">
         <v>1</v>
       </c>
-      <c r="C53" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D53" s="8"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="9"/>
-      <c r="B54" s="12">
+      <c r="C54" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D54" s="8"/>
+    </row>
+    <row r="55" ht="25.5" spans="1:4">
+      <c r="A55" s="9"/>
+      <c r="B55" s="14">
         <v>1</v>
       </c>
-      <c r="C54" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D54" s="8"/>
-    </row>
-    <row r="55" ht="25.5" spans="1:4">
-      <c r="A55" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B55" s="12">
-        <v>2</v>
-      </c>
       <c r="C55" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D55" s="8"/>
     </row>
-    <row r="56" ht="41.25" spans="1:4">
-      <c r="A56" s="16"/>
-      <c r="B56" s="7">
-        <v>5</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>74</v>
+    <row r="56" ht="25.5" spans="1:4">
+      <c r="A56" s="9"/>
+      <c r="B56" s="14">
+        <v>1</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" ht="54" spans="1:4">
-      <c r="A57" s="16"/>
-      <c r="B57" s="7">
-        <v>6</v>
+    <row r="57" ht="25.5" spans="1:4">
+      <c r="A57" s="9"/>
+      <c r="B57" s="14">
+        <v>1</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="58" ht="14.25" spans="1:4">
-      <c r="A58" s="16"/>
-      <c r="B58" s="17">
-        <v>5</v>
+        <v>77</v>
+      </c>
+      <c r="D57" s="8"/>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="9"/>
+      <c r="B58" s="14">
+        <v>1</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D58" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="59" ht="28.5" spans="1:4">
-      <c r="A59" s="16"/>
-      <c r="B59" s="17">
-        <v>5</v>
-      </c>
-      <c r="C59" s="8" t="s">
+      <c r="D58" s="8"/>
+    </row>
+    <row r="59" ht="25.5" spans="1:4">
+      <c r="A59" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="D59" s="8" t="s">
+      <c r="B59" s="14">
+        <v>2</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="60" ht="25.5" spans="1:4">
-      <c r="A60" s="16"/>
-      <c r="B60" s="17">
-        <v>1</v>
+      <c r="D59" s="8"/>
+    </row>
+    <row r="60" ht="39.75" spans="1:4">
+      <c r="A60" s="15"/>
+      <c r="B60" s="7">
+        <v>5</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D60" s="8"/>
     </row>
-    <row r="61" ht="96.75" spans="1:4">
-      <c r="A61" s="16"/>
-      <c r="B61" s="17">
-        <v>5</v>
+    <row r="61" ht="52.5" spans="1:4">
+      <c r="A61" s="15"/>
+      <c r="B61" s="7">
+        <v>6</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>82</v>
@@ -2241,9 +2257,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="62" ht="96.75" spans="1:4">
-      <c r="A62" s="16"/>
-      <c r="B62" s="17">
+    <row r="62" ht="13.5" spans="1:4">
+      <c r="A62" s="15"/>
+      <c r="B62" s="16">
         <v>5</v>
       </c>
       <c r="C62" s="8" t="s">
@@ -2253,9 +2269,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" ht="55.5" spans="1:4">
-      <c r="A63" s="16"/>
-      <c r="B63" s="17">
+    <row r="63" ht="27" spans="1:4">
+      <c r="A63" s="15"/>
+      <c r="B63" s="16">
         <v>5</v>
       </c>
       <c r="C63" s="8" t="s">
@@ -2265,255 +2281,301 @@
         <v>87</v>
       </c>
     </row>
-    <row r="64" ht="111" spans="1:4">
-      <c r="A64" s="16"/>
-      <c r="B64" s="17">
-        <v>5</v>
+    <row r="64" ht="25.5" spans="1:4">
+      <c r="A64" s="15"/>
+      <c r="B64" s="16">
+        <v>1</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="D64" s="8"/>
+    </row>
+    <row r="65" ht="93" spans="1:4">
+      <c r="A65" s="15"/>
+      <c r="B65" s="16">
+        <v>5</v>
+      </c>
+      <c r="C65" s="8" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="16"/>
-      <c r="B65" s="17">
-        <v>5</v>
-      </c>
-      <c r="C65" s="8" t="s">
+      <c r="D65" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D65" s="8"/>
-    </row>
-    <row r="66" ht="27" spans="1:4">
-      <c r="A66" s="16"/>
-      <c r="B66" s="17">
+    </row>
+    <row r="66" ht="93" spans="1:4">
+      <c r="A66" s="15"/>
+      <c r="B66" s="16">
         <v>5</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D66" s="8"/>
-    </row>
-    <row r="67" ht="41.25" spans="1:4">
-      <c r="A67" s="16"/>
-      <c r="B67" s="17">
+      <c r="D66" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" ht="53.25" spans="1:4">
+      <c r="A67" s="15"/>
+      <c r="B67" s="16">
         <v>5</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="16"/>
-      <c r="B68" s="17">
-        <v>2</v>
-      </c>
-      <c r="C68" t="s">
         <v>94</v>
       </c>
-      <c r="D68" s="8"/>
-    </row>
-    <row r="69" ht="25.5" spans="1:4">
-      <c r="A69" s="16"/>
-      <c r="B69" s="17">
-        <v>2</v>
-      </c>
-      <c r="C69" s="2" t="s">
+    </row>
+    <row r="68" ht="106.5" spans="1:4">
+      <c r="A68" s="15"/>
+      <c r="B68" s="16">
+        <v>5</v>
+      </c>
+      <c r="C68" s="8" t="s">
         <v>95</v>
       </c>
+      <c r="D68" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="15"/>
+      <c r="B69" s="16">
+        <v>5</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="D69" s="8"/>
     </row>
-    <row r="70" ht="25.5" spans="1:4">
-      <c r="A70" s="16"/>
-      <c r="B70" s="17">
-        <v>2</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>96</v>
+    <row r="70" ht="26.25" spans="1:4">
+      <c r="A70" s="15"/>
+      <c r="B70" s="16">
+        <v>5</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="16"/>
-      <c r="B71" s="17">
-        <v>2</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="D71" s="8"/>
-    </row>
-    <row r="72" ht="25.5" spans="1:4">
-      <c r="A72" s="16"/>
-      <c r="B72" s="17">
-        <v>2</v>
-      </c>
-      <c r="C72" s="10" t="s">
-        <v>98</v>
+    <row r="71" ht="39.75" spans="1:4">
+      <c r="A71" s="15"/>
+      <c r="B71" s="16">
+        <v>5</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="15"/>
+      <c r="B72" s="16">
+        <v>2</v>
+      </c>
+      <c r="C72" t="s">
+        <v>101</v>
       </c>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" ht="27" spans="1:4">
-      <c r="A73" s="16"/>
-      <c r="B73" s="17">
+    <row r="73" ht="25.5" spans="1:4">
+      <c r="A73" s="15"/>
+      <c r="B73" s="16">
+        <v>2</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D73" s="8"/>
+    </row>
+    <row r="74" ht="25.5" spans="1:4">
+      <c r="A74" s="15"/>
+      <c r="B74" s="16">
+        <v>2</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D74" s="8"/>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="15"/>
+      <c r="B75" s="16">
+        <v>2</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D75" s="8"/>
+    </row>
+    <row r="76" ht="25.5" spans="1:4">
+      <c r="A76" s="15"/>
+      <c r="B76" s="16">
+        <v>2</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D76" s="8"/>
+    </row>
+    <row r="77" ht="26.25" spans="1:4">
+      <c r="A77" s="15"/>
+      <c r="B77" s="16">
         <v>1</v>
       </c>
-      <c r="C73" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="D73" s="8"/>
-    </row>
-    <row r="74" ht="27" spans="1:4">
-      <c r="A74" s="16"/>
-      <c r="B74" s="17">
-        <v>2</v>
-      </c>
-      <c r="C74" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D74" s="8"/>
-    </row>
-    <row r="75" ht="25.5" spans="1:4">
-      <c r="A75" s="16"/>
-      <c r="B75" s="19">
+      <c r="C77" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D77" s="8"/>
+    </row>
+    <row r="78" ht="26.25" spans="1:4">
+      <c r="A78" s="15"/>
+      <c r="B78" s="16">
+        <v>2</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D78" s="8"/>
+    </row>
+    <row r="79" ht="25.5" spans="1:4">
+      <c r="A79" s="15"/>
+      <c r="B79" s="18">
         <v>3</v>
       </c>
-      <c r="C75" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D75" s="8"/>
-    </row>
-    <row r="76" ht="25.5" spans="1:4">
-      <c r="A76" s="16"/>
-      <c r="B76" s="17">
+      <c r="C79" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D79" s="8"/>
+    </row>
+    <row r="80" ht="25.5" spans="1:4">
+      <c r="A80" s="15"/>
+      <c r="B80" s="16">
         <v>1</v>
       </c>
-      <c r="C76" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="D76" s="8"/>
-    </row>
-    <row r="77" ht="25.5" spans="1:4">
-      <c r="A77" s="16"/>
-      <c r="B77" s="17">
+      <c r="C80" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D80" s="8"/>
+    </row>
+    <row r="81" ht="25.5" spans="1:4">
+      <c r="A81" s="15"/>
+      <c r="B81" s="16">
         <v>1</v>
       </c>
-      <c r="C77" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="D77" s="8"/>
-    </row>
-    <row r="78" ht="27" spans="1:4">
-      <c r="A78" s="16"/>
-      <c r="B78" s="17">
+      <c r="C81" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D81" s="8"/>
+    </row>
+    <row r="82" ht="26.25" spans="1:4">
+      <c r="A82" s="15"/>
+      <c r="B82" s="16">
         <v>1</v>
       </c>
-      <c r="C78" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D78" s="8"/>
-    </row>
-    <row r="79" ht="27" spans="1:4">
-      <c r="A79" s="16"/>
-      <c r="B79" s="17">
+      <c r="C82" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D82" s="8"/>
+    </row>
+    <row r="83" ht="26.25" spans="1:4">
+      <c r="A83" s="15"/>
+      <c r="B83" s="16">
         <v>1</v>
       </c>
-      <c r="C79" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D79" s="8"/>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="16"/>
-      <c r="B80" s="17">
+      <c r="C83" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D83" s="8"/>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="15"/>
+      <c r="B84" s="16">
         <v>1</v>
       </c>
-      <c r="C80" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D80" s="8"/>
-    </row>
-    <row r="81" ht="69.75" spans="1:4">
-      <c r="A81" s="16"/>
-      <c r="B81" s="17">
-        <v>5</v>
-      </c>
-      <c r="C81" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="82" ht="25.5" spans="1:4">
-      <c r="A82" s="16"/>
-      <c r="B82" s="20">
-        <v>3</v>
-      </c>
-      <c r="C82" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D82" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="83" ht="55.5" spans="1:4">
-      <c r="A83" s="16"/>
-      <c r="B83" s="17">
-        <v>5</v>
-      </c>
-      <c r="C83" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="84" ht="27" spans="1:4">
-      <c r="A84" s="16"/>
-      <c r="B84" s="17">
-        <v>2</v>
-      </c>
-      <c r="C84" s="21" t="s">
+      <c r="C84" s="10" t="s">
         <v>113</v>
       </c>
       <c r="D84" s="8"/>
     </row>
-    <row r="85" ht="123.75" spans="1:4">
-      <c r="A85" s="22"/>
-      <c r="B85" s="17">
-        <v>5</v>
-      </c>
-      <c r="C85" s="8" t="s">
+    <row r="85" ht="66.75" spans="1:4">
+      <c r="A85" s="15"/>
+      <c r="B85" s="16">
+        <v>5</v>
+      </c>
+      <c r="C85" s="10" t="s">
         <v>114</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="23" t="s">
+    <row r="86" ht="25.5" spans="1:4">
+      <c r="A86" s="15"/>
+      <c r="B86" s="19">
+        <v>3</v>
+      </c>
+      <c r="C86" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="B86" s="23"/>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
+      <c r="D86" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="87" ht="53.25" spans="1:4">
+      <c r="A87" s="15"/>
+      <c r="B87" s="16">
+        <v>5</v>
+      </c>
+      <c r="C87" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="88" ht="28.5" spans="1:4">
+      <c r="A88" s="15"/>
+      <c r="B88" s="16">
+        <v>2</v>
+      </c>
+      <c r="C88" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D88" s="8"/>
+    </row>
+    <row r="89" ht="119.25" spans="1:4">
+      <c r="A89" s="21"/>
+      <c r="B89" s="16">
+        <v>5</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B90" s="22"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="A12:A24"/>
-    <mergeCell ref="A25:A54"/>
-    <mergeCell ref="A55:A85"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A27"/>
+    <mergeCell ref="A28:A58"/>
+    <mergeCell ref="A59:A89"/>
   </mergeCells>
-  <conditionalFormatting sqref="B14:B1048576 B1:B13">
+  <conditionalFormatting sqref="B$1:B$1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
add reading note for pspnet
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="13140"/>
+    <workbookView windowWidth="27720" windowHeight="13290"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202">
   <si>
     <t>Scope</t>
   </si>
@@ -517,6 +517,17 @@
   </si>
   <si>
     <t>El-gan: Embedding loss driven generative adversarial networks for lane detection</t>
+  </si>
+  <si>
+    <t>(PSPnet) Pyramid Scene Parsing Network</t>
+  </si>
+  <si>
+    <t>提供了除了global avg pool之外的sub-region context的信息，使得语意分割更准确，不同于aspp, pspnet更强调context imformation，而aspp更强调scale invariant
+加了deep supervision， 用aux loss提高训练效果；
+提到了很多细节，ablantion 很充分</t>
+  </si>
+  <si>
+    <t>Large Kernel Matters -- Improve Semantic Segmentation by Global Convolutional Network</t>
   </si>
   <si>
     <t>Semantic Instance Segmentation with a Discriminative Loss Function</t>
@@ -661,10 +672,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -716,6 +727,30 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -731,15 +766,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -769,47 +797,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -825,6 +814,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -846,15 +850,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -887,7 +898,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -899,7 +910,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -911,7 +1000,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -923,49 +1024,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -977,37 +1048,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1019,55 +1066,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1133,11 +1144,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1151,32 +1168,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1202,6 +1198,36 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1215,168 +1241,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1480,8 +1491,8 @@
     <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
     <cellStyle name="Accent2" xfId="17" builtinId="33"/>
     <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
     <cellStyle name="Neutral" xfId="21" builtinId="28"/>
     <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
@@ -1497,19 +1508,19 @@
     <cellStyle name="Good" xfId="33" builtinId="26"/>
     <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
     <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
+    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
+    <cellStyle name="Comma" xfId="46" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -1554,11 +1565,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1814,18 +1820,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G145"/>
+  <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D119" sqref="D119"/>
+      <selection pane="bottomLeft" activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -1852,7 +1859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="13.5" spans="1:4">
+    <row r="2" ht="14.25" spans="1:4">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1864,7 +1871,7 @@
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" ht="13.5" spans="1:4">
+    <row r="3" ht="14.25" spans="1:4">
       <c r="A3" s="9"/>
       <c r="B3" s="10">
         <v>5</v>
@@ -1874,7 +1881,7 @@
       </c>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" ht="13.5" spans="1:4">
+    <row r="4" ht="14.25" spans="1:4">
       <c r="A4" s="9"/>
       <c r="B4" s="10">
         <v>5</v>
@@ -1884,7 +1891,7 @@
       </c>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" ht="13.5" spans="1:4">
+    <row r="5" ht="14.25" spans="1:4">
       <c r="A5" s="9"/>
       <c r="B5" s="10">
         <v>5</v>
@@ -1896,7 +1903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="13.5" spans="1:4">
+    <row r="6" ht="14.25" spans="1:4">
       <c r="A6" s="9"/>
       <c r="B6" s="10"/>
       <c r="C6" s="12" t="s">
@@ -1916,7 +1923,7 @@
       </c>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" ht="26.25" spans="1:4">
+    <row r="8" ht="27" spans="1:4">
       <c r="A8" s="9"/>
       <c r="B8" s="10">
         <v>2</v>
@@ -1936,7 +1943,7 @@
       </c>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" ht="39" spans="1:4">
+    <row r="10" ht="39.75" spans="1:4">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -1950,7 +1957,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" ht="13.5" spans="1:4">
+    <row r="11" ht="14.25" spans="1:4">
       <c r="A11" s="9"/>
       <c r="B11" s="13">
         <v>5</v>
@@ -2014,7 +2021,7 @@
       </c>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" ht="52.5" spans="1:4">
+    <row r="17" ht="54" spans="1:4">
       <c r="A17" s="9"/>
       <c r="B17" s="16">
         <v>2</v>
@@ -2058,7 +2065,7 @@
       </c>
       <c r="D20" s="11"/>
     </row>
-    <row r="21" ht="27" spans="1:4">
+    <row r="21" ht="28.5" spans="1:4">
       <c r="A21" s="9"/>
       <c r="B21" s="14">
         <v>5</v>
@@ -2110,7 +2117,7 @@
       </c>
       <c r="D25" s="11"/>
     </row>
-    <row r="26" ht="13.5" spans="1:4">
+    <row r="26" ht="14.25" spans="1:4">
       <c r="A26" s="9"/>
       <c r="B26" s="16">
         <v>2</v>
@@ -2140,7 +2147,7 @@
       </c>
       <c r="D28" s="11"/>
     </row>
-    <row r="29" ht="79.5" spans="1:4">
+    <row r="29" ht="82.5" spans="1:4">
       <c r="A29" s="9"/>
       <c r="B29" s="14">
         <v>5</v>
@@ -2192,7 +2199,7 @@
       </c>
       <c r="D33" s="11"/>
     </row>
-    <row r="34" ht="80.25" spans="1:4">
+    <row r="34" ht="84" spans="1:4">
       <c r="A34" s="9"/>
       <c r="B34" s="14">
         <v>5</v>
@@ -2204,7 +2211,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" ht="27" spans="1:4">
+    <row r="35" ht="28.5" spans="1:4">
       <c r="A35" s="9"/>
       <c r="B35" s="14">
         <v>5</v>
@@ -2236,7 +2243,7 @@
       </c>
       <c r="D37" s="11"/>
     </row>
-    <row r="38" ht="39.75" spans="1:4">
+    <row r="38" ht="41.25" spans="1:4">
       <c r="A38" s="9"/>
       <c r="B38" s="14">
         <v>5</v>
@@ -2258,7 +2265,7 @@
       </c>
       <c r="D39" s="11"/>
     </row>
-    <row r="40" ht="78.75" spans="1:4">
+    <row r="40" ht="81" spans="1:4">
       <c r="A40" s="9"/>
       <c r="B40" s="14">
         <v>5</v>
@@ -2270,7 +2277,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" ht="27" spans="1:4">
+    <row r="41" ht="28.5" spans="1:4">
       <c r="A41" s="9"/>
       <c r="B41" s="14">
         <v>5</v>
@@ -2416,7 +2423,7 @@
       <c r="F53" s="17"/>
       <c r="G53" s="17"/>
     </row>
-    <row r="54" ht="51.75" spans="1:7">
+    <row r="54" ht="52.5" spans="1:7">
       <c r="A54" s="9"/>
       <c r="B54" s="16">
         <v>2</v>
@@ -2500,7 +2507,7 @@
       </c>
       <c r="D59" s="11"/>
     </row>
-    <row r="60" ht="40.5" spans="1:4">
+    <row r="60" ht="42.75" spans="1:4">
       <c r="A60" s="9"/>
       <c r="B60" s="10">
         <v>5</v>
@@ -2532,7 +2539,7 @@
       </c>
       <c r="D62" s="11"/>
     </row>
-    <row r="63" ht="80.25" spans="1:4">
+    <row r="63" ht="84" spans="1:4">
       <c r="A63" s="9"/>
       <c r="B63" s="10">
         <v>5</v>
@@ -2654,7 +2661,7 @@
       </c>
       <c r="D74" s="11"/>
     </row>
-    <row r="75" ht="40.5" spans="1:4">
+    <row r="75" ht="42.75" spans="1:4">
       <c r="A75" s="9"/>
       <c r="B75" s="10">
         <v>5</v>
@@ -2778,7 +2785,7 @@
       </c>
       <c r="D86" s="11"/>
     </row>
-    <row r="87" ht="39.75" spans="1:4">
+    <row r="87" ht="41.25" spans="1:4">
       <c r="A87" s="18"/>
       <c r="B87" s="10">
         <v>5</v>
@@ -2788,7 +2795,7 @@
       </c>
       <c r="D87" s="11"/>
     </row>
-    <row r="88" ht="52.5" spans="1:4">
+    <row r="88" ht="54" spans="1:4">
       <c r="A88" s="18"/>
       <c r="B88" s="10">
         <v>6</v>
@@ -2800,7 +2807,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="89" ht="13.5" spans="1:4">
+    <row r="89" ht="14.25" spans="1:4">
       <c r="A89" s="18"/>
       <c r="B89" s="19">
         <v>5</v>
@@ -2812,7 +2819,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="90" ht="27" spans="1:4">
+    <row r="90" ht="28.5" spans="1:4">
       <c r="A90" s="18"/>
       <c r="B90" s="19">
         <v>5</v>
@@ -2834,7 +2841,7 @@
       </c>
       <c r="D91" s="11"/>
     </row>
-    <row r="92" ht="93" spans="1:4">
+    <row r="92" ht="96.75" spans="1:4">
       <c r="A92" s="18"/>
       <c r="B92" s="19">
         <v>5</v>
@@ -2846,7 +2853,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="93" ht="93" spans="1:4">
+    <row r="93" ht="96.75" spans="1:4">
       <c r="A93" s="18"/>
       <c r="B93" s="19">
         <v>5</v>
@@ -2858,7 +2865,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="94" ht="53.25" spans="1:4">
+    <row r="94" ht="55.5" spans="1:4">
       <c r="A94" s="18"/>
       <c r="B94" s="19">
         <v>5</v>
@@ -2870,7 +2877,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="95" ht="106.5" spans="1:4">
+    <row r="95" ht="111" spans="1:4">
       <c r="A95" s="18"/>
       <c r="B95" s="19">
         <v>5</v>
@@ -2892,7 +2899,7 @@
       </c>
       <c r="D96" s="11"/>
     </row>
-    <row r="97" ht="26.25" spans="1:4">
+    <row r="97" ht="27" spans="1:4">
       <c r="A97" s="18"/>
       <c r="B97" s="19">
         <v>5</v>
@@ -2902,7 +2909,7 @@
       </c>
       <c r="D97" s="11"/>
     </row>
-    <row r="98" ht="39.75" spans="1:4">
+    <row r="98" ht="41.25" spans="1:4">
       <c r="A98" s="18"/>
       <c r="B98" s="19">
         <v>5</v>
@@ -2996,7 +3003,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="107" ht="39.75" spans="1:4">
+    <row r="107" ht="41.25" spans="1:4">
       <c r="A107" s="18"/>
       <c r="B107" s="19">
         <v>5</v>
@@ -3008,7 +3015,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="108" ht="156.75" spans="1:4">
+    <row r="108" ht="160.5" spans="1:4">
       <c r="A108" s="18"/>
       <c r="B108" s="19">
         <v>5</v>
@@ -3020,7 +3027,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="109" ht="27" spans="1:4">
+    <row r="109" ht="28.5" spans="1:4">
       <c r="A109" s="18"/>
       <c r="B109" s="19">
         <v>5</v>
@@ -3032,7 +3039,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="110" ht="54" spans="1:4">
+    <row r="110" ht="57" spans="1:4">
       <c r="A110" s="18"/>
       <c r="B110" s="19">
         <v>5</v>
@@ -3044,7 +3051,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="111" ht="54" spans="1:4">
+    <row r="111" ht="57" spans="1:4">
       <c r="A111" s="18"/>
       <c r="B111" s="19">
         <v>5</v>
@@ -3076,195 +3083,193 @@
       </c>
       <c r="D113" s="11"/>
     </row>
-    <row r="114" ht="25.5" spans="1:4">
+    <row r="114" ht="57" spans="1:4">
       <c r="A114" s="18"/>
       <c r="B114" s="19"/>
       <c r="C114" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D114" s="11"/>
-    </row>
-    <row r="115" ht="66.75" spans="1:4">
+      <c r="D114" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="115" ht="25.5" spans="1:4">
       <c r="A115" s="18"/>
-      <c r="B115" s="19">
-        <v>5</v>
-      </c>
+      <c r="B115" s="19"/>
       <c r="C115" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D115" s="11" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="116" ht="38.25" spans="1:4">
+      <c r="D115" s="11"/>
+    </row>
+    <row r="116" ht="25.5" spans="1:4">
       <c r="A116" s="18"/>
-      <c r="B116" s="19">
-        <v>0</v>
-      </c>
+      <c r="B116" s="19"/>
       <c r="C116" s="2" t="s">
         <v>160</v>
       </c>
       <c r="D116" s="11"/>
     </row>
-    <row r="117" ht="25.5" spans="1:4">
+    <row r="117" ht="69.75" spans="1:4">
       <c r="A117" s="18"/>
       <c r="B117" s="19">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C117" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D117" s="11"/>
-    </row>
-    <row r="118" ht="26.25" spans="1:4">
+      <c r="D117" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="118" ht="38.25" spans="1:4">
       <c r="A118" s="18"/>
       <c r="B118" s="19">
         <v>0</v>
       </c>
-      <c r="C118" s="12" t="s">
-        <v>162</v>
+      <c r="C118" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="D118" s="11"/>
     </row>
     <row r="119" ht="25.5" spans="1:4">
       <c r="A119" s="18"/>
-      <c r="B119" s="19"/>
-      <c r="C119" s="12" t="s">
-        <v>163</v>
+      <c r="B119" s="19">
+        <v>0</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="D119" s="11"/>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" ht="27" spans="1:4">
       <c r="A120" s="18"/>
-      <c r="B120" s="19"/>
+      <c r="B120" s="19">
+        <v>0</v>
+      </c>
       <c r="C120" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D120" s="11"/>
     </row>
-    <row r="121" ht="26.25" spans="1:4">
+    <row r="121" ht="25.5" spans="1:4">
       <c r="A121" s="18"/>
       <c r="B121" s="19"/>
       <c r="C121" s="12" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D121" s="11"/>
     </row>
-    <row r="122" ht="25.5" spans="1:4">
+    <row r="122" spans="1:4">
       <c r="A122" s="18"/>
-      <c r="B122" s="20">
-        <v>1</v>
-      </c>
+      <c r="B122" s="19"/>
       <c r="C122" s="12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D122" s="11"/>
     </row>
-    <row r="123" ht="25.5" spans="1:4">
+    <row r="123" ht="27" spans="1:4">
       <c r="A123" s="18"/>
-      <c r="B123" s="19">
-        <v>1</v>
-      </c>
+      <c r="B123" s="19"/>
       <c r="C123" s="12" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D123" s="11"/>
     </row>
     <row r="124" ht="25.5" spans="1:4">
       <c r="A124" s="18"/>
-      <c r="B124" s="19">
+      <c r="B124" s="20">
         <v>1</v>
       </c>
       <c r="C124" s="12" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D124" s="11"/>
     </row>
-    <row r="125" ht="26.25" spans="1:4">
+    <row r="125" ht="25.5" spans="1:4">
       <c r="A125" s="18"/>
       <c r="B125" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C125" s="12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D125" s="11"/>
     </row>
-    <row r="126" ht="66.75" spans="1:4">
+    <row r="126" ht="25.5" spans="1:4">
       <c r="A126" s="18"/>
       <c r="B126" s="19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C126" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D126" s="11" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="127" ht="25.5" spans="1:4">
+      <c r="D126" s="11"/>
+    </row>
+    <row r="127" ht="27" spans="1:4">
       <c r="A127" s="18"/>
-      <c r="B127" s="19"/>
+      <c r="B127" s="19">
+        <v>0</v>
+      </c>
       <c r="C127" s="12" t="s">
         <v>172</v>
       </c>
       <c r="D127" s="11"/>
     </row>
-    <row r="128" ht="26.25" spans="1:4">
+    <row r="128" ht="69.75" spans="1:4">
       <c r="A128" s="18"/>
-      <c r="B128" s="19"/>
+      <c r="B128" s="19">
+        <v>5</v>
+      </c>
       <c r="C128" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D128" s="11"/>
-    </row>
-    <row r="129" spans="1:4">
+      <c r="D128" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="129" ht="25.5" spans="1:4">
       <c r="A129" s="18"/>
       <c r="B129" s="19"/>
       <c r="C129" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D129" s="11"/>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" ht="27" spans="1:4">
       <c r="A130" s="18"/>
       <c r="B130" s="19"/>
       <c r="C130" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D130" s="11"/>
     </row>
-    <row r="131" ht="25.5" spans="1:4">
+    <row r="131" spans="1:4">
       <c r="A131" s="18"/>
-      <c r="B131" s="19">
-        <v>5</v>
-      </c>
+      <c r="B131" s="19"/>
       <c r="C131" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D131" s="11"/>
     </row>
-    <row r="132" ht="25.5" spans="1:4">
+    <row r="132" spans="1:4">
       <c r="A132" s="18"/>
       <c r="B132" s="19"/>
       <c r="C132" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D132" s="11"/>
     </row>
-    <row r="133" ht="27" spans="1:4">
+    <row r="133" ht="25.5" spans="1:4">
       <c r="A133" s="18"/>
       <c r="B133" s="19">
         <v>5</v>
       </c>
       <c r="C133" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="D133" s="11" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="134" spans="1:4">
+      <c r="D133" s="11"/>
+    </row>
+    <row r="134" ht="25.5" spans="1:4">
       <c r="A134" s="18"/>
       <c r="B134" s="19"/>
       <c r="C134" s="12" t="s">
@@ -3272,118 +3277,138 @@
       </c>
       <c r="D134" s="11"/>
     </row>
-    <row r="135" ht="24" spans="1:4">
+    <row r="135" ht="28.5" spans="1:4">
       <c r="A135" s="18"/>
       <c r="B135" s="19">
-        <v>1</v>
-      </c>
-      <c r="C135" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C135" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="D135" s="11"/>
-    </row>
-    <row r="136" ht="25.5" spans="1:4">
+      <c r="D135" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" s="18"/>
-      <c r="B136" s="19">
-        <v>1</v>
-      </c>
+      <c r="B136" s="19"/>
       <c r="C136" s="12" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D136" s="11"/>
     </row>
-    <row r="137" ht="25.5" spans="1:4">
+    <row r="137" ht="24" spans="1:4">
       <c r="A137" s="18"/>
       <c r="B137" s="19">
-        <v>5</v>
-      </c>
-      <c r="C137" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="D137" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C137" s="21" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="138" ht="53.25" spans="1:4">
+      <c r="D137" s="11"/>
+    </row>
+    <row r="138" ht="25.5" spans="1:4">
       <c r="A138" s="18"/>
       <c r="B138" s="19">
-        <v>5</v>
-      </c>
-      <c r="C138" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C138" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="D138" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="139" ht="28.5" spans="1:4">
+      <c r="D138" s="11"/>
+    </row>
+    <row r="139" ht="25.5" spans="1:4">
       <c r="A139" s="18"/>
       <c r="B139" s="19">
-        <v>2</v>
-      </c>
-      <c r="C139" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C139" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D139" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="D139" s="11"/>
-    </row>
-    <row r="140" ht="119.25" spans="1:4">
-      <c r="A140" s="23"/>
+    </row>
+    <row r="140" ht="55.5" spans="1:4">
+      <c r="A140" s="18"/>
       <c r="B140" s="19">
         <v>5</v>
       </c>
-      <c r="C140" s="11" t="s">
+      <c r="C140" s="22" t="s">
         <v>188</v>
       </c>
       <c r="D140" s="11" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="141" ht="26.25" spans="1:4">
-      <c r="A141" s="24" t="s">
+    <row r="141" ht="27" spans="1:4">
+      <c r="A141" s="18"/>
+      <c r="B141" s="19">
+        <v>2</v>
+      </c>
+      <c r="C141" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="B141" s="25"/>
-      <c r="C141" s="12" t="s">
+      <c r="D141" s="11"/>
+    </row>
+    <row r="142" ht="123.75" spans="1:4">
+      <c r="A142" s="23"/>
+      <c r="B142" s="19">
+        <v>5</v>
+      </c>
+      <c r="C142" s="11" t="s">
         <v>191</v>
       </c>
-      <c r="D141" s="12"/>
-    </row>
-    <row r="142" spans="1:4">
-      <c r="A142" s="24"/>
-      <c r="B142" s="25"/>
-      <c r="C142" s="12" t="s">
+      <c r="D142" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="D142" s="12"/>
-    </row>
-    <row r="143" ht="25.5" spans="1:3">
-      <c r="A143" t="s">
+    </row>
+    <row r="143" ht="27" spans="1:4">
+      <c r="A143" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="C143" s="2" t="s">
+      <c r="B143" s="25"/>
+      <c r="C143" s="12" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="144" ht="146.25" spans="2:4">
-      <c r="B144" s="19">
-        <v>5</v>
-      </c>
-      <c r="C144" s="2" t="s">
+      <c r="D143" s="12"/>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="24"/>
+      <c r="B144" s="25"/>
+      <c r="C144" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="D144" s="2" t="s">
+      <c r="D144" s="12"/>
+    </row>
+    <row r="145" ht="25.5" spans="1:3">
+      <c r="A145" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="145" ht="39" spans="2:4">
-      <c r="B145" s="19">
-        <v>5</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D145" s="2" t="s">
+    </row>
+    <row r="146" ht="152.25" spans="2:4">
+      <c r="B146" s="19">
+        <v>5</v>
+      </c>
+      <c r="C146" s="2" t="s">
         <v>198</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="147" ht="39.75" spans="2:4">
+      <c r="B147" s="19">
+        <v>5</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -3393,10 +3418,10 @@
     <mergeCell ref="A10:A17"/>
     <mergeCell ref="A18:A46"/>
     <mergeCell ref="A47:A85"/>
-    <mergeCell ref="A86:A140"/>
-    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="A86:A142"/>
+    <mergeCell ref="A143:A144"/>
   </mergeCells>
-  <conditionalFormatting sqref="B$1:B$1048576">
+  <conditionalFormatting sqref="B116:B1048576 B1:B114 B115">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
add comment for stripnet
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15120" windowHeight="25890"/>
+    <workbookView windowWidth="27720" windowHeight="13290"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210">
   <si>
     <t>Scope</t>
   </si>
@@ -615,6 +615,10 @@
   </si>
   <si>
     <t>StripNet: Towards Topology Consistent Strip Structure Segmentation</t>
+  </si>
+  <si>
+    <t>提出了一种由粗到精检测带状特征的方法：粗检测先确定整个带状目标的边界（确定RoI)，精检测时，用RoIAlign把对应的feature取出来，再划分RoI内的边界细分；
+做label的方法很值得借鉴：gt_label边界是1个像素，train的时候，gt_label先用低通滤波一下（变成高斯分布的一条带）再train更容易减小错误</t>
   </si>
   <si>
     <t>3D-LaneNet_end-to-end 3D multiple lane detection</t>
@@ -695,11 +699,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -736,13 +740,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -764,6 +761,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -780,37 +799,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -834,23 +824,37 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -870,23 +874,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -897,6 +887,13 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -933,19 +930,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -963,31 +960,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -999,13 +990,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1017,19 +1014,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1047,25 +1038,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1077,37 +1098,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1192,7 +1189,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1208,30 +1205,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1262,6 +1235,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1275,152 +1272,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1472,12 +1469,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1487,28 +1478,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1871,9 +1856,9 @@
   <dimension ref="A1:G152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
+      <selection pane="bottomLeft" activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -2073,7 +2058,7 @@
       <c r="D17" s="11"/>
     </row>
     <row r="18" ht="25.5" spans="1:4">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="16">
@@ -2085,7 +2070,7 @@
       <c r="D18" s="11"/>
     </row>
     <row r="19" ht="37" customHeight="1" spans="1:4">
-      <c r="A19" s="17"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="10">
         <v>5</v>
       </c>
@@ -2097,7 +2082,7 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="17"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="16">
         <v>3</v>
       </c>
@@ -2107,7 +2092,7 @@
       <c r="D20" s="11"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="17"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="14">
         <v>5</v>
       </c>
@@ -2117,7 +2102,7 @@
       <c r="D21" s="11"/>
     </row>
     <row r="22" ht="28.5" spans="1:4">
-      <c r="A22" s="17"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="14">
         <v>5</v>
       </c>
@@ -2129,7 +2114,7 @@
       </c>
     </row>
     <row r="23" ht="25.5" spans="1:4">
-      <c r="A23" s="17"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="16">
         <v>3</v>
       </c>
@@ -2139,7 +2124,7 @@
       <c r="D23" s="11"/>
     </row>
     <row r="24" ht="25.5" spans="1:4">
-      <c r="A24" s="17"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="16">
         <v>3</v>
       </c>
@@ -2149,7 +2134,7 @@
       <c r="D24" s="11"/>
     </row>
     <row r="25" ht="25.5" spans="1:4">
-      <c r="A25" s="17"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="16">
         <v>3</v>
       </c>
@@ -2159,7 +2144,7 @@
       <c r="D25" s="11"/>
     </row>
     <row r="26" ht="25.5" spans="1:4">
-      <c r="A26" s="17"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="16">
         <v>3</v>
       </c>
@@ -2169,7 +2154,7 @@
       <c r="D26" s="11"/>
     </row>
     <row r="27" ht="14.25" spans="1:4">
-      <c r="A27" s="17"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="16">
         <v>2</v>
       </c>
@@ -2179,7 +2164,7 @@
       <c r="D27" s="11"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="17"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="16">
         <v>2</v>
       </c>
@@ -2189,7 +2174,7 @@
       <c r="D28" s="11"/>
     </row>
     <row r="29" ht="25.5" spans="1:4">
-      <c r="A29" s="17"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="16">
         <v>2</v>
       </c>
@@ -2199,7 +2184,7 @@
       <c r="D29" s="11"/>
     </row>
     <row r="30" ht="82.5" spans="1:4">
-      <c r="A30" s="17"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="14">
         <v>5</v>
       </c>
@@ -2211,7 +2196,7 @@
       </c>
     </row>
     <row r="31" ht="25.5" spans="1:4">
-      <c r="A31" s="17"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="14">
         <v>1</v>
       </c>
@@ -2221,7 +2206,7 @@
       <c r="D31" s="11"/>
     </row>
     <row r="32" ht="25.5" spans="1:4">
-      <c r="A32" s="17"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="16">
         <v>2</v>
       </c>
@@ -2231,8 +2216,8 @@
       <c r="D32" s="11"/>
     </row>
     <row r="33" ht="25.5" spans="1:4">
-      <c r="A33" s="17"/>
-      <c r="B33" s="18">
+      <c r="A33" s="9"/>
+      <c r="B33" s="14">
         <v>5</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -2241,8 +2226,8 @@
       <c r="D33" s="11"/>
     </row>
     <row r="34" ht="25.5" spans="1:4">
-      <c r="A34" s="17"/>
-      <c r="B34" s="18">
+      <c r="A34" s="9"/>
+      <c r="B34" s="14">
         <v>5</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -2251,7 +2236,7 @@
       <c r="D34" s="11"/>
     </row>
     <row r="35" ht="84" spans="1:4">
-      <c r="A35" s="17"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="14">
         <v>5</v>
       </c>
@@ -2263,7 +2248,7 @@
       </c>
     </row>
     <row r="36" ht="28.5" spans="1:4">
-      <c r="A36" s="17"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="14">
         <v>5</v>
       </c>
@@ -2275,7 +2260,7 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="17"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="16">
         <v>2</v>
       </c>
@@ -2285,7 +2270,7 @@
       <c r="D37" s="11"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="17"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="16">
         <v>2</v>
       </c>
@@ -2295,7 +2280,7 @@
       <c r="D38" s="11"/>
     </row>
     <row r="39" ht="41.25" spans="1:4">
-      <c r="A39" s="17"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="14">
         <v>5</v>
       </c>
@@ -2307,7 +2292,7 @@
       </c>
     </row>
     <row r="40" ht="25.5" spans="1:4">
-      <c r="A40" s="17"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="16">
         <v>2</v>
       </c>
@@ -2317,7 +2302,7 @@
       <c r="D40" s="11"/>
     </row>
     <row r="41" ht="81" spans="1:4">
-      <c r="A41" s="17"/>
+      <c r="A41" s="9"/>
       <c r="B41" s="14">
         <v>5</v>
       </c>
@@ -2329,7 +2314,7 @@
       </c>
     </row>
     <row r="42" ht="28.5" spans="1:4">
-      <c r="A42" s="17"/>
+      <c r="A42" s="9"/>
       <c r="B42" s="14">
         <v>5</v>
       </c>
@@ -2341,8 +2326,8 @@
       </c>
     </row>
     <row r="43" ht="25.5" spans="1:4">
-      <c r="A43" s="17"/>
-      <c r="B43" s="18">
+      <c r="A43" s="9"/>
+      <c r="B43" s="14">
         <v>5</v>
       </c>
       <c r="C43" s="12" t="s">
@@ -2351,8 +2336,8 @@
       <c r="D43" s="11"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="17"/>
-      <c r="B44" s="18">
+      <c r="A44" s="9"/>
+      <c r="B44" s="14">
         <v>5</v>
       </c>
       <c r="C44" s="12" t="s">
@@ -2361,7 +2346,7 @@
       <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="17"/>
+      <c r="A45" s="9"/>
       <c r="B45" s="16">
         <v>2</v>
       </c>
@@ -2371,7 +2356,7 @@
       <c r="D45" s="11"/>
     </row>
     <row r="46" ht="53" customHeight="1" spans="1:4">
-      <c r="A46" s="17"/>
+      <c r="A46" s="9"/>
       <c r="B46" s="14">
         <v>5</v>
       </c>
@@ -2383,7 +2368,7 @@
       </c>
     </row>
     <row r="47" ht="41" customHeight="1" spans="1:4">
-      <c r="A47" s="17"/>
+      <c r="A47" s="9"/>
       <c r="B47" s="14">
         <v>5</v>
       </c>
@@ -2455,10 +2440,10 @@
         <v>74</v>
       </c>
       <c r="D53" s="11"/>
-      <c r="F53" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="G53" s="19" t="s">
+      <c r="F53" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G53" s="17" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2471,8 +2456,8 @@
         <v>76</v>
       </c>
       <c r="D54" s="11"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="19"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
     </row>
     <row r="55" ht="52.5" spans="1:7">
       <c r="A55" s="9"/>
@@ -2845,7 +2830,7 @@
       <c r="D88" s="11"/>
     </row>
     <row r="89" ht="25.5" spans="1:4">
-      <c r="A89" s="20" t="s">
+      <c r="A89" s="18" t="s">
         <v>118</v>
       </c>
       <c r="B89" s="16">
@@ -2857,7 +2842,7 @@
       <c r="D89" s="11"/>
     </row>
     <row r="90" ht="41.25" spans="1:4">
-      <c r="A90" s="20"/>
+      <c r="A90" s="18"/>
       <c r="B90" s="10">
         <v>5</v>
       </c>
@@ -2867,7 +2852,7 @@
       <c r="D90" s="11"/>
     </row>
     <row r="91" ht="54" spans="1:4">
-      <c r="A91" s="20"/>
+      <c r="A91" s="18"/>
       <c r="B91" s="10">
         <v>6</v>
       </c>
@@ -2879,8 +2864,8 @@
       </c>
     </row>
     <row r="92" ht="14.25" spans="1:4">
-      <c r="A92" s="20"/>
-      <c r="B92" s="21">
+      <c r="A92" s="18"/>
+      <c r="B92" s="19">
         <v>5</v>
       </c>
       <c r="C92" s="11" t="s">
@@ -2891,8 +2876,8 @@
       </c>
     </row>
     <row r="93" ht="28.5" spans="1:4">
-      <c r="A93" s="20"/>
-      <c r="B93" s="21">
+      <c r="A93" s="18"/>
+      <c r="B93" s="19">
         <v>5</v>
       </c>
       <c r="C93" s="11" t="s">
@@ -2903,8 +2888,8 @@
       </c>
     </row>
     <row r="94" ht="25.5" spans="1:4">
-      <c r="A94" s="20"/>
-      <c r="B94" s="21">
+      <c r="A94" s="18"/>
+      <c r="B94" s="19">
         <v>1</v>
       </c>
       <c r="C94" s="11" t="s">
@@ -2913,8 +2898,8 @@
       <c r="D94" s="11"/>
     </row>
     <row r="95" ht="96.75" spans="1:4">
-      <c r="A95" s="20"/>
-      <c r="B95" s="21">
+      <c r="A95" s="18"/>
+      <c r="B95" s="19">
         <v>5</v>
       </c>
       <c r="C95" s="11" t="s">
@@ -2925,8 +2910,8 @@
       </c>
     </row>
     <row r="96" ht="96.75" spans="1:4">
-      <c r="A96" s="20"/>
-      <c r="B96" s="21">
+      <c r="A96" s="18"/>
+      <c r="B96" s="19">
         <v>5</v>
       </c>
       <c r="C96" s="11" t="s">
@@ -2937,8 +2922,8 @@
       </c>
     </row>
     <row r="97" ht="55.5" spans="1:4">
-      <c r="A97" s="20"/>
-      <c r="B97" s="21">
+      <c r="A97" s="18"/>
+      <c r="B97" s="19">
         <v>5</v>
       </c>
       <c r="C97" s="11" t="s">
@@ -2949,8 +2934,8 @@
       </c>
     </row>
     <row r="98" ht="111" spans="1:4">
-      <c r="A98" s="20"/>
-      <c r="B98" s="21">
+      <c r="A98" s="18"/>
+      <c r="B98" s="19">
         <v>5</v>
       </c>
       <c r="C98" s="11" t="s">
@@ -2961,8 +2946,8 @@
       </c>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="20"/>
-      <c r="B99" s="21">
+      <c r="A99" s="18"/>
+      <c r="B99" s="19">
         <v>5</v>
       </c>
       <c r="C99" s="11" t="s">
@@ -2971,8 +2956,8 @@
       <c r="D99" s="11"/>
     </row>
     <row r="100" ht="27" spans="1:4">
-      <c r="A100" s="20"/>
-      <c r="B100" s="21">
+      <c r="A100" s="18"/>
+      <c r="B100" s="19">
         <v>5</v>
       </c>
       <c r="C100" s="11" t="s">
@@ -2981,8 +2966,8 @@
       <c r="D100" s="11"/>
     </row>
     <row r="101" ht="41.25" spans="1:4">
-      <c r="A101" s="20"/>
-      <c r="B101" s="21">
+      <c r="A101" s="18"/>
+      <c r="B101" s="19">
         <v>5</v>
       </c>
       <c r="C101" s="11" t="s">
@@ -2993,8 +2978,8 @@
       </c>
     </row>
     <row r="102" ht="25.5" spans="1:4">
-      <c r="A102" s="20"/>
-      <c r="B102" s="21">
+      <c r="A102" s="18"/>
+      <c r="B102" s="19">
         <v>2</v>
       </c>
       <c r="C102" s="12" t="s">
@@ -3003,8 +2988,8 @@
       <c r="D102" s="11"/>
     </row>
     <row r="103" ht="25.5" spans="1:4">
-      <c r="A103" s="20"/>
-      <c r="B103" s="21">
+      <c r="A103" s="18"/>
+      <c r="B103" s="19">
         <v>2</v>
       </c>
       <c r="C103" s="12" t="s">
@@ -3013,8 +2998,8 @@
       <c r="D103" s="11"/>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="20"/>
-      <c r="B104" s="21">
+      <c r="A104" s="18"/>
+      <c r="B104" s="19">
         <v>1</v>
       </c>
       <c r="C104" t="s">
@@ -3023,8 +3008,8 @@
       <c r="D104" s="11"/>
     </row>
     <row r="105" ht="25.5" spans="1:4">
-      <c r="A105" s="20"/>
-      <c r="B105" s="21">
+      <c r="A105" s="18"/>
+      <c r="B105" s="19">
         <v>2</v>
       </c>
       <c r="C105" s="2" t="s">
@@ -3033,8 +3018,8 @@
       <c r="D105" s="11"/>
     </row>
     <row r="106" ht="25.5" spans="1:4">
-      <c r="A106" s="20"/>
-      <c r="B106" s="21">
+      <c r="A106" s="18"/>
+      <c r="B106" s="19">
         <v>2</v>
       </c>
       <c r="C106" s="12" t="s">
@@ -3043,8 +3028,8 @@
       <c r="D106" s="11"/>
     </row>
     <row r="107" spans="1:4">
-      <c r="A107" s="20"/>
-      <c r="B107" s="21">
+      <c r="A107" s="18"/>
+      <c r="B107" s="19">
         <v>2</v>
       </c>
       <c r="C107" s="12" t="s">
@@ -3053,8 +3038,8 @@
       <c r="D107" s="11"/>
     </row>
     <row r="108" ht="25.5" spans="1:4">
-      <c r="A108" s="20"/>
-      <c r="B108" s="21">
+      <c r="A108" s="18"/>
+      <c r="B108" s="19">
         <v>2</v>
       </c>
       <c r="C108" s="12" t="s">
@@ -3063,8 +3048,8 @@
       <c r="D108" s="11"/>
     </row>
     <row r="109" ht="25.5" spans="1:4">
-      <c r="A109" s="20"/>
-      <c r="B109" s="21">
+      <c r="A109" s="18"/>
+      <c r="B109" s="19">
         <v>5</v>
       </c>
       <c r="C109" s="12" t="s">
@@ -3075,8 +3060,8 @@
       </c>
     </row>
     <row r="110" ht="41.25" spans="1:4">
-      <c r="A110" s="20"/>
-      <c r="B110" s="21">
+      <c r="A110" s="18"/>
+      <c r="B110" s="19">
         <v>5</v>
       </c>
       <c r="C110" s="12" t="s">
@@ -3087,8 +3072,8 @@
       </c>
     </row>
     <row r="111" ht="160.5" spans="1:4">
-      <c r="A111" s="20"/>
-      <c r="B111" s="21">
+      <c r="A111" s="18"/>
+      <c r="B111" s="19">
         <v>5</v>
       </c>
       <c r="C111" s="12" t="s">
@@ -3099,8 +3084,8 @@
       </c>
     </row>
     <row r="112" ht="28.5" spans="1:4">
-      <c r="A112" s="20"/>
-      <c r="B112" s="21">
+      <c r="A112" s="18"/>
+      <c r="B112" s="19">
         <v>5</v>
       </c>
       <c r="C112" s="12" t="s">
@@ -3111,8 +3096,8 @@
       </c>
     </row>
     <row r="113" ht="57" spans="1:4">
-      <c r="A113" s="20"/>
-      <c r="B113" s="21">
+      <c r="A113" s="18"/>
+      <c r="B113" s="19">
         <v>5</v>
       </c>
       <c r="C113" s="12" t="s">
@@ -3123,8 +3108,8 @@
       </c>
     </row>
     <row r="114" ht="57" spans="1:4">
-      <c r="A114" s="20"/>
-      <c r="B114" s="21">
+      <c r="A114" s="18"/>
+      <c r="B114" s="19">
         <v>5</v>
       </c>
       <c r="C114" s="12" t="s">
@@ -3135,8 +3120,8 @@
       </c>
     </row>
     <row r="115" spans="1:4">
-      <c r="A115" s="20"/>
-      <c r="B115" s="21">
+      <c r="A115" s="18"/>
+      <c r="B115" s="19">
         <v>2</v>
       </c>
       <c r="C115" s="2" t="s">
@@ -3145,8 +3130,8 @@
       <c r="D115" s="11"/>
     </row>
     <row r="116" ht="25.5" spans="1:4">
-      <c r="A116" s="20"/>
-      <c r="B116" s="21">
+      <c r="A116" s="18"/>
+      <c r="B116" s="19">
         <v>2</v>
       </c>
       <c r="C116" s="2" t="s">
@@ -3155,8 +3140,8 @@
       <c r="D116" s="11"/>
     </row>
     <row r="117" ht="57" spans="1:4">
-      <c r="A117" s="20"/>
-      <c r="B117" s="21">
+      <c r="A117" s="18"/>
+      <c r="B117" s="19">
         <v>5</v>
       </c>
       <c r="C117" s="2" t="s">
@@ -3167,8 +3152,8 @@
       </c>
     </row>
     <row r="118" ht="69.75" spans="1:4">
-      <c r="A118" s="20"/>
-      <c r="B118" s="21">
+      <c r="A118" s="18"/>
+      <c r="B118" s="19">
         <v>5</v>
       </c>
       <c r="C118" s="2" t="s">
@@ -3179,18 +3164,18 @@
       </c>
     </row>
     <row r="119" spans="1:4">
-      <c r="A119" s="20"/>
-      <c r="B119" s="21">
-        <v>1</v>
-      </c>
-      <c r="C119" s="22" t="s">
+      <c r="A119" s="18"/>
+      <c r="B119" s="19">
+        <v>1</v>
+      </c>
+      <c r="C119" s="2" t="s">
         <v>165</v>
       </c>
       <c r="D119" s="11"/>
     </row>
     <row r="120" ht="25.5" spans="1:4">
-      <c r="A120" s="20"/>
-      <c r="B120" s="21">
+      <c r="A120" s="18"/>
+      <c r="B120" s="19">
         <v>1</v>
       </c>
       <c r="C120" s="2" t="s">
@@ -3199,8 +3184,8 @@
       <c r="D120" s="11"/>
     </row>
     <row r="121" ht="25.5" spans="1:4">
-      <c r="A121" s="20"/>
-      <c r="B121" s="21">
+      <c r="A121" s="18"/>
+      <c r="B121" s="19">
         <v>1</v>
       </c>
       <c r="C121" s="2" t="s">
@@ -3209,8 +3194,8 @@
       <c r="D121" s="11"/>
     </row>
     <row r="122" ht="69.75" spans="1:4">
-      <c r="A122" s="20"/>
-      <c r="B122" s="21">
+      <c r="A122" s="18"/>
+      <c r="B122" s="19">
         <v>5</v>
       </c>
       <c r="C122" s="2" t="s">
@@ -3221,8 +3206,8 @@
       </c>
     </row>
     <row r="123" ht="38.25" spans="1:4">
-      <c r="A123" s="20"/>
-      <c r="B123" s="21">
+      <c r="A123" s="18"/>
+      <c r="B123" s="19">
         <v>1</v>
       </c>
       <c r="C123" s="2" t="s">
@@ -3231,8 +3216,8 @@
       <c r="D123" s="11"/>
     </row>
     <row r="124" ht="25.5" spans="1:4">
-      <c r="A124" s="20"/>
-      <c r="B124" s="21">
+      <c r="A124" s="18"/>
+      <c r="B124" s="19">
         <v>1</v>
       </c>
       <c r="C124" s="2" t="s">
@@ -3241,8 +3226,8 @@
       <c r="D124" s="11"/>
     </row>
     <row r="125" ht="27" spans="1:4">
-      <c r="A125" s="20"/>
-      <c r="B125" s="21">
+      <c r="A125" s="18"/>
+      <c r="B125" s="19">
         <v>1</v>
       </c>
       <c r="C125" s="12" t="s">
@@ -3251,8 +3236,8 @@
       <c r="D125" s="11"/>
     </row>
     <row r="126" ht="25.5" spans="1:4">
-      <c r="A126" s="20"/>
-      <c r="B126" s="21">
+      <c r="A126" s="18"/>
+      <c r="B126" s="19">
         <v>1</v>
       </c>
       <c r="C126" s="12" t="s">
@@ -3261,8 +3246,8 @@
       <c r="D126" s="11"/>
     </row>
     <row r="127" spans="1:4">
-      <c r="A127" s="20"/>
-      <c r="B127" s="21">
+      <c r="A127" s="18"/>
+      <c r="B127" s="19">
         <v>1</v>
       </c>
       <c r="C127" s="12" t="s">
@@ -3271,8 +3256,8 @@
       <c r="D127" s="11"/>
     </row>
     <row r="128" ht="27" spans="1:4">
-      <c r="A128" s="20"/>
-      <c r="B128" s="21">
+      <c r="A128" s="18"/>
+      <c r="B128" s="19">
         <v>1</v>
       </c>
       <c r="C128" s="12" t="s">
@@ -3281,8 +3266,8 @@
       <c r="D128" s="11"/>
     </row>
     <row r="129" ht="25.5" spans="1:4">
-      <c r="A129" s="20"/>
-      <c r="B129" s="23">
+      <c r="A129" s="18"/>
+      <c r="B129" s="20">
         <v>1</v>
       </c>
       <c r="C129" s="12" t="s">
@@ -3291,8 +3276,8 @@
       <c r="D129" s="11"/>
     </row>
     <row r="130" ht="25.5" spans="1:4">
-      <c r="A130" s="20"/>
-      <c r="B130" s="21">
+      <c r="A130" s="18"/>
+      <c r="B130" s="19">
         <v>1</v>
       </c>
       <c r="C130" s="12" t="s">
@@ -3301,8 +3286,8 @@
       <c r="D130" s="11"/>
     </row>
     <row r="131" ht="25.5" spans="1:4">
-      <c r="A131" s="20"/>
-      <c r="B131" s="21">
+      <c r="A131" s="18"/>
+      <c r="B131" s="19">
         <v>1</v>
       </c>
       <c r="C131" s="12" t="s">
@@ -3311,8 +3296,8 @@
       <c r="D131" s="11"/>
     </row>
     <row r="132" ht="27" spans="1:4">
-      <c r="A132" s="20"/>
-      <c r="B132" s="21">
+      <c r="A132" s="18"/>
+      <c r="B132" s="19">
         <v>1</v>
       </c>
       <c r="C132" s="12" t="s">
@@ -3321,8 +3306,8 @@
       <c r="D132" s="11"/>
     </row>
     <row r="133" ht="69.75" spans="1:4">
-      <c r="A133" s="20"/>
-      <c r="B133" s="21">
+      <c r="A133" s="18"/>
+      <c r="B133" s="19">
         <v>5</v>
       </c>
       <c r="C133" s="12" t="s">
@@ -3333,8 +3318,8 @@
       </c>
     </row>
     <row r="134" ht="25.5" spans="1:4">
-      <c r="A134" s="20"/>
-      <c r="B134" s="21">
+      <c r="A134" s="18"/>
+      <c r="B134" s="19">
         <v>1</v>
       </c>
       <c r="C134" s="12" t="s">
@@ -3343,8 +3328,8 @@
       <c r="D134" s="11"/>
     </row>
     <row r="135" ht="27" spans="1:4">
-      <c r="A135" s="20"/>
-      <c r="B135" s="21">
+      <c r="A135" s="18"/>
+      <c r="B135" s="19">
         <v>1</v>
       </c>
       <c r="C135" s="12" t="s">
@@ -3353,8 +3338,8 @@
       <c r="D135" s="11"/>
     </row>
     <row r="136" spans="1:4">
-      <c r="A136" s="20"/>
-      <c r="B136" s="21">
+      <c r="A136" s="18"/>
+      <c r="B136" s="19">
         <v>1</v>
       </c>
       <c r="C136" s="12" t="s">
@@ -3363,8 +3348,8 @@
       <c r="D136" s="11"/>
     </row>
     <row r="137" spans="1:4">
-      <c r="A137" s="20"/>
-      <c r="B137" s="21">
+      <c r="A137" s="18"/>
+      <c r="B137" s="19">
         <v>1</v>
       </c>
       <c r="C137" s="12" t="s">
@@ -3373,8 +3358,8 @@
       <c r="D137" s="11"/>
     </row>
     <row r="138" ht="25.5" spans="1:4">
-      <c r="A138" s="20"/>
-      <c r="B138" s="21">
+      <c r="A138" s="18"/>
+      <c r="B138" s="19">
         <v>5</v>
       </c>
       <c r="C138" s="12" t="s">
@@ -3382,159 +3367,161 @@
       </c>
       <c r="D138" s="11"/>
     </row>
-    <row r="139" ht="25.5" spans="1:4">
-      <c r="A139" s="20"/>
-      <c r="B139" s="21">
+    <row r="139" ht="57" spans="1:4">
+      <c r="A139" s="18"/>
+      <c r="B139" s="19">
         <v>1</v>
       </c>
       <c r="C139" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="D139" s="11"/>
+      <c r="D139" s="11" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="140" ht="28.5" spans="1:4">
-      <c r="A140" s="20"/>
-      <c r="B140" s="21">
+      <c r="A140" s="18"/>
+      <c r="B140" s="19">
         <v>5</v>
       </c>
       <c r="C140" s="12" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D140" s="11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="141" ht="24" spans="1:4">
-      <c r="A141" s="20"/>
-      <c r="B141" s="21">
-        <v>1</v>
-      </c>
-      <c r="C141" s="24" t="s">
-        <v>190</v>
+      <c r="A141" s="18"/>
+      <c r="B141" s="19">
+        <v>1</v>
+      </c>
+      <c r="C141" s="21" t="s">
+        <v>191</v>
       </c>
       <c r="D141" s="11"/>
     </row>
     <row r="142" ht="25.5" spans="1:4">
-      <c r="A142" s="20"/>
-      <c r="B142" s="21">
+      <c r="A142" s="18"/>
+      <c r="B142" s="19">
         <v>1</v>
       </c>
       <c r="C142" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D142" s="11"/>
     </row>
     <row r="143" ht="25.5" spans="1:4">
-      <c r="A143" s="20"/>
-      <c r="B143" s="21">
+      <c r="A143" s="18"/>
+      <c r="B143" s="19">
         <v>5</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D143" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="144" ht="55.5" spans="1:4">
-      <c r="A144" s="20"/>
-      <c r="B144" s="21">
-        <v>5</v>
-      </c>
-      <c r="C144" s="25" t="s">
-        <v>194</v>
+      <c r="A144" s="18"/>
+      <c r="B144" s="19">
+        <v>5</v>
+      </c>
+      <c r="C144" s="22" t="s">
+        <v>195</v>
       </c>
       <c r="D144" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="145" ht="27" spans="1:4">
-      <c r="A145" s="20"/>
-      <c r="B145" s="21">
-        <v>2</v>
-      </c>
-      <c r="C145" s="25" t="s">
-        <v>196</v>
+      <c r="A145" s="18"/>
+      <c r="B145" s="19">
+        <v>2</v>
+      </c>
+      <c r="C145" s="22" t="s">
+        <v>197</v>
       </c>
       <c r="D145" s="11"/>
     </row>
     <row r="146" ht="123.75" spans="1:4">
-      <c r="A146" s="26"/>
-      <c r="B146" s="21">
+      <c r="A146" s="23"/>
+      <c r="B146" s="19">
         <v>5</v>
       </c>
       <c r="C146" s="11" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D146" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="147" ht="25.5" spans="1:4">
-      <c r="A147" s="27" t="s">
-        <v>199</v>
-      </c>
-      <c r="B147" s="28">
+      <c r="A147" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="B147" s="25">
         <v>1</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D147" s="12"/>
     </row>
     <row r="148" ht="27" spans="1:4">
-      <c r="A148" s="27"/>
-      <c r="B148" s="28">
+      <c r="A148" s="24"/>
+      <c r="B148" s="25">
         <v>1</v>
       </c>
       <c r="C148" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D148" s="12"/>
     </row>
     <row r="149" spans="1:4">
-      <c r="A149" s="27"/>
-      <c r="B149" s="28">
+      <c r="A149" s="24"/>
+      <c r="B149" s="25">
         <v>1</v>
       </c>
       <c r="C149" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D149" s="12"/>
     </row>
     <row r="150" ht="25.5" spans="1:3">
-      <c r="A150" s="29" t="s">
-        <v>203</v>
+      <c r="A150" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="B150" s="1">
         <v>1</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="151" ht="152.25" spans="1:4">
-      <c r="A151" s="29"/>
-      <c r="B151" s="21">
+      <c r="A151" s="1"/>
+      <c r="B151" s="19">
         <v>5</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="152" ht="39.75" spans="1:4">
-      <c r="A152" s="29"/>
-      <c r="B152" s="21">
+      <c r="A152" s="1"/>
+      <c r="B152" s="19">
         <v>5</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -3548,7 +3535,7 @@
     <mergeCell ref="A147:A149"/>
     <mergeCell ref="A150:A152"/>
   </mergeCells>
-  <conditionalFormatting sqref="B120:B1048576 B1:B118 B119">
+  <conditionalFormatting sqref="B:B">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
add note for stripnet
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="13290"/>
+    <workbookView windowWidth="27720" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -618,7 +618,8 @@
   </si>
   <si>
     <t>提出了一种由粗到精检测带状特征的方法：粗检测先确定整个带状目标的边界（确定RoI)，精检测时，用RoIAlign把对应的feature取出来，再划分RoI内的边界细分；
-做label的方法很值得借鉴：gt_label边界是1个像素，train的时候，gt_label先用低通滤波一下（变成高斯分布的一条带）再train更容易减小错误</t>
+做label的方法很值得借鉴：gt_label边界是1个像素，train的时候，gt_label先用低通滤波一下（变成高斯分布的一条带）再train更容易减小错误
+decompose the original segmantation problam into more easily solved boundary-regression problems, in a coarse-to-fine manner</t>
   </si>
   <si>
     <t>3D-LaneNet_end-to-end 3D multiple lane detection</t>
@@ -698,10 +699,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -753,9 +754,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -763,13 +764,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -783,6 +777,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -791,19 +793,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -814,32 +823,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -847,6 +832,22 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -861,32 +862,32 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -924,19 +925,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -948,19 +955,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -978,13 +979,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -996,13 +997,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1014,7 +1069,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1026,85 +1099,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1170,21 +1171,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1209,13 +1195,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1231,6 +1221,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1272,148 +1273,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1517,8 +1518,8 @@
     <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
     <cellStyle name="Accent2" xfId="17" builtinId="33"/>
     <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
-    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
     <cellStyle name="Neutral" xfId="21" builtinId="28"/>
     <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
@@ -1534,19 +1535,19 @@
     <cellStyle name="Good" xfId="33" builtinId="26"/>
     <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
     <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
-    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
-    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
-    <cellStyle name="Comma" xfId="46" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
-    <cellStyle name="Percent" xfId="48" builtinId="5"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -1591,6 +1592,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1846,19 +1852,18 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:G152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D139" sqref="D139"/>
+      <selection pane="bottomLeft" activeCell="C139" sqref="C139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -1885,7 +1890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="14.25" spans="1:4">
+    <row r="2" ht="13.5" spans="1:4">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -1897,7 +1902,7 @@
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" ht="14.25" spans="1:4">
+    <row r="3" ht="13.5" spans="1:4">
       <c r="A3" s="9"/>
       <c r="B3" s="10">
         <v>5</v>
@@ -1907,7 +1912,7 @@
       </c>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" ht="14.25" spans="1:4">
+    <row r="4" ht="13.5" spans="1:4">
       <c r="A4" s="9"/>
       <c r="B4" s="10">
         <v>5</v>
@@ -1917,7 +1922,7 @@
       </c>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" ht="14.25" spans="1:4">
+    <row r="5" ht="13.5" spans="1:4">
       <c r="A5" s="9"/>
       <c r="B5" s="10">
         <v>5</v>
@@ -1929,7 +1934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="14.25" spans="1:4">
+    <row r="6" ht="13.5" spans="1:4">
       <c r="A6" s="9"/>
       <c r="B6" s="10"/>
       <c r="C6" s="12" t="s">
@@ -1949,7 +1954,7 @@
       </c>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" ht="27" spans="1:4">
+    <row r="8" ht="26.25" spans="1:4">
       <c r="A8" s="9"/>
       <c r="B8" s="10">
         <v>2</v>
@@ -1969,7 +1974,7 @@
       </c>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" ht="39.75" spans="1:4">
+    <row r="10" ht="39" spans="1:4">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -1983,7 +1988,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" ht="14.25" spans="1:4">
+    <row r="11" ht="13.5" spans="1:4">
       <c r="A11" s="9"/>
       <c r="B11" s="13">
         <v>5</v>
@@ -2047,7 +2052,7 @@
       </c>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" ht="54" spans="1:4">
+    <row r="17" ht="52.5" spans="1:4">
       <c r="A17" s="9"/>
       <c r="B17" s="16">
         <v>2</v>
@@ -2101,7 +2106,7 @@
       </c>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" ht="28.5" spans="1:4">
+    <row r="22" ht="27" spans="1:4">
       <c r="A22" s="9"/>
       <c r="B22" s="14">
         <v>5</v>
@@ -2153,7 +2158,7 @@
       </c>
       <c r="D26" s="11"/>
     </row>
-    <row r="27" ht="14.25" spans="1:4">
+    <row r="27" ht="13.5" spans="1:4">
       <c r="A27" s="9"/>
       <c r="B27" s="16">
         <v>2</v>
@@ -2183,7 +2188,7 @@
       </c>
       <c r="D29" s="11"/>
     </row>
-    <row r="30" ht="82.5" spans="1:4">
+    <row r="30" ht="79.5" spans="1:4">
       <c r="A30" s="9"/>
       <c r="B30" s="14">
         <v>5</v>
@@ -2235,7 +2240,7 @@
       </c>
       <c r="D34" s="11"/>
     </row>
-    <row r="35" ht="84" spans="1:4">
+    <row r="35" ht="80.25" spans="1:4">
       <c r="A35" s="9"/>
       <c r="B35" s="14">
         <v>5</v>
@@ -2247,7 +2252,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" ht="28.5" spans="1:4">
+    <row r="36" ht="27" spans="1:4">
       <c r="A36" s="9"/>
       <c r="B36" s="14">
         <v>5</v>
@@ -2279,7 +2284,7 @@
       </c>
       <c r="D38" s="11"/>
     </row>
-    <row r="39" ht="41.25" spans="1:4">
+    <row r="39" ht="39.75" spans="1:4">
       <c r="A39" s="9"/>
       <c r="B39" s="14">
         <v>5</v>
@@ -2301,7 +2306,7 @@
       </c>
       <c r="D40" s="11"/>
     </row>
-    <row r="41" ht="81" spans="1:4">
+    <row r="41" ht="78.75" spans="1:4">
       <c r="A41" s="9"/>
       <c r="B41" s="14">
         <v>5</v>
@@ -2313,7 +2318,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" ht="28.5" spans="1:4">
+    <row r="42" ht="27" spans="1:4">
       <c r="A42" s="9"/>
       <c r="B42" s="14">
         <v>5</v>
@@ -2459,7 +2464,7 @@
       <c r="F54" s="17"/>
       <c r="G54" s="17"/>
     </row>
-    <row r="55" ht="52.5" spans="1:7">
+    <row r="55" ht="51.75" spans="1:7">
       <c r="A55" s="9"/>
       <c r="B55" s="16">
         <v>2</v>
@@ -2543,7 +2548,7 @@
       </c>
       <c r="D60" s="11"/>
     </row>
-    <row r="61" ht="42.75" spans="1:4">
+    <row r="61" ht="40.5" spans="1:4">
       <c r="A61" s="9"/>
       <c r="B61" s="10">
         <v>5</v>
@@ -2575,7 +2580,7 @@
       </c>
       <c r="D63" s="11"/>
     </row>
-    <row r="64" ht="84" spans="1:4">
+    <row r="64" ht="80.25" spans="1:4">
       <c r="A64" s="9"/>
       <c r="B64" s="10">
         <v>5</v>
@@ -2697,7 +2702,7 @@
       </c>
       <c r="D75" s="11"/>
     </row>
-    <row r="76" ht="42.75" spans="1:4">
+    <row r="76" ht="40.5" spans="1:4">
       <c r="A76" s="9"/>
       <c r="B76" s="10">
         <v>5</v>
@@ -2841,7 +2846,7 @@
       </c>
       <c r="D89" s="11"/>
     </row>
-    <row r="90" ht="41.25" spans="1:4">
+    <row r="90" ht="39.75" spans="1:4">
       <c r="A90" s="18"/>
       <c r="B90" s="10">
         <v>5</v>
@@ -2851,7 +2856,7 @@
       </c>
       <c r="D90" s="11"/>
     </row>
-    <row r="91" ht="54" spans="1:4">
+    <row r="91" ht="52.5" spans="1:4">
       <c r="A91" s="18"/>
       <c r="B91" s="10">
         <v>6</v>
@@ -2863,7 +2868,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="92" ht="14.25" spans="1:4">
+    <row r="92" ht="13.5" spans="1:4">
       <c r="A92" s="18"/>
       <c r="B92" s="19">
         <v>5</v>
@@ -2875,7 +2880,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="93" ht="28.5" spans="1:4">
+    <row r="93" ht="27" spans="1:4">
       <c r="A93" s="18"/>
       <c r="B93" s="19">
         <v>5</v>
@@ -2897,7 +2902,7 @@
       </c>
       <c r="D94" s="11"/>
     </row>
-    <row r="95" ht="96.75" spans="1:4">
+    <row r="95" ht="93" spans="1:4">
       <c r="A95" s="18"/>
       <c r="B95" s="19">
         <v>5</v>
@@ -2909,7 +2914,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="96" ht="96.75" spans="1:4">
+    <row r="96" ht="93" spans="1:4">
       <c r="A96" s="18"/>
       <c r="B96" s="19">
         <v>5</v>
@@ -2921,7 +2926,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="97" ht="55.5" spans="1:4">
+    <row r="97" ht="53.25" spans="1:4">
       <c r="A97" s="18"/>
       <c r="B97" s="19">
         <v>5</v>
@@ -2933,7 +2938,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="98" ht="111" spans="1:4">
+    <row r="98" ht="106.5" spans="1:4">
       <c r="A98" s="18"/>
       <c r="B98" s="19">
         <v>5</v>
@@ -2955,7 +2960,7 @@
       </c>
       <c r="D99" s="11"/>
     </row>
-    <row r="100" ht="27" spans="1:4">
+    <row r="100" ht="26.25" spans="1:4">
       <c r="A100" s="18"/>
       <c r="B100" s="19">
         <v>5</v>
@@ -2965,7 +2970,7 @@
       </c>
       <c r="D100" s="11"/>
     </row>
-    <row r="101" ht="41.25" spans="1:4">
+    <row r="101" ht="39.75" spans="1:4">
       <c r="A101" s="18"/>
       <c r="B101" s="19">
         <v>5</v>
@@ -3059,7 +3064,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="110" ht="41.25" spans="1:4">
+    <row r="110" ht="39.75" spans="1:4">
       <c r="A110" s="18"/>
       <c r="B110" s="19">
         <v>5</v>
@@ -3071,7 +3076,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="111" ht="160.5" spans="1:4">
+    <row r="111" ht="156.75" spans="1:4">
       <c r="A111" s="18"/>
       <c r="B111" s="19">
         <v>5</v>
@@ -3083,7 +3088,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="112" ht="28.5" spans="1:4">
+    <row r="112" ht="27" spans="1:4">
       <c r="A112" s="18"/>
       <c r="B112" s="19">
         <v>5</v>
@@ -3095,7 +3100,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="113" ht="57" spans="1:4">
+    <row r="113" ht="54" spans="1:4">
       <c r="A113" s="18"/>
       <c r="B113" s="19">
         <v>5</v>
@@ -3107,7 +3112,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="114" ht="57" spans="1:4">
+    <row r="114" ht="54" spans="1:4">
       <c r="A114" s="18"/>
       <c r="B114" s="19">
         <v>5</v>
@@ -3139,7 +3144,7 @@
       </c>
       <c r="D116" s="11"/>
     </row>
-    <row r="117" ht="57" spans="1:4">
+    <row r="117" ht="54" spans="1:4">
       <c r="A117" s="18"/>
       <c r="B117" s="19">
         <v>5</v>
@@ -3151,7 +3156,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="118" ht="69.75" spans="1:4">
+    <row r="118" ht="66.75" spans="1:4">
       <c r="A118" s="18"/>
       <c r="B118" s="19">
         <v>5</v>
@@ -3193,7 +3198,7 @@
       </c>
       <c r="D121" s="11"/>
     </row>
-    <row r="122" ht="69.75" spans="1:4">
+    <row r="122" ht="66.75" spans="1:4">
       <c r="A122" s="18"/>
       <c r="B122" s="19">
         <v>5</v>
@@ -3225,7 +3230,7 @@
       </c>
       <c r="D124" s="11"/>
     </row>
-    <row r="125" ht="27" spans="1:4">
+    <row r="125" ht="26.25" spans="1:4">
       <c r="A125" s="18"/>
       <c r="B125" s="19">
         <v>1</v>
@@ -3255,7 +3260,7 @@
       </c>
       <c r="D127" s="11"/>
     </row>
-    <row r="128" ht="27" spans="1:4">
+    <row r="128" ht="26.25" spans="1:4">
       <c r="A128" s="18"/>
       <c r="B128" s="19">
         <v>1</v>
@@ -3295,7 +3300,7 @@
       </c>
       <c r="D131" s="11"/>
     </row>
-    <row r="132" ht="27" spans="1:4">
+    <row r="132" ht="26.25" spans="1:4">
       <c r="A132" s="18"/>
       <c r="B132" s="19">
         <v>1</v>
@@ -3305,7 +3310,7 @@
       </c>
       <c r="D132" s="11"/>
     </row>
-    <row r="133" ht="69.75" spans="1:4">
+    <row r="133" ht="66.75" spans="1:4">
       <c r="A133" s="18"/>
       <c r="B133" s="19">
         <v>5</v>
@@ -3327,7 +3332,7 @@
       </c>
       <c r="D134" s="11"/>
     </row>
-    <row r="135" ht="27" spans="1:4">
+    <row r="135" ht="26.25" spans="1:4">
       <c r="A135" s="18"/>
       <c r="B135" s="19">
         <v>1</v>
@@ -3367,10 +3372,10 @@
       </c>
       <c r="D138" s="11"/>
     </row>
-    <row r="139" ht="57" spans="1:4">
+    <row r="139" ht="92.25" spans="1:4">
       <c r="A139" s="18"/>
       <c r="B139" s="19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C139" s="12" t="s">
         <v>187</v>
@@ -3379,7 +3384,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="140" ht="28.5" spans="1:4">
+    <row r="140" ht="27" spans="1:4">
       <c r="A140" s="18"/>
       <c r="B140" s="19">
         <v>5</v>
@@ -3423,7 +3428,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="144" ht="55.5" spans="1:4">
+    <row r="144" ht="53.25" spans="1:4">
       <c r="A144" s="18"/>
       <c r="B144" s="19">
         <v>5</v>
@@ -3435,7 +3440,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="145" ht="27" spans="1:4">
+    <row r="145" ht="28.5" spans="1:4">
       <c r="A145" s="18"/>
       <c r="B145" s="19">
         <v>2</v>
@@ -3445,7 +3450,7 @@
       </c>
       <c r="D145" s="11"/>
     </row>
-    <row r="146" ht="123.75" spans="1:4">
+    <row r="146" ht="119.25" spans="1:4">
       <c r="A146" s="23"/>
       <c r="B146" s="19">
         <v>5</v>
@@ -3469,7 +3474,7 @@
       </c>
       <c r="D147" s="12"/>
     </row>
-    <row r="148" ht="27" spans="1:4">
+    <row r="148" ht="26.25" spans="1:4">
       <c r="A148" s="24"/>
       <c r="B148" s="25">
         <v>1</v>
@@ -3500,7 +3505,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="151" ht="152.25" spans="1:4">
+    <row r="151" ht="146.25" spans="1:4">
       <c r="A151" s="1"/>
       <c r="B151" s="19">
         <v>5</v>
@@ -3512,7 +3517,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="152" ht="39.75" spans="1:4">
+    <row r="152" ht="39" spans="1:4">
       <c r="A152" s="1"/>
       <c r="B152" s="19">
         <v>5</v>
@@ -3535,7 +3540,7 @@
     <mergeCell ref="A147:A149"/>
     <mergeCell ref="A150:A152"/>
   </mergeCells>
-  <conditionalFormatting sqref="B:B">
+  <conditionalFormatting sqref="B$1:B$1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
add note for An overview of multi-task learning in deep neural networks
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\reading_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93393EEF-29D0-4993-A378-A3EECF9844A5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB61527-13BA-48D2-87DE-5A9253A037B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="213">
   <si>
     <t>Scope</t>
   </si>
@@ -666,9 +666,6 @@
   </si>
   <si>
     <t>joint segmentation and detection</t>
-  </si>
-  <si>
-    <t>An overview of multi-task learning in deep neural networks</t>
   </si>
   <si>
     <t>Multinet: Realtime joint semantic reasoning for autonomous driving（检测， 语意分割融合的多任务模型）</t>
@@ -701,6 +698,19 @@
   </si>
   <si>
     <t>主要是一个proposal based的object detection的survey</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multi-Task Learning Using Uncertainty to Weigh Losses for Scene Geometry and Semantics</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>why does MTL work: 1. implicit data augmentation; 2. attention focusing; 3. eavesdropping; 4. representation bias; 5. regularization
+到底如何共享backbone是需要尝试的</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>An overview of multi-task learning in deep neural networks</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -856,7 +866,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -920,23 +930,26 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1254,11 +1267,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G152"/>
+  <dimension ref="A1:G153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C147" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14"/>
@@ -1286,7 +1299,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="6">
@@ -1298,7 +1311,7 @@
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="22"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="8">
         <v>5</v>
       </c>
@@ -1308,7 +1321,7 @@
       <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="22"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="8">
         <v>5</v>
       </c>
@@ -1318,7 +1331,7 @@
       <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="22"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="8">
         <v>5</v>
       </c>
@@ -1330,7 +1343,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="22"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="8"/>
       <c r="C6" s="10" t="s">
         <v>10</v>
@@ -1338,7 +1351,7 @@
       <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" ht="28">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="25" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="8">
@@ -1350,7 +1363,7 @@
       <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" ht="28">
-      <c r="A8" s="22"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="8">
         <v>2</v>
       </c>
@@ -1360,7 +1373,7 @@
       <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" ht="28">
-      <c r="A9" s="22"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="8">
         <v>2</v>
       </c>
@@ -1370,7 +1383,7 @@
       <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" ht="56">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="24" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="8">
@@ -1384,7 +1397,7 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="22"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="11">
         <v>5</v>
       </c>
@@ -1396,7 +1409,7 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="22"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="12">
         <v>5</v>
       </c>
@@ -1406,7 +1419,7 @@
       <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" ht="28">
-      <c r="A13" s="22"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="8">
         <v>5</v>
       </c>
@@ -1418,7 +1431,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="22"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="8">
         <v>1</v>
       </c>
@@ -1428,7 +1441,7 @@
       <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" ht="28">
-      <c r="A15" s="22"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="12">
         <v>2</v>
       </c>
@@ -1438,7 +1451,7 @@
       <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" ht="28">
-      <c r="A16" s="22"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="14">
         <v>2</v>
       </c>
@@ -1448,7 +1461,7 @@
       <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" ht="70">
-      <c r="A17" s="22"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="14">
         <v>2</v>
       </c>
@@ -1458,7 +1471,7 @@
       <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" ht="28">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="25" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="14">
@@ -1470,7 +1483,7 @@
       <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" ht="37" customHeight="1">
-      <c r="A19" s="22"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="8">
         <v>5</v>
       </c>
@@ -1482,7 +1495,7 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="22"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="14">
         <v>3</v>
       </c>
@@ -1492,7 +1505,7 @@
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="22"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="12">
         <v>5</v>
       </c>
@@ -1502,7 +1515,7 @@
       <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" ht="28">
-      <c r="A22" s="22"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="12">
         <v>5</v>
       </c>
@@ -1514,7 +1527,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="28">
-      <c r="A23" s="22"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="14">
         <v>3</v>
       </c>
@@ -1524,7 +1537,7 @@
       <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" ht="28">
-      <c r="A24" s="22"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="14">
         <v>3</v>
       </c>
@@ -1534,7 +1547,7 @@
       <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" ht="28">
-      <c r="A25" s="22"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="14">
         <v>3</v>
       </c>
@@ -1544,7 +1557,7 @@
       <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4" ht="28">
-      <c r="A26" s="22"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="14">
         <v>3</v>
       </c>
@@ -1554,7 +1567,7 @@
       <c r="D26" s="9"/>
     </row>
     <row r="27" spans="1:4" ht="28">
-      <c r="A27" s="22"/>
+      <c r="A27" s="25"/>
       <c r="B27" s="14">
         <v>2</v>
       </c>
@@ -1564,7 +1577,7 @@
       <c r="D27" s="9"/>
     </row>
     <row r="28" spans="1:4" ht="28">
-      <c r="A28" s="22"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="14">
         <v>2</v>
       </c>
@@ -1574,7 +1587,7 @@
       <c r="D28" s="9"/>
     </row>
     <row r="29" spans="1:4" ht="28">
-      <c r="A29" s="22"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="14">
         <v>2</v>
       </c>
@@ -1584,7 +1597,7 @@
       <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:4" ht="112">
-      <c r="A30" s="22"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="12">
         <v>5</v>
       </c>
@@ -1596,7 +1609,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="28">
-      <c r="A31" s="22"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="12">
         <v>1</v>
       </c>
@@ -1606,7 +1619,7 @@
       <c r="D31" s="9"/>
     </row>
     <row r="32" spans="1:4" ht="42">
-      <c r="A32" s="22"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="14">
         <v>2</v>
       </c>
@@ -1616,7 +1629,7 @@
       <c r="D32" s="9"/>
     </row>
     <row r="33" spans="1:4" ht="28">
-      <c r="A33" s="22"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="12">
         <v>5</v>
       </c>
@@ -1626,7 +1639,7 @@
       <c r="D33" s="9"/>
     </row>
     <row r="34" spans="1:4" ht="28">
-      <c r="A34" s="22"/>
+      <c r="A34" s="25"/>
       <c r="B34" s="12">
         <v>5</v>
       </c>
@@ -1636,7 +1649,7 @@
       <c r="D34" s="9"/>
     </row>
     <row r="35" spans="1:4" ht="84">
-      <c r="A35" s="22"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="12">
         <v>5</v>
       </c>
@@ -1648,7 +1661,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="28">
-      <c r="A36" s="22"/>
+      <c r="A36" s="25"/>
       <c r="B36" s="12">
         <v>5</v>
       </c>
@@ -1660,7 +1673,7 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="22"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="14">
         <v>2</v>
       </c>
@@ -1670,7 +1683,7 @@
       <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="22"/>
+      <c r="A38" s="25"/>
       <c r="B38" s="14">
         <v>2</v>
       </c>
@@ -1680,7 +1693,7 @@
       <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:4" ht="56">
-      <c r="A39" s="22"/>
+      <c r="A39" s="25"/>
       <c r="B39" s="12">
         <v>5</v>
       </c>
@@ -1692,7 +1705,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="28">
-      <c r="A40" s="22"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="14">
         <v>2</v>
       </c>
@@ -1702,7 +1715,7 @@
       <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:4" ht="98">
-      <c r="A41" s="22"/>
+      <c r="A41" s="25"/>
       <c r="B41" s="12">
         <v>5</v>
       </c>
@@ -1714,7 +1727,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="28">
-      <c r="A42" s="22"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="12">
         <v>5</v>
       </c>
@@ -1726,7 +1739,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="28">
-      <c r="A43" s="22"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="12">
         <v>5</v>
       </c>
@@ -1736,7 +1749,7 @@
       <c r="D43" s="9"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="22"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="12">
         <v>5</v>
       </c>
@@ -1746,7 +1759,7 @@
       <c r="D44" s="9"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="22"/>
+      <c r="A45" s="25"/>
       <c r="B45" s="14">
         <v>2</v>
       </c>
@@ -1756,7 +1769,7 @@
       <c r="D45" s="9"/>
     </row>
     <row r="46" spans="1:4" ht="53" customHeight="1">
-      <c r="A46" s="22"/>
+      <c r="A46" s="25"/>
       <c r="B46" s="12">
         <v>5</v>
       </c>
@@ -1768,7 +1781,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="41" customHeight="1">
-      <c r="A47" s="22"/>
+      <c r="A47" s="25"/>
       <c r="B47" s="12">
         <v>5</v>
       </c>
@@ -1780,7 +1793,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="28">
-      <c r="A48" s="22" t="s">
+      <c r="A48" s="25" t="s">
         <v>68</v>
       </c>
       <c r="B48" s="12">
@@ -1792,7 +1805,7 @@
       <c r="D48" s="9"/>
     </row>
     <row r="49" spans="1:7" ht="28">
-      <c r="A49" s="22"/>
+      <c r="A49" s="25"/>
       <c r="B49" s="12">
         <v>2</v>
       </c>
@@ -1802,7 +1815,7 @@
       <c r="D49" s="9"/>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="22"/>
+      <c r="A50" s="25"/>
       <c r="B50" s="12">
         <v>2</v>
       </c>
@@ -1812,7 +1825,7 @@
       <c r="D50" s="9"/>
     </row>
     <row r="51" spans="1:7" ht="28">
-      <c r="A51" s="22"/>
+      <c r="A51" s="25"/>
       <c r="B51" s="12">
         <v>2</v>
       </c>
@@ -1822,7 +1835,7 @@
       <c r="D51" s="9"/>
     </row>
     <row r="52" spans="1:7" ht="28">
-      <c r="A52" s="22"/>
+      <c r="A52" s="25"/>
       <c r="B52" s="12">
         <v>2</v>
       </c>
@@ -1832,7 +1845,7 @@
       <c r="D52" s="9"/>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="22"/>
+      <c r="A53" s="25"/>
       <c r="B53" s="12">
         <v>5</v>
       </c>
@@ -1848,7 +1861,7 @@
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="22"/>
+      <c r="A54" s="25"/>
       <c r="B54" s="12">
         <v>2</v>
       </c>
@@ -1860,7 +1873,7 @@
       <c r="G54" s="15"/>
     </row>
     <row r="55" spans="1:7" ht="56">
-      <c r="A55" s="22"/>
+      <c r="A55" s="25"/>
       <c r="B55" s="14">
         <v>2</v>
       </c>
@@ -1876,7 +1889,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="28">
-      <c r="A56" s="22"/>
+      <c r="A56" s="25"/>
       <c r="B56" s="14">
         <v>3</v>
       </c>
@@ -1892,7 +1905,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="28">
-      <c r="A57" s="22"/>
+      <c r="A57" s="25"/>
       <c r="B57" s="14">
         <v>3</v>
       </c>
@@ -1908,7 +1921,7 @@
       </c>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="22"/>
+      <c r="A58" s="25"/>
       <c r="B58" s="14">
         <v>3</v>
       </c>
@@ -1924,7 +1937,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" ht="28">
-      <c r="A59" s="22"/>
+      <c r="A59" s="25"/>
       <c r="B59" s="14">
         <v>3</v>
       </c>
@@ -1934,7 +1947,7 @@
       <c r="D59" s="9"/>
     </row>
     <row r="60" spans="1:7" ht="28">
-      <c r="A60" s="22"/>
+      <c r="A60" s="25"/>
       <c r="B60" s="14">
         <v>3</v>
       </c>
@@ -1944,7 +1957,7 @@
       <c r="D60" s="9"/>
     </row>
     <row r="61" spans="1:7" ht="42">
-      <c r="A61" s="22"/>
+      <c r="A61" s="25"/>
       <c r="B61" s="8">
         <v>5</v>
       </c>
@@ -1956,7 +1969,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="28">
-      <c r="A62" s="22"/>
+      <c r="A62" s="25"/>
       <c r="B62" s="14">
         <v>3</v>
       </c>
@@ -1966,7 +1979,7 @@
       <c r="D62" s="9"/>
     </row>
     <row r="63" spans="1:7" ht="28">
-      <c r="A63" s="22"/>
+      <c r="A63" s="25"/>
       <c r="B63" s="14">
         <v>3</v>
       </c>
@@ -1976,7 +1989,7 @@
       <c r="D63" s="9"/>
     </row>
     <row r="64" spans="1:7" ht="84">
-      <c r="A64" s="22"/>
+      <c r="A64" s="25"/>
       <c r="B64" s="8">
         <v>5</v>
       </c>
@@ -1988,7 +2001,7 @@
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="22"/>
+      <c r="A65" s="25"/>
       <c r="B65" s="8">
         <v>2</v>
       </c>
@@ -1998,7 +2011,7 @@
       <c r="D65" s="9"/>
     </row>
     <row r="66" spans="1:4" ht="28">
-      <c r="A66" s="22"/>
+      <c r="A66" s="25"/>
       <c r="B66" s="14">
         <v>2</v>
       </c>
@@ -2008,7 +2021,7 @@
       <c r="D66" s="9"/>
     </row>
     <row r="67" spans="1:4" ht="28">
-      <c r="A67" s="22"/>
+      <c r="A67" s="25"/>
       <c r="B67" s="14">
         <v>2</v>
       </c>
@@ -2018,7 +2031,7 @@
       <c r="D67" s="9"/>
     </row>
     <row r="68" spans="1:4" ht="28">
-      <c r="A68" s="22"/>
+      <c r="A68" s="25"/>
       <c r="B68" s="14">
         <v>2</v>
       </c>
@@ -2028,7 +2041,7 @@
       <c r="D68" s="9"/>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="22"/>
+      <c r="A69" s="25"/>
       <c r="B69" s="14">
         <v>2</v>
       </c>
@@ -2038,7 +2051,7 @@
       <c r="D69" s="9"/>
     </row>
     <row r="70" spans="1:4" ht="28">
-      <c r="A70" s="22"/>
+      <c r="A70" s="25"/>
       <c r="B70" s="14">
         <v>2</v>
       </c>
@@ -2048,7 +2061,7 @@
       <c r="D70" s="9"/>
     </row>
     <row r="71" spans="1:4" ht="28">
-      <c r="A71" s="22"/>
+      <c r="A71" s="25"/>
       <c r="B71" s="14">
         <v>2</v>
       </c>
@@ -2058,7 +2071,7 @@
       <c r="D71" s="9"/>
     </row>
     <row r="72" spans="1:4" ht="28">
-      <c r="A72" s="22"/>
+      <c r="A72" s="25"/>
       <c r="B72" s="14">
         <v>2</v>
       </c>
@@ -2068,7 +2081,7 @@
       <c r="D72" s="9"/>
     </row>
     <row r="73" spans="1:4" ht="28">
-      <c r="A73" s="22"/>
+      <c r="A73" s="25"/>
       <c r="B73" s="14">
         <v>2</v>
       </c>
@@ -2078,7 +2091,7 @@
       <c r="D73" s="9"/>
     </row>
     <row r="74" spans="1:4" ht="28">
-      <c r="A74" s="22"/>
+      <c r="A74" s="25"/>
       <c r="B74" s="14">
         <v>2</v>
       </c>
@@ -2088,7 +2101,7 @@
       <c r="D74" s="9"/>
     </row>
     <row r="75" spans="1:4" ht="28">
-      <c r="A75" s="22"/>
+      <c r="A75" s="25"/>
       <c r="B75" s="16">
         <v>5</v>
       </c>
@@ -2096,11 +2109,11 @@
         <v>103</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="42">
-      <c r="A76" s="22"/>
+      <c r="A76" s="25"/>
       <c r="B76" s="8">
         <v>5</v>
       </c>
@@ -2112,7 +2125,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="28">
-      <c r="A77" s="22"/>
+      <c r="A77" s="25"/>
       <c r="B77" s="14">
         <v>2</v>
       </c>
@@ -2122,7 +2135,7 @@
       <c r="D77" s="9"/>
     </row>
     <row r="78" spans="1:4" ht="28">
-      <c r="A78" s="22"/>
+      <c r="A78" s="25"/>
       <c r="B78" s="8">
         <v>2</v>
       </c>
@@ -2132,7 +2145,7 @@
       <c r="D78" s="9"/>
     </row>
     <row r="79" spans="1:4" ht="28">
-      <c r="A79" s="22"/>
+      <c r="A79" s="25"/>
       <c r="B79" s="8">
         <v>2</v>
       </c>
@@ -2142,7 +2155,7 @@
       <c r="D79" s="9"/>
     </row>
     <row r="80" spans="1:4" ht="42">
-      <c r="A80" s="22"/>
+      <c r="A80" s="25"/>
       <c r="B80" s="8">
         <v>1</v>
       </c>
@@ -2152,7 +2165,7 @@
       <c r="D80" s="9"/>
     </row>
     <row r="81" spans="1:4" ht="28">
-      <c r="A81" s="22"/>
+      <c r="A81" s="25"/>
       <c r="B81" s="8">
         <v>1</v>
       </c>
@@ -2162,7 +2175,7 @@
       <c r="D81" s="9"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="22"/>
+      <c r="A82" s="25"/>
       <c r="B82" s="8">
         <v>1</v>
       </c>
@@ -2172,7 +2185,7 @@
       <c r="D82" s="9"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="22"/>
+      <c r="A83" s="25"/>
       <c r="B83" s="14">
         <v>1</v>
       </c>
@@ -2182,7 +2195,7 @@
       <c r="D83" s="9"/>
     </row>
     <row r="84" spans="1:4" ht="28">
-      <c r="A84" s="22"/>
+      <c r="A84" s="25"/>
       <c r="B84" s="14">
         <v>1</v>
       </c>
@@ -2192,7 +2205,7 @@
       <c r="D84" s="9"/>
     </row>
     <row r="85" spans="1:4" ht="28">
-      <c r="A85" s="22"/>
+      <c r="A85" s="25"/>
       <c r="B85" s="14">
         <v>1</v>
       </c>
@@ -2202,7 +2215,7 @@
       <c r="D85" s="9"/>
     </row>
     <row r="86" spans="1:4" ht="28">
-      <c r="A86" s="22"/>
+      <c r="A86" s="25"/>
       <c r="B86" s="14">
         <v>1</v>
       </c>
@@ -2212,7 +2225,7 @@
       <c r="D86" s="9"/>
     </row>
     <row r="87" spans="1:4" ht="28">
-      <c r="A87" s="22"/>
+      <c r="A87" s="25"/>
       <c r="B87" s="14">
         <v>1</v>
       </c>
@@ -2222,7 +2235,7 @@
       <c r="D87" s="9"/>
     </row>
     <row r="88" spans="1:4" ht="28">
-      <c r="A88" s="22"/>
+      <c r="A88" s="25"/>
       <c r="B88" s="14">
         <v>1</v>
       </c>
@@ -2232,7 +2245,7 @@
       <c r="D88" s="9"/>
     </row>
     <row r="89" spans="1:4" ht="28">
-      <c r="A89" s="23" t="s">
+      <c r="A89" s="21" t="s">
         <v>118</v>
       </c>
       <c r="B89" s="14">
@@ -2244,7 +2257,7 @@
       <c r="D89" s="9"/>
     </row>
     <row r="90" spans="1:4" ht="42">
-      <c r="A90" s="23"/>
+      <c r="A90" s="21"/>
       <c r="B90" s="8">
         <v>5</v>
       </c>
@@ -2254,7 +2267,7 @@
       <c r="D90" s="9"/>
     </row>
     <row r="91" spans="1:4" ht="70">
-      <c r="A91" s="23"/>
+      <c r="A91" s="21"/>
       <c r="B91" s="8">
         <v>6</v>
       </c>
@@ -2266,7 +2279,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="28">
-      <c r="A92" s="23"/>
+      <c r="A92" s="21"/>
       <c r="B92" s="16">
         <v>5</v>
       </c>
@@ -2278,7 +2291,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" ht="28">
-      <c r="A93" s="23"/>
+      <c r="A93" s="21"/>
       <c r="B93" s="16">
         <v>5</v>
       </c>
@@ -2290,7 +2303,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="28">
-      <c r="A94" s="23"/>
+      <c r="A94" s="21"/>
       <c r="B94" s="16">
         <v>1</v>
       </c>
@@ -2300,7 +2313,7 @@
       <c r="D94" s="9"/>
     </row>
     <row r="95" spans="1:4" ht="112">
-      <c r="A95" s="23"/>
+      <c r="A95" s="21"/>
       <c r="B95" s="16">
         <v>5</v>
       </c>
@@ -2312,7 +2325,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" ht="112">
-      <c r="A96" s="23"/>
+      <c r="A96" s="21"/>
       <c r="B96" s="16">
         <v>5</v>
       </c>
@@ -2324,7 +2337,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="70">
-      <c r="A97" s="23"/>
+      <c r="A97" s="21"/>
       <c r="B97" s="16">
         <v>5</v>
       </c>
@@ -2336,7 +2349,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="112">
-      <c r="A98" s="23"/>
+      <c r="A98" s="21"/>
       <c r="B98" s="16">
         <v>5</v>
       </c>
@@ -2348,7 +2361,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="28">
-      <c r="A99" s="23"/>
+      <c r="A99" s="21"/>
       <c r="B99" s="16">
         <v>5</v>
       </c>
@@ -2358,7 +2371,7 @@
       <c r="D99" s="9"/>
     </row>
     <row r="100" spans="1:4" ht="56">
-      <c r="A100" s="23"/>
+      <c r="A100" s="21"/>
       <c r="B100" s="16">
         <v>5</v>
       </c>
@@ -2368,7 +2381,7 @@
       <c r="D100" s="9"/>
     </row>
     <row r="101" spans="1:4" ht="42">
-      <c r="A101" s="23"/>
+      <c r="A101" s="21"/>
       <c r="B101" s="16">
         <v>5</v>
       </c>
@@ -2380,7 +2393,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="28">
-      <c r="A102" s="23"/>
+      <c r="A102" s="21"/>
       <c r="B102" s="16">
         <v>2</v>
       </c>
@@ -2390,7 +2403,7 @@
       <c r="D102" s="9"/>
     </row>
     <row r="103" spans="1:4" ht="42">
-      <c r="A103" s="23"/>
+      <c r="A103" s="21"/>
       <c r="B103" s="16">
         <v>2</v>
       </c>
@@ -2400,7 +2413,7 @@
       <c r="D103" s="9"/>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="23"/>
+      <c r="A104" s="21"/>
       <c r="B104" s="16">
         <v>1</v>
       </c>
@@ -2410,7 +2423,7 @@
       <c r="D104" s="9"/>
     </row>
     <row r="105" spans="1:4" ht="28">
-      <c r="A105" s="23"/>
+      <c r="A105" s="21"/>
       <c r="B105" s="16">
         <v>2</v>
       </c>
@@ -2420,7 +2433,7 @@
       <c r="D105" s="9"/>
     </row>
     <row r="106" spans="1:4" ht="42">
-      <c r="A106" s="23"/>
+      <c r="A106" s="21"/>
       <c r="B106" s="16">
         <v>2</v>
       </c>
@@ -2430,7 +2443,7 @@
       <c r="D106" s="9"/>
     </row>
     <row r="107" spans="1:4">
-      <c r="A107" s="23"/>
+      <c r="A107" s="21"/>
       <c r="B107" s="16">
         <v>2</v>
       </c>
@@ -2440,7 +2453,7 @@
       <c r="D107" s="9"/>
     </row>
     <row r="108" spans="1:4" ht="28">
-      <c r="A108" s="23"/>
+      <c r="A108" s="21"/>
       <c r="B108" s="16">
         <v>2</v>
       </c>
@@ -2450,7 +2463,7 @@
       <c r="D108" s="9"/>
     </row>
     <row r="109" spans="1:4" ht="42">
-      <c r="A109" s="23"/>
+      <c r="A109" s="21"/>
       <c r="B109" s="16">
         <v>5</v>
       </c>
@@ -2462,7 +2475,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" ht="56">
-      <c r="A110" s="23"/>
+      <c r="A110" s="21"/>
       <c r="B110" s="16">
         <v>5</v>
       </c>
@@ -2474,7 +2487,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="210">
-      <c r="A111" s="23"/>
+      <c r="A111" s="21"/>
       <c r="B111" s="16">
         <v>5</v>
       </c>
@@ -2486,7 +2499,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="42">
-      <c r="A112" s="23"/>
+      <c r="A112" s="21"/>
       <c r="B112" s="16">
         <v>5</v>
       </c>
@@ -2498,7 +2511,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="56">
-      <c r="A113" s="23"/>
+      <c r="A113" s="21"/>
       <c r="B113" s="16">
         <v>5</v>
       </c>
@@ -2510,7 +2523,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" ht="56">
-      <c r="A114" s="23"/>
+      <c r="A114" s="21"/>
       <c r="B114" s="16">
         <v>5</v>
       </c>
@@ -2522,7 +2535,7 @@
       </c>
     </row>
     <row r="115" spans="1:4">
-      <c r="A115" s="23"/>
+      <c r="A115" s="21"/>
       <c r="B115" s="16">
         <v>2</v>
       </c>
@@ -2532,7 +2545,7 @@
       <c r="D115" s="9"/>
     </row>
     <row r="116" spans="1:4" ht="28">
-      <c r="A116" s="23"/>
+      <c r="A116" s="21"/>
       <c r="B116" s="16">
         <v>2</v>
       </c>
@@ -2542,7 +2555,7 @@
       <c r="D116" s="9"/>
     </row>
     <row r="117" spans="1:4" ht="70">
-      <c r="A117" s="23"/>
+      <c r="A117" s="21"/>
       <c r="B117" s="16">
         <v>5</v>
       </c>
@@ -2554,7 +2567,7 @@
       </c>
     </row>
     <row r="118" spans="1:4" ht="70">
-      <c r="A118" s="23"/>
+      <c r="A118" s="21"/>
       <c r="B118" s="16">
         <v>5</v>
       </c>
@@ -2566,7 +2579,7 @@
       </c>
     </row>
     <row r="119" spans="1:4" ht="28">
-      <c r="A119" s="23"/>
+      <c r="A119" s="21"/>
       <c r="B119" s="16">
         <v>1</v>
       </c>
@@ -2576,7 +2589,7 @@
       <c r="D119" s="9"/>
     </row>
     <row r="120" spans="1:4" ht="28">
-      <c r="A120" s="23"/>
+      <c r="A120" s="21"/>
       <c r="B120" s="16">
         <v>1</v>
       </c>
@@ -2586,7 +2599,7 @@
       <c r="D120" s="9"/>
     </row>
     <row r="121" spans="1:4" ht="28">
-      <c r="A121" s="23"/>
+      <c r="A121" s="21"/>
       <c r="B121" s="16">
         <v>1</v>
       </c>
@@ -2596,7 +2609,7 @@
       <c r="D121" s="9"/>
     </row>
     <row r="122" spans="1:4" ht="98">
-      <c r="A122" s="23"/>
+      <c r="A122" s="21"/>
       <c r="B122" s="16">
         <v>5</v>
       </c>
@@ -2608,7 +2621,7 @@
       </c>
     </row>
     <row r="123" spans="1:4" ht="42">
-      <c r="A123" s="23"/>
+      <c r="A123" s="21"/>
       <c r="B123" s="16">
         <v>1</v>
       </c>
@@ -2618,7 +2631,7 @@
       <c r="D123" s="9"/>
     </row>
     <row r="124" spans="1:4" ht="42">
-      <c r="A124" s="23"/>
+      <c r="A124" s="21"/>
       <c r="B124" s="16">
         <v>1</v>
       </c>
@@ -2628,7 +2641,7 @@
       <c r="D124" s="9"/>
     </row>
     <row r="125" spans="1:4" ht="42">
-      <c r="A125" s="23"/>
+      <c r="A125" s="21"/>
       <c r="B125" s="16">
         <v>1</v>
       </c>
@@ -2638,7 +2651,7 @@
       <c r="D125" s="9"/>
     </row>
     <row r="126" spans="1:4" ht="42">
-      <c r="A126" s="23"/>
+      <c r="A126" s="21"/>
       <c r="B126" s="16">
         <v>1</v>
       </c>
@@ -2648,7 +2661,7 @@
       <c r="D126" s="9"/>
     </row>
     <row r="127" spans="1:4" ht="28">
-      <c r="A127" s="23"/>
+      <c r="A127" s="21"/>
       <c r="B127" s="16">
         <v>1</v>
       </c>
@@ -2658,7 +2671,7 @@
       <c r="D127" s="9"/>
     </row>
     <row r="128" spans="1:4" ht="42">
-      <c r="A128" s="23"/>
+      <c r="A128" s="21"/>
       <c r="B128" s="16">
         <v>1</v>
       </c>
@@ -2668,7 +2681,7 @@
       <c r="D128" s="9"/>
     </row>
     <row r="129" spans="1:4" ht="28">
-      <c r="A129" s="23"/>
+      <c r="A129" s="21"/>
       <c r="B129" s="17">
         <v>1</v>
       </c>
@@ -2678,7 +2691,7 @@
       <c r="D129" s="9"/>
     </row>
     <row r="130" spans="1:4" ht="28">
-      <c r="A130" s="23"/>
+      <c r="A130" s="21"/>
       <c r="B130" s="16">
         <v>1</v>
       </c>
@@ -2688,7 +2701,7 @@
       <c r="D130" s="9"/>
     </row>
     <row r="131" spans="1:4" ht="28">
-      <c r="A131" s="23"/>
+      <c r="A131" s="21"/>
       <c r="B131" s="16">
         <v>1</v>
       </c>
@@ -2698,7 +2711,7 @@
       <c r="D131" s="9"/>
     </row>
     <row r="132" spans="1:4" ht="28">
-      <c r="A132" s="23"/>
+      <c r="A132" s="21"/>
       <c r="B132" s="16">
         <v>1</v>
       </c>
@@ -2708,7 +2721,7 @@
       <c r="D132" s="9"/>
     </row>
     <row r="133" spans="1:4" ht="70">
-      <c r="A133" s="23"/>
+      <c r="A133" s="21"/>
       <c r="B133" s="16">
         <v>5</v>
       </c>
@@ -2720,7 +2733,7 @@
       </c>
     </row>
     <row r="134" spans="1:4" ht="28">
-      <c r="A134" s="23"/>
+      <c r="A134" s="21"/>
       <c r="B134" s="16">
         <v>1</v>
       </c>
@@ -2730,7 +2743,7 @@
       <c r="D134" s="9"/>
     </row>
     <row r="135" spans="1:4" ht="28">
-      <c r="A135" s="23"/>
+      <c r="A135" s="21"/>
       <c r="B135" s="16">
         <v>1</v>
       </c>
@@ -2740,7 +2753,7 @@
       <c r="D135" s="9"/>
     </row>
     <row r="136" spans="1:4" ht="28">
-      <c r="A136" s="23"/>
+      <c r="A136" s="21"/>
       <c r="B136" s="16">
         <v>1</v>
       </c>
@@ -2750,7 +2763,7 @@
       <c r="D136" s="9"/>
     </row>
     <row r="137" spans="1:4">
-      <c r="A137" s="23"/>
+      <c r="A137" s="21"/>
       <c r="B137" s="16">
         <v>1</v>
       </c>
@@ -2760,7 +2773,7 @@
       <c r="D137" s="9"/>
     </row>
     <row r="138" spans="1:4" ht="42">
-      <c r="A138" s="23"/>
+      <c r="A138" s="21"/>
       <c r="B138" s="16">
         <v>5</v>
       </c>
@@ -2770,7 +2783,7 @@
       <c r="D138" s="9"/>
     </row>
     <row r="139" spans="1:4" ht="126">
-      <c r="A139" s="23"/>
+      <c r="A139" s="21"/>
       <c r="B139" s="16">
         <v>5</v>
       </c>
@@ -2782,7 +2795,7 @@
       </c>
     </row>
     <row r="140" spans="1:4" ht="42">
-      <c r="A140" s="23"/>
+      <c r="A140" s="21"/>
       <c r="B140" s="16">
         <v>5</v>
       </c>
@@ -2794,7 +2807,7 @@
       </c>
     </row>
     <row r="141" spans="1:4" ht="26">
-      <c r="A141" s="23"/>
+      <c r="A141" s="21"/>
       <c r="B141" s="16">
         <v>1</v>
       </c>
@@ -2804,7 +2817,7 @@
       <c r="D141" s="9"/>
     </row>
     <row r="142" spans="1:4" ht="28">
-      <c r="A142" s="23"/>
+      <c r="A142" s="21"/>
       <c r="B142" s="16">
         <v>1</v>
       </c>
@@ -2814,7 +2827,7 @@
       <c r="D142" s="9"/>
     </row>
     <row r="143" spans="1:4" ht="42">
-      <c r="A143" s="23"/>
+      <c r="A143" s="21"/>
       <c r="B143" s="16">
         <v>5</v>
       </c>
@@ -2826,7 +2839,7 @@
       </c>
     </row>
     <row r="144" spans="1:4" ht="70">
-      <c r="A144" s="23"/>
+      <c r="A144" s="21"/>
       <c r="B144" s="16">
         <v>5</v>
       </c>
@@ -2838,7 +2851,7 @@
       </c>
     </row>
     <row r="145" spans="1:4" ht="49.5">
-      <c r="A145" s="23"/>
+      <c r="A145" s="21"/>
       <c r="B145" s="16">
         <v>2</v>
       </c>
@@ -2848,7 +2861,7 @@
       <c r="D145" s="9"/>
     </row>
     <row r="146" spans="1:4" ht="154">
-      <c r="A146" s="24"/>
+      <c r="A146" s="22"/>
       <c r="B146" s="16">
         <v>5</v>
       </c>
@@ -2859,78 +2872,88 @@
         <v>199</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="28">
-      <c r="A147" s="25" t="s">
+    <row r="147" spans="1:4" ht="56">
+      <c r="A147" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="B147" s="20">
-        <v>1</v>
-      </c>
-      <c r="C147" s="10" t="s">
+      <c r="B147" s="26">
+        <v>1</v>
+      </c>
+      <c r="C147" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="D147" s="27"/>
+    </row>
+    <row r="148" spans="1:4" ht="42" customHeight="1">
+      <c r="B148" s="16">
+        <v>5</v>
+      </c>
+      <c r="C148" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D148" s="10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="42">
+      <c r="A149" s="10"/>
+      <c r="B149" s="20">
+        <v>1</v>
+      </c>
+      <c r="C149" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="D147" s="10"/>
-    </row>
-    <row r="148" spans="1:4" ht="42">
-      <c r="A148" s="25"/>
-      <c r="B148" s="20">
-        <v>1</v>
-      </c>
-      <c r="C148" s="10" t="s">
+      <c r="D149" s="10"/>
+    </row>
+    <row r="150" spans="1:4" ht="28">
+      <c r="A150" s="10"/>
+      <c r="B150" s="20">
+        <v>1</v>
+      </c>
+      <c r="C150" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="D148" s="10"/>
-    </row>
-    <row r="149" spans="1:4" ht="28">
-      <c r="A149" s="25"/>
-      <c r="B149" s="20">
-        <v>1</v>
-      </c>
-      <c r="C149" s="10" t="s">
+      <c r="D150" s="10"/>
+    </row>
+    <row r="151" spans="1:4" ht="42">
+      <c r="A151" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="D149" s="10"/>
-    </row>
-    <row r="150" spans="1:4" ht="42">
-      <c r="A150" s="26" t="s">
+      <c r="B151" s="1">
+        <v>1</v>
+      </c>
+      <c r="C151" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B150" s="1">
-        <v>1</v>
-      </c>
-      <c r="C150" s="2" t="s">
+    </row>
+    <row r="152" spans="1:4" ht="182">
+      <c r="A152" s="23"/>
+      <c r="B152" s="16">
+        <v>5</v>
+      </c>
+      <c r="C152" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" ht="182">
-      <c r="A151" s="26"/>
-      <c r="B151" s="16">
-        <v>5</v>
-      </c>
-      <c r="C151" s="2" t="s">
+      <c r="D152" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="D151" s="2" t="s">
+    </row>
+    <row r="153" spans="1:4" ht="56">
+      <c r="A153" s="23"/>
+      <c r="B153" s="16">
+        <v>5</v>
+      </c>
+      <c r="C153" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" ht="56">
-      <c r="A152" s="26"/>
-      <c r="B152" s="16">
-        <v>5</v>
-      </c>
-      <c r="C152" s="2" t="s">
+      <c r="D153" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D152" s="2" t="s">
-        <v>209</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="A89:A146"/>
-    <mergeCell ref="A147:A149"/>
-    <mergeCell ref="A150:A152"/>
+    <mergeCell ref="A151:A153"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A17"/>

</xml_diff>

<commit_message>
add note for Semantic Instance Segmentation with a Discriminative Loss Function
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\reading_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB61527-13BA-48D2-87DE-5A9253A037B8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECC186A-895F-4E4E-B792-C87F1FF17374}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="214">
   <si>
     <t>Scope</t>
   </si>
@@ -556,9 +556,6 @@
   </si>
   <si>
     <t>Semantic Instance Segmentation via Deep Metric Learning</t>
-  </si>
-  <si>
-    <t>Semantic Instance Segmentation with a Discriminative Loss Function</t>
   </si>
   <si>
     <t>Towards End-to-End Lane Detection: an Instance Segmentation Approach</t>
@@ -711,6 +708,17 @@
   </si>
   <si>
     <t>An overview of multi-task learning in deep neural networks</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>提出了一种proprosal free的instance segmentation的方法：网络输出每个像素的embedding， 在embedding的空间进行聚类。
+Embedding的训练用的loss有3项：variance term: 同一类在embedding空间靠近；distance term：不同类的均值的中心在embedded空间远离；regularization term: 各个聚类中心靠近原点；这个loss也可以用于classification和semantic segmentation
+优点：对复杂遮挡比较有效
+缺点：需要训练集和测试机的图片比较一致（due to the holistic treatment of the image), 对前序的semantic mask的要求比较高，mask不准的话，instance也不准</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Semantic Instance Segmentation with a Discriminative Loss Function</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -930,6 +938,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -944,12 +958,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1269,9 +1277,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C147" sqref="C147"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14"/>
@@ -1299,7 +1307,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="26" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="6">
@@ -1311,7 +1319,7 @@
       <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="25"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="8">
         <v>5</v>
       </c>
@@ -1321,7 +1329,7 @@
       <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="25"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="8">
         <v>5</v>
       </c>
@@ -1331,7 +1339,7 @@
       <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="25"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="8">
         <v>5</v>
       </c>
@@ -1343,7 +1351,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="25"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="8"/>
       <c r="C6" s="10" t="s">
         <v>10</v>
@@ -1351,7 +1359,7 @@
       <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" ht="28">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="27" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="8">
@@ -1363,7 +1371,7 @@
       <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" ht="28">
-      <c r="A8" s="25"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="8">
         <v>2</v>
       </c>
@@ -1373,7 +1381,7 @@
       <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" ht="28">
-      <c r="A9" s="25"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="8">
         <v>2</v>
       </c>
@@ -1383,7 +1391,7 @@
       <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" ht="56">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="8">
@@ -1397,7 +1405,7 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="25"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="11">
         <v>5</v>
       </c>
@@ -1409,7 +1417,7 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="25"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="12">
         <v>5</v>
       </c>
@@ -1419,7 +1427,7 @@
       <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" ht="28">
-      <c r="A13" s="25"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="8">
         <v>5</v>
       </c>
@@ -1431,7 +1439,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="25"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="8">
         <v>1</v>
       </c>
@@ -1441,7 +1449,7 @@
       <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" ht="28">
-      <c r="A15" s="25"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="12">
         <v>2</v>
       </c>
@@ -1451,7 +1459,7 @@
       <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" ht="28">
-      <c r="A16" s="25"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="14">
         <v>2</v>
       </c>
@@ -1461,7 +1469,7 @@
       <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" ht="70">
-      <c r="A17" s="25"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="14">
         <v>2</v>
       </c>
@@ -1471,7 +1479,7 @@
       <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" ht="28">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="27" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="14">
@@ -1483,7 +1491,7 @@
       <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" ht="37" customHeight="1">
-      <c r="A19" s="25"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="8">
         <v>5</v>
       </c>
@@ -1495,7 +1503,7 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="25"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="14">
         <v>3</v>
       </c>
@@ -1505,7 +1513,7 @@
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="25"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="12">
         <v>5</v>
       </c>
@@ -1515,7 +1523,7 @@
       <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" ht="28">
-      <c r="A22" s="25"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="12">
         <v>5</v>
       </c>
@@ -1527,7 +1535,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="28">
-      <c r="A23" s="25"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="14">
         <v>3</v>
       </c>
@@ -1537,7 +1545,7 @@
       <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" ht="28">
-      <c r="A24" s="25"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="14">
         <v>3</v>
       </c>
@@ -1547,7 +1555,7 @@
       <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" ht="28">
-      <c r="A25" s="25"/>
+      <c r="A25" s="27"/>
       <c r="B25" s="14">
         <v>3</v>
       </c>
@@ -1557,7 +1565,7 @@
       <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4" ht="28">
-      <c r="A26" s="25"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="14">
         <v>3</v>
       </c>
@@ -1567,7 +1575,7 @@
       <c r="D26" s="9"/>
     </row>
     <row r="27" spans="1:4" ht="28">
-      <c r="A27" s="25"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="14">
         <v>2</v>
       </c>
@@ -1577,7 +1585,7 @@
       <c r="D27" s="9"/>
     </row>
     <row r="28" spans="1:4" ht="28">
-      <c r="A28" s="25"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="14">
         <v>2</v>
       </c>
@@ -1587,7 +1595,7 @@
       <c r="D28" s="9"/>
     </row>
     <row r="29" spans="1:4" ht="28">
-      <c r="A29" s="25"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="14">
         <v>2</v>
       </c>
@@ -1597,7 +1605,7 @@
       <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:4" ht="112">
-      <c r="A30" s="25"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="12">
         <v>5</v>
       </c>
@@ -1609,7 +1617,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="28">
-      <c r="A31" s="25"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="12">
         <v>1</v>
       </c>
@@ -1619,7 +1627,7 @@
       <c r="D31" s="9"/>
     </row>
     <row r="32" spans="1:4" ht="42">
-      <c r="A32" s="25"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="14">
         <v>2</v>
       </c>
@@ -1629,7 +1637,7 @@
       <c r="D32" s="9"/>
     </row>
     <row r="33" spans="1:4" ht="28">
-      <c r="A33" s="25"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="12">
         <v>5</v>
       </c>
@@ -1639,7 +1647,7 @@
       <c r="D33" s="9"/>
     </row>
     <row r="34" spans="1:4" ht="28">
-      <c r="A34" s="25"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="12">
         <v>5</v>
       </c>
@@ -1649,7 +1657,7 @@
       <c r="D34" s="9"/>
     </row>
     <row r="35" spans="1:4" ht="84">
-      <c r="A35" s="25"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="12">
         <v>5</v>
       </c>
@@ -1661,7 +1669,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="28">
-      <c r="A36" s="25"/>
+      <c r="A36" s="27"/>
       <c r="B36" s="12">
         <v>5</v>
       </c>
@@ -1673,7 +1681,7 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="25"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="14">
         <v>2</v>
       </c>
@@ -1683,7 +1691,7 @@
       <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="25"/>
+      <c r="A38" s="27"/>
       <c r="B38" s="14">
         <v>2</v>
       </c>
@@ -1693,7 +1701,7 @@
       <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:4" ht="56">
-      <c r="A39" s="25"/>
+      <c r="A39" s="27"/>
       <c r="B39" s="12">
         <v>5</v>
       </c>
@@ -1705,7 +1713,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="28">
-      <c r="A40" s="25"/>
+      <c r="A40" s="27"/>
       <c r="B40" s="14">
         <v>2</v>
       </c>
@@ -1715,7 +1723,7 @@
       <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:4" ht="98">
-      <c r="A41" s="25"/>
+      <c r="A41" s="27"/>
       <c r="B41" s="12">
         <v>5</v>
       </c>
@@ -1727,7 +1735,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="28">
-      <c r="A42" s="25"/>
+      <c r="A42" s="27"/>
       <c r="B42" s="12">
         <v>5</v>
       </c>
@@ -1739,7 +1747,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="28">
-      <c r="A43" s="25"/>
+      <c r="A43" s="27"/>
       <c r="B43" s="12">
         <v>5</v>
       </c>
@@ -1749,7 +1757,7 @@
       <c r="D43" s="9"/>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="25"/>
+      <c r="A44" s="27"/>
       <c r="B44" s="12">
         <v>5</v>
       </c>
@@ -1759,7 +1767,7 @@
       <c r="D44" s="9"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="25"/>
+      <c r="A45" s="27"/>
       <c r="B45" s="14">
         <v>2</v>
       </c>
@@ -1769,7 +1777,7 @@
       <c r="D45" s="9"/>
     </row>
     <row r="46" spans="1:4" ht="53" customHeight="1">
-      <c r="A46" s="25"/>
+      <c r="A46" s="27"/>
       <c r="B46" s="12">
         <v>5</v>
       </c>
@@ -1781,7 +1789,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="41" customHeight="1">
-      <c r="A47" s="25"/>
+      <c r="A47" s="27"/>
       <c r="B47" s="12">
         <v>5</v>
       </c>
@@ -1793,7 +1801,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="28">
-      <c r="A48" s="25" t="s">
+      <c r="A48" s="27" t="s">
         <v>68</v>
       </c>
       <c r="B48" s="12">
@@ -1805,7 +1813,7 @@
       <c r="D48" s="9"/>
     </row>
     <row r="49" spans="1:7" ht="28">
-      <c r="A49" s="25"/>
+      <c r="A49" s="27"/>
       <c r="B49" s="12">
         <v>2</v>
       </c>
@@ -1815,7 +1823,7 @@
       <c r="D49" s="9"/>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="25"/>
+      <c r="A50" s="27"/>
       <c r="B50" s="12">
         <v>2</v>
       </c>
@@ -1825,7 +1833,7 @@
       <c r="D50" s="9"/>
     </row>
     <row r="51" spans="1:7" ht="28">
-      <c r="A51" s="25"/>
+      <c r="A51" s="27"/>
       <c r="B51" s="12">
         <v>2</v>
       </c>
@@ -1835,7 +1843,7 @@
       <c r="D51" s="9"/>
     </row>
     <row r="52" spans="1:7" ht="28">
-      <c r="A52" s="25"/>
+      <c r="A52" s="27"/>
       <c r="B52" s="12">
         <v>2</v>
       </c>
@@ -1845,7 +1853,7 @@
       <c r="D52" s="9"/>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="25"/>
+      <c r="A53" s="27"/>
       <c r="B53" s="12">
         <v>5</v>
       </c>
@@ -1861,7 +1869,7 @@
       </c>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="25"/>
+      <c r="A54" s="27"/>
       <c r="B54" s="12">
         <v>2</v>
       </c>
@@ -1873,7 +1881,7 @@
       <c r="G54" s="15"/>
     </row>
     <row r="55" spans="1:7" ht="56">
-      <c r="A55" s="25"/>
+      <c r="A55" s="27"/>
       <c r="B55" s="14">
         <v>2</v>
       </c>
@@ -1889,7 +1897,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="28">
-      <c r="A56" s="25"/>
+      <c r="A56" s="27"/>
       <c r="B56" s="14">
         <v>3</v>
       </c>
@@ -1905,7 +1913,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="28">
-      <c r="A57" s="25"/>
+      <c r="A57" s="27"/>
       <c r="B57" s="14">
         <v>3</v>
       </c>
@@ -1921,7 +1929,7 @@
       </c>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="25"/>
+      <c r="A58" s="27"/>
       <c r="B58" s="14">
         <v>3</v>
       </c>
@@ -1937,7 +1945,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" ht="28">
-      <c r="A59" s="25"/>
+      <c r="A59" s="27"/>
       <c r="B59" s="14">
         <v>3</v>
       </c>
@@ -1947,7 +1955,7 @@
       <c r="D59" s="9"/>
     </row>
     <row r="60" spans="1:7" ht="28">
-      <c r="A60" s="25"/>
+      <c r="A60" s="27"/>
       <c r="B60" s="14">
         <v>3</v>
       </c>
@@ -1957,7 +1965,7 @@
       <c r="D60" s="9"/>
     </row>
     <row r="61" spans="1:7" ht="42">
-      <c r="A61" s="25"/>
+      <c r="A61" s="27"/>
       <c r="B61" s="8">
         <v>5</v>
       </c>
@@ -1969,7 +1977,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="28">
-      <c r="A62" s="25"/>
+      <c r="A62" s="27"/>
       <c r="B62" s="14">
         <v>3</v>
       </c>
@@ -1979,7 +1987,7 @@
       <c r="D62" s="9"/>
     </row>
     <row r="63" spans="1:7" ht="28">
-      <c r="A63" s="25"/>
+      <c r="A63" s="27"/>
       <c r="B63" s="14">
         <v>3</v>
       </c>
@@ -1989,7 +1997,7 @@
       <c r="D63" s="9"/>
     </row>
     <row r="64" spans="1:7" ht="84">
-      <c r="A64" s="25"/>
+      <c r="A64" s="27"/>
       <c r="B64" s="8">
         <v>5</v>
       </c>
@@ -2001,7 +2009,7 @@
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="25"/>
+      <c r="A65" s="27"/>
       <c r="B65" s="8">
         <v>2</v>
       </c>
@@ -2011,7 +2019,7 @@
       <c r="D65" s="9"/>
     </row>
     <row r="66" spans="1:4" ht="28">
-      <c r="A66" s="25"/>
+      <c r="A66" s="27"/>
       <c r="B66" s="14">
         <v>2</v>
       </c>
@@ -2021,7 +2029,7 @@
       <c r="D66" s="9"/>
     </row>
     <row r="67" spans="1:4" ht="28">
-      <c r="A67" s="25"/>
+      <c r="A67" s="27"/>
       <c r="B67" s="14">
         <v>2</v>
       </c>
@@ -2031,7 +2039,7 @@
       <c r="D67" s="9"/>
     </row>
     <row r="68" spans="1:4" ht="28">
-      <c r="A68" s="25"/>
+      <c r="A68" s="27"/>
       <c r="B68" s="14">
         <v>2</v>
       </c>
@@ -2041,7 +2049,7 @@
       <c r="D68" s="9"/>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="25"/>
+      <c r="A69" s="27"/>
       <c r="B69" s="14">
         <v>2</v>
       </c>
@@ -2051,7 +2059,7 @@
       <c r="D69" s="9"/>
     </row>
     <row r="70" spans="1:4" ht="28">
-      <c r="A70" s="25"/>
+      <c r="A70" s="27"/>
       <c r="B70" s="14">
         <v>2</v>
       </c>
@@ -2061,7 +2069,7 @@
       <c r="D70" s="9"/>
     </row>
     <row r="71" spans="1:4" ht="28">
-      <c r="A71" s="25"/>
+      <c r="A71" s="27"/>
       <c r="B71" s="14">
         <v>2</v>
       </c>
@@ -2071,7 +2079,7 @@
       <c r="D71" s="9"/>
     </row>
     <row r="72" spans="1:4" ht="28">
-      <c r="A72" s="25"/>
+      <c r="A72" s="27"/>
       <c r="B72" s="14">
         <v>2</v>
       </c>
@@ -2081,7 +2089,7 @@
       <c r="D72" s="9"/>
     </row>
     <row r="73" spans="1:4" ht="28">
-      <c r="A73" s="25"/>
+      <c r="A73" s="27"/>
       <c r="B73" s="14">
         <v>2</v>
       </c>
@@ -2091,7 +2099,7 @@
       <c r="D73" s="9"/>
     </row>
     <row r="74" spans="1:4" ht="28">
-      <c r="A74" s="25"/>
+      <c r="A74" s="27"/>
       <c r="B74" s="14">
         <v>2</v>
       </c>
@@ -2101,7 +2109,7 @@
       <c r="D74" s="9"/>
     </row>
     <row r="75" spans="1:4" ht="28">
-      <c r="A75" s="25"/>
+      <c r="A75" s="27"/>
       <c r="B75" s="16">
         <v>5</v>
       </c>
@@ -2109,11 +2117,11 @@
         <v>103</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="42">
-      <c r="A76" s="25"/>
+      <c r="A76" s="27"/>
       <c r="B76" s="8">
         <v>5</v>
       </c>
@@ -2125,7 +2133,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="28">
-      <c r="A77" s="25"/>
+      <c r="A77" s="27"/>
       <c r="B77" s="14">
         <v>2</v>
       </c>
@@ -2135,7 +2143,7 @@
       <c r="D77" s="9"/>
     </row>
     <row r="78" spans="1:4" ht="28">
-      <c r="A78" s="25"/>
+      <c r="A78" s="27"/>
       <c r="B78" s="8">
         <v>2</v>
       </c>
@@ -2145,7 +2153,7 @@
       <c r="D78" s="9"/>
     </row>
     <row r="79" spans="1:4" ht="28">
-      <c r="A79" s="25"/>
+      <c r="A79" s="27"/>
       <c r="B79" s="8">
         <v>2</v>
       </c>
@@ -2155,7 +2163,7 @@
       <c r="D79" s="9"/>
     </row>
     <row r="80" spans="1:4" ht="42">
-      <c r="A80" s="25"/>
+      <c r="A80" s="27"/>
       <c r="B80" s="8">
         <v>1</v>
       </c>
@@ -2165,7 +2173,7 @@
       <c r="D80" s="9"/>
     </row>
     <row r="81" spans="1:4" ht="28">
-      <c r="A81" s="25"/>
+      <c r="A81" s="27"/>
       <c r="B81" s="8">
         <v>1</v>
       </c>
@@ -2175,7 +2183,7 @@
       <c r="D81" s="9"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="25"/>
+      <c r="A82" s="27"/>
       <c r="B82" s="8">
         <v>1</v>
       </c>
@@ -2185,7 +2193,7 @@
       <c r="D82" s="9"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="25"/>
+      <c r="A83" s="27"/>
       <c r="B83" s="14">
         <v>1</v>
       </c>
@@ -2195,7 +2203,7 @@
       <c r="D83" s="9"/>
     </row>
     <row r="84" spans="1:4" ht="28">
-      <c r="A84" s="25"/>
+      <c r="A84" s="27"/>
       <c r="B84" s="14">
         <v>1</v>
       </c>
@@ -2205,7 +2213,7 @@
       <c r="D84" s="9"/>
     </row>
     <row r="85" spans="1:4" ht="28">
-      <c r="A85" s="25"/>
+      <c r="A85" s="27"/>
       <c r="B85" s="14">
         <v>1</v>
       </c>
@@ -2215,7 +2223,7 @@
       <c r="D85" s="9"/>
     </row>
     <row r="86" spans="1:4" ht="28">
-      <c r="A86" s="25"/>
+      <c r="A86" s="27"/>
       <c r="B86" s="14">
         <v>1</v>
       </c>
@@ -2225,7 +2233,7 @@
       <c r="D86" s="9"/>
     </row>
     <row r="87" spans="1:4" ht="28">
-      <c r="A87" s="25"/>
+      <c r="A87" s="27"/>
       <c r="B87" s="14">
         <v>1</v>
       </c>
@@ -2235,7 +2243,7 @@
       <c r="D87" s="9"/>
     </row>
     <row r="88" spans="1:4" ht="28">
-      <c r="A88" s="25"/>
+      <c r="A88" s="27"/>
       <c r="B88" s="14">
         <v>1</v>
       </c>
@@ -2245,7 +2253,7 @@
       <c r="D88" s="9"/>
     </row>
     <row r="89" spans="1:4" ht="28">
-      <c r="A89" s="21" t="s">
+      <c r="A89" s="23" t="s">
         <v>118</v>
       </c>
       <c r="B89" s="14">
@@ -2257,7 +2265,7 @@
       <c r="D89" s="9"/>
     </row>
     <row r="90" spans="1:4" ht="42">
-      <c r="A90" s="21"/>
+      <c r="A90" s="23"/>
       <c r="B90" s="8">
         <v>5</v>
       </c>
@@ -2267,7 +2275,7 @@
       <c r="D90" s="9"/>
     </row>
     <row r="91" spans="1:4" ht="70">
-      <c r="A91" s="21"/>
+      <c r="A91" s="23"/>
       <c r="B91" s="8">
         <v>6</v>
       </c>
@@ -2279,7 +2287,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="28">
-      <c r="A92" s="21"/>
+      <c r="A92" s="23"/>
       <c r="B92" s="16">
         <v>5</v>
       </c>
@@ -2291,7 +2299,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" ht="28">
-      <c r="A93" s="21"/>
+      <c r="A93" s="23"/>
       <c r="B93" s="16">
         <v>5</v>
       </c>
@@ -2303,7 +2311,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="28">
-      <c r="A94" s="21"/>
+      <c r="A94" s="23"/>
       <c r="B94" s="16">
         <v>1</v>
       </c>
@@ -2313,7 +2321,7 @@
       <c r="D94" s="9"/>
     </row>
     <row r="95" spans="1:4" ht="112">
-      <c r="A95" s="21"/>
+      <c r="A95" s="23"/>
       <c r="B95" s="16">
         <v>5</v>
       </c>
@@ -2325,7 +2333,7 @@
       </c>
     </row>
     <row r="96" spans="1:4" ht="112">
-      <c r="A96" s="21"/>
+      <c r="A96" s="23"/>
       <c r="B96" s="16">
         <v>5</v>
       </c>
@@ -2337,7 +2345,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="70">
-      <c r="A97" s="21"/>
+      <c r="A97" s="23"/>
       <c r="B97" s="16">
         <v>5</v>
       </c>
@@ -2349,7 +2357,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="112">
-      <c r="A98" s="21"/>
+      <c r="A98" s="23"/>
       <c r="B98" s="16">
         <v>5</v>
       </c>
@@ -2361,7 +2369,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="28">
-      <c r="A99" s="21"/>
+      <c r="A99" s="23"/>
       <c r="B99" s="16">
         <v>5</v>
       </c>
@@ -2371,7 +2379,7 @@
       <c r="D99" s="9"/>
     </row>
     <row r="100" spans="1:4" ht="56">
-      <c r="A100" s="21"/>
+      <c r="A100" s="23"/>
       <c r="B100" s="16">
         <v>5</v>
       </c>
@@ -2381,7 +2389,7 @@
       <c r="D100" s="9"/>
     </row>
     <row r="101" spans="1:4" ht="42">
-      <c r="A101" s="21"/>
+      <c r="A101" s="23"/>
       <c r="B101" s="16">
         <v>5</v>
       </c>
@@ -2393,7 +2401,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="28">
-      <c r="A102" s="21"/>
+      <c r="A102" s="23"/>
       <c r="B102" s="16">
         <v>2</v>
       </c>
@@ -2403,7 +2411,7 @@
       <c r="D102" s="9"/>
     </row>
     <row r="103" spans="1:4" ht="42">
-      <c r="A103" s="21"/>
+      <c r="A103" s="23"/>
       <c r="B103" s="16">
         <v>2</v>
       </c>
@@ -2413,7 +2421,7 @@
       <c r="D103" s="9"/>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="21"/>
+      <c r="A104" s="23"/>
       <c r="B104" s="16">
         <v>1</v>
       </c>
@@ -2423,7 +2431,7 @@
       <c r="D104" s="9"/>
     </row>
     <row r="105" spans="1:4" ht="28">
-      <c r="A105" s="21"/>
+      <c r="A105" s="23"/>
       <c r="B105" s="16">
         <v>2</v>
       </c>
@@ -2433,7 +2441,7 @@
       <c r="D105" s="9"/>
     </row>
     <row r="106" spans="1:4" ht="42">
-      <c r="A106" s="21"/>
+      <c r="A106" s="23"/>
       <c r="B106" s="16">
         <v>2</v>
       </c>
@@ -2443,7 +2451,7 @@
       <c r="D106" s="9"/>
     </row>
     <row r="107" spans="1:4">
-      <c r="A107" s="21"/>
+      <c r="A107" s="23"/>
       <c r="B107" s="16">
         <v>2</v>
       </c>
@@ -2453,7 +2461,7 @@
       <c r="D107" s="9"/>
     </row>
     <row r="108" spans="1:4" ht="28">
-      <c r="A108" s="21"/>
+      <c r="A108" s="23"/>
       <c r="B108" s="16">
         <v>2</v>
       </c>
@@ -2463,7 +2471,7 @@
       <c r="D108" s="9"/>
     </row>
     <row r="109" spans="1:4" ht="42">
-      <c r="A109" s="21"/>
+      <c r="A109" s="23"/>
       <c r="B109" s="16">
         <v>5</v>
       </c>
@@ -2475,7 +2483,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" ht="56">
-      <c r="A110" s="21"/>
+      <c r="A110" s="23"/>
       <c r="B110" s="16">
         <v>5</v>
       </c>
@@ -2487,7 +2495,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="210">
-      <c r="A111" s="21"/>
+      <c r="A111" s="23"/>
       <c r="B111" s="16">
         <v>5</v>
       </c>
@@ -2499,7 +2507,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="42">
-      <c r="A112" s="21"/>
+      <c r="A112" s="23"/>
       <c r="B112" s="16">
         <v>5</v>
       </c>
@@ -2511,7 +2519,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="56">
-      <c r="A113" s="21"/>
+      <c r="A113" s="23"/>
       <c r="B113" s="16">
         <v>5</v>
       </c>
@@ -2523,7 +2531,7 @@
       </c>
     </row>
     <row r="114" spans="1:4" ht="56">
-      <c r="A114" s="21"/>
+      <c r="A114" s="23"/>
       <c r="B114" s="16">
         <v>5</v>
       </c>
@@ -2535,7 +2543,7 @@
       </c>
     </row>
     <row r="115" spans="1:4">
-      <c r="A115" s="21"/>
+      <c r="A115" s="23"/>
       <c r="B115" s="16">
         <v>2</v>
       </c>
@@ -2545,7 +2553,7 @@
       <c r="D115" s="9"/>
     </row>
     <row r="116" spans="1:4" ht="28">
-      <c r="A116" s="21"/>
+      <c r="A116" s="23"/>
       <c r="B116" s="16">
         <v>2</v>
       </c>
@@ -2555,7 +2563,7 @@
       <c r="D116" s="9"/>
     </row>
     <row r="117" spans="1:4" ht="70">
-      <c r="A117" s="21"/>
+      <c r="A117" s="23"/>
       <c r="B117" s="16">
         <v>5</v>
       </c>
@@ -2567,7 +2575,7 @@
       </c>
     </row>
     <row r="118" spans="1:4" ht="70">
-      <c r="A118" s="21"/>
+      <c r="A118" s="23"/>
       <c r="B118" s="16">
         <v>5</v>
       </c>
@@ -2579,7 +2587,7 @@
       </c>
     </row>
     <row r="119" spans="1:4" ht="28">
-      <c r="A119" s="21"/>
+      <c r="A119" s="23"/>
       <c r="B119" s="16">
         <v>1</v>
       </c>
@@ -2589,7 +2597,7 @@
       <c r="D119" s="9"/>
     </row>
     <row r="120" spans="1:4" ht="28">
-      <c r="A120" s="21"/>
+      <c r="A120" s="23"/>
       <c r="B120" s="16">
         <v>1</v>
       </c>
@@ -2598,301 +2606,303 @@
       </c>
       <c r="D120" s="9"/>
     </row>
-    <row r="121" spans="1:4" ht="28">
-      <c r="A121" s="21"/>
+    <row r="121" spans="1:4" ht="140">
+      <c r="A121" s="23"/>
       <c r="B121" s="16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C121" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D121" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="98">
+      <c r="A122" s="23"/>
+      <c r="B122" s="16">
+        <v>5</v>
+      </c>
+      <c r="C122" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D121" s="9"/>
-    </row>
-    <row r="122" spans="1:4" ht="98">
-      <c r="A122" s="21"/>
-      <c r="B122" s="16">
-        <v>5</v>
-      </c>
-      <c r="C122" s="2" t="s">
+      <c r="D122" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="D122" s="9" t="s">
+    </row>
+    <row r="123" spans="1:4" ht="42">
+      <c r="A123" s="23"/>
+      <c r="B123" s="16">
+        <v>1</v>
+      </c>
+      <c r="C123" s="2" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" ht="42">
-      <c r="A123" s="21"/>
-      <c r="B123" s="16">
-        <v>1</v>
-      </c>
-      <c r="C123" s="2" t="s">
+      <c r="D123" s="9"/>
+    </row>
+    <row r="124" spans="1:4" ht="42">
+      <c r="A124" s="23"/>
+      <c r="B124" s="16">
+        <v>1</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D123" s="9"/>
-    </row>
-    <row r="124" spans="1:4" ht="42">
-      <c r="A124" s="21"/>
-      <c r="B124" s="16">
-        <v>1</v>
-      </c>
-      <c r="C124" s="2" t="s">
+      <c r="D124" s="9"/>
+    </row>
+    <row r="125" spans="1:4" ht="42">
+      <c r="A125" s="23"/>
+      <c r="B125" s="16">
+        <v>1</v>
+      </c>
+      <c r="C125" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="D124" s="9"/>
-    </row>
-    <row r="125" spans="1:4" ht="42">
-      <c r="A125" s="21"/>
-      <c r="B125" s="16">
-        <v>1</v>
-      </c>
-      <c r="C125" s="10" t="s">
+      <c r="D125" s="9"/>
+    </row>
+    <row r="126" spans="1:4" ht="42">
+      <c r="A126" s="23"/>
+      <c r="B126" s="16">
+        <v>1</v>
+      </c>
+      <c r="C126" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="D125" s="9"/>
-    </row>
-    <row r="126" spans="1:4" ht="42">
-      <c r="A126" s="21"/>
-      <c r="B126" s="16">
-        <v>1</v>
-      </c>
-      <c r="C126" s="10" t="s">
+      <c r="D126" s="9"/>
+    </row>
+    <row r="127" spans="1:4" ht="28">
+      <c r="A127" s="23"/>
+      <c r="B127" s="16">
+        <v>1</v>
+      </c>
+      <c r="C127" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="D126" s="9"/>
-    </row>
-    <row r="127" spans="1:4" ht="28">
-      <c r="A127" s="21"/>
-      <c r="B127" s="16">
-        <v>1</v>
-      </c>
-      <c r="C127" s="10" t="s">
+      <c r="D127" s="9"/>
+    </row>
+    <row r="128" spans="1:4" ht="42">
+      <c r="A128" s="23"/>
+      <c r="B128" s="16">
+        <v>1</v>
+      </c>
+      <c r="C128" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="D127" s="9"/>
-    </row>
-    <row r="128" spans="1:4" ht="42">
-      <c r="A128" s="21"/>
-      <c r="B128" s="16">
-        <v>1</v>
-      </c>
-      <c r="C128" s="10" t="s">
+      <c r="D128" s="9"/>
+    </row>
+    <row r="129" spans="1:4" ht="28">
+      <c r="A129" s="23"/>
+      <c r="B129" s="17">
+        <v>1</v>
+      </c>
+      <c r="C129" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="D128" s="9"/>
-    </row>
-    <row r="129" spans="1:4" ht="28">
-      <c r="A129" s="21"/>
-      <c r="B129" s="17">
-        <v>1</v>
-      </c>
-      <c r="C129" s="10" t="s">
+      <c r="D129" s="9"/>
+    </row>
+    <row r="130" spans="1:4" ht="28">
+      <c r="A130" s="23"/>
+      <c r="B130" s="16">
+        <v>1</v>
+      </c>
+      <c r="C130" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="D129" s="9"/>
-    </row>
-    <row r="130" spans="1:4" ht="28">
-      <c r="A130" s="21"/>
-      <c r="B130" s="16">
-        <v>1</v>
-      </c>
-      <c r="C130" s="10" t="s">
+      <c r="D130" s="9"/>
+    </row>
+    <row r="131" spans="1:4" ht="28">
+      <c r="A131" s="23"/>
+      <c r="B131" s="16">
+        <v>1</v>
+      </c>
+      <c r="C131" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="D130" s="9"/>
-    </row>
-    <row r="131" spans="1:4" ht="28">
-      <c r="A131" s="21"/>
-      <c r="B131" s="16">
-        <v>1</v>
-      </c>
-      <c r="C131" s="10" t="s">
+      <c r="D131" s="9"/>
+    </row>
+    <row r="132" spans="1:4" ht="28">
+      <c r="A132" s="23"/>
+      <c r="B132" s="16">
+        <v>1</v>
+      </c>
+      <c r="C132" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="D131" s="9"/>
-    </row>
-    <row r="132" spans="1:4" ht="28">
-      <c r="A132" s="21"/>
-      <c r="B132" s="16">
-        <v>1</v>
-      </c>
-      <c r="C132" s="10" t="s">
+      <c r="D132" s="9"/>
+    </row>
+    <row r="133" spans="1:4" ht="70">
+      <c r="A133" s="23"/>
+      <c r="B133" s="16">
+        <v>5</v>
+      </c>
+      <c r="C133" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="D132" s="9"/>
-    </row>
-    <row r="133" spans="1:4" ht="70">
-      <c r="A133" s="21"/>
-      <c r="B133" s="16">
-        <v>5</v>
-      </c>
-      <c r="C133" s="10" t="s">
+      <c r="D133" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D133" s="9" t="s">
+    </row>
+    <row r="134" spans="1:4" ht="28">
+      <c r="A134" s="23"/>
+      <c r="B134" s="16">
+        <v>1</v>
+      </c>
+      <c r="C134" s="10" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" ht="28">
-      <c r="A134" s="21"/>
-      <c r="B134" s="16">
-        <v>1</v>
-      </c>
-      <c r="C134" s="10" t="s">
+      <c r="D134" s="9"/>
+    </row>
+    <row r="135" spans="1:4" ht="28">
+      <c r="A135" s="23"/>
+      <c r="B135" s="16">
+        <v>1</v>
+      </c>
+      <c r="C135" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="D134" s="9"/>
-    </row>
-    <row r="135" spans="1:4" ht="28">
-      <c r="A135" s="21"/>
-      <c r="B135" s="16">
-        <v>1</v>
-      </c>
-      <c r="C135" s="10" t="s">
+      <c r="D135" s="9"/>
+    </row>
+    <row r="136" spans="1:4" ht="28">
+      <c r="A136" s="23"/>
+      <c r="B136" s="16">
+        <v>1</v>
+      </c>
+      <c r="C136" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="D135" s="9"/>
-    </row>
-    <row r="136" spans="1:4" ht="28">
-      <c r="A136" s="21"/>
-      <c r="B136" s="16">
-        <v>1</v>
-      </c>
-      <c r="C136" s="10" t="s">
+      <c r="D136" s="9"/>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="23"/>
+      <c r="B137" s="16">
+        <v>1</v>
+      </c>
+      <c r="C137" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="D136" s="9"/>
-    </row>
-    <row r="137" spans="1:4">
-      <c r="A137" s="21"/>
-      <c r="B137" s="16">
-        <v>1</v>
-      </c>
-      <c r="C137" s="10" t="s">
+      <c r="D137" s="9"/>
+    </row>
+    <row r="138" spans="1:4" ht="42">
+      <c r="A138" s="23"/>
+      <c r="B138" s="16">
+        <v>5</v>
+      </c>
+      <c r="C138" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="D137" s="9"/>
-    </row>
-    <row r="138" spans="1:4" ht="42">
-      <c r="A138" s="21"/>
-      <c r="B138" s="16">
-        <v>5</v>
-      </c>
-      <c r="C138" s="10" t="s">
+      <c r="D138" s="9"/>
+    </row>
+    <row r="139" spans="1:4" ht="126">
+      <c r="A139" s="23"/>
+      <c r="B139" s="16">
+        <v>5</v>
+      </c>
+      <c r="C139" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="D138" s="9"/>
-    </row>
-    <row r="139" spans="1:4" ht="126">
-      <c r="A139" s="21"/>
-      <c r="B139" s="16">
-        <v>5</v>
-      </c>
-      <c r="C139" s="10" t="s">
+      <c r="D139" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="D139" s="9" t="s">
+    </row>
+    <row r="140" spans="1:4" ht="42">
+      <c r="A140" s="23"/>
+      <c r="B140" s="16">
+        <v>5</v>
+      </c>
+      <c r="C140" s="10" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" ht="42">
-      <c r="A140" s="21"/>
-      <c r="B140" s="16">
-        <v>5</v>
-      </c>
-      <c r="C140" s="10" t="s">
+      <c r="D140" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="D140" s="9" t="s">
+    </row>
+    <row r="141" spans="1:4" ht="26">
+      <c r="A141" s="23"/>
+      <c r="B141" s="16">
+        <v>1</v>
+      </c>
+      <c r="C141" s="18" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" ht="26">
-      <c r="A141" s="21"/>
-      <c r="B141" s="16">
-        <v>1</v>
-      </c>
-      <c r="C141" s="18" t="s">
+      <c r="D141" s="9"/>
+    </row>
+    <row r="142" spans="1:4" ht="28">
+      <c r="A142" s="23"/>
+      <c r="B142" s="16">
+        <v>1</v>
+      </c>
+      <c r="C142" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="D141" s="9"/>
-    </row>
-    <row r="142" spans="1:4" ht="28">
-      <c r="A142" s="21"/>
-      <c r="B142" s="16">
-        <v>1</v>
-      </c>
-      <c r="C142" s="10" t="s">
+      <c r="D142" s="9"/>
+    </row>
+    <row r="143" spans="1:4" ht="42">
+      <c r="A143" s="23"/>
+      <c r="B143" s="16">
+        <v>5</v>
+      </c>
+      <c r="C143" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="D142" s="9"/>
-    </row>
-    <row r="143" spans="1:4" ht="42">
-      <c r="A143" s="21"/>
-      <c r="B143" s="16">
-        <v>5</v>
-      </c>
-      <c r="C143" s="10" t="s">
+      <c r="D143" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="D143" s="9" t="s">
+    </row>
+    <row r="144" spans="1:4" ht="70">
+      <c r="A144" s="23"/>
+      <c r="B144" s="16">
+        <v>5</v>
+      </c>
+      <c r="C144" s="19" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" ht="70">
-      <c r="A144" s="21"/>
-      <c r="B144" s="16">
-        <v>5</v>
-      </c>
-      <c r="C144" s="19" t="s">
+      <c r="D144" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="D144" s="9" t="s">
+    </row>
+    <row r="145" spans="1:4" ht="49.5">
+      <c r="A145" s="23"/>
+      <c r="B145" s="16">
+        <v>2</v>
+      </c>
+      <c r="C145" s="19" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" ht="49.5">
-      <c r="A145" s="21"/>
-      <c r="B145" s="16">
-        <v>2</v>
-      </c>
-      <c r="C145" s="19" t="s">
+      <c r="D145" s="9"/>
+    </row>
+    <row r="146" spans="1:4" ht="154">
+      <c r="A146" s="24"/>
+      <c r="B146" s="16">
+        <v>5</v>
+      </c>
+      <c r="C146" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="D145" s="9"/>
-    </row>
-    <row r="146" spans="1:4" ht="154">
-      <c r="A146" s="22"/>
-      <c r="B146" s="16">
-        <v>5</v>
-      </c>
-      <c r="C146" s="9" t="s">
+      <c r="D146" s="9" t="s">
         <v>198</v>
-      </c>
-      <c r="D146" s="9" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="56">
       <c r="A147" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="B147" s="26">
-        <v>1</v>
-      </c>
-      <c r="C147" s="27" t="s">
-        <v>210</v>
-      </c>
-      <c r="D147" s="27"/>
+        <v>199</v>
+      </c>
+      <c r="B147" s="21">
+        <v>1</v>
+      </c>
+      <c r="C147" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="D147" s="22"/>
     </row>
     <row r="148" spans="1:4" ht="42" customHeight="1">
       <c r="B148" s="16">
         <v>5</v>
       </c>
       <c r="C148" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D148" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="42">
@@ -2901,7 +2911,7 @@
         <v>1</v>
       </c>
       <c r="C149" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D149" s="10"/>
     </row>
@@ -2911,43 +2921,43 @@
         <v>1</v>
       </c>
       <c r="C150" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D150" s="10"/>
+    </row>
+    <row r="151" spans="1:4" ht="42">
+      <c r="A151" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="D150" s="10"/>
-    </row>
-    <row r="151" spans="1:4" ht="42">
-      <c r="A151" s="23" t="s">
+      <c r="B151" s="1">
+        <v>1</v>
+      </c>
+      <c r="C151" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B151" s="1">
-        <v>1</v>
-      </c>
-      <c r="C151" s="2" t="s">
+    </row>
+    <row r="152" spans="1:4" ht="182">
+      <c r="A152" s="25"/>
+      <c r="B152" s="16">
+        <v>5</v>
+      </c>
+      <c r="C152" s="2" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" ht="182">
-      <c r="A152" s="23"/>
-      <c r="B152" s="16">
-        <v>5</v>
-      </c>
-      <c r="C152" s="2" t="s">
+      <c r="D152" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D152" s="2" t="s">
+    </row>
+    <row r="153" spans="1:4" ht="56">
+      <c r="A153" s="25"/>
+      <c r="B153" s="16">
+        <v>5</v>
+      </c>
+      <c r="C153" s="2" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" ht="56">
-      <c r="A153" s="23"/>
-      <c r="B153" s="16">
-        <v>5</v>
-      </c>
-      <c r="C153" s="2" t="s">
+      <c r="D153" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="D153" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add some new paper which site SCNN
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="13140"/>
+    <workbookView windowWidth="15120" windowHeight="25770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="226">
   <si>
     <t>Scope</t>
   </si>
@@ -578,7 +578,7 @@
 由于GCN主要提升的是object内部的分类效果，针对边界，提出了boundary refinement module</t>
   </si>
   <si>
-    <t>learning a similarity meri discriminatively, with application to face verification</t>
+    <t>learning a similarity mertric discriminatively, with application to face verification</t>
   </si>
   <si>
     <t>Recurrent Pixel Embedding for Instance Grouping</t>
@@ -637,6 +637,12 @@
   <si>
     <t>1. 提出采用轮廓作为feature, 和RGB图同时作为输入的连体FCN, 能将F1 score提高2%, 同时加快training的速度
 2. 在featureMap后加入location prior(也就是每个activation点的坐标), 可以有效去除诸如把天空分类为道路的情况</t>
+  </si>
+  <si>
+    <t>Multiple Encoder-Decoder net for Lane Detection</t>
+  </si>
+  <si>
+    <t>Exploring New Backbone and Attention Module for Semantic Segmentation in Street Scenes</t>
   </si>
   <si>
     <t>DeepLanes_End-to-End Lane Position Estimation using Deep Neural Networks</t>
@@ -753,9 +759,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -815,6 +821,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -830,45 +860,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -876,9 +867,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -893,31 +884,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -930,8 +898,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -945,7 +914,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -978,7 +984,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -990,79 +1038,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1080,6 +1062,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1092,19 +1098,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1116,25 +1146,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1146,19 +1158,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1224,6 +1230,39 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1235,26 +1274,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1274,17 +1293,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1307,15 +1322,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -1326,142 +1332,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1471,7 +1477,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1521,9 +1527,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1917,12 +1920,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G162"/>
+  <dimension ref="A1:G161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D75" sqref="D75"/>
+      <selection pane="bottomLeft" activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -2124,7 +2127,7 @@
       <c r="D17" s="11"/>
     </row>
     <row r="18" ht="25.5" spans="1:4">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="16">
@@ -2136,7 +2139,7 @@
       <c r="D18" s="11"/>
     </row>
     <row r="19" ht="27" spans="1:4">
-      <c r="A19" s="17"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="14">
         <v>5</v>
       </c>
@@ -2148,7 +2151,7 @@
       </c>
     </row>
     <row r="20" ht="37" customHeight="1" spans="1:4">
-      <c r="A20" s="17"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="10">
         <v>5</v>
       </c>
@@ -2160,7 +2163,7 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="17"/>
+      <c r="A21" s="9"/>
       <c r="B21" s="16">
         <v>3</v>
       </c>
@@ -2170,7 +2173,7 @@
       <c r="D21" s="11"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="17"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="14">
         <v>5</v>
       </c>
@@ -2180,7 +2183,7 @@
       <c r="D22" s="11"/>
     </row>
     <row r="23" ht="27" spans="1:4">
-      <c r="A23" s="17"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="14">
         <v>5</v>
       </c>
@@ -2192,7 +2195,7 @@
       </c>
     </row>
     <row r="24" ht="25.5" spans="1:4">
-      <c r="A24" s="17"/>
+      <c r="A24" s="9"/>
       <c r="B24" s="16">
         <v>3</v>
       </c>
@@ -2202,7 +2205,7 @@
       <c r="D24" s="11"/>
     </row>
     <row r="25" ht="25.5" spans="1:4">
-      <c r="A25" s="17"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="16">
         <v>3</v>
       </c>
@@ -2212,7 +2215,7 @@
       <c r="D25" s="11"/>
     </row>
     <row r="26" ht="25.5" spans="1:4">
-      <c r="A26" s="17"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="16">
         <v>3</v>
       </c>
@@ -2222,7 +2225,7 @@
       <c r="D26" s="11"/>
     </row>
     <row r="27" ht="25.5" spans="1:4">
-      <c r="A27" s="17"/>
+      <c r="A27" s="9"/>
       <c r="B27" s="16">
         <v>3</v>
       </c>
@@ -2232,7 +2235,7 @@
       <c r="D27" s="11"/>
     </row>
     <row r="28" ht="13.5" spans="1:4">
-      <c r="A28" s="17"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="16">
         <v>2</v>
       </c>
@@ -2242,7 +2245,7 @@
       <c r="D28" s="11"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="17"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="16">
         <v>2</v>
       </c>
@@ -2252,7 +2255,7 @@
       <c r="D29" s="11"/>
     </row>
     <row r="30" ht="25.5" spans="1:4">
-      <c r="A30" s="17"/>
+      <c r="A30" s="9"/>
       <c r="B30" s="16">
         <v>2</v>
       </c>
@@ -2262,7 +2265,7 @@
       <c r="D30" s="11"/>
     </row>
     <row r="31" ht="79.5" spans="1:4">
-      <c r="A31" s="17"/>
+      <c r="A31" s="9"/>
       <c r="B31" s="14">
         <v>5</v>
       </c>
@@ -2274,7 +2277,7 @@
       </c>
     </row>
     <row r="32" ht="27" spans="1:4">
-      <c r="A32" s="17"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="14">
         <v>5</v>
       </c>
@@ -2286,7 +2289,7 @@
       </c>
     </row>
     <row r="33" ht="25.5" spans="1:4">
-      <c r="A33" s="17"/>
+      <c r="A33" s="9"/>
       <c r="B33" s="16">
         <v>2</v>
       </c>
@@ -2296,7 +2299,7 @@
       <c r="D33" s="11"/>
     </row>
     <row r="34" ht="25.5" spans="1:4">
-      <c r="A34" s="17"/>
+      <c r="A34" s="9"/>
       <c r="B34" s="14">
         <v>5</v>
       </c>
@@ -2306,7 +2309,7 @@
       <c r="D34" s="11"/>
     </row>
     <row r="35" ht="25.5" spans="1:4">
-      <c r="A35" s="17"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="14">
         <v>5</v>
       </c>
@@ -2316,7 +2319,7 @@
       <c r="D35" s="11"/>
     </row>
     <row r="36" ht="80.25" spans="1:4">
-      <c r="A36" s="17"/>
+      <c r="A36" s="9"/>
       <c r="B36" s="14">
         <v>5</v>
       </c>
@@ -2328,7 +2331,7 @@
       </c>
     </row>
     <row r="37" ht="27" spans="1:4">
-      <c r="A37" s="17"/>
+      <c r="A37" s="9"/>
       <c r="B37" s="14">
         <v>5</v>
       </c>
@@ -2340,7 +2343,7 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="17"/>
+      <c r="A38" s="9"/>
       <c r="B38" s="16">
         <v>2</v>
       </c>
@@ -2350,7 +2353,7 @@
       <c r="D38" s="11"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="17"/>
+      <c r="A39" s="9"/>
       <c r="B39" s="16">
         <v>2</v>
       </c>
@@ -2360,7 +2363,7 @@
       <c r="D39" s="11"/>
     </row>
     <row r="40" ht="39.75" spans="1:4">
-      <c r="A40" s="17"/>
+      <c r="A40" s="9"/>
       <c r="B40" s="14">
         <v>5</v>
       </c>
@@ -2372,7 +2375,7 @@
       </c>
     </row>
     <row r="41" ht="25.5" spans="1:4">
-      <c r="A41" s="17"/>
+      <c r="A41" s="9"/>
       <c r="B41" s="16">
         <v>2</v>
       </c>
@@ -2382,7 +2385,7 @@
       <c r="D41" s="11"/>
     </row>
     <row r="42" ht="78.75" spans="1:4">
-      <c r="A42" s="17"/>
+      <c r="A42" s="9"/>
       <c r="B42" s="14">
         <v>5</v>
       </c>
@@ -2394,7 +2397,7 @@
       </c>
     </row>
     <row r="43" ht="27" spans="1:4">
-      <c r="A43" s="17"/>
+      <c r="A43" s="9"/>
       <c r="B43" s="14">
         <v>5</v>
       </c>
@@ -2406,7 +2409,7 @@
       </c>
     </row>
     <row r="44" ht="25.5" spans="1:4">
-      <c r="A44" s="17"/>
+      <c r="A44" s="9"/>
       <c r="B44" s="14">
         <v>5</v>
       </c>
@@ -2416,7 +2419,7 @@
       <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="17"/>
+      <c r="A45" s="9"/>
       <c r="B45" s="14">
         <v>5</v>
       </c>
@@ -2426,7 +2429,7 @@
       <c r="D45" s="11"/>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="17"/>
+      <c r="A46" s="9"/>
       <c r="B46" s="16">
         <v>2</v>
       </c>
@@ -2436,7 +2439,7 @@
       <c r="D46" s="11"/>
     </row>
     <row r="47" ht="53" customHeight="1" spans="1:4">
-      <c r="A47" s="17"/>
+      <c r="A47" s="9"/>
       <c r="B47" s="14">
         <v>5</v>
       </c>
@@ -2448,7 +2451,7 @@
       </c>
     </row>
     <row r="48" ht="41" customHeight="1" spans="1:4">
-      <c r="A48" s="17"/>
+      <c r="A48" s="9"/>
       <c r="B48" s="14">
         <v>5</v>
       </c>
@@ -2520,10 +2523,10 @@
         <v>78</v>
       </c>
       <c r="D54" s="11"/>
-      <c r="F54" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G54" s="18" t="s">
+      <c r="F54" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G54" s="17" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2536,8 +2539,8 @@
         <v>80</v>
       </c>
       <c r="D55" s="11"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
     </row>
     <row r="56" ht="51.75" spans="1:7">
       <c r="A56" s="9"/>
@@ -2769,7 +2772,7 @@
     </row>
     <row r="76" ht="13.5" spans="1:4">
       <c r="A76" s="9"/>
-      <c r="B76" s="19">
+      <c r="B76" s="18">
         <v>5</v>
       </c>
       <c r="C76" s="2" t="s">
@@ -2922,7 +2925,7 @@
       <c r="D90" s="11"/>
     </row>
     <row r="91" ht="25.5" spans="1:4">
-      <c r="A91" s="20" t="s">
+      <c r="A91" s="19" t="s">
         <v>124</v>
       </c>
       <c r="B91" s="16">
@@ -2934,7 +2937,7 @@
       <c r="D91" s="11"/>
     </row>
     <row r="92" ht="39.75" spans="1:4">
-      <c r="A92" s="20"/>
+      <c r="A92" s="19"/>
       <c r="B92" s="10">
         <v>5</v>
       </c>
@@ -2944,7 +2947,7 @@
       <c r="D92" s="11"/>
     </row>
     <row r="93" ht="66" spans="1:4">
-      <c r="A93" s="20"/>
+      <c r="A93" s="19"/>
       <c r="B93" s="10">
         <v>6</v>
       </c>
@@ -2956,8 +2959,8 @@
       </c>
     </row>
     <row r="94" ht="13.5" spans="1:4">
-      <c r="A94" s="20"/>
-      <c r="B94" s="19">
+      <c r="A94" s="19"/>
+      <c r="B94" s="18">
         <v>5</v>
       </c>
       <c r="C94" s="11" t="s">
@@ -2968,8 +2971,8 @@
       </c>
     </row>
     <row r="95" ht="27" spans="1:4">
-      <c r="A95" s="20"/>
-      <c r="B95" s="19">
+      <c r="A95" s="19"/>
+      <c r="B95" s="18">
         <v>5</v>
       </c>
       <c r="C95" s="11" t="s">
@@ -2980,8 +2983,8 @@
       </c>
     </row>
     <row r="96" ht="25.5" spans="1:4">
-      <c r="A96" s="20"/>
-      <c r="B96" s="19">
+      <c r="A96" s="19"/>
+      <c r="B96" s="18">
         <v>1</v>
       </c>
       <c r="C96" s="11" t="s">
@@ -2990,8 +2993,8 @@
       <c r="D96" s="11"/>
     </row>
     <row r="97" ht="93" spans="1:4">
-      <c r="A97" s="20"/>
-      <c r="B97" s="19">
+      <c r="A97" s="19"/>
+      <c r="B97" s="18">
         <v>5</v>
       </c>
       <c r="C97" s="11" t="s">
@@ -3002,8 +3005,8 @@
       </c>
     </row>
     <row r="98" ht="93" spans="1:4">
-      <c r="A98" s="20"/>
-      <c r="B98" s="19">
+      <c r="A98" s="19"/>
+      <c r="B98" s="18">
         <v>5</v>
       </c>
       <c r="C98" s="11" t="s">
@@ -3014,8 +3017,8 @@
       </c>
     </row>
     <row r="99" ht="53.25" spans="1:4">
-      <c r="A99" s="20"/>
-      <c r="B99" s="19">
+      <c r="A99" s="19"/>
+      <c r="B99" s="18">
         <v>5</v>
       </c>
       <c r="C99" s="11" t="s">
@@ -3026,8 +3029,8 @@
       </c>
     </row>
     <row r="100" ht="106.5" spans="1:4">
-      <c r="A100" s="20"/>
-      <c r="B100" s="19">
+      <c r="A100" s="19"/>
+      <c r="B100" s="18">
         <v>5</v>
       </c>
       <c r="C100" s="11" t="s">
@@ -3038,8 +3041,8 @@
       </c>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="20"/>
-      <c r="B101" s="19">
+      <c r="A101" s="19"/>
+      <c r="B101" s="18">
         <v>5</v>
       </c>
       <c r="C101" s="11" t="s">
@@ -3048,8 +3051,8 @@
       <c r="D101" s="11"/>
     </row>
     <row r="102" ht="26.25" spans="1:4">
-      <c r="A102" s="20"/>
-      <c r="B102" s="19">
+      <c r="A102" s="19"/>
+      <c r="B102" s="18">
         <v>5</v>
       </c>
       <c r="C102" s="11" t="s">
@@ -3058,8 +3061,8 @@
       <c r="D102" s="11"/>
     </row>
     <row r="103" ht="39.75" spans="1:4">
-      <c r="A103" s="20"/>
-      <c r="B103" s="19">
+      <c r="A103" s="19"/>
+      <c r="B103" s="18">
         <v>5</v>
       </c>
       <c r="C103" s="11" t="s">
@@ -3070,8 +3073,8 @@
       </c>
     </row>
     <row r="104" ht="25.5" spans="1:4">
-      <c r="A104" s="20"/>
-      <c r="B104" s="19">
+      <c r="A104" s="19"/>
+      <c r="B104" s="18">
         <v>2</v>
       </c>
       <c r="C104" s="12" t="s">
@@ -3080,8 +3083,8 @@
       <c r="D104" s="11"/>
     </row>
     <row r="105" ht="25.5" spans="1:4">
-      <c r="A105" s="20"/>
-      <c r="B105" s="19">
+      <c r="A105" s="19"/>
+      <c r="B105" s="18">
         <v>2</v>
       </c>
       <c r="C105" s="12" t="s">
@@ -3090,8 +3093,8 @@
       <c r="D105" s="11"/>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="20"/>
-      <c r="B106" s="19">
+      <c r="A106" s="19"/>
+      <c r="B106" s="18">
         <v>1</v>
       </c>
       <c r="C106" t="s">
@@ -3100,8 +3103,8 @@
       <c r="D106" s="11"/>
     </row>
     <row r="107" ht="25.5" spans="1:4">
-      <c r="A107" s="20"/>
-      <c r="B107" s="19">
+      <c r="A107" s="19"/>
+      <c r="B107" s="18">
         <v>2</v>
       </c>
       <c r="C107" s="2" t="s">
@@ -3110,8 +3113,8 @@
       <c r="D107" s="11"/>
     </row>
     <row r="108" ht="25.5" spans="1:4">
-      <c r="A108" s="20"/>
-      <c r="B108" s="19">
+      <c r="A108" s="19"/>
+      <c r="B108" s="18">
         <v>2</v>
       </c>
       <c r="C108" s="12" t="s">
@@ -3120,8 +3123,8 @@
       <c r="D108" s="11"/>
     </row>
     <row r="109" spans="1:4">
-      <c r="A109" s="20"/>
-      <c r="B109" s="19">
+      <c r="A109" s="19"/>
+      <c r="B109" s="18">
         <v>2</v>
       </c>
       <c r="C109" s="12" t="s">
@@ -3130,8 +3133,8 @@
       <c r="D109" s="11"/>
     </row>
     <row r="110" ht="25.5" spans="1:4">
-      <c r="A110" s="20"/>
-      <c r="B110" s="19">
+      <c r="A110" s="19"/>
+      <c r="B110" s="18">
         <v>2</v>
       </c>
       <c r="C110" s="12" t="s">
@@ -3140,8 +3143,8 @@
       <c r="D110" s="11"/>
     </row>
     <row r="111" ht="25.5" spans="1:4">
-      <c r="A111" s="20"/>
-      <c r="B111" s="19">
+      <c r="A111" s="19"/>
+      <c r="B111" s="18">
         <v>5</v>
       </c>
       <c r="C111" s="12" t="s">
@@ -3152,8 +3155,8 @@
       </c>
     </row>
     <row r="112" ht="39.75" spans="1:4">
-      <c r="A112" s="20"/>
-      <c r="B112" s="19">
+      <c r="A112" s="19"/>
+      <c r="B112" s="18">
         <v>5</v>
       </c>
       <c r="C112" s="12" t="s">
@@ -3164,8 +3167,8 @@
       </c>
     </row>
     <row r="113" ht="156.75" spans="1:4">
-      <c r="A113" s="20"/>
-      <c r="B113" s="19">
+      <c r="A113" s="19"/>
+      <c r="B113" s="18">
         <v>5</v>
       </c>
       <c r="C113" s="12" t="s">
@@ -3176,8 +3179,8 @@
       </c>
     </row>
     <row r="114" ht="27" spans="1:4">
-      <c r="A114" s="20"/>
-      <c r="B114" s="19">
+      <c r="A114" s="19"/>
+      <c r="B114" s="18">
         <v>5</v>
       </c>
       <c r="C114" s="12" t="s">
@@ -3188,8 +3191,8 @@
       </c>
     </row>
     <row r="115" ht="54" spans="1:4">
-      <c r="A115" s="20"/>
-      <c r="B115" s="19">
+      <c r="A115" s="19"/>
+      <c r="B115" s="18">
         <v>5</v>
       </c>
       <c r="C115" s="12" t="s">
@@ -3200,8 +3203,8 @@
       </c>
     </row>
     <row r="116" ht="54" spans="1:4">
-      <c r="A116" s="20"/>
-      <c r="B116" s="19">
+      <c r="A116" s="19"/>
+      <c r="B116" s="18">
         <v>5</v>
       </c>
       <c r="C116" s="12" t="s">
@@ -3212,9 +3215,9 @@
       </c>
     </row>
     <row r="117" ht="25.5" spans="1:4">
-      <c r="A117" s="20"/>
-      <c r="B117" s="21">
-        <v>1</v>
+      <c r="A117" s="19"/>
+      <c r="B117" s="20">
+        <v>2</v>
       </c>
       <c r="C117" s="12" t="s">
         <v>165</v>
@@ -3222,8 +3225,8 @@
       <c r="D117" s="11"/>
     </row>
     <row r="118" ht="25.5" spans="1:4">
-      <c r="A118" s="20"/>
-      <c r="B118" s="19">
+      <c r="A118" s="19"/>
+      <c r="B118" s="18">
         <v>1</v>
       </c>
       <c r="C118" s="12" t="s">
@@ -3232,8 +3235,8 @@
       <c r="D118" s="11"/>
     </row>
     <row r="119" ht="25.5" spans="1:4">
-      <c r="A119" s="20"/>
-      <c r="B119" s="19">
+      <c r="A119" s="19"/>
+      <c r="B119" s="18">
         <v>1</v>
       </c>
       <c r="C119" s="12" t="s">
@@ -3242,8 +3245,8 @@
       <c r="D119" s="11"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="20"/>
-      <c r="B120" s="19">
+      <c r="A120" s="19"/>
+      <c r="B120" s="18">
         <v>2</v>
       </c>
       <c r="C120" s="2" t="s">
@@ -3252,8 +3255,8 @@
       <c r="D120" s="11"/>
     </row>
     <row r="121" ht="25.5" spans="1:4">
-      <c r="A121" s="20"/>
-      <c r="B121" s="19">
+      <c r="A121" s="19"/>
+      <c r="B121" s="18">
         <v>2</v>
       </c>
       <c r="C121" s="2" t="s">
@@ -3262,8 +3265,8 @@
       <c r="D121" s="11"/>
     </row>
     <row r="122" ht="54" spans="1:4">
-      <c r="A122" s="20"/>
-      <c r="B122" s="19">
+      <c r="A122" s="19"/>
+      <c r="B122" s="18">
         <v>5</v>
       </c>
       <c r="C122" s="2" t="s">
@@ -3274,8 +3277,8 @@
       </c>
     </row>
     <row r="123" ht="66.75" spans="1:4">
-      <c r="A123" s="20"/>
-      <c r="B123" s="19">
+      <c r="A123" s="19"/>
+      <c r="B123" s="18">
         <v>5</v>
       </c>
       <c r="C123" s="2" t="s">
@@ -3286,8 +3289,8 @@
       </c>
     </row>
     <row r="124" ht="25.5" spans="1:4">
-      <c r="A124" s="20"/>
-      <c r="B124" s="19">
+      <c r="A124" s="19"/>
+      <c r="B124" s="18">
         <v>1</v>
       </c>
       <c r="C124" s="2" t="s">
@@ -3296,8 +3299,8 @@
       <c r="D124" s="11"/>
     </row>
     <row r="125" spans="1:4">
-      <c r="A125" s="20"/>
-      <c r="B125" s="19">
+      <c r="A125" s="19"/>
+      <c r="B125" s="18">
         <v>2</v>
       </c>
       <c r="C125" s="2" t="s">
@@ -3306,8 +3309,8 @@
       <c r="D125" s="11"/>
     </row>
     <row r="126" ht="25.5" spans="1:4">
-      <c r="A126" s="20"/>
-      <c r="B126" s="19">
+      <c r="A126" s="19"/>
+      <c r="B126" s="18">
         <v>1</v>
       </c>
       <c r="C126" s="2" t="s">
@@ -3316,8 +3319,8 @@
       <c r="D126" s="11"/>
     </row>
     <row r="127" spans="1:4">
-      <c r="A127" s="20"/>
-      <c r="B127" s="19">
+      <c r="A127" s="19"/>
+      <c r="B127" s="18">
         <v>2</v>
       </c>
       <c r="C127" s="2" t="s">
@@ -3326,8 +3329,8 @@
       <c r="D127" s="11"/>
     </row>
     <row r="128" ht="25.5" spans="1:4">
-      <c r="A128" s="20"/>
-      <c r="B128" s="19">
+      <c r="A128" s="19"/>
+      <c r="B128" s="18">
         <v>2</v>
       </c>
       <c r="C128" s="2" t="s">
@@ -3336,8 +3339,8 @@
       <c r="D128" s="11"/>
     </row>
     <row r="129" ht="108" spans="1:4">
-      <c r="A129" s="20"/>
-      <c r="B129" s="19">
+      <c r="A129" s="19"/>
+      <c r="B129" s="18">
         <v>5</v>
       </c>
       <c r="C129" s="2" t="s">
@@ -3348,8 +3351,8 @@
       </c>
     </row>
     <row r="130" ht="66.75" spans="1:4">
-      <c r="A130" s="20"/>
-      <c r="B130" s="19">
+      <c r="A130" s="19"/>
+      <c r="B130" s="18">
         <v>5</v>
       </c>
       <c r="C130" s="2" t="s">
@@ -3360,8 +3363,8 @@
       </c>
     </row>
     <row r="131" ht="38.25" spans="1:4">
-      <c r="A131" s="20"/>
-      <c r="B131" s="19">
+      <c r="A131" s="19"/>
+      <c r="B131" s="18">
         <v>1</v>
       </c>
       <c r="C131" s="2" t="s">
@@ -3370,8 +3373,8 @@
       <c r="D131" s="11"/>
     </row>
     <row r="132" ht="25.5" spans="1:4">
-      <c r="A132" s="20"/>
-      <c r="B132" s="19">
+      <c r="A132" s="19"/>
+      <c r="B132" s="18">
         <v>1</v>
       </c>
       <c r="C132" s="2" t="s">
@@ -3380,8 +3383,8 @@
       <c r="D132" s="11"/>
     </row>
     <row r="133" ht="26.25" spans="1:4">
-      <c r="A133" s="20"/>
-      <c r="B133" s="19">
+      <c r="A133" s="19"/>
+      <c r="B133" s="18">
         <v>1</v>
       </c>
       <c r="C133" s="12" t="s">
@@ -3390,8 +3393,8 @@
       <c r="D133" s="11"/>
     </row>
     <row r="134" spans="1:4">
-      <c r="A134" s="20"/>
-      <c r="B134" s="19">
+      <c r="A134" s="19"/>
+      <c r="B134" s="18">
         <v>1</v>
       </c>
       <c r="C134" s="12" t="s">
@@ -3400,8 +3403,8 @@
       <c r="D134" s="11"/>
     </row>
     <row r="135" ht="66.75" spans="1:4">
-      <c r="A135" s="20"/>
-      <c r="B135" s="19">
+      <c r="A135" s="19"/>
+      <c r="B135" s="18">
         <v>5</v>
       </c>
       <c r="C135" s="12" t="s">
@@ -3411,276 +3414,284 @@
         <v>188</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
-      <c r="A136" s="20"/>
+    <row r="136" ht="26.25" spans="1:4">
+      <c r="A136" s="19"/>
+      <c r="B136" s="18">
+        <v>1</v>
+      </c>
+      <c r="C136" s="12" t="s">
+        <v>189</v>
+      </c>
       <c r="D136" s="11"/>
     </row>
-    <row r="137" spans="1:4">
-      <c r="A137" s="20"/>
-      <c r="D137" s="11"/>
+    <row r="137" ht="66.75" spans="1:4">
+      <c r="A137" s="19"/>
+      <c r="B137" s="18">
+        <v>5</v>
+      </c>
+      <c r="C137" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D137" s="11" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="138" spans="1:4">
-      <c r="A138" s="20"/>
+      <c r="A138" s="19"/>
+      <c r="B138" s="18">
+        <v>1</v>
+      </c>
+      <c r="C138" s="12" t="s">
+        <v>192</v>
+      </c>
       <c r="D138" s="11"/>
     </row>
-    <row r="139" ht="26.25" spans="1:4">
-      <c r="A139" s="20"/>
-      <c r="B139" s="19">
+    <row r="139" ht="25.5" spans="1:4">
+      <c r="A139" s="19"/>
+      <c r="B139" s="18">
         <v>1</v>
       </c>
       <c r="C139" s="12" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D139" s="11"/>
     </row>
-    <row r="140" ht="66.75" spans="1:4">
-      <c r="A140" s="20"/>
-      <c r="B140" s="19">
-        <v>5</v>
+    <row r="140" ht="25.5" spans="1:4">
+      <c r="A140" s="19"/>
+      <c r="B140" s="18">
+        <v>1</v>
       </c>
       <c r="C140" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D140" s="11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="141" ht="25.5" spans="1:4">
-      <c r="A141" s="20"/>
-      <c r="B141" s="19">
+        <v>194</v>
+      </c>
+      <c r="D140" s="11"/>
+    </row>
+    <row r="141" ht="26.25" spans="1:4">
+      <c r="A141" s="19"/>
+      <c r="B141" s="18">
         <v>1</v>
       </c>
       <c r="C141" s="12" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D141" s="11"/>
     </row>
-    <row r="142" ht="26.25" spans="1:4">
-      <c r="A142" s="20"/>
-      <c r="B142" s="19">
+    <row r="142" spans="1:4">
+      <c r="A142" s="19"/>
+      <c r="B142" s="18">
         <v>1</v>
       </c>
       <c r="C142" s="12" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D142" s="11"/>
     </row>
     <row r="143" spans="1:4">
-      <c r="A143" s="20"/>
-      <c r="B143" s="19">
+      <c r="A143" s="19"/>
+      <c r="B143" s="18">
         <v>1</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D143" s="11"/>
     </row>
     <row r="144" spans="1:4">
-      <c r="A144" s="20"/>
-      <c r="B144" s="19">
+      <c r="A144" s="19"/>
+      <c r="B144" s="18">
         <v>1</v>
       </c>
       <c r="C144" s="12" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D144" s="11"/>
     </row>
-    <row r="145" spans="1:4">
-      <c r="A145" s="20"/>
-      <c r="B145" s="19">
+    <row r="145" ht="26.25" spans="1:4">
+      <c r="A145" s="19"/>
+      <c r="B145" s="18">
         <v>1</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D145" s="11"/>
     </row>
-    <row r="146" ht="26.25" spans="1:4">
-      <c r="A146" s="20"/>
-      <c r="B146" s="19">
-        <v>1</v>
+    <row r="146" ht="25.5" spans="1:4">
+      <c r="A146" s="19"/>
+      <c r="B146" s="18">
+        <v>5</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D146" s="11"/>
     </row>
-    <row r="147" ht="25.5" spans="1:4">
-      <c r="A147" s="20"/>
-      <c r="B147" s="19">
+    <row r="147" ht="92.25" spans="1:4">
+      <c r="A147" s="19"/>
+      <c r="B147" s="18">
         <v>5</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D147" s="11"/>
-    </row>
-    <row r="148" ht="92.25" spans="1:4">
-      <c r="A148" s="20"/>
-      <c r="B148" s="19">
+        <v>201</v>
+      </c>
+      <c r="D147" s="11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="148" ht="27" spans="1:4">
+      <c r="A148" s="19"/>
+      <c r="B148" s="18">
         <v>5</v>
       </c>
       <c r="C148" s="12" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D148" s="11" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="149" ht="27" spans="1:4">
-      <c r="A149" s="20"/>
-      <c r="B149" s="19">
-        <v>5</v>
-      </c>
-      <c r="C149" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="D149" s="11" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="150" ht="24" spans="1:4">
-      <c r="A150" s="20"/>
-      <c r="B150" s="19">
-        <v>1</v>
-      </c>
-      <c r="C150" s="22" t="s">
-        <v>203</v>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="149" ht="24" spans="1:4">
+      <c r="A149" s="19"/>
+      <c r="B149" s="18">
+        <v>1</v>
+      </c>
+      <c r="C149" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="D149" s="11"/>
+    </row>
+    <row r="150" ht="25.5" spans="1:4">
+      <c r="A150" s="19"/>
+      <c r="B150" s="18">
+        <v>1</v>
+      </c>
+      <c r="C150" s="12" t="s">
+        <v>206</v>
       </c>
       <c r="D150" s="11"/>
     </row>
     <row r="151" ht="25.5" spans="1:4">
-      <c r="A151" s="20"/>
-      <c r="B151" s="19">
-        <v>1</v>
+      <c r="A151" s="19"/>
+      <c r="B151" s="18">
+        <v>5</v>
       </c>
       <c r="C151" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="D151" s="11"/>
-    </row>
-    <row r="152" ht="25.5" spans="1:4">
-      <c r="A152" s="20"/>
-      <c r="B152" s="19">
-        <v>5</v>
-      </c>
-      <c r="C152" s="12" t="s">
-        <v>205</v>
+        <v>207</v>
+      </c>
+      <c r="D151" s="11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="152" ht="53.25" spans="1:4">
+      <c r="A152" s="19"/>
+      <c r="B152" s="18">
+        <v>5</v>
+      </c>
+      <c r="C152" s="22" t="s">
+        <v>209</v>
       </c>
       <c r="D152" s="11" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="153" ht="53.25" spans="1:4">
-      <c r="A153" s="20"/>
-      <c r="B153" s="19">
-        <v>5</v>
-      </c>
-      <c r="C153" s="23" t="s">
-        <v>207</v>
-      </c>
-      <c r="D153" s="11" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="154" ht="28.5" spans="1:4">
-      <c r="A154" s="20"/>
-      <c r="B154" s="19">
-        <v>2</v>
-      </c>
-      <c r="C154" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="D154" s="11"/>
-    </row>
-    <row r="155" ht="119.25" spans="1:4">
-      <c r="A155" s="24"/>
-      <c r="B155" s="19">
-        <v>5</v>
-      </c>
-      <c r="C155" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="D155" s="11" t="s">
+    </row>
+    <row r="153" ht="28.5" spans="1:4">
+      <c r="A153" s="19"/>
+      <c r="B153" s="18">
+        <v>2</v>
+      </c>
+      <c r="C153" s="22" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="156" ht="38.25" spans="1:4">
-      <c r="A156" s="12" t="s">
+      <c r="D153" s="11"/>
+    </row>
+    <row r="154" ht="119.25" spans="1:4">
+      <c r="A154" s="23"/>
+      <c r="B154" s="18">
+        <v>5</v>
+      </c>
+      <c r="C154" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="B156" s="25">
-        <v>1</v>
-      </c>
-      <c r="C156" s="26" t="s">
+      <c r="D154" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="D156" s="26"/>
-    </row>
-    <row r="157" ht="42" customHeight="1" spans="2:4">
-      <c r="B157" s="19">
-        <v>5</v>
+    </row>
+    <row r="155" ht="38.25" spans="1:4">
+      <c r="A155" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B155" s="24">
+        <v>1</v>
+      </c>
+      <c r="C155" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D155" s="25"/>
+    </row>
+    <row r="156" ht="42" customHeight="1" spans="2:4">
+      <c r="B156" s="18">
+        <v>5</v>
+      </c>
+      <c r="C156" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="D156" s="12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="157" ht="26.25" spans="1:4">
+      <c r="A157" s="12"/>
+      <c r="B157" s="26">
+        <v>1</v>
       </c>
       <c r="C157" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="D157" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="158" ht="26.25" spans="1:4">
+        <v>218</v>
+      </c>
+      <c r="D157" s="12"/>
+    </row>
+    <row r="158" spans="1:4">
       <c r="A158" s="12"/>
-      <c r="B158" s="27">
+      <c r="B158" s="26">
         <v>1</v>
       </c>
       <c r="C158" s="12" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D158" s="12"/>
     </row>
-    <row r="159" spans="1:4">
-      <c r="A159" s="12"/>
-      <c r="B159" s="27">
-        <v>1</v>
-      </c>
-      <c r="C159" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="D159" s="12"/>
-    </row>
-    <row r="160" ht="25.5" spans="1:3">
-      <c r="A160" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B160" s="1">
-        <v>1</v>
+    <row r="159" ht="25.5" spans="1:3">
+      <c r="A159" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B159" s="1">
+        <v>1</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="160" ht="146.25" spans="1:4">
+      <c r="A160" s="1"/>
+      <c r="B160" s="18">
+        <v>5</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="161" ht="146.25" spans="1:4">
+        <v>222</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="161" ht="39" spans="1:4">
       <c r="A161" s="1"/>
-      <c r="B161" s="19">
+      <c r="B161" s="18">
         <v>5</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="162" ht="39" spans="1:4">
-      <c r="A162" s="1"/>
-      <c r="B162" s="19">
-        <v>5</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D162" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3690,10 +3701,10 @@
     <mergeCell ref="A10:A17"/>
     <mergeCell ref="A18:A48"/>
     <mergeCell ref="A49:A90"/>
-    <mergeCell ref="A91:A155"/>
-    <mergeCell ref="A160:A162"/>
+    <mergeCell ref="A91:A154"/>
+    <mergeCell ref="A159:A161"/>
   </mergeCells>
-  <conditionalFormatting sqref="B1:B135 B139:B1048576">
+  <conditionalFormatting sqref="B$1:B$1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
add some papers whiching citing SCNN
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15120" windowHeight="12750"/>
+    <workbookView windowWidth="27720" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="231">
   <si>
     <t>Scope</t>
   </si>
@@ -111,6 +111,17 @@
     <t>feature engine</t>
   </si>
   <si>
+    <t>CBAM: Convolutional block attention module</t>
+  </si>
+  <si>
+    <t>提出了一个先channel-wise attention再spatial-wise attention的注意力模块，在分类和object detection上都取得了很好的效果；
+1. channel-wise attention: 在SE-net的基础上， 增加max-pooling feature: max-pooling gather distinctive object features to infer finer channel-wise attention
+2. spatial-wise attention: 也同时使用max-pool和avg-pool的feature, concat后的feature用7x7的卷积再卷一下</t>
+  </si>
+  <si>
+    <t>Deep Pyramidal Residual Networks</t>
+  </si>
+  <si>
     <t>understanding image representations by measuring their equivariance and equivalence</t>
   </si>
   <si>
@@ -578,6 +589,12 @@
 由于GCN主要提升的是object内部的分类效果，针对边界，提出了boundary refinement module</t>
   </si>
   <si>
+    <t>Pyramid Attention Network for Semantic Segmentation</t>
+  </si>
+  <si>
+    <t>GAU: 用高层级的feature作为低层级feature的attention; FPA: feature pyrimid attention, 对hight level feature的u-shape的attention</t>
+  </si>
+  <si>
     <t>learning a similarity mertric discriminatively, with application to face verification</t>
   </si>
   <si>
@@ -648,10 +665,19 @@
     <t>Multiple Encoder-Decoder net for Lane Detection</t>
   </si>
   <si>
-    <t>Exploring New Backbone and Attention Module for Semantic Segmentation in Street Scenes</t>
+    <t>参考文献很丰富:
+1. 对于backbone的思考：a. the feature in backbone should contain abundant spatial and semantic information; b. the backbone can impllement end-to-end framework without incresing the computation burdent too much
+2. special attention很有趣: channel方向取max, avg， 过卷积和sigmoid后形成H, W方向的attention</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Spatial-Temproal Based Lane Detection Using Deep Learning</t>
     </r>
     <r>
@@ -670,6 +696,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>deep neural network for structural prediction and lane detection in traffic scene</t>
     </r>
     <r>
@@ -782,9 +815,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
@@ -844,14 +877,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -859,9 +884,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -874,41 +899,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -919,13 +911,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -946,7 +931,61 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -959,30 +998,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1021,13 +1054,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1039,31 +1072,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1075,25 +1096,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1105,13 +1114,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1129,13 +1150,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1147,43 +1168,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1201,7 +1186,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1267,35 +1300,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1332,6 +1347,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1341,26 +1374,26 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1369,152 +1402,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1564,6 +1597,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1963,12 +1999,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G161"/>
+  <dimension ref="A1:G164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C145" sqref="C145"/>
+      <selection pane="bottomLeft" activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -2169,371 +2205,373 @@
       </c>
       <c r="D17" s="11"/>
     </row>
-    <row r="18" ht="25.5" spans="1:4">
-      <c r="A18" s="9" t="s">
+    <row r="18" ht="93" spans="1:4">
+      <c r="A18" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="16">
-        <v>1</v>
+      <c r="B18" s="10">
+        <v>5</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="11"/>
-    </row>
-    <row r="19" ht="27" spans="1:4">
-      <c r="A19" s="9"/>
-      <c r="B19" s="14">
-        <v>5</v>
+      <c r="D18" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="17"/>
+      <c r="B19" s="16">
+        <v>2</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" ht="37" customHeight="1" spans="1:4">
-      <c r="A20" s="9"/>
-      <c r="B20" s="10">
-        <v>5</v>
+      <c r="D19" s="11"/>
+    </row>
+    <row r="20" ht="25.5" spans="1:4">
+      <c r="A20" s="17"/>
+      <c r="B20" s="16">
+        <v>1</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" ht="27" spans="1:4">
+      <c r="A21" s="17"/>
+      <c r="B21" s="14">
+        <v>5</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="9"/>
-      <c r="B21" s="16">
-        <v>3</v>
-      </c>
-      <c r="C21" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="11"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="9"/>
-      <c r="B22" s="14">
+    </row>
+    <row r="22" ht="37" customHeight="1" spans="1:4">
+      <c r="A22" s="17"/>
+      <c r="B22" s="10">
         <v>5</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="11"/>
-    </row>
-    <row r="23" ht="27" spans="1:4">
-      <c r="A23" s="9"/>
-      <c r="B23" s="14">
-        <v>5</v>
+      <c r="D22" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="17"/>
+      <c r="B23" s="16">
+        <v>3</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" ht="25.5" spans="1:4">
-      <c r="A24" s="9"/>
-      <c r="B24" s="16">
-        <v>3</v>
-      </c>
-      <c r="C24" s="12" t="s">
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="17"/>
+      <c r="B24" s="14">
+        <v>5</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>38</v>
       </c>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" ht="25.5" spans="1:4">
-      <c r="A25" s="9"/>
-      <c r="B25" s="16">
-        <v>3</v>
-      </c>
-      <c r="C25" s="2" t="s">
+    <row r="25" ht="27" spans="1:4">
+      <c r="A25" s="17"/>
+      <c r="B25" s="14">
+        <v>5</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="11"/>
+      <c r="D25" s="11" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="26" ht="25.5" spans="1:4">
-      <c r="A26" s="9"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="16">
         <v>3</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>40</v>
+      <c r="C26" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="D26" s="11"/>
     </row>
     <row r="27" ht="25.5" spans="1:4">
-      <c r="A27" s="9"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="16">
         <v>3</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D27" s="11"/>
     </row>
-    <row r="28" ht="13.5" spans="1:4">
-      <c r="A28" s="9"/>
+    <row r="28" ht="25.5" spans="1:4">
+      <c r="A28" s="17"/>
       <c r="B28" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D28" s="11"/>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="9"/>
+    <row r="29" ht="25.5" spans="1:4">
+      <c r="A29" s="17"/>
       <c r="B29" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D29" s="11"/>
     </row>
-    <row r="30" ht="25.5" spans="1:4">
-      <c r="A30" s="9"/>
+    <row r="30" ht="13.5" spans="1:4">
+      <c r="A30" s="17"/>
       <c r="B30" s="16">
         <v>2</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D30" s="11"/>
     </row>
-    <row r="31" ht="79.5" spans="1:4">
-      <c r="A31" s="9"/>
-      <c r="B31" s="14">
-        <v>5</v>
+    <row r="31" spans="1:4">
+      <c r="A31" s="17"/>
+      <c r="B31" s="16">
+        <v>2</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="11" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="32" ht="27" spans="1:4">
-      <c r="A32" s="9"/>
-      <c r="B32" s="14">
-        <v>5</v>
+      <c r="D31" s="11"/>
+    </row>
+    <row r="32" ht="25.5" spans="1:4">
+      <c r="A32" s="17"/>
+      <c r="B32" s="16">
+        <v>2</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="11"/>
+    </row>
+    <row r="33" ht="79.5" spans="1:4">
+      <c r="A33" s="17"/>
+      <c r="B33" s="14">
+        <v>5</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="33" ht="25.5" spans="1:4">
-      <c r="A33" s="9"/>
-      <c r="B33" s="16">
-        <v>2</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="11"/>
-    </row>
-    <row r="34" ht="25.5" spans="1:4">
-      <c r="A34" s="9"/>
+    </row>
+    <row r="34" ht="27" spans="1:4">
+      <c r="A34" s="17"/>
       <c r="B34" s="14">
         <v>5</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="11"/>
+      <c r="D34" s="11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="35" ht="25.5" spans="1:4">
-      <c r="A35" s="9"/>
-      <c r="B35" s="14">
-        <v>5</v>
+      <c r="A35" s="17"/>
+      <c r="B35" s="16">
+        <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D35" s="11"/>
     </row>
-    <row r="36" ht="80.25" spans="1:4">
-      <c r="A36" s="9"/>
+    <row r="36" ht="25.5" spans="1:4">
+      <c r="A36" s="17"/>
       <c r="B36" s="14">
         <v>5</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D36" s="11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="37" ht="27" spans="1:4">
-      <c r="A37" s="9"/>
+      <c r="D36" s="11"/>
+    </row>
+    <row r="37" ht="25.5" spans="1:4">
+      <c r="A37" s="17"/>
       <c r="B37" s="14">
         <v>5</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="11"/>
+    </row>
+    <row r="38" ht="80.25" spans="1:4">
+      <c r="A38" s="17"/>
+      <c r="B38" s="14">
+        <v>5</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="9"/>
-      <c r="B38" s="16">
-        <v>2</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="D38" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="11"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="9"/>
-      <c r="B39" s="16">
-        <v>2</v>
-      </c>
-      <c r="C39" t="s">
+    </row>
+    <row r="39" ht="27" spans="1:4">
+      <c r="A39" s="17"/>
+      <c r="B39" s="14">
+        <v>5</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="11"/>
-    </row>
-    <row r="40" ht="39.75" spans="1:4">
-      <c r="A40" s="9"/>
-      <c r="B40" s="14">
-        <v>5</v>
-      </c>
-      <c r="C40" s="2" t="s">
+      <c r="D39" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D40" s="11" t="s">
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="17"/>
+      <c r="B40" s="16">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="41" ht="25.5" spans="1:4">
-      <c r="A41" s="9"/>
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="17"/>
       <c r="B41" s="16">
         <v>2</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" t="s">
         <v>60</v>
       </c>
       <c r="D41" s="11"/>
     </row>
-    <row r="42" ht="78.75" spans="1:4">
-      <c r="A42" s="9"/>
+    <row r="42" ht="39.75" spans="1:4">
+      <c r="A42" s="17"/>
       <c r="B42" s="14">
         <v>5</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="43" ht="27" spans="1:4">
-      <c r="A43" s="9"/>
-      <c r="B43" s="14">
-        <v>5</v>
-      </c>
-      <c r="C43" s="12" t="s">
+    <row r="43" ht="25.5" spans="1:4">
+      <c r="A43" s="17"/>
+      <c r="B43" s="16">
+        <v>2</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44" ht="78.75" spans="1:4">
+      <c r="A44" s="17"/>
+      <c r="B44" s="14">
+        <v>5</v>
+      </c>
+      <c r="C44" s="11" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="44" ht="25.5" spans="1:4">
-      <c r="A44" s="9"/>
-      <c r="B44" s="14">
-        <v>5</v>
-      </c>
-      <c r="C44" s="12" t="s">
+      <c r="D44" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D44" s="11"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="9"/>
+    </row>
+    <row r="45" ht="27" spans="1:4">
+      <c r="A45" s="17"/>
       <c r="B45" s="14">
         <v>5</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="11"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="9"/>
-      <c r="B46" s="16">
-        <v>2</v>
+      <c r="D45" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" ht="25.5" spans="1:4">
+      <c r="A46" s="17"/>
+      <c r="B46" s="14">
+        <v>5</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D46" s="11"/>
     </row>
-    <row r="47" ht="53" customHeight="1" spans="1:4">
-      <c r="A47" s="9"/>
+    <row r="47" spans="1:4">
+      <c r="A47" s="17"/>
       <c r="B47" s="14">
         <v>5</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D47" s="11" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="48" ht="41" customHeight="1" spans="1:4">
-      <c r="A48" s="9"/>
-      <c r="B48" s="14">
-        <v>5</v>
-      </c>
-      <c r="C48" s="2" t="s">
+      <c r="D47" s="11"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="17"/>
+      <c r="B48" s="16">
+        <v>2</v>
+      </c>
+      <c r="C48" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D48" s="11" t="s">
+      <c r="D48" s="11"/>
+    </row>
+    <row r="49" ht="53" customHeight="1" spans="1:4">
+      <c r="A49" s="17"/>
+      <c r="B49" s="14">
+        <v>5</v>
+      </c>
+      <c r="C49" s="12" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="49" ht="25.5" spans="1:4">
-      <c r="A49" s="9" t="s">
+      <c r="D49" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B49" s="14">
-        <v>2</v>
-      </c>
-      <c r="C49" s="2" t="s">
+    </row>
+    <row r="50" ht="41" customHeight="1" spans="1:4">
+      <c r="A50" s="17"/>
+      <c r="B50" s="14">
+        <v>5</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D49" s="11"/>
-    </row>
-    <row r="50" ht="25.5" spans="1:4">
-      <c r="A50" s="9"/>
-      <c r="B50" s="14">
-        <v>2</v>
-      </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D50" s="11"/>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="9"/>
+    </row>
+    <row r="51" ht="25.5" spans="1:4">
+      <c r="A51" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="B51" s="14">
         <v>2</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D51" s="11"/>
     </row>
@@ -2543,123 +2581,117 @@
         <v>2</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D52" s="11"/>
     </row>
-    <row r="53" ht="25.5" spans="1:4">
+    <row r="53" spans="1:4">
       <c r="A53" s="9"/>
       <c r="B53" s="14">
         <v>2</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D53" s="11"/>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" ht="25.5" spans="1:4">
       <c r="A54" s="9"/>
       <c r="B54" s="14">
-        <v>5</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>78</v>
+        <v>2</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="D54" s="11"/>
-      <c r="F54" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G54" s="17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
+    </row>
+    <row r="55" ht="25.5" spans="1:4">
       <c r="A55" s="9"/>
       <c r="B55" s="14">
         <v>2</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="2" t="s">
         <v>80</v>
       </c>
       <c r="D55" s="11"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-    </row>
-    <row r="56" ht="51.75" spans="1:7">
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="9"/>
-      <c r="B56" s="16">
-        <v>2</v>
+      <c r="B56" s="14">
+        <v>5</v>
       </c>
       <c r="C56" s="11" t="s">
         <v>81</v>
       </c>
       <c r="D56" s="11"/>
-      <c r="F56" s="1">
-        <v>0</v>
-      </c>
-      <c r="G56" t="s">
+      <c r="F56" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G56" s="18" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="57" ht="25.5" spans="1:7">
+    <row r="57" spans="1:7">
       <c r="A57" s="9"/>
-      <c r="B57" s="16">
-        <v>3</v>
+      <c r="B57" s="14">
+        <v>2</v>
       </c>
       <c r="C57" s="11" t="s">
         <v>83</v>
       </c>
       <c r="D57" s="11"/>
-      <c r="F57" s="1">
-        <v>1</v>
-      </c>
-      <c r="G57" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+    </row>
+    <row r="58" ht="51.75" spans="1:7">
       <c r="A58" s="9"/>
       <c r="B58" s="16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D58" s="11"/>
       <c r="F58" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G58" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" ht="25.5" spans="1:7">
       <c r="A59" s="9"/>
       <c r="B59" s="16">
         <v>3</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D59" s="11"/>
       <c r="F59" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G59" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="9"/>
       <c r="B60" s="16">
         <v>3</v>
       </c>
       <c r="C60" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" s="11"/>
+      <c r="F60" s="1">
+        <v>2</v>
+      </c>
+      <c r="G60" t="s">
         <v>89</v>
       </c>
-      <c r="D60" s="11"/>
-    </row>
-    <row r="61" ht="25.5" spans="1:4">
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="9"/>
       <c r="B61" s="16">
         <v>3</v>
@@ -2668,18 +2700,22 @@
         <v>90</v>
       </c>
       <c r="D61" s="11"/>
-    </row>
-    <row r="62" ht="40.5" spans="1:4">
+      <c r="F61" s="1">
+        <v>3</v>
+      </c>
+      <c r="G61" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="9"/>
-      <c r="B62" s="10">
-        <v>5</v>
+      <c r="B62" s="16">
+        <v>3</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D62" s="11" t="s">
         <v>92</v>
       </c>
+      <c r="D62" s="11"/>
     </row>
     <row r="63" ht="25.5" spans="1:4">
       <c r="A63" s="9"/>
@@ -2691,85 +2727,87 @@
       </c>
       <c r="D63" s="11"/>
     </row>
-    <row r="64" ht="25.5" spans="1:4">
+    <row r="64" ht="40.5" spans="1:4">
       <c r="A64" s="9"/>
-      <c r="B64" s="16">
-        <v>3</v>
+      <c r="B64" s="10">
+        <v>5</v>
       </c>
       <c r="C64" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D64" s="11"/>
-    </row>
-    <row r="65" ht="80.25" spans="1:4">
+      <c r="D64" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" ht="25.5" spans="1:4">
       <c r="A65" s="9"/>
-      <c r="B65" s="10">
-        <v>5</v>
+      <c r="B65" s="16">
+        <v>3</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D65" s="11" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="D65" s="11"/>
+    </row>
+    <row r="66" ht="25.5" spans="1:4">
       <c r="A66" s="9"/>
-      <c r="B66" s="10">
-        <v>2</v>
-      </c>
-      <c r="C66" s="12" t="s">
+      <c r="B66" s="16">
+        <v>3</v>
+      </c>
+      <c r="C66" s="11" t="s">
         <v>97</v>
       </c>
       <c r="D66" s="11"/>
     </row>
-    <row r="67" ht="25.5" spans="1:4">
+    <row r="67" ht="80.25" spans="1:4">
       <c r="A67" s="9"/>
-      <c r="B67" s="16">
-        <v>2</v>
-      </c>
-      <c r="C67" s="2" t="s">
+      <c r="B67" s="10">
+        <v>5</v>
+      </c>
+      <c r="C67" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D67" s="11"/>
-    </row>
-    <row r="68" ht="25.5" spans="1:4">
+      <c r="D67" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="9"/>
-      <c r="B68" s="16">
-        <v>2</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>99</v>
+      <c r="B68" s="10">
+        <v>2</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>100</v>
       </c>
       <c r="D68" s="11"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" ht="25.5" spans="1:4">
       <c r="A69" s="9"/>
       <c r="B69" s="16">
         <v>2</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D69" s="11"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" ht="25.5" spans="1:4">
       <c r="A70" s="9"/>
       <c r="B70" s="16">
         <v>2</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D70" s="11"/>
     </row>
-    <row r="71" ht="25.5" spans="1:4">
+    <row r="71" spans="1:4">
       <c r="A71" s="9"/>
       <c r="B71" s="16">
         <v>2</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D71" s="11"/>
     </row>
@@ -2779,7 +2817,7 @@
         <v>2</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D72" s="11"/>
     </row>
@@ -2789,17 +2827,17 @@
         <v>2</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D73" s="11"/>
     </row>
-    <row r="74" ht="25.5" spans="1:4">
+    <row r="74" spans="1:4">
       <c r="A74" s="9"/>
       <c r="B74" s="16">
         <v>2</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D74" s="11"/>
     </row>
@@ -2809,131 +2847,131 @@
         <v>2</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D75" s="11"/>
     </row>
-    <row r="76" ht="13.5" spans="1:4">
+    <row r="76" ht="25.5" spans="1:4">
       <c r="A76" s="9"/>
-      <c r="B76" s="18">
-        <v>5</v>
+      <c r="B76" s="16">
+        <v>2</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D76" s="11" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="77" ht="40.5" spans="1:4">
+      <c r="D76" s="11"/>
+    </row>
+    <row r="77" ht="25.5" spans="1:4">
       <c r="A77" s="9"/>
-      <c r="B77" s="10">
-        <v>5</v>
+      <c r="B77" s="16">
+        <v>2</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D77" s="11" t="s">
+      <c r="D77" s="11"/>
+    </row>
+    <row r="78" ht="13.5" spans="1:4">
+      <c r="A78" s="9"/>
+      <c r="B78" s="19">
+        <v>5</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="78" ht="25.5" spans="1:4">
-      <c r="A78" s="9"/>
-      <c r="B78" s="16">
-        <v>2</v>
-      </c>
-      <c r="C78" s="2" t="s">
+      <c r="D78" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D78" s="11"/>
-    </row>
-    <row r="79" spans="1:4">
+    </row>
+    <row r="79" ht="40.5" spans="1:4">
       <c r="A79" s="9"/>
       <c r="B79" s="10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D79" s="11"/>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="D79" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="80" ht="25.5" spans="1:4">
       <c r="A80" s="9"/>
-      <c r="B80" s="10">
+      <c r="B80" s="16">
         <v>2</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D80" s="11"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="9"/>
       <c r="B81" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D81" s="11"/>
     </row>
-    <row r="82" ht="25.5" spans="1:4">
+    <row r="82" spans="1:4">
       <c r="A82" s="9"/>
       <c r="B82" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D82" s="11"/>
     </row>
-    <row r="83" ht="25.5" spans="1:4">
+    <row r="83" spans="1:4">
       <c r="A83" s="9"/>
       <c r="B83" s="10">
         <v>1</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D83" s="11"/>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" ht="25.5" spans="1:4">
       <c r="A84" s="9"/>
       <c r="B84" s="10">
         <v>1</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D84" s="11"/>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" ht="25.5" spans="1:4">
       <c r="A85" s="9"/>
-      <c r="B85" s="16">
+      <c r="B85" s="10">
         <v>1</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D85" s="11"/>
     </row>
-    <row r="86" ht="25.5" spans="1:4">
+    <row r="86" spans="1:4">
       <c r="A86" s="9"/>
-      <c r="B86" s="16">
+      <c r="B86" s="10">
         <v>1</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D86" s="11"/>
     </row>
-    <row r="87" ht="25.5" spans="1:4">
+    <row r="87" spans="1:4">
       <c r="A87" s="9"/>
       <c r="B87" s="16">
         <v>1</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D87" s="11"/>
     </row>
@@ -2943,7 +2981,7 @@
         <v>1</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D88" s="11"/>
     </row>
@@ -2952,92 +2990,90 @@
       <c r="B89" s="16">
         <v>1</v>
       </c>
-      <c r="C89" s="11" t="s">
-        <v>122</v>
+      <c r="C89" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="D89" s="11"/>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" ht="25.5" spans="1:4">
       <c r="A90" s="9"/>
       <c r="B90" s="16">
         <v>1</v>
       </c>
-      <c r="C90" s="11" t="s">
-        <v>123</v>
+      <c r="C90" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="D90" s="11"/>
     </row>
     <row r="91" ht="25.5" spans="1:4">
-      <c r="A91" s="19" t="s">
-        <v>124</v>
-      </c>
+      <c r="A91" s="9"/>
       <c r="B91" s="16">
-        <v>2</v>
-      </c>
-      <c r="C91" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" s="11" t="s">
         <v>125</v>
       </c>
       <c r="D91" s="11"/>
     </row>
-    <row r="92" ht="39.75" spans="1:4">
-      <c r="A92" s="19"/>
-      <c r="B92" s="10">
-        <v>5</v>
+    <row r="92" spans="1:4">
+      <c r="A92" s="9"/>
+      <c r="B92" s="16">
+        <v>1</v>
       </c>
       <c r="C92" s="11" t="s">
         <v>126</v>
       </c>
       <c r="D92" s="11"/>
     </row>
-    <row r="93" ht="66" spans="1:4">
-      <c r="A93" s="19"/>
-      <c r="B93" s="10">
-        <v>6</v>
-      </c>
-      <c r="C93" s="11" t="s">
+    <row r="93" ht="25.5" spans="1:4">
+      <c r="A93" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="D93" s="11" t="s">
+      <c r="B93" s="16">
+        <v>2</v>
+      </c>
+      <c r="C93" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="94" ht="13.5" spans="1:4">
-      <c r="A94" s="19"/>
-      <c r="B94" s="18">
+      <c r="D93" s="11"/>
+    </row>
+    <row r="94" ht="39.75" spans="1:4">
+      <c r="A94" s="20"/>
+      <c r="B94" s="10">
         <v>5</v>
       </c>
       <c r="C94" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D94" s="11" t="s">
+      <c r="D94" s="11"/>
+    </row>
+    <row r="95" ht="66" spans="1:4">
+      <c r="A95" s="20"/>
+      <c r="B95" s="10">
+        <v>6</v>
+      </c>
+      <c r="C95" s="11" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="95" ht="27" spans="1:4">
-      <c r="A95" s="19"/>
-      <c r="B95" s="18">
-        <v>5</v>
-      </c>
-      <c r="C95" s="11" t="s">
+      <c r="D95" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="D95" s="11" t="s">
+    </row>
+    <row r="96" ht="13.5" spans="1:4">
+      <c r="A96" s="20"/>
+      <c r="B96" s="19">
+        <v>5</v>
+      </c>
+      <c r="C96" s="11" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="96" ht="25.5" spans="1:4">
-      <c r="A96" s="19"/>
-      <c r="B96" s="18">
-        <v>1</v>
-      </c>
-      <c r="C96" s="11" t="s">
+      <c r="D96" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="D96" s="11"/>
-    </row>
-    <row r="97" ht="93" spans="1:4">
-      <c r="A97" s="19"/>
-      <c r="B97" s="18">
+    </row>
+    <row r="97" ht="27" spans="1:4">
+      <c r="A97" s="20"/>
+      <c r="B97" s="19">
         <v>5</v>
       </c>
       <c r="C97" s="11" t="s">
@@ -3047,694 +3083,728 @@
         <v>135</v>
       </c>
     </row>
-    <row r="98" ht="93" spans="1:4">
-      <c r="A98" s="19"/>
-      <c r="B98" s="18">
-        <v>5</v>
+    <row r="98" ht="25.5" spans="1:4">
+      <c r="A98" s="20"/>
+      <c r="B98" s="19">
+        <v>1</v>
       </c>
       <c r="C98" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="D98" s="11" t="s">
+      <c r="D98" s="11"/>
+    </row>
+    <row r="99" ht="93" spans="1:4">
+      <c r="A99" s="20"/>
+      <c r="B99" s="19">
+        <v>5</v>
+      </c>
+      <c r="C99" s="11" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="99" ht="53.25" spans="1:4">
-      <c r="A99" s="19"/>
-      <c r="B99" s="18">
-        <v>5</v>
-      </c>
-      <c r="C99" s="11" t="s">
+      <c r="D99" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="D99" s="11" t="s">
+    </row>
+    <row r="100" ht="93" spans="1:4">
+      <c r="A100" s="20"/>
+      <c r="B100" s="19">
+        <v>5</v>
+      </c>
+      <c r="C100" s="11" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="100" ht="106.5" spans="1:4">
-      <c r="A100" s="19"/>
-      <c r="B100" s="18">
-        <v>5</v>
-      </c>
-      <c r="C100" s="11" t="s">
+      <c r="D100" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="D100" s="11" t="s">
+    </row>
+    <row r="101" ht="53.25" spans="1:4">
+      <c r="A101" s="20"/>
+      <c r="B101" s="19">
+        <v>5</v>
+      </c>
+      <c r="C101" s="11" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="19"/>
-      <c r="B101" s="18">
-        <v>5</v>
-      </c>
-      <c r="C101" s="11" t="s">
+      <c r="D101" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="D101" s="11"/>
-    </row>
-    <row r="102" ht="26.25" spans="1:4">
-      <c r="A102" s="19"/>
-      <c r="B102" s="18">
+    </row>
+    <row r="102" ht="106.5" spans="1:4">
+      <c r="A102" s="20"/>
+      <c r="B102" s="19">
         <v>5</v>
       </c>
       <c r="C102" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="D102" s="11"/>
-    </row>
-    <row r="103" ht="39.75" spans="1:4">
-      <c r="A103" s="19"/>
-      <c r="B103" s="18">
+      <c r="D102" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="20"/>
+      <c r="B103" s="19">
         <v>5</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="D103" s="11" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="104" ht="25.5" spans="1:4">
-      <c r="A104" s="19"/>
-      <c r="B104" s="18">
-        <v>2</v>
-      </c>
-      <c r="C104" s="12" t="s">
+      <c r="D103" s="11"/>
+    </row>
+    <row r="104" ht="26.25" spans="1:4">
+      <c r="A104" s="20"/>
+      <c r="B104" s="19">
+        <v>5</v>
+      </c>
+      <c r="C104" s="11" t="s">
         <v>146</v>
       </c>
       <c r="D104" s="11"/>
     </row>
-    <row r="105" ht="25.5" spans="1:4">
-      <c r="A105" s="19"/>
-      <c r="B105" s="18">
-        <v>2</v>
-      </c>
-      <c r="C105" s="12" t="s">
+    <row r="105" ht="39.75" spans="1:4">
+      <c r="A105" s="20"/>
+      <c r="B105" s="19">
+        <v>5</v>
+      </c>
+      <c r="C105" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="D105" s="11"/>
-    </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="19"/>
-      <c r="B106" s="18">
+      <c r="D105" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="106" ht="25.5" spans="1:4">
+      <c r="A106" s="20"/>
+      <c r="B106" s="19">
+        <v>2</v>
+      </c>
+      <c r="C106" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D106" s="11"/>
+    </row>
+    <row r="107" ht="25.5" spans="1:4">
+      <c r="A107" s="20"/>
+      <c r="B107" s="19">
+        <v>2</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D107" s="11"/>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="20"/>
+      <c r="B108" s="19">
         <v>1</v>
       </c>
-      <c r="C106" t="s">
-        <v>148</v>
-      </c>
-      <c r="D106" s="11"/>
-    </row>
-    <row r="107" ht="25.5" spans="1:4">
-      <c r="A107" s="19"/>
-      <c r="B107" s="18">
-        <v>2</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D107" s="11"/>
-    </row>
-    <row r="108" ht="25.5" spans="1:4">
-      <c r="A108" s="19"/>
-      <c r="B108" s="18">
-        <v>2</v>
-      </c>
-      <c r="C108" s="12" t="s">
-        <v>150</v>
+      <c r="C108" t="s">
+        <v>151</v>
       </c>
       <c r="D108" s="11"/>
     </row>
-    <row r="109" spans="1:4">
-      <c r="A109" s="19"/>
-      <c r="B109" s="18">
-        <v>2</v>
-      </c>
-      <c r="C109" s="12" t="s">
-        <v>151</v>
+    <row r="109" ht="25.5" spans="1:4">
+      <c r="A109" s="20"/>
+      <c r="B109" s="19">
+        <v>2</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="D109" s="11"/>
     </row>
     <row r="110" ht="25.5" spans="1:4">
-      <c r="A110" s="19"/>
-      <c r="B110" s="18">
+      <c r="A110" s="20"/>
+      <c r="B110" s="19">
         <v>2</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D110" s="11"/>
     </row>
-    <row r="111" ht="25.5" spans="1:4">
-      <c r="A111" s="19"/>
-      <c r="B111" s="18">
-        <v>5</v>
+    <row r="111" spans="1:4">
+      <c r="A111" s="20"/>
+      <c r="B111" s="19">
+        <v>2</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="D111" s="11" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="112" ht="39.75" spans="1:4">
-      <c r="A112" s="19"/>
-      <c r="B112" s="18">
-        <v>5</v>
+      <c r="D111" s="11"/>
+    </row>
+    <row r="112" ht="25.5" spans="1:4">
+      <c r="A112" s="20"/>
+      <c r="B112" s="19">
+        <v>2</v>
       </c>
       <c r="C112" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="D112" s="11" t="s">
+      <c r="D112" s="11"/>
+    </row>
+    <row r="113" ht="25.5" spans="1:4">
+      <c r="A113" s="20"/>
+      <c r="B113" s="19">
+        <v>5</v>
+      </c>
+      <c r="C113" s="12" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="113" ht="156.75" spans="1:4">
-      <c r="A113" s="19"/>
-      <c r="B113" s="18">
-        <v>5</v>
-      </c>
-      <c r="C113" s="12" t="s">
+      <c r="D113" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="D113" s="11" t="s">
+    </row>
+    <row r="114" ht="39.75" spans="1:4">
+      <c r="A114" s="20"/>
+      <c r="B114" s="19">
+        <v>5</v>
+      </c>
+      <c r="C114" s="12" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="114" ht="27" spans="1:4">
-      <c r="A114" s="19"/>
-      <c r="B114" s="18">
-        <v>5</v>
-      </c>
-      <c r="C114" s="12" t="s">
+      <c r="D114" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="D114" s="11" t="s">
+    </row>
+    <row r="115" ht="156.75" spans="1:4">
+      <c r="A115" s="20"/>
+      <c r="B115" s="19">
+        <v>5</v>
+      </c>
+      <c r="C115" s="12" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="115" ht="54" spans="1:4">
-      <c r="A115" s="19"/>
-      <c r="B115" s="18">
-        <v>5</v>
-      </c>
-      <c r="C115" s="12" t="s">
+      <c r="D115" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="D115" s="11" t="s">
+    </row>
+    <row r="116" ht="27" spans="1:4">
+      <c r="A116" s="20"/>
+      <c r="B116" s="19">
+        <v>5</v>
+      </c>
+      <c r="C116" s="12" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="116" ht="54" spans="1:4">
-      <c r="A116" s="19"/>
-      <c r="B116" s="18">
-        <v>5</v>
-      </c>
-      <c r="C116" s="12" t="s">
+      <c r="D116" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="D116" s="11" t="s">
+    </row>
+    <row r="117" ht="54" spans="1:4">
+      <c r="A117" s="20"/>
+      <c r="B117" s="19">
+        <v>5</v>
+      </c>
+      <c r="C117" s="12" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="117" ht="25.5" spans="1:4">
-      <c r="A117" s="19"/>
-      <c r="B117" s="20">
-        <v>2</v>
-      </c>
-      <c r="C117" s="12" t="s">
+      <c r="D117" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="D117" s="11"/>
-    </row>
-    <row r="118" ht="25.5" spans="1:4">
-      <c r="A118" s="19"/>
-      <c r="B118" s="18">
-        <v>1</v>
+    </row>
+    <row r="118" ht="54" spans="1:4">
+      <c r="A118" s="20"/>
+      <c r="B118" s="19">
+        <v>5</v>
       </c>
       <c r="C118" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="D118" s="11"/>
+      <c r="D118" s="11" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="119" ht="25.5" spans="1:4">
-      <c r="A119" s="19"/>
-      <c r="B119" s="18">
+      <c r="A119" s="20"/>
+      <c r="B119" s="21">
+        <v>2</v>
+      </c>
+      <c r="C119" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="D119" s="11"/>
+    </row>
+    <row r="120" ht="25.5" spans="1:4">
+      <c r="A120" s="20"/>
+      <c r="B120" s="19">
         <v>1</v>
       </c>
-      <c r="C119" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="D119" s="11"/>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="A120" s="19"/>
-      <c r="B120" s="18">
-        <v>2</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>168</v>
+      <c r="C120" s="12" t="s">
+        <v>169</v>
       </c>
       <c r="D120" s="11"/>
     </row>
     <row r="121" ht="25.5" spans="1:4">
-      <c r="A121" s="19"/>
-      <c r="B121" s="18">
-        <v>2</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>169</v>
+      <c r="A121" s="20"/>
+      <c r="B121" s="19">
+        <v>1</v>
+      </c>
+      <c r="C121" s="12" t="s">
+        <v>170</v>
       </c>
       <c r="D121" s="11"/>
     </row>
-    <row r="122" ht="54" spans="1:4">
-      <c r="A122" s="19"/>
-      <c r="B122" s="18">
-        <v>5</v>
+    <row r="122" spans="1:4">
+      <c r="A122" s="20"/>
+      <c r="B122" s="19">
+        <v>2</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D122" s="11" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="123" ht="66.75" spans="1:4">
-      <c r="A123" s="19"/>
-      <c r="B123" s="18">
-        <v>5</v>
+      <c r="D122" s="11"/>
+    </row>
+    <row r="123" ht="25.5" spans="1:4">
+      <c r="A123" s="20"/>
+      <c r="B123" s="19">
+        <v>2</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D123" s="11" t="s">
+      <c r="D123" s="11"/>
+    </row>
+    <row r="124" ht="54" spans="1:4">
+      <c r="A124" s="20"/>
+      <c r="B124" s="19">
+        <v>5</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="124" ht="25.5" spans="1:4">
-      <c r="A124" s="19"/>
-      <c r="B124" s="18">
-        <v>1</v>
-      </c>
-      <c r="C124" s="2" t="s">
+      <c r="D124" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="D124" s="11"/>
-    </row>
-    <row r="125" spans="1:4">
-      <c r="A125" s="19"/>
-      <c r="B125" s="18">
-        <v>2</v>
+    </row>
+    <row r="125" ht="66.75" spans="1:4">
+      <c r="A125" s="20"/>
+      <c r="B125" s="19">
+        <v>5</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D125" s="11"/>
-    </row>
-    <row r="126" ht="25.5" spans="1:4">
-      <c r="A126" s="19"/>
-      <c r="B126" s="18">
+      <c r="D125" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="126" ht="27" spans="1:4">
+      <c r="A126" s="20"/>
+      <c r="B126" s="19">
+        <v>5</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D126" s="11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="127" ht="25.5" spans="1:4">
+      <c r="A127" s="20"/>
+      <c r="B127" s="19">
         <v>1</v>
       </c>
-      <c r="C126" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D126" s="11"/>
-    </row>
-    <row r="127" spans="1:4">
-      <c r="A127" s="19"/>
-      <c r="B127" s="18">
-        <v>2</v>
-      </c>
       <c r="C127" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D127" s="11"/>
     </row>
-    <row r="128" ht="25.5" spans="1:4">
-      <c r="A128" s="19"/>
-      <c r="B128" s="18">
+    <row r="128" spans="1:4">
+      <c r="A128" s="20"/>
+      <c r="B128" s="19">
         <v>2</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D128" s="11"/>
     </row>
-    <row r="129" ht="108" spans="1:4">
-      <c r="A129" s="19"/>
-      <c r="B129" s="18">
-        <v>5</v>
+    <row r="129" ht="25.5" spans="1:4">
+      <c r="A129" s="20"/>
+      <c r="B129" s="19">
+        <v>1</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D129" s="11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="130" ht="66.75" spans="1:4">
-      <c r="A130" s="19"/>
-      <c r="B130" s="18">
-        <v>5</v>
+        <v>181</v>
+      </c>
+      <c r="D129" s="11"/>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="20"/>
+      <c r="B130" s="19">
+        <v>2</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D130" s="11" t="s">
         <v>182</v>
       </c>
+      <c r="D130" s="11"/>
     </row>
     <row r="131" ht="25.5" spans="1:4">
-      <c r="A131" s="19"/>
-      <c r="B131" s="18">
-        <v>1</v>
+      <c r="A131" s="20"/>
+      <c r="B131" s="19">
+        <v>2</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>183</v>
       </c>
       <c r="D131" s="11"/>
     </row>
-    <row r="132" ht="38.25" spans="1:4">
-      <c r="A132" s="19"/>
-      <c r="B132" s="18">
-        <v>1</v>
+    <row r="132" ht="108" spans="1:4">
+      <c r="A132" s="20"/>
+      <c r="B132" s="19">
+        <v>5</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D132" s="11"/>
-    </row>
-    <row r="133" ht="25.5" spans="1:4">
-      <c r="A133" s="19"/>
-      <c r="B133" s="18">
+      <c r="D132" s="11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="133" ht="66.75" spans="1:4">
+      <c r="A133" s="20"/>
+      <c r="B133" s="19">
+        <v>5</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D133" s="11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="134" ht="25.5" spans="1:4">
+      <c r="A134" s="20"/>
+      <c r="B134" s="19">
         <v>1</v>
       </c>
-      <c r="C133" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D133" s="11"/>
-    </row>
-    <row r="134" ht="26.25" spans="1:4">
-      <c r="A134" s="19"/>
-      <c r="B134" s="18">
+      <c r="C134" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D134" s="11"/>
+    </row>
+    <row r="135" ht="38.25" spans="1:4">
+      <c r="A135" s="20"/>
+      <c r="B135" s="19">
         <v>1</v>
       </c>
-      <c r="C134" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="D134" s="11"/>
-    </row>
-    <row r="135" spans="1:4">
-      <c r="A135" s="19"/>
-      <c r="B135" s="18">
+      <c r="C135" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D135" s="11"/>
+    </row>
+    <row r="136" ht="25.5" spans="1:4">
+      <c r="A136" s="20"/>
+      <c r="B136" s="19">
         <v>1</v>
       </c>
-      <c r="C135" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="D135" s="11"/>
-    </row>
-    <row r="136" ht="66.75" spans="1:4">
-      <c r="A136" s="19"/>
-      <c r="B136" s="18">
-        <v>5</v>
-      </c>
-      <c r="C136" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="D136" s="11" t="s">
-        <v>189</v>
-      </c>
+      <c r="C136" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D136" s="11"/>
     </row>
     <row r="137" ht="26.25" spans="1:4">
-      <c r="A137" s="19"/>
-      <c r="B137" s="18">
+      <c r="A137" s="20"/>
+      <c r="B137" s="19">
         <v>1</v>
       </c>
       <c r="C137" s="12" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D137" s="11"/>
     </row>
-    <row r="138" ht="66.75" spans="1:4">
-      <c r="A138" s="19"/>
-      <c r="B138" s="18">
-        <v>5</v>
+    <row r="138" spans="1:4">
+      <c r="A138" s="20"/>
+      <c r="B138" s="19">
+        <v>1</v>
       </c>
       <c r="C138" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="D138" s="11" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="139" ht="25.5" spans="1:4">
-      <c r="A139" s="19"/>
-      <c r="B139" s="18">
-        <v>1</v>
+      <c r="D138" s="11"/>
+    </row>
+    <row r="139" ht="66.75" spans="1:4">
+      <c r="A139" s="20"/>
+      <c r="B139" s="19">
+        <v>5</v>
       </c>
       <c r="C139" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="D139" s="21"/>
-    </row>
-    <row r="140" spans="1:4">
-      <c r="A140" s="19"/>
-      <c r="B140" s="18">
+      <c r="D139" s="11" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="140" ht="26.25" spans="1:4">
+      <c r="A140" s="20"/>
+      <c r="B140" s="19">
         <v>1</v>
       </c>
       <c r="C140" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D140" s="21"/>
-    </row>
-    <row r="141" ht="25.5" spans="1:4">
-      <c r="A141" s="19"/>
-      <c r="B141" s="18">
+        <v>195</v>
+      </c>
+      <c r="D140" s="11"/>
+    </row>
+    <row r="141" ht="66.75" spans="1:4">
+      <c r="A141" s="20"/>
+      <c r="B141" s="19">
+        <v>5</v>
+      </c>
+      <c r="C141" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D141" s="11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="142" ht="25.5" spans="1:4">
+      <c r="A142" s="20"/>
+      <c r="B142" s="19">
         <v>1</v>
       </c>
-      <c r="C141" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="D141" s="21"/>
-    </row>
-    <row r="142" ht="26.25" spans="1:4">
-      <c r="A142" s="19"/>
-      <c r="B142" s="18">
+      <c r="C142" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="D142" s="22"/>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="20"/>
+      <c r="B143" s="19">
         <v>1</v>
       </c>
-      <c r="C142" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="D142" s="21"/>
-    </row>
-    <row r="143" spans="1:4">
-      <c r="A143" s="19"/>
-      <c r="B143" s="18">
+      <c r="C143" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D143" s="22"/>
+    </row>
+    <row r="144" ht="91.5" spans="1:4">
+      <c r="A144" s="20"/>
+      <c r="B144" s="19">
+        <v>5</v>
+      </c>
+      <c r="C144" s="12"/>
+      <c r="D144" s="22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="145" ht="26.25" spans="1:4">
+      <c r="A145" s="20"/>
+      <c r="B145" s="19">
         <v>1</v>
       </c>
-      <c r="C143" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="D143" s="21"/>
-    </row>
-    <row r="144" ht="39.75" spans="1:4">
-      <c r="A144" s="19"/>
-      <c r="B144" s="18">
+      <c r="C145" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="D145" s="22"/>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="20"/>
+      <c r="B146" s="19">
         <v>1</v>
       </c>
-      <c r="C144" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="D144" s="21"/>
-    </row>
-    <row r="145" ht="25.5" spans="1:4">
-      <c r="A145" s="19"/>
-      <c r="B145" s="18">
+      <c r="C146" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="D146" s="22"/>
+    </row>
+    <row r="147" ht="39.75" spans="1:4">
+      <c r="A147" s="20"/>
+      <c r="B147" s="19">
         <v>1</v>
       </c>
-      <c r="C145" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="D145" s="21"/>
-    </row>
-    <row r="146" ht="25.5" spans="1:4">
-      <c r="A146" s="19"/>
-      <c r="B146" s="18">
-        <v>5</v>
-      </c>
-      <c r="C146" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="D146" s="21"/>
-    </row>
-    <row r="147" ht="92.25" spans="1:4">
-      <c r="A147" s="19"/>
-      <c r="B147" s="18">
-        <v>5</v>
-      </c>
-      <c r="C147" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="D147" s="21" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="148" ht="27" spans="1:4">
-      <c r="A148" s="19"/>
-      <c r="B148" s="18">
-        <v>5</v>
-      </c>
-      <c r="C148" s="12" t="s">
+      <c r="C147" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="D148" s="21" t="s">
+      <c r="D147" s="22"/>
+    </row>
+    <row r="148" ht="25.5" spans="1:4">
+      <c r="A148" s="20"/>
+      <c r="B148" s="19">
+        <v>1</v>
+      </c>
+      <c r="C148" s="23" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="149" ht="24" spans="1:4">
-      <c r="A149" s="19"/>
-      <c r="B149" s="18">
-        <v>1</v>
-      </c>
-      <c r="C149" s="23" t="s">
+      <c r="D148" s="22"/>
+    </row>
+    <row r="149" ht="25.5" spans="1:4">
+      <c r="A149" s="20"/>
+      <c r="B149" s="19">
+        <v>5</v>
+      </c>
+      <c r="C149" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="D149" s="21"/>
-    </row>
-    <row r="150" ht="25.5" spans="1:4">
-      <c r="A150" s="19"/>
-      <c r="B150" s="18">
-        <v>1</v>
+      <c r="D149" s="22"/>
+    </row>
+    <row r="150" ht="92.25" spans="1:4">
+      <c r="A150" s="20"/>
+      <c r="B150" s="19">
+        <v>5</v>
       </c>
       <c r="C150" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="D150" s="21"/>
-    </row>
-    <row r="151" ht="25.5" spans="1:4">
-      <c r="A151" s="19"/>
-      <c r="B151" s="18">
+      <c r="D150" s="22" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="151" ht="27" spans="1:4">
+      <c r="A151" s="20"/>
+      <c r="B151" s="19">
         <v>5</v>
       </c>
       <c r="C151" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="D151" s="11" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="152" ht="53.25" spans="1:4">
-      <c r="A152" s="19"/>
-      <c r="B152" s="18">
-        <v>5</v>
+      <c r="D151" s="22" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="152" ht="24" spans="1:4">
+      <c r="A152" s="20"/>
+      <c r="B152" s="19">
+        <v>1</v>
       </c>
       <c r="C152" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="D152" s="11" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="153" ht="28.5" spans="1:4">
-      <c r="A153" s="19"/>
-      <c r="B153" s="18">
-        <v>2</v>
-      </c>
-      <c r="C153" s="24" t="s">
+      <c r="D152" s="22"/>
+    </row>
+    <row r="153" ht="25.5" spans="1:4">
+      <c r="A153" s="20"/>
+      <c r="B153" s="19">
+        <v>1</v>
+      </c>
+      <c r="C153" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="D153" s="11"/>
-    </row>
-    <row r="154" ht="119.25" spans="1:4">
-      <c r="A154" s="25"/>
-      <c r="B154" s="18">
-        <v>5</v>
-      </c>
-      <c r="C154" s="11" t="s">
+      <c r="D153" s="22"/>
+    </row>
+    <row r="154" ht="25.5" spans="1:4">
+      <c r="A154" s="20"/>
+      <c r="B154" s="19">
+        <v>5</v>
+      </c>
+      <c r="C154" s="12" t="s">
         <v>212</v>
       </c>
       <c r="D154" s="11" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="155" ht="38.25" spans="1:4">
-      <c r="A155" s="12" t="s">
+    <row r="155" ht="53.25" spans="1:4">
+      <c r="A155" s="20"/>
+      <c r="B155" s="19">
+        <v>5</v>
+      </c>
+      <c r="C155" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="B155" s="26">
+      <c r="D155" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="156" ht="28.5" spans="1:4">
+      <c r="A156" s="20"/>
+      <c r="B156" s="19">
+        <v>2</v>
+      </c>
+      <c r="C156" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="D156" s="11"/>
+    </row>
+    <row r="157" ht="119.25" spans="1:4">
+      <c r="A157" s="26"/>
+      <c r="B157" s="19">
+        <v>5</v>
+      </c>
+      <c r="C157" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="D157" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="158" ht="38.25" spans="1:4">
+      <c r="A158" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B158" s="27">
         <v>1</v>
       </c>
-      <c r="C155" s="27" t="s">
-        <v>215</v>
-      </c>
-      <c r="D155" s="27"/>
-    </row>
-    <row r="156" ht="42" customHeight="1" spans="2:4">
-      <c r="B156" s="18">
-        <v>5</v>
-      </c>
-      <c r="C156" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="D156" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="157" ht="26.25" spans="1:4">
-      <c r="A157" s="12"/>
-      <c r="B157" s="28">
+      <c r="C158" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="D158" s="28"/>
+    </row>
+    <row r="159" ht="42" customHeight="1" spans="2:4">
+      <c r="B159" s="19">
+        <v>5</v>
+      </c>
+      <c r="C159" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D159" s="12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="160" ht="26.25" spans="1:4">
+      <c r="A160" s="12"/>
+      <c r="B160" s="29">
         <v>1</v>
       </c>
-      <c r="C157" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="D157" s="12"/>
-    </row>
-    <row r="158" spans="1:4">
-      <c r="A158" s="12"/>
-      <c r="B158" s="28">
+      <c r="C160" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="D160" s="12"/>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" s="12"/>
+      <c r="B161" s="29">
         <v>1</v>
       </c>
-      <c r="C158" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="D158" s="12"/>
-    </row>
-    <row r="159" ht="25.5" spans="1:3">
-      <c r="A159" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B159" s="1">
+      <c r="C161" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="D161" s="12"/>
+    </row>
+    <row r="162" ht="25.5" spans="1:3">
+      <c r="A162" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B162" s="1">
         <v>1</v>
       </c>
-      <c r="C159" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="160" ht="146.25" spans="1:4">
-      <c r="A160" s="1"/>
-      <c r="B160" s="18">
-        <v>5</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D160" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="161" ht="39" spans="1:4">
-      <c r="A161" s="1"/>
-      <c r="B161" s="18">
-        <v>5</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D161" s="2" t="s">
-        <v>225</v>
+      <c r="C162" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="163" ht="146.25" spans="1:4">
+      <c r="A163" s="1"/>
+      <c r="B163" s="19">
+        <v>5</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="164" ht="39" spans="1:4">
+      <c r="A164" s="1"/>
+      <c r="B164" s="19">
+        <v>5</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3742,10 +3812,10 @@
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A17"/>
-    <mergeCell ref="A18:A48"/>
-    <mergeCell ref="A49:A90"/>
-    <mergeCell ref="A91:A154"/>
-    <mergeCell ref="A159:A161"/>
+    <mergeCell ref="A18:A50"/>
+    <mergeCell ref="A51:A92"/>
+    <mergeCell ref="A93:A157"/>
+    <mergeCell ref="A162:A164"/>
   </mergeCells>
   <conditionalFormatting sqref="B$1:B$1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
@@ -3759,7 +3829,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C120" r:id="rId1" display="Panoptic Segmentation" tooltip="https://arxiv.org/abs/1801.00868"/>
+    <hyperlink ref="C122" r:id="rId1" display="Panoptic Segmentation" tooltip="https://arxiv.org/abs/1801.00868"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
add some papers for multi task learning
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="13170"/>
+    <workbookView windowWidth="15120" windowHeight="25770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="238">
   <si>
     <t>Scope</t>
   </si>
@@ -128,7 +128,8 @@
     <t>What Uncertainties Do We Need in Bayesian Deep Learning for Computer Vision</t>
   </si>
   <si>
-    <t>understanding image representations by measuring their equivariance and equivalence</t>
+    <t>understanding image representations by measuring their equivariance and equivalence
+可以配合他的博士论文阅读：Geometry and Uncertainty in Deep Learning for Computer Vision</t>
   </si>
   <si>
     <t>Frequency principle: Fourier analysis sheds light on deep nerual networks</t>
@@ -766,16 +767,19 @@
 到底如何共享backbone是需要尝试的</t>
   </si>
   <si>
+    <t xml:space="preserve"> Auxiliary Tasks in Multi-task Learning</t>
+  </si>
+  <si>
+    <t>Real-time Joint Object Detection and Semantic Segmentation Network for Automated Driving</t>
+  </si>
+  <si>
+    <t>NeurALL_Towards a Unified Model for Visual Perception in Automated Driving</t>
+  </si>
+  <si>
     <t>Multinet: Realtime joint semantic reasoning for autonomous driving（检测， 语意分割融合的多任务模型）</t>
   </si>
   <si>
     <t>Fast Scene Understanding for Autonomous Driving</t>
-  </si>
-  <si>
-    <t>Lane detection</t>
-  </si>
-  <si>
-    <t>a learning-based approach for lane Departure warning systems with a personalied driver model</t>
   </si>
   <si>
     <t>[综述, 2010]Recent progress in road and lane detection_a survey</t>
@@ -800,10 +804,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -855,14 +859,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -870,16 +866,48 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -894,7 +922,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -915,8 +950,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -924,45 +960,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -976,16 +974,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -996,6 +986,20 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1032,7 +1036,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1044,25 +1108,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1074,19 +1186,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1098,121 +1216,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1278,6 +1282,39 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1289,6 +1326,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1308,41 +1360,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1355,173 +1379,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1971,12 +1975,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G166"/>
+  <dimension ref="A1:G168"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C162" sqref="C162"/>
+      <selection pane="bottomLeft" activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -2221,7 +2225,7 @@
       </c>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" ht="25.5" spans="1:4">
+    <row r="22" ht="51.75" spans="1:4">
       <c r="A22" s="9"/>
       <c r="B22" s="16">
         <v>1</v>
@@ -3752,8 +3756,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="162" ht="26.25" spans="1:4">
-      <c r="A162" s="12"/>
+    <row r="162" ht="42" customHeight="1" spans="2:4">
       <c r="B162" s="27">
         <v>1</v>
       </c>
@@ -3762,8 +3765,7 @@
       </c>
       <c r="D162" s="12"/>
     </row>
-    <row r="163" spans="1:4">
-      <c r="A163" s="12"/>
+    <row r="163" ht="42" customHeight="1" spans="2:4">
       <c r="B163" s="27">
         <v>1</v>
       </c>
@@ -3772,39 +3774,57 @@
       </c>
       <c r="D163" s="12"/>
     </row>
-    <row r="164" ht="25.5" spans="1:3">
-      <c r="A164" s="1" t="s">
+    <row r="164" ht="42" customHeight="1" spans="2:4">
+      <c r="B164" s="27">
+        <v>1</v>
+      </c>
+      <c r="C164" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="B164" s="1">
-        <v>1</v>
-      </c>
-      <c r="C164" s="2" t="s">
+      <c r="D164" s="12"/>
+    </row>
+    <row r="165" ht="26.25" spans="1:4">
+      <c r="A165" s="12"/>
+      <c r="B165" s="27">
+        <v>1</v>
+      </c>
+      <c r="C165" s="12" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="165" ht="146.25" spans="1:4">
-      <c r="A165" s="1"/>
-      <c r="B165" s="18">
-        <v>5</v>
-      </c>
-      <c r="C165" s="2" t="s">
+      <c r="D165" s="12"/>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" s="12"/>
+      <c r="B166" s="27">
+        <v>2</v>
+      </c>
+      <c r="C166" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="D165" s="2" t="s">
+      <c r="D166" s="12"/>
+    </row>
+    <row r="167" ht="146.25" spans="1:4">
+      <c r="A167" s="1"/>
+      <c r="B167" s="18">
+        <v>5</v>
+      </c>
+      <c r="C167" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="166" ht="39" spans="1:4">
-      <c r="A166" s="1"/>
-      <c r="B166" s="18">
-        <v>5</v>
-      </c>
-      <c r="C166" s="2" t="s">
+      <c r="D167" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="D166" s="2" t="s">
+    </row>
+    <row r="168" ht="39" spans="1:4">
+      <c r="A168" s="1"/>
+      <c r="B168" s="18">
+        <v>5</v>
+      </c>
+      <c r="C168" s="2" t="s">
         <v>236</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -3815,7 +3835,7 @@
     <mergeCell ref="A18:A52"/>
     <mergeCell ref="A53:A94"/>
     <mergeCell ref="A95:A159"/>
-    <mergeCell ref="A164:A166"/>
+    <mergeCell ref="A167:A168"/>
   </mergeCells>
   <conditionalFormatting sqref="B$1:B$1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
add reading note for yolo
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15120" windowHeight="25770"/>
+    <workbookView windowWidth="27720" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="239">
   <si>
     <t>Scope</t>
   </si>
@@ -298,6 +298,11 @@
     <t>1. You Only Look Once: Unified, Real-Time Object Detection
 2. YOLO9000: better, faster, stronger
 3. Yolov3：An Incremental Improvement</t>
+  </si>
+  <si>
+    <t>v1: 不用anchor， 直接预测bbox的长度和宽度， 缺点是localization错误高，对小物体检测不好
+v2: 加了anchor(easier to learn)， anchor的尺寸通过聚类的出来， 最后用WordTree分9000类
+v3: muilti level feature， darknet-53</t>
   </si>
   <si>
     <t>立刻，马上，重要而紧急</t>
@@ -805,9 +810,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -859,8 +864,70 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -881,63 +948,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -945,14 +957,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -966,8 +970,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -982,22 +1001,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1036,7 +1041,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1048,7 +1053,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1060,7 +1089,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1072,31 +1203,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1108,115 +1215,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1282,35 +1287,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1330,32 +1326,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1374,8 +1355,32 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1384,148 +1389,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1978,9 +1983,9 @@
   <dimension ref="A1:G168"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C159" sqref="C159"/>
+      <selection pane="bottomLeft" activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -2641,20 +2646,22 @@
       <c r="F59" s="17"/>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" ht="51.75" spans="1:7">
+    <row r="60" ht="67.5" spans="1:7">
       <c r="A60" s="9"/>
-      <c r="B60" s="16">
-        <v>2</v>
+      <c r="B60" s="14">
+        <v>5</v>
       </c>
       <c r="C60" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D60" s="11"/>
+      <c r="D60" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="F60" s="1">
         <v>0</v>
       </c>
       <c r="G60" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" ht="25.5" spans="1:7">
@@ -2663,14 +2670,14 @@
         <v>3</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D61" s="11"/>
       <c r="F61" s="1">
         <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -2679,14 +2686,14 @@
         <v>3</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D62" s="11"/>
       <c r="F62" s="1">
         <v>2</v>
       </c>
       <c r="G62" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2695,14 +2702,14 @@
         <v>3</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D63" s="11"/>
       <c r="F63" s="1">
         <v>3</v>
       </c>
       <c r="G63" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2711,7 +2718,7 @@
         <v>3</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D64" s="11"/>
     </row>
@@ -2721,7 +2728,7 @@
         <v>3</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D65" s="11"/>
     </row>
@@ -2731,10 +2738,10 @@
         <v>5</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" ht="25.5" spans="1:4">
@@ -2743,7 +2750,7 @@
         <v>3</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D67" s="11"/>
     </row>
@@ -2753,7 +2760,7 @@
         <v>3</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D68" s="11"/>
     </row>
@@ -2763,10 +2770,10 @@
         <v>5</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2775,7 +2782,7 @@
         <v>2</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D70" s="11"/>
     </row>
@@ -2785,7 +2792,7 @@
         <v>2</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D71" s="11"/>
     </row>
@@ -2795,7 +2802,7 @@
         <v>2</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D72" s="11"/>
     </row>
@@ -2805,7 +2812,7 @@
         <v>2</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D73" s="11"/>
     </row>
@@ -2815,7 +2822,7 @@
         <v>2</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D74" s="11"/>
     </row>
@@ -2825,7 +2832,7 @@
         <v>2</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D75" s="11"/>
     </row>
@@ -2835,7 +2842,7 @@
         <v>2</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D76" s="11"/>
     </row>
@@ -2845,7 +2852,7 @@
         <v>2</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D77" s="11"/>
     </row>
@@ -2855,7 +2862,7 @@
         <v>2</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D78" s="11"/>
     </row>
@@ -2865,7 +2872,7 @@
         <v>2</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D79" s="11"/>
     </row>
@@ -2875,10 +2882,10 @@
         <v>5</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" ht="40.5" spans="1:4">
@@ -2887,10 +2894,10 @@
         <v>5</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" ht="25.5" spans="1:4">
@@ -2899,7 +2906,7 @@
         <v>2</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D82" s="11"/>
     </row>
@@ -2909,7 +2916,7 @@
         <v>2</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D83" s="11"/>
     </row>
@@ -2919,7 +2926,7 @@
         <v>2</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D84" s="11"/>
     </row>
@@ -2929,7 +2936,7 @@
         <v>1</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D85" s="11"/>
     </row>
@@ -2939,7 +2946,7 @@
         <v>1</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D86" s="11"/>
     </row>
@@ -2949,7 +2956,7 @@
         <v>1</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D87" s="11"/>
     </row>
@@ -2959,7 +2966,7 @@
         <v>1</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D88" s="11"/>
     </row>
@@ -2969,7 +2976,7 @@
         <v>1</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D89" s="11"/>
     </row>
@@ -2979,7 +2986,7 @@
         <v>1</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D90" s="11"/>
     </row>
@@ -2989,7 +2996,7 @@
         <v>1</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D91" s="11"/>
     </row>
@@ -2999,7 +3006,7 @@
         <v>1</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D92" s="11"/>
     </row>
@@ -3009,7 +3016,7 @@
         <v>1</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D93" s="11"/>
     </row>
@@ -3019,19 +3026,19 @@
         <v>1</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D94" s="11"/>
     </row>
     <row r="95" ht="25.5" spans="1:4">
       <c r="A95" s="19" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B95" s="16">
         <v>2</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D95" s="11"/>
     </row>
@@ -3041,7 +3048,7 @@
         <v>5</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D96" s="11"/>
     </row>
@@ -3051,10 +3058,10 @@
         <v>6</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="98" ht="13.5" spans="1:4">
@@ -3063,10 +3070,10 @@
         <v>5</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="99" ht="27" spans="1:4">
@@ -3075,10 +3082,10 @@
         <v>5</v>
       </c>
       <c r="C99" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D99" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="100" ht="25.5" spans="1:4">
@@ -3087,7 +3094,7 @@
         <v>1</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D100" s="11"/>
     </row>
@@ -3097,10 +3104,10 @@
         <v>5</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="102" ht="93" spans="1:4">
@@ -3109,10 +3116,10 @@
         <v>5</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D102" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="103" ht="53.25" spans="1:4">
@@ -3121,10 +3128,10 @@
         <v>5</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D103" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="104" ht="106.5" spans="1:4">
@@ -3133,10 +3140,10 @@
         <v>5</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -3145,7 +3152,7 @@
         <v>5</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D105" s="11"/>
     </row>
@@ -3155,7 +3162,7 @@
         <v>5</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D106" s="11"/>
     </row>
@@ -3165,10 +3172,10 @@
         <v>5</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D107" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="108" ht="25.5" spans="1:4">
@@ -3177,7 +3184,7 @@
         <v>2</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D108" s="11"/>
     </row>
@@ -3187,7 +3194,7 @@
         <v>2</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D109" s="11"/>
     </row>
@@ -3197,7 +3204,7 @@
         <v>1</v>
       </c>
       <c r="C110" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D110" s="11"/>
     </row>
@@ -3207,7 +3214,7 @@
         <v>2</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D111" s="11"/>
     </row>
@@ -3217,7 +3224,7 @@
         <v>2</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D112" s="11"/>
     </row>
@@ -3227,7 +3234,7 @@
         <v>2</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D113" s="11"/>
     </row>
@@ -3237,7 +3244,7 @@
         <v>2</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D114" s="11"/>
     </row>
@@ -3247,10 +3254,10 @@
         <v>5</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D115" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="116" ht="39.75" spans="1:4">
@@ -3259,10 +3266,10 @@
         <v>5</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D116" s="11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="117" ht="156.75" spans="1:4">
@@ -3271,10 +3278,10 @@
         <v>5</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D117" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="118" ht="27" spans="1:4">
@@ -3283,10 +3290,10 @@
         <v>5</v>
       </c>
       <c r="C118" s="12" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D118" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="119" ht="54" spans="1:4">
@@ -3295,10 +3302,10 @@
         <v>5</v>
       </c>
       <c r="C119" s="12" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D119" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="120" ht="54" spans="1:4">
@@ -3307,10 +3314,10 @@
         <v>5</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D120" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="121" ht="25.5" spans="1:4">
@@ -3319,7 +3326,7 @@
         <v>2</v>
       </c>
       <c r="C121" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D121" s="11"/>
     </row>
@@ -3329,7 +3336,7 @@
         <v>1</v>
       </c>
       <c r="C122" s="12" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D122" s="11"/>
     </row>
@@ -3339,7 +3346,7 @@
         <v>1</v>
       </c>
       <c r="C123" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D123" s="11"/>
     </row>
@@ -3349,7 +3356,7 @@
         <v>1</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D124" s="11"/>
     </row>
@@ -3359,7 +3366,7 @@
         <v>2</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D125" s="11"/>
     </row>
@@ -3369,10 +3376,10 @@
         <v>5</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D126" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="127" ht="66.75" spans="1:4">
@@ -3381,10 +3388,10 @@
         <v>5</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D127" s="11" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="128" ht="27" spans="1:4">
@@ -3393,10 +3400,10 @@
         <v>5</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D128" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="129" ht="25.5" spans="1:4">
@@ -3405,7 +3412,7 @@
         <v>1</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D129" s="11"/>
     </row>
@@ -3415,7 +3422,7 @@
         <v>2</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D130" s="11"/>
     </row>
@@ -3425,7 +3432,7 @@
         <v>1</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D131" s="11"/>
     </row>
@@ -3435,7 +3442,7 @@
         <v>2</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D132" s="11"/>
     </row>
@@ -3445,7 +3452,7 @@
         <v>2</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D133" s="11"/>
     </row>
@@ -3455,10 +3462,10 @@
         <v>5</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D134" s="11" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="135" ht="66.75" spans="1:4">
@@ -3467,10 +3474,10 @@
         <v>5</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D135" s="11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="136" ht="25.5" spans="1:4">
@@ -3479,7 +3486,7 @@
         <v>1</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D136" s="11"/>
     </row>
@@ -3489,7 +3496,7 @@
         <v>1</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D137" s="11"/>
     </row>
@@ -3499,7 +3506,7 @@
         <v>1</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D138" s="11"/>
     </row>
@@ -3509,7 +3516,7 @@
         <v>1</v>
       </c>
       <c r="C139" s="12" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D139" s="11"/>
     </row>
@@ -3519,7 +3526,7 @@
         <v>1</v>
       </c>
       <c r="C140" s="12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D140" s="11"/>
     </row>
@@ -3529,10 +3536,10 @@
         <v>5</v>
       </c>
       <c r="C141" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D141" s="11" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="142" ht="26.25" spans="1:4">
@@ -3541,7 +3548,7 @@
         <v>1</v>
       </c>
       <c r="C142" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D142" s="11"/>
     </row>
@@ -3551,10 +3558,10 @@
         <v>5</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D143" s="11" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="144" ht="25.5" spans="1:4">
@@ -3563,7 +3570,7 @@
         <v>1</v>
       </c>
       <c r="C144" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D144" s="21"/>
     </row>
@@ -3573,7 +3580,7 @@
         <v>1</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D145" s="21"/>
     </row>
@@ -3583,10 +3590,10 @@
         <v>5</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D146" s="21" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="147" ht="26.25" spans="1:4">
@@ -3595,7 +3602,7 @@
         <v>1</v>
       </c>
       <c r="C147" s="22" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D147" s="21"/>
     </row>
@@ -3605,7 +3612,7 @@
         <v>1</v>
       </c>
       <c r="C148" s="22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D148" s="21"/>
     </row>
@@ -3615,7 +3622,7 @@
         <v>1</v>
       </c>
       <c r="C149" s="22" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D149" s="21"/>
     </row>
@@ -3625,7 +3632,7 @@
         <v>1</v>
       </c>
       <c r="C150" s="22" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D150" s="21"/>
     </row>
@@ -3635,7 +3642,7 @@
         <v>5</v>
       </c>
       <c r="C151" s="22" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D151" s="21"/>
     </row>
@@ -3645,10 +3652,10 @@
         <v>5</v>
       </c>
       <c r="C152" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D152" s="21" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="153" ht="27" spans="1:4">
@@ -3657,10 +3664,10 @@
         <v>5</v>
       </c>
       <c r="C153" s="12" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D153" s="21" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="154" ht="24" spans="1:4">
@@ -3669,7 +3676,7 @@
         <v>1</v>
       </c>
       <c r="C154" s="23" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D154" s="21"/>
     </row>
@@ -3679,10 +3686,10 @@
         <v>5</v>
       </c>
       <c r="C155" s="12" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D155" s="21" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="156" ht="25.5" spans="1:4">
@@ -3691,10 +3698,10 @@
         <v>5</v>
       </c>
       <c r="C156" s="12" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D156" s="11" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="157" ht="53.25" spans="1:4">
@@ -3703,10 +3710,10 @@
         <v>5</v>
       </c>
       <c r="C157" s="24" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D157" s="11" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="158" ht="28.5" spans="1:4">
@@ -3715,7 +3722,7 @@
         <v>2</v>
       </c>
       <c r="C158" s="24" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D158" s="11"/>
     </row>
@@ -3725,24 +3732,24 @@
         <v>5</v>
       </c>
       <c r="C159" s="11" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D159" s="11" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="160" ht="54" spans="1:4">
       <c r="A160" s="12" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B160" s="18">
         <v>5</v>
       </c>
       <c r="C160" s="26" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D160" s="26" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="161" ht="42" customHeight="1" spans="2:4">
@@ -3750,10 +3757,10 @@
         <v>5</v>
       </c>
       <c r="C161" s="12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D161" s="12" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="162" ht="42" customHeight="1" spans="2:4">
@@ -3761,7 +3768,7 @@
         <v>1</v>
       </c>
       <c r="C162" s="12" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D162" s="12"/>
     </row>
@@ -3770,7 +3777,7 @@
         <v>1</v>
       </c>
       <c r="C163" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D163" s="12"/>
     </row>
@@ -3779,7 +3786,7 @@
         <v>1</v>
       </c>
       <c r="C164" s="12" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D164" s="12"/>
     </row>
@@ -3789,7 +3796,7 @@
         <v>1</v>
       </c>
       <c r="C165" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D165" s="12"/>
     </row>
@@ -3799,7 +3806,7 @@
         <v>2</v>
       </c>
       <c r="C166" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D166" s="12"/>
     </row>
@@ -3809,10 +3816,10 @@
         <v>5</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="168" ht="39" spans="1:4">
@@ -3821,10 +3828,10 @@
         <v>5</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add reading note for neurall
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="244">
   <si>
     <t>Scope</t>
   </si>
@@ -781,10 +781,25 @@
     <t>NeurALL_Towards a Unified Model for Visual Perception in Automated Driving</t>
   </si>
   <si>
+    <t>自动驾驶视觉任务有: 1. object recogonition: 包含具有类别的物体识别和语义分割；2. general object detection: 包括静态物体识别和动态物体识别；3. 距离相关预测， 比如自由度；4. 场景识别，恶劣天气识别和在线校准等；多任务学习不一定能提升准确率，但是能够在减少计算量的前提下获得不错的效果；参考文献很丰富</t>
+  </si>
+  <si>
     <t>Multinet: Realtime joint semantic reasoning for autonomous driving（检测， 语意分割融合的多任务模型）</t>
   </si>
   <si>
     <t>Fast Scene Understanding for Autonomous Driving</t>
+  </si>
+  <si>
+    <t>自动驾驶相关综述</t>
+  </si>
+  <si>
+    <t>Autonomous vehicle perception: The technology of today and tomorrow</t>
+  </si>
+  <si>
+    <t>很好的一篇综述，主要review了无人车上的不同sensor和localizaiton和map的算法，但是没有详细说明preception的任务主要有哪些？</t>
+  </si>
+  <si>
+    <t>Algorithm and hardware implementation for visual perception system in autonomous vehicle: a survey</t>
   </si>
   <si>
     <t>[综述, 2010]Recent progress in road and lane detection_a survey</t>
@@ -809,10 +824,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -864,21 +879,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -887,24 +887,30 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -920,6 +926,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -927,7 +949,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -936,6 +965,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -956,45 +993,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1041,19 +1056,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1065,91 +1122,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1167,7 +1140,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1179,7 +1164,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1191,7 +1194,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1203,25 +1206,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1291,7 +1306,33 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1307,21 +1348,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1343,11 +1369,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1356,16 +1380,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1389,148 +1404,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1980,12 +1995,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G168"/>
+  <dimension ref="A1:G170"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C155" sqref="C155"/>
+      <selection pane="bottomLeft" activeCell="C164" sqref="C164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -3782,13 +3797,15 @@
       <c r="D163" s="12"/>
     </row>
     <row r="164" ht="42" customHeight="1" spans="2:4">
-      <c r="B164" s="27">
-        <v>1</v>
+      <c r="B164" s="18">
+        <v>5</v>
       </c>
       <c r="C164" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="D164" s="12"/>
+      <c r="D164" s="12" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="165" ht="26.25" spans="1:4">
       <c r="A165" s="12"/>
@@ -3796,7 +3813,7 @@
         <v>1</v>
       </c>
       <c r="C165" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D165" s="12"/>
     </row>
@@ -3806,32 +3823,54 @@
         <v>2</v>
       </c>
       <c r="C166" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D166" s="12"/>
     </row>
-    <row r="167" ht="146.25" spans="1:4">
-      <c r="A167" s="1"/>
+    <row r="167" ht="27" spans="1:4">
+      <c r="A167" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="B167" s="18">
         <v>5</v>
       </c>
-      <c r="C167" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D167" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="168" ht="39" spans="1:4">
+      <c r="C167" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="D167" s="12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="168" ht="25.5" spans="1:4">
       <c r="A168" s="1"/>
-      <c r="B168" s="18">
-        <v>5</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D168" s="2" t="s">
-        <v>238</v>
+      <c r="B168" s="27"/>
+      <c r="C168" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="D168" s="12"/>
+    </row>
+    <row r="169" ht="146.25" spans="1:4">
+      <c r="A169" s="1"/>
+      <c r="B169" s="18">
+        <v>5</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="170" ht="39" spans="1:4">
+      <c r="A170" s="1"/>
+      <c r="B170" s="18">
+        <v>5</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3842,7 +3881,7 @@
     <mergeCell ref="A18:A52"/>
     <mergeCell ref="A53:A94"/>
     <mergeCell ref="A95:A159"/>
-    <mergeCell ref="A167:A168"/>
+    <mergeCell ref="A167:A170"/>
   </mergeCells>
   <conditionalFormatting sqref="B$1:B$1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
add some papers on autonomous driving perception
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="13170"/>
+    <workbookView windowWidth="15120" windowHeight="25770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="259">
   <si>
     <t>Scope</t>
   </si>
@@ -31,7 +31,7 @@
     <t>开发平台</t>
   </si>
   <si>
-    <t>pytorch 完成一个模型, 比如object detection</t>
+    <t>pytorch 完成一个模型, 可以尝试一下没有用过的东西，比如RNN或者GAN，尤其是训练要好好看一下</t>
   </si>
   <si>
     <t>tensorflow， models/object_detcion熟悉</t>
@@ -434,6 +434,22 @@
     <t>DetNet: A Backbone network for Object Detection</t>
   </si>
   <si>
+    <t>Real-time category-based and general obstacle detection for autonomous driving</t>
+  </si>
+  <si>
+    <t>ssd+stixelNet的多任务结构，同时输出带类别的bbox，pose和general obstacle(column based)
+general obstacle detection: to identify in each image column the row position of the nearest roughly verical obstacle
+AGT: 用AGT(automated ground truth)产生general obstacle的训练数据，需要激光雷达配合</t>
+  </si>
+  <si>
+    <t>MODNet_Motion and Appearance Based Moving Object Detection Network for Autonomous Drving</t>
+  </si>
+  <si>
+    <t>一个能够同事检测物体和分割运动物体的网络
+输入为视频;
+用当前帧和它对应的光流（结合前一帧）同时给出bbox和运动的物体</t>
+  </si>
+  <si>
     <t>Segmentation</t>
   </si>
   <si>
@@ -484,6 +500,9 @@
 代码需要详细读一下</t>
   </si>
   <si>
+    <t>DeeperLab: Single-Shot Image Parser</t>
+  </si>
+  <si>
     <t>Spatial As Deep: Spatial CNN for Traffic Scene Understanding</t>
   </si>
   <si>
@@ -584,6 +603,11 @@
   </si>
   <si>
     <t>Panoptic Segmentation</t>
+  </si>
+  <si>
+    <t>全景分割是语义分割的扩展，每个pixel除了class label之外，还有一个instance label，对于同一类的stuff，index可以认为一致；全景分割的instance是不重叠的；
+提出了全景分割的标准PanopticQuality， 在instance的IoU大于0.5的情况下，每个gt的instance至多有一个prediction的instance， 因此tp, fp, fn定义为：tp：matched pairs of segmens; fp: unmatched predicted segments; fn: unmatched ground truth segments： PQ= (sum(IoU(p,g) for (p,g) in tp) / (tp + 0.5*fp + 0.5*fn)
+算法在SQ(segmentation quality)上和人类水平接近，但是在RQ(Recoginition Quality)上还大幅落后于人类</t>
   </si>
   <si>
     <t>El-gan: Embedding loss driven generative adversarial networks for lane detection</t>
@@ -755,7 +779,25 @@
 这篇文章的思路比较像SE-net, 但是encoder的计算方法比较新, 文章中的测试效果也比se-net要好一些</t>
   </si>
   <si>
-    <t>joint segmentation and detection</t>
+    <t>visual geometry</t>
+  </si>
+  <si>
+    <t>Neural RGB-&gt; D Sensing: Depth and Uncertainty from a Video Camera</t>
+  </si>
+  <si>
+    <t>Bounding boxes, segmentations and object coordinates: How important is recognition for 3d scene flow estimation in autonomous driving scenarios?</t>
+  </si>
+  <si>
+    <t>Pixel objectness: learning to segment generic objects automatically in images and videos</t>
+  </si>
+  <si>
+    <t>DeepVO: Towards End-to-End Visual Odometry with Deep Recurrent Convolutional Neural Networks</t>
+  </si>
+  <si>
+    <t>vo网络的要求：1. can learn geometric feature representation; 2. can derive connections among consecutive images, 所以文章提出了cnn+rnn的结构</t>
+  </si>
+  <si>
+    <t>multi-task</t>
   </si>
   <si>
     <t>Multi-Task Learning Using Uncertainty to Weigh Losses for Scene Geometry and Semantics</t>
@@ -778,28 +820,49 @@
     <t>Real-time Joint Object Detection and Semantic Segmentation Network for Automated Driving</t>
   </si>
   <si>
+    <t>backbone: resnet10, object detection: yolo_v2, semantic segmentation: fcn8</t>
+  </si>
+  <si>
     <t>NeurALL_Towards a Unified Model for Visual Perception in Automated Driving</t>
   </si>
   <si>
-    <t>自动驾驶视觉任务有: 1. object recogonition: 包含具有类别的物体识别和语义分割；2. general object detection: 包括静态物体识别和动态物体识别；3. 距离相关预测， 比如自由度；4. 场景识别，恶劣天气识别和在线校准等；多任务学习不一定能提升准确率，但是能够在减少计算量的前提下获得不错的效果；参考文献很丰富</t>
+    <t>自动驾驶视觉任务有: 1. object recogonition: 包含具有类别的物体识别和语义分割；2. general object detection: 包括静态物体识别和动态物体识别；3. 距离相关预测， 比如自由度；4. 场景识别，恶劣天气识别和在线校准等；
+多任务学习不一定能提升准确率，但是能够在减少计算量的前提下获得不错的效果；
+参考文献很丰富</t>
   </si>
   <si>
     <t>Multinet: Realtime joint semantic reasoning for autonomous driving（检测， 语意分割融合的多任务模型）</t>
   </si>
   <si>
+    <t>object detection decoder的设计有意思：每个点的roi不靠anchor， 直接预测生成，然后再去roiAlign，保证了scale invariance
+训练的时候， 每个task单独forward（每个task的参数，batchsieze不一致）， 仅backward的时候把gradient合起来</t>
+  </si>
+  <si>
     <t>Fast Scene Understanding for Autonomous Driving</t>
   </si>
   <si>
-    <t>自动驾驶相关综述</t>
+    <t>1. 用Enet做backbone，instance segmentation用了proposal free的方法</t>
+  </si>
+  <si>
+    <t>Visual SLAM for Automated Driving: Exploring the Application of Deep Learning</t>
+  </si>
+  <si>
+    <t>很好的一篇综述文章，综述了视觉slam的典型流水线，应用场景，挑战和深度学习在其中扮演的角色，for now， visual slam uses cnn is not mature for deployment in commecial commotial automated driving system
+fundamental pipline: tracking-&gt;mapping-&gt;global_optimization-&gt;relocalization
+Use case: cameras have high resolution, so VisualSLAM suits for situation that require a detailed knowlagde about the environment or generate ambiguous signals from other sensors, such as 
+parking, highway driving and uban driving
+deep learing opportunities:
+1. tracking/odometry
+2. depth estimation: 
+3. optical flow
+4. Semantic Segmentation
+5. Camera pose estimation</t>
   </si>
   <si>
     <t>Autonomous vehicle perception: The technology of today and tomorrow</t>
   </si>
   <si>
     <t>很好的一篇综述，主要review了无人车上的不同sensor和localizaiton和map的算法，但是没有详细说明preception的任务主要有哪些？</t>
-  </si>
-  <si>
-    <t>Algorithm and hardware implementation for visual perception system in autonomous vehicle: a survey</t>
   </si>
   <si>
     <t>[综述, 2010]Recent progress in road and lane detection_a survey</t>
@@ -824,10 +887,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -879,8 +942,23 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -894,8 +972,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -909,40 +1025,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -964,44 +1049,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1015,9 +1071,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1062,7 +1125,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1080,55 +1269,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1140,103 +1299,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1326,6 +1389,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1338,16 +1416,34 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1366,190 +1462,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1627,6 +1690,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1995,20 +2061,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G170"/>
+  <dimension ref="A1:G177"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C164" sqref="C164"/>
+      <selection pane="bottomLeft" activeCell="D164" sqref="D164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="13.54" customWidth="1"/>
+    <col min="1" max="1" width="11.4066666666667" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.9066666666667" style="2" customWidth="1"/>
-    <col min="4" max="4" width="65.4533333333333" style="2" customWidth="1"/>
+    <col min="3" max="3" width="41.14" style="2" customWidth="1"/>
+    <col min="4" max="4" width="74.7133333333333" style="2" customWidth="1"/>
     <col min="6" max="6" width="7.81333333333333" customWidth="1"/>
     <col min="7" max="7" width="26.18" customWidth="1"/>
   </cols>
@@ -2027,7 +2093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="13.5" spans="1:4">
+    <row r="2" ht="27" spans="1:4">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -2159,7 +2225,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" ht="80.25" spans="1:4">
+    <row r="14" ht="67.5" spans="1:4">
       <c r="A14" s="9"/>
       <c r="B14" s="10">
         <v>5</v>
@@ -2299,7 +2365,7 @@
       </c>
       <c r="D26" s="11"/>
     </row>
-    <row r="27" ht="27" spans="1:4">
+    <row r="27" ht="25.5" spans="1:4">
       <c r="A27" s="9"/>
       <c r="B27" s="14">
         <v>5</v>
@@ -2381,7 +2447,7 @@
       </c>
       <c r="D34" s="11"/>
     </row>
-    <row r="35" ht="79.5" spans="1:4">
+    <row r="35" ht="78.75" spans="1:4">
       <c r="A35" s="9"/>
       <c r="B35" s="14">
         <v>5</v>
@@ -2435,7 +2501,7 @@
       </c>
       <c r="D39" s="11"/>
     </row>
-    <row r="40" ht="80.25" spans="1:4">
+    <row r="40" ht="66.75" spans="1:4">
       <c r="A40" s="9"/>
       <c r="B40" s="14">
         <v>5</v>
@@ -2459,7 +2525,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" ht="27" spans="1:4">
+    <row r="42" ht="26.25" spans="1:4">
       <c r="A42" s="9"/>
       <c r="B42" s="14">
         <v>5</v>
@@ -2481,7 +2547,7 @@
       </c>
       <c r="D43" s="11"/>
     </row>
-    <row r="44" ht="39.75" spans="1:4">
+    <row r="44" ht="39" spans="1:4">
       <c r="A44" s="9"/>
       <c r="B44" s="14">
         <v>5</v>
@@ -2503,7 +2569,7 @@
       </c>
       <c r="D45" s="11"/>
     </row>
-    <row r="46" ht="78.75" spans="1:4">
+    <row r="46" ht="66" spans="1:4">
       <c r="A46" s="9"/>
       <c r="B46" s="14">
         <v>5</v>
@@ -2515,7 +2581,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" ht="27" spans="1:4">
+    <row r="47" ht="25.5" spans="1:4">
       <c r="A47" s="9"/>
       <c r="B47" s="14">
         <v>5</v>
@@ -2661,7 +2727,7 @@
       <c r="F59" s="17"/>
       <c r="G59" s="17"/>
     </row>
-    <row r="60" ht="67.5" spans="1:7">
+    <row r="60" ht="51.75" spans="1:7">
       <c r="A60" s="9"/>
       <c r="B60" s="14">
         <v>5</v>
@@ -2779,7 +2845,7 @@
       </c>
       <c r="D68" s="11"/>
     </row>
-    <row r="69" ht="80.25" spans="1:4">
+    <row r="69" ht="66.75" spans="1:4">
       <c r="A69" s="9"/>
       <c r="B69" s="10">
         <v>5</v>
@@ -2903,7 +2969,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="81" ht="40.5" spans="1:4">
+    <row r="81" ht="27" spans="1:4">
       <c r="A81" s="9"/>
       <c r="B81" s="10">
         <v>5</v>
@@ -2948,7 +3014,7 @@
     <row r="85" spans="1:4">
       <c r="A85" s="9"/>
       <c r="B85" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>121</v>
@@ -2958,7 +3024,7 @@
     <row r="86" ht="25.5" spans="1:4">
       <c r="A86" s="9"/>
       <c r="B86" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>122</v>
@@ -2968,7 +3034,7 @@
     <row r="87" ht="25.5" spans="1:4">
       <c r="A87" s="9"/>
       <c r="B87" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>123</v>
@@ -2978,7 +3044,7 @@
     <row r="88" spans="1:4">
       <c r="A88" s="9"/>
       <c r="B88" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>124</v>
@@ -2987,8 +3053,8 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="9"/>
-      <c r="B89" s="16">
-        <v>1</v>
+      <c r="B89" s="10">
+        <v>2</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>125</v>
@@ -2997,8 +3063,8 @@
     </row>
     <row r="90" ht="25.5" spans="1:4">
       <c r="A90" s="9"/>
-      <c r="B90" s="16">
-        <v>1</v>
+      <c r="B90" s="10">
+        <v>2</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>126</v>
@@ -3007,8 +3073,8 @@
     </row>
     <row r="91" ht="25.5" spans="1:4">
       <c r="A91" s="9"/>
-      <c r="B91" s="16">
-        <v>1</v>
+      <c r="B91" s="10">
+        <v>2</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>127</v>
@@ -3017,8 +3083,8 @@
     </row>
     <row r="92" ht="25.5" spans="1:4">
       <c r="A92" s="9"/>
-      <c r="B92" s="16">
-        <v>1</v>
+      <c r="B92" s="10">
+        <v>2</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>128</v>
@@ -3027,8 +3093,8 @@
     </row>
     <row r="93" ht="25.5" spans="1:4">
       <c r="A93" s="9"/>
-      <c r="B93" s="16">
-        <v>1</v>
+      <c r="B93" s="10">
+        <v>2</v>
       </c>
       <c r="C93" s="11" t="s">
         <v>129</v>
@@ -3037,64 +3103,64 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="9"/>
-      <c r="B94" s="16">
-        <v>1</v>
+      <c r="B94" s="10">
+        <v>2</v>
       </c>
       <c r="C94" s="11" t="s">
         <v>130</v>
       </c>
       <c r="D94" s="11"/>
     </row>
-    <row r="95" ht="25.5" spans="1:4">
-      <c r="A95" s="19" t="s">
+    <row r="95" ht="78" spans="1:4">
+      <c r="A95" s="9"/>
+      <c r="B95" s="10">
+        <v>5</v>
+      </c>
+      <c r="C95" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B95" s="16">
-        <v>2</v>
-      </c>
-      <c r="C95" s="2" t="s">
+      <c r="D95" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="D95" s="11"/>
-    </row>
-    <row r="96" ht="39.75" spans="1:4">
-      <c r="A96" s="19"/>
+    </row>
+    <row r="96" ht="40.5" spans="1:4">
+      <c r="A96" s="9"/>
       <c r="B96" s="10">
         <v>5</v>
       </c>
-      <c r="C96" s="11" t="s">
+      <c r="C96" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="D96" s="11"/>
-    </row>
-    <row r="97" ht="66" spans="1:4">
-      <c r="A97" s="19"/>
-      <c r="B97" s="10">
+      <c r="D96" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="97" ht="25.5" spans="1:4">
+      <c r="A97" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="B97" s="16">
+        <v>2</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D97" s="11"/>
+    </row>
+    <row r="98" ht="39.75" spans="1:4">
+      <c r="A98" s="19"/>
+      <c r="B98" s="10">
+        <v>5</v>
+      </c>
+      <c r="C98" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D98" s="11"/>
+    </row>
+    <row r="99" ht="52.5" spans="1:4">
+      <c r="A99" s="19"/>
+      <c r="B99" s="10">
         <v>6</v>
-      </c>
-      <c r="C97" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="D97" s="11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="98" ht="13.5" spans="1:4">
-      <c r="A98" s="19"/>
-      <c r="B98" s="18">
-        <v>5</v>
-      </c>
-      <c r="C98" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="D98" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="99" ht="27" spans="1:4">
-      <c r="A99" s="19"/>
-      <c r="B99" s="18">
-        <v>5</v>
       </c>
       <c r="C99" s="11" t="s">
         <v>138</v>
@@ -3103,41 +3169,41 @@
         <v>139</v>
       </c>
     </row>
-    <row r="100" ht="25.5" spans="1:4">
+    <row r="100" ht="13.5" spans="1:4">
       <c r="A100" s="19"/>
       <c r="B100" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C100" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="D100" s="11"/>
-    </row>
-    <row r="101" ht="93" spans="1:4">
+      <c r="D100" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="101" ht="25.5" spans="1:4">
       <c r="A101" s="19"/>
       <c r="B101" s="18">
         <v>5</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="102" ht="93" spans="1:4">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="102" ht="25.5" spans="1:4">
       <c r="A102" s="19"/>
       <c r="B102" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D102" s="11" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="103" ht="53.25" spans="1:4">
+      <c r="D102" s="11"/>
+    </row>
+    <row r="103" ht="92.25" spans="1:4">
       <c r="A103" s="19"/>
       <c r="B103" s="18">
         <v>5</v>
@@ -3149,7 +3215,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="104" ht="106.5" spans="1:4">
+    <row r="104" ht="92.25" spans="1:4">
       <c r="A104" s="19"/>
       <c r="B104" s="18">
         <v>5</v>
@@ -3164,14 +3230,14 @@
     <row r="105" spans="1:4">
       <c r="A105" s="19"/>
       <c r="B105" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C105" s="11" t="s">
         <v>149</v>
       </c>
       <c r="D105" s="11"/>
     </row>
-    <row r="106" ht="26.25" spans="1:4">
+    <row r="106" ht="53.25" spans="1:4">
       <c r="A106" s="19"/>
       <c r="B106" s="18">
         <v>5</v>
@@ -3179,57 +3245,61 @@
       <c r="C106" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="D106" s="11"/>
-    </row>
-    <row r="107" ht="39.75" spans="1:4">
+      <c r="D106" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="107" ht="106.5" spans="1:4">
       <c r="A107" s="19"/>
       <c r="B107" s="18">
         <v>5</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D107" s="11" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="108" ht="25.5" spans="1:4">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108" s="19"/>
       <c r="B108" s="18">
-        <v>2</v>
-      </c>
-      <c r="C108" s="12" t="s">
-        <v>153</v>
+        <v>5</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>154</v>
       </c>
       <c r="D108" s="11"/>
     </row>
-    <row r="109" ht="25.5" spans="1:4">
+    <row r="109" ht="26.25" spans="1:4">
       <c r="A109" s="19"/>
       <c r="B109" s="18">
-        <v>2</v>
-      </c>
-      <c r="C109" s="12" t="s">
-        <v>154</v>
+        <v>5</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="D109" s="11"/>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" ht="39.75" spans="1:4">
       <c r="A110" s="19"/>
       <c r="B110" s="18">
-        <v>1</v>
-      </c>
-      <c r="C110" t="s">
-        <v>155</v>
-      </c>
-      <c r="D110" s="11"/>
+        <v>5</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D110" s="11" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="111" ht="25.5" spans="1:4">
       <c r="A111" s="19"/>
       <c r="B111" s="18">
         <v>2</v>
       </c>
-      <c r="C111" s="2" t="s">
-        <v>156</v>
+      <c r="C111" s="12" t="s">
+        <v>158</v>
       </c>
       <c r="D111" s="11"/>
     </row>
@@ -3239,17 +3309,17 @@
         <v>2</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D112" s="11"/>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="19"/>
       <c r="B113" s="18">
-        <v>2</v>
-      </c>
-      <c r="C113" s="12" t="s">
-        <v>158</v>
+        <v>1</v>
+      </c>
+      <c r="C113" t="s">
+        <v>160</v>
       </c>
       <c r="D113" s="11"/>
     </row>
@@ -3258,304 +3328,304 @@
       <c r="B114" s="18">
         <v>2</v>
       </c>
-      <c r="C114" s="12" t="s">
-        <v>159</v>
+      <c r="C114" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="D114" s="11"/>
     </row>
     <row r="115" ht="25.5" spans="1:4">
       <c r="A115" s="19"/>
       <c r="B115" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="D115" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="116" ht="39.75" spans="1:4">
+        <v>162</v>
+      </c>
+      <c r="D115" s="11"/>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" s="19"/>
       <c r="B116" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D116" s="11" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="117" ht="156.75" spans="1:4">
+      <c r="D116" s="11"/>
+    </row>
+    <row r="117" ht="25.5" spans="1:4">
       <c r="A117" s="19"/>
       <c r="B117" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C117" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="D117" s="11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="118" ht="27" spans="1:4">
+      <c r="D117" s="11"/>
+    </row>
+    <row r="118" ht="25.5" spans="1:4">
       <c r="A118" s="19"/>
       <c r="B118" s="18">
         <v>5</v>
       </c>
       <c r="C118" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D118" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="D118" s="11" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="119" ht="54" spans="1:4">
+    </row>
+    <row r="119" ht="39" spans="1:4">
       <c r="A119" s="19"/>
       <c r="B119" s="18">
         <v>5</v>
       </c>
       <c r="C119" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="D119" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="D119" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="120" ht="54" spans="1:4">
+    </row>
+    <row r="120" ht="144" spans="1:4">
       <c r="A120" s="19"/>
       <c r="B120" s="18">
         <v>5</v>
       </c>
       <c r="C120" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="D120" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="D120" s="11" t="s">
+    </row>
+    <row r="121" ht="27" spans="1:4">
+      <c r="A121" s="19"/>
+      <c r="B121" s="18">
+        <v>5</v>
+      </c>
+      <c r="C121" s="12" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="121" ht="25.5" spans="1:4">
-      <c r="A121" s="19"/>
-      <c r="B121" s="20">
-        <v>2</v>
-      </c>
-      <c r="C121" s="12" t="s">
+      <c r="D121" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="D121" s="11"/>
-    </row>
-    <row r="122" ht="25.5" spans="1:4">
+    </row>
+    <row r="122" ht="40.5" spans="1:4">
       <c r="A122" s="19"/>
       <c r="B122" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C122" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D122" s="11"/>
-    </row>
-    <row r="123" ht="25.5" spans="1:4">
+      <c r="D122" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="123" ht="40.5" spans="1:4">
       <c r="A123" s="19"/>
       <c r="B123" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C123" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="D123" s="11"/>
-    </row>
-    <row r="124" spans="1:4">
+        <v>175</v>
+      </c>
+      <c r="D123" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="124" ht="25.5" spans="1:4">
       <c r="A124" s="19"/>
-      <c r="B124" s="18">
-        <v>1</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>175</v>
+      <c r="B124" s="20">
+        <v>2</v>
+      </c>
+      <c r="C124" s="12" t="s">
+        <v>177</v>
       </c>
       <c r="D124" s="11"/>
     </row>
     <row r="125" ht="25.5" spans="1:4">
       <c r="A125" s="19"/>
       <c r="B125" s="18">
-        <v>2</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>176</v>
+        <v>1</v>
+      </c>
+      <c r="C125" s="12" t="s">
+        <v>178</v>
       </c>
       <c r="D125" s="11"/>
     </row>
-    <row r="126" ht="54" spans="1:4">
+    <row r="126" ht="25.5" spans="1:4">
       <c r="A126" s="19"/>
       <c r="B126" s="18">
-        <v>5</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D126" s="11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="127" ht="66.75" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="C126" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D126" s="11"/>
+    </row>
+    <row r="127" ht="93.75" spans="1:4">
       <c r="A127" s="19"/>
       <c r="B127" s="18">
         <v>5</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D127" s="11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="128" ht="27" spans="1:4">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="128" ht="25.5" spans="1:4">
       <c r="A128" s="19"/>
       <c r="B128" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D128" s="11" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="129" ht="25.5" spans="1:4">
+      <c r="D128" s="11"/>
+    </row>
+    <row r="129" ht="54" spans="1:4">
       <c r="A129" s="19"/>
       <c r="B129" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D129" s="11"/>
-    </row>
-    <row r="130" spans="1:4">
+      <c r="D129" s="11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="130" ht="40.5" spans="1:4">
       <c r="A130" s="19"/>
       <c r="B130" s="18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D130" s="11"/>
-    </row>
-    <row r="131" ht="25.5" spans="1:4">
+        <v>185</v>
+      </c>
+      <c r="D130" s="11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="131" ht="27" spans="1:4">
       <c r="A131" s="19"/>
       <c r="B131" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D131" s="11"/>
-    </row>
-    <row r="132" spans="1:4">
+        <v>187</v>
+      </c>
+      <c r="D131" s="11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="132" ht="25.5" spans="1:4">
       <c r="A132" s="19"/>
       <c r="B132" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D132" s="11"/>
     </row>
-    <row r="133" ht="25.5" spans="1:4">
+    <row r="133" spans="1:4">
       <c r="A133" s="19"/>
       <c r="B133" s="18">
         <v>2</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D133" s="11"/>
     </row>
-    <row r="134" ht="108" spans="1:4">
+    <row r="134" ht="25.5" spans="1:4">
       <c r="A134" s="19"/>
       <c r="B134" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D134" s="11" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="135" ht="66.75" spans="1:4">
+        <v>191</v>
+      </c>
+      <c r="D134" s="11"/>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" s="19"/>
       <c r="B135" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D135" s="11" t="s">
-        <v>191</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="D135" s="11"/>
     </row>
     <row r="136" ht="25.5" spans="1:4">
       <c r="A136" s="19"/>
       <c r="B136" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D136" s="11"/>
     </row>
-    <row r="137" ht="38.25" spans="1:4">
+    <row r="137" ht="108" spans="1:4">
       <c r="A137" s="19"/>
       <c r="B137" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="D137" s="11"/>
-    </row>
-    <row r="138" ht="25.5" spans="1:4">
+        <v>194</v>
+      </c>
+      <c r="D137" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="138" ht="66.75" spans="1:4">
       <c r="A138" s="19"/>
       <c r="B138" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D138" s="11"/>
-    </row>
-    <row r="139" ht="26.25" spans="1:4">
+        <v>196</v>
+      </c>
+      <c r="D138" s="11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="139" ht="25.5" spans="1:4">
       <c r="A139" s="19"/>
       <c r="B139" s="18">
         <v>1</v>
       </c>
-      <c r="C139" s="12" t="s">
-        <v>195</v>
+      <c r="C139" s="2" t="s">
+        <v>198</v>
       </c>
       <c r="D139" s="11"/>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" ht="38.25" spans="1:4">
       <c r="A140" s="19"/>
       <c r="B140" s="18">
         <v>1</v>
       </c>
-      <c r="C140" s="12" t="s">
-        <v>196</v>
+      <c r="C140" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="D140" s="11"/>
     </row>
-    <row r="141" ht="66.75" spans="1:4">
+    <row r="141" ht="25.5" spans="1:4">
       <c r="A141" s="19"/>
       <c r="B141" s="18">
-        <v>5</v>
-      </c>
-      <c r="C141" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="D141" s="11" t="s">
-        <v>198</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D141" s="11"/>
     </row>
     <row r="142" ht="26.25" spans="1:4">
       <c r="A142" s="19"/>
@@ -3563,61 +3633,61 @@
         <v>1</v>
       </c>
       <c r="C142" s="12" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D142" s="11"/>
     </row>
-    <row r="143" ht="66.75" spans="1:4">
+    <row r="143" spans="1:4">
       <c r="A143" s="19"/>
       <c r="B143" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="D143" s="11" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="144" ht="25.5" spans="1:4">
+        <v>202</v>
+      </c>
+      <c r="D143" s="11"/>
+    </row>
+    <row r="144" ht="66.75" spans="1:4">
       <c r="A144" s="19"/>
       <c r="B144" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C144" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="D144" s="21"/>
-    </row>
-    <row r="145" spans="1:4">
+        <v>203</v>
+      </c>
+      <c r="D144" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="145" ht="26.25" spans="1:4">
       <c r="A145" s="19"/>
       <c r="B145" s="18">
         <v>1</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="D145" s="21"/>
-    </row>
-    <row r="146" ht="91.5" spans="1:4">
+        <v>205</v>
+      </c>
+      <c r="D145" s="11"/>
+    </row>
+    <row r="146" ht="66.75" spans="1:4">
       <c r="A146" s="19"/>
       <c r="B146" s="18">
         <v>5</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="D146" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="147" ht="26.25" spans="1:4">
+        <v>206</v>
+      </c>
+      <c r="D146" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="147" ht="25.5" spans="1:4">
       <c r="A147" s="19"/>
       <c r="B147" s="18">
         <v>1</v>
       </c>
-      <c r="C147" s="22" t="s">
-        <v>206</v>
+      <c r="C147" s="12" t="s">
+        <v>208</v>
       </c>
       <c r="D147" s="21"/>
     </row>
@@ -3626,262 +3696,352 @@
       <c r="B148" s="18">
         <v>1</v>
       </c>
-      <c r="C148" s="22" t="s">
-        <v>207</v>
+      <c r="C148" s="12" t="s">
+        <v>209</v>
       </c>
       <c r="D148" s="21"/>
     </row>
-    <row r="149" ht="39.75" spans="1:4">
+    <row r="149" ht="78.75" spans="1:4">
       <c r="A149" s="19"/>
       <c r="B149" s="18">
-        <v>1</v>
-      </c>
-      <c r="C149" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="D149" s="21"/>
-    </row>
-    <row r="150" ht="25.5" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C149" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="D149" s="21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="150" ht="26.25" spans="1:4">
       <c r="A150" s="19"/>
       <c r="B150" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C150" s="22" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D150" s="21"/>
     </row>
-    <row r="151" ht="25.5" spans="1:4">
+    <row r="151" spans="1:4">
       <c r="A151" s="19"/>
       <c r="B151" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C151" s="22" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D151" s="21"/>
     </row>
-    <row r="152" ht="92.25" spans="1:4">
+    <row r="152" ht="39.75" spans="1:4">
       <c r="A152" s="19"/>
       <c r="B152" s="18">
-        <v>5</v>
-      </c>
-      <c r="C152" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="D152" s="21" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="153" ht="27" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="C152" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="D152" s="21"/>
+    </row>
+    <row r="153" ht="25.5" spans="1:4">
       <c r="A153" s="19"/>
       <c r="B153" s="18">
-        <v>5</v>
-      </c>
-      <c r="C153" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="D153" s="21" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="154" ht="24" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="C153" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="D153" s="21"/>
+    </row>
+    <row r="154" ht="25.5" spans="1:4">
       <c r="A154" s="19"/>
       <c r="B154" s="18">
-        <v>1</v>
-      </c>
-      <c r="C154" s="23" t="s">
-        <v>215</v>
+        <v>5</v>
+      </c>
+      <c r="C154" s="22" t="s">
+        <v>216</v>
       </c>
       <c r="D154" s="21"/>
     </row>
-    <row r="155" ht="147" spans="1:4">
+    <row r="155" ht="92.25" spans="1:4">
       <c r="A155" s="19"/>
       <c r="B155" s="18">
         <v>5</v>
       </c>
       <c r="C155" s="12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D155" s="21" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="156" ht="25.5" spans="1:4">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="156" ht="27" spans="1:4">
       <c r="A156" s="19"/>
       <c r="B156" s="18">
         <v>5</v>
       </c>
       <c r="C156" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="D156" s="11" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="157" ht="53.25" spans="1:4">
+      <c r="D156" s="21" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="157" ht="24" spans="1:4">
       <c r="A157" s="19"/>
       <c r="B157" s="18">
-        <v>5</v>
-      </c>
-      <c r="C157" s="24" t="s">
-        <v>220</v>
-      </c>
-      <c r="D157" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C157" s="23" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="158" ht="28.5" spans="1:4">
+      <c r="D157" s="21"/>
+    </row>
+    <row r="158" ht="146.25" spans="1:4">
       <c r="A158" s="19"/>
       <c r="B158" s="18">
-        <v>2</v>
-      </c>
-      <c r="C158" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C158" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="D158" s="11"/>
-    </row>
-    <row r="159" ht="119.25" spans="1:4">
-      <c r="A159" s="25"/>
+      <c r="D158" s="21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="159" ht="25.5" spans="1:4">
+      <c r="A159" s="19"/>
       <c r="B159" s="18">
         <v>5</v>
       </c>
-      <c r="C159" s="11" t="s">
-        <v>223</v>
+      <c r="C159" s="12" t="s">
+        <v>224</v>
       </c>
       <c r="D159" s="11" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="160" ht="54" spans="1:4">
-      <c r="A160" s="12" t="s">
         <v>225</v>
       </c>
+    </row>
+    <row r="160" ht="53.25" spans="1:4">
+      <c r="A160" s="19"/>
       <c r="B160" s="18">
         <v>5</v>
       </c>
-      <c r="C160" s="26" t="s">
+      <c r="C160" s="24" t="s">
         <v>226</v>
       </c>
-      <c r="D160" s="26" t="s">
+      <c r="D160" s="11" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="161" ht="42" customHeight="1" spans="2:4">
+    <row r="161" ht="28.5" spans="1:4">
+      <c r="A161" s="19"/>
       <c r="B161" s="18">
-        <v>5</v>
-      </c>
-      <c r="C161" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C161" s="24" t="s">
         <v>228</v>
       </c>
-      <c r="D161" s="12" t="s">
+      <c r="D161" s="11"/>
+    </row>
+    <row r="162" ht="105.75" spans="1:4">
+      <c r="A162" s="25"/>
+      <c r="B162" s="18">
+        <v>5</v>
+      </c>
+      <c r="C162" s="11" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="162" ht="42" customHeight="1" spans="2:4">
-      <c r="B162" s="27">
+      <c r="D162" s="11" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="163" ht="25.5" spans="1:4">
+      <c r="A163" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="B163" s="18">
         <v>1</v>
       </c>
-      <c r="C162" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="D162" s="12"/>
-    </row>
-    <row r="163" ht="42" customHeight="1" spans="2:4">
-      <c r="B163" s="27">
+      <c r="C163" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D163" s="11"/>
+    </row>
+    <row r="164" ht="51" spans="1:4">
+      <c r="A164" s="26"/>
+      <c r="B164" s="18">
         <v>1</v>
       </c>
-      <c r="C163" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="D163" s="12"/>
-    </row>
-    <row r="164" ht="42" customHeight="1" spans="2:4">
-      <c r="B164" s="18">
-        <v>5</v>
-      </c>
       <c r="C164" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="D164" s="12" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="165" ht="26.25" spans="1:4">
-      <c r="A165" s="12"/>
-      <c r="B165" s="27">
+      <c r="D164" s="11"/>
+    </row>
+    <row r="165" ht="25.5" spans="1:4">
+      <c r="A165" s="26"/>
+      <c r="B165" s="18">
         <v>1</v>
       </c>
       <c r="C165" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="D165" s="12"/>
-    </row>
-    <row r="166" spans="1:4">
-      <c r="A166" s="12"/>
-      <c r="B166" s="27">
-        <v>2</v>
-      </c>
-      <c r="C166" s="12" t="s">
+      <c r="D165" s="11"/>
+    </row>
+    <row r="166" ht="28.5" spans="1:4">
+      <c r="A166" s="26"/>
+      <c r="B166" s="18">
+        <v>5</v>
+      </c>
+      <c r="C166" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="D166" s="12"/>
-    </row>
-    <row r="167" ht="27" spans="1:4">
-      <c r="A167" s="1" t="s">
+      <c r="D166" s="11" t="s">
         <v>236</v>
       </c>
+    </row>
+    <row r="167" ht="40.5" spans="1:4">
+      <c r="A167" s="26" t="s">
+        <v>237</v>
+      </c>
       <c r="B167" s="18">
         <v>5</v>
       </c>
-      <c r="C167" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="D167" s="12" t="s">
+      <c r="C167" s="27" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="168" ht="25.5" spans="1:4">
-      <c r="A168" s="1"/>
-      <c r="B168" s="27"/>
+      <c r="D167" s="27" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="168" ht="42" customHeight="1" spans="1:4">
+      <c r="A168" s="26"/>
+      <c r="B168" s="18">
+        <v>5</v>
+      </c>
       <c r="C168" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="D168" s="12"/>
-    </row>
-    <row r="169" ht="146.25" spans="1:4">
-      <c r="A169" s="1"/>
-      <c r="B169" s="18">
-        <v>5</v>
-      </c>
-      <c r="C169" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="D169" s="2" t="s">
+      <c r="D168" s="12" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="170" ht="39" spans="1:4">
-      <c r="A170" s="1"/>
+    <row r="169" ht="42" customHeight="1" spans="1:4">
+      <c r="A169" s="26"/>
+      <c r="B169" s="28">
+        <v>2</v>
+      </c>
+      <c r="C169" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D169" s="12"/>
+    </row>
+    <row r="170" ht="42" customHeight="1" spans="1:4">
+      <c r="A170" s="26"/>
       <c r="B170" s="18">
         <v>5</v>
       </c>
-      <c r="C170" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D170" s="2" t="s">
+      <c r="C170" s="12" t="s">
         <v>243</v>
       </c>
+      <c r="D170" s="12" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="171" ht="82" customHeight="1" spans="1:4">
+      <c r="A171" s="26"/>
+      <c r="B171" s="18">
+        <v>5</v>
+      </c>
+      <c r="C171" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="D171" s="12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="172" ht="54" spans="1:4">
+      <c r="A172" s="26"/>
+      <c r="B172" s="28">
+        <v>5</v>
+      </c>
+      <c r="C172" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="D172" s="12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="173" ht="13.5" spans="1:4">
+      <c r="A173" s="26"/>
+      <c r="B173" s="18">
+        <v>5</v>
+      </c>
+      <c r="C173" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="D173" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="174" ht="220" customHeight="1" spans="1:4">
+      <c r="A174" s="26"/>
+      <c r="B174" s="18">
+        <v>5</v>
+      </c>
+      <c r="C174" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="D174" s="12" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="175" ht="27" spans="1:4">
+      <c r="A175" s="26"/>
+      <c r="B175" s="18">
+        <v>5</v>
+      </c>
+      <c r="C175" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="D175" s="12" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="176" ht="119.25" spans="1:4">
+      <c r="A176" s="26"/>
+      <c r="B176" s="18">
+        <v>5</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D176" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="177" ht="39" spans="1:4">
+      <c r="A177" s="26"/>
+      <c r="B177" s="18">
+        <v>5</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D177" s="2" t="s">
+        <v>258</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A17"/>
     <mergeCell ref="A18:A52"/>
-    <mergeCell ref="A53:A94"/>
-    <mergeCell ref="A95:A159"/>
-    <mergeCell ref="A167:A170"/>
+    <mergeCell ref="A53:A96"/>
+    <mergeCell ref="A97:A162"/>
+    <mergeCell ref="A163:A166"/>
+    <mergeCell ref="A167:A173"/>
+    <mergeCell ref="A174:A177"/>
   </mergeCells>
   <conditionalFormatting sqref="B$1:B$1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
@@ -3895,7 +4055,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C124" r:id="rId1" display="Panoptic Segmentation" tooltip="https://arxiv.org/abs/1801.00868"/>
+    <hyperlink ref="C127" r:id="rId1" display="Panoptic Segmentation" tooltip="https://arxiv.org/abs/1801.00868"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
add some paper for stixels
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15120" windowHeight="25770"/>
+    <workbookView windowWidth="27720" windowHeight="13170" tabRatio="354"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="268">
   <si>
     <t>Scope</t>
   </si>
@@ -503,6 +503,42 @@
     <t>DeeperLab: Single-Shot Image Parser</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1. 推理时间和instance数量基本无关，对复杂场景的parsing比较有优势；
+2. semantic segmentation的loss只propagate top k最高的，且面积小于64x64的instance的loss weight为3
+3. instance segmentation借助了keypoint detection的内容，通过key point heatmap， the long-range offset map, the short-range offset map, the middle-range offset map来区分instance map, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>讲真，这一部分没有看懂，作者也没有说为什么选key-point based的方法来左instance segmentation(暂时理解为作者之前有过key-point做instance segmentation的工作)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+4. 提出了一个新的全景分割指标， panoptic covering， 倾向于让大物体分对，作为对PQ的补充（PQ倾向于让数量多的thing分对）
+参考文献非常多，但是没有说明为什么用基于key-points的方法</t>
+    </r>
+  </si>
+  <si>
     <t>Spatial As Deep: Spatial CNN for Traffic Scene Understanding</t>
   </si>
   <si>
@@ -607,6 +643,7 @@
   <si>
     <t>全景分割是语义分割的扩展，每个pixel除了class label之外，还有一个instance label，对于同一类的stuff，index可以认为一致；全景分割的instance是不重叠的；
 提出了全景分割的标准PanopticQuality， 在instance的IoU大于0.5的情况下，每个gt的instance至多有一个prediction的instance， 因此tp, fp, fn定义为：tp：matched pairs of segmens; fp: unmatched predicted segments; fn: unmatched ground truth segments： PQ= (sum(IoU(p,g) for (p,g) in tp) / (tp + 0.5*fp + 0.5*fn)
+PQ的认为stuff class为一个instance, 这样，当instance比较多的时候，PQ会倾向于把thing分对（因为thing的个数比较多） 
 算法在SQ(segmentation quality)上和人类水平接近，但是在RQ(Recoginition Quality)上还大幅落后于人类</t>
   </si>
   <si>
@@ -779,13 +816,42 @@
 这篇文章的思路比较像SE-net, 但是encoder的计算方法比较新, 文章中的测试效果也比se-net要好一些</t>
   </si>
   <si>
-    <t>visual geometry</t>
+    <t>autonomous driving preception</t>
+  </si>
+  <si>
+    <t>The Stixel World - A Compact Medium Level Representation of the 3D-World</t>
+  </si>
+  <si>
+    <t>对于从地面(free-space)起始的障碍物效果比较好，但是对于飞在空中的障碍物比如交通灯等效果不好；
+提起stixel的步骤为：计算Depth(SGM)-&gt;计算occupy grid-&gt;计算free space(stixel下界)-&gt;计算stixel上界(结合free space和disparity map)-&gt;提取stixel(确定其depth：parabolic fit, 出去outliers)</t>
+  </si>
+  <si>
+    <t>The Stixel World_A Medium-level Representation of Traffic Scene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stixel is a kind of superpixel where each superpixels is a thin stick-like segment with a class label(support, vertical, sky) and a 3D planar depth model
+</t>
+  </si>
+  <si>
+    <t>semantic stixel: Depth is Not Enough</t>
+  </si>
+  <si>
+    <t>Detecting Unexpected Obstacles for Self-Drving Cars_Fusing Deep Learning and Geometirc Modeling</t>
+  </si>
+  <si>
+    <t>1. 把语义分割stixel化， 使得对空间的描述更加充分；
+2. RGB Camara: hight resolution for low/small object detection
+3. stixel: perform well for detecting medium-sized objects objects at close to medium range, with reduced performance for longer ranges and smaller obstacles
+4. 最后的small uexpexct obstacle用probalistic的方法， 融合了来自UON stixel， FPHT stixel和disparity map的三种信息</t>
   </si>
   <si>
     <t>Neural RGB-&gt; D Sensing: Depth and Uncertainty from a Video Camera</t>
   </si>
   <si>
     <t>Bounding boxes, segmentations and object coordinates: How important is recognition for 3d scene flow estimation in autonomous driving scenarios?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Pixel objectness: learning to segment generic objects automatically in images and videos</t>
@@ -887,12 +953,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -964,32 +1030,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1012,14 +1055,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1033,23 +1069,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1063,9 +1093,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1078,11 +1114,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1125,7 +1198,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1137,7 +1222,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1149,7 +1300,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1161,19 +1342,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1185,121 +1366,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1365,6 +1438,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1389,21 +1477,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1411,6 +1484,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1426,15 +1508,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1467,139 +1540,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2061,12 +2134,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G177"/>
+  <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D164" sqref="D164"/>
+      <selection pane="bottomLeft" activeCell="D135" sqref="D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -2074,7 +2147,7 @@
     <col min="1" max="1" width="11.4066666666667" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
     <col min="3" max="3" width="41.14" style="2" customWidth="1"/>
-    <col min="4" max="4" width="74.7133333333333" style="2" customWidth="1"/>
+    <col min="4" max="4" width="68.7266666666667" style="2" customWidth="1"/>
     <col min="6" max="6" width="7.81333333333333" customWidth="1"/>
     <col min="7" max="7" width="26.18" customWidth="1"/>
   </cols>
@@ -2167,7 +2240,7 @@
       </c>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" ht="25.5" spans="1:4">
       <c r="A9" s="9"/>
       <c r="B9" s="10">
         <v>2</v>
@@ -2177,7 +2250,7 @@
       </c>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" ht="39" spans="1:4">
+    <row r="10" ht="51.75" spans="1:4">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -2365,7 +2438,7 @@
       </c>
       <c r="D26" s="11"/>
     </row>
-    <row r="27" ht="25.5" spans="1:4">
+    <row r="27" ht="26.25" spans="1:4">
       <c r="A27" s="9"/>
       <c r="B27" s="14">
         <v>5</v>
@@ -2471,7 +2544,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" ht="25.5" spans="1:4">
+    <row r="37" ht="38.25" spans="1:4">
       <c r="A37" s="9"/>
       <c r="B37" s="16">
         <v>2</v>
@@ -2547,7 +2620,7 @@
       </c>
       <c r="D43" s="11"/>
     </row>
-    <row r="44" ht="39" spans="1:4">
+    <row r="44" ht="39.75" spans="1:4">
       <c r="A44" s="9"/>
       <c r="B44" s="14">
         <v>5</v>
@@ -2581,7 +2654,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" ht="25.5" spans="1:4">
+    <row r="47" ht="27" spans="1:4">
       <c r="A47" s="9"/>
       <c r="B47" s="14">
         <v>5</v>
@@ -2793,7 +2866,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" ht="25.5" spans="1:4">
       <c r="A64" s="9"/>
       <c r="B64" s="16">
         <v>3</v>
@@ -2887,7 +2960,7 @@
       </c>
       <c r="D72" s="11"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" ht="25.5" spans="1:4">
       <c r="A73" s="9"/>
       <c r="B73" s="16">
         <v>2</v>
@@ -2957,7 +3030,7 @@
       </c>
       <c r="D79" s="11"/>
     </row>
-    <row r="80" ht="13.5" spans="1:4">
+    <row r="80" ht="25.5" spans="1:4">
       <c r="A80" s="9"/>
       <c r="B80" s="18">
         <v>5</v>
@@ -3147,7 +3220,7 @@
       </c>
       <c r="D97" s="11"/>
     </row>
-    <row r="98" ht="39.75" spans="1:4">
+    <row r="98" ht="39" spans="1:4">
       <c r="A98" s="19"/>
       <c r="B98" s="10">
         <v>5</v>
@@ -3169,7 +3242,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="100" ht="13.5" spans="1:4">
+    <row r="100" ht="25.5" spans="1:4">
       <c r="A100" s="19"/>
       <c r="B100" s="18">
         <v>5</v>
@@ -3227,15 +3300,17 @@
         <v>148</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" ht="147.75" spans="1:4">
       <c r="A105" s="19"/>
       <c r="B105" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C105" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="D105" s="11"/>
+      <c r="D105" s="8" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="106" ht="53.25" spans="1:4">
       <c r="A106" s="19"/>
@@ -3243,10 +3318,10 @@
         <v>5</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D106" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="107" ht="106.5" spans="1:4">
@@ -3255,19 +3330,19 @@
         <v>5</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D107" s="11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="108" ht="25.5" spans="1:4">
       <c r="A108" s="19"/>
       <c r="B108" s="18">
         <v>5</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D108" s="11"/>
     </row>
@@ -3277,7 +3352,7 @@
         <v>5</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D109" s="11"/>
     </row>
@@ -3287,10 +3362,10 @@
         <v>5</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D110" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="111" ht="25.5" spans="1:4">
@@ -3299,7 +3374,7 @@
         <v>2</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D111" s="11"/>
     </row>
@@ -3309,7 +3384,7 @@
         <v>2</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D112" s="11"/>
     </row>
@@ -3319,7 +3394,7 @@
         <v>1</v>
       </c>
       <c r="C113" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D113" s="11"/>
     </row>
@@ -3329,17 +3404,17 @@
         <v>2</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D114" s="11"/>
     </row>
-    <row r="115" ht="25.5" spans="1:4">
+    <row r="115" ht="38.25" spans="1:4">
       <c r="A115" s="19"/>
       <c r="B115" s="18">
         <v>2</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D115" s="11"/>
     </row>
@@ -3349,7 +3424,7 @@
         <v>2</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D116" s="11"/>
     </row>
@@ -3359,7 +3434,7 @@
         <v>2</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D117" s="11"/>
     </row>
@@ -3369,10 +3444,10 @@
         <v>5</v>
       </c>
       <c r="C118" s="12" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D118" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="119" ht="39" spans="1:4">
@@ -3381,10 +3456,10 @@
         <v>5</v>
       </c>
       <c r="C119" s="12" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D119" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="120" ht="144" spans="1:4">
@@ -3393,10 +3468,10 @@
         <v>5</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D120" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="121" ht="27" spans="1:4">
@@ -3405,10 +3480,10 @@
         <v>5</v>
       </c>
       <c r="C121" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D121" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="122" ht="40.5" spans="1:4">
@@ -3417,10 +3492,10 @@
         <v>5</v>
       </c>
       <c r="C122" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D122" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="123" ht="40.5" spans="1:4">
@@ -3429,10 +3504,10 @@
         <v>5</v>
       </c>
       <c r="C123" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D123" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="124" ht="25.5" spans="1:4">
@@ -3441,7 +3516,7 @@
         <v>2</v>
       </c>
       <c r="C124" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D124" s="11"/>
     </row>
@@ -3451,7 +3526,7 @@
         <v>1</v>
       </c>
       <c r="C125" s="12" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D125" s="11"/>
     </row>
@@ -3461,20 +3536,20 @@
         <v>1</v>
       </c>
       <c r="C126" s="12" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D126" s="11"/>
     </row>
-    <row r="127" ht="93.75" spans="1:4">
+    <row r="127" ht="134.25" spans="1:4">
       <c r="A127" s="19"/>
       <c r="B127" s="18">
         <v>5</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D127" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="128" ht="25.5" spans="1:4">
@@ -3483,7 +3558,7 @@
         <v>2</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D128" s="11"/>
     </row>
@@ -3493,10 +3568,10 @@
         <v>5</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D129" s="11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="130" ht="40.5" spans="1:4">
@@ -3505,10 +3580,10 @@
         <v>5</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D130" s="11" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="131" ht="27" spans="1:4">
@@ -3517,10 +3592,10 @@
         <v>5</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D131" s="11" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="132" ht="25.5" spans="1:4">
@@ -3529,7 +3604,7 @@
         <v>1</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D132" s="11"/>
     </row>
@@ -3539,7 +3614,7 @@
         <v>2</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D133" s="11"/>
     </row>
@@ -3549,7 +3624,7 @@
         <v>1</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D134" s="11"/>
     </row>
@@ -3559,7 +3634,7 @@
         <v>2</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D135" s="11"/>
     </row>
@@ -3569,7 +3644,7 @@
         <v>2</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D136" s="11"/>
     </row>
@@ -3579,10 +3654,10 @@
         <v>5</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D137" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="138" ht="66.75" spans="1:4">
@@ -3591,10 +3666,10 @@
         <v>5</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D138" s="11" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="139" ht="25.5" spans="1:4">
@@ -3603,7 +3678,7 @@
         <v>1</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D139" s="11"/>
     </row>
@@ -3613,7 +3688,7 @@
         <v>1</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D140" s="11"/>
     </row>
@@ -3623,7 +3698,7 @@
         <v>1</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D141" s="11"/>
     </row>
@@ -3633,7 +3708,7 @@
         <v>1</v>
       </c>
       <c r="C142" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D142" s="11"/>
     </row>
@@ -3643,7 +3718,7 @@
         <v>1</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D143" s="11"/>
     </row>
@@ -3653,10 +3728,10 @@
         <v>5</v>
       </c>
       <c r="C144" s="12" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D144" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="145" ht="26.25" spans="1:4">
@@ -3665,7 +3740,7 @@
         <v>1</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D145" s="11"/>
     </row>
@@ -3675,10 +3750,10 @@
         <v>5</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D146" s="11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="147" ht="25.5" spans="1:4">
@@ -3687,7 +3762,7 @@
         <v>1</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D147" s="21"/>
     </row>
@@ -3697,7 +3772,7 @@
         <v>1</v>
       </c>
       <c r="C148" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D148" s="21"/>
     </row>
@@ -3707,10 +3782,10 @@
         <v>5</v>
       </c>
       <c r="C149" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D149" s="21" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="150" ht="26.25" spans="1:4">
@@ -3719,7 +3794,7 @@
         <v>5</v>
       </c>
       <c r="C150" s="22" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D150" s="21"/>
     </row>
@@ -3729,7 +3804,7 @@
         <v>1</v>
       </c>
       <c r="C151" s="22" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D151" s="21"/>
     </row>
@@ -3739,7 +3814,7 @@
         <v>1</v>
       </c>
       <c r="C152" s="22" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D152" s="21"/>
     </row>
@@ -3749,7 +3824,7 @@
         <v>1</v>
       </c>
       <c r="C153" s="22" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D153" s="21"/>
     </row>
@@ -3759,7 +3834,7 @@
         <v>5</v>
       </c>
       <c r="C154" s="22" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D154" s="21"/>
     </row>
@@ -3769,10 +3844,10 @@
         <v>5</v>
       </c>
       <c r="C155" s="12" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D155" s="21" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="156" ht="27" spans="1:4">
@@ -3781,10 +3856,10 @@
         <v>5</v>
       </c>
       <c r="C156" s="12" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D156" s="21" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="157" ht="24" spans="1:4">
@@ -3793,7 +3868,7 @@
         <v>1</v>
       </c>
       <c r="C157" s="23" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D157" s="21"/>
     </row>
@@ -3803,10 +3878,10 @@
         <v>5</v>
       </c>
       <c r="C158" s="12" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D158" s="21" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="159" ht="25.5" spans="1:4">
@@ -3815,10 +3890,10 @@
         <v>5</v>
       </c>
       <c r="C159" s="12" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D159" s="11" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="160" ht="53.25" spans="1:4">
@@ -3827,10 +3902,10 @@
         <v>5</v>
       </c>
       <c r="C160" s="24" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D160" s="11" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="161" ht="28.5" spans="1:4">
@@ -3839,196 +3914,244 @@
         <v>2</v>
       </c>
       <c r="C161" s="24" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D161" s="11"/>
     </row>
-    <row r="162" ht="105.75" spans="1:4">
+    <row r="162" ht="119.25" spans="1:4">
       <c r="A162" s="25"/>
       <c r="B162" s="18">
         <v>5</v>
       </c>
       <c r="C162" s="11" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D162" s="11" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="163" ht="25.5" spans="1:4">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="163" ht="66.75" spans="1:4">
       <c r="A163" s="26" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B163" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C163" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="D163" s="11"/>
-    </row>
-    <row r="164" ht="51" spans="1:4">
+        <v>233</v>
+      </c>
+      <c r="D163" s="11" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="164" ht="38.25" spans="1:4">
       <c r="A164" s="26"/>
       <c r="B164" s="18">
         <v>1</v>
       </c>
       <c r="C164" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="D164" s="11"/>
-    </row>
-    <row r="165" ht="25.5" spans="1:4">
+        <v>235</v>
+      </c>
+      <c r="D164" s="11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
       <c r="A165" s="26"/>
       <c r="B165" s="18">
         <v>1</v>
       </c>
       <c r="C165" s="12" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D165" s="11"/>
     </row>
-    <row r="166" ht="28.5" spans="1:4">
+    <row r="166" ht="109" customHeight="1" spans="1:4">
       <c r="A166" s="26"/>
       <c r="B166" s="18">
         <v>5</v>
       </c>
-      <c r="C166" s="24" t="s">
-        <v>235</v>
+      <c r="C166" s="12" t="s">
+        <v>238</v>
       </c>
       <c r="D166" s="11" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="167" ht="40.5" spans="1:4">
-      <c r="A167" s="26" t="s">
-        <v>237</v>
-      </c>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="167" ht="25.5" spans="1:4">
+      <c r="A167" s="26"/>
       <c r="B167" s="18">
-        <v>5</v>
-      </c>
-      <c r="C167" s="27" t="s">
-        <v>238</v>
-      </c>
-      <c r="D167" s="27" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="168" ht="42" customHeight="1" spans="1:4">
+        <v>2</v>
+      </c>
+      <c r="C167" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="D167" s="11"/>
+    </row>
+    <row r="168" ht="51" spans="1:4">
       <c r="A168" s="26"/>
       <c r="B168" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C168" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="D168" s="12" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="169" ht="42" customHeight="1" spans="1:4">
+      <c r="D168" s="11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="169" ht="25.5" spans="1:4">
       <c r="A169" s="26"/>
-      <c r="B169" s="28">
+      <c r="B169" s="18">
         <v>2</v>
       </c>
       <c r="C169" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="D169" s="12"/>
-    </row>
-    <row r="170" ht="42" customHeight="1" spans="1:4">
+        <v>243</v>
+      </c>
+      <c r="D169" s="11"/>
+    </row>
+    <row r="170" ht="28.5" spans="1:4">
       <c r="A170" s="26"/>
       <c r="B170" s="18">
         <v>5</v>
       </c>
-      <c r="C170" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="D170" s="12" t="s">
+      <c r="C170" s="24" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="171" ht="82" customHeight="1" spans="1:4">
-      <c r="A171" s="26"/>
+      <c r="D170" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="171" ht="40.5" spans="1:4">
+      <c r="A171" s="26" t="s">
+        <v>246</v>
+      </c>
       <c r="B171" s="18">
         <v>5</v>
       </c>
-      <c r="C171" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="D171" s="12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="172" ht="54" spans="1:4">
+      <c r="C171" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="D171" s="27" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="172" ht="42" customHeight="1" spans="1:4">
       <c r="A172" s="26"/>
-      <c r="B172" s="28">
+      <c r="B172" s="18">
         <v>5</v>
       </c>
       <c r="C172" s="12" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D172" s="12" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="173" ht="13.5" spans="1:4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="173" ht="42" customHeight="1" spans="1:4">
       <c r="A173" s="26"/>
-      <c r="B173" s="18">
-        <v>5</v>
+      <c r="B173" s="28">
+        <v>2</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="D173" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="174" ht="220" customHeight="1" spans="1:4">
+        <v>251</v>
+      </c>
+      <c r="D173" s="12"/>
+    </row>
+    <row r="174" ht="42" customHeight="1" spans="1:4">
       <c r="A174" s="26"/>
       <c r="B174" s="18">
         <v>5</v>
       </c>
       <c r="C174" s="12" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D174" s="12" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="175" ht="27" spans="1:4">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="175" ht="82" customHeight="1" spans="1:4">
       <c r="A175" s="26"/>
       <c r="B175" s="18">
         <v>5</v>
       </c>
       <c r="C175" s="12" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D175" s="12" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="176" ht="119.25" spans="1:4">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="176" ht="54" spans="1:4">
       <c r="A176" s="26"/>
-      <c r="B176" s="18">
-        <v>5</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="D176" s="2" t="s">
+      <c r="B176" s="28">
+        <v>5</v>
+      </c>
+      <c r="C176" s="12" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="177" ht="39" spans="1:4">
+      <c r="D176" s="12" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="177" ht="13.5" spans="1:4">
       <c r="A177" s="26"/>
       <c r="B177" s="18">
         <v>5</v>
       </c>
-      <c r="C177" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="D177" s="2" t="s">
+      <c r="C177" s="12" t="s">
         <v>258</v>
+      </c>
+      <c r="D177" s="12" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="178" ht="220" customHeight="1" spans="1:4">
+      <c r="A178" s="26"/>
+      <c r="B178" s="18">
+        <v>5</v>
+      </c>
+      <c r="C178" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="D178" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="179" ht="27" spans="1:4">
+      <c r="A179" s="26"/>
+      <c r="B179" s="18">
+        <v>5</v>
+      </c>
+      <c r="C179" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="D179" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="180" ht="119.25" spans="1:4">
+      <c r="A180" s="26"/>
+      <c r="B180" s="18">
+        <v>5</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D180" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="181" ht="39" spans="1:4">
+      <c r="A181" s="26"/>
+      <c r="B181" s="18">
+        <v>5</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D181" s="2" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -4039,9 +4162,9 @@
     <mergeCell ref="A18:A52"/>
     <mergeCell ref="A53:A96"/>
     <mergeCell ref="A97:A162"/>
-    <mergeCell ref="A163:A166"/>
-    <mergeCell ref="A167:A173"/>
-    <mergeCell ref="A174:A177"/>
+    <mergeCell ref="A163:A170"/>
+    <mergeCell ref="A171:A177"/>
+    <mergeCell ref="A178:A181"/>
   </mergeCells>
   <conditionalFormatting sqref="B$1:B$1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
add reading note for DFANet
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="13170" tabRatio="354"/>
+    <workbookView windowWidth="14625" windowHeight="25770" tabRatio="354"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="275">
   <si>
     <t>Scope</t>
   </si>
@@ -122,6 +122,12 @@
     <t>Deep Pyramidal Residual Networks</t>
   </si>
   <si>
+    <t>Stacked Hourglass Networks for Human Pose Estimation</t>
+  </si>
+  <si>
+    <t>Res2Net: A New Multi-scale Backbone Architecture</t>
+  </si>
+  <si>
     <t>A Comprehensive Survey on Graph Neural Networks</t>
   </si>
   <si>
@@ -450,12 +456,6 @@
 用当前帧和它对应的光流（结合前一帧）同时给出bbox和运动的物体</t>
   </si>
   <si>
-    <t>Segmentation</t>
-  </si>
-  <si>
-    <t>End-to-End Joint Semantic Segmentation of Actors and Actions in Video </t>
-  </si>
-  <si>
     <t>Beyond pixels: A comprehensive survey from bottom-up to semantic image segmentation and cosegmentation(文章偏早)</t>
   </si>
   <si>
@@ -477,9 +477,6 @@
   </si>
   <si>
     <t>1. 提出（集成）了很多想法和新模块，在当年是很跨时代的: PRelu, spatial-dropout以及在各个模块的设计上</t>
-  </si>
-  <si>
-    <t>Learning deconvolution network for semantic segmentation</t>
   </si>
   <si>
     <t>Understanding Convolution for Semantic Segmentation</t>
@@ -503,40 +500,11 @@
     <t>DeeperLab: Single-Shot Image Parser</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">1. 推理时间和instance数量基本无关，对复杂场景的parsing比较有优势；
+    <t>1. 推理时间和instance数量基本无关，对复杂场景的parsing比较有优势；
 2. semantic segmentation的loss只propagate top k最高的，且面积小于64x64的instance的loss weight为3
-3. instance segmentation借助了keypoint detection的内容，通过key point heatmap， the long-range offset map, the short-range offset map, the middle-range offset map来区分instance map, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>讲真，这一部分没有看懂，作者也没有说为什么选key-point based的方法来左instance segmentation(暂时理解为作者之前有过key-point做instance segmentation的工作)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+3. instance segmentation借助了keypoint detection的内容，通过key point heatmap， the long-range offset map, the short-range offset map, the middle-range offset map来区分instance map, 讲真，这一部分没有看懂，作者也没有说为什么选key-point based的方法来左instance segmentation(暂时理解为作者之前有过key-point做instance segmentation的工作)
 4. 提出了一个新的全景分割指标， panoptic covering， 倾向于让大物体分对，作为对PQ的补充（PQ倾向于让数量多的thing分对）
 参考文献非常多，但是没有说明为什么用基于key-points的方法</t>
-    </r>
   </si>
   <si>
     <t>Spatial As Deep: Spatial CNN for Traffic Scene Understanding</t>
@@ -561,13 +529,6 @@
 https://www.jiqizhixin.com/articles/2017-07-14-10</t>
   </si>
   <si>
-    <t>BiSeNet: Bilateral Segmentation Network for Real-time Semantic Segmentation</t>
-  </si>
-  <si>
-    <t>1. spatial path和context path分开, 同时满足速度和语义信息的提取
-2. context path 有用auxiliary loss</t>
-  </si>
-  <si>
     <t>Multi-Scale Context Interwining for Semantic Segmentation</t>
   </si>
   <si>
@@ -633,9 +594,6 @@
   </si>
   <si>
     <t>Not All Pixels Are Equal: Difficulty-aware Semantic Segmentation via Deep Layer Cascade</t>
-  </si>
-  <si>
-    <t>ICNet for Real-Time Semantic Segmentation on High-Resolution Images</t>
   </si>
   <si>
     <t>Panoptic Segmentation</t>
@@ -647,9 +605,6 @@
 算法在SQ(segmentation quality)上和人类水平接近，但是在RQ(Recoginition Quality)上还大幅落后于人类</t>
   </si>
   <si>
-    <t>El-gan: Embedding loss driven generative adversarial networks for lane detection</t>
-  </si>
-  <si>
     <t>(PSPnet) Pyramid Scene Parsing Network</t>
   </si>
   <si>
@@ -671,7 +626,142 @@
     <t>GAU: 用高层级的feature作为低层级feature的attention; FPA: feature pyrimid attention, 对hight level feature的u-shape的attention</t>
   </si>
   <si>
-    <t>learning a similarity mertric discriminatively, with application to face verification</t>
+    <t>DeepLanes_End-to-End Lane Position Estimation using Deep Neural Networks</t>
+  </si>
+  <si>
+    <t>Deep fully convolutional networks with random data augmentation for enhanced generalization in road detection</t>
+  </si>
+  <si>
+    <t>Training constrained deconvolutional networks for road scene semantic segmentation</t>
+  </si>
+  <si>
+    <t>End-to-end ego lane estimation based on sequential transfer learning for self-driving cars(着重在训练方法)</t>
+  </si>
+  <si>
+    <t>Traffic-Sign Detection and Classification in the Wild</t>
+  </si>
+  <si>
+    <t>VPGNet_vanishing point guided network for lane and road marking detection and recognition</t>
+  </si>
+  <si>
+    <t>1. 构建了一个不同天气/光照条件下的自动驾驶数据集, 20000张图, 17类, 且标注了消失点;
+2. 提出了一个多任务的车道线/道路标识检测和分类的网络, 通过加入预测消失点的任务, 来加强网络全局信息的获取
+文章在loss设计, 训连过程上都有很多值得借鉴的地方!</t>
+  </si>
+  <si>
+    <t>an empirical evaluation of deep learning on highway driving(类似于综述)</t>
+  </si>
+  <si>
+    <t>Embedding Structured Contour and Location Prior in Siamesed Fully Convolutional Networks for Road Detection</t>
+  </si>
+  <si>
+    <t>1. 提出采用轮廓作为feature, 和RGB图同时作为输入的连体FCN, 能将F1 score提高2%, 同时加快training的速度
+2. 在featureMap后加入location prior(也就是每个activation点的坐标), 可以有效去除诸如把天空分类为道路的情况</t>
+  </si>
+  <si>
+    <t>Tree-structured Kronecker Convolutional Networks for Semantic Segmentation</t>
+  </si>
+  <si>
+    <t>Multiple Encoder-Decoder net for Lane Detection</t>
+  </si>
+  <si>
+    <t>Exploring New Backbone and Attention Module for Semantic Segmentation in Street Scenes</t>
+  </si>
+  <si>
+    <t>参考文献很丰富:
+1. 对于backbone的思考：a. the feature in backbone should contain abundant spatial and semantic information; b. the backbone can impllement end-to-end framework without incresing the computation burdent too much
+2. special attention很有趣: channel方向取max, avg， 过卷积和sigmoid后形成H, W方向的attention</t>
+  </si>
+  <si>
+    <t>Spatial-Temproal Based Lane Detection Using Deep Learning（有在嵌入式系统上实现）</t>
+  </si>
+  <si>
+    <t>Deep Multi-Sensor Lane Detection</t>
+  </si>
+  <si>
+    <t>deep neural network for structural prediction and lane detection in traffic scene（geometry information, multi-task）</t>
+  </si>
+  <si>
+    <t>Line-CNN: End-to-End Traffic Line Detection With Line Proposal Unit</t>
+  </si>
+  <si>
+    <t>LineNet: a Zoomable CNN for Crowdsourced High Definition Maps Modeling in Urban Environments</t>
+  </si>
+  <si>
+    <t>StripNet: Towards Topology Consistent Strip Structure Segmentation</t>
+  </si>
+  <si>
+    <t>提出了一种由粗到精检测带状特征的方法：粗检测先确定整个带状目标的边界（确定RoI)，精检测时，用RoIAlign把对应的feature取出来，再划分RoI内的边界细分；
+做label的方法很值得借鉴：gt_label边界是1个像素，train的时候，gt_label先用低通滤波一下（变成高斯分布的一条带）再train更容易减小错误
+decompose the original segmantation problam into more easily solved boundary-regression problems, in a coarse-to-fine manner</t>
+  </si>
+  <si>
+    <t>3D-LaneNet_end-to-end 3D multiple lane detection</t>
+  </si>
+  <si>
+    <t>预测路面的坐标系， 用IPM把feature map投影到top-view，然后，以w方向的每个点代表的直线为anchor，直接回归出对于该直线的修正值和概率，作为车道线的预测。。。赞！！</t>
+  </si>
+  <si>
+    <t>EL-GAN: Embedding Loss Driven Generative Adversarial Networks for Lane Detection</t>
+  </si>
+  <si>
+    <t>Find Your Own Way: Weakly-Supervised Segmentation of Path Proposals for Urban Autonomy</t>
+  </si>
+  <si>
+    <t>对于没有车道线的场景, 用weakly supervised的方法产生label进行分割</t>
+  </si>
+  <si>
+    <t>ExFuse: Enhancing Feature Fusion for Semantic Segmentation</t>
+  </si>
+  <si>
+    <t>1. 文章认为, 在encoder-docoder结构中, 弥合height-level和low-level特征之间semantic和resolution的差异, 是decoder特征融合的关键.
+2. 离loss近的能得到更多信息</t>
+  </si>
+  <si>
+    <t>Context Encoding for Semantic Segmentation</t>
+  </si>
+  <si>
+    <t>用大类别: 比如卧室, 厨房等作为attention, 提高细分, 比如台灯, 碗等小类别的分类准确率
+增加上下文信息,不单纯是增大receptive filed, 还可以用attention机制, 比如本文中通过attention来获取图片"场景"的信息, 对出现某类别的可能性进行加权
+改结构的作用大于增加loss
+这篇文章的思路比较像SE-net, 但是encoder的计算方法比较新, 文章中的测试效果也比se-net要好一些</t>
+  </si>
+  <si>
+    <t>Real-time
+semantic Segmentation</t>
+  </si>
+  <si>
+    <t>ICNet for Real-Time Semantic Segmentation on High-Resolution Images</t>
+  </si>
+  <si>
+    <t>BiSeNet: Bilateral Segmentation Network for Real-time Semantic Segmentation</t>
+  </si>
+  <si>
+    <t>1. spatial path和context path分开, 同时满足速度和语义信息的提取
+2. context path 有用auxiliary loss</t>
+  </si>
+  <si>
+    <t>DFANet: Deep Feature Aggregation for Real-Time Semantic Segmentation</t>
+  </si>
+  <si>
+    <t>Taitan X上 1024x1024能够跑到100fps， 非常非常快了
+重点propose 了一种结构，把不同level的feature融合在一起，卷积层最大的stride是64
+sub-net work aggregation: stack of backbones by feeding the output of previous backbone to the next, allow hight level features to be processed again to further evaluate and re-access higher orderspatial relationship
+sub-stage aggregation: always from high resolution to low resolution...其实没有太看懂这部分的动机，一个可能的原因是通过多个路径来减少vanishing gradient
+为了使结构简单，提出并复用了一个Xceptiion的修改版back bone
+FC attention provides evidence for the effect of hight-dimensional context</t>
+  </si>
+  <si>
+    <t>proposal free instance segmentation/ object detection</t>
+  </si>
+  <si>
+    <t>Instance-sensitive Fully Convolutional Networks</t>
+  </si>
+  <si>
+    <t>FCOS: Fully Convolutional One-Stage Object Detection</t>
+  </si>
+  <si>
+    <t>Pixel-level Encoding and Depth Layering for Instance-level Semantic Labeling</t>
   </si>
   <si>
     <t>Recurrent Pixel Embedding for Instance Grouping</t>
@@ -684,6 +774,15 @@
   </si>
   <si>
     <t>Distance metric learning for large margin nearest neighbor classification</t>
+  </si>
+  <si>
+    <t>SGN_Sequential Grouping Networks for Instance Segmentation</t>
+  </si>
+  <si>
+    <t>Deep Watershed Transform for Instance Segmentation</t>
+  </si>
+  <si>
+    <t>Joint Graph Decomposition &amp; Node Labeling_Problem, Algorithms, Applications</t>
   </si>
   <si>
     <t>Semantic Instance Segmentation with a Discriminative Loss Function</t>
@@ -700,85 +799,6 @@
   <si>
     <t>针对目前多分类车道线在变道的时候不work的情况, 把网络结构改为一个二分类分割网络(背景,线)和一个embedding网络(某个像素属于某个instance), 把分割网络出来的结果作为mask, 拿出embedding网络对应的像素来做聚类, 实现变道的时候也能分出4条线;
 设计类H-net, 能够为每张图片输出透视变换的参数, 方便在top-view上做曲线拟合</t>
-  </si>
-  <si>
-    <t>DeepLanes_End-to-End Lane Position Estimation using Deep Neural Networks</t>
-  </si>
-  <si>
-    <t>Deep fully convolutional networks with random data augmentation for enhanced generalization in road detection</t>
-  </si>
-  <si>
-    <t>Training constrained deconvolutional networks for road scene semantic segmentation</t>
-  </si>
-  <si>
-    <t>End-to-end ego lane estimation based on sequential transfer learning for self-driving cars(着重在训练方法)</t>
-  </si>
-  <si>
-    <t>Traffic-Sign Detection and Classification in the Wild</t>
-  </si>
-  <si>
-    <t>VPGNet_vanishing point guided network for lane and road marking detection and recognition</t>
-  </si>
-  <si>
-    <t>1. 构建了一个不同天气/光照条件下的自动驾驶数据集, 20000张图, 17类, 且标注了消失点;
-2. 提出了一个多任务的车道线/道路标识检测和分类的网络, 通过加入预测消失点的任务, 来加强网络全局信息的获取
-文章在loss设计, 训连过程上都有很多值得借鉴的地方!</t>
-  </si>
-  <si>
-    <t>an empirical evaluation of deep learning on highway driving(类似于综述)</t>
-  </si>
-  <si>
-    <t>Embedding Structured Contour and Location Prior in Siamesed Fully Convolutional Networks for Road Detection</t>
-  </si>
-  <si>
-    <t>1. 提出采用轮廓作为feature, 和RGB图同时作为输入的连体FCN, 能将F1 score提高2%, 同时加快training的速度
-2. 在featureMap后加入location prior(也就是每个activation点的坐标), 可以有效去除诸如把天空分类为道路的情况</t>
-  </si>
-  <si>
-    <t>Tree-structured Kronecker Convolutional Networks for Semantic Segmentation</t>
-  </si>
-  <si>
-    <t>Multiple Encoder-Decoder net for Lane Detection</t>
-  </si>
-  <si>
-    <t>Exploring New Backbone and Attention Module for Semantic Segmentation in Street Scenes</t>
-  </si>
-  <si>
-    <t>参考文献很丰富:
-1. 对于backbone的思考：a. the feature in backbone should contain abundant spatial and semantic information; b. the backbone can impllement end-to-end framework without incresing the computation burdent too much
-2. special attention很有趣: channel方向取max, avg， 过卷积和sigmoid后形成H, W方向的attention</t>
-  </si>
-  <si>
-    <t>Spatial-Temproal Based Lane Detection Using Deep Learning（有在嵌入式系统上实现）</t>
-  </si>
-  <si>
-    <t>Deep Multi-Sensor Lane Detection</t>
-  </si>
-  <si>
-    <t>deep neural network for structural prediction and lane detection in traffic scene（geometry information, multi-task）</t>
-  </si>
-  <si>
-    <t>Line-CNN: End-to-End Traffic Line Detection With Line Proposal Unit</t>
-  </si>
-  <si>
-    <t>LineNet: a Zoomable CNN for Crowdsourced High Definition Maps Modeling in Urban Environments</t>
-  </si>
-  <si>
-    <t>StripNet: Towards Topology Consistent Strip Structure Segmentation</t>
-  </si>
-  <si>
-    <t>提出了一种由粗到精检测带状特征的方法：粗检测先确定整个带状目标的边界（确定RoI)，精检测时，用RoIAlign把对应的feature取出来，再划分RoI内的边界细分；
-做label的方法很值得借鉴：gt_label边界是1个像素，train的时候，gt_label先用低通滤波一下（变成高斯分布的一条带）再train更容易减小错误
-decompose the original segmantation problam into more easily solved boundary-regression problems, in a coarse-to-fine manner</t>
-  </si>
-  <si>
-    <t>3D-LaneNet_end-to-end 3D multiple lane detection</t>
-  </si>
-  <si>
-    <t>预测路面的坐标系， 用IPM把feature map投影到top-view，然后，以w方向的每个点代表的直线为anchor，直接回归出对于该直线的修正值和概率，作为车道线的预测。。。赞！！</t>
-  </si>
-  <si>
-    <t>EL-GAN: Embedding Loss Driven Generative Adversarial Networks for Lane Detection</t>
   </si>
   <si>
     <t>Learning to Cluster for Proposal-Free Instance Segmentation</t>
@@ -791,31 +811,6 @@
 弊端是，被遮挡的物体会被分成两个东西</t>
   </si>
   <si>
-    <t>Find Your Own Way: Weakly-Supervised Segmentation of Path Proposals for Urban Autonomy</t>
-  </si>
-  <si>
-    <t>对于没有车道线的场景, 用weakly supervised的方法产生label进行分割</t>
-  </si>
-  <si>
-    <t>ExFuse: Enhancing Feature Fusion for Semantic Segmentation</t>
-  </si>
-  <si>
-    <t>1. 文章认为, 在encoder-docoder结构中, 弥合height-level和low-level特征之间semantic和resolution的差异, 是decoder特征融合的关键.
-2. 离loss近的能得到更多信息</t>
-  </si>
-  <si>
-    <t>Associating Inter-Image Salient Instances for Weakly Supervised Semantic Segmentation </t>
-  </si>
-  <si>
-    <t>Context Encoding for Semantic Segmentation</t>
-  </si>
-  <si>
-    <t>用大类别: 比如卧室, 厨房等作为attention, 提高细分, 比如台灯, 碗等小类别的分类准确率
-增加上下文信息,不单纯是增大receptive filed, 还可以用attention机制, 比如本文中通过attention来获取图片"场景"的信息, 对出现某类别的可能性进行加权
-改结构的作用大于增加loss
-这篇文章的思路比较像SE-net, 但是encoder的计算方法比较新, 文章中的测试效果也比se-net要好一些</t>
-  </si>
-  <si>
     <t>autonomous driving preception</t>
   </si>
   <si>
@@ -908,6 +903,9 @@
   </si>
   <si>
     <t>1. 用Enet做backbone，instance segmentation用了proposal free的方法</t>
+  </si>
+  <si>
+    <t>自动驾驶综述</t>
   </si>
   <si>
     <t>Visual SLAM for Automated Driving: Exploring the Application of Deep Learning</t>
@@ -958,7 +956,7 @@
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1008,9 +1006,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1023,23 +1020,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1055,6 +1068,59 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1063,23 +1129,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1097,65 +1147,6 @@
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1192,7 +1183,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1204,19 +1231,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1228,25 +1333,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1258,121 +1363,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1438,21 +1429,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1479,17 +1455,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -1498,16 +1463,27 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1535,157 +1511,172 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1766,6 +1757,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2134,12 +2128,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G181"/>
+  <dimension ref="A1:G190"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D135" sqref="D135"/>
+      <selection pane="bottomLeft" activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -2364,7 +2358,7 @@
       </c>
       <c r="D19" s="11"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" ht="25.5" spans="1:4">
       <c r="A20" s="9"/>
       <c r="B20" s="16">
         <v>1</v>
@@ -2374,7 +2368,7 @@
       </c>
       <c r="D20" s="11"/>
     </row>
-    <row r="21" ht="25.5" spans="1:4">
+    <row r="21" spans="1:4">
       <c r="A21" s="9"/>
       <c r="B21" s="16">
         <v>1</v>
@@ -2384,7 +2378,7 @@
       </c>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" ht="51.75" spans="1:4">
+    <row r="22" ht="27" customHeight="1" spans="1:4">
       <c r="A22" s="9"/>
       <c r="B22" s="16">
         <v>1</v>
@@ -2394,88 +2388,88 @@
       </c>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" ht="27" spans="1:4">
+    <row r="23" ht="25.5" spans="1:4">
       <c r="A23" s="9"/>
-      <c r="B23" s="14">
-        <v>5</v>
+      <c r="B23" s="16">
+        <v>1</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" ht="51.75" spans="1:4">
+      <c r="A24" s="9"/>
+      <c r="B24" s="16">
+        <v>1</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" ht="37" customHeight="1" spans="1:4">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10">
-        <v>5</v>
-      </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="11"/>
+    </row>
+    <row r="25" ht="27" spans="1:4">
+      <c r="A25" s="9"/>
+      <c r="B25" s="14">
+        <v>5</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D25" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="9"/>
-      <c r="B25" s="16">
+    <row r="26" ht="37" customHeight="1" spans="1:4">
+      <c r="A26" s="9"/>
+      <c r="B26" s="10">
+        <v>5</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="9"/>
+      <c r="B27" s="16">
         <v>3</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="11"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="9"/>
-      <c r="B26" s="14">
-        <v>5</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="11"/>
-    </row>
-    <row r="27" ht="26.25" spans="1:4">
-      <c r="A27" s="9"/>
-      <c r="B27" s="14">
-        <v>5</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="11"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="9"/>
+      <c r="B28" s="14">
+        <v>5</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="28" ht="25.5" spans="1:4">
-      <c r="A28" s="9"/>
-      <c r="B28" s="16">
-        <v>3</v>
-      </c>
-      <c r="C28" s="12" t="s">
+      <c r="D28" s="11"/>
+    </row>
+    <row r="29" ht="26.25" spans="1:4">
+      <c r="A29" s="9"/>
+      <c r="B29" s="14">
+        <v>5</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="11"/>
-    </row>
-    <row r="29" ht="25.5" spans="1:4">
-      <c r="A29" s="9"/>
-      <c r="B29" s="16">
-        <v>3</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="11"/>
     </row>
     <row r="30" ht="25.5" spans="1:4">
       <c r="A30" s="9"/>
       <c r="B30" s="16">
         <v>3</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D30" s="11"/>
@@ -2490,27 +2484,27 @@
       </c>
       <c r="D31" s="11"/>
     </row>
-    <row r="32" ht="13.5" spans="1:4">
+    <row r="32" ht="25.5" spans="1:4">
       <c r="A32" s="9"/>
       <c r="B32" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D32" s="11"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" ht="25.5" spans="1:4">
       <c r="A33" s="9"/>
       <c r="B33" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D33" s="11"/>
     </row>
-    <row r="34" ht="25.5" spans="1:4">
+    <row r="34" ht="13.5" spans="1:4">
       <c r="A34" s="9"/>
       <c r="B34" s="16">
         <v>2</v>
@@ -2520,61 +2514,61 @@
       </c>
       <c r="D34" s="11"/>
     </row>
-    <row r="35" ht="78.75" spans="1:4">
+    <row r="35" spans="1:4">
       <c r="A35" s="9"/>
-      <c r="B35" s="14">
-        <v>5</v>
+      <c r="B35" s="16">
+        <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" ht="25.5" spans="1:4">
+      <c r="A36" s="9"/>
+      <c r="B36" s="16">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="36" ht="27" spans="1:4">
-      <c r="A36" s="9"/>
-      <c r="B36" s="14">
-        <v>5</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="11"/>
+    </row>
+    <row r="37" ht="79.5" spans="1:4">
+      <c r="A37" s="9"/>
+      <c r="B37" s="14">
+        <v>5</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D37" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" ht="38.25" spans="1:4">
-      <c r="A37" s="9"/>
-      <c r="B37" s="16">
-        <v>2</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="11"/>
-    </row>
-    <row r="38" ht="25.5" spans="1:4">
+    <row r="38" ht="27" spans="1:4">
       <c r="A38" s="9"/>
       <c r="B38" s="14">
         <v>5</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="11"/>
-    </row>
-    <row r="39" ht="25.5" spans="1:4">
+    </row>
+    <row r="39" ht="38.25" spans="1:4">
       <c r="A39" s="9"/>
-      <c r="B39" s="14">
-        <v>5</v>
+      <c r="B39" s="16">
+        <v>2</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>56</v>
       </c>
       <c r="D39" s="11"/>
     </row>
-    <row r="40" ht="66.75" spans="1:4">
+    <row r="40" ht="25.5" spans="1:4">
       <c r="A40" s="9"/>
       <c r="B40" s="14">
         <v>5</v>
@@ -2582,121 +2576,121 @@
       <c r="C40" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" ht="27" spans="1:4">
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" ht="25.5" spans="1:4">
       <c r="A41" s="9"/>
       <c r="B41" s="14">
         <v>5</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" ht="26.25" spans="1:4">
+        <v>58</v>
+      </c>
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" ht="66.75" spans="1:4">
       <c r="A42" s="9"/>
       <c r="B42" s="14">
         <v>5</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" ht="27" spans="1:4">
+      <c r="A43" s="9"/>
+      <c r="B43" s="14">
+        <v>5</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D43" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="9"/>
-      <c r="B43" s="16">
-        <v>2</v>
-      </c>
-      <c r="C43" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" s="11"/>
-    </row>
-    <row r="44" ht="39.75" spans="1:4">
+    <row r="44" ht="26.25" spans="1:4">
       <c r="A44" s="9"/>
       <c r="B44" s="14">
         <v>5</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D44" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="45" ht="25.5" spans="1:4">
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="9"/>
       <c r="B45" s="16">
         <v>2</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>66</v>
+      <c r="C45" t="s">
+        <v>65</v>
       </c>
       <c r="D45" s="11"/>
     </row>
-    <row r="46" ht="66" spans="1:4">
+    <row r="46" ht="39.75" spans="1:4">
       <c r="A46" s="9"/>
       <c r="B46" s="14">
         <v>5</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D46" s="11" t="s">
+    </row>
+    <row r="47" ht="25.5" spans="1:4">
+      <c r="A47" s="9"/>
+      <c r="B47" s="16">
+        <v>2</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="47" ht="27" spans="1:4">
-      <c r="A47" s="9"/>
-      <c r="B47" s="14">
-        <v>5</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="48" ht="25.5" spans="1:4">
+      <c r="D47" s="11"/>
+    </row>
+    <row r="48" ht="78.75" spans="1:4">
       <c r="A48" s="9"/>
       <c r="B48" s="14">
         <v>5</v>
       </c>
-      <c r="C48" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D48" s="11"/>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="C48" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" ht="27" spans="1:4">
       <c r="A49" s="9"/>
       <c r="B49" s="14">
         <v>5</v>
       </c>
       <c r="C49" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D49" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D49" s="11"/>
-    </row>
-    <row r="50" spans="1:4">
+    </row>
+    <row r="50" ht="25.5" spans="1:4">
       <c r="A50" s="9"/>
-      <c r="B50" s="16">
-        <v>2</v>
+      <c r="B50" s="14">
+        <v>5</v>
       </c>
       <c r="C50" s="12" t="s">
         <v>73</v>
       </c>
       <c r="D50" s="11"/>
     </row>
-    <row r="51" ht="53" customHeight="1" spans="1:4">
+    <row r="51" spans="1:4">
       <c r="A51" s="9"/>
       <c r="B51" s="14">
         <v>5</v>
@@ -2704,46 +2698,46 @@
       <c r="C51" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="D51" s="11"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="9"/>
+      <c r="B52" s="16">
+        <v>2</v>
+      </c>
+      <c r="C52" s="12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="52" ht="41" customHeight="1" spans="1:4">
-      <c r="A52" s="9"/>
-      <c r="B52" s="14">
-        <v>5</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="D52" s="11"/>
+    </row>
+    <row r="53" ht="53" customHeight="1" spans="1:4">
+      <c r="A53" s="9"/>
+      <c r="B53" s="14">
+        <v>5</v>
+      </c>
+      <c r="C53" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D53" s="11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="53" ht="25.5" spans="1:4">
-      <c r="A53" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B53" s="14">
-        <v>2</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D53" s="11"/>
-    </row>
-    <row r="54" ht="25.5" spans="1:4">
+    <row r="54" ht="41" customHeight="1" spans="1:4">
       <c r="A54" s="9"/>
       <c r="B54" s="14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" ht="25.5" spans="1:4">
+      <c r="A55" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D54" s="11"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="9"/>
       <c r="B55" s="14">
         <v>2</v>
       </c>
@@ -2762,7 +2756,7 @@
       </c>
       <c r="D56" s="11"/>
     </row>
-    <row r="57" ht="25.5" spans="1:4">
+    <row r="57" spans="1:4">
       <c r="A57" s="9"/>
       <c r="B57" s="14">
         <v>2</v>
@@ -2772,131 +2766,129 @@
       </c>
       <c r="D57" s="11"/>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" ht="25.5" spans="1:4">
       <c r="A58" s="9"/>
       <c r="B58" s="14">
-        <v>5</v>
-      </c>
-      <c r="C58" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>84</v>
       </c>
       <c r="D58" s="11"/>
-      <c r="F58" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G58" s="17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
+    </row>
+    <row r="59" ht="25.5" spans="1:4">
       <c r="A59" s="9"/>
       <c r="B59" s="14">
         <v>2</v>
       </c>
-      <c r="C59" s="11" t="s">
-        <v>86</v>
+      <c r="C59" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="D59" s="11"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-    </row>
-    <row r="60" ht="51.75" spans="1:7">
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="9"/>
       <c r="B60" s="14">
         <v>5</v>
       </c>
       <c r="C60" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D60" s="11"/>
+      <c r="F60" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G60" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D60" s="11" t="s">
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="9"/>
+      <c r="B61" s="14">
+        <v>2</v>
+      </c>
+      <c r="C61" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="F60" s="1">
+      <c r="D61" s="11"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
+    </row>
+    <row r="62" ht="51.75" spans="1:7">
+      <c r="A62" s="9"/>
+      <c r="B62" s="14">
+        <v>5</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F62" s="1">
         <v>0</v>
       </c>
-      <c r="G60" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="61" ht="25.5" spans="1:7">
-      <c r="A61" s="9"/>
-      <c r="B61" s="16">
-        <v>3</v>
-      </c>
-      <c r="C61" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D61" s="11"/>
-      <c r="F61" s="1">
-        <v>1</v>
-      </c>
-      <c r="G61" t="s">
+      <c r="G62" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="9"/>
-      <c r="B62" s="16">
-        <v>3</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D62" s="11"/>
-      <c r="F62" s="1">
-        <v>2</v>
-      </c>
-      <c r="G62" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
+    <row r="63" ht="25.5" spans="1:7">
       <c r="A63" s="9"/>
       <c r="B63" s="16">
         <v>3</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D63" s="11"/>
       <c r="F63" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G63" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="64" ht="25.5" spans="1:4">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="9"/>
       <c r="B64" s="16">
         <v>3</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D64" s="11"/>
-    </row>
-    <row r="65" ht="25.5" spans="1:4">
+      <c r="F64" s="1">
+        <v>2</v>
+      </c>
+      <c r="G64" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="9"/>
       <c r="B65" s="16">
         <v>3</v>
       </c>
       <c r="C65" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D65" s="11"/>
+      <c r="F65" s="1">
+        <v>3</v>
+      </c>
+      <c r="G65" t="s">
         <v>97</v>
       </c>
-      <c r="D65" s="11"/>
-    </row>
-    <row r="66" ht="40.5" spans="1:4">
+    </row>
+    <row r="66" ht="25.5" spans="1:4">
       <c r="A66" s="9"/>
-      <c r="B66" s="10">
-        <v>5</v>
+      <c r="B66" s="16">
+        <v>3</v>
       </c>
       <c r="C66" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D66" s="11" t="s">
-        <v>99</v>
-      </c>
+      <c r="D66" s="11"/>
     </row>
     <row r="67" ht="25.5" spans="1:4">
       <c r="A67" s="9"/>
@@ -2904,58 +2896,60 @@
         <v>3</v>
       </c>
       <c r="C67" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D67" s="11"/>
+    </row>
+    <row r="68" ht="40.5" spans="1:4">
+      <c r="A68" s="9"/>
+      <c r="B68" s="10">
+        <v>5</v>
+      </c>
+      <c r="C68" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D67" s="11"/>
-    </row>
-    <row r="68" ht="25.5" spans="1:4">
-      <c r="A68" s="9"/>
-      <c r="B68" s="16">
+      <c r="D68" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" ht="25.5" spans="1:4">
+      <c r="A69" s="9"/>
+      <c r="B69" s="16">
         <v>3</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="D68" s="11"/>
-    </row>
-    <row r="69" ht="66.75" spans="1:4">
-      <c r="A69" s="9"/>
-      <c r="B69" s="10">
-        <v>5</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D69" s="11" t="s">
+      <c r="D69" s="11"/>
+    </row>
+    <row r="70" ht="25.5" spans="1:4">
+      <c r="A70" s="9"/>
+      <c r="B70" s="16">
+        <v>3</v>
+      </c>
+      <c r="C70" s="11" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="9"/>
-      <c r="B70" s="10">
-        <v>2</v>
-      </c>
-      <c r="C70" s="12" t="s">
+      <c r="D70" s="11"/>
+    </row>
+    <row r="71" ht="66.75" spans="1:4">
+      <c r="A71" s="9"/>
+      <c r="B71" s="10">
+        <v>5</v>
+      </c>
+      <c r="C71" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="D70" s="11"/>
-    </row>
-    <row r="71" ht="25.5" spans="1:4">
-      <c r="A71" s="9"/>
-      <c r="B71" s="16">
-        <v>2</v>
-      </c>
-      <c r="C71" s="2" t="s">
+      <c r="D71" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D71" s="11"/>
-    </row>
-    <row r="72" ht="25.5" spans="1:4">
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="9"/>
-      <c r="B72" s="16">
-        <v>2</v>
-      </c>
-      <c r="C72" s="2" t="s">
+      <c r="B72" s="10">
+        <v>2</v>
+      </c>
+      <c r="C72" s="12" t="s">
         <v>106</v>
       </c>
       <c r="D72" s="11"/>
@@ -2970,7 +2964,7 @@
       </c>
       <c r="D73" s="11"/>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" ht="25.5" spans="1:4">
       <c r="A74" s="9"/>
       <c r="B74" s="16">
         <v>2</v>
@@ -3010,7 +3004,7 @@
       </c>
       <c r="D77" s="11"/>
     </row>
-    <row r="78" ht="25.5" spans="1:4">
+    <row r="78" spans="1:4">
       <c r="A78" s="9"/>
       <c r="B78" s="16">
         <v>2</v>
@@ -3032,51 +3026,51 @@
     </row>
     <row r="80" ht="25.5" spans="1:4">
       <c r="A80" s="9"/>
-      <c r="B80" s="18">
-        <v>5</v>
+      <c r="B80" s="16">
+        <v>2</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D80" s="11" t="s">
+      <c r="D80" s="11"/>
+    </row>
+    <row r="81" ht="25.5" spans="1:4">
+      <c r="A81" s="9"/>
+      <c r="B81" s="16">
+        <v>2</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="81" ht="27" spans="1:4">
-      <c r="A81" s="9"/>
-      <c r="B81" s="10">
-        <v>5</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D81" s="11" t="s">
-        <v>117</v>
-      </c>
+      <c r="D81" s="11"/>
     </row>
     <row r="82" ht="25.5" spans="1:4">
       <c r="A82" s="9"/>
-      <c r="B82" s="16">
-        <v>2</v>
+      <c r="B82" s="18">
+        <v>5</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D82" s="11"/>
-    </row>
-    <row r="83" spans="1:4">
+        <v>116</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="83" ht="40.5" spans="1:4">
       <c r="A83" s="9"/>
       <c r="B83" s="10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C83" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D83" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="D83" s="11"/>
-    </row>
-    <row r="84" spans="1:4">
+    </row>
+    <row r="84" ht="25.5" spans="1:4">
       <c r="A84" s="9"/>
-      <c r="B84" s="10">
+      <c r="B84" s="16">
         <v>2</v>
       </c>
       <c r="C84" s="2" t="s">
@@ -3094,7 +3088,7 @@
       </c>
       <c r="D85" s="11"/>
     </row>
-    <row r="86" ht="25.5" spans="1:4">
+    <row r="86" spans="1:4">
       <c r="A86" s="9"/>
       <c r="B86" s="10">
         <v>2</v>
@@ -3104,7 +3098,7 @@
       </c>
       <c r="D86" s="11"/>
     </row>
-    <row r="87" ht="25.5" spans="1:4">
+    <row r="87" spans="1:4">
       <c r="A87" s="9"/>
       <c r="B87" s="10">
         <v>2</v>
@@ -3114,7 +3108,7 @@
       </c>
       <c r="D87" s="11"/>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" ht="25.5" spans="1:4">
       <c r="A88" s="9"/>
       <c r="B88" s="10">
         <v>2</v>
@@ -3124,7 +3118,7 @@
       </c>
       <c r="D88" s="11"/>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" ht="25.5" spans="1:4">
       <c r="A89" s="9"/>
       <c r="B89" s="10">
         <v>2</v>
@@ -3134,7 +3128,7 @@
       </c>
       <c r="D89" s="11"/>
     </row>
-    <row r="90" ht="25.5" spans="1:4">
+    <row r="90" spans="1:4">
       <c r="A90" s="9"/>
       <c r="B90" s="10">
         <v>2</v>
@@ -3144,7 +3138,7 @@
       </c>
       <c r="D90" s="11"/>
     </row>
-    <row r="91" ht="25.5" spans="1:4">
+    <row r="91" spans="1:4">
       <c r="A91" s="9"/>
       <c r="B91" s="10">
         <v>2</v>
@@ -3169,89 +3163,85 @@
       <c r="B93" s="10">
         <v>2</v>
       </c>
-      <c r="C93" s="11" t="s">
+      <c r="C93" s="2" t="s">
         <v>129</v>
       </c>
       <c r="D93" s="11"/>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" ht="25.5" spans="1:4">
       <c r="A94" s="9"/>
       <c r="B94" s="10">
         <v>2</v>
       </c>
-      <c r="C94" s="11" t="s">
+      <c r="C94" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D94" s="11"/>
     </row>
-    <row r="95" ht="78" spans="1:4">
+    <row r="95" ht="25.5" spans="1:4">
       <c r="A95" s="9"/>
       <c r="B95" s="10">
-        <v>5</v>
-      </c>
-      <c r="C95" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="D95" s="11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="96" ht="40.5" spans="1:4">
+      <c r="D95" s="11"/>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" s="9"/>
       <c r="B96" s="10">
-        <v>5</v>
-      </c>
-      <c r="C96" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D96" s="11"/>
+    </row>
+    <row r="97" ht="78" spans="1:4">
+      <c r="A97" s="9"/>
+      <c r="B97" s="10">
+        <v>5</v>
+      </c>
+      <c r="C97" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="D96" s="11" t="s">
+      <c r="D97" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="97" ht="25.5" spans="1:4">
-      <c r="A97" s="19" t="s">
+    <row r="98" ht="40.5" spans="1:4">
+      <c r="A98" s="9"/>
+      <c r="B98" s="10">
+        <v>5</v>
+      </c>
+      <c r="C98" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B97" s="16">
-        <v>2</v>
-      </c>
-      <c r="C97" s="2" t="s">
+      <c r="D98" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="D97" s="11"/>
-    </row>
-    <row r="98" ht="39" spans="1:4">
-      <c r="A98" s="19"/>
-      <c r="B98" s="10">
-        <v>5</v>
-      </c>
-      <c r="C98" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="D98" s="11"/>
-    </row>
-    <row r="99" ht="52.5" spans="1:4">
+    </row>
+    <row r="99" ht="39" spans="1:4">
       <c r="A99" s="19"/>
       <c r="B99" s="10">
+        <v>5</v>
+      </c>
+      <c r="C99" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D99" s="11"/>
+    </row>
+    <row r="100" ht="52.5" spans="1:4">
+      <c r="A100" s="19"/>
+      <c r="B100" s="10">
         <v>6</v>
       </c>
-      <c r="C99" s="11" t="s">
+      <c r="C100" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="D99" s="11" t="s">
+      <c r="D100" s="11" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="100" ht="25.5" spans="1:4">
-      <c r="A100" s="19"/>
-      <c r="B100" s="18">
-        <v>5</v>
-      </c>
-      <c r="C100" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="D100" s="11" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="101" ht="25.5" spans="1:4">
@@ -3260,21 +3250,23 @@
         <v>5</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="102" ht="25.5" spans="1:4">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="102" ht="27" spans="1:4">
       <c r="A102" s="19"/>
       <c r="B102" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="D102" s="11"/>
+        <v>142</v>
+      </c>
+      <c r="D102" s="11" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="103" ht="92.25" spans="1:4">
       <c r="A103" s="19"/>
@@ -3282,22 +3274,22 @@
         <v>5</v>
       </c>
       <c r="C103" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D103" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="D103" s="11" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="104" ht="92.25" spans="1:4">
+    </row>
+    <row r="104" ht="93" spans="1:4">
       <c r="A104" s="19"/>
       <c r="B104" s="18">
         <v>5</v>
       </c>
       <c r="C104" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D104" s="11" t="s">
         <v>147</v>
-      </c>
-      <c r="D104" s="11" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="105" ht="147.75" spans="1:4">
@@ -3306,10 +3298,10 @@
         <v>5</v>
       </c>
       <c r="C105" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D105" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="D105" s="8" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="106" ht="53.25" spans="1:4">
@@ -3318,10 +3310,10 @@
         <v>5</v>
       </c>
       <c r="C106" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D106" s="11" t="s">
         <v>151</v>
-      </c>
-      <c r="D106" s="11" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="107" ht="106.5" spans="1:4">
@@ -3330,10 +3322,10 @@
         <v>5</v>
       </c>
       <c r="C107" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D107" s="11" t="s">
         <v>153</v>
-      </c>
-      <c r="D107" s="11" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="108" ht="25.5" spans="1:4">
@@ -3342,7 +3334,7 @@
         <v>5</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D108" s="11"/>
     </row>
@@ -3352,21 +3344,19 @@
         <v>5</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D109" s="11"/>
     </row>
-    <row r="110" ht="39.75" spans="1:4">
+    <row r="110" ht="25.5" spans="1:4">
       <c r="A110" s="19"/>
       <c r="B110" s="18">
-        <v>5</v>
-      </c>
-      <c r="C110" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="D110" s="11" t="s">
-        <v>158</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C110" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D110" s="11"/>
     </row>
     <row r="111" ht="25.5" spans="1:4">
       <c r="A111" s="19"/>
@@ -3374,116 +3364,118 @@
         <v>2</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D111" s="11"/>
     </row>
-    <row r="112" ht="25.5" spans="1:4">
+    <row r="112" spans="1:4">
       <c r="A112" s="19"/>
       <c r="B112" s="18">
-        <v>2</v>
-      </c>
-      <c r="C112" s="12" t="s">
-        <v>160</v>
+        <v>1</v>
+      </c>
+      <c r="C112" t="s">
+        <v>158</v>
       </c>
       <c r="D112" s="11"/>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" ht="25.5" spans="1:4">
       <c r="A113" s="19"/>
       <c r="B113" s="18">
-        <v>1</v>
-      </c>
-      <c r="C113" t="s">
-        <v>161</v>
+        <v>2</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="D113" s="11"/>
     </row>
-    <row r="114" ht="25.5" spans="1:4">
+    <row r="114" ht="38.25" spans="1:4">
       <c r="A114" s="19"/>
       <c r="B114" s="18">
         <v>2</v>
       </c>
-      <c r="C114" s="2" t="s">
-        <v>162</v>
+      <c r="C114" s="12" t="s">
+        <v>160</v>
       </c>
       <c r="D114" s="11"/>
     </row>
-    <row r="115" ht="38.25" spans="1:4">
+    <row r="115" spans="1:4">
       <c r="A115" s="19"/>
       <c r="B115" s="18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D115" s="11"/>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" ht="25.5" spans="1:4">
       <c r="A116" s="19"/>
       <c r="B116" s="18">
         <v>2</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D116" s="11"/>
     </row>
     <row r="117" ht="25.5" spans="1:4">
       <c r="A117" s="19"/>
       <c r="B117" s="18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D117" s="11"/>
-    </row>
-    <row r="118" ht="25.5" spans="1:4">
+        <v>163</v>
+      </c>
+      <c r="D117" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="118" ht="39" spans="1:4">
       <c r="A118" s="19"/>
       <c r="B118" s="18">
         <v>5</v>
       </c>
       <c r="C118" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D118" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="D118" s="11" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="119" ht="39" spans="1:4">
+    </row>
+    <row r="119" ht="144" spans="1:4">
       <c r="A119" s="19"/>
       <c r="B119" s="18">
         <v>5</v>
       </c>
       <c r="C119" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="D119" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="D119" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="120" ht="144" spans="1:4">
+    </row>
+    <row r="120" ht="27" spans="1:4">
       <c r="A120" s="19"/>
       <c r="B120" s="18">
         <v>5</v>
       </c>
       <c r="C120" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="D120" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="D120" s="11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="121" ht="27" spans="1:4">
+    </row>
+    <row r="121" ht="40.5" spans="1:4">
       <c r="A121" s="19"/>
       <c r="B121" s="18">
         <v>5</v>
       </c>
       <c r="C121" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D121" s="11" t="s">
         <v>172</v>
-      </c>
-      <c r="D121" s="11" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="122" ht="40.5" spans="1:4">
@@ -3492,55 +3484,57 @@
         <v>5</v>
       </c>
       <c r="C122" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D122" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="D122" s="11" t="s">
+    </row>
+    <row r="123" ht="25.5" spans="1:4">
+      <c r="A123" s="19"/>
+      <c r="B123" s="20">
+        <v>2</v>
+      </c>
+      <c r="C123" s="12" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="123" ht="40.5" spans="1:4">
-      <c r="A123" s="19"/>
-      <c r="B123" s="18">
-        <v>5</v>
-      </c>
-      <c r="C123" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="D123" s="11" t="s">
-        <v>177</v>
-      </c>
+      <c r="D123" s="11"/>
     </row>
     <row r="124" ht="25.5" spans="1:4">
       <c r="A124" s="19"/>
-      <c r="B124" s="20">
-        <v>2</v>
+      <c r="B124" s="18">
+        <v>1</v>
       </c>
       <c r="C124" s="12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D124" s="11"/>
     </row>
-    <row r="125" ht="25.5" spans="1:4">
+    <row r="125" ht="134.25" spans="1:4">
       <c r="A125" s="19"/>
       <c r="B125" s="18">
-        <v>1</v>
-      </c>
-      <c r="C125" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="D125" s="11"/>
-    </row>
-    <row r="126" ht="25.5" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D125" s="11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="126" ht="54" spans="1:4">
       <c r="A126" s="19"/>
       <c r="B126" s="18">
-        <v>1</v>
-      </c>
-      <c r="C126" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D126" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="D126" s="11"/>
-    </row>
-    <row r="127" ht="134.25" spans="1:4">
+    </row>
+    <row r="127" ht="40.5" spans="1:4">
       <c r="A127" s="19"/>
       <c r="B127" s="18">
         <v>5</v>
@@ -3552,619 +3546,697 @@
         <v>182</v>
       </c>
     </row>
-    <row r="128" ht="25.5" spans="1:4">
+    <row r="128" ht="27" spans="1:4">
       <c r="A128" s="19"/>
       <c r="B128" s="18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D128" s="11"/>
-    </row>
-    <row r="129" ht="54" spans="1:4">
+      <c r="D128" s="11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="129" ht="25.5" spans="1:4">
       <c r="A129" s="19"/>
       <c r="B129" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D129" s="11" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="130" ht="40.5" spans="1:4">
+      <c r="D129" s="11"/>
+    </row>
+    <row r="130" ht="38.25" spans="1:4">
       <c r="A130" s="19"/>
       <c r="B130" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D130" s="11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="131" ht="27" spans="1:4">
+      <c r="D130" s="11"/>
+    </row>
+    <row r="131" ht="25.5" spans="1:4">
       <c r="A131" s="19"/>
       <c r="B131" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D131" s="11" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="132" ht="25.5" spans="1:4">
+        <v>187</v>
+      </c>
+      <c r="D131" s="11"/>
+    </row>
+    <row r="132" ht="26.25" spans="1:4">
       <c r="A132" s="19"/>
       <c r="B132" s="18">
         <v>1</v>
       </c>
-      <c r="C132" s="2" t="s">
-        <v>190</v>
+      <c r="C132" s="12" t="s">
+        <v>188</v>
       </c>
       <c r="D132" s="11"/>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="19"/>
       <c r="B133" s="18">
-        <v>2</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>191</v>
+        <v>1</v>
+      </c>
+      <c r="C133" s="12" t="s">
+        <v>189</v>
       </c>
       <c r="D133" s="11"/>
     </row>
-    <row r="134" ht="25.5" spans="1:4">
+    <row r="134" ht="66.75" spans="1:4">
       <c r="A134" s="19"/>
       <c r="B134" s="18">
-        <v>1</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D134" s="11"/>
-    </row>
-    <row r="135" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C134" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D134" s="11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="135" ht="26.25" spans="1:4">
       <c r="A135" s="19"/>
       <c r="B135" s="18">
-        <v>2</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>193</v>
+        <v>1</v>
+      </c>
+      <c r="C135" s="12" t="s">
+        <v>192</v>
       </c>
       <c r="D135" s="11"/>
     </row>
-    <row r="136" ht="25.5" spans="1:4">
+    <row r="136" ht="66.75" spans="1:4">
       <c r="A136" s="19"/>
       <c r="B136" s="18">
-        <v>2</v>
-      </c>
-      <c r="C136" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C136" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="D136" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="D136" s="11"/>
-    </row>
-    <row r="137" ht="108" spans="1:4">
+    </row>
+    <row r="137" ht="25.5" spans="1:4">
       <c r="A137" s="19"/>
       <c r="B137" s="18">
-        <v>5</v>
-      </c>
-      <c r="C137" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C137" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="D137" s="11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="138" ht="66.75" spans="1:4">
+      <c r="D137" s="21"/>
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138" s="19"/>
       <c r="B138" s="18">
-        <v>5</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D138" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="139" ht="25.5" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="C138" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D138" s="21"/>
+    </row>
+    <row r="139" ht="91.5" spans="1:4">
       <c r="A139" s="19"/>
       <c r="B139" s="18">
-        <v>1</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D139" s="11"/>
-    </row>
-    <row r="140" ht="38.25" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C139" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="D139" s="21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="140" ht="26.25" spans="1:4">
       <c r="A140" s="19"/>
       <c r="B140" s="18">
-        <v>1</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D140" s="11"/>
-    </row>
-    <row r="141" ht="25.5" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C140" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="D140" s="21"/>
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141" s="19"/>
       <c r="B141" s="18">
         <v>1</v>
       </c>
-      <c r="C141" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D141" s="11"/>
-    </row>
-    <row r="142" ht="26.25" spans="1:4">
+      <c r="C141" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="D141" s="21"/>
+    </row>
+    <row r="142" ht="39.75" spans="1:4">
       <c r="A142" s="19"/>
       <c r="B142" s="18">
         <v>1</v>
       </c>
-      <c r="C142" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="D142" s="11"/>
-    </row>
-    <row r="143" spans="1:4">
+      <c r="C142" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="D142" s="21"/>
+    </row>
+    <row r="143" ht="25.5" spans="1:4">
       <c r="A143" s="19"/>
       <c r="B143" s="18">
         <v>1</v>
       </c>
-      <c r="C143" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="D143" s="11"/>
-    </row>
-    <row r="144" ht="66.75" spans="1:4">
+      <c r="C143" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D143" s="21"/>
+    </row>
+    <row r="144" ht="25.5" spans="1:4">
       <c r="A144" s="19"/>
       <c r="B144" s="18">
         <v>5</v>
       </c>
-      <c r="C144" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="D144" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="145" ht="26.25" spans="1:4">
+      <c r="C144" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="D144" s="21"/>
+    </row>
+    <row r="145" ht="92.25" spans="1:4">
       <c r="A145" s="19"/>
       <c r="B145" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="D145" s="11"/>
-    </row>
-    <row r="146" ht="66.75" spans="1:4">
+        <v>204</v>
+      </c>
+      <c r="D145" s="21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="146" ht="27" spans="1:4">
       <c r="A146" s="19"/>
       <c r="B146" s="18">
         <v>5</v>
       </c>
       <c r="C146" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="D146" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="D146" s="11" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="147" ht="25.5" spans="1:4">
+    </row>
+    <row r="147" ht="24" spans="1:4">
       <c r="A147" s="19"/>
       <c r="B147" s="18">
         <v>1</v>
       </c>
-      <c r="C147" s="12" t="s">
-        <v>209</v>
+      <c r="C147" s="23" t="s">
+        <v>208</v>
       </c>
       <c r="D147" s="21"/>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" ht="25.5" spans="1:4">
       <c r="A148" s="19"/>
       <c r="B148" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C148" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D148" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="D148" s="21"/>
-    </row>
-    <row r="149" ht="78.75" spans="1:4">
+    </row>
+    <row r="149" ht="53.25" spans="1:4">
       <c r="A149" s="19"/>
       <c r="B149" s="18">
         <v>5</v>
       </c>
-      <c r="C149" s="12" t="s">
+      <c r="C149" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="D149" s="21" t="s">
+      <c r="D149" s="11" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="150" ht="26.25" spans="1:4">
-      <c r="A150" s="19"/>
+    <row r="150" ht="119.25" spans="1:4">
+      <c r="A150" s="25"/>
       <c r="B150" s="18">
         <v>5</v>
       </c>
-      <c r="C150" s="22" t="s">
+      <c r="C150" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="D150" s="21"/>
-    </row>
-    <row r="151" spans="1:4">
-      <c r="A151" s="19"/>
+      <c r="D150" s="11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="151" ht="25.5" spans="1:4">
+      <c r="A151" s="26" t="s">
+        <v>215</v>
+      </c>
       <c r="B151" s="18">
         <v>1</v>
       </c>
-      <c r="C151" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="D151" s="21"/>
+      <c r="C151" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="D151" s="11"/>
     </row>
     <row r="152" ht="39.75" spans="1:4">
-      <c r="A152" s="19"/>
+      <c r="A152" s="26"/>
       <c r="B152" s="18">
-        <v>1</v>
-      </c>
-      <c r="C152" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="D152" s="21"/>
-    </row>
-    <row r="153" ht="25.5" spans="1:4">
-      <c r="A153" s="19"/>
+        <v>5</v>
+      </c>
+      <c r="C152" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="D152" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="153" ht="131" customHeight="1" spans="1:4">
+      <c r="A153" s="26"/>
       <c r="B153" s="18">
         <v>1</v>
       </c>
-      <c r="C153" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="D153" s="21"/>
-    </row>
-    <row r="154" ht="25.5" spans="1:4">
-      <c r="A154" s="19"/>
-      <c r="B154" s="18">
-        <v>5</v>
-      </c>
-      <c r="C154" s="22" t="s">
-        <v>217</v>
-      </c>
-      <c r="D154" s="21"/>
-    </row>
-    <row r="155" ht="92.25" spans="1:4">
-      <c r="A155" s="19"/>
-      <c r="B155" s="18">
-        <v>5</v>
-      </c>
-      <c r="C155" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="D155" s="21" t="s">
+      <c r="C153" s="12" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="156" ht="27" spans="1:4">
-      <c r="A156" s="19"/>
-      <c r="B156" s="18">
-        <v>5</v>
-      </c>
-      <c r="C156" s="12" t="s">
+      <c r="D153" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="D156" s="21" t="s">
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" s="26"/>
+      <c r="B154" s="18"/>
+      <c r="C154" s="12"/>
+      <c r="D154" s="11"/>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" s="26"/>
+      <c r="B155" s="18"/>
+      <c r="C155" s="12"/>
+      <c r="D155" s="11"/>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" s="26"/>
+      <c r="B156" s="18"/>
+      <c r="C156" s="12"/>
+      <c r="D156" s="11"/>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="26"/>
+      <c r="B157" s="18"/>
+      <c r="C157" s="12"/>
+      <c r="D157" s="11"/>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="26"/>
+      <c r="B158" s="18"/>
+      <c r="C158" s="12"/>
+      <c r="D158" s="11"/>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" s="26" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="157" ht="24" spans="1:4">
-      <c r="A157" s="19"/>
-      <c r="B157" s="18">
+      <c r="B159" s="18">
+        <v>2</v>
+      </c>
+      <c r="C159" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="D159" s="11"/>
+    </row>
+    <row r="160" ht="25.5" spans="1:4">
+      <c r="A160" s="26"/>
+      <c r="B160" s="18">
         <v>1</v>
       </c>
-      <c r="C157" s="23" t="s">
-        <v>222</v>
-      </c>
-      <c r="D157" s="21"/>
-    </row>
-    <row r="158" ht="146.25" spans="1:4">
-      <c r="A158" s="19"/>
-      <c r="B158" s="18">
-        <v>5</v>
-      </c>
-      <c r="C158" s="12" t="s">
+      <c r="C160" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="D158" s="21" t="s">
+      <c r="D160" s="11"/>
+    </row>
+    <row r="161" ht="25.5" spans="1:4">
+      <c r="A161" s="26"/>
+      <c r="B161" s="18">
+        <v>1</v>
+      </c>
+      <c r="C161" s="12" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="159" ht="25.5" spans="1:4">
-      <c r="A159" s="19"/>
-      <c r="B159" s="18">
-        <v>5</v>
-      </c>
-      <c r="C159" s="12" t="s">
+      <c r="D161" s="11"/>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="26"/>
+      <c r="B162" s="18">
+        <v>1</v>
+      </c>
+      <c r="C162" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D159" s="11" t="s">
+      <c r="D162" s="11"/>
+    </row>
+    <row r="163" ht="25.5" spans="1:4">
+      <c r="A163" s="26"/>
+      <c r="B163" s="18">
+        <v>1</v>
+      </c>
+      <c r="C163" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="160" ht="53.25" spans="1:4">
-      <c r="A160" s="19"/>
-      <c r="B160" s="18">
-        <v>5</v>
-      </c>
-      <c r="C160" s="24" t="s">
-        <v>227</v>
-      </c>
-      <c r="D160" s="11" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="161" ht="28.5" spans="1:4">
-      <c r="A161" s="19"/>
-      <c r="B161" s="18">
-        <v>2</v>
-      </c>
-      <c r="C161" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="D161" s="11"/>
-    </row>
-    <row r="162" ht="119.25" spans="1:4">
-      <c r="A162" s="25"/>
-      <c r="B162" s="18">
-        <v>5</v>
-      </c>
-      <c r="C162" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="D162" s="11" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="163" ht="66.75" spans="1:4">
-      <c r="A163" s="26" t="s">
-        <v>232</v>
-      </c>
-      <c r="B163" s="18">
-        <v>5</v>
-      </c>
-      <c r="C163" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="D163" s="11" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="164" ht="38.25" spans="1:4">
+      <c r="D163" s="11"/>
+    </row>
+    <row r="164" spans="1:4">
       <c r="A164" s="26"/>
       <c r="B164" s="18">
         <v>1</v>
       </c>
-      <c r="C164" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="D164" s="11" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4">
+      <c r="C164" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D164" s="11"/>
+    </row>
+    <row r="165" ht="25.5" spans="1:4">
       <c r="A165" s="26"/>
       <c r="B165" s="18">
         <v>1</v>
       </c>
-      <c r="C165" s="12" t="s">
-        <v>237</v>
+      <c r="C165" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="D165" s="11"/>
     </row>
-    <row r="166" ht="109" customHeight="1" spans="1:4">
+    <row r="166" ht="25.5" spans="1:4">
       <c r="A166" s="26"/>
       <c r="B166" s="18">
-        <v>5</v>
-      </c>
-      <c r="C166" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="D166" s="11" t="s">
-        <v>239</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D166" s="11"/>
     </row>
     <row r="167" ht="25.5" spans="1:4">
       <c r="A167" s="26"/>
       <c r="B167" s="18">
-        <v>2</v>
-      </c>
-      <c r="C167" s="12" t="s">
-        <v>240</v>
+        <v>1</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="D167" s="11"/>
     </row>
-    <row r="168" ht="51" spans="1:4">
+    <row r="168" ht="25.5" spans="1:4">
       <c r="A168" s="26"/>
       <c r="B168" s="18">
-        <v>2</v>
-      </c>
-      <c r="C168" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="D168" s="11" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="169" ht="25.5" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D168" s="11"/>
+    </row>
+    <row r="169" ht="108" spans="1:4">
       <c r="A169" s="26"/>
       <c r="B169" s="18">
-        <v>2</v>
-      </c>
-      <c r="C169" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="D169" s="11"/>
-    </row>
-    <row r="170" ht="28.5" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D169" s="11" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="170" ht="66.75" spans="1:4">
       <c r="A170" s="26"/>
       <c r="B170" s="18">
         <v>5</v>
       </c>
-      <c r="C170" s="24" t="s">
-        <v>244</v>
+      <c r="C170" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="D170" s="11" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="171" ht="40.5" spans="1:4">
-      <c r="A171" s="26" t="s">
-        <v>246</v>
-      </c>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="171" ht="147" spans="1:4">
+      <c r="A171" s="26"/>
       <c r="B171" s="18">
         <v>5</v>
       </c>
-      <c r="C171" s="27" t="s">
-        <v>247</v>
+      <c r="C171" s="12" t="s">
+        <v>236</v>
       </c>
       <c r="D171" s="27" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="172" ht="42" customHeight="1" spans="1:4">
-      <c r="A172" s="26"/>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="172" ht="66.75" spans="1:4">
+      <c r="A172" s="26" t="s">
+        <v>238</v>
+      </c>
       <c r="B172" s="18">
         <v>5</v>
       </c>
       <c r="C172" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="D172" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="173" ht="42" customHeight="1" spans="1:4">
+        <v>239</v>
+      </c>
+      <c r="D172" s="11" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="173" ht="38.25" spans="1:4">
       <c r="A173" s="26"/>
-      <c r="B173" s="28">
-        <v>2</v>
+      <c r="B173" s="18">
+        <v>1</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="D173" s="12"/>
-    </row>
-    <row r="174" ht="42" customHeight="1" spans="1:4">
+        <v>241</v>
+      </c>
+      <c r="D173" s="11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
       <c r="A174" s="26"/>
       <c r="B174" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C174" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="D174" s="12" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="175" ht="82" customHeight="1" spans="1:4">
+        <v>243</v>
+      </c>
+      <c r="D174" s="11"/>
+    </row>
+    <row r="175" ht="109" customHeight="1" spans="1:4">
       <c r="A175" s="26"/>
       <c r="B175" s="18">
         <v>5</v>
       </c>
       <c r="C175" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="D175" s="12" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="176" ht="54" spans="1:4">
+        <v>244</v>
+      </c>
+      <c r="D175" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="176" ht="25.5" spans="1:4">
       <c r="A176" s="26"/>
-      <c r="B176" s="28">
-        <v>5</v>
+      <c r="B176" s="18">
+        <v>2</v>
       </c>
       <c r="C176" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="D176" s="12" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="177" ht="13.5" spans="1:4">
+        <v>246</v>
+      </c>
+      <c r="D176" s="11"/>
+    </row>
+    <row r="177" ht="51" spans="1:4">
       <c r="A177" s="26"/>
       <c r="B177" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C177" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="D177" s="12" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="178" ht="220" customHeight="1" spans="1:4">
+        <v>247</v>
+      </c>
+      <c r="D177" s="11" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="178" ht="25.5" spans="1:4">
       <c r="A178" s="26"/>
       <c r="B178" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C178" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="D178" s="12" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="179" ht="27" spans="1:4">
+        <v>249</v>
+      </c>
+      <c r="D178" s="11"/>
+    </row>
+    <row r="179" ht="28.5" spans="1:4">
       <c r="A179" s="26"/>
       <c r="B179" s="18">
         <v>5</v>
       </c>
-      <c r="C179" s="12" t="s">
-        <v>262</v>
-      </c>
-      <c r="D179" s="12" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="180" ht="119.25" spans="1:4">
-      <c r="A180" s="26"/>
+      <c r="C179" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="D179" s="11" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="180" ht="54" spans="1:4">
+      <c r="A180" s="26" t="s">
+        <v>252</v>
+      </c>
       <c r="B180" s="18">
         <v>5</v>
       </c>
-      <c r="C180" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D180" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="181" ht="39" spans="1:4">
+      <c r="C180" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="D180" s="28" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="181" ht="42" customHeight="1" spans="1:4">
       <c r="A181" s="26"/>
       <c r="B181" s="18">
         <v>5</v>
       </c>
-      <c r="C181" s="2" t="s">
+      <c r="C181" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="D181" s="12" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="182" ht="42" customHeight="1" spans="1:4">
+      <c r="A182" s="26"/>
+      <c r="B182" s="29">
+        <v>2</v>
+      </c>
+      <c r="C182" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="D182" s="12"/>
+    </row>
+    <row r="183" ht="42" customHeight="1" spans="1:4">
+      <c r="A183" s="26"/>
+      <c r="B183" s="18">
+        <v>5</v>
+      </c>
+      <c r="C183" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="D183" s="12" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="184" ht="82" customHeight="1" spans="1:4">
+      <c r="A184" s="26"/>
+      <c r="B184" s="18">
+        <v>5</v>
+      </c>
+      <c r="C184" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="D184" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="185" ht="54" spans="1:4">
+      <c r="A185" s="26"/>
+      <c r="B185" s="29">
+        <v>5</v>
+      </c>
+      <c r="C185" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="D185" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="186" ht="13.5" spans="1:4">
+      <c r="A186" s="26"/>
+      <c r="B186" s="18">
+        <v>5</v>
+      </c>
+      <c r="C186" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D186" s="12" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="187" ht="220" customHeight="1" spans="1:4">
+      <c r="A187" s="26" t="s">
         <v>266</v>
       </c>
-      <c r="D181" s="2" t="s">
+      <c r="B187" s="18">
+        <v>5</v>
+      </c>
+      <c r="C187" s="12" t="s">
         <v>267</v>
       </c>
+      <c r="D187" s="12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="188" ht="27" spans="1:4">
+      <c r="A188" s="26"/>
+      <c r="B188" s="18">
+        <v>5</v>
+      </c>
+      <c r="C188" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="D188" s="12" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="189" ht="132.75" spans="1:4">
+      <c r="A189" s="26"/>
+      <c r="B189" s="18">
+        <v>5</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="190" ht="39" spans="1:4">
+      <c r="A190" s="26"/>
+      <c r="B190" s="18">
+        <v>5</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>274</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A17"/>
-    <mergeCell ref="A18:A52"/>
-    <mergeCell ref="A53:A96"/>
-    <mergeCell ref="A97:A162"/>
-    <mergeCell ref="A163:A170"/>
-    <mergeCell ref="A171:A177"/>
-    <mergeCell ref="A178:A181"/>
+    <mergeCell ref="A18:A54"/>
+    <mergeCell ref="A55:A98"/>
+    <mergeCell ref="A99:A150"/>
+    <mergeCell ref="A151:A158"/>
+    <mergeCell ref="A159:A171"/>
+    <mergeCell ref="A172:A179"/>
+    <mergeCell ref="A180:A186"/>
+    <mergeCell ref="A187:A190"/>
   </mergeCells>
   <conditionalFormatting sqref="B$1:B$1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
@@ -4178,7 +4250,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C127" r:id="rId1" display="Panoptic Segmentation" tooltip="https://arxiv.org/abs/1801.00868"/>
+    <hyperlink ref="C125" r:id="rId1" display="Panoptic Segmentation" tooltip="https://arxiv.org/abs/1801.00868"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
add some cvpr2019 parpers on semantic segmentation
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14625" windowHeight="25770" tabRatio="354"/>
+    <workbookView windowWidth="27225" windowHeight="13170" tabRatio="354"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="229">
   <si>
     <t>Scope</t>
   </si>
@@ -244,6 +244,9 @@
     <t>An Empirical Study of Spatial Attention Mechanisms in Deep Networks</t>
   </si>
   <si>
+    <t>object detection</t>
+  </si>
+  <si>
     <t>1. (Done)SSD: Single Shot MultiBox Detector</t>
   </si>
   <si>
@@ -553,6 +556,9 @@
     <t>(cvpr2019)Devil is in the Edges: Learning Semantic Boundaries from Noisy Annotations</t>
   </si>
   <si>
+    <t>treat the underlying ground truth boundaries as a latent variable that is jointly optimized druing training</t>
+  </si>
+  <si>
     <t>(cvpr2019, 感觉像是一种剪枝的方法) SparseMask: Differentiable Connectivity Learning for Dense Image Prediction</t>
   </si>
   <si>
@@ -581,6 +587,15 @@
   </si>
   <si>
     <t>Taking A Closer Look at Domain Shift: Category-level Adversaries for Semantics Consistent Domain Adaptation</t>
+  </si>
+  <si>
+    <t>A Simple Pooling-Based Design for Real-Time Salient Object Detection</t>
+  </si>
+  <si>
+    <t>Decoders Matter for Semantic Segmentation_Data-Dependent Decoding Enables Flexible Feature Aggregation</t>
+  </si>
+  <si>
+    <t>In Defense of Pre-trained ImageNet Architectures for Real-time Semantic Segmentation of Road-driving Images</t>
   </si>
   <si>
     <t>Real-time
@@ -604,7 +619,8 @@
 重点propose 了一种结构，把不同level的feature融合在一起，卷积层最大的stride是64
 sub-net work aggregation: stack of backbones by feeding the output of previous backbone to the next, allow hight level features to be processed again to further evaluate and re-access higher orderspatial relationship
 sub-stage aggregation: always from high resolution to low resolution...其实没有太看懂这部分的动机，一个可能的原因是通过多个路径来减少vanishing gradient
-为了使结构简单，提出并复用了一个Xceptiion的修改版back bone
+为了使结构简单，提出并复用了一个Xceptiion的修改版back bone，可以使得收敛更好；
+加decoder， 可以使得梯度更容易传导，优化更容易一些
 FC attention provides evidence for the effect of hight-dimensional context</t>
   </si>
   <si>
@@ -795,10 +811,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -843,8 +859,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -866,8 +890,85 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -881,56 +982,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -944,44 +997,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1020,7 +1036,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1032,7 +1048,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1050,157 +1210,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1291,30 +1307,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1325,17 +1317,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1357,163 +1338,198 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1582,9 +1598,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1964,10 +1977,10 @@
   <sheetPr/>
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C111" sqref="C111"/>
+      <selection pane="bottomLeft" activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -2068,7 +2081,7 @@
       </c>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" ht="25.5" spans="1:4">
+    <row r="9" spans="1:4">
       <c r="A9" s="9"/>
       <c r="B9" s="10">
         <v>2</v>
@@ -2078,7 +2091,7 @@
       </c>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" ht="51.75" spans="1:4">
+    <row r="10" ht="39" spans="1:4">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -2182,7 +2195,7 @@
       </c>
       <c r="D18" s="11"/>
     </row>
-    <row r="19" ht="25.5" spans="1:4">
+    <row r="19" spans="1:4">
       <c r="A19" s="9"/>
       <c r="B19" s="16">
         <v>1</v>
@@ -2302,7 +2315,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" ht="38.25" spans="1:4">
+    <row r="30" ht="25.5" spans="1:4">
       <c r="A30" s="9"/>
       <c r="B30" s="16">
         <v>2</v>
@@ -2404,7 +2417,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" ht="25.5" spans="1:4">
+    <row r="39" spans="1:4">
       <c r="A39" s="9"/>
       <c r="B39" s="14">
         <v>5</v>
@@ -2494,27 +2507,29 @@
       <c r="A48" s="9"/>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="9"/>
+      <c r="A49" s="9" t="s">
+        <v>71</v>
+      </c>
       <c r="B49" s="14">
         <v>5</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D49" s="11"/>
       <c r="F49" s="19"/>
       <c r="G49" s="19"/>
     </row>
-    <row r="50" ht="51.75" spans="1:6">
+    <row r="50" ht="40.5" spans="1:6">
       <c r="A50" s="9"/>
       <c r="B50" s="14">
         <v>5</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F50" s="1"/>
     </row>
@@ -2524,10 +2539,10 @@
         <v>5</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" ht="66.75" spans="1:4">
@@ -2536,22 +2551,22 @@
         <v>5</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="53" ht="25.5" spans="1:4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" ht="13.5" spans="1:4">
       <c r="A53" s="9"/>
       <c r="B53" s="17">
         <v>5</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" ht="40.5" spans="1:4">
@@ -2560,10 +2575,10 @@
         <v>5</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" ht="25.5" spans="1:4">
@@ -2572,7 +2587,7 @@
         <v>2</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D55" s="11"/>
     </row>
@@ -2582,10 +2597,10 @@
         <v>5</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" ht="40.5" spans="1:4">
@@ -2594,10 +2609,10 @@
         <v>5</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" ht="25.5" spans="1:4">
@@ -2606,7 +2621,7 @@
         <v>1</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D58" s="11"/>
     </row>
@@ -2637,7 +2652,7 @@
         <v>5</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D63" s="11"/>
     </row>
@@ -2647,22 +2662,22 @@
         <v>6</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="65" ht="25.5" spans="1:4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="65" ht="13.5" spans="1:4">
       <c r="A65" s="18"/>
       <c r="B65" s="17">
         <v>5</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" ht="27" spans="1:4">
@@ -2671,10 +2686,10 @@
         <v>5</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" ht="92.25" spans="1:4">
@@ -2683,10 +2698,10 @@
         <v>5</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="68" ht="93" spans="1:4">
@@ -2695,10 +2710,10 @@
         <v>5</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="69" ht="147.75" spans="1:4">
@@ -2707,10 +2722,10 @@
         <v>5</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70" ht="53.25" spans="1:4">
@@ -2719,10 +2734,10 @@
         <v>5</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" ht="106.5" spans="1:4">
@@ -2731,19 +2746,19 @@
         <v>5</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="72" ht="25.5" spans="1:4">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="18"/>
       <c r="B72" s="17">
         <v>5</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D72" s="11"/>
     </row>
@@ -2753,7 +2768,7 @@
         <v>5</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D73" s="11"/>
     </row>
@@ -2763,7 +2778,7 @@
         <v>2</v>
       </c>
       <c r="C74" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D74" s="11"/>
     </row>
@@ -2773,7 +2788,7 @@
         <v>5</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D75" s="11"/>
     </row>
@@ -2783,7 +2798,7 @@
         <v>2</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D76" s="11"/>
     </row>
@@ -2793,10 +2808,10 @@
         <v>5</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="78" ht="39" spans="1:4">
@@ -2805,10 +2820,10 @@
         <v>5</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" ht="144" spans="1:4">
@@ -2817,10 +2832,10 @@
         <v>5</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" ht="27" spans="1:4">
@@ -2829,10 +2844,10 @@
         <v>5</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="81" ht="40.5" spans="1:4">
@@ -2841,10 +2856,10 @@
         <v>5</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="82" ht="40.5" spans="1:4">
@@ -2853,10 +2868,10 @@
         <v>5</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="83" ht="134.25" spans="1:4">
@@ -2865,10 +2880,10 @@
         <v>5</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="84" ht="54" spans="1:4">
@@ -2877,10 +2892,10 @@
         <v>5</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="85" ht="40.5" spans="1:4">
@@ -2889,10 +2904,10 @@
         <v>5</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="86" ht="27" spans="1:4">
@@ -2901,10 +2916,10 @@
         <v>5</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="87" ht="25.5" spans="1:4">
@@ -2913,7 +2928,7 @@
         <v>2</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D87" s="11"/>
     </row>
@@ -2923,7 +2938,7 @@
         <v>2</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D88" s="11"/>
     </row>
@@ -2933,7 +2948,7 @@
         <v>2</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D89" s="11"/>
     </row>
@@ -2943,7 +2958,7 @@
         <v>2</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D90" s="11"/>
     </row>
@@ -2953,7 +2968,7 @@
         <v>2</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D91" s="11"/>
     </row>
@@ -2963,10 +2978,10 @@
         <v>5</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="93" ht="26.25" spans="1:4">
@@ -2975,7 +2990,7 @@
         <v>2</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D93" s="11"/>
     </row>
@@ -2985,10 +3000,10 @@
         <v>5</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="95" ht="25.5" spans="1:4">
@@ -2997,7 +3012,7 @@
         <v>2</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D95" s="20"/>
     </row>
@@ -3007,10 +3022,10 @@
         <v>5</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D96" s="20" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="97" ht="26.25" spans="1:4">
@@ -3019,7 +3034,7 @@
         <v>5</v>
       </c>
       <c r="C97" s="21" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D97" s="20"/>
     </row>
@@ -3029,7 +3044,7 @@
         <v>2</v>
       </c>
       <c r="C98" s="21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D98" s="20"/>
     </row>
@@ -3039,7 +3054,7 @@
         <v>2</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D99" s="20"/>
     </row>
@@ -3049,7 +3064,7 @@
         <v>5</v>
       </c>
       <c r="C100" s="21" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D100" s="20"/>
     </row>
@@ -3059,10 +3074,10 @@
         <v>5</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D101" s="20" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="102" ht="27" spans="1:4">
@@ -3071,10 +3086,10 @@
         <v>5</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D102" s="20" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="103" ht="25.5" spans="1:4">
@@ -3083,10 +3098,10 @@
         <v>5</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D103" s="11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="104" ht="53.25" spans="1:4">
@@ -3095,527 +3110,541 @@
         <v>5</v>
       </c>
       <c r="C104" s="22" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="105" ht="119.25" spans="1:4">
-      <c r="A105" s="23"/>
+      <c r="A105" s="18"/>
       <c r="B105" s="17">
         <v>5</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="106" ht="25.5" spans="1:4">
-      <c r="A106" s="23"/>
-      <c r="B106" s="24">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="106" ht="31" customHeight="1" spans="1:4">
+      <c r="A106" s="18"/>
+      <c r="B106" s="23">
         <v>1</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D106" s="12"/>
+        <v>158</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="107" ht="39" spans="1:4">
-      <c r="A107" s="23"/>
-      <c r="B107" s="24">
+      <c r="A107" s="18"/>
+      <c r="B107" s="23">
         <v>1</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D107" s="12"/>
     </row>
     <row r="108" ht="25.5" spans="1:4">
-      <c r="A108" s="23"/>
-      <c r="B108" s="24">
+      <c r="A108" s="18"/>
+      <c r="B108" s="23">
         <v>1</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D108" s="12"/>
     </row>
     <row r="109" ht="25.5" spans="1:4">
-      <c r="A109" s="23"/>
-      <c r="B109" s="24">
+      <c r="A109" s="18"/>
+      <c r="B109" s="23">
         <v>1</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D109" s="12"/>
     </row>
     <row r="110" ht="25.5" spans="1:4">
-      <c r="A110" s="23"/>
-      <c r="B110" s="24">
+      <c r="A110" s="18"/>
+      <c r="B110" s="23">
         <v>1</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D110" s="12"/>
     </row>
     <row r="111" ht="25.5" spans="1:4">
-      <c r="A111" s="23"/>
-      <c r="B111" s="24">
+      <c r="A111" s="18"/>
+      <c r="B111" s="23">
         <v>1</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D111" s="12"/>
     </row>
     <row r="112" ht="25.5" spans="1:4">
-      <c r="A112" s="23"/>
-      <c r="B112" s="24">
+      <c r="A112" s="18"/>
+      <c r="B112" s="23">
         <v>1</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D112" s="12"/>
     </row>
     <row r="113" ht="25.5" spans="1:4">
-      <c r="A113" s="23"/>
-      <c r="B113" s="24">
+      <c r="A113" s="18"/>
+      <c r="B113" s="23">
         <v>1</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D113" s="12"/>
     </row>
     <row r="114" ht="25.5" spans="1:4">
-      <c r="A114" s="23"/>
-      <c r="B114" s="24">
+      <c r="A114" s="18"/>
+      <c r="B114" s="23">
         <v>1</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D114" s="12"/>
     </row>
     <row r="115" ht="25.5" spans="1:4">
-      <c r="A115" s="23"/>
-      <c r="B115" s="24">
+      <c r="A115" s="18"/>
+      <c r="B115" s="23">
         <v>1</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D115" s="12"/>
     </row>
     <row r="116" ht="25.5" spans="1:4">
-      <c r="A116" s="23"/>
-      <c r="B116" s="24">
+      <c r="A116" s="18"/>
+      <c r="B116" s="23">
         <v>1</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D116" s="12"/>
     </row>
-    <row r="117" spans="1:4">
-      <c r="A117" s="23"/>
-      <c r="B117" s="24"/>
-      <c r="C117" s="12"/>
+    <row r="117" ht="25.5" spans="1:4">
+      <c r="A117" s="18"/>
+      <c r="B117" s="23">
+        <v>1</v>
+      </c>
+      <c r="C117" s="12" t="s">
+        <v>170</v>
+      </c>
       <c r="D117" s="12"/>
     </row>
-    <row r="118" spans="1:4">
-      <c r="A118" s="23"/>
-      <c r="B118" s="24"/>
-      <c r="C118" s="12"/>
+    <row r="118" ht="25.5" spans="1:4">
+      <c r="A118" s="18"/>
+      <c r="B118" s="23">
+        <v>1</v>
+      </c>
+      <c r="C118" s="12" t="s">
+        <v>171</v>
+      </c>
       <c r="D118" s="12"/>
     </row>
-    <row r="119" spans="1:4">
-      <c r="A119" s="23"/>
-      <c r="B119" s="24"/>
-      <c r="C119" s="12"/>
+    <row r="119" ht="25.5" spans="1:4">
+      <c r="A119" s="18"/>
+      <c r="B119" s="23">
+        <v>1</v>
+      </c>
+      <c r="C119" s="12" t="s">
+        <v>172</v>
+      </c>
       <c r="D119" s="12"/>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="23"/>
-      <c r="B120" s="24"/>
+      <c r="A120" s="18"/>
+      <c r="B120" s="23"/>
       <c r="C120" s="12"/>
       <c r="D120" s="12"/>
     </row>
     <row r="121" spans="1:1">
-      <c r="A121" s="25"/>
+      <c r="A121" s="24"/>
     </row>
     <row r="122" ht="25.5" spans="1:4">
-      <c r="A122" s="26" t="s">
-        <v>168</v>
+      <c r="A122" s="25" t="s">
+        <v>173</v>
       </c>
       <c r="B122" s="17">
         <v>1</v>
       </c>
       <c r="C122" s="12" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="D122" s="11"/>
     </row>
     <row r="123" ht="39.75" spans="1:4">
-      <c r="A123" s="26"/>
+      <c r="A123" s="25"/>
       <c r="B123" s="17">
         <v>5</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="D123" s="11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="124" ht="131" customHeight="1" spans="1:4">
-      <c r="A124" s="26"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="124" ht="235" customHeight="1" spans="1:4">
+      <c r="A124" s="25"/>
       <c r="B124" s="17">
         <v>5</v>
       </c>
       <c r="C124" s="12" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D124" s="11" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="125" spans="1:4">
-      <c r="A125" s="26" t="s">
-        <v>174</v>
+      <c r="A125" s="25" t="s">
+        <v>179</v>
       </c>
       <c r="B125" s="17">
         <v>2</v>
       </c>
       <c r="C125" s="12" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="D125" s="11"/>
     </row>
     <row r="126" spans="1:4">
-      <c r="A126" s="26"/>
+      <c r="A126" s="25"/>
       <c r="B126" s="17">
         <v>1</v>
       </c>
       <c r="C126" s="12" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="D126" s="11"/>
     </row>
     <row r="127" ht="25.5" spans="1:4">
-      <c r="A127" s="26"/>
+      <c r="A127" s="25"/>
       <c r="B127" s="17">
         <v>1</v>
       </c>
       <c r="C127" s="12" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D127" s="11"/>
     </row>
     <row r="128" spans="1:4">
-      <c r="A128" s="26"/>
+      <c r="A128" s="25"/>
       <c r="B128" s="17">
         <v>1</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="D128" s="11"/>
     </row>
     <row r="129" spans="1:4">
-      <c r="A129" s="26"/>
+      <c r="A129" s="25"/>
       <c r="B129" s="17">
         <v>1</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D129" s="11"/>
     </row>
     <row r="130" spans="1:4">
-      <c r="A130" s="26"/>
+      <c r="A130" s="25"/>
       <c r="B130" s="17">
         <v>1</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D130" s="11"/>
     </row>
     <row r="131" ht="25.5" spans="1:4">
-      <c r="A131" s="26"/>
+      <c r="A131" s="25"/>
       <c r="B131" s="17">
         <v>1</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="D131" s="11"/>
     </row>
     <row r="132" ht="25.5" spans="1:4">
-      <c r="A132" s="26"/>
+      <c r="A132" s="25"/>
       <c r="B132" s="17">
         <v>1</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D132" s="11"/>
     </row>
-    <row r="133" ht="25.5" spans="1:4">
-      <c r="A133" s="26"/>
+    <row r="133" spans="1:4">
+      <c r="A133" s="25"/>
       <c r="B133" s="17">
         <v>1</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="D133" s="11"/>
     </row>
     <row r="134" ht="25.5" spans="1:4">
-      <c r="A134" s="26"/>
+      <c r="A134" s="25"/>
       <c r="B134" s="17">
         <v>1</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="D134" s="11"/>
     </row>
     <row r="135" ht="25.5" spans="1:4">
-      <c r="A135" s="26"/>
+      <c r="A135" s="25"/>
       <c r="B135" s="17">
         <v>1</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D135" s="11"/>
     </row>
     <row r="136" ht="108" spans="1:4">
-      <c r="A136" s="26"/>
+      <c r="A136" s="25"/>
       <c r="B136" s="17">
         <v>5</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="D136" s="11" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="137" ht="66.75" spans="1:4">
-      <c r="A137" s="26"/>
+      <c r="A137" s="25"/>
       <c r="B137" s="17">
         <v>5</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="D137" s="11" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="138" ht="147" spans="1:4">
-      <c r="A138" s="26"/>
+      <c r="A138" s="25"/>
       <c r="B138" s="17">
         <v>5</v>
       </c>
       <c r="C138" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D138" s="27" t="s">
-        <v>191</v>
+        <v>195</v>
+      </c>
+      <c r="D138" s="26" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="139" ht="66.75" spans="1:4">
-      <c r="A139" s="26" t="s">
-        <v>192</v>
+      <c r="A139" s="25" t="s">
+        <v>197</v>
       </c>
       <c r="B139" s="17">
         <v>5</v>
       </c>
       <c r="C139" s="12" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="D139" s="11" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="140" ht="38.25" spans="1:4">
-      <c r="A140" s="26"/>
+      <c r="A140" s="25"/>
       <c r="B140" s="17">
         <v>5</v>
       </c>
       <c r="C140" s="12" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="D140" s="11" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="141" spans="1:4">
-      <c r="A141" s="26"/>
+      <c r="A141" s="25"/>
       <c r="B141" s="17">
         <v>2</v>
       </c>
       <c r="C141" s="12" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="D141" s="11"/>
     </row>
     <row r="142" ht="109" customHeight="1" spans="1:4">
-      <c r="A142" s="26"/>
+      <c r="A142" s="25"/>
       <c r="B142" s="17">
         <v>5</v>
       </c>
       <c r="C142" s="12" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="D142" s="11" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="143" ht="28.5" spans="1:4">
-      <c r="A143" s="26"/>
+      <c r="A143" s="25"/>
       <c r="B143" s="17">
         <v>5</v>
       </c>
       <c r="C143" s="22" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D143" s="11" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="144" ht="54" spans="1:4">
-      <c r="A144" s="26" t="s">
-        <v>202</v>
+      <c r="A144" s="25" t="s">
+        <v>207</v>
       </c>
       <c r="B144" s="17">
         <v>5</v>
       </c>
-      <c r="C144" s="28" t="s">
-        <v>203</v>
-      </c>
-      <c r="D144" s="28" t="s">
-        <v>204</v>
+      <c r="C144" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="D144" s="27" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="145" ht="42" customHeight="1" spans="1:4">
-      <c r="A145" s="26"/>
+      <c r="A145" s="25"/>
       <c r="B145" s="17">
         <v>5</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="D145" s="12" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
     </row>
     <row r="146" ht="42" customHeight="1" spans="1:4">
-      <c r="A146" s="26"/>
+      <c r="A146" s="25"/>
       <c r="B146" s="17">
         <v>5</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="D146" s="12" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="147" ht="82" customHeight="1" spans="1:4">
-      <c r="A147" s="26"/>
+      <c r="A147" s="25"/>
       <c r="B147" s="17">
         <v>5</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="D147" s="12" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
     </row>
     <row r="148" ht="54" spans="1:4">
-      <c r="A148" s="26"/>
-      <c r="B148" s="24">
+      <c r="A148" s="25"/>
+      <c r="B148" s="23">
         <v>5</v>
       </c>
       <c r="C148" s="12" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="D148" s="12" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
     </row>
     <row r="149" ht="13.5" spans="1:4">
-      <c r="A149" s="26"/>
+      <c r="A149" s="25"/>
       <c r="B149" s="17">
         <v>5</v>
       </c>
       <c r="C149" s="12" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D149" s="12" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="150" ht="220" customHeight="1" spans="1:4">
-      <c r="A150" s="26" t="s">
-        <v>215</v>
+      <c r="A150" s="25" t="s">
+        <v>220</v>
       </c>
       <c r="B150" s="17">
         <v>5</v>
       </c>
       <c r="C150" s="12" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="D150" s="12" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="151" ht="27" spans="1:4">
-      <c r="A151" s="26"/>
+      <c r="A151" s="25"/>
       <c r="B151" s="17">
         <v>5</v>
       </c>
       <c r="C151" s="12" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="D151" s="12" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="152" ht="132.75" spans="1:4">
-      <c r="A152" s="26"/>
+      <c r="A152" s="25"/>
       <c r="B152" s="17">
         <v>5</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
     </row>
     <row r="153" ht="39" spans="1:4">
-      <c r="A153" s="26"/>
+      <c r="A153" s="25"/>
       <c r="B153" s="17">
         <v>5</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add reading note on HRnet
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14670" windowHeight="25125" tabRatio="354"/>
+    <workbookView windowWidth="14565" windowHeight="11730" tabRatio="354"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="262">
   <si>
     <t>Scope</t>
   </si>
@@ -689,13 +689,41 @@
     <t>Task Decomposition and Synchronization for Semantic Biomedical Image Segmentation</t>
   </si>
   <si>
-    <t>(HRnet)Deep High-Resolution Representation Learning for Human Pose Estimation</t>
+    <t>(HRnetV1)Deep High-Resolution Representation Learning for Human Pose Estimation</t>
+  </si>
+  <si>
+    <t>创新点：
+1. 同时保持不同分辨率的feature map; 2. deep fusion: 在网络不同阶段都去融合不同分辨率的特征；</t>
   </si>
   <si>
     <t>(HRnet_V2)High-Resolution Representations for Labeling Pixels and Regions</t>
   </si>
   <si>
-    <t>参考文献相当丰富啊～related work中有不少相关工作， 对尤其对语义分割的文章的review比较充分</t>
+    <r>
+      <t>参考文献相当丰富啊～related work中有不少相关工作， 对尤其对语义分割的文章的review比较充分
+输入图片两次3x3 stride=2的卷积到1/4之的每个stage都保持1/4的分辨率，并且每个stage都添加一个low-resolution的feature map；网络中会fuse一下各个resolution的feature map，总共8个（</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>创新点在于高分辨率和低分辨率相互融合，而不是单向的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>）；最小的resolution为1/32；网络最后concate所有resolution的feature map 
+实验很充分</t>
+    </r>
   </si>
   <si>
     <t>Real-time
@@ -1721,7 +1749,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1796,6 +1824,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
@@ -2074,7 +2105,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14131290" y="5391150"/>
+          <a:off x="14131290" y="6362700"/>
           <a:ext cx="5536565" cy="2550795"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2351,10 +2382,10 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D186" sqref="D186"/>
+      <selection pane="bottomLeft" activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="15.75" outlineLevelCol="6"/>
@@ -3266,7 +3297,7 @@
       <c r="D85" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="E85" s="25" t="s">
+      <c r="E85" s="26" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3281,7 +3312,7 @@
       <c r="D86" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="E86" s="26" t="s">
+      <c r="E86" s="27" t="s">
         <v>126</v>
       </c>
     </row>
@@ -3574,7 +3605,7 @@
       <c r="D112" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="E112" s="26" t="s">
+      <c r="E112" s="27" t="s">
         <v>126</v>
       </c>
     </row>
@@ -3730,26 +3761,28 @@
     <row r="127" ht="31.5" spans="1:5">
       <c r="A127" s="20"/>
       <c r="B127" s="17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C127" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="D127" s="12"/>
+      <c r="D127" s="12" t="s">
+        <v>186</v>
+      </c>
       <c r="E127" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="128" ht="31.5" spans="1:5">
+    <row r="128" ht="108" spans="1:5">
       <c r="A128" s="20"/>
       <c r="B128" s="24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C128" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="D128" s="12" t="s">
         <v>187</v>
+      </c>
+      <c r="D128" s="25" t="s">
+        <v>188</v>
       </c>
       <c r="E128" t="s">
         <v>123</v>
@@ -3762,544 +3795,544 @@
       <c r="D129" s="12"/>
     </row>
     <row r="130" ht="31.5" hidden="1" spans="1:4">
-      <c r="A130" s="27" t="s">
-        <v>188</v>
+      <c r="A130" s="28" t="s">
+        <v>189</v>
       </c>
       <c r="B130" s="18">
         <v>1</v>
       </c>
       <c r="C130" s="12" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D130" s="11"/>
     </row>
     <row r="131" ht="141.75" hidden="1" spans="1:4">
-      <c r="A131" s="27"/>
+      <c r="A131" s="28"/>
       <c r="B131" s="24">
         <v>5</v>
       </c>
       <c r="C131" s="12" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D131" s="11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="132" ht="31.5" hidden="1" spans="1:4">
-      <c r="A132" s="27"/>
+      <c r="A132" s="28"/>
       <c r="B132" s="24">
         <v>1</v>
       </c>
       <c r="C132" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D132" s="11"/>
     </row>
     <row r="133" ht="31.5" hidden="1" spans="1:4">
-      <c r="A133" s="27"/>
+      <c r="A133" s="28"/>
       <c r="B133" s="18">
         <v>1</v>
       </c>
       <c r="C133" s="12" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D133" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="134" ht="31.5" hidden="1" spans="1:4">
-      <c r="A134" s="27"/>
+      <c r="A134" s="28"/>
       <c r="B134" s="18">
         <v>1</v>
       </c>
       <c r="C134" s="12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D134" s="11" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="135" ht="31.5" hidden="1" spans="1:4">
-      <c r="A135" s="27"/>
+      <c r="A135" s="28"/>
       <c r="B135" s="24">
         <v>1</v>
       </c>
       <c r="C135" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D135" s="12"/>
     </row>
     <row r="136" ht="31.5" hidden="1" spans="1:4">
-      <c r="A136" s="27"/>
+      <c r="A136" s="28"/>
       <c r="B136" s="18">
         <v>1</v>
       </c>
-      <c r="C136" s="28" t="s">
-        <v>198</v>
+      <c r="C136" s="29" t="s">
+        <v>199</v>
       </c>
       <c r="D136" s="11"/>
     </row>
     <row r="137" ht="60.75" hidden="1" spans="1:4">
-      <c r="A137" s="27"/>
+      <c r="A137" s="28"/>
       <c r="B137" s="18">
         <v>5</v>
       </c>
       <c r="C137" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="138" ht="31.5" hidden="1" spans="1:4">
-      <c r="A138" s="27"/>
+      <c r="A138" s="28"/>
       <c r="B138" s="18">
         <v>1</v>
       </c>
       <c r="C138" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D138" s="11"/>
     </row>
     <row r="139" ht="31.5" hidden="1" spans="1:4">
-      <c r="A139" s="27"/>
+      <c r="A139" s="28"/>
       <c r="B139" s="18">
         <v>1</v>
       </c>
       <c r="C139" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D139" s="11"/>
     </row>
     <row r="140" ht="47.25" hidden="1" spans="1:4">
-      <c r="A140" s="27"/>
+      <c r="A140" s="28"/>
       <c r="B140" s="18">
         <v>5</v>
       </c>
       <c r="C140" s="11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D140" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="141" ht="235" hidden="1" customHeight="1" spans="1:4">
-      <c r="A141" s="27"/>
+      <c r="A141" s="28"/>
       <c r="B141" s="18">
         <v>5</v>
       </c>
       <c r="C141" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D141" s="11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="142" ht="208" customHeight="1" spans="1:5">
-      <c r="A142" s="27"/>
+      <c r="A142" s="28"/>
       <c r="B142" s="18">
         <v>5</v>
       </c>
       <c r="C142" s="12" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D142" s="11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E142" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="143" ht="20" hidden="1" customHeight="1" spans="1:4">
-      <c r="A143" s="27"/>
+      <c r="A143" s="28"/>
       <c r="B143" s="18"/>
       <c r="C143" s="12"/>
       <c r="D143" s="11"/>
     </row>
     <row r="144" ht="20" hidden="1" customHeight="1" spans="1:4">
-      <c r="A144" s="27"/>
+      <c r="A144" s="28"/>
       <c r="B144" s="18"/>
       <c r="C144" s="12"/>
       <c r="D144" s="11"/>
     </row>
     <row r="145" ht="20" hidden="1" customHeight="1" spans="1:4">
-      <c r="A145" s="27"/>
+      <c r="A145" s="28"/>
       <c r="B145" s="18"/>
       <c r="C145" s="12"/>
       <c r="D145" s="11"/>
     </row>
     <row r="146" ht="20" hidden="1" customHeight="1" spans="1:4">
-      <c r="A146" s="27"/>
+      <c r="A146" s="28"/>
       <c r="B146" s="18"/>
       <c r="C146" s="12"/>
       <c r="D146" s="11"/>
     </row>
     <row r="147" ht="28" hidden="1" customHeight="1" spans="1:4">
-      <c r="A147" s="27"/>
+      <c r="A147" s="28"/>
       <c r="B147" s="18"/>
       <c r="C147" s="12"/>
       <c r="D147" s="11"/>
     </row>
     <row r="148" hidden="1" spans="1:4">
-      <c r="A148" s="27" t="s">
-        <v>209</v>
+      <c r="A148" s="28" t="s">
+        <v>210</v>
       </c>
       <c r="B148" s="18">
         <v>2</v>
       </c>
       <c r="C148" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D148" s="11"/>
     </row>
     <row r="149" ht="31.5" hidden="1" spans="1:4">
-      <c r="A149" s="27"/>
+      <c r="A149" s="28"/>
       <c r="B149" s="18">
         <v>1</v>
       </c>
       <c r="C149" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D149" s="11"/>
     </row>
     <row r="150" hidden="1" spans="1:4">
-      <c r="A150" s="27"/>
+      <c r="A150" s="28"/>
       <c r="B150" s="18">
         <v>1</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D150" s="11"/>
     </row>
     <row r="151" hidden="1" spans="1:4">
-      <c r="A151" s="27"/>
+      <c r="A151" s="28"/>
       <c r="B151" s="18">
         <v>1</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D151" s="11"/>
     </row>
     <row r="152" hidden="1" spans="1:4">
-      <c r="A152" s="27"/>
+      <c r="A152" s="28"/>
       <c r="B152" s="18">
         <v>1</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D152" s="11"/>
     </row>
     <row r="153" ht="31.5" hidden="1" spans="1:4">
-      <c r="A153" s="27"/>
+      <c r="A153" s="28"/>
       <c r="B153" s="18">
         <v>1</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D153" s="11"/>
     </row>
     <row r="154" ht="31.5" hidden="1" spans="1:4">
-      <c r="A154" s="27"/>
+      <c r="A154" s="28"/>
       <c r="B154" s="18">
         <v>1</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D154" s="11"/>
     </row>
     <row r="155" hidden="1" spans="1:4">
-      <c r="A155" s="27"/>
+      <c r="A155" s="28"/>
       <c r="B155" s="18">
         <v>1</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D155" s="11"/>
     </row>
     <row r="156" ht="31.5" hidden="1" spans="1:4">
-      <c r="A156" s="27"/>
+      <c r="A156" s="28"/>
       <c r="B156" s="18">
         <v>1</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D156" s="11"/>
     </row>
     <row r="157" ht="31.5" hidden="1" spans="1:4">
-      <c r="A157" s="27"/>
+      <c r="A157" s="28"/>
       <c r="B157" s="18">
         <v>1</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D157" s="11"/>
     </row>
     <row r="158" hidden="1" spans="1:4">
-      <c r="A158" s="27"/>
+      <c r="A158" s="28"/>
       <c r="B158" s="18">
         <v>1</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D158" s="11"/>
     </row>
     <row r="159" hidden="1" spans="1:4">
-      <c r="A159" s="27"/>
+      <c r="A159" s="28"/>
       <c r="B159" s="18"/>
       <c r="D159" s="11"/>
     </row>
     <row r="160" hidden="1" spans="1:4">
-      <c r="A160" s="27"/>
+      <c r="A160" s="28"/>
       <c r="B160" s="18"/>
       <c r="D160" s="11"/>
     </row>
     <row r="161" hidden="1" spans="1:4">
-      <c r="A161" s="27"/>
+      <c r="A161" s="28"/>
       <c r="B161" s="18"/>
       <c r="D161" s="11"/>
     </row>
     <row r="162" hidden="1" spans="1:4">
-      <c r="A162" s="27"/>
+      <c r="A162" s="28"/>
       <c r="B162" s="18"/>
       <c r="D162" s="11"/>
     </row>
     <row r="163" ht="126" hidden="1" spans="1:4">
-      <c r="A163" s="27"/>
+      <c r="A163" s="28"/>
       <c r="B163" s="18">
         <v>5</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D163" s="11" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="164" ht="78.75" hidden="1" spans="1:4">
-      <c r="A164" s="27"/>
+      <c r="A164" s="28"/>
       <c r="B164" s="18">
         <v>5</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D164" s="11" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="165" ht="171" hidden="1" spans="1:4">
-      <c r="A165" s="27"/>
+      <c r="A165" s="28"/>
       <c r="B165" s="18">
         <v>5</v>
       </c>
       <c r="C165" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="D165" s="29" t="s">
         <v>226</v>
       </c>
+      <c r="D165" s="30" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="166" ht="47.25" hidden="1" spans="1:4">
-      <c r="A166" s="27" t="s">
-        <v>227</v>
+      <c r="A166" s="28" t="s">
+        <v>228</v>
       </c>
       <c r="B166" s="18"/>
       <c r="C166" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="D166" s="29" t="s">
         <v>229</v>
       </c>
+      <c r="D166" s="30" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="167" ht="78.75" hidden="1" spans="1:4">
-      <c r="A167" s="27"/>
+      <c r="A167" s="28"/>
       <c r="B167" s="18">
         <v>5</v>
       </c>
       <c r="C167" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D167" s="11" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="168" ht="47.25" hidden="1" spans="1:4">
-      <c r="A168" s="27"/>
+      <c r="A168" s="28"/>
       <c r="B168" s="18">
         <v>5</v>
       </c>
       <c r="C168" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D168" s="11" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="169" hidden="1" spans="1:4">
-      <c r="A169" s="27"/>
+      <c r="A169" s="28"/>
       <c r="B169" s="18">
         <v>2</v>
       </c>
       <c r="C169" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D169" s="11"/>
     </row>
     <row r="170" ht="109" hidden="1" customHeight="1" spans="1:4">
-      <c r="A170" s="27"/>
+      <c r="A170" s="28"/>
       <c r="B170" s="18">
         <v>5</v>
       </c>
       <c r="C170" s="12" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D170" s="11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="171" ht="31.5" hidden="1" spans="1:4">
-      <c r="A171" s="27"/>
+      <c r="A171" s="28"/>
       <c r="B171" s="18">
         <v>5</v>
       </c>
       <c r="C171" s="23" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D171" s="11" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="172" ht="63" hidden="1" spans="1:4">
-      <c r="A172" s="27" t="s">
-        <v>239</v>
+      <c r="A172" s="28" t="s">
+        <v>240</v>
       </c>
       <c r="B172" s="18">
         <v>5</v>
       </c>
-      <c r="C172" s="30" t="s">
-        <v>240</v>
-      </c>
-      <c r="D172" s="30" t="s">
+      <c r="C172" s="31" t="s">
         <v>241</v>
       </c>
+      <c r="D172" s="31" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="173" ht="42" hidden="1" customHeight="1" spans="1:4">
-      <c r="A173" s="27"/>
+      <c r="A173" s="28"/>
       <c r="B173" s="18">
         <v>5</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D173" s="12" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="174" ht="42" hidden="1" customHeight="1" spans="1:4">
-      <c r="A174" s="27"/>
+      <c r="A174" s="28"/>
       <c r="B174" s="18">
         <v>5</v>
       </c>
       <c r="C174" s="12" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D174" s="12" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="175" ht="82" hidden="1" customHeight="1" spans="1:4">
-      <c r="A175" s="27"/>
+      <c r="A175" s="28"/>
       <c r="B175" s="18">
         <v>5</v>
       </c>
       <c r="C175" s="12" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D175" s="12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="176" ht="63" hidden="1" spans="1:4">
-      <c r="A176" s="27"/>
+      <c r="A176" s="28"/>
       <c r="B176" s="24">
         <v>5</v>
       </c>
       <c r="C176" s="12" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D176" s="12" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="177" hidden="1" spans="1:4">
-      <c r="A177" s="27"/>
+      <c r="A177" s="28"/>
       <c r="B177" s="18">
         <v>5</v>
       </c>
       <c r="C177" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D177" s="12" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="178" ht="220" hidden="1" customHeight="1" spans="1:4">
-      <c r="A178" s="27" t="s">
-        <v>252</v>
+      <c r="A178" s="28" t="s">
+        <v>253</v>
       </c>
       <c r="B178" s="18">
         <v>5</v>
       </c>
       <c r="C178" s="12" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D178" s="12" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="179" ht="31.5" hidden="1" spans="1:4">
-      <c r="A179" s="27"/>
+      <c r="A179" s="28"/>
       <c r="B179" s="18">
         <v>5</v>
       </c>
       <c r="C179" s="12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D179" s="12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="180" ht="173.25" hidden="1" spans="1:4">
-      <c r="A180" s="27"/>
+      <c r="A180" s="28"/>
       <c r="B180" s="18">
         <v>5</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="181" ht="47.25" hidden="1" spans="1:4">
-      <c r="A181" s="27"/>
+      <c r="A181" s="28"/>
       <c r="B181" s="18">
         <v>5</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add reading note for fastdraw
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14565" windowHeight="11730" tabRatio="354"/>
+    <workbookView windowWidth="27270" windowHeight="12525" tabRatio="354"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$181</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$186</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="260">
   <si>
     <t>Scope</t>
   </si>
@@ -267,6 +267,9 @@
     <t>EfficientNet: Rethinking Model Scaling for Convolutinal Neural Networks</t>
   </si>
   <si>
+    <t>ImageNet-trained CNNs are biased towards texture; increasing shape bias improves accuracy and robustness</t>
+  </si>
+  <si>
     <t>object detection</t>
   </si>
   <si>
@@ -430,6 +433,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>同一类别的不连续(intra-class inconsistency)主要是因为缺乏全局特征. 可以用</t>
     </r>
     <r>
@@ -652,7 +662,7 @@
   </si>
   <si>
     <t>Not All Areas Are Equal: Transfer Learning for Semantic Segmentation via Hierarchical Region Selection
-综合数据到真是数据的迁移</t>
+综合数据到真实数据的迁移</t>
   </si>
   <si>
     <t>Improving Semantic Segmentation via Video Propagation and Label Relaxation</t>
@@ -680,9 +690,6 @@
 之后可以尝试实现一下</t>
   </si>
   <si>
-    <t>(2019.05)Agnostic Lane Detection</t>
-  </si>
-  <si>
     <t>Harvesting informatation fromcaptions for weakly suipervised semantic segmentation</t>
   </si>
   <si>
@@ -700,6 +707,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>参考文献相当丰富啊～related work中有不少相关工作， 对尤其对语义分割的文章的review比较充分
 输入图片两次3x3 stride=2的卷积到1/4之的每个stage都保持1/4的分辨率，并且每个stage都添加一个low-resolution的feature map；网络中会fuse一下各个resolution的feature map，总共8个（</t>
     </r>
@@ -726,13 +740,6 @@
     </r>
   </si>
   <si>
-    <t>Real-time
-semantic Segmentation</t>
-  </si>
-  <si>
-    <t>(2017)ICNet for Real-Time Semantic Segmentation on High-Resolution Images</t>
-  </si>
-  <si>
     <t>(cvpr2019)In Defense of Pre-trained ImageNet Architectures for Real-time Semantic Segmentation of Road-driving Images</t>
   </si>
   <si>
@@ -746,18 +753,6 @@
   </si>
   <si>
     <t>(cvpr2019)A Simple Pooling-Based Design for Real-Time Salient Object Detection</t>
-  </si>
-  <si>
-    <t>(eccv2018)ESPNet: Efficient Spatial Pyramid of Dilated Convolutions for Semantic Segmentation</t>
-  </si>
-  <si>
-    <t>已经开源：https://github.com/sacmehta/ESPNet</t>
-  </si>
-  <si>
-    <t>(T-ITS2017)ERFNet: Efficient Residual Factorized ConvNet for Real-time Semantic Segmentation</t>
-  </si>
-  <si>
-    <t>已经开源：https://github.com/Eromera/erfnet</t>
   </si>
   <si>
     <t>Structured Knowledge Distillation for Semantic Segmentation</t>
@@ -900,6 +895,64 @@
 弊端是，被遮挡的物体会被分成两个东西</t>
   </si>
   <si>
+    <t>车道线检测</t>
+  </si>
+  <si>
+    <t>(2019) Agnostic Lane detection</t>
+  </si>
+  <si>
+    <t>(2019) FastDraw: Addressing the Long Tail of Lane Detection by Adapting a Sequential Prediction Network</t>
+  </si>
+  <si>
+    <r>
+      <t>end to end的车道线检测; 用了style transfer的方法，能够快速adapt到新的场景； 90FPS on 1080
+对车道线检测的需求：1. able to represent any number of lines of any length; 2. run in real-time; 3. adapt quikly to new scenes
+网络输出一张各个点在车道线上的概率；一张每个点的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>下</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>一行上各个点和这个点在一条车道线上的概率；一张每个点的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>上</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>一行上各个点和这个点在一条车道线上的概率；共3张图；这样，可以从任何一个点开始，画出整条车道线；
+用MUNIT(一种GAN), 把现有数据集的风格迁移出不同场景数据，混合训练，提高模型的精度泛化能力， to bias the network towards shape instead of texture
+network trained to do simple task on simple dataset learn low-level dircsriminative features that do not generalize, Unsupervised style transfer for data augmentation is offered as a naive but effective regularization of this phenomenon</t>
+    </r>
+  </si>
+  <si>
     <t>自动驾驶感知相关</t>
   </si>
   <si>
@@ -1033,8 +1086,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1087,6 +1140,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -1095,7 +1187,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1111,22 +1203,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1139,11 +1216,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1155,16 +1231,23 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1178,9 +1261,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1189,35 +1271,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1269,19 +1322,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1293,37 +1334,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1341,13 +1376,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1359,13 +1418,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1377,13 +1472,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1395,49 +1484,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1449,7 +1496,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1502,11 +1555,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1526,17 +1603,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1558,29 +1631,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1604,142 +1657,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1831,9 +1884,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1841,6 +1891,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1961,7 +2014,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>713740</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>134620</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1979,7 +2032,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14424025" y="519430"/>
+          <a:off x="14424025" y="48287305"/>
           <a:ext cx="3658870" cy="2015490"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2003,7 +2056,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1755140</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>1853565</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2021,7 +2074,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14131290" y="2400300"/>
+          <a:off x="14131290" y="50168175"/>
           <a:ext cx="2499360" cy="1853565"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2045,8 +2098,8 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>742315</xdr:colOff>
-      <xdr:row>126</xdr:row>
-      <xdr:rowOff>233680</xdr:rowOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>33655</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2063,7 +2116,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14131290" y="2419350"/>
+          <a:off x="14131290" y="75866625"/>
           <a:ext cx="3980180" cy="2386330"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2081,13 +2134,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>138</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>619760</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>138</xdr:row>
       <xdr:rowOff>2569845</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2105,7 +2158,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14131290" y="6362700"/>
+          <a:off x="14131290" y="88795225"/>
           <a:ext cx="5536565" cy="2550795"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2379,13 +2432,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:G181"/>
+  <sheetPr/>
+  <dimension ref="A1:G186"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C85" sqref="C85"/>
+      <selection pane="bottomLeft" activeCell="C165" sqref="C165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="15.75" outlineLevelCol="6"/>
@@ -2412,7 +2465,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="31.5" hidden="1" spans="1:4">
+    <row r="2" ht="31.5" spans="1:4">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -2424,7 +2477,7 @@
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" hidden="1" spans="1:4">
+    <row r="3" spans="1:4">
       <c r="A3" s="9"/>
       <c r="B3" s="10">
         <v>5</v>
@@ -2434,7 +2487,7 @@
       </c>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" hidden="1" spans="1:4">
+    <row r="4" spans="1:4">
       <c r="A4" s="9"/>
       <c r="B4" s="10">
         <v>5</v>
@@ -2444,7 +2497,7 @@
       </c>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" hidden="1" spans="1:4">
+    <row r="5" spans="1:4">
       <c r="A5" s="9"/>
       <c r="B5" s="10">
         <v>5</v>
@@ -2456,7 +2509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" hidden="1" spans="1:4">
+    <row r="6" spans="1:4">
       <c r="A6" s="9"/>
       <c r="B6" s="10"/>
       <c r="C6" s="12" t="s">
@@ -2464,7 +2517,7 @@
       </c>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" ht="31.5" hidden="1" spans="1:4">
+    <row r="7" ht="31.5" spans="1:4">
       <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
@@ -2476,7 +2529,7 @@
       </c>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" ht="31.5" hidden="1" spans="1:4">
+    <row r="8" ht="31.5" spans="1:4">
       <c r="A8" s="9"/>
       <c r="B8" s="10">
         <v>2</v>
@@ -2486,7 +2539,7 @@
       </c>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" hidden="1" spans="1:4">
+    <row r="9" ht="31.5" spans="1:4">
       <c r="A9" s="9"/>
       <c r="B9" s="10">
         <v>2</v>
@@ -2496,7 +2549,7 @@
       </c>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" ht="47.25" hidden="1" spans="1:4">
+    <row r="10" ht="63" spans="1:4">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -2510,7 +2563,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" hidden="1" spans="1:4">
+    <row r="11" spans="1:4">
       <c r="A11" s="9"/>
       <c r="B11" s="13">
         <v>5</v>
@@ -2522,7 +2575,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" hidden="1" spans="1:4">
+    <row r="12" spans="1:4">
       <c r="A12" s="9"/>
       <c r="B12" s="14">
         <v>5</v>
@@ -2532,7 +2585,7 @@
       </c>
       <c r="D12" s="11"/>
     </row>
-    <row r="13" ht="31.5" hidden="1" spans="1:4">
+    <row r="13" ht="31.5" spans="1:4">
       <c r="A13" s="9"/>
       <c r="B13" s="10">
         <v>5</v>
@@ -2544,7 +2597,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" ht="94.5" hidden="1" spans="1:4">
+    <row r="14" ht="78.75" spans="1:4">
       <c r="A14" s="9"/>
       <c r="B14" s="10">
         <v>5</v>
@@ -2556,7 +2609,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" ht="31.5" hidden="1" spans="1:4">
+    <row r="15" ht="31.5" spans="1:4">
       <c r="A15" s="9"/>
       <c r="B15" s="14">
         <v>2</v>
@@ -2566,7 +2619,7 @@
       </c>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" ht="31.5" hidden="1" spans="1:4">
+    <row r="16" ht="31.5" spans="1:4">
       <c r="A16" s="9"/>
       <c r="B16" s="16">
         <v>2</v>
@@ -2576,7 +2629,7 @@
       </c>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" ht="110.25" hidden="1" spans="1:4">
+    <row r="17" ht="94.5" spans="1:4">
       <c r="A17" s="9" t="s">
         <v>27</v>
       </c>
@@ -2590,7 +2643,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" hidden="1" spans="1:4">
+    <row r="18" spans="1:4">
       <c r="A18" s="9"/>
       <c r="B18" s="16">
         <v>2</v>
@@ -2600,7 +2653,7 @@
       </c>
       <c r="D18" s="11"/>
     </row>
-    <row r="19" ht="47.25" hidden="1" spans="1:4">
+    <row r="19" ht="31.5" spans="1:4">
       <c r="A19" s="9"/>
       <c r="B19" s="14">
         <v>5</v>
@@ -2612,7 +2665,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" ht="37" hidden="1" customHeight="1" spans="1:4">
+    <row r="20" ht="37" customHeight="1" spans="1:4">
       <c r="A20" s="9"/>
       <c r="B20" s="10">
         <v>5</v>
@@ -2624,7 +2677,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" hidden="1" spans="1:4">
+    <row r="21" spans="1:4">
       <c r="A21" s="9"/>
       <c r="B21" s="14">
         <v>5</v>
@@ -2634,7 +2687,7 @@
       </c>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" ht="31.5" hidden="1" spans="1:4">
+    <row r="22" ht="31.5" spans="1:4">
       <c r="A22" s="9"/>
       <c r="B22" s="14">
         <v>5</v>
@@ -2646,7 +2699,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" ht="110.25" hidden="1" spans="1:4">
+    <row r="23" ht="94.5" spans="1:4">
       <c r="A23" s="9"/>
       <c r="B23" s="14">
         <v>5</v>
@@ -2658,7 +2711,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" ht="31.5" hidden="1" spans="1:4">
+    <row r="24" ht="31.5" spans="1:4">
       <c r="A24" s="9"/>
       <c r="B24" s="14">
         <v>5</v>
@@ -2670,7 +2723,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" ht="31.5" hidden="1" spans="1:4">
+    <row r="25" ht="47.25" spans="1:4">
       <c r="A25" s="9"/>
       <c r="B25" s="16">
         <v>2</v>
@@ -2680,7 +2733,7 @@
       </c>
       <c r="D25" s="11"/>
     </row>
-    <row r="26" ht="31.5" hidden="1" spans="1:4">
+    <row r="26" ht="31.5" spans="1:4">
       <c r="A26" s="9"/>
       <c r="B26" s="14">
         <v>5</v>
@@ -2690,7 +2743,7 @@
       </c>
       <c r="D26" s="11"/>
     </row>
-    <row r="27" ht="31.5" hidden="1" spans="1:4">
+    <row r="27" ht="31.5" spans="1:4">
       <c r="A27" s="9"/>
       <c r="B27" s="14">
         <v>5</v>
@@ -2700,7 +2753,7 @@
       </c>
       <c r="D27" s="11"/>
     </row>
-    <row r="28" ht="94.5" hidden="1" spans="1:4">
+    <row r="28" ht="78.75" spans="1:4">
       <c r="A28" s="9"/>
       <c r="B28" s="14">
         <v>5</v>
@@ -2712,7 +2765,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" ht="31.5" hidden="1" spans="1:4">
+    <row r="29" ht="31.5" spans="1:4">
       <c r="A29" s="9"/>
       <c r="B29" s="14">
         <v>5</v>
@@ -2724,7 +2777,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" ht="31.5" hidden="1" spans="1:4">
+    <row r="30" ht="31.5" spans="1:4">
       <c r="A30" s="9"/>
       <c r="B30" s="14">
         <v>5</v>
@@ -2736,7 +2789,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" ht="47.25" hidden="1" spans="1:4">
+    <row r="31" ht="47.25" spans="1:4">
       <c r="A31" s="9"/>
       <c r="B31" s="14">
         <v>5</v>
@@ -2748,7 +2801,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" ht="94.5" hidden="1" spans="1:4">
+    <row r="32" ht="78.75" spans="1:4">
       <c r="A32" s="9"/>
       <c r="B32" s="14">
         <v>5</v>
@@ -2760,7 +2813,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" ht="31.5" hidden="1" spans="1:4">
+    <row r="33" ht="31.5" spans="1:4">
       <c r="A33" s="9"/>
       <c r="B33" s="14">
         <v>5</v>
@@ -2772,7 +2825,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" hidden="1" spans="1:4">
+    <row r="34" ht="31.5" spans="1:4">
       <c r="A34" s="9"/>
       <c r="B34" s="14">
         <v>5</v>
@@ -2782,7 +2835,7 @@
       </c>
       <c r="D34" s="11"/>
     </row>
-    <row r="35" hidden="1" spans="1:4">
+    <row r="35" spans="1:4">
       <c r="A35" s="9"/>
       <c r="B35" s="14">
         <v>5</v>
@@ -2792,7 +2845,7 @@
       </c>
       <c r="D35" s="11"/>
     </row>
-    <row r="36" hidden="1" spans="1:4">
+    <row r="36" spans="1:4">
       <c r="A36" s="9"/>
       <c r="B36" s="16">
         <v>2</v>
@@ -2802,7 +2855,7 @@
       </c>
       <c r="D36" s="11"/>
     </row>
-    <row r="37" ht="53" hidden="1" customHeight="1" spans="1:4">
+    <row r="37" ht="53" customHeight="1" spans="1:4">
       <c r="A37" s="9"/>
       <c r="B37" s="14">
         <v>5</v>
@@ -2814,7 +2867,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" ht="53" hidden="1" customHeight="1" spans="1:4">
+    <row r="38" ht="53" customHeight="1" spans="1:4">
       <c r="A38" s="9"/>
       <c r="B38" s="14">
         <v>5</v>
@@ -2826,7 +2879,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" ht="53" hidden="1" customHeight="1" spans="1:4">
+    <row r="39" ht="53" customHeight="1" spans="1:4">
       <c r="A39" s="9"/>
       <c r="B39" s="14">
         <v>1</v>
@@ -2836,7 +2889,7 @@
       </c>
       <c r="D39" s="11"/>
     </row>
-    <row r="40" ht="53" hidden="1" customHeight="1" spans="1:4">
+    <row r="40" ht="53" customHeight="1" spans="1:4">
       <c r="A40" s="9"/>
       <c r="B40" s="14">
         <v>1</v>
@@ -2846,7 +2899,7 @@
       </c>
       <c r="D40" s="11"/>
     </row>
-    <row r="41" ht="53" hidden="1" customHeight="1" spans="1:4">
+    <row r="41" ht="53" customHeight="1" spans="1:4">
       <c r="A41" s="9"/>
       <c r="B41" s="16">
         <v>1</v>
@@ -2856,7 +2909,7 @@
       </c>
       <c r="D41" s="11"/>
     </row>
-    <row r="42" ht="53" hidden="1" customHeight="1" spans="1:4">
+    <row r="42" ht="53" customHeight="1" spans="1:4">
       <c r="A42" s="9"/>
       <c r="B42" s="16">
         <v>1</v>
@@ -2866,7 +2919,7 @@
       </c>
       <c r="D42" s="11"/>
     </row>
-    <row r="43" ht="53" hidden="1" customHeight="1" spans="1:4">
+    <row r="43" ht="53" customHeight="1" spans="1:4">
       <c r="A43" s="9"/>
       <c r="B43" s="16">
         <v>1</v>
@@ -2876,7 +2929,7 @@
       </c>
       <c r="D43" s="11"/>
     </row>
-    <row r="44" ht="53" hidden="1" customHeight="1" spans="1:4">
+    <row r="44" ht="53" customHeight="1" spans="1:4">
       <c r="A44" s="9"/>
       <c r="B44" s="16">
         <v>1</v>
@@ -2886,7 +2939,7 @@
       </c>
       <c r="D44" s="11"/>
     </row>
-    <row r="45" ht="70" hidden="1" customHeight="1" spans="1:4">
+    <row r="45" ht="70" customHeight="1" spans="1:4">
       <c r="A45" s="9"/>
       <c r="B45" s="16">
         <v>1</v>
@@ -2896,7 +2949,7 @@
       </c>
       <c r="D45" s="11"/>
     </row>
-    <row r="46" ht="53" hidden="1" customHeight="1" spans="1:4">
+    <row r="46" ht="53" customHeight="1" spans="1:4">
       <c r="A46" s="9"/>
       <c r="B46" s="14">
         <v>1</v>
@@ -2906,7 +2959,7 @@
       </c>
       <c r="D46" s="11"/>
     </row>
-    <row r="47" ht="53" hidden="1" customHeight="1" spans="1:4">
+    <row r="47" ht="53" customHeight="1" spans="1:4">
       <c r="A47" s="9"/>
       <c r="B47" s="14">
         <v>5</v>
@@ -2918,7 +2971,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" ht="53" hidden="1" customHeight="1" spans="1:4">
+    <row r="48" ht="53" customHeight="1" spans="1:4">
       <c r="A48" s="9"/>
       <c r="B48" s="14">
         <v>1</v>
@@ -2928,7 +2981,7 @@
       </c>
       <c r="D48" s="12"/>
     </row>
-    <row r="49" ht="53" hidden="1" customHeight="1" spans="1:4">
+    <row r="49" ht="53" customHeight="1" spans="1:4">
       <c r="A49" s="9"/>
       <c r="B49" s="17">
         <v>1</v>
@@ -2938,7 +2991,7 @@
       </c>
       <c r="D49" s="12"/>
     </row>
-    <row r="50" ht="53" hidden="1" customHeight="1" spans="1:4">
+    <row r="50" ht="53" customHeight="1" spans="1:4">
       <c r="A50" s="9"/>
       <c r="B50" s="17">
         <v>1</v>
@@ -2948,342 +3001,348 @@
       </c>
       <c r="D50" s="12"/>
     </row>
-    <row r="51" ht="53" hidden="1" customHeight="1" spans="1:1">
+    <row r="51" ht="53" customHeight="1" spans="1:3">
       <c r="A51" s="9"/>
-    </row>
-    <row r="52" ht="53" hidden="1" customHeight="1" spans="1:4">
+      <c r="B51" s="17">
+        <v>1</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" ht="53" customHeight="1" spans="1:4">
       <c r="A52" s="9"/>
       <c r="B52" s="17"/>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
     </row>
-    <row r="53" ht="53" hidden="1" customHeight="1" spans="1:4">
+    <row r="53" ht="53" customHeight="1" spans="1:4">
       <c r="A53" s="9"/>
       <c r="B53" s="17"/>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
     </row>
-    <row r="54" ht="41" hidden="1" customHeight="1" spans="1:1">
+    <row r="54" ht="41" customHeight="1" spans="1:1">
       <c r="A54" s="9"/>
     </row>
-    <row r="55" hidden="1" spans="1:7">
+    <row r="55" spans="1:7">
       <c r="A55" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B55" s="14">
         <v>5</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D55" s="11"/>
       <c r="F55" s="19"/>
       <c r="G55" s="19"/>
     </row>
-    <row r="56" ht="78.75" hidden="1" spans="1:6">
+    <row r="56" ht="63" spans="1:6">
       <c r="A56" s="9"/>
       <c r="B56" s="14">
         <v>5</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" ht="47.25" hidden="1" spans="1:4">
+    <row r="57" ht="47.25" spans="1:4">
       <c r="A57" s="9"/>
       <c r="B57" s="10">
         <v>5</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="58" ht="94.5" hidden="1" spans="1:4">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" ht="78.75" spans="1:4">
       <c r="A58" s="9"/>
       <c r="B58" s="10">
         <v>5</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="59" hidden="1" spans="1:4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" ht="31.5" spans="1:4">
       <c r="A59" s="9"/>
       <c r="B59" s="18">
         <v>5</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="60" ht="47.25" hidden="1" spans="1:4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="60" ht="31.5" spans="1:4">
       <c r="A60" s="9"/>
       <c r="B60" s="10">
         <v>5</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="61" ht="31.5" hidden="1" spans="1:4">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" ht="31.5" spans="1:4">
       <c r="A61" s="9"/>
       <c r="B61" s="10">
         <v>2</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D61" s="11"/>
     </row>
-    <row r="62" ht="123.75" hidden="1" spans="1:4">
+    <row r="62" ht="94.5" spans="1:4">
       <c r="A62" s="9"/>
       <c r="B62" s="10">
         <v>5</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="63" ht="47.25" hidden="1" spans="1:4">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" ht="47.25" spans="1:4">
       <c r="A63" s="9"/>
       <c r="B63" s="10">
         <v>5</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="64" ht="31.5" hidden="1" spans="1:4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="64" ht="47.25" spans="1:4">
       <c r="A64" s="9"/>
       <c r="B64" s="10">
         <v>1</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D64" s="11"/>
     </row>
-    <row r="65" hidden="1" spans="1:4">
+    <row r="65" spans="1:4">
       <c r="A65" s="9"/>
       <c r="B65" s="10"/>
       <c r="C65" s="12"/>
       <c r="D65" s="11"/>
     </row>
-    <row r="66" hidden="1" spans="1:4">
+    <row r="66" spans="1:4">
       <c r="A66" s="9"/>
       <c r="B66" s="10"/>
       <c r="C66" s="12"/>
       <c r="D66" s="11"/>
     </row>
-    <row r="67" hidden="1" spans="1:4">
+    <row r="67" spans="1:4">
       <c r="A67" s="9"/>
       <c r="B67" s="10"/>
       <c r="C67" s="12"/>
       <c r="D67" s="11"/>
     </row>
-    <row r="68" hidden="1" spans="1:1">
+    <row r="68" spans="1:1">
       <c r="A68" s="9"/>
     </row>
-    <row r="69" ht="47.25" hidden="1" spans="1:4">
+    <row r="69" ht="47.25" spans="1:4">
       <c r="A69" s="20"/>
       <c r="B69" s="10">
         <v>5</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D69" s="11"/>
     </row>
-    <row r="70" ht="78.75" hidden="1" spans="1:4">
+    <row r="70" ht="63" spans="1:4">
       <c r="A70" s="20"/>
       <c r="B70" s="10">
         <v>6</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="71" hidden="1" spans="1:4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="71" ht="31.5" spans="1:4">
       <c r="A71" s="20"/>
       <c r="B71" s="18">
         <v>5</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="72" ht="31.5" hidden="1" spans="1:4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" ht="31.5" spans="1:4">
       <c r="A72" s="20"/>
       <c r="B72" s="18">
         <v>5</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="73" ht="110.25" hidden="1" spans="1:4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="73" ht="110.25" spans="1:4">
       <c r="A73" s="20"/>
       <c r="B73" s="18">
         <v>5</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="74" ht="123.75" hidden="1" spans="1:4">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" ht="92.25" spans="1:4">
       <c r="A74" s="20"/>
       <c r="B74" s="18">
         <v>5</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="75" ht="189" hidden="1" spans="1:4">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="75" ht="157.5" spans="1:4">
       <c r="A75" s="20"/>
       <c r="B75" s="18">
         <v>5</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="76" ht="60.75" hidden="1" spans="1:4">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="76" ht="60.75" spans="1:4">
       <c r="A76" s="20"/>
       <c r="B76" s="18">
         <v>5</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="77" ht="126" hidden="1" spans="1:4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="77" ht="126" spans="1:4">
       <c r="A77" s="20"/>
       <c r="B77" s="18">
         <v>5</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="78" hidden="1" spans="1:4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" ht="31.5" spans="1:4">
       <c r="A78" s="20"/>
       <c r="B78" s="18">
         <v>5</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D78" s="11"/>
     </row>
-    <row r="79" ht="31.5" hidden="1" spans="1:4">
+    <row r="79" ht="60.75" spans="1:4">
       <c r="A79" s="20"/>
       <c r="B79" s="18">
         <v>5</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D79" s="11"/>
     </row>
-    <row r="80" hidden="1" spans="1:4">
+    <row r="80" spans="1:4">
       <c r="A80" s="20"/>
       <c r="B80" s="18">
         <v>2</v>
       </c>
       <c r="C80" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D80" s="11"/>
     </row>
-    <row r="81" hidden="1" spans="1:4">
+    <row r="81" spans="1:4">
       <c r="A81" s="20"/>
       <c r="B81" s="18">
         <v>5</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D81" s="11"/>
     </row>
-    <row r="82" ht="31.5" hidden="1" spans="1:4">
+    <row r="82" ht="31.5" spans="1:4">
       <c r="A82" s="20"/>
       <c r="B82" s="18">
         <v>2</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D82" s="11"/>
     </row>
-    <row r="83" ht="31.5" hidden="1" spans="1:4">
+    <row r="83" ht="47.25" spans="1:4">
       <c r="A83" s="20"/>
       <c r="B83" s="18">
         <v>5</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="84" ht="47.25" hidden="1" spans="1:4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="84" ht="47.25" spans="1:4">
       <c r="A84" s="20"/>
       <c r="B84" s="18">
         <v>5</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="85" ht="173.25" spans="1:5">
@@ -3292,424 +3351,424 @@
         <v>5</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E85" s="26" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="86" ht="155" hidden="1" customHeight="1" spans="1:5">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="86" ht="155" customHeight="1" spans="1:5">
       <c r="A86" s="20"/>
       <c r="B86" s="18">
         <v>5</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="E86" s="27" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="87" ht="63" hidden="1" spans="1:4">
+      <c r="E86" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="87" ht="47.25" spans="1:4">
       <c r="A87" s="20"/>
       <c r="B87" s="18">
         <v>5</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="88" ht="63" hidden="1" spans="1:4">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="88" ht="47.25" spans="1:4">
       <c r="A88" s="20"/>
       <c r="B88" s="18">
         <v>5</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="89" ht="155.25" hidden="1" spans="1:4">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="89" ht="141.75" spans="1:4">
       <c r="A89" s="20"/>
       <c r="B89" s="18">
         <v>5</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="90" ht="63" hidden="1" spans="1:4">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="90" ht="63" spans="1:4">
       <c r="A90" s="20"/>
       <c r="B90" s="18">
         <v>5</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="91" ht="78.75" hidden="1" spans="1:4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="91" ht="47.25" spans="1:4">
       <c r="A91" s="20"/>
       <c r="B91" s="18">
         <v>5</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="92" ht="31.5" hidden="1" spans="1:4">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="92" ht="31.5" spans="1:4">
       <c r="A92" s="20"/>
       <c r="B92" s="18">
         <v>5</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="93" ht="31.5" hidden="1" spans="1:4">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="93" ht="31.5" spans="1:4">
       <c r="A93" s="20"/>
       <c r="B93" s="18">
         <v>2</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D93" s="11"/>
     </row>
-    <row r="94" ht="47.25" hidden="1" spans="1:4">
+    <row r="94" ht="47.25" spans="1:4">
       <c r="A94" s="20"/>
       <c r="B94" s="18">
         <v>2</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D94" s="11"/>
     </row>
-    <row r="95" ht="31.5" hidden="1" spans="1:4">
+    <row r="95" ht="31.5" spans="1:4">
       <c r="A95" s="20"/>
       <c r="B95" s="18">
         <v>2</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D95" s="11"/>
     </row>
-    <row r="96" ht="31.5" hidden="1" spans="1:4">
+    <row r="96" ht="47.25" spans="1:4">
       <c r="A96" s="20"/>
       <c r="B96" s="18">
         <v>2</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D96" s="11"/>
     </row>
-    <row r="97" hidden="1" spans="1:4">
+    <row r="97" ht="31.5" spans="1:4">
       <c r="A97" s="20"/>
       <c r="B97" s="18">
         <v>2</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D97" s="11"/>
     </row>
-    <row r="98" ht="78.75" hidden="1" spans="1:4">
+    <row r="98" ht="63" spans="1:4">
       <c r="A98" s="20"/>
       <c r="B98" s="18">
         <v>5</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="99" ht="31.5" hidden="1" spans="1:4">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="99" ht="31.5" spans="1:4">
       <c r="A99" s="20"/>
       <c r="B99" s="18">
         <v>2</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D99" s="11"/>
     </row>
-    <row r="100" ht="76.5" hidden="1" spans="1:4">
+    <row r="100" ht="60.75" spans="1:4">
       <c r="A100" s="20"/>
       <c r="B100" s="18">
         <v>5</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D100" s="11" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="101" ht="31.5" hidden="1" spans="1:4">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="101" ht="31.5" spans="1:4">
       <c r="A101" s="20"/>
       <c r="B101" s="18">
         <v>2</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D101" s="21"/>
     </row>
-    <row r="102" ht="110.25" hidden="1" spans="1:4">
+    <row r="102" ht="94.5" spans="1:4">
       <c r="A102" s="20"/>
       <c r="B102" s="18">
         <v>5</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D102" s="21" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="103" ht="31.5" hidden="1" spans="1:4">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="103" ht="31.5" spans="1:4">
       <c r="A103" s="20"/>
       <c r="B103" s="18">
         <v>5</v>
       </c>
       <c r="C103" s="22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D103" s="21"/>
     </row>
-    <row r="104" ht="47.25" hidden="1" spans="1:4">
+    <row r="104" ht="47.25" spans="1:4">
       <c r="A104" s="20"/>
       <c r="B104" s="18">
         <v>2</v>
       </c>
       <c r="C104" s="22" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D104" s="21"/>
     </row>
-    <row r="105" ht="31.5" hidden="1" spans="1:4">
+    <row r="105" ht="31.5" spans="1:4">
       <c r="A105" s="20"/>
       <c r="B105" s="18">
         <v>2</v>
       </c>
       <c r="C105" s="22" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D105" s="21"/>
     </row>
-    <row r="106" ht="31.5" hidden="1" spans="1:4">
+    <row r="106" ht="47.25" spans="1:4">
       <c r="A106" s="20"/>
       <c r="B106" s="18">
         <v>5</v>
       </c>
       <c r="C106" s="22" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D106" s="21"/>
     </row>
-    <row r="107" ht="110.25" hidden="1" spans="1:4">
+    <row r="107" ht="110.25" spans="1:4">
       <c r="A107" s="20"/>
       <c r="B107" s="18">
         <v>5</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D107" s="21" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="108" ht="31.5" hidden="1" spans="1:4">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="108" ht="31.5" spans="1:4">
       <c r="A108" s="20"/>
       <c r="B108" s="18">
         <v>5</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D108" s="21" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="109" ht="31.5" hidden="1" spans="1:4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="109" ht="47.25" spans="1:4">
       <c r="A109" s="20"/>
       <c r="B109" s="18">
         <v>5</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D109" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="110" ht="63" hidden="1" spans="1:4">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="110" ht="63" spans="1:4">
       <c r="A110" s="20"/>
       <c r="B110" s="18">
         <v>5</v>
       </c>
       <c r="C110" s="23" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D110" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="111" ht="141.75" hidden="1" spans="1:4">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="111" ht="126" spans="1:4">
       <c r="A111" s="20"/>
       <c r="B111" s="18">
         <v>5</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="112" ht="31" hidden="1" customHeight="1" spans="1:5">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="112" ht="31" customHeight="1" spans="1:5">
       <c r="A112" s="20"/>
       <c r="B112" s="24">
         <v>1</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D112" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="E112" s="27" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="113" ht="47.25" hidden="1" spans="1:4">
+        <v>168</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="113" ht="47.25" spans="1:4">
       <c r="A113" s="20"/>
       <c r="B113" s="24">
         <v>2</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D113" s="12"/>
     </row>
-    <row r="114" ht="47.25" hidden="1" spans="1:4">
+    <row r="114" ht="47.25" spans="1:4">
       <c r="A114" s="20"/>
       <c r="B114" s="24">
         <v>5</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D114" s="12" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="115" ht="31.5" hidden="1" spans="1:4">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="115" ht="31.5" spans="1:4">
       <c r="A115" s="20"/>
       <c r="B115" s="24">
         <v>2</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D115" s="12"/>
     </row>
-    <row r="116" ht="63" hidden="1" spans="1:4">
+    <row r="116" ht="60.75" spans="1:4">
       <c r="A116" s="20"/>
       <c r="B116" s="24">
         <v>5</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="117" ht="45" hidden="1" spans="1:4">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="117" ht="60.75" spans="1:4">
       <c r="A117" s="20"/>
       <c r="B117" s="24">
         <v>1</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D117" s="12"/>
     </row>
-    <row r="118" ht="31.5" hidden="1" spans="1:4">
+    <row r="118" ht="31.5" spans="1:4">
       <c r="A118" s="20"/>
       <c r="B118" s="24">
         <v>1</v>
       </c>
       <c r="C118" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D118" s="12"/>
     </row>
-    <row r="119" ht="31.5" hidden="1" spans="1:4">
+    <row r="119" ht="31.5" spans="1:4">
       <c r="A119" s="20"/>
       <c r="B119" s="24">
         <v>1</v>
       </c>
       <c r="C119" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D119" s="12"/>
     </row>
-    <row r="120" ht="31.5" hidden="1" spans="1:4">
+    <row r="120" ht="47.25" spans="1:4">
       <c r="A120" s="20"/>
       <c r="B120" s="24">
         <v>1</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D120" s="12"/>
     </row>
-    <row r="121" ht="31.5" hidden="1" spans="1:4">
+    <row r="121" ht="47.25" spans="1:4">
       <c r="A121" s="20"/>
       <c r="B121" s="24">
         <v>1</v>
       </c>
       <c r="C121" s="12" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D121" s="12"/>
     </row>
-    <row r="122" ht="31.5" hidden="1" spans="1:4">
+    <row r="122" ht="47.25" spans="1:4">
       <c r="A122" s="20"/>
       <c r="B122" s="24">
         <v>1</v>
       </c>
       <c r="C122" s="12" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D122" s="12"/>
     </row>
@@ -3719,26 +3778,24 @@
         <v>5</v>
       </c>
       <c r="C123" s="12" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D123" s="12" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E123" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="124" hidden="1" spans="1:4">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124" s="20"/>
       <c r="B124" s="24">
         <v>1</v>
       </c>
-      <c r="C124" s="12" t="s">
-        <v>182</v>
-      </c>
+      <c r="C124" s="12"/>
       <c r="D124" s="12"/>
     </row>
-    <row r="125" ht="31.5" hidden="1" spans="1:4">
+    <row r="125" ht="31.5" spans="1:4">
       <c r="A125" s="20"/>
       <c r="B125" s="24">
         <v>1</v>
@@ -3748,7 +3805,7 @@
       </c>
       <c r="D125" s="12"/>
     </row>
-    <row r="126" ht="31.5" hidden="1" spans="1:4">
+    <row r="126" ht="31.5" spans="1:4">
       <c r="A126" s="20"/>
       <c r="B126" s="24">
         <v>1</v>
@@ -3770,7 +3827,7 @@
         <v>186</v>
       </c>
       <c r="E127" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="128" ht="108" spans="1:5">
@@ -3785,579 +3842,594 @@
         <v>188</v>
       </c>
       <c r="E128" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="129" hidden="1" spans="1:4">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" s="20"/>
       <c r="B129" s="24"/>
       <c r="C129" s="12"/>
       <c r="D129" s="12"/>
     </row>
-    <row r="130" ht="31.5" hidden="1" spans="1:4">
-      <c r="A130" s="28" t="s">
+    <row r="130" ht="126" spans="1:4">
+      <c r="A130" s="27"/>
+      <c r="B130" s="24">
+        <v>5</v>
+      </c>
+      <c r="C130" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="B130" s="18">
+      <c r="D130" s="11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="131" ht="31.5" spans="1:4">
+      <c r="A131" s="27"/>
+      <c r="B131" s="24">
         <v>1</v>
-      </c>
-      <c r="C130" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D130" s="11"/>
-    </row>
-    <row r="131" ht="141.75" hidden="1" spans="1:4">
-      <c r="A131" s="28"/>
-      <c r="B131" s="24">
-        <v>5</v>
       </c>
       <c r="C131" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="D131" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="132" ht="31.5" hidden="1" spans="1:4">
-      <c r="A132" s="28"/>
+      <c r="D131" s="11"/>
+    </row>
+    <row r="132" ht="31.5" spans="1:4">
+      <c r="A132" s="27"/>
       <c r="B132" s="24">
         <v>1</v>
       </c>
       <c r="C132" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="D132" s="11"/>
-    </row>
-    <row r="133" ht="31.5" hidden="1" spans="1:4">
-      <c r="A133" s="28"/>
+        <v>192</v>
+      </c>
+      <c r="D132" s="12"/>
+    </row>
+    <row r="133" ht="31.5" spans="1:4">
+      <c r="A133" s="27"/>
       <c r="B133" s="18">
         <v>1</v>
       </c>
-      <c r="C133" s="12" t="s">
+      <c r="C133" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="D133" s="11"/>
+    </row>
+    <row r="134" ht="47.25" spans="1:4">
+      <c r="A134" s="27"/>
+      <c r="B134" s="18">
+        <v>5</v>
+      </c>
+      <c r="C134" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="D133" s="11" t="s">
+      <c r="D134" s="8" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="134" ht="31.5" hidden="1" spans="1:4">
-      <c r="A134" s="28"/>
-      <c r="B134" s="18">
+    <row r="135" ht="31.5" spans="1:4">
+      <c r="A135" s="27"/>
+      <c r="B135" s="18">
         <v>1</v>
       </c>
-      <c r="C134" s="12" t="s">
+      <c r="C135" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="D134" s="11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="135" ht="31.5" hidden="1" spans="1:4">
-      <c r="A135" s="28"/>
-      <c r="B135" s="24">
-        <v>1</v>
-      </c>
-      <c r="C135" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D135" s="12"/>
-    </row>
-    <row r="136" ht="31.5" hidden="1" spans="1:4">
-      <c r="A136" s="28"/>
+      <c r="D135" s="11"/>
+    </row>
+    <row r="136" ht="31.5" spans="1:4">
+      <c r="A136" s="27"/>
       <c r="B136" s="18">
         <v>1</v>
       </c>
-      <c r="C136" s="29" t="s">
+      <c r="C136" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="D136" s="11"/>
+    </row>
+    <row r="137" ht="47.25" spans="1:4">
+      <c r="A137" s="27"/>
+      <c r="B137" s="18">
+        <v>5</v>
+      </c>
+      <c r="C137" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="D137" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="D136" s="11"/>
-    </row>
-    <row r="137" ht="60.75" hidden="1" spans="1:4">
-      <c r="A137" s="28"/>
-      <c r="B137" s="18">
-        <v>5</v>
-      </c>
-      <c r="C137" s="12" t="s">
+    </row>
+    <row r="138" ht="235" customHeight="1" spans="1:4">
+      <c r="A138" s="27"/>
+      <c r="B138" s="18">
+        <v>5</v>
+      </c>
+      <c r="C138" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="D137" s="8" t="s">
+      <c r="D138" s="11" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="138" ht="31.5" hidden="1" spans="1:4">
-      <c r="A138" s="28"/>
-      <c r="B138" s="18">
-        <v>1</v>
-      </c>
-      <c r="C138" s="12" t="s">
+    <row r="139" ht="208" customHeight="1" spans="1:5">
+      <c r="A139" s="27"/>
+      <c r="B139" s="18">
+        <v>5</v>
+      </c>
+      <c r="C139" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="D138" s="11"/>
-    </row>
-    <row r="139" ht="31.5" hidden="1" spans="1:4">
-      <c r="A139" s="28"/>
-      <c r="B139" s="18">
-        <v>1</v>
-      </c>
-      <c r="C139" s="12" t="s">
+      <c r="D139" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="D139" s="11"/>
-    </row>
-    <row r="140" ht="47.25" hidden="1" spans="1:4">
-      <c r="A140" s="28"/>
-      <c r="B140" s="18">
-        <v>5</v>
-      </c>
-      <c r="C140" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="D140" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="141" ht="235" hidden="1" customHeight="1" spans="1:4">
-      <c r="A141" s="28"/>
-      <c r="B141" s="18">
-        <v>5</v>
-      </c>
-      <c r="C141" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="D141" s="11" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="142" ht="208" customHeight="1" spans="1:5">
-      <c r="A142" s="28"/>
-      <c r="B142" s="18">
-        <v>5</v>
-      </c>
-      <c r="C142" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="D142" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="E142" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="143" ht="20" hidden="1" customHeight="1" spans="1:4">
-      <c r="A143" s="28"/>
+      <c r="E139" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="140" ht="20" customHeight="1" spans="1:4">
+      <c r="A140" s="27"/>
+      <c r="B140" s="18"/>
+      <c r="C140" s="12"/>
+      <c r="D140" s="11"/>
+    </row>
+    <row r="141" ht="20" customHeight="1" spans="1:4">
+      <c r="A141" s="27"/>
+      <c r="B141" s="18"/>
+      <c r="C141" s="12"/>
+      <c r="D141" s="11"/>
+    </row>
+    <row r="142" ht="20" customHeight="1" spans="1:4">
+      <c r="A142" s="27"/>
+      <c r="B142" s="18"/>
+      <c r="C142" s="12"/>
+      <c r="D142" s="11"/>
+    </row>
+    <row r="143" ht="20" customHeight="1" spans="1:4">
+      <c r="A143" s="27"/>
       <c r="B143" s="18"/>
       <c r="C143" s="12"/>
       <c r="D143" s="11"/>
     </row>
-    <row r="144" ht="20" hidden="1" customHeight="1" spans="1:4">
-      <c r="A144" s="28"/>
+    <row r="144" ht="28" customHeight="1" spans="1:4">
+      <c r="A144" s="27"/>
       <c r="B144" s="18"/>
       <c r="C144" s="12"/>
       <c r="D144" s="11"/>
     </row>
-    <row r="145" ht="20" hidden="1" customHeight="1" spans="1:4">
-      <c r="A145" s="28"/>
-      <c r="B145" s="18"/>
-      <c r="C145" s="12"/>
+    <row r="145" spans="1:4">
+      <c r="A145" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="B145" s="18">
+        <v>2</v>
+      </c>
+      <c r="C145" s="12" t="s">
+        <v>205</v>
+      </c>
       <c r="D145" s="11"/>
     </row>
-    <row r="146" ht="20" hidden="1" customHeight="1" spans="1:4">
-      <c r="A146" s="28"/>
-      <c r="B146" s="18"/>
-      <c r="C146" s="12"/>
+    <row r="146" ht="31.5" spans="1:4">
+      <c r="A146" s="27"/>
+      <c r="B146" s="18">
+        <v>1</v>
+      </c>
+      <c r="C146" s="12" t="s">
+        <v>206</v>
+      </c>
       <c r="D146" s="11"/>
     </row>
-    <row r="147" ht="28" hidden="1" customHeight="1" spans="1:4">
-      <c r="A147" s="28"/>
-      <c r="B147" s="18"/>
-      <c r="C147" s="12"/>
+    <row r="147" ht="31.5" spans="1:4">
+      <c r="A147" s="27"/>
+      <c r="B147" s="18">
+        <v>1</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>207</v>
+      </c>
       <c r="D147" s="11"/>
     </row>
-    <row r="148" hidden="1" spans="1:4">
-      <c r="A148" s="28" t="s">
-        <v>210</v>
-      </c>
+    <row r="148" ht="31.5" spans="1:4">
+      <c r="A148" s="27"/>
       <c r="B148" s="18">
-        <v>2</v>
-      </c>
-      <c r="C148" s="12" t="s">
-        <v>211</v>
+        <v>1</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="D148" s="11"/>
     </row>
-    <row r="149" ht="31.5" hidden="1" spans="1:4">
-      <c r="A149" s="28"/>
+    <row r="149" ht="31.5" spans="1:4">
+      <c r="A149" s="27"/>
       <c r="B149" s="18">
         <v>1</v>
       </c>
-      <c r="C149" s="12" t="s">
-        <v>212</v>
+      <c r="C149" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="D149" s="11"/>
     </row>
-    <row r="150" hidden="1" spans="1:4">
-      <c r="A150" s="28"/>
+    <row r="150" ht="31.5" spans="1:4">
+      <c r="A150" s="27"/>
       <c r="B150" s="18">
         <v>1</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D150" s="11"/>
     </row>
-    <row r="151" hidden="1" spans="1:4">
-      <c r="A151" s="28"/>
+    <row r="151" ht="31.5" spans="1:4">
+      <c r="A151" s="27"/>
       <c r="B151" s="18">
         <v>1</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D151" s="11"/>
     </row>
-    <row r="152" hidden="1" spans="1:4">
-      <c r="A152" s="28"/>
+    <row r="152" ht="31.5" spans="1:4">
+      <c r="A152" s="27"/>
       <c r="B152" s="18">
         <v>1</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D152" s="11"/>
     </row>
-    <row r="153" ht="31.5" hidden="1" spans="1:4">
-      <c r="A153" s="28"/>
+    <row r="153" ht="31.5" spans="1:4">
+      <c r="A153" s="27"/>
       <c r="B153" s="18">
         <v>1</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D153" s="11"/>
     </row>
-    <row r="154" ht="31.5" hidden="1" spans="1:4">
-      <c r="A154" s="28"/>
+    <row r="154" ht="31.5" spans="1:4">
+      <c r="A154" s="27"/>
       <c r="B154" s="18">
         <v>1</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D154" s="11"/>
     </row>
-    <row r="155" hidden="1" spans="1:4">
-      <c r="A155" s="28"/>
+    <row r="155" spans="1:4">
+      <c r="A155" s="27"/>
       <c r="B155" s="18">
         <v>1</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D155" s="11"/>
     </row>
-    <row r="156" ht="31.5" hidden="1" spans="1:4">
-      <c r="A156" s="28"/>
-      <c r="B156" s="18">
-        <v>1</v>
-      </c>
-      <c r="C156" s="2" t="s">
-        <v>219</v>
-      </c>
+    <row r="156" spans="1:4">
+      <c r="A156" s="27"/>
+      <c r="B156" s="18"/>
       <c r="D156" s="11"/>
     </row>
-    <row r="157" ht="31.5" hidden="1" spans="1:4">
-      <c r="A157" s="28"/>
-      <c r="B157" s="18">
-        <v>1</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>220</v>
-      </c>
+    <row r="157" spans="1:4">
+      <c r="A157" s="27"/>
+      <c r="B157" s="18"/>
       <c r="D157" s="11"/>
     </row>
-    <row r="158" hidden="1" spans="1:4">
-      <c r="A158" s="28"/>
-      <c r="B158" s="18">
-        <v>1</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>221</v>
-      </c>
+    <row r="158" spans="1:4">
+      <c r="A158" s="27"/>
+      <c r="B158" s="18"/>
       <c r="D158" s="11"/>
     </row>
-    <row r="159" hidden="1" spans="1:4">
-      <c r="A159" s="28"/>
+    <row r="159" spans="1:4">
+      <c r="A159" s="27"/>
       <c r="B159" s="18"/>
       <c r="D159" s="11"/>
     </row>
-    <row r="160" hidden="1" spans="1:4">
-      <c r="A160" s="28"/>
-      <c r="B160" s="18"/>
-      <c r="D160" s="11"/>
-    </row>
-    <row r="161" hidden="1" spans="1:4">
-      <c r="A161" s="28"/>
-      <c r="B161" s="18"/>
-      <c r="D161" s="11"/>
-    </row>
-    <row r="162" hidden="1" spans="1:4">
-      <c r="A162" s="28"/>
-      <c r="B162" s="18"/>
-      <c r="D162" s="11"/>
-    </row>
-    <row r="163" ht="126" hidden="1" spans="1:4">
-      <c r="A163" s="28"/>
-      <c r="B163" s="18">
-        <v>5</v>
-      </c>
-      <c r="C163" s="2" t="s">
+    <row r="160" ht="126" spans="1:4">
+      <c r="A160" s="27"/>
+      <c r="B160" s="18">
+        <v>5</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D160" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="161" ht="78.75" spans="1:4">
+      <c r="A161" s="27"/>
+      <c r="B161" s="18">
+        <v>5</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D161" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="162" ht="139.5" spans="1:4">
+      <c r="A162" s="27"/>
+      <c r="B162" s="18">
+        <v>5</v>
+      </c>
+      <c r="C162" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D162" s="29" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="D163" s="11" t="s">
+      <c r="B163" s="18"/>
+      <c r="C163" s="12" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="164" ht="78.75" hidden="1" spans="1:4">
-      <c r="A164" s="28"/>
+      <c r="D163" s="29"/>
+    </row>
+    <row r="164" ht="202.5" spans="1:4">
+      <c r="A164" s="27"/>
       <c r="B164" s="18">
         <v>5</v>
       </c>
-      <c r="C164" s="2" t="s">
+      <c r="C164" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="D164" s="11" t="s">
+      <c r="D164" s="30" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="165" ht="171" hidden="1" spans="1:4">
-      <c r="A165" s="28"/>
-      <c r="B165" s="18">
-        <v>5</v>
-      </c>
-      <c r="C165" s="12" t="s">
+    <row r="165" spans="1:4">
+      <c r="A165" s="27"/>
+      <c r="B165" s="18"/>
+      <c r="C165" s="12"/>
+      <c r="D165" s="29"/>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" s="27"/>
+      <c r="B166" s="18"/>
+      <c r="C166" s="12"/>
+      <c r="D166" s="29"/>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="27"/>
+      <c r="B167" s="18"/>
+      <c r="C167" s="12"/>
+      <c r="D167" s="29"/>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" s="27"/>
+      <c r="B168" s="18"/>
+      <c r="C168" s="12"/>
+      <c r="D168" s="29"/>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" s="27"/>
+      <c r="B169" s="18"/>
+      <c r="C169" s="12"/>
+      <c r="D169" s="29"/>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" s="27"/>
+      <c r="B170" s="18"/>
+      <c r="C170" s="12"/>
+      <c r="D170" s="29"/>
+    </row>
+    <row r="171" ht="31.5" spans="1:4">
+      <c r="A171" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="D165" s="30" t="s">
+      <c r="B171" s="18"/>
+      <c r="C171" s="12" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="166" ht="47.25" hidden="1" spans="1:4">
-      <c r="A166" s="28" t="s">
+      <c r="D171" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="B166" s="18"/>
-      <c r="C166" s="12" t="s">
+    </row>
+    <row r="172" ht="47.25" spans="1:4">
+      <c r="A172" s="27"/>
+      <c r="B172" s="18">
+        <v>5</v>
+      </c>
+      <c r="C172" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="D166" s="30" t="s">
+      <c r="D172" s="11" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="167" ht="78.75" hidden="1" spans="1:4">
-      <c r="A167" s="28"/>
-      <c r="B167" s="18">
-        <v>5</v>
-      </c>
-      <c r="C167" s="12" t="s">
+    <row r="173" ht="47.25" spans="1:4">
+      <c r="A173" s="27"/>
+      <c r="B173" s="18">
+        <v>5</v>
+      </c>
+      <c r="C173" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="D167" s="11" t="s">
+      <c r="D173" s="11" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="168" ht="47.25" hidden="1" spans="1:4">
-      <c r="A168" s="28"/>
-      <c r="B168" s="18">
-        <v>5</v>
-      </c>
-      <c r="C168" s="12" t="s">
+    <row r="174" spans="1:4">
+      <c r="A174" s="27"/>
+      <c r="B174" s="18">
+        <v>2</v>
+      </c>
+      <c r="C174" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="D168" s="11" t="s">
+      <c r="D174" s="11"/>
+    </row>
+    <row r="175" ht="109" customHeight="1" spans="1:4">
+      <c r="A175" s="27"/>
+      <c r="B175" s="18">
+        <v>5</v>
+      </c>
+      <c r="C175" s="12" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="169" hidden="1" spans="1:4">
-      <c r="A169" s="28"/>
-      <c r="B169" s="18">
-        <v>2</v>
-      </c>
-      <c r="C169" s="12" t="s">
+      <c r="D175" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="D169" s="11"/>
-    </row>
-    <row r="170" ht="109" hidden="1" customHeight="1" spans="1:4">
-      <c r="A170" s="28"/>
-      <c r="B170" s="18">
-        <v>5</v>
-      </c>
-      <c r="C170" s="12" t="s">
+    </row>
+    <row r="176" ht="42.75" spans="1:4">
+      <c r="A176" s="27"/>
+      <c r="B176" s="18">
+        <v>5</v>
+      </c>
+      <c r="C176" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="D170" s="11" t="s">
+      <c r="D176" s="11" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="171" ht="31.5" hidden="1" spans="1:4">
-      <c r="A171" s="28"/>
-      <c r="B171" s="18">
-        <v>5</v>
-      </c>
-      <c r="C171" s="23" t="s">
+    <row r="177" ht="47.25" spans="1:4">
+      <c r="A177" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="D171" s="11" t="s">
+      <c r="B177" s="18">
+        <v>5</v>
+      </c>
+      <c r="C177" s="31" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="172" ht="63" hidden="1" spans="1:4">
-      <c r="A172" s="28" t="s">
+      <c r="D177" s="31" t="s">
         <v>240</v>
       </c>
-      <c r="B172" s="18">
-        <v>5</v>
-      </c>
-      <c r="C172" s="31" t="s">
+    </row>
+    <row r="178" ht="42" customHeight="1" spans="1:4">
+      <c r="A178" s="27"/>
+      <c r="B178" s="18">
+        <v>5</v>
+      </c>
+      <c r="C178" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="D172" s="31" t="s">
+      <c r="D178" s="12" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="173" ht="42" hidden="1" customHeight="1" spans="1:4">
-      <c r="A173" s="28"/>
-      <c r="B173" s="18">
-        <v>5</v>
-      </c>
-      <c r="C173" s="12" t="s">
+    <row r="179" ht="42" customHeight="1" spans="1:4">
+      <c r="A179" s="27"/>
+      <c r="B179" s="18">
+        <v>5</v>
+      </c>
+      <c r="C179" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="D173" s="12" t="s">
+      <c r="D179" s="12" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="174" ht="42" hidden="1" customHeight="1" spans="1:4">
-      <c r="A174" s="28"/>
-      <c r="B174" s="18">
-        <v>5</v>
-      </c>
-      <c r="C174" s="12" t="s">
+    <row r="180" ht="82" customHeight="1" spans="1:4">
+      <c r="A180" s="27"/>
+      <c r="B180" s="18">
+        <v>5</v>
+      </c>
+      <c r="C180" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="D174" s="12" t="s">
+      <c r="D180" s="12" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="175" ht="82" hidden="1" customHeight="1" spans="1:4">
-      <c r="A175" s="28"/>
-      <c r="B175" s="18">
-        <v>5</v>
-      </c>
-      <c r="C175" s="12" t="s">
+    <row r="181" ht="60.75" spans="1:4">
+      <c r="A181" s="27"/>
+      <c r="B181" s="24">
+        <v>5</v>
+      </c>
+      <c r="C181" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="D175" s="12" t="s">
+      <c r="D181" s="12" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="176" ht="63" hidden="1" spans="1:4">
-      <c r="A176" s="28"/>
-      <c r="B176" s="24">
-        <v>5</v>
-      </c>
-      <c r="C176" s="12" t="s">
+    <row r="182" ht="31.5" spans="1:4">
+      <c r="A182" s="27"/>
+      <c r="B182" s="18">
+        <v>5</v>
+      </c>
+      <c r="C182" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="D176" s="12" t="s">
+      <c r="D182" s="12" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="177" hidden="1" spans="1:4">
-      <c r="A177" s="28"/>
-      <c r="B177" s="18">
-        <v>5</v>
-      </c>
-      <c r="C177" s="12" t="s">
+    <row r="183" ht="220" customHeight="1" spans="1:4">
+      <c r="A183" s="27" t="s">
         <v>251</v>
       </c>
-      <c r="D177" s="12" t="s">
+      <c r="B183" s="18">
+        <v>5</v>
+      </c>
+      <c r="C183" s="12" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="178" ht="220" hidden="1" customHeight="1" spans="1:4">
-      <c r="A178" s="28" t="s">
+      <c r="D183" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="B178" s="18">
-        <v>5</v>
-      </c>
-      <c r="C178" s="12" t="s">
+    </row>
+    <row r="184" ht="31.5" spans="1:4">
+      <c r="A184" s="27"/>
+      <c r="B184" s="18">
+        <v>5</v>
+      </c>
+      <c r="C184" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="D178" s="12" t="s">
+      <c r="D184" s="12" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="179" ht="31.5" hidden="1" spans="1:4">
-      <c r="A179" s="28"/>
-      <c r="B179" s="18">
-        <v>5</v>
-      </c>
-      <c r="C179" s="12" t="s">
+    <row r="185" ht="141.75" spans="1:4">
+      <c r="A185" s="27"/>
+      <c r="B185" s="18">
+        <v>5</v>
+      </c>
+      <c r="C185" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="D179" s="12" t="s">
+      <c r="D185" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="180" ht="173.25" hidden="1" spans="1:4">
-      <c r="A180" s="28"/>
-      <c r="B180" s="18">
-        <v>5</v>
-      </c>
-      <c r="C180" s="2" t="s">
+    <row r="186" ht="47.25" spans="1:4">
+      <c r="A186" s="27"/>
+      <c r="B186" s="18">
+        <v>5</v>
+      </c>
+      <c r="C186" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D180" s="2" t="s">
+      <c r="D186" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="181" ht="47.25" hidden="1" spans="1:4">
-      <c r="A181" s="28"/>
-      <c r="B181" s="18">
-        <v>5</v>
-      </c>
-      <c r="C181" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="D181" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="E1:E181">
-    <filterColumn colId="0">
-      <customFilters>
-        <customFilter operator="equal" val="edge"/>
-      </customFilters>
-    </filterColumn>
-    <extLst/>
-  </autoFilter>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A16"/>
     <mergeCell ref="A17:A54"/>
     <mergeCell ref="A55:A68"/>
     <mergeCell ref="A69:A129"/>
-    <mergeCell ref="A130:A141"/>
-    <mergeCell ref="A148:A165"/>
-    <mergeCell ref="A166:A171"/>
-    <mergeCell ref="A172:A177"/>
-    <mergeCell ref="A178:A181"/>
+    <mergeCell ref="A130:A144"/>
+    <mergeCell ref="A145:A162"/>
+    <mergeCell ref="A163:A170"/>
+    <mergeCell ref="A171:A176"/>
+    <mergeCell ref="A177:A182"/>
+    <mergeCell ref="A183:A186"/>
   </mergeCells>
-  <conditionalFormatting sqref="B131">
+  <conditionalFormatting sqref="B130">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4368,7 +4440,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B50 B52:B53 B132:B1048576 B55:B67 B69:B130">
+  <conditionalFormatting sqref="B1:B53 B55:B67 B69:B129 B131:B1048576">
     <cfRule type="cellIs" dxfId="0" priority="4" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
add some new cvpr2019 paper
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27270" windowHeight="12525" tabRatio="354"/>
+    <workbookView windowWidth="14670" windowHeight="25125" tabRatio="354"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$186</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$187</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="266">
   <si>
     <t>Scope</t>
   </si>
@@ -231,6 +231,9 @@
     <t>An Empirical Study of Spatial Attention Mechanisms in Deep Networks</t>
   </si>
   <si>
+    <t>Stand-Alone Self-Attention in Vision Models</t>
+  </si>
+  <si>
     <t>Stacked Hourglass Networks for Human Pose Estimation</t>
   </si>
   <si>
@@ -270,6 +273,9 @@
     <t>ImageNet-trained CNNs are biased towards texture; increasing shape bias improves accuracy and robustness</t>
   </si>
   <si>
+    <t>further advantages of data augmentation on convolutional neural networks</t>
+  </si>
+  <si>
     <t>object detection</t>
   </si>
   <si>
@@ -333,6 +339,9 @@
   </si>
   <si>
     <t>(cvpr 2019)An Energy and GPU-Computation Efficient Backbone Network for Real-Time Object Detection</t>
+  </si>
+  <si>
+    <t>SkyNet: A Champion Model for DAC-SDC on Low Power Object Detection</t>
   </si>
   <si>
     <t>Beyond pixels: A comprehensive survey from bottom-up to semantic image segmentation and cosegmentation(文章偏早)</t>
@@ -680,6 +689,9 @@
     <t>Decoders Matter for Semantic Segmentation_Data-Dependent Decoding Enables Flexible Feature Aggregation</t>
   </si>
   <si>
+    <t>Context reinforced Semantic Segmentation</t>
+  </si>
+  <si>
     <t>SEMEDA: Enhancing Segmentation Precision with Semantic Edge Aware Loss</t>
   </si>
   <si>
@@ -869,6 +881,9 @@
     <t>Segmentation is All You Need</t>
   </si>
   <si>
+    <t>instance segmentation by jointly optimizing spatial embeddings and clustering Bandwidth</t>
+  </si>
+  <si>
     <t>Semantic Instance Segmentation with a Discriminative Loss Function</t>
   </si>
   <si>
@@ -901,10 +916,22 @@
     <t>(2019) Agnostic Lane detection</t>
   </si>
   <si>
+    <t>是一篇研究生的学期报告
+用proposal free的instance segmentation的方法检测车道线， 增加了line points和drivable area两个辅助任务
+车道线的embedding branch和其他branch分开测</t>
+  </si>
+  <si>
     <t>(2019) FastDraw: Addressing the Long Tail of Lane Detection by Adapting a Sequential Prediction Network</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>end to end的车道线检测; 用了style transfer的方法，能够快速adapt到新的场景； 90FPS on 1080
 对车道线检测的需求：1. able to represent any number of lines of any length; 2. run in real-time; 3. adapt quikly to new scenes
 网络输出一张各个点在车道线上的概率；一张每个点的</t>
@@ -1084,10 +1111,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1132,19 +1159,11 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1156,6 +1175,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1179,13 +1213,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -1194,16 +1221,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1217,21 +1266,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1240,29 +1289,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1322,19 +1349,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1346,13 +1361,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1364,7 +1373,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1376,121 +1385,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1503,6 +1422,114 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1555,6 +1582,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1574,7 +1636,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1582,34 +1659,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1628,177 +1679,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1878,11 +1905,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2008,13 +2035,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>292735</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>319405</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>713740</xdr:colOff>
-      <xdr:row>85</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>134620</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2032,7 +2059,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14424025" y="48287305"/>
+          <a:off x="14424025" y="49160430"/>
           <a:ext cx="3658870" cy="2015490"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2050,13 +2077,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>85</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>1755140</xdr:colOff>
-      <xdr:row>85</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>1853565</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2074,7 +2101,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14131290" y="50168175"/>
+          <a:off x="14131290" y="51041300"/>
           <a:ext cx="2499360" cy="1853565"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2092,14 +2119,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>742315</xdr:colOff>
-      <xdr:row>124</xdr:row>
-      <xdr:rowOff>33655</xdr:rowOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>233680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2116,7 +2143,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14131290" y="75866625"/>
+          <a:off x="14131290" y="76939775"/>
           <a:ext cx="3980180" cy="2386330"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2134,13 +2161,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>138</xdr:row>
+      <xdr:row>139</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>619760</xdr:colOff>
-      <xdr:row>138</xdr:row>
+      <xdr:row>139</xdr:row>
       <xdr:rowOff>2569845</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2158,7 +2185,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14131290" y="88795225"/>
+          <a:off x="14131290" y="89668350"/>
           <a:ext cx="5536565" cy="2550795"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2433,12 +2460,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G186"/>
+  <dimension ref="A1:G187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C165" sqref="C165"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="15.75" outlineLevelCol="6"/>
@@ -2901,10 +2928,10 @@
     </row>
     <row r="41" ht="53" customHeight="1" spans="1:4">
       <c r="A41" s="9"/>
-      <c r="B41" s="16">
+      <c r="B41" s="14">
         <v>1</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="12" t="s">
         <v>66</v>
       </c>
       <c r="D41" s="11"/>
@@ -2939,7 +2966,7 @@
       </c>
       <c r="D44" s="11"/>
     </row>
-    <row r="45" ht="70" customHeight="1" spans="1:4">
+    <row r="45" ht="53" customHeight="1" spans="1:4">
       <c r="A45" s="9"/>
       <c r="B45" s="16">
         <v>1</v>
@@ -2949,12 +2976,12 @@
       </c>
       <c r="D45" s="11"/>
     </row>
-    <row r="46" ht="53" customHeight="1" spans="1:4">
+    <row r="46" ht="70" customHeight="1" spans="1:4">
       <c r="A46" s="9"/>
-      <c r="B46" s="14">
+      <c r="B46" s="16">
         <v>1</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="11" t="s">
         <v>71</v>
       </c>
       <c r="D46" s="11"/>
@@ -2962,31 +2989,31 @@
     <row r="47" ht="53" customHeight="1" spans="1:4">
       <c r="A47" s="9"/>
       <c r="B47" s="14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C47" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D47" s="11" t="s">
-        <v>73</v>
-      </c>
+      <c r="D47" s="11"/>
     </row>
     <row r="48" ht="53" customHeight="1" spans="1:4">
       <c r="A48" s="9"/>
       <c r="B48" s="14">
-        <v>1</v>
-      </c>
-      <c r="C48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D48" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D48" s="12"/>
     </row>
     <row r="49" ht="53" customHeight="1" spans="1:4">
       <c r="A49" s="9"/>
-      <c r="B49" s="17">
+      <c r="B49" s="14">
         <v>1</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="2" t="s">
         <v>75</v>
       </c>
       <c r="D49" s="12"/>
@@ -2996,12 +3023,12 @@
       <c r="B50" s="17">
         <v>1</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="12" t="s">
         <v>76</v>
       </c>
       <c r="D50" s="12"/>
     </row>
-    <row r="51" ht="53" customHeight="1" spans="1:3">
+    <row r="51" ht="53" customHeight="1" spans="1:4">
       <c r="A51" s="9"/>
       <c r="B51" s="17">
         <v>1</v>
@@ -3009,52 +3036,53 @@
       <c r="C51" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="52" ht="53" customHeight="1" spans="1:4">
+      <c r="D51" s="12"/>
+    </row>
+    <row r="52" ht="53" customHeight="1" spans="1:3">
       <c r="A52" s="9"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
+      <c r="B52" s="17">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="53" ht="53" customHeight="1" spans="1:4">
       <c r="A53" s="9"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="12"/>
+      <c r="B53" s="17">
+        <v>1</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>79</v>
+      </c>
       <c r="D53" s="12"/>
     </row>
-    <row r="54" ht="41" customHeight="1" spans="1:1">
+    <row r="54" ht="53" customHeight="1" spans="1:4">
       <c r="A54" s="9"/>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B55" s="14">
-        <v>5</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D55" s="11"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
-    </row>
-    <row r="56" ht="63" spans="1:6">
-      <c r="A56" s="9"/>
+      <c r="B54" s="17"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+    </row>
+    <row r="55" ht="41" customHeight="1" spans="1:1">
+      <c r="A55" s="9"/>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="B56" s="14">
         <v>5</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D56" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="F56" s="1"/>
-    </row>
-    <row r="57" ht="47.25" spans="1:4">
+      <c r="D56" s="11"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+    </row>
+    <row r="57" ht="63" spans="1:6">
       <c r="A57" s="9"/>
-      <c r="B57" s="10">
+      <c r="B57" s="14">
         <v>5</v>
       </c>
       <c r="C57" s="11" t="s">
@@ -3063,8 +3091,9 @@
       <c r="D57" s="11" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="58" ht="78.75" spans="1:4">
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" ht="47.25" spans="1:4">
       <c r="A58" s="9"/>
       <c r="B58" s="10">
         <v>5</v>
@@ -3076,12 +3105,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="59" ht="31.5" spans="1:4">
+    <row r="59" ht="78.75" spans="1:4">
       <c r="A59" s="9"/>
-      <c r="B59" s="18">
-        <v>5</v>
-      </c>
-      <c r="C59" s="2" t="s">
+      <c r="B59" s="10">
+        <v>5</v>
+      </c>
+      <c r="C59" s="11" t="s">
         <v>86</v>
       </c>
       <c r="D59" s="11" t="s">
@@ -3090,7 +3119,7 @@
     </row>
     <row r="60" ht="31.5" spans="1:4">
       <c r="A60" s="9"/>
-      <c r="B60" s="10">
+      <c r="B60" s="18">
         <v>5</v>
       </c>
       <c r="C60" s="2" t="s">
@@ -3103,26 +3132,26 @@
     <row r="61" ht="31.5" spans="1:4">
       <c r="A61" s="9"/>
       <c r="B61" s="10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D61" s="11"/>
-    </row>
-    <row r="62" ht="94.5" spans="1:4">
+      <c r="D61" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" ht="31.5" spans="1:4">
       <c r="A62" s="9"/>
       <c r="B62" s="10">
-        <v>5</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="D62" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="63" ht="47.25" spans="1:4">
+      <c r="D62" s="11"/>
+    </row>
+    <row r="63" ht="94.5" spans="1:4">
       <c r="A63" s="9"/>
       <c r="B63" s="10">
         <v>5</v>
@@ -3137,23 +3166,33 @@
     <row r="64" ht="47.25" spans="1:4">
       <c r="A64" s="9"/>
       <c r="B64" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C64" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D64" s="11"/>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="D64" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="65" ht="47.25" spans="1:4">
       <c r="A65" s="9"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="12"/>
+      <c r="B65" s="10">
+        <v>1</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>97</v>
+      </c>
       <c r="D65" s="11"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" ht="31.5" spans="1:4">
       <c r="A66" s="9"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="12"/>
+      <c r="B66" s="10">
+        <v>1</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="D66" s="11"/>
     </row>
     <row r="67" spans="1:4">
@@ -3162,41 +3201,35 @@
       <c r="C67" s="12"/>
       <c r="D67" s="11"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:4">
       <c r="A68" s="9"/>
-    </row>
-    <row r="69" ht="47.25" spans="1:4">
-      <c r="A69" s="20"/>
-      <c r="B69" s="10">
-        <v>5</v>
-      </c>
-      <c r="C69" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D69" s="11"/>
-    </row>
-    <row r="70" ht="63" spans="1:4">
+      <c r="B68" s="10"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="11"/>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="9"/>
+    </row>
+    <row r="70" ht="47.25" spans="1:4">
       <c r="A70" s="20"/>
       <c r="B70" s="10">
+        <v>5</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D70" s="11"/>
+    </row>
+    <row r="71" ht="63" spans="1:4">
+      <c r="A71" s="20"/>
+      <c r="B71" s="10">
         <v>6</v>
       </c>
-      <c r="C70" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="71" ht="31.5" spans="1:4">
-      <c r="A71" s="20"/>
-      <c r="B71" s="18">
-        <v>5</v>
-      </c>
       <c r="C71" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="72" ht="31.5" spans="1:4">
@@ -3205,133 +3238,133 @@
         <v>5</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="73" ht="110.25" spans="1:4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="73" ht="31.5" spans="1:4">
       <c r="A73" s="20"/>
       <c r="B73" s="18">
         <v>5</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="74" ht="92.25" spans="1:4">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="74" ht="110.25" spans="1:4">
       <c r="A74" s="20"/>
       <c r="B74" s="18">
         <v>5</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="75" ht="157.5" spans="1:4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="75" ht="92.25" spans="1:4">
       <c r="A75" s="20"/>
       <c r="B75" s="18">
         <v>5</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="D75" s="8" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="76" ht="60.75" spans="1:4">
+      <c r="D75" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="76" ht="157.5" spans="1:4">
       <c r="A76" s="20"/>
       <c r="B76" s="18">
         <v>5</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="D76" s="11" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="77" ht="126" spans="1:4">
+      <c r="D76" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="77" ht="60.75" spans="1:4">
       <c r="A77" s="20"/>
       <c r="B77" s="18">
         <v>5</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="78" ht="31.5" spans="1:4">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" ht="126" spans="1:4">
       <c r="A78" s="20"/>
       <c r="B78" s="18">
         <v>5</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="D78" s="11"/>
-    </row>
-    <row r="79" ht="60.75" spans="1:4">
+        <v>114</v>
+      </c>
+      <c r="D78" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="79" ht="31.5" spans="1:4">
       <c r="A79" s="20"/>
       <c r="B79" s="18">
         <v>5</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D79" s="11"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" ht="60.75" spans="1:4">
       <c r="A80" s="20"/>
       <c r="B80" s="18">
-        <v>2</v>
-      </c>
-      <c r="C80" t="s">
-        <v>115</v>
+        <v>5</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>117</v>
       </c>
       <c r="D80" s="11"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="20"/>
       <c r="B81" s="18">
-        <v>5</v>
-      </c>
-      <c r="C81" s="12" t="s">
-        <v>116</v>
+        <v>2</v>
+      </c>
+      <c r="C81" t="s">
+        <v>118</v>
       </c>
       <c r="D81" s="11"/>
     </row>
-    <row r="82" ht="31.5" spans="1:4">
+    <row r="82" spans="1:4">
       <c r="A82" s="20"/>
       <c r="B82" s="18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D82" s="11"/>
     </row>
-    <row r="83" ht="47.25" spans="1:4">
+    <row r="83" ht="31.5" spans="1:4">
       <c r="A83" s="20"/>
       <c r="B83" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D83" s="11" t="s">
-        <v>119</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="D83" s="11"/>
     </row>
     <row r="84" ht="47.25" spans="1:4">
       <c r="A84" s="20"/>
@@ -3339,28 +3372,25 @@
         <v>5</v>
       </c>
       <c r="C84" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="85" ht="173.25" spans="1:5">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="85" ht="47.25" spans="1:4">
       <c r="A85" s="20"/>
       <c r="B85" s="18">
         <v>5</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="D85" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="E85" s="26" t="s">
+      <c r="D85" s="11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="86" ht="155" customHeight="1" spans="1:5">
+    <row r="86" ht="173.25" spans="1:5">
       <c r="A86" s="20"/>
       <c r="B86" s="18">
         <v>5</v>
@@ -3368,14 +3398,14 @@
       <c r="C86" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="D86" s="11" t="s">
+      <c r="D86" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="E86" s="25" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="87" ht="47.25" spans="1:4">
+    <row r="87" ht="155" customHeight="1" spans="1:5">
       <c r="A87" s="20"/>
       <c r="B87" s="18">
         <v>5</v>
@@ -3385,6 +3415,9 @@
       </c>
       <c r="D87" s="11" t="s">
         <v>129</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="88" ht="47.25" spans="1:4">
@@ -3393,342 +3426,344 @@
         <v>5</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="89" ht="141.75" spans="1:4">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="89" ht="47.25" spans="1:4">
       <c r="A89" s="20"/>
       <c r="B89" s="18">
         <v>5</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>132</v>
+      <c r="C89" s="12" t="s">
+        <v>133</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="90" ht="63" spans="1:4">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="90" ht="141.75" spans="1:4">
       <c r="A90" s="20"/>
       <c r="B90" s="18">
         <v>5</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="91" ht="47.25" spans="1:4">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="91" ht="63" spans="1:4">
       <c r="A91" s="20"/>
       <c r="B91" s="18">
         <v>5</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="92" ht="31.5" spans="1:4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="92" ht="47.25" spans="1:4">
       <c r="A92" s="20"/>
       <c r="B92" s="18">
         <v>5</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="93" ht="31.5" spans="1:4">
       <c r="A93" s="20"/>
       <c r="B93" s="18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D93" s="11"/>
-    </row>
-    <row r="94" ht="47.25" spans="1:4">
+        <v>141</v>
+      </c>
+      <c r="D93" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="94" ht="31.5" spans="1:4">
       <c r="A94" s="20"/>
       <c r="B94" s="18">
         <v>2</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D94" s="11"/>
     </row>
-    <row r="95" ht="31.5" spans="1:4">
+    <row r="95" ht="47.25" spans="1:4">
       <c r="A95" s="20"/>
       <c r="B95" s="18">
         <v>2</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D95" s="11"/>
     </row>
-    <row r="96" ht="47.25" spans="1:4">
+    <row r="96" ht="31.5" spans="1:4">
       <c r="A96" s="20"/>
       <c r="B96" s="18">
         <v>2</v>
       </c>
-      <c r="C96" s="12" t="s">
-        <v>143</v>
+      <c r="C96" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="D96" s="11"/>
     </row>
-    <row r="97" ht="31.5" spans="1:4">
+    <row r="97" ht="47.25" spans="1:4">
       <c r="A97" s="20"/>
       <c r="B97" s="18">
         <v>2</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D97" s="11"/>
     </row>
-    <row r="98" ht="63" spans="1:4">
+    <row r="98" ht="31.5" spans="1:4">
       <c r="A98" s="20"/>
       <c r="B98" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="D98" s="11" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="99" ht="31.5" spans="1:4">
+        <v>147</v>
+      </c>
+      <c r="D98" s="11"/>
+    </row>
+    <row r="99" ht="63" spans="1:4">
       <c r="A99" s="20"/>
       <c r="B99" s="18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="D99" s="11"/>
-    </row>
-    <row r="100" ht="60.75" spans="1:4">
+        <v>148</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="100" ht="31.5" spans="1:4">
       <c r="A100" s="20"/>
       <c r="B100" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="D100" s="11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="101" ht="31.5" spans="1:4">
+        <v>150</v>
+      </c>
+      <c r="D100" s="11"/>
+    </row>
+    <row r="101" ht="60.75" spans="1:4">
       <c r="A101" s="20"/>
       <c r="B101" s="18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="D101" s="21"/>
-    </row>
-    <row r="102" ht="94.5" spans="1:4">
+        <v>151</v>
+      </c>
+      <c r="D101" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="102" ht="31.5" spans="1:4">
       <c r="A102" s="20"/>
       <c r="B102" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="D102" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="103" ht="31.5" spans="1:4">
+        <v>153</v>
+      </c>
+      <c r="D102" s="21"/>
+    </row>
+    <row r="103" ht="94.5" spans="1:4">
       <c r="A103" s="20"/>
       <c r="B103" s="18">
         <v>5</v>
       </c>
-      <c r="C103" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="D103" s="21"/>
-    </row>
-    <row r="104" ht="47.25" spans="1:4">
+      <c r="C103" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D103" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="104" ht="31.5" spans="1:4">
       <c r="A104" s="20"/>
       <c r="B104" s="18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C104" s="22" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D104" s="21"/>
     </row>
-    <row r="105" ht="31.5" spans="1:4">
+    <row r="105" ht="47.25" spans="1:4">
       <c r="A105" s="20"/>
       <c r="B105" s="18">
         <v>2</v>
       </c>
       <c r="C105" s="22" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D105" s="21"/>
     </row>
-    <row r="106" ht="47.25" spans="1:4">
+    <row r="106" ht="31.5" spans="1:4">
       <c r="A106" s="20"/>
       <c r="B106" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C106" s="22" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D106" s="21"/>
     </row>
-    <row r="107" ht="110.25" spans="1:4">
+    <row r="107" ht="47.25" spans="1:4">
       <c r="A107" s="20"/>
       <c r="B107" s="18">
         <v>5</v>
       </c>
-      <c r="C107" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D107" s="21" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="108" ht="31.5" spans="1:4">
+      <c r="C107" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="D107" s="21"/>
+    </row>
+    <row r="108" ht="110.25" spans="1:4">
       <c r="A108" s="20"/>
       <c r="B108" s="18">
         <v>5</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D108" s="21" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="109" ht="47.25" spans="1:4">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="109" ht="31.5" spans="1:4">
       <c r="A109" s="20"/>
       <c r="B109" s="18">
         <v>5</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="D109" s="11" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="110" ht="63" spans="1:4">
+      <c r="D109" s="21" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="110" ht="47.25" spans="1:4">
       <c r="A110" s="20"/>
       <c r="B110" s="18">
         <v>5</v>
       </c>
-      <c r="C110" s="23" t="s">
-        <v>163</v>
+      <c r="C110" s="12" t="s">
+        <v>164</v>
       </c>
       <c r="D110" s="11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="111" ht="126" spans="1:4">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="111" ht="63" spans="1:4">
       <c r="A111" s="20"/>
       <c r="B111" s="18">
         <v>5</v>
       </c>
-      <c r="C111" s="11" t="s">
-        <v>165</v>
+      <c r="C111" s="23" t="s">
+        <v>166</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="112" ht="31" customHeight="1" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="112" ht="126" spans="1:4">
       <c r="A112" s="20"/>
-      <c r="B112" s="24">
-        <v>1</v>
-      </c>
-      <c r="C112" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="D112" s="12" t="s">
+      <c r="B112" s="18">
+        <v>5</v>
+      </c>
+      <c r="C112" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="E112" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="113" ht="47.25" spans="1:4">
+      <c r="D112" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="113" ht="31" customHeight="1" spans="1:5">
       <c r="A113" s="20"/>
       <c r="B113" s="24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="D113" s="12"/>
+        <v>170</v>
+      </c>
+      <c r="D113" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="114" ht="47.25" spans="1:4">
       <c r="A114" s="20"/>
       <c r="B114" s="24">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D114" s="12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="115" ht="31.5" spans="1:4">
+        <v>172</v>
+      </c>
+      <c r="D114" s="12"/>
+    </row>
+    <row r="115" ht="47.25" spans="1:4">
       <c r="A115" s="20"/>
       <c r="B115" s="24">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="D115" s="12"/>
-    </row>
-    <row r="116" ht="60.75" spans="1:4">
+        <v>173</v>
+      </c>
+      <c r="D115" s="12" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="116" ht="31.5" spans="1:4">
       <c r="A116" s="20"/>
       <c r="B116" s="24">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="D116" s="12" t="s">
-        <v>174</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="D116" s="12"/>
     </row>
     <row r="117" ht="60.75" spans="1:4">
       <c r="A117" s="20"/>
       <c r="B117" s="24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="D117" s="12"/>
-    </row>
-    <row r="118" ht="31.5" spans="1:4">
+        <v>176</v>
+      </c>
+      <c r="D117" s="12" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="118" ht="60.75" spans="1:4">
       <c r="A118" s="20"/>
       <c r="B118" s="24">
         <v>1</v>
       </c>
       <c r="C118" s="12" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D118" s="12"/>
     </row>
@@ -3738,17 +3773,17 @@
         <v>1</v>
       </c>
       <c r="C119" s="12" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D119" s="12"/>
     </row>
-    <row r="120" ht="47.25" spans="1:4">
+    <row r="120" ht="31.5" spans="1:4">
       <c r="A120" s="20"/>
       <c r="B120" s="24">
         <v>1</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D120" s="12"/>
     </row>
@@ -3758,7 +3793,7 @@
         <v>1</v>
       </c>
       <c r="C121" s="12" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D121" s="12"/>
     </row>
@@ -3768,42 +3803,44 @@
         <v>1</v>
       </c>
       <c r="C122" s="12" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D122" s="12"/>
     </row>
-    <row r="123" ht="171" spans="1:5">
+    <row r="123" ht="47.25" spans="1:4">
       <c r="A123" s="20"/>
       <c r="B123" s="24">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C123" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="D123" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="E123" t="s">
-        <v>124</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="D123" s="12"/>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="20"/>
       <c r="B124" s="24">
         <v>1</v>
       </c>
-      <c r="C124" s="12"/>
+      <c r="C124" s="12" t="s">
+        <v>184</v>
+      </c>
       <c r="D124" s="12"/>
     </row>
-    <row r="125" ht="31.5" spans="1:4">
+    <row r="125" ht="171" spans="1:5">
       <c r="A125" s="20"/>
       <c r="B125" s="24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C125" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="D125" s="12"/>
+        <v>185</v>
+      </c>
+      <c r="D125" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="E125" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="126" ht="31.5" spans="1:4">
       <c r="A126" s="20"/>
@@ -3811,67 +3848,67 @@
         <v>1</v>
       </c>
       <c r="C126" s="12" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D126" s="12"/>
     </row>
-    <row r="127" ht="31.5" spans="1:5">
+    <row r="127" ht="31.5" spans="1:4">
       <c r="A127" s="20"/>
-      <c r="B127" s="17">
-        <v>5</v>
+      <c r="B127" s="24">
+        <v>1</v>
       </c>
       <c r="C127" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="D127" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="E127" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="128" ht="108" spans="1:5">
+        <v>188</v>
+      </c>
+      <c r="D127" s="12"/>
+    </row>
+    <row r="128" ht="31.5" spans="1:5">
       <c r="A128" s="20"/>
-      <c r="B128" s="24">
+      <c r="B128" s="17">
         <v>5</v>
       </c>
       <c r="C128" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="D128" s="25" t="s">
-        <v>188</v>
+        <v>189</v>
+      </c>
+      <c r="D128" s="12" t="s">
+        <v>190</v>
       </c>
       <c r="E128" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" ht="108" spans="1:5">
       <c r="A129" s="20"/>
-      <c r="B129" s="24"/>
-      <c r="C129" s="12"/>
-      <c r="D129" s="12"/>
-    </row>
-    <row r="130" ht="126" spans="1:4">
-      <c r="A130" s="27"/>
-      <c r="B130" s="24">
-        <v>5</v>
-      </c>
-      <c r="C130" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="D130" s="11" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="131" ht="31.5" spans="1:4">
+      <c r="B129" s="24">
+        <v>5</v>
+      </c>
+      <c r="C129" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D129" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="E129" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="20"/>
+      <c r="B130" s="24"/>
+      <c r="C130" s="12"/>
+      <c r="D130" s="12"/>
+    </row>
+    <row r="131" ht="126" spans="1:4">
       <c r="A131" s="27"/>
       <c r="B131" s="24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C131" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="D131" s="11"/>
+        <v>193</v>
+      </c>
+      <c r="D131" s="11" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="132" ht="31.5" spans="1:4">
       <c r="A132" s="27"/>
@@ -3879,41 +3916,41 @@
         <v>1</v>
       </c>
       <c r="C132" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="D132" s="12"/>
+        <v>195</v>
+      </c>
+      <c r="D132" s="11"/>
     </row>
     <row r="133" ht="31.5" spans="1:4">
       <c r="A133" s="27"/>
-      <c r="B133" s="18">
+      <c r="B133" s="24">
         <v>1</v>
       </c>
-      <c r="C133" s="28" t="s">
-        <v>193</v>
-      </c>
-      <c r="D133" s="11"/>
-    </row>
-    <row r="134" ht="47.25" spans="1:4">
+      <c r="C133" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D133" s="12"/>
+    </row>
+    <row r="134" ht="31.5" spans="1:4">
       <c r="A134" s="27"/>
       <c r="B134" s="18">
-        <v>5</v>
-      </c>
-      <c r="C134" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D134" s="8" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="135" ht="31.5" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="C134" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="D134" s="11"/>
+    </row>
+    <row r="135" ht="47.25" spans="1:4">
       <c r="A135" s="27"/>
       <c r="B135" s="18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C135" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="D135" s="11"/>
+        <v>198</v>
+      </c>
+      <c r="D135" s="8" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="136" ht="31.5" spans="1:4">
       <c r="A136" s="27"/>
@@ -3921,54 +3958,58 @@
         <v>1</v>
       </c>
       <c r="C136" s="12" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D136" s="11"/>
     </row>
-    <row r="137" ht="47.25" spans="1:4">
+    <row r="137" ht="31.5" spans="1:4">
       <c r="A137" s="27"/>
       <c r="B137" s="18">
-        <v>5</v>
-      </c>
-      <c r="C137" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="D137" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="138" ht="235" customHeight="1" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="C137" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="D137" s="11"/>
+    </row>
+    <row r="138" ht="47.25" spans="1:4">
       <c r="A138" s="27"/>
       <c r="B138" s="18">
         <v>5</v>
       </c>
-      <c r="C138" s="12" t="s">
-        <v>200</v>
+      <c r="C138" s="11" t="s">
+        <v>202</v>
       </c>
       <c r="D138" s="11" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="139" ht="208" customHeight="1" spans="1:5">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="139" ht="235" customHeight="1" spans="1:4">
       <c r="A139" s="27"/>
       <c r="B139" s="18">
         <v>5</v>
       </c>
       <c r="C139" s="12" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D139" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="E139" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="140" ht="20" customHeight="1" spans="1:4">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="140" ht="208" customHeight="1" spans="1:5">
       <c r="A140" s="27"/>
-      <c r="B140" s="18"/>
-      <c r="C140" s="12"/>
-      <c r="D140" s="11"/>
+      <c r="B140" s="18">
+        <v>5</v>
+      </c>
+      <c r="C140" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="D140" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="E140" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="141" ht="20" customHeight="1" spans="1:4">
       <c r="A141" s="27"/>
@@ -3988,31 +4029,27 @@
       <c r="C143" s="12"/>
       <c r="D143" s="11"/>
     </row>
-    <row r="144" ht="28" customHeight="1" spans="1:4">
+    <row r="144" ht="20" customHeight="1" spans="1:4">
       <c r="A144" s="27"/>
       <c r="B144" s="18"/>
       <c r="C144" s="12"/>
       <c r="D144" s="11"/>
     </row>
-    <row r="145" spans="1:4">
-      <c r="A145" s="27" t="s">
-        <v>204</v>
-      </c>
-      <c r="B145" s="18">
+    <row r="145" ht="28" customHeight="1" spans="1:4">
+      <c r="A145" s="27"/>
+      <c r="B145" s="18"/>
+      <c r="C145" s="12"/>
+      <c r="D145" s="11"/>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="B146" s="18">
         <v>2</v>
       </c>
-      <c r="C145" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="D145" s="11"/>
-    </row>
-    <row r="146" ht="31.5" spans="1:4">
-      <c r="A146" s="27"/>
-      <c r="B146" s="18">
-        <v>1</v>
-      </c>
       <c r="C146" s="12" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D146" s="11"/>
     </row>
@@ -4021,8 +4058,8 @@
       <c r="B147" s="18">
         <v>1</v>
       </c>
-      <c r="C147" s="2" t="s">
-        <v>207</v>
+      <c r="C147" s="12" t="s">
+        <v>210</v>
       </c>
       <c r="D147" s="11"/>
     </row>
@@ -4032,7 +4069,7 @@
         <v>1</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D148" s="11"/>
     </row>
@@ -4042,7 +4079,7 @@
         <v>1</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D149" s="11"/>
     </row>
@@ -4052,7 +4089,7 @@
         <v>1</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D150" s="11"/>
     </row>
@@ -4062,7 +4099,7 @@
         <v>1</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D151" s="11"/>
     </row>
@@ -4072,7 +4109,7 @@
         <v>1</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D152" s="11"/>
     </row>
@@ -4082,7 +4119,7 @@
         <v>1</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D153" s="11"/>
     </row>
@@ -4092,28 +4129,38 @@
         <v>1</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D154" s="11"/>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" ht="31.5" spans="1:4">
       <c r="A155" s="27"/>
       <c r="B155" s="18">
         <v>1</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D155" s="11"/>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" s="27"/>
-      <c r="B156" s="18"/>
+      <c r="B156" s="18">
+        <v>1</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>219</v>
+      </c>
       <c r="D156" s="11"/>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" ht="31.5" spans="1:4">
       <c r="A157" s="27"/>
-      <c r="B157" s="18"/>
+      <c r="B157" s="18">
+        <v>1</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>220</v>
+      </c>
       <c r="D157" s="11"/>
     </row>
     <row r="158" spans="1:4">
@@ -4126,69 +4173,72 @@
       <c r="B159" s="18"/>
       <c r="D159" s="11"/>
     </row>
-    <row r="160" ht="126" spans="1:4">
+    <row r="160" spans="1:4">
       <c r="A160" s="27"/>
-      <c r="B160" s="18">
-        <v>5</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D160" s="11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="161" ht="78.75" spans="1:4">
+      <c r="B160" s="18"/>
+      <c r="D160" s="11"/>
+    </row>
+    <row r="161" ht="126" spans="1:4">
       <c r="A161" s="27"/>
       <c r="B161" s="18">
         <v>5</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="D161" s="11" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="162" ht="139.5" spans="1:4">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="162" ht="78.75" spans="1:4">
       <c r="A162" s="27"/>
       <c r="B162" s="18">
         <v>5</v>
       </c>
-      <c r="C162" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="D162" s="29" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4">
-      <c r="A163" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="B163" s="18"/>
+      <c r="C162" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D162" s="11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="163" ht="139.5" spans="1:4">
+      <c r="A163" s="27"/>
+      <c r="B163" s="18">
+        <v>5</v>
+      </c>
       <c r="C163" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="D163" s="29"/>
-    </row>
-    <row r="164" ht="202.5" spans="1:4">
-      <c r="A164" s="27"/>
+        <v>225</v>
+      </c>
+      <c r="D163" s="29" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="164" ht="47.25" spans="1:4">
+      <c r="A164" s="27" t="s">
+        <v>227</v>
+      </c>
       <c r="B164" s="18">
         <v>5</v>
       </c>
       <c r="C164" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="D164" s="30" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4">
+        <v>228</v>
+      </c>
+      <c r="D164" s="29" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="165" ht="202.5" spans="1:4">
       <c r="A165" s="27"/>
-      <c r="B165" s="18"/>
-      <c r="C165" s="12"/>
-      <c r="D165" s="29"/>
+      <c r="B165" s="18">
+        <v>5</v>
+      </c>
+      <c r="C165" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="D165" s="30" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" s="27"/>
@@ -4220,28 +4270,22 @@
       <c r="C170" s="12"/>
       <c r="D170" s="29"/>
     </row>
-    <row r="171" ht="31.5" spans="1:4">
-      <c r="A171" s="27" t="s">
-        <v>226</v>
-      </c>
+    <row r="171" spans="1:4">
+      <c r="A171" s="27"/>
       <c r="B171" s="18"/>
-      <c r="C171" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D171" s="29" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="172" ht="47.25" spans="1:4">
-      <c r="A172" s="27"/>
-      <c r="B172" s="18">
-        <v>5</v>
-      </c>
+      <c r="C171" s="12"/>
+      <c r="D171" s="29"/>
+    </row>
+    <row r="172" ht="31.5" spans="1:4">
+      <c r="A172" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="B172" s="18"/>
       <c r="C172" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="D172" s="11" t="s">
-        <v>230</v>
+        <v>233</v>
+      </c>
+      <c r="D172" s="29" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="173" ht="47.25" spans="1:4">
@@ -4250,70 +4294,70 @@
         <v>5</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D173" s="11" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="174" ht="47.25" spans="1:4">
       <c r="A174" s="27"/>
       <c r="B174" s="18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C174" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="D174" s="11"/>
-    </row>
-    <row r="175" ht="109" customHeight="1" spans="1:4">
+        <v>237</v>
+      </c>
+      <c r="D174" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
       <c r="A175" s="27"/>
       <c r="B175" s="18">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C175" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="D175" s="11" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="176" ht="42.75" spans="1:4">
+        <v>239</v>
+      </c>
+      <c r="D175" s="11"/>
+    </row>
+    <row r="176" ht="109" customHeight="1" spans="1:4">
       <c r="A176" s="27"/>
       <c r="B176" s="18">
         <v>5</v>
       </c>
-      <c r="C176" s="23" t="s">
-        <v>236</v>
+      <c r="C176" s="12" t="s">
+        <v>240</v>
       </c>
       <c r="D176" s="11" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="177" ht="47.25" spans="1:4">
-      <c r="A177" s="27" t="s">
-        <v>238</v>
-      </c>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="177" ht="42.75" spans="1:4">
+      <c r="A177" s="27"/>
       <c r="B177" s="18">
         <v>5</v>
       </c>
-      <c r="C177" s="31" t="s">
-        <v>239</v>
-      </c>
-      <c r="D177" s="31" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="178" ht="42" customHeight="1" spans="1:4">
-      <c r="A178" s="27"/>
+      <c r="C177" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="D177" s="11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="178" ht="47.25" spans="1:4">
+      <c r="A178" s="27" t="s">
+        <v>244</v>
+      </c>
       <c r="B178" s="18">
         <v>5</v>
       </c>
-      <c r="C178" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="D178" s="12" t="s">
-        <v>242</v>
+      <c r="C178" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="D178" s="31" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="179" ht="42" customHeight="1" spans="1:4">
@@ -4322,96 +4366,108 @@
         <v>5</v>
       </c>
       <c r="C179" s="12" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D179" s="12" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="180" ht="82" customHeight="1" spans="1:4">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="180" ht="42" customHeight="1" spans="1:4">
       <c r="A180" s="27"/>
       <c r="B180" s="18">
         <v>5</v>
       </c>
       <c r="C180" s="12" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="D180" s="12" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="181" ht="60.75" spans="1:4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="181" ht="82" customHeight="1" spans="1:4">
       <c r="A181" s="27"/>
-      <c r="B181" s="24">
+      <c r="B181" s="18">
         <v>5</v>
       </c>
       <c r="C181" s="12" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="D181" s="12" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="182" ht="31.5" spans="1:4">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="182" ht="60.75" spans="1:4">
       <c r="A182" s="27"/>
-      <c r="B182" s="18">
+      <c r="B182" s="24">
         <v>5</v>
       </c>
       <c r="C182" s="12" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D182" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="183" ht="220" customHeight="1" spans="1:4">
-      <c r="A183" s="27" t="s">
-        <v>251</v>
-      </c>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="183" ht="31.5" spans="1:4">
+      <c r="A183" s="27"/>
       <c r="B183" s="18">
         <v>5</v>
       </c>
       <c r="C183" s="12" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D183" s="12" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="184" ht="31.5" spans="1:4">
-      <c r="A184" s="27"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="184" ht="220" customHeight="1" spans="1:4">
+      <c r="A184" s="27" t="s">
+        <v>257</v>
+      </c>
       <c r="B184" s="18">
         <v>5</v>
       </c>
       <c r="C184" s="12" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="D184" s="12" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="185" ht="141.75" spans="1:4">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="185" ht="31.5" spans="1:4">
       <c r="A185" s="27"/>
       <c r="B185" s="18">
         <v>5</v>
       </c>
-      <c r="C185" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="D185" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="186" ht="47.25" spans="1:4">
+      <c r="C185" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="D185" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="186" ht="141.75" spans="1:4">
       <c r="A186" s="27"/>
       <c r="B186" s="18">
         <v>5</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>259</v>
+        <v>263</v>
+      </c>
+    </row>
+    <row r="187" ht="47.25" spans="1:4">
+      <c r="A187" s="27"/>
+      <c r="B187" s="18">
+        <v>5</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D187" s="2" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -4419,17 +4475,17 @@
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A16"/>
-    <mergeCell ref="A17:A54"/>
-    <mergeCell ref="A55:A68"/>
-    <mergeCell ref="A69:A129"/>
-    <mergeCell ref="A130:A144"/>
-    <mergeCell ref="A145:A162"/>
-    <mergeCell ref="A163:A170"/>
-    <mergeCell ref="A171:A176"/>
-    <mergeCell ref="A177:A182"/>
-    <mergeCell ref="A183:A186"/>
+    <mergeCell ref="A17:A55"/>
+    <mergeCell ref="A56:A69"/>
+    <mergeCell ref="A70:A130"/>
+    <mergeCell ref="A131:A145"/>
+    <mergeCell ref="A146:A163"/>
+    <mergeCell ref="A164:A171"/>
+    <mergeCell ref="A172:A177"/>
+    <mergeCell ref="A178:A183"/>
+    <mergeCell ref="A184:A187"/>
   </mergeCells>
-  <conditionalFormatting sqref="B130">
+  <conditionalFormatting sqref="B131">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4440,7 +4496,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B53 B55:B67 B69:B129 B131:B1048576">
+  <conditionalFormatting sqref="B1:B54 B56:B68 B70:B130 B132:B1048576">
     <cfRule type="cellIs" dxfId="0" priority="4" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -4452,7 +4508,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C89" r:id="rId2" display="Panoptic Segmentation" tooltip="https://arxiv.org/abs/1801.00868"/>
+    <hyperlink ref="C90" r:id="rId2" display="Panoptic Segmentation" tooltip="https://arxiv.org/abs/1801.00868"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
add paper psudo lidar
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="13140" tabRatio="354"/>
+    <workbookView windowWidth="14670" windowHeight="6345" tabRatio="354"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$225</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$235</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="341">
   <si>
     <t>Scope</t>
   </si>
@@ -568,6 +568,38 @@
     <t>(2019 NeurISP) object as distribution</t>
   </si>
   <si>
+    <t>Line as object: datasets and framework for semantic line segment detection</t>
+  </si>
+  <si>
+    <t>3d 
+object detection</t>
+  </si>
+  <si>
+    <t>Realtime 3D object Detection for Automated Driving Using Stereo Vision and Semantic Information</t>
+  </si>
+  <si>
+    <t>语义的作用之一：levarage the class specific shape prior
+流程：语义分割/目标检测/深度估计 -&gt; object pixels聚类到一起 -&gt; 映射到grid map上fit bbox
+fit bbox的流程：open操作去除outlier -&gt; convex_hull -&gt; 让到先验box 里面的点最多；
+bbox的confidence用object所有点的confidence和真实的distance来出；
+这个方法多所有的障碍物类别都有用；</t>
+  </si>
+  <si>
+    <t>stereo R-CNN based 3D object Detection for autonomous Driving</t>
+  </si>
+  <si>
+    <t>SOAT of image based methord; 开源：https://github.com/HKUST-Aerial-Robotics/Stereo-RCNN
+takes the advantages of dense object constraints in raw stereo images， formulating the 3D object localization as a lerning-aided geometry problem
+各部分作用：
+1）stereo RPN: 对左右两幅图都产生proposal， anchor能够包住左右两个框， 对左右两个框的w, u, deta_w, deta_u都产生回归值；
+2）stereo regression: 回归3d框的物体类别， 左图/右图的分别的boxes(和RPN一样，v, h公用，其它四个单独回归)， bbox的尺寸， 和viewpoint angle;
+3) keypoint Prediction: 回归3d-box的底部四个point投影到左图的位置；
+4) 3D Box Estimation: 用2） 3）两步的值回归3d-box，目的是使得3d框投影到2d图片上能够和2d-bbox及keypoint贴合（corse-bbox）
+5) Dense 3d-bbox alignment: 4) 中得到的z还是不准确，因此可以用这个z作为初始值，找一个能使得左图/右图的车的下半部分photomtric  error最小的z*（因为下半部分和框贴得比较紧密，可以按照框的尺寸+z近似给出disparity）,  然后，固定z*, 再用4中的方法把3d-bbox的其它点再算一遍（rectif again）， 得到fine-bbox;
+提升：Dense 3d-bbox alignment最大（用image的信息来确认z, 而不是先算z再算box）， keypoint~=3d_bbox_rctify
+trick: uncertainty_weighting提升比较大， 还用了left/right flip</t>
+  </si>
+  <si>
     <t>image semantic segmentation</t>
   </si>
   <si>
@@ -1587,8 +1619,8 @@
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1640,14 +1672,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -1656,7 +1680,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1670,8 +1694,100 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1685,75 +1801,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -1761,24 +1808,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1836,19 +1868,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1860,61 +2006,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1932,85 +2036,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2072,30 +2104,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -2128,20 +2136,20 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2160,157 +2168,181 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2371,12 +2403,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2386,14 +2427,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2521,7 +2562,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="4C4C4C"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -2774,15 +2815,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G225"/>
+  <dimension ref="A1:G235"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A190" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D195" sqref="D195"/>
+      <selection pane="bottomLeft" activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="12.75" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="15.75" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="13.4266666666667" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
@@ -2806,7 +2847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="40.5" spans="1:4">
+    <row r="2" ht="56.25" spans="1:4">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -2818,7 +2859,7 @@
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" ht="13.5" spans="1:4">
+    <row r="3" ht="18.75" spans="1:4">
       <c r="A3" s="9"/>
       <c r="B3" s="10">
         <v>5</v>
@@ -2828,7 +2869,7 @@
       </c>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" ht="13.5" spans="1:4">
+    <row r="4" ht="18.75" spans="1:4">
       <c r="A4" s="9"/>
       <c r="B4" s="10">
         <v>5</v>
@@ -2838,7 +2879,7 @@
       </c>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" ht="13.5" spans="1:4">
+    <row r="5" ht="18.75" spans="1:4">
       <c r="A5" s="9"/>
       <c r="B5" s="10">
         <v>5</v>
@@ -2850,7 +2891,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="13.5" spans="1:4">
+    <row r="6" ht="18.75" spans="1:4">
       <c r="A6" s="9"/>
       <c r="B6" s="10"/>
       <c r="C6" s="12" t="s">
@@ -2858,7 +2899,7 @@
       </c>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" ht="25.5" spans="1:4">
+    <row r="7" ht="31.5" spans="1:4">
       <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
@@ -2870,7 +2911,7 @@
       </c>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" ht="25.5" spans="1:4">
+    <row r="8" ht="31.5" spans="1:4">
       <c r="A8" s="9"/>
       <c r="B8" s="10"/>
       <c r="C8" s="12" t="s">
@@ -2878,7 +2919,7 @@
       </c>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" ht="64.5" spans="1:4">
+    <row r="9" ht="81.75" spans="1:4">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -2892,7 +2933,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" ht="13.5" spans="1:4">
+    <row r="10" ht="18.75" spans="1:4">
       <c r="A10" s="9"/>
       <c r="B10" s="13">
         <v>5</v>
@@ -2914,7 +2955,7 @@
       </c>
       <c r="D11" s="11"/>
     </row>
-    <row r="12" ht="25.5" spans="1:4">
+    <row r="12" ht="31.5" spans="1:4">
       <c r="A12" s="9"/>
       <c r="B12" s="10">
         <v>5</v>
@@ -2926,7 +2967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" ht="67.5" spans="1:4">
+    <row r="13" ht="93.75" spans="1:4">
       <c r="A13" s="9"/>
       <c r="B13" s="10">
         <v>5</v>
@@ -2938,7 +2979,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" ht="93" spans="1:4">
+    <row r="14" ht="125.25" spans="1:4">
       <c r="A14" s="9" t="s">
         <v>24</v>
       </c>
@@ -2952,7 +2993,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" ht="27" spans="1:4">
+    <row r="15" ht="37.5" spans="1:4">
       <c r="A15" s="9"/>
       <c r="B15" s="14">
         <v>5</v>
@@ -2991,7 +3032,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" ht="26.25" spans="1:4">
+    <row r="18" ht="34.5" spans="1:4">
       <c r="A18" s="9"/>
       <c r="B18" s="14">
         <v>5</v>
@@ -3003,7 +3044,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" ht="78.75" spans="1:4">
+    <row r="19" ht="103.5" spans="1:4">
       <c r="A19" s="9"/>
       <c r="B19" s="14">
         <v>5</v>
@@ -3015,7 +3056,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" ht="38.25" spans="1:4">
+    <row r="20" ht="47.25" spans="1:4">
       <c r="A20" s="9"/>
       <c r="B20" s="14">
         <v>5</v>
@@ -3027,7 +3068,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" ht="38.25" spans="1:4">
+    <row r="21" ht="47.25" spans="1:4">
       <c r="A21" s="9"/>
       <c r="B21" s="16">
         <v>1</v>
@@ -3037,7 +3078,7 @@
       </c>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" ht="38.25" spans="1:4">
+    <row r="22" ht="47.25" spans="1:4">
       <c r="A22" s="9"/>
       <c r="B22" s="14">
         <v>5</v>
@@ -3047,7 +3088,7 @@
       </c>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" ht="25.5" spans="1:4">
+    <row r="23" ht="31.5" spans="1:4">
       <c r="A23" s="9"/>
       <c r="B23" s="14">
         <v>5</v>
@@ -3057,7 +3098,7 @@
       </c>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" ht="66.75" spans="1:4">
+    <row r="24" ht="90.75" spans="1:4">
       <c r="A24" s="9"/>
       <c r="B24" s="14">
         <v>5</v>
@@ -3069,7 +3110,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" ht="27" spans="1:4">
+    <row r="25" ht="37.5" spans="1:4">
       <c r="A25" s="9"/>
       <c r="B25" s="14">
         <v>5</v>
@@ -3081,7 +3122,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" ht="26.25" spans="1:5">
+    <row r="26" ht="34.5" spans="1:5">
       <c r="A26" s="9"/>
       <c r="B26" s="14">
         <v>5</v>
@@ -3096,7 +3137,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" ht="39.75" spans="1:4">
+    <row r="27" ht="53.25" spans="1:4">
       <c r="A27" s="9"/>
       <c r="B27" s="14">
         <v>5</v>
@@ -3108,7 +3149,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" ht="66" spans="1:4">
+    <row r="28" ht="87.75" spans="1:4">
       <c r="A28" s="9"/>
       <c r="B28" s="14">
         <v>5</v>
@@ -3120,7 +3161,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" ht="25.5" spans="1:4">
+    <row r="29" ht="31.5" spans="1:4">
       <c r="A29" s="9"/>
       <c r="B29" s="14">
         <v>5</v>
@@ -3132,7 +3173,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" ht="25.5" spans="1:4">
+    <row r="30" ht="31.5" spans="1:4">
       <c r="A30" s="9"/>
       <c r="B30" s="14">
         <v>5</v>
@@ -3490,8 +3531,8 @@
       <c r="A63" s="18"/>
       <c r="B63" s="14"/>
     </row>
-    <row r="64" ht="25.5" spans="1:7">
-      <c r="A64" s="9" t="s">
+    <row r="64" ht="31.5" spans="1:7">
+      <c r="A64" s="20" t="s">
         <v>103</v>
       </c>
       <c r="B64" s="14">
@@ -3501,11 +3542,11 @@
         <v>104</v>
       </c>
       <c r="D64" s="11"/>
-      <c r="F64" s="20"/>
-      <c r="G64" s="20"/>
-    </row>
-    <row r="65" ht="64.5" spans="1:6">
-      <c r="A65" s="9"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="21"/>
+    </row>
+    <row r="65" ht="81.75" spans="1:6">
+      <c r="A65" s="20"/>
       <c r="B65" s="14">
         <v>5</v>
       </c>
@@ -3517,8 +3558,8 @@
       </c>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" ht="40.5" spans="1:4">
-      <c r="A66" s="9"/>
+    <row r="66" ht="56.25" spans="1:4">
+      <c r="A66" s="20"/>
       <c r="B66" s="10">
         <v>5</v>
       </c>
@@ -3529,8 +3570,8 @@
         <v>108</v>
       </c>
     </row>
-    <row r="67" ht="66.75" spans="1:4">
-      <c r="A67" s="9"/>
+    <row r="67" ht="90.75" spans="1:4">
+      <c r="A67" s="20"/>
       <c r="B67" s="10">
         <v>5</v>
       </c>
@@ -3541,9 +3582,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="68" ht="25.5" spans="1:4">
-      <c r="A68" s="9"/>
-      <c r="B68" s="21">
+    <row r="68" ht="31.5" spans="1:4">
+      <c r="A68" s="20"/>
+      <c r="B68" s="22">
         <v>5</v>
       </c>
       <c r="C68" s="2" t="s">
@@ -3553,8 +3594,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="69" ht="27" spans="1:4">
-      <c r="A69" s="9"/>
+    <row r="69" ht="37.5" spans="1:4">
+      <c r="A69" s="20"/>
       <c r="B69" s="10">
         <v>5</v>
       </c>
@@ -3565,8 +3606,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="70" ht="25.5" spans="1:4">
-      <c r="A70" s="9"/>
+    <row r="70" ht="31.5" spans="1:4">
+      <c r="A70" s="20"/>
       <c r="B70" s="10">
         <v>2</v>
       </c>
@@ -3575,8 +3616,8 @@
       </c>
       <c r="D70" s="11"/>
     </row>
-    <row r="71" ht="78" spans="1:4">
-      <c r="A71" s="9"/>
+    <row r="71" ht="100.5" spans="1:4">
+      <c r="A71" s="20"/>
       <c r="B71" s="10">
         <v>5</v>
       </c>
@@ -3587,8 +3628,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="72" ht="40.5" spans="1:4">
-      <c r="A72" s="9"/>
+    <row r="72" ht="56.25" spans="1:4">
+      <c r="A72" s="20"/>
       <c r="B72" s="10">
         <v>5</v>
       </c>
@@ -3599,8 +3640,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="73" ht="38.25" spans="1:4">
-      <c r="A73" s="9"/>
+    <row r="73" ht="47.25" spans="1:4">
+      <c r="A73" s="20"/>
       <c r="B73" s="10">
         <v>1</v>
       </c>
@@ -3609,8 +3650,8 @@
       </c>
       <c r="D73" s="11"/>
     </row>
-    <row r="74" ht="25.5" spans="1:4">
-      <c r="A74" s="9"/>
+    <row r="74" ht="31.5" spans="1:4">
+      <c r="A74" s="20"/>
       <c r="B74" s="10">
         <v>1</v>
       </c>
@@ -3620,7 +3661,7 @@
       <c r="D74" s="11"/>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="9"/>
+      <c r="A75" s="20"/>
       <c r="B75" s="10">
         <v>1</v>
       </c>
@@ -3629,1625 +3670,1704 @@
       </c>
       <c r="D75" s="11"/>
     </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="9"/>
-      <c r="B76" s="10"/>
-      <c r="C76" s="12"/>
+    <row r="76" ht="31.5" spans="1:4">
+      <c r="A76" s="20"/>
+      <c r="B76" s="10">
+        <v>1</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>123</v>
+      </c>
       <c r="D76" s="11"/>
     </row>
-    <row r="77" spans="1:1">
-      <c r="A77" s="9"/>
-    </row>
-    <row r="78" ht="51.75" spans="1:4">
-      <c r="A78" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="B78" s="10">
-        <v>5</v>
-      </c>
-      <c r="C78" s="11" t="s">
+    <row r="77" spans="1:4">
+      <c r="A77" s="20"/>
+      <c r="B77" s="23"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="20"/>
+      <c r="B78" s="23"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="20"/>
+      <c r="B79" s="23"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="20"/>
+      <c r="B80" s="23"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="20"/>
+      <c r="B81" s="23"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+    </row>
+    <row r="82" ht="93.75" spans="1:4">
+      <c r="A82" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="D78" s="11"/>
-    </row>
-    <row r="79" ht="52.5" spans="1:4">
-      <c r="A79" s="22"/>
-      <c r="B79" s="10">
+      <c r="B82" s="23">
+        <v>5</v>
+      </c>
+      <c r="C82" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D82" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="83" ht="375.75" spans="1:4">
+      <c r="A83" s="24"/>
+      <c r="B83" s="23">
+        <v>5</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D83" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="24"/>
+      <c r="B84" s="23"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="24"/>
+      <c r="B85" s="23"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="24"/>
+      <c r="B86" s="23"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="24"/>
+    </row>
+    <row r="88" ht="66" spans="1:4">
+      <c r="A88" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B88" s="10">
+        <v>5</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D88" s="11"/>
+    </row>
+    <row r="89" ht="69" spans="1:4">
+      <c r="A89" s="25"/>
+      <c r="B89" s="10">
         <v>6</v>
       </c>
-      <c r="C79" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="80" ht="25.5" spans="1:4">
-      <c r="A80" s="22"/>
-      <c r="B80" s="21">
-        <v>5</v>
-      </c>
-      <c r="C80" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="D80" s="11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="81" ht="38.25" spans="1:4">
-      <c r="A81" s="22"/>
-      <c r="B81" s="21">
-        <v>5</v>
-      </c>
-      <c r="C81" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="D81" s="11" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="82" ht="92.25" spans="1:4">
-      <c r="A82" s="22"/>
-      <c r="B82" s="21">
-        <v>5</v>
-      </c>
-      <c r="C82" s="11" t="s">
+      <c r="C89" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="D82" s="11" t="s">
+      <c r="D89" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="83" ht="92.25" spans="1:4">
-      <c r="A83" s="22"/>
-      <c r="B83" s="21">
-        <v>5</v>
-      </c>
-      <c r="C83" s="11" t="s">
+    <row r="90" ht="31.5" spans="1:4">
+      <c r="A90" s="25"/>
+      <c r="B90" s="22">
+        <v>5</v>
+      </c>
+      <c r="C90" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="D83" s="11" t="s">
+      <c r="D90" s="11" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="84" ht="147.75" spans="1:4">
-      <c r="A84" s="22"/>
-      <c r="B84" s="21">
-        <v>5</v>
-      </c>
-      <c r="C84" s="11" t="s">
+    <row r="91" ht="47.25" spans="1:4">
+      <c r="A91" s="25"/>
+      <c r="B91" s="22">
+        <v>5</v>
+      </c>
+      <c r="C91" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="D84" s="8" t="s">
+      <c r="D91" s="11" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="85" ht="53.25" spans="1:4">
-      <c r="A85" s="22"/>
-      <c r="B85" s="21">
-        <v>5</v>
-      </c>
-      <c r="C85" s="11" t="s">
+    <row r="92" ht="122.25" spans="1:4">
+      <c r="A92" s="25"/>
+      <c r="B92" s="22">
+        <v>5</v>
+      </c>
+      <c r="C92" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="D85" s="11" t="s">
+      <c r="D92" s="11" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="86" ht="106.5" spans="1:4">
-      <c r="A86" s="22"/>
-      <c r="B86" s="21">
-        <v>5</v>
-      </c>
-      <c r="C86" s="11" t="s">
+    <row r="93" ht="122.25" spans="1:4">
+      <c r="A93" s="25"/>
+      <c r="B93" s="22">
+        <v>5</v>
+      </c>
+      <c r="C93" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D86" s="11" t="s">
+      <c r="D93" s="11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="87" ht="25.5" spans="1:4">
-      <c r="A87" s="22"/>
-      <c r="B87" s="21">
-        <v>5</v>
-      </c>
-      <c r="C87" s="11" t="s">
+    <row r="94" ht="203.25" spans="1:4">
+      <c r="A94" s="25"/>
+      <c r="B94" s="22">
+        <v>5</v>
+      </c>
+      <c r="C94" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="D87" s="11"/>
-    </row>
-    <row r="88" ht="52.5" spans="1:4">
-      <c r="A88" s="22"/>
-      <c r="B88" s="21">
-        <v>5</v>
-      </c>
-      <c r="C88" s="11" t="s">
+      <c r="D94" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="D88" s="11"/>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="22"/>
-      <c r="B89" s="21">
+    </row>
+    <row r="95" ht="72" spans="1:4">
+      <c r="A95" s="25"/>
+      <c r="B95" s="22">
+        <v>5</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="96" ht="144" spans="1:4">
+      <c r="A96" s="25"/>
+      <c r="B96" s="22">
+        <v>5</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="97" ht="31.5" spans="1:4">
+      <c r="A97" s="25"/>
+      <c r="B97" s="22">
+        <v>5</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="D97" s="11"/>
+    </row>
+    <row r="98" ht="69" spans="1:4">
+      <c r="A98" s="25"/>
+      <c r="B98" s="22">
+        <v>5</v>
+      </c>
+      <c r="C98" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D98" s="11"/>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="25"/>
+      <c r="B99" s="22">
         <v>2</v>
       </c>
-      <c r="C89" t="s">
-        <v>143</v>
-      </c>
-      <c r="D89" s="11"/>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="22"/>
-      <c r="B90" s="21">
-        <v>5</v>
-      </c>
-      <c r="C90" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="D90" s="11"/>
-    </row>
-    <row r="91" ht="38.25" spans="1:4">
-      <c r="A91" s="22"/>
-      <c r="B91" s="21">
+      <c r="C99" t="s">
+        <v>149</v>
+      </c>
+      <c r="D99" s="11"/>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="25"/>
+      <c r="B100" s="22">
+        <v>5</v>
+      </c>
+      <c r="C100" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D100" s="11"/>
+    </row>
+    <row r="101" ht="47.25" spans="1:4">
+      <c r="A101" s="25"/>
+      <c r="B101" s="22">
         <v>2</v>
       </c>
-      <c r="C91" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="D91" s="11"/>
-    </row>
-    <row r="92" ht="38.25" spans="1:4">
-      <c r="A92" s="22"/>
-      <c r="B92" s="21">
-        <v>5</v>
-      </c>
-      <c r="C92" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="D92" s="11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="93" ht="51" spans="1:4">
-      <c r="A93" s="22"/>
-      <c r="B93" s="21">
-        <v>5</v>
-      </c>
-      <c r="C93" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="D93" s="11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="94" ht="144" spans="1:5">
-      <c r="A94" s="22"/>
-      <c r="B94" s="21">
-        <v>5</v>
-      </c>
-      <c r="C94" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="D94" s="8" t="s">
+      <c r="C101" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="E94" s="27" t="s">
+      <c r="D101" s="11"/>
+    </row>
+    <row r="102" ht="47.25" spans="1:4">
+      <c r="A102" s="25"/>
+      <c r="B102" s="22">
+        <v>5</v>
+      </c>
+      <c r="C102" s="12" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="95" ht="155" customHeight="1" spans="1:5">
-      <c r="A95" s="22"/>
-      <c r="B95" s="21">
-        <v>5</v>
-      </c>
-      <c r="C95" s="12" t="s">
+      <c r="D102" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="D95" s="11" t="s">
+    </row>
+    <row r="103" ht="63" spans="1:4">
+      <c r="A103" s="25"/>
+      <c r="B103" s="22">
+        <v>5</v>
+      </c>
+      <c r="C103" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="E95" s="2" t="s">
+      <c r="D103" s="11" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="96" ht="40.5" spans="1:4">
-      <c r="A96" s="22"/>
-      <c r="B96" s="21">
-        <v>5</v>
-      </c>
-      <c r="C96" s="12" t="s">
+    <row r="104" ht="188.25" spans="1:5">
+      <c r="A104" s="25"/>
+      <c r="B104" s="22">
+        <v>5</v>
+      </c>
+      <c r="C104" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="D96" s="11" t="s">
+      <c r="D104" s="8" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="97" ht="40.5" spans="1:4">
-      <c r="A97" s="22"/>
-      <c r="B97" s="21">
-        <v>5</v>
-      </c>
-      <c r="C97" s="12" t="s">
+      <c r="E104" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="D97" s="11" t="s">
+    </row>
+    <row r="105" ht="155" customHeight="1" spans="1:5">
+      <c r="A105" s="25"/>
+      <c r="B105" s="22">
+        <v>5</v>
+      </c>
+      <c r="C105" s="12" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="98" ht="120.75" spans="1:4">
-      <c r="A98" s="22"/>
-      <c r="B98" s="21">
-        <v>5</v>
-      </c>
-      <c r="C98" s="2" t="s">
+      <c r="D105" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="D98" s="11" t="s">
+      <c r="E105" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="99" ht="54" spans="1:4">
-      <c r="A99" s="22"/>
-      <c r="B99" s="21">
-        <v>5</v>
-      </c>
-      <c r="C99" s="2" t="s">
+    <row r="106" ht="56.25" spans="1:4">
+      <c r="A106" s="25"/>
+      <c r="B106" s="22">
+        <v>5</v>
+      </c>
+      <c r="C106" s="12" t="s">
         <v>162</v>
       </c>
-      <c r="D99" s="11" t="s">
+      <c r="D106" s="11" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="100" ht="40.5" spans="1:4">
-      <c r="A100" s="22"/>
-      <c r="B100" s="21">
-        <v>5</v>
-      </c>
-      <c r="C100" s="2" t="s">
+    <row r="107" ht="56.25" spans="1:4">
+      <c r="A107" s="25"/>
+      <c r="B107" s="22">
+        <v>5</v>
+      </c>
+      <c r="C107" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="D100" s="11" t="s">
+      <c r="D107" s="11" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="101" ht="27" spans="1:4">
-      <c r="A101" s="22"/>
-      <c r="B101" s="21">
-        <v>5</v>
-      </c>
-      <c r="C101" s="2" t="s">
+    <row r="108" ht="165.75" spans="1:4">
+      <c r="A108" s="25"/>
+      <c r="B108" s="22">
+        <v>5</v>
+      </c>
+      <c r="C108" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D101" s="11" t="s">
+      <c r="D108" s="11" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="102" ht="25.5" spans="1:4">
-      <c r="A102" s="22"/>
-      <c r="B102" s="21">
+    <row r="109" ht="75" spans="1:4">
+      <c r="A109" s="25"/>
+      <c r="B109" s="22">
+        <v>5</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D109" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="110" ht="56.25" spans="1:4">
+      <c r="A110" s="25"/>
+      <c r="B110" s="22">
+        <v>5</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D110" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="111" ht="37.5" spans="1:4">
+      <c r="A111" s="25"/>
+      <c r="B111" s="22">
+        <v>5</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D111" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="112" ht="31.5" spans="1:4">
+      <c r="A112" s="25"/>
+      <c r="B112" s="22">
         <v>2</v>
       </c>
-      <c r="C102" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D102" s="11"/>
-    </row>
-    <row r="103" ht="51" spans="1:4">
-      <c r="A103" s="22"/>
-      <c r="B103" s="21">
+      <c r="C112" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D112" s="11"/>
+    </row>
+    <row r="113" ht="63" spans="1:4">
+      <c r="A113" s="25"/>
+      <c r="B113" s="22">
         <v>2</v>
       </c>
-      <c r="C103" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D103" s="11"/>
-    </row>
-    <row r="104" ht="38.25" spans="1:4">
-      <c r="A104" s="22"/>
-      <c r="B104" s="21">
+      <c r="C113" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D113" s="11"/>
+    </row>
+    <row r="114" ht="47.25" spans="1:4">
+      <c r="A114" s="25"/>
+      <c r="B114" s="22">
         <v>2</v>
       </c>
-      <c r="C104" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D104" s="11"/>
-    </row>
-    <row r="105" ht="39" spans="1:4">
-      <c r="A105" s="22"/>
-      <c r="B105" s="21">
+      <c r="C114" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D114" s="11"/>
+    </row>
+    <row r="115" ht="50.25" spans="1:4">
+      <c r="A115" s="25"/>
+      <c r="B115" s="22">
         <v>2</v>
       </c>
-      <c r="C105" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="D105" s="11"/>
-    </row>
-    <row r="106" ht="25.5" spans="1:4">
-      <c r="A106" s="22"/>
-      <c r="B106" s="21">
+      <c r="C115" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="D115" s="11"/>
+    </row>
+    <row r="116" ht="31.5" spans="1:4">
+      <c r="A116" s="25"/>
+      <c r="B116" s="22">
         <v>2</v>
       </c>
-      <c r="C106" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="D106" s="11"/>
-    </row>
-    <row r="107" ht="66.75" spans="1:4">
-      <c r="A107" s="22"/>
-      <c r="B107" s="21">
-        <v>5</v>
-      </c>
-      <c r="C107" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="D107" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="108" ht="26.25" spans="1:4">
-      <c r="A108" s="22"/>
-      <c r="B108" s="21">
+      <c r="C116" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="D116" s="11"/>
+    </row>
+    <row r="117" ht="90.75" spans="1:4">
+      <c r="A117" s="25"/>
+      <c r="B117" s="22">
+        <v>5</v>
+      </c>
+      <c r="C117" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D117" s="11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="118" ht="34.5" spans="1:4">
+      <c r="A118" s="25"/>
+      <c r="B118" s="22">
         <v>2</v>
       </c>
-      <c r="C108" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="D108" s="11"/>
-    </row>
-    <row r="109" ht="66.75" spans="1:4">
-      <c r="A109" s="22"/>
-      <c r="B109" s="21">
-        <v>5</v>
-      </c>
-      <c r="C109" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="D109" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="110" ht="38.25" spans="1:4">
-      <c r="A110" s="22"/>
-      <c r="B110" s="21">
+      <c r="C118" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="D118" s="11"/>
+    </row>
+    <row r="119" ht="90.75" spans="1:4">
+      <c r="A119" s="25"/>
+      <c r="B119" s="22">
+        <v>5</v>
+      </c>
+      <c r="C119" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="D119" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="120" ht="47.25" spans="1:4">
+      <c r="A120" s="25"/>
+      <c r="B120" s="22">
         <v>2</v>
       </c>
-      <c r="C110" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="D110" s="23"/>
-    </row>
-    <row r="111" ht="78.75" spans="1:4">
-      <c r="A111" s="22"/>
-      <c r="B111" s="21">
-        <v>5</v>
-      </c>
-      <c r="C111" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="D111" s="23" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="112" ht="39.75" spans="1:4">
-      <c r="A112" s="22"/>
-      <c r="B112" s="21">
-        <v>5</v>
-      </c>
-      <c r="C112" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="D112" s="23"/>
-    </row>
-    <row r="113" ht="52.5" spans="1:4">
-      <c r="A113" s="22"/>
-      <c r="B113" s="21">
+      <c r="C120" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="D120" s="26"/>
+    </row>
+    <row r="121" ht="103.5" spans="1:4">
+      <c r="A121" s="25"/>
+      <c r="B121" s="22">
+        <v>5</v>
+      </c>
+      <c r="C121" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="D121" s="26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="122" ht="53.25" spans="1:4">
+      <c r="A122" s="25"/>
+      <c r="B122" s="22">
+        <v>5</v>
+      </c>
+      <c r="C122" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="D122" s="26"/>
+    </row>
+    <row r="123" ht="69" spans="1:4">
+      <c r="A123" s="25"/>
+      <c r="B123" s="22">
         <v>2</v>
       </c>
-      <c r="C113" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="D113" s="23"/>
-    </row>
-    <row r="114" ht="25.5" spans="1:4">
-      <c r="A114" s="22"/>
-      <c r="B114" s="21">
+      <c r="C123" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="D123" s="26"/>
+    </row>
+    <row r="124" ht="31.5" spans="1:4">
+      <c r="A124" s="25"/>
+      <c r="B124" s="22">
         <v>2</v>
       </c>
-      <c r="C114" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="D114" s="23"/>
-    </row>
-    <row r="115" ht="38.25" spans="1:4">
-      <c r="A115" s="22"/>
-      <c r="B115" s="21">
-        <v>5</v>
-      </c>
-      <c r="C115" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="D115" s="23"/>
-    </row>
-    <row r="116" ht="92.25" spans="1:4">
-      <c r="A116" s="22"/>
-      <c r="B116" s="21">
-        <v>5</v>
-      </c>
-      <c r="C116" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="D116" s="23" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="117" ht="27" spans="1:4">
-      <c r="A117" s="22"/>
-      <c r="B117" s="21">
-        <v>5</v>
-      </c>
-      <c r="C117" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="D117" s="23" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="118" ht="38.25" spans="1:4">
-      <c r="A118" s="22"/>
-      <c r="B118" s="21">
-        <v>5</v>
-      </c>
-      <c r="C118" s="12" t="s">
+      <c r="C124" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="D118" s="11" t="s">
+      <c r="D124" s="26"/>
+    </row>
+    <row r="125" ht="47.25" spans="1:4">
+      <c r="A125" s="25"/>
+      <c r="B125" s="22">
+        <v>5</v>
+      </c>
+      <c r="C125" s="27" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="119" ht="53.25" spans="1:4">
-      <c r="A119" s="22"/>
-      <c r="B119" s="21">
-        <v>5</v>
-      </c>
-      <c r="C119" s="25" t="s">
+      <c r="D125" s="26"/>
+    </row>
+    <row r="126" ht="122.25" spans="1:4">
+      <c r="A126" s="25"/>
+      <c r="B126" s="22">
+        <v>5</v>
+      </c>
+      <c r="C126" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="D119" s="11" t="s">
+      <c r="D126" s="26" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="120" ht="105.75" spans="1:4">
-      <c r="A120" s="22"/>
-      <c r="B120" s="21">
-        <v>5</v>
-      </c>
-      <c r="C120" s="11" t="s">
+    <row r="127" ht="37.5" spans="1:4">
+      <c r="A127" s="25"/>
+      <c r="B127" s="22">
+        <v>5</v>
+      </c>
+      <c r="C127" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="D120" s="11" t="s">
+      <c r="D127" s="26" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="121" ht="31" customHeight="1" spans="1:5">
-      <c r="A121" s="22"/>
-      <c r="B121" s="26">
+    <row r="128" ht="47.25" spans="1:4">
+      <c r="A128" s="25"/>
+      <c r="B128" s="22">
+        <v>5</v>
+      </c>
+      <c r="C128" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D128" s="11" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="129" ht="72" spans="1:4">
+      <c r="A129" s="25"/>
+      <c r="B129" s="22">
+        <v>5</v>
+      </c>
+      <c r="C129" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="D129" s="11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="130" ht="141" spans="1:4">
+      <c r="A130" s="25"/>
+      <c r="B130" s="22">
+        <v>5</v>
+      </c>
+      <c r="C130" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D130" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="131" ht="31" customHeight="1" spans="1:5">
+      <c r="A131" s="25"/>
+      <c r="B131" s="30">
         <v>1</v>
       </c>
-      <c r="C121" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="D121" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="122" ht="39" spans="1:4">
-      <c r="A122" s="22"/>
-      <c r="B122" s="26">
+      <c r="C131" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="D131" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="132" ht="50.25" spans="1:4">
+      <c r="A132" s="25"/>
+      <c r="B132" s="30">
         <v>2</v>
       </c>
-      <c r="C122" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="D122" s="12"/>
-    </row>
-    <row r="123" ht="40.5" spans="1:4">
-      <c r="A123" s="22"/>
-      <c r="B123" s="26">
-        <v>5</v>
-      </c>
-      <c r="C123" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D123" s="12" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="124" ht="54" spans="1:4">
-      <c r="A124" s="22"/>
-      <c r="B124" s="26">
-        <v>5</v>
-      </c>
-      <c r="C124" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="D124" s="12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="125" ht="51.75" spans="1:4">
-      <c r="A125" s="22"/>
-      <c r="B125" s="26">
+      <c r="C132" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="D132" s="12"/>
+    </row>
+    <row r="133" ht="56.25" spans="1:4">
+      <c r="A133" s="25"/>
+      <c r="B133" s="30">
+        <v>5</v>
+      </c>
+      <c r="C133" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D133" s="12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="134" ht="75" spans="1:4">
+      <c r="A134" s="25"/>
+      <c r="B134" s="30">
+        <v>5</v>
+      </c>
+      <c r="C134" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="D134" s="12" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="135" ht="66" spans="1:4">
+      <c r="A135" s="25"/>
+      <c r="B135" s="30">
         <v>1</v>
       </c>
-      <c r="C125" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="D125" s="12"/>
-    </row>
-    <row r="126" ht="25.5" spans="1:4">
-      <c r="A126" s="22"/>
-      <c r="B126" s="26">
+      <c r="C135" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D135" s="12"/>
+    </row>
+    <row r="136" ht="31.5" spans="1:4">
+      <c r="A136" s="25"/>
+      <c r="B136" s="30">
         <v>1</v>
       </c>
-      <c r="C126" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="D126" s="12" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="127" ht="38.25" spans="1:4">
-      <c r="A127" s="22"/>
-      <c r="B127" s="26">
+      <c r="C136" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D136" s="12" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="137" ht="47.25" spans="1:4">
+      <c r="A137" s="25"/>
+      <c r="B137" s="30">
         <v>1</v>
       </c>
-      <c r="C127" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="D127" s="12"/>
-    </row>
-    <row r="128" ht="51" spans="1:4">
-      <c r="A128" s="22"/>
-      <c r="B128" s="26">
+      <c r="C137" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="D137" s="12"/>
+    </row>
+    <row r="138" ht="63" spans="1:4">
+      <c r="A138" s="25"/>
+      <c r="B138" s="30">
         <v>1</v>
       </c>
-      <c r="C128" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="D128" s="12"/>
-    </row>
-    <row r="129" ht="51" spans="1:4">
-      <c r="A129" s="22"/>
-      <c r="B129" s="26">
+      <c r="C138" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="D138" s="12"/>
+    </row>
+    <row r="139" ht="63" spans="1:4">
+      <c r="A139" s="25"/>
+      <c r="B139" s="30">
         <v>1</v>
       </c>
-      <c r="C129" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="D129" s="12"/>
-    </row>
-    <row r="130" ht="25.5" spans="1:4">
-      <c r="A130" s="22"/>
-      <c r="B130" s="26">
+      <c r="C139" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="D139" s="12"/>
+    </row>
+    <row r="140" ht="31.5" spans="1:4">
+      <c r="A140" s="25"/>
+      <c r="B140" s="30">
         <v>1</v>
       </c>
-      <c r="C130" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="D130" s="12"/>
-    </row>
-    <row r="131" ht="144.75" spans="1:5">
-      <c r="A131" s="22"/>
-      <c r="B131" s="26">
-        <v>5</v>
-      </c>
-      <c r="C131" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="D131" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="E131" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="132" ht="38.25" spans="1:4">
-      <c r="A132" s="22"/>
-      <c r="B132" s="26">
+      <c r="C140" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="D140" s="12"/>
+    </row>
+    <row r="141" ht="191.25" spans="1:5">
+      <c r="A141" s="25"/>
+      <c r="B141" s="30">
+        <v>5</v>
+      </c>
+      <c r="C141" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="D141" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="E141" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="142" ht="47.25" spans="1:4">
+      <c r="A142" s="25"/>
+      <c r="B142" s="30">
         <v>1</v>
       </c>
-      <c r="C132" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="D132" s="12"/>
-    </row>
-    <row r="133" ht="38.25" spans="1:4">
-      <c r="A133" s="22"/>
-      <c r="B133" s="26">
+      <c r="C142" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="D142" s="12"/>
+    </row>
+    <row r="143" ht="47.25" spans="1:4">
+      <c r="A143" s="25"/>
+      <c r="B143" s="30">
         <v>1</v>
       </c>
-      <c r="C133" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="D133" s="12"/>
-    </row>
-    <row r="134" ht="38.25" spans="1:5">
-      <c r="A134" s="22"/>
-      <c r="B134" s="17">
-        <v>5</v>
-      </c>
-      <c r="C134" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="D134" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="E134" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="135" ht="105.75" spans="1:5">
-      <c r="A135" s="22"/>
-      <c r="B135" s="26">
-        <v>5</v>
-      </c>
-      <c r="C135" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="D135" s="28" t="s">
-        <v>216</v>
-      </c>
-      <c r="E135" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="136" ht="25.5" spans="1:4">
-      <c r="A136" s="22"/>
-      <c r="B136" s="26">
+      <c r="C143" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="D143" s="12"/>
+    </row>
+    <row r="144" ht="47.25" spans="1:5">
+      <c r="A144" s="25"/>
+      <c r="B144" s="17">
+        <v>5</v>
+      </c>
+      <c r="C144" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="D144" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="E144" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="145" ht="141" spans="1:5">
+      <c r="A145" s="25"/>
+      <c r="B145" s="30">
+        <v>5</v>
+      </c>
+      <c r="C145" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D145" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="E145" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="146" ht="31.5" spans="1:4">
+      <c r="A146" s="25"/>
+      <c r="B146" s="30">
         <v>1</v>
       </c>
-      <c r="C136" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="D136" s="28"/>
-    </row>
-    <row r="137" ht="207" customHeight="1" spans="1:5">
-      <c r="A137" s="22"/>
-      <c r="B137" s="26">
-        <v>5</v>
-      </c>
-      <c r="C137" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="D137" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="E137" t="s">
+      <c r="C146" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="D146" s="31"/>
+    </row>
+    <row r="147" ht="207" customHeight="1" spans="1:5">
+      <c r="A147" s="25"/>
+      <c r="B147" s="30">
+        <v>5</v>
+      </c>
+      <c r="C147" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="D147" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="E147" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="138" ht="38.25" spans="1:5">
-      <c r="A138" s="22"/>
-      <c r="B138" s="26">
+    <row r="148" ht="47.25" spans="1:5">
+      <c r="A148" s="25"/>
+      <c r="B148" s="30">
         <v>2</v>
       </c>
-      <c r="C138" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="D138" s="28"/>
-      <c r="E138" t="s">
+      <c r="C148" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="D148" s="31"/>
+      <c r="E148" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="139" ht="119.25" spans="1:5">
-      <c r="A139" s="22"/>
-      <c r="B139" s="26">
-        <v>5</v>
-      </c>
-      <c r="C139" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="D139" s="28" t="s">
-        <v>222</v>
-      </c>
-      <c r="E139" t="s">
+    <row r="149" ht="159.75" spans="1:5">
+      <c r="A149" s="25"/>
+      <c r="B149" s="30">
+        <v>5</v>
+      </c>
+      <c r="C149" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D149" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="E149" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="140" ht="25.5" spans="1:5">
-      <c r="A140" s="22"/>
-      <c r="B140" s="26">
+    <row r="150" ht="31.5" spans="1:5">
+      <c r="A150" s="25"/>
+      <c r="B150" s="30">
         <v>1</v>
       </c>
-      <c r="C140" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="D140" s="28"/>
-      <c r="E140" t="s">
+      <c r="C150" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="D150" s="31"/>
+      <c r="E150" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="141" ht="66" spans="1:5">
-      <c r="A141" s="22"/>
-      <c r="B141" s="26">
-        <v>5</v>
-      </c>
-      <c r="C141" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="D141" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="E141" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="142" ht="81" customHeight="1" spans="1:4">
-      <c r="A142" s="22"/>
-      <c r="B142" s="26">
-        <v>5</v>
-      </c>
-      <c r="C142" s="29" t="s">
-        <v>226</v>
-      </c>
-      <c r="D142" s="28" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="143" ht="42" customHeight="1" spans="1:4">
-      <c r="A143" s="22"/>
-      <c r="B143" s="26"/>
-      <c r="C143" s="29" t="s">
-        <v>228</v>
-      </c>
-      <c r="D143" s="28" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="144" ht="25.5" spans="1:5">
-      <c r="A144" s="22"/>
-      <c r="B144" s="26"/>
-      <c r="C144" s="12" t="s">
+    <row r="151" ht="87.75" spans="1:5">
+      <c r="A151" s="25"/>
+      <c r="B151" s="30">
+        <v>5</v>
+      </c>
+      <c r="C151" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="D144" s="28"/>
-      <c r="E144" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="145" ht="38.25" spans="1:4">
-      <c r="A145" s="22"/>
-      <c r="B145" s="26"/>
-      <c r="C145" s="12" t="s">
+      <c r="D151" s="11" t="s">
         <v>231</v>
-      </c>
-      <c r="D145" s="28"/>
-    </row>
-    <row r="146" ht="38.25" spans="1:4">
-      <c r="A146" s="22"/>
-      <c r="B146" s="26"/>
-      <c r="C146" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="D146" s="28"/>
-    </row>
-    <row r="147" ht="38.25" spans="1:4">
-      <c r="A147" s="22"/>
-      <c r="B147" s="26"/>
-      <c r="C147" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="D147" s="28"/>
-    </row>
-    <row r="148" ht="38.25" spans="1:4">
-      <c r="A148" s="22"/>
-      <c r="B148" s="26"/>
-      <c r="C148" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="D148" s="28"/>
-    </row>
-    <row r="149" ht="54" spans="1:4">
-      <c r="A149" s="22"/>
-      <c r="B149" s="26">
-        <v>5</v>
-      </c>
-      <c r="C149" s="29" t="s">
-        <v>235</v>
-      </c>
-      <c r="D149" s="28" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="150" ht="38.25" spans="1:4">
-      <c r="A150" s="22"/>
-      <c r="B150" s="26"/>
-      <c r="C150" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="D150" s="28"/>
-    </row>
-    <row r="151" ht="27" spans="1:5">
-      <c r="A151" s="22"/>
-      <c r="B151" s="26">
-        <v>5</v>
-      </c>
-      <c r="C151" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="D151" s="28" t="s">
-        <v>239</v>
       </c>
       <c r="E151" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="152" ht="38.25" spans="1:4">
-      <c r="A152" s="22"/>
-      <c r="B152" s="26"/>
-      <c r="C152" s="12" t="s">
+    <row r="152" ht="81" customHeight="1" spans="1:4">
+      <c r="A152" s="25"/>
+      <c r="B152" s="30">
+        <v>5</v>
+      </c>
+      <c r="C152" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="D152" s="31" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="153" ht="42" customHeight="1" spans="1:4">
+      <c r="A153" s="25"/>
+      <c r="B153" s="30"/>
+      <c r="C153" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="D153" s="31" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="154" ht="31.5" spans="1:5">
+      <c r="A154" s="25"/>
+      <c r="B154" s="30"/>
+      <c r="C154" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="D154" s="31"/>
+      <c r="E154" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="155" ht="47.25" spans="1:4">
+      <c r="A155" s="25"/>
+      <c r="B155" s="30"/>
+      <c r="C155" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="D155" s="31"/>
+    </row>
+    <row r="156" ht="47.25" spans="1:4">
+      <c r="A156" s="25"/>
+      <c r="B156" s="30"/>
+      <c r="C156" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="D156" s="31"/>
+    </row>
+    <row r="157" ht="47.25" spans="1:4">
+      <c r="A157" s="25"/>
+      <c r="B157" s="30"/>
+      <c r="C157" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="D157" s="31"/>
+    </row>
+    <row r="158" ht="47.25" spans="1:4">
+      <c r="A158" s="25"/>
+      <c r="B158" s="30"/>
+      <c r="C158" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="D152" s="28"/>
-    </row>
-    <row r="153" ht="67.5" spans="1:4">
-      <c r="A153" s="22"/>
-      <c r="B153" s="26">
-        <v>5</v>
-      </c>
-      <c r="C153" s="12" t="s">
+      <c r="D158" s="31"/>
+    </row>
+    <row r="159" ht="75" spans="1:4">
+      <c r="A159" s="25"/>
+      <c r="B159" s="30">
+        <v>5</v>
+      </c>
+      <c r="C159" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="D153" s="28" t="s">
+      <c r="D159" s="31" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="154" ht="161.25" spans="1:4">
-      <c r="A154" s="22"/>
-      <c r="B154" s="26">
-        <v>5</v>
-      </c>
-      <c r="C154" s="12" t="s">
+    <row r="160" ht="47.25" spans="1:4">
+      <c r="A160" s="25"/>
+      <c r="B160" s="30"/>
+      <c r="C160" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="D154" s="28" t="s">
+      <c r="D160" s="31"/>
+    </row>
+    <row r="161" ht="37.5" spans="1:5">
+      <c r="A161" s="25"/>
+      <c r="B161" s="30">
+        <v>5</v>
+      </c>
+      <c r="C161" s="32" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="155" ht="121.5" spans="1:4">
-      <c r="A155" s="22"/>
-      <c r="B155" s="26">
-        <v>5</v>
-      </c>
-      <c r="C155" s="12" t="s">
+      <c r="D161" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="D155" s="28" t="s">
+      <c r="E161" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="162" ht="47.25" spans="1:4">
+      <c r="A162" s="25"/>
+      <c r="B162" s="30"/>
+      <c r="C162" s="12" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="156" spans="1:4">
-      <c r="A156" s="22"/>
-      <c r="B156" s="26"/>
-      <c r="C156" s="12"/>
-      <c r="D156" s="28"/>
-    </row>
-    <row r="157" spans="1:4">
-      <c r="A157" s="22"/>
-      <c r="B157" s="26"/>
-      <c r="C157" s="12"/>
-      <c r="D157" s="28"/>
-    </row>
-    <row r="158" ht="106.5" spans="1:4">
-      <c r="A158" s="30" t="s">
+      <c r="D162" s="31"/>
+    </row>
+    <row r="163" ht="93.75" spans="1:4">
+      <c r="A163" s="25"/>
+      <c r="B163" s="30">
+        <v>5</v>
+      </c>
+      <c r="C163" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="B158" s="26">
-        <v>5</v>
-      </c>
-      <c r="C158" s="12" t="s">
+      <c r="D163" s="31" t="s">
         <v>248</v>
       </c>
-      <c r="D158" s="11" t="s">
+    </row>
+    <row r="164" ht="222" spans="1:4">
+      <c r="A164" s="25"/>
+      <c r="B164" s="30">
+        <v>5</v>
+      </c>
+      <c r="C164" s="12" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="159" ht="38.25" spans="1:4">
-      <c r="A159" s="30"/>
-      <c r="B159" s="26">
+      <c r="D164" s="31" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="165" ht="168.75" spans="1:4">
+      <c r="A165" s="25"/>
+      <c r="B165" s="30">
+        <v>5</v>
+      </c>
+      <c r="C165" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="D165" s="31" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" s="25"/>
+      <c r="B166" s="30"/>
+      <c r="C166" s="12"/>
+      <c r="D166" s="31"/>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="25"/>
+      <c r="B167" s="30"/>
+      <c r="C167" s="12"/>
+      <c r="D167" s="31"/>
+    </row>
+    <row r="168" ht="144" spans="1:4">
+      <c r="A168" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="B168" s="30">
+        <v>5</v>
+      </c>
+      <c r="C168" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="D168" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="169" ht="47.25" spans="1:4">
+      <c r="A169" s="33"/>
+      <c r="B169" s="30">
         <v>1</v>
       </c>
-      <c r="C159" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="D159" s="11"/>
-    </row>
-    <row r="160" ht="25.5" spans="1:4">
-      <c r="A160" s="30"/>
-      <c r="B160" s="26">
+      <c r="C169" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="D169" s="11"/>
+    </row>
+    <row r="170" ht="31.5" spans="1:4">
+      <c r="A170" s="33"/>
+      <c r="B170" s="30">
         <v>1</v>
       </c>
-      <c r="C160" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="D160" s="12"/>
-    </row>
-    <row r="161" ht="25.5" spans="1:4">
-      <c r="A161" s="30"/>
-      <c r="B161" s="21">
+      <c r="C170" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="D170" s="12"/>
+    </row>
+    <row r="171" ht="31.5" spans="1:4">
+      <c r="A171" s="33"/>
+      <c r="B171" s="22">
         <v>1</v>
       </c>
-      <c r="C161" s="19" t="s">
-        <v>252</v>
-      </c>
-      <c r="D161" s="11"/>
-    </row>
-    <row r="162" ht="40.5" spans="1:4">
-      <c r="A162" s="30"/>
-      <c r="B162" s="21">
-        <v>5</v>
-      </c>
-      <c r="C162" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="D162" s="8" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="163" ht="38.25" spans="1:4">
-      <c r="A163" s="30"/>
-      <c r="B163" s="21">
+      <c r="C171" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="D171" s="11"/>
+    </row>
+    <row r="172" ht="56.25" spans="1:4">
+      <c r="A172" s="33"/>
+      <c r="B172" s="22">
+        <v>5</v>
+      </c>
+      <c r="C172" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D172" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="173" ht="47.25" spans="1:4">
+      <c r="A173" s="33"/>
+      <c r="B173" s="22">
         <v>1</v>
       </c>
-      <c r="C163" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="D163" s="11"/>
-    </row>
-    <row r="164" ht="38.25" spans="1:4">
-      <c r="A164" s="30"/>
-      <c r="B164" s="21">
+      <c r="C173" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="D173" s="11"/>
+    </row>
+    <row r="174" ht="47.25" spans="1:4">
+      <c r="A174" s="33"/>
+      <c r="B174" s="22">
         <v>1</v>
       </c>
-      <c r="C164" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="D164" s="11"/>
-    </row>
-    <row r="165" ht="39.75" spans="1:4">
-      <c r="A165" s="30"/>
-      <c r="B165" s="21">
-        <v>5</v>
-      </c>
-      <c r="C165" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="D165" s="11" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="166" ht="235" customHeight="1" spans="1:4">
-      <c r="A166" s="30"/>
-      <c r="B166" s="21">
-        <v>5</v>
-      </c>
-      <c r="C166" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="D166" s="11" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="167" ht="208" customHeight="1" spans="1:5">
-      <c r="A167" s="30"/>
-      <c r="B167" s="21">
-        <v>5</v>
-      </c>
-      <c r="C167" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="D167" s="11" t="s">
+      <c r="C174" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="E167" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="168" ht="38" customHeight="1" spans="1:3">
-      <c r="A168" s="30"/>
-      <c r="B168" s="21">
+      <c r="D174" s="11"/>
+    </row>
+    <row r="175" ht="53.25" spans="1:4">
+      <c r="A175" s="33"/>
+      <c r="B175" s="22">
+        <v>5</v>
+      </c>
+      <c r="C175" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="D175" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="176" ht="235" customHeight="1" spans="1:4">
+      <c r="A176" s="33"/>
+      <c r="B176" s="22">
+        <v>5</v>
+      </c>
+      <c r="C176" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="D176" s="11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="177" ht="208" customHeight="1" spans="1:5">
+      <c r="A177" s="33"/>
+      <c r="B177" s="22">
+        <v>5</v>
+      </c>
+      <c r="C177" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="D177" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="E177" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="178" ht="38" customHeight="1" spans="1:3">
+      <c r="A178" s="33"/>
+      <c r="B178" s="22">
         <v>1</v>
       </c>
-      <c r="C168" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="169" ht="38" customHeight="1" spans="1:4">
-      <c r="A169" s="30"/>
-      <c r="B169" s="21">
+      <c r="C178" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="179" ht="38" customHeight="1" spans="1:4">
+      <c r="A179" s="33"/>
+      <c r="B179" s="22">
         <v>1</v>
       </c>
-      <c r="C169" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="D169" s="11"/>
-    </row>
-    <row r="170" ht="51" customHeight="1" spans="1:4">
-      <c r="A170" s="30"/>
-      <c r="B170" s="21">
+      <c r="C179" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D179" s="11"/>
+    </row>
+    <row r="180" ht="51" customHeight="1" spans="1:4">
+      <c r="A180" s="33"/>
+      <c r="B180" s="22">
         <v>1</v>
       </c>
-      <c r="C170" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="D170" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="171" ht="28" customHeight="1" spans="1:4">
-      <c r="A171" s="30"/>
-      <c r="B171" s="21"/>
-      <c r="C171" s="12"/>
-      <c r="D171" s="11"/>
-    </row>
-    <row r="172" ht="34" customHeight="1" spans="1:4">
-      <c r="A172" s="30" t="s">
-        <v>267</v>
-      </c>
-      <c r="B172" s="21">
-        <v>2</v>
-      </c>
-      <c r="C172" s="12" t="s">
-        <v>268</v>
-      </c>
-      <c r="D172" s="11" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="173" ht="37" customHeight="1" spans="1:4">
-      <c r="A173" s="30"/>
-      <c r="B173" s="26">
-        <v>1</v>
-      </c>
-      <c r="C173" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="D173" s="11"/>
-    </row>
-    <row r="174" ht="39" customHeight="1" spans="1:4">
-      <c r="A174" s="30"/>
-      <c r="B174" s="21">
-        <v>2</v>
-      </c>
-      <c r="C174" s="12" t="s">
+      <c r="C180" s="12" t="s">
         <v>271</v>
       </c>
-      <c r="D174" s="11"/>
-    </row>
-    <row r="175" ht="28" customHeight="1" spans="1:4">
-      <c r="A175" s="30"/>
-      <c r="B175" s="21"/>
-      <c r="C175" s="12"/>
-      <c r="D175" s="11"/>
-    </row>
-    <row r="176" ht="28" customHeight="1" spans="1:4">
-      <c r="A176" s="30"/>
-      <c r="B176" s="21"/>
-      <c r="C176" s="12"/>
-      <c r="D176" s="11"/>
-    </row>
-    <row r="177" ht="28" customHeight="1" spans="1:4">
-      <c r="A177" s="30"/>
-      <c r="B177" s="21"/>
-      <c r="C177" s="12"/>
-      <c r="D177" s="11"/>
-    </row>
-    <row r="178" ht="28" customHeight="1" spans="1:4">
-      <c r="A178" s="30"/>
-      <c r="B178" s="21"/>
-      <c r="C178" s="12"/>
-      <c r="D178" s="11"/>
-    </row>
-    <row r="179" ht="28" customHeight="1" spans="1:4">
-      <c r="A179" s="30"/>
-      <c r="B179" s="21"/>
-      <c r="C179" s="12"/>
-      <c r="D179" s="11"/>
-    </row>
-    <row r="180" ht="28" customHeight="1" spans="1:4">
-      <c r="A180" s="30"/>
-      <c r="B180" s="21"/>
-      <c r="C180" s="12"/>
-      <c r="D180" s="11"/>
+      <c r="D180" s="2" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="181" ht="28" customHeight="1" spans="1:4">
-      <c r="A181" s="30"/>
-      <c r="B181" s="21"/>
+      <c r="A181" s="33"/>
+      <c r="B181" s="22"/>
       <c r="C181" s="12"/>
       <c r="D181" s="11"/>
     </row>
-    <row r="182" ht="28" customHeight="1" spans="1:4">
-      <c r="A182" s="30"/>
-      <c r="B182" s="21"/>
-      <c r="C182" s="12"/>
-      <c r="D182" s="11"/>
-    </row>
-    <row r="183" ht="25.5" spans="1:4">
-      <c r="A183" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="B183" s="21">
+    <row r="182" ht="34" customHeight="1" spans="1:4">
+      <c r="A182" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="B182" s="22">
         <v>2</v>
       </c>
+      <c r="C182" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D182" s="11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="183" ht="58" customHeight="1" spans="1:4">
+      <c r="A183" s="33"/>
+      <c r="B183" s="30">
+        <v>1</v>
+      </c>
       <c r="C183" s="12" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D183" s="11"/>
     </row>
-    <row r="184" ht="38.25" spans="1:4">
-      <c r="A184" s="30"/>
-      <c r="B184" s="21">
+    <row r="184" ht="39" customHeight="1" spans="1:4">
+      <c r="A184" s="33"/>
+      <c r="B184" s="22">
+        <v>2</v>
+      </c>
+      <c r="C184" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="D184" s="11"/>
+    </row>
+    <row r="185" ht="28" customHeight="1" spans="1:4">
+      <c r="A185" s="33"/>
+      <c r="B185" s="22"/>
+      <c r="C185" s="12"/>
+      <c r="D185" s="11"/>
+    </row>
+    <row r="186" ht="28" customHeight="1" spans="1:4">
+      <c r="A186" s="33"/>
+      <c r="B186" s="22"/>
+      <c r="C186" s="12"/>
+      <c r="D186" s="11"/>
+    </row>
+    <row r="187" ht="28" customHeight="1" spans="1:4">
+      <c r="A187" s="33"/>
+      <c r="B187" s="22"/>
+      <c r="C187" s="12"/>
+      <c r="D187" s="11"/>
+    </row>
+    <row r="188" ht="28" customHeight="1" spans="1:4">
+      <c r="A188" s="33"/>
+      <c r="B188" s="22"/>
+      <c r="C188" s="12"/>
+      <c r="D188" s="11"/>
+    </row>
+    <row r="189" ht="28" customHeight="1" spans="1:4">
+      <c r="A189" s="33"/>
+      <c r="B189" s="22"/>
+      <c r="C189" s="12"/>
+      <c r="D189" s="11"/>
+    </row>
+    <row r="190" ht="28" customHeight="1" spans="1:4">
+      <c r="A190" s="33"/>
+      <c r="B190" s="22"/>
+      <c r="C190" s="12"/>
+      <c r="D190" s="11"/>
+    </row>
+    <row r="191" ht="28" customHeight="1" spans="1:4">
+      <c r="A191" s="33"/>
+      <c r="B191" s="22"/>
+      <c r="C191" s="12"/>
+      <c r="D191" s="11"/>
+    </row>
+    <row r="192" ht="28" customHeight="1" spans="1:4">
+      <c r="A192" s="33"/>
+      <c r="B192" s="22"/>
+      <c r="C192" s="12"/>
+      <c r="D192" s="11"/>
+    </row>
+    <row r="193" ht="31.5" spans="1:4">
+      <c r="A193" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="B193" s="22">
+        <v>2</v>
+      </c>
+      <c r="C193" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="D193" s="11"/>
+    </row>
+    <row r="194" ht="47.25" spans="1:4">
+      <c r="A194" s="33"/>
+      <c r="B194" s="22">
         <v>1</v>
       </c>
-      <c r="C184" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="D184" s="11"/>
-    </row>
-    <row r="185" ht="25.5" spans="1:4">
-      <c r="A185" s="30"/>
-      <c r="B185" s="21">
+      <c r="C194" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="D194" s="11"/>
+    </row>
+    <row r="195" ht="31.5" spans="1:4">
+      <c r="A195" s="33"/>
+      <c r="B195" s="22">
         <v>1</v>
       </c>
-      <c r="C185" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="D185" s="11"/>
-    </row>
-    <row r="186" ht="25.5" spans="1:4">
-      <c r="A186" s="30"/>
-      <c r="B186" s="21">
+      <c r="C195" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D195" s="11"/>
+    </row>
+    <row r="196" ht="31.5" spans="1:4">
+      <c r="A196" s="33"/>
+      <c r="B196" s="22">
         <v>1</v>
       </c>
-      <c r="C186" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="D186" s="11"/>
-    </row>
-    <row r="187" ht="25.5" spans="1:4">
-      <c r="A187" s="30"/>
-      <c r="B187" s="21">
+      <c r="C196" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D196" s="11"/>
+    </row>
+    <row r="197" ht="31.5" spans="1:4">
+      <c r="A197" s="33"/>
+      <c r="B197" s="22">
         <v>1</v>
       </c>
-      <c r="C187" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="D187" s="11"/>
-    </row>
-    <row r="188" ht="25.5" spans="1:4">
-      <c r="A188" s="30"/>
-      <c r="B188" s="21">
+      <c r="C197" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D197" s="11"/>
+    </row>
+    <row r="198" ht="31.5" spans="1:4">
+      <c r="A198" s="33"/>
+      <c r="B198" s="22">
         <v>1</v>
       </c>
-      <c r="C188" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D188" s="11"/>
-    </row>
-    <row r="189" ht="25.5" spans="1:4">
-      <c r="A189" s="30"/>
-      <c r="B189" s="21">
+      <c r="C198" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D198" s="11"/>
+    </row>
+    <row r="199" ht="31.5" spans="1:4">
+      <c r="A199" s="33"/>
+      <c r="B199" s="22">
         <v>1</v>
       </c>
-      <c r="C189" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="D189" s="11"/>
-    </row>
-    <row r="190" ht="25.5" spans="1:4">
-      <c r="A190" s="30"/>
-      <c r="B190" s="21">
+      <c r="C199" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D199" s="11"/>
+    </row>
+    <row r="200" ht="31.5" spans="1:4">
+      <c r="A200" s="33"/>
+      <c r="B200" s="22">
         <v>1</v>
       </c>
-      <c r="C190" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="D190" s="11"/>
-    </row>
-    <row r="191" ht="38.25" spans="1:4">
-      <c r="A191" s="30"/>
-      <c r="B191" s="21">
+      <c r="C200" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D200" s="11"/>
+    </row>
+    <row r="201" ht="47.25" spans="1:4">
+      <c r="A201" s="33"/>
+      <c r="B201" s="22">
         <v>1</v>
       </c>
-      <c r="C191" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="D191" s="11"/>
-    </row>
-    <row r="192" ht="25.5" spans="1:4">
-      <c r="A192" s="30"/>
-      <c r="B192" s="21">
+      <c r="C201" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D201" s="11"/>
+    </row>
+    <row r="202" ht="31.5" spans="1:4">
+      <c r="A202" s="33"/>
+      <c r="B202" s="22">
         <v>1</v>
       </c>
-      <c r="C192" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="D192" s="11"/>
-    </row>
-    <row r="193" spans="1:4">
-      <c r="A193" s="30"/>
-      <c r="B193" s="21">
+      <c r="C202" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D202" s="11"/>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" s="33"/>
+      <c r="B203" s="22">
         <v>1</v>
       </c>
-      <c r="C193" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="D193" s="11"/>
-    </row>
-    <row r="194" ht="38.25" spans="1:4">
-      <c r="A194" s="30"/>
-      <c r="B194" s="21">
+      <c r="C203" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D203" s="11"/>
+    </row>
+    <row r="204" ht="47.25" spans="1:4">
+      <c r="A204" s="33"/>
+      <c r="B204" s="22">
         <v>1</v>
       </c>
-      <c r="C194" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D194" s="11"/>
-    </row>
-    <row r="195" ht="38.25" spans="1:4">
-      <c r="A195" s="30"/>
-      <c r="B195" s="21">
+      <c r="C204" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D204" s="11"/>
+    </row>
+    <row r="205" ht="47.25" spans="1:4">
+      <c r="A205" s="33"/>
+      <c r="B205" s="22">
         <v>1</v>
       </c>
-      <c r="C195" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="D195" s="11"/>
-    </row>
-    <row r="196" ht="81" spans="1:4">
-      <c r="A196" s="30"/>
-      <c r="B196" s="21">
-        <v>5</v>
-      </c>
-      <c r="C196" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="D196" s="11" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4">
-      <c r="A197" s="30"/>
-      <c r="B197" s="21"/>
-      <c r="D197" s="11"/>
-    </row>
-    <row r="198" ht="108" spans="1:4">
-      <c r="A198" s="30"/>
-      <c r="B198" s="21">
-        <v>5</v>
-      </c>
-      <c r="C198" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="D198" s="11" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="199" ht="66.75" spans="1:4">
-      <c r="A199" s="30"/>
-      <c r="B199" s="21">
-        <v>5</v>
-      </c>
-      <c r="C199" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="D199" s="11" t="s">
+      <c r="C205" s="2" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="200" ht="146.25" spans="1:4">
-      <c r="A200" s="30"/>
-      <c r="B200" s="21">
-        <v>5</v>
-      </c>
-      <c r="C200" s="12" t="s">
+      <c r="D205" s="11"/>
+    </row>
+    <row r="206" ht="112.5" spans="1:4">
+      <c r="A206" s="33"/>
+      <c r="B206" s="22">
+        <v>5</v>
+      </c>
+      <c r="C206" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="D200" s="31" t="s">
+      <c r="D206" s="11" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="201" ht="54" spans="1:4">
-      <c r="A201" s="30" t="s">
+    <row r="207" spans="1:4">
+      <c r="A207" s="33"/>
+      <c r="B207" s="22"/>
+      <c r="D207" s="11"/>
+    </row>
+    <row r="208" ht="150" spans="1:4">
+      <c r="A208" s="33"/>
+      <c r="B208" s="22">
+        <v>5</v>
+      </c>
+      <c r="C208" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B201" s="21">
-        <v>5</v>
-      </c>
-      <c r="C201" s="12" t="s">
+      <c r="D208" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="D201" s="31" t="s">
+    </row>
+    <row r="209" ht="90.75" spans="1:4">
+      <c r="A209" s="33"/>
+      <c r="B209" s="22">
+        <v>5</v>
+      </c>
+      <c r="C209" s="2" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="202" ht="183" spans="1:4">
-      <c r="A202" s="30"/>
-      <c r="B202" s="21">
-        <v>5</v>
-      </c>
-      <c r="C202" s="12" t="s">
+      <c r="D209" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="D202" s="32" t="s">
+    </row>
+    <row r="210" ht="197.25" spans="1:4">
+      <c r="A210" s="33"/>
+      <c r="B210" s="22">
+        <v>5</v>
+      </c>
+      <c r="C210" s="12" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="203" spans="1:4">
-      <c r="A203" s="30"/>
-      <c r="B203" s="21"/>
-      <c r="C203" s="12"/>
-      <c r="D203" s="31"/>
-    </row>
-    <row r="204" spans="1:4">
-      <c r="A204" s="30"/>
-      <c r="B204" s="21"/>
-      <c r="C204" s="12"/>
-      <c r="D204" s="31"/>
-    </row>
-    <row r="205" spans="1:4">
-      <c r="A205" s="30"/>
-      <c r="B205" s="21"/>
-      <c r="C205" s="12"/>
-      <c r="D205" s="31"/>
-    </row>
-    <row r="206" spans="1:4">
-      <c r="A206" s="30"/>
-      <c r="B206" s="21"/>
-      <c r="C206" s="12"/>
-      <c r="D206" s="31"/>
-    </row>
-    <row r="207" spans="1:4">
-      <c r="A207" s="30"/>
-      <c r="B207" s="21"/>
-      <c r="C207" s="12"/>
-      <c r="D207" s="31"/>
-    </row>
-    <row r="208" spans="1:4">
-      <c r="A208" s="30"/>
-      <c r="B208" s="21"/>
-      <c r="C208" s="12"/>
-      <c r="D208" s="31"/>
-    </row>
-    <row r="209" ht="25.5" spans="1:4">
-      <c r="A209" s="30" t="s">
+      <c r="D210" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="B209" s="21"/>
-      <c r="C209" s="12" t="s">
+    </row>
+    <row r="211" ht="75" spans="1:4">
+      <c r="A211" s="33" t="s">
         <v>300</v>
       </c>
-      <c r="D209" s="31" t="s">
+      <c r="B211" s="22">
+        <v>5</v>
+      </c>
+      <c r="C211" s="12" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="210" ht="40.5" spans="1:4">
-      <c r="A210" s="30"/>
-      <c r="B210" s="21">
-        <v>5</v>
-      </c>
-      <c r="C210" s="12" t="s">
+      <c r="D211" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="D210" s="11" t="s">
+    </row>
+    <row r="212" ht="238.5" spans="1:4">
+      <c r="A212" s="33"/>
+      <c r="B212" s="22">
+        <v>5</v>
+      </c>
+      <c r="C212" s="12" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="211" ht="38.25" spans="1:4">
-      <c r="A211" s="30"/>
-      <c r="B211" s="21">
-        <v>5</v>
-      </c>
-      <c r="C211" s="12" t="s">
+      <c r="D212" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="D211" s="11" t="s">
+    </row>
+    <row r="213" spans="1:4">
+      <c r="A213" s="33"/>
+      <c r="B213" s="22"/>
+      <c r="C213" s="12"/>
+      <c r="D213" s="34"/>
+    </row>
+    <row r="214" spans="1:4">
+      <c r="A214" s="33"/>
+      <c r="B214" s="22"/>
+      <c r="C214" s="12"/>
+      <c r="D214" s="34"/>
+    </row>
+    <row r="215" spans="1:4">
+      <c r="A215" s="33"/>
+      <c r="B215" s="22"/>
+      <c r="C215" s="12"/>
+      <c r="D215" s="34"/>
+    </row>
+    <row r="216" spans="1:4">
+      <c r="A216" s="33"/>
+      <c r="B216" s="22"/>
+      <c r="C216" s="12"/>
+      <c r="D216" s="34"/>
+    </row>
+    <row r="217" spans="1:4">
+      <c r="A217" s="33"/>
+      <c r="B217" s="22"/>
+      <c r="C217" s="12"/>
+      <c r="D217" s="34"/>
+    </row>
+    <row r="218" spans="1:4">
+      <c r="A218" s="33"/>
+      <c r="B218" s="22"/>
+      <c r="C218" s="12"/>
+      <c r="D218" s="34"/>
+    </row>
+    <row r="219" ht="31.5" spans="1:4">
+      <c r="A219" s="33" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="212" spans="1:4">
-      <c r="A212" s="30"/>
-      <c r="B212" s="21">
+      <c r="B219" s="22"/>
+      <c r="C219" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="D219" s="34" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="220" ht="56.25" spans="1:4">
+      <c r="A220" s="33"/>
+      <c r="B220" s="22">
+        <v>5</v>
+      </c>
+      <c r="C220" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="D220" s="11" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="221" ht="47.25" spans="1:4">
+      <c r="A221" s="33"/>
+      <c r="B221" s="22">
+        <v>5</v>
+      </c>
+      <c r="C221" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="D221" s="11" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4">
+      <c r="A222" s="33"/>
+      <c r="B222" s="22">
         <v>2</v>
       </c>
-      <c r="C212" s="12" t="s">
-        <v>306</v>
-      </c>
-      <c r="D212" s="11"/>
-    </row>
-    <row r="213" ht="109" customHeight="1" spans="1:4">
-      <c r="A213" s="30"/>
-      <c r="B213" s="21">
-        <v>5</v>
-      </c>
-      <c r="C213" s="12" t="s">
-        <v>307</v>
-      </c>
-      <c r="D213" s="11" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="214" ht="42.75" spans="1:4">
-      <c r="A214" s="30"/>
-      <c r="B214" s="21">
-        <v>5</v>
-      </c>
-      <c r="C214" s="25" t="s">
-        <v>309</v>
-      </c>
-      <c r="D214" s="11" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="215" ht="40.5" spans="1:4">
-      <c r="A215" s="30" t="s">
-        <v>311</v>
-      </c>
-      <c r="B215" s="21">
-        <v>5</v>
-      </c>
-      <c r="C215" s="33" t="s">
+      <c r="C222" s="12" t="s">
         <v>312</v>
       </c>
-      <c r="D215" s="33" t="s">
+      <c r="D222" s="11"/>
+    </row>
+    <row r="223" ht="109" customHeight="1" spans="1:4">
+      <c r="A223" s="33"/>
+      <c r="B223" s="22">
+        <v>5</v>
+      </c>
+      <c r="C223" s="12" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="216" ht="67" customHeight="1" spans="1:4">
-      <c r="A216" s="30"/>
-      <c r="B216" s="21">
-        <v>5</v>
-      </c>
-      <c r="C216" s="12" t="s">
+      <c r="D223" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="D216" s="12" t="s">
+    </row>
+    <row r="224" ht="42.75" spans="1:4">
+      <c r="A224" s="33"/>
+      <c r="B224" s="22">
+        <v>5</v>
+      </c>
+      <c r="C224" s="29" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="217" ht="42" customHeight="1" spans="1:4">
-      <c r="A217" s="30"/>
-      <c r="B217" s="21">
-        <v>5</v>
-      </c>
-      <c r="C217" s="12" t="s">
+      <c r="D224" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="D217" s="12" t="s">
+    </row>
+    <row r="225" ht="56.25" spans="1:4">
+      <c r="A225" s="33" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="218" ht="82" customHeight="1" spans="1:4">
-      <c r="A218" s="30"/>
-      <c r="B218" s="21">
-        <v>5</v>
-      </c>
-      <c r="C218" s="12" t="s">
+      <c r="B225" s="22">
+        <v>5</v>
+      </c>
+      <c r="C225" s="36" t="s">
         <v>318</v>
       </c>
-      <c r="D218" s="12" t="s">
+      <c r="D225" s="36" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="219" ht="54" spans="1:4">
-      <c r="A219" s="30"/>
-      <c r="B219" s="26">
-        <v>5</v>
-      </c>
-      <c r="C219" s="12" t="s">
+    <row r="226" ht="67" customHeight="1" spans="1:4">
+      <c r="A226" s="33"/>
+      <c r="B226" s="22">
+        <v>5</v>
+      </c>
+      <c r="C226" s="12" t="s">
         <v>320</v>
       </c>
-      <c r="D219" s="12" t="s">
+      <c r="D226" s="12" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="220" ht="25.5" spans="1:4">
-      <c r="A220" s="30"/>
-      <c r="B220" s="21">
-        <v>5</v>
-      </c>
-      <c r="C220" s="12" t="s">
+    <row r="227" ht="42" customHeight="1" spans="1:4">
+      <c r="A227" s="33"/>
+      <c r="B227" s="22">
+        <v>5</v>
+      </c>
+      <c r="C227" s="12" t="s">
         <v>322</v>
       </c>
-      <c r="D220" s="12" t="s">
+      <c r="D227" s="12" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="221" ht="220" customHeight="1" spans="1:4">
-      <c r="A221" s="30" t="s">
+    <row r="228" ht="82" customHeight="1" spans="1:4">
+      <c r="A228" s="33"/>
+      <c r="B228" s="22">
+        <v>5</v>
+      </c>
+      <c r="C228" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="B221" s="21">
-        <v>5</v>
-      </c>
-      <c r="C221" s="12" t="s">
+      <c r="D228" s="12" t="s">
         <v>325</v>
       </c>
-      <c r="D221" s="12" t="s">
+    </row>
+    <row r="229" ht="75" spans="1:4">
+      <c r="A229" s="33"/>
+      <c r="B229" s="30">
+        <v>5</v>
+      </c>
+      <c r="C229" s="12" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="222" ht="27" spans="1:4">
-      <c r="A222" s="30"/>
-      <c r="B222" s="21">
-        <v>5</v>
-      </c>
-      <c r="C222" s="12" t="s">
+      <c r="D229" s="12" t="s">
         <v>327</v>
       </c>
-      <c r="D222" s="12" t="s">
+    </row>
+    <row r="230" ht="31.5" spans="1:4">
+      <c r="A230" s="33"/>
+      <c r="B230" s="22">
+        <v>5</v>
+      </c>
+      <c r="C230" s="12" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="223" ht="119.25" spans="1:4">
-      <c r="A223" s="30"/>
-      <c r="B223" s="21">
-        <v>5</v>
-      </c>
-      <c r="C223" s="2" t="s">
+      <c r="D230" s="12" t="s">
         <v>329</v>
       </c>
-      <c r="D223" s="2" t="s">
+    </row>
+    <row r="231" ht="220" customHeight="1" spans="1:4">
+      <c r="A231" s="33" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="224" ht="104.25" spans="1:4">
-      <c r="A224" s="30"/>
-      <c r="B224" s="21"/>
-      <c r="C224" s="2" t="s">
+      <c r="B231" s="22">
+        <v>5</v>
+      </c>
+      <c r="C231" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="D224" s="19" t="s">
+      <c r="D231" s="12" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="225" ht="64.5" spans="1:4">
-      <c r="A225" s="30"/>
-      <c r="B225" s="21">
-        <v>5</v>
-      </c>
-      <c r="C225" s="2" t="s">
+    <row r="232" ht="37.5" spans="1:4">
+      <c r="A232" s="33"/>
+      <c r="B232" s="22">
+        <v>5</v>
+      </c>
+      <c r="C232" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="D225" s="2" t="s">
+      <c r="D232" s="12" t="s">
         <v>334</v>
       </c>
     </row>
+    <row r="233" ht="159.75" spans="1:4">
+      <c r="A233" s="33"/>
+      <c r="B233" s="22">
+        <v>5</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D233" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="234" ht="135" spans="1:4">
+      <c r="A234" s="33"/>
+      <c r="B234" s="22"/>
+      <c r="C234" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="D234" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="235" ht="81.75" spans="1:4">
+      <c r="A235" s="33"/>
+      <c r="B235" s="22">
+        <v>5</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="D235" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="E1:E225">
+  <autoFilter ref="E1:E235">
     <extLst/>
   </autoFilter>
-  <mergeCells count="15">
+  <mergeCells count="16">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="A14:A54"/>
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="A59:A63"/>
-    <mergeCell ref="A64:A77"/>
-    <mergeCell ref="A78:A157"/>
-    <mergeCell ref="A158:A171"/>
-    <mergeCell ref="A172:A182"/>
-    <mergeCell ref="A183:A200"/>
-    <mergeCell ref="A201:A208"/>
-    <mergeCell ref="A209:A214"/>
-    <mergeCell ref="A215:A220"/>
-    <mergeCell ref="A221:A225"/>
+    <mergeCell ref="A64:A81"/>
+    <mergeCell ref="A82:A87"/>
+    <mergeCell ref="A88:A167"/>
+    <mergeCell ref="A168:A181"/>
+    <mergeCell ref="A182:A192"/>
+    <mergeCell ref="A193:A210"/>
+    <mergeCell ref="A211:A218"/>
+    <mergeCell ref="A219:A224"/>
+    <mergeCell ref="A225:A230"/>
+    <mergeCell ref="A231:A235"/>
   </mergeCells>
-  <conditionalFormatting sqref="B158">
+  <conditionalFormatting sqref="B168">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -5258,7 +5378,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B53 B78:B157 B55:B76 B159:B1048576">
+  <conditionalFormatting sqref="B1:B53 B55:B86 B169:B1048576 B88:B167">
     <cfRule type="cellIs" dxfId="0" priority="4" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -5270,7 +5390,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C98" r:id="rId1" display="Panoptic Segmentation" tooltip="https://arxiv.org/abs/1801.00868"/>
+    <hyperlink ref="C108" r:id="rId1" display="Panoptic Segmentation" tooltip="https://arxiv.org/abs/1801.00868"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
add reading note for psudo-lidar
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14670" windowHeight="6345" tabRatio="354"/>
+    <workbookView windowWidth="27720" windowHeight="13140" tabRatio="354"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$235</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$233</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344">
   <si>
     <t>Scope</t>
   </si>
@@ -600,6 +600,20 @@
 trick: uncertainty_weighting提升比较大， 还用了left/right flip</t>
   </si>
   <si>
+    <t>psudo-lidar from visual depth estimation: bridging the gap in 3d object detection for autonomous driving</t>
+  </si>
+  <si>
+    <t>1. 双目的disparity在俯视图下的效果会更好,  因为这个时候长和宽 invariant to depth
+2. disparity 到psudo-lidar的转换: 高于雷达高度1m的点丢弃, 雷达的反射强度都设置为1;</t>
+  </si>
+  <si>
+    <t>Pseudo-LiDAR++: Accurate Depth for 3D Object Detection in Autonomous Driving</t>
+  </si>
+  <si>
+    <t>1. 目前深度估计对远处物体不准的原因是因为都是先估计disparity再用disparity的导数算depth, 这样其实是over-emphasis了近处的物体, 因此本文提出了直接估计depth的cost
+2. 同时, 提出了一种用低线束的激光进一步提高深度估计结果的方法(graph based)</t>
+  </si>
+  <si>
     <t>image semantic segmentation</t>
   </si>
   <si>
@@ -1338,7 +1352,7 @@
     <t>Segmentation is All You Need</t>
   </si>
   <si>
-    <t>instance segmentation by jointly optimizing spatial embeddings and clustering Bandwidth</t>
+    <t>(2019, cvpr) instance segmentation by jointly optimizing spatial embeddings and clustering Bandwidth</t>
   </si>
   <si>
     <t>The Best of Both Modes: Separately Leverageing RGB and Depth for Unseen Object Instance Segmentation</t>
@@ -1471,9 +1485,6 @@
 </t>
   </si>
   <si>
-    <t>semantic stixel: Depth is Not Enough</t>
-  </si>
-  <si>
     <t>Detecting Unexpected Obstacles for Self-Drving Cars_Fusing Deep Learning and Geometirc Modeling</t>
   </si>
   <si>
@@ -1617,10 +1628,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1672,6 +1683,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -1680,7 +1699,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1694,6 +1713,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -1702,45 +1728,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1756,15 +1743,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1778,16 +1766,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1802,9 +1783,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1868,7 +1879,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1880,13 +1909,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1898,7 +1933,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1910,31 +2029,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1946,31 +2041,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1982,67 +2053,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2105,21 +2116,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -2134,22 +2130,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2171,9 +2162,20 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2192,157 +2194,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2402,9 +2413,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2562,7 +2570,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="4C4C4C"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -2815,15 +2823,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G235"/>
+  <dimension ref="A1:G233"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D94" sqref="D94"/>
+      <selection pane="bottomLeft" activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="15.75" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="13.4266666666667" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
@@ -2847,7 +2855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="56.25" spans="1:4">
+    <row r="2" ht="40.5" spans="1:4">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -2859,7 +2867,7 @@
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" ht="18.75" spans="1:4">
+    <row r="3" ht="13.5" spans="1:4">
       <c r="A3" s="9"/>
       <c r="B3" s="10">
         <v>5</v>
@@ -2869,7 +2877,7 @@
       </c>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" ht="18.75" spans="1:4">
+    <row r="4" ht="13.5" spans="1:4">
       <c r="A4" s="9"/>
       <c r="B4" s="10">
         <v>5</v>
@@ -2879,7 +2887,7 @@
       </c>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" ht="18.75" spans="1:4">
+    <row r="5" ht="13.5" spans="1:4">
       <c r="A5" s="9"/>
       <c r="B5" s="10">
         <v>5</v>
@@ -2891,7 +2899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="18.75" spans="1:4">
+    <row r="6" ht="13.5" spans="1:4">
       <c r="A6" s="9"/>
       <c r="B6" s="10"/>
       <c r="C6" s="12" t="s">
@@ -2899,7 +2907,7 @@
       </c>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" ht="31.5" spans="1:4">
+    <row r="7" ht="25.5" spans="1:4">
       <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
@@ -2911,7 +2919,7 @@
       </c>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" ht="31.5" spans="1:4">
+    <row r="8" ht="25.5" spans="1:4">
       <c r="A8" s="9"/>
       <c r="B8" s="10"/>
       <c r="C8" s="12" t="s">
@@ -2919,7 +2927,7 @@
       </c>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" ht="81.75" spans="1:4">
+    <row r="9" ht="64.5" spans="1:4">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -2933,7 +2941,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" ht="18.75" spans="1:4">
+    <row r="10" ht="13.5" spans="1:4">
       <c r="A10" s="9"/>
       <c r="B10" s="13">
         <v>5</v>
@@ -2955,7 +2963,7 @@
       </c>
       <c r="D11" s="11"/>
     </row>
-    <row r="12" ht="31.5" spans="1:4">
+    <row r="12" ht="25.5" spans="1:4">
       <c r="A12" s="9"/>
       <c r="B12" s="10">
         <v>5</v>
@@ -2967,7 +2975,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" ht="93.75" spans="1:4">
+    <row r="13" ht="67.5" spans="1:4">
       <c r="A13" s="9"/>
       <c r="B13" s="10">
         <v>5</v>
@@ -2979,7 +2987,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" ht="125.25" spans="1:4">
+    <row r="14" ht="93" spans="1:4">
       <c r="A14" s="9" t="s">
         <v>24</v>
       </c>
@@ -2993,7 +3001,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" ht="37.5" spans="1:4">
+    <row r="15" ht="27" spans="1:4">
       <c r="A15" s="9"/>
       <c r="B15" s="14">
         <v>5</v>
@@ -3032,7 +3040,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" ht="34.5" spans="1:4">
+    <row r="18" ht="26.25" spans="1:4">
       <c r="A18" s="9"/>
       <c r="B18" s="14">
         <v>5</v>
@@ -3044,7 +3052,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" ht="103.5" spans="1:4">
+    <row r="19" ht="78.75" spans="1:4">
       <c r="A19" s="9"/>
       <c r="B19" s="14">
         <v>5</v>
@@ -3056,7 +3064,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" ht="47.25" spans="1:4">
+    <row r="20" ht="38.25" spans="1:4">
       <c r="A20" s="9"/>
       <c r="B20" s="14">
         <v>5</v>
@@ -3068,7 +3076,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" ht="47.25" spans="1:4">
+    <row r="21" ht="38.25" spans="1:4">
       <c r="A21" s="9"/>
       <c r="B21" s="16">
         <v>1</v>
@@ -3078,7 +3086,7 @@
       </c>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" ht="47.25" spans="1:4">
+    <row r="22" ht="38.25" spans="1:4">
       <c r="A22" s="9"/>
       <c r="B22" s="14">
         <v>5</v>
@@ -3088,7 +3096,7 @@
       </c>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" ht="31.5" spans="1:4">
+    <row r="23" ht="25.5" spans="1:4">
       <c r="A23" s="9"/>
       <c r="B23" s="14">
         <v>5</v>
@@ -3098,7 +3106,7 @@
       </c>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" ht="90.75" spans="1:4">
+    <row r="24" ht="66.75" spans="1:4">
       <c r="A24" s="9"/>
       <c r="B24" s="14">
         <v>5</v>
@@ -3110,7 +3118,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" ht="37.5" spans="1:4">
+    <row r="25" ht="27" spans="1:4">
       <c r="A25" s="9"/>
       <c r="B25" s="14">
         <v>5</v>
@@ -3122,7 +3130,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" ht="34.5" spans="1:5">
+    <row r="26" ht="26.25" spans="1:5">
       <c r="A26" s="9"/>
       <c r="B26" s="14">
         <v>5</v>
@@ -3137,7 +3145,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" ht="53.25" spans="1:4">
+    <row r="27" ht="39.75" spans="1:4">
       <c r="A27" s="9"/>
       <c r="B27" s="14">
         <v>5</v>
@@ -3149,7 +3157,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" ht="87.75" spans="1:4">
+    <row r="28" ht="66" spans="1:4">
       <c r="A28" s="9"/>
       <c r="B28" s="14">
         <v>5</v>
@@ -3161,7 +3169,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" ht="31.5" spans="1:4">
+    <row r="29" ht="25.5" spans="1:4">
       <c r="A29" s="9"/>
       <c r="B29" s="14">
         <v>5</v>
@@ -3173,7 +3181,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" ht="31.5" spans="1:4">
+    <row r="30" ht="25.5" spans="1:4">
       <c r="A30" s="9"/>
       <c r="B30" s="14">
         <v>5</v>
@@ -3531,8 +3539,8 @@
       <c r="A63" s="18"/>
       <c r="B63" s="14"/>
     </row>
-    <row r="64" ht="31.5" spans="1:7">
-      <c r="A64" s="20" t="s">
+    <row r="64" ht="25.5" spans="1:7">
+      <c r="A64" s="9" t="s">
         <v>103</v>
       </c>
       <c r="B64" s="14">
@@ -3542,11 +3550,11 @@
         <v>104</v>
       </c>
       <c r="D64" s="11"/>
-      <c r="F64" s="21"/>
-      <c r="G64" s="21"/>
-    </row>
-    <row r="65" ht="81.75" spans="1:6">
-      <c r="A65" s="20"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="20"/>
+    </row>
+    <row r="65" ht="64.5" spans="1:6">
+      <c r="A65" s="9"/>
       <c r="B65" s="14">
         <v>5</v>
       </c>
@@ -3558,8 +3566,8 @@
       </c>
       <c r="F65" s="1"/>
     </row>
-    <row r="66" ht="56.25" spans="1:4">
-      <c r="A66" s="20"/>
+    <row r="66" ht="40.5" spans="1:4">
+      <c r="A66" s="9"/>
       <c r="B66" s="10">
         <v>5</v>
       </c>
@@ -3570,8 +3578,8 @@
         <v>108</v>
       </c>
     </row>
-    <row r="67" ht="90.75" spans="1:4">
-      <c r="A67" s="20"/>
+    <row r="67" ht="66.75" spans="1:4">
+      <c r="A67" s="9"/>
       <c r="B67" s="10">
         <v>5</v>
       </c>
@@ -3582,9 +3590,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="68" ht="31.5" spans="1:4">
-      <c r="A68" s="20"/>
-      <c r="B68" s="22">
+    <row r="68" ht="25.5" spans="1:4">
+      <c r="A68" s="9"/>
+      <c r="B68" s="21">
         <v>5</v>
       </c>
       <c r="C68" s="2" t="s">
@@ -3594,8 +3602,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="69" ht="37.5" spans="1:4">
-      <c r="A69" s="20"/>
+    <row r="69" ht="27" spans="1:4">
+      <c r="A69" s="9"/>
       <c r="B69" s="10">
         <v>5</v>
       </c>
@@ -3606,8 +3614,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="70" ht="31.5" spans="1:4">
-      <c r="A70" s="20"/>
+    <row r="70" ht="25.5" spans="1:4">
+      <c r="A70" s="9"/>
       <c r="B70" s="10">
         <v>2</v>
       </c>
@@ -3616,8 +3624,8 @@
       </c>
       <c r="D70" s="11"/>
     </row>
-    <row r="71" ht="100.5" spans="1:4">
-      <c r="A71" s="20"/>
+    <row r="71" ht="78" spans="1:4">
+      <c r="A71" s="9"/>
       <c r="B71" s="10">
         <v>5</v>
       </c>
@@ -3628,8 +3636,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="72" ht="56.25" spans="1:4">
-      <c r="A72" s="20"/>
+    <row r="72" ht="40.5" spans="1:4">
+      <c r="A72" s="9"/>
       <c r="B72" s="10">
         <v>5</v>
       </c>
@@ -3640,8 +3648,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="73" ht="47.25" spans="1:4">
-      <c r="A73" s="20"/>
+    <row r="73" ht="38.25" spans="1:4">
+      <c r="A73" s="9"/>
       <c r="B73" s="10">
         <v>1</v>
       </c>
@@ -3650,8 +3658,8 @@
       </c>
       <c r="D73" s="11"/>
     </row>
-    <row r="74" ht="31.5" spans="1:4">
-      <c r="A74" s="20"/>
+    <row r="74" ht="25.5" spans="1:4">
+      <c r="A74" s="9"/>
       <c r="B74" s="10">
         <v>1</v>
       </c>
@@ -3661,7 +3669,7 @@
       <c r="D74" s="11"/>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="20"/>
+      <c r="A75" s="9"/>
       <c r="B75" s="10">
         <v>1</v>
       </c>
@@ -3670,8 +3678,8 @@
       </c>
       <c r="D75" s="11"/>
     </row>
-    <row r="76" ht="31.5" spans="1:4">
-      <c r="A76" s="20"/>
+    <row r="76" ht="25.5" spans="1:4">
+      <c r="A76" s="9"/>
       <c r="B76" s="10">
         <v>1</v>
       </c>
@@ -3681,40 +3689,40 @@
       <c r="D76" s="11"/>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="20"/>
-      <c r="B77" s="23"/>
+      <c r="A77" s="9"/>
+      <c r="B77" s="22"/>
       <c r="C77" s="12"/>
       <c r="D77" s="12"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="20"/>
-      <c r="B78" s="23"/>
+      <c r="A78" s="9"/>
+      <c r="B78" s="22"/>
       <c r="C78" s="12"/>
       <c r="D78" s="12"/>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="20"/>
-      <c r="B79" s="23"/>
+      <c r="A79" s="9"/>
+      <c r="B79" s="22"/>
       <c r="C79" s="12"/>
       <c r="D79" s="12"/>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="20"/>
-      <c r="B80" s="23"/>
+      <c r="A80" s="9"/>
+      <c r="B80" s="22"/>
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="20"/>
-      <c r="B81" s="23"/>
+      <c r="A81" s="9"/>
+      <c r="B81" s="22"/>
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>
     </row>
-    <row r="82" ht="93.75" spans="1:4">
-      <c r="A82" s="24" t="s">
+    <row r="82" ht="67.5" spans="1:4">
+      <c r="A82" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="B82" s="23">
+      <c r="B82" s="22">
         <v>5</v>
       </c>
       <c r="C82" s="12" t="s">
@@ -3724,9 +3732,9 @@
         <v>126</v>
       </c>
     </row>
-    <row r="83" ht="375.75" spans="1:4">
-      <c r="A83" s="24"/>
-      <c r="B83" s="23">
+    <row r="83" ht="279" spans="1:4">
+      <c r="A83" s="23"/>
+      <c r="B83" s="22">
         <v>5</v>
       </c>
       <c r="C83" s="12" t="s">
@@ -3736,1617 +3744,1614 @@
         <v>128</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="24"/>
-      <c r="B84" s="23"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="24"/>
-      <c r="B85" s="23"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
+    <row r="84" ht="51" spans="1:4">
+      <c r="A84" s="23"/>
+      <c r="B84" s="22">
+        <v>5</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="85" ht="40.5" spans="1:4">
+      <c r="A85" s="23"/>
+      <c r="B85" s="22">
+        <v>5</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="24"/>
-      <c r="B86" s="23"/>
+      <c r="A86" s="23"/>
+      <c r="B86" s="22"/>
       <c r="C86" s="12"/>
       <c r="D86" s="12"/>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="24"/>
-    </row>
-    <row r="88" ht="66" spans="1:4">
-      <c r="A88" s="25" t="s">
-        <v>129</v>
+      <c r="A87" s="23"/>
+    </row>
+    <row r="88" ht="51.75" spans="1:4">
+      <c r="A88" s="24" t="s">
+        <v>133</v>
       </c>
       <c r="B88" s="10">
         <v>5</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D88" s="11"/>
     </row>
-    <row r="89" ht="69" spans="1:4">
-      <c r="A89" s="25"/>
+    <row r="89" ht="52.5" spans="1:4">
+      <c r="A89" s="24"/>
       <c r="B89" s="10">
         <v>6</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="90" ht="31.5" spans="1:4">
-      <c r="A90" s="25"/>
-      <c r="B90" s="22">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="90" ht="25.5" spans="1:4">
+      <c r="A90" s="24"/>
+      <c r="B90" s="21">
         <v>5</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="91" ht="47.25" spans="1:4">
-      <c r="A91" s="25"/>
-      <c r="B91" s="22">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="91" ht="38.25" spans="1:4">
+      <c r="A91" s="24"/>
+      <c r="B91" s="21">
         <v>5</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="92" ht="122.25" spans="1:4">
-      <c r="A92" s="25"/>
-      <c r="B92" s="22">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="92" ht="92.25" spans="1:4">
+      <c r="A92" s="24"/>
+      <c r="B92" s="21">
         <v>5</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="93" ht="122.25" spans="1:4">
-      <c r="A93" s="25"/>
-      <c r="B93" s="22">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="93" ht="92.25" spans="1:4">
+      <c r="A93" s="24"/>
+      <c r="B93" s="21">
         <v>5</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="94" ht="203.25" spans="1:4">
-      <c r="A94" s="25"/>
-      <c r="B94" s="22">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="94" ht="147.75" spans="1:4">
+      <c r="A94" s="24"/>
+      <c r="B94" s="21">
         <v>5</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="95" ht="72" spans="1:4">
-      <c r="A95" s="25"/>
-      <c r="B95" s="22">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="95" ht="53.25" spans="1:4">
+      <c r="A95" s="24"/>
+      <c r="B95" s="21">
         <v>5</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="96" ht="144" spans="1:4">
-      <c r="A96" s="25"/>
-      <c r="B96" s="22">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="96" ht="106.5" spans="1:4">
+      <c r="A96" s="24"/>
+      <c r="B96" s="21">
         <v>5</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="97" ht="31.5" spans="1:4">
-      <c r="A97" s="25"/>
-      <c r="B97" s="22">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="97" ht="25.5" spans="1:4">
+      <c r="A97" s="24"/>
+      <c r="B97" s="21">
         <v>5</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D97" s="11"/>
     </row>
-    <row r="98" ht="69" spans="1:4">
-      <c r="A98" s="25"/>
-      <c r="B98" s="22">
+    <row r="98" ht="52.5" spans="1:4">
+      <c r="A98" s="24"/>
+      <c r="B98" s="21">
         <v>5</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D98" s="11"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="25"/>
-      <c r="B99" s="22">
+      <c r="A99" s="24"/>
+      <c r="B99" s="21">
         <v>2</v>
       </c>
       <c r="C99" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D99" s="11"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="25"/>
-      <c r="B100" s="22">
+      <c r="A100" s="24"/>
+      <c r="B100" s="21">
         <v>5</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D100" s="11"/>
     </row>
-    <row r="101" ht="47.25" spans="1:4">
-      <c r="A101" s="25"/>
-      <c r="B101" s="22">
+    <row r="101" ht="38.25" spans="1:4">
+      <c r="A101" s="24"/>
+      <c r="B101" s="21">
         <v>2</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D101" s="11"/>
     </row>
-    <row r="102" ht="47.25" spans="1:4">
-      <c r="A102" s="25"/>
-      <c r="B102" s="22">
+    <row r="102" ht="38.25" spans="1:4">
+      <c r="A102" s="24"/>
+      <c r="B102" s="21">
         <v>5</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D102" s="11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="103" ht="63" spans="1:4">
-      <c r="A103" s="25"/>
-      <c r="B103" s="22">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="103" ht="51" spans="1:4">
+      <c r="A103" s="24"/>
+      <c r="B103" s="21">
         <v>5</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D103" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="104" ht="188.25" spans="1:5">
-      <c r="A104" s="25"/>
-      <c r="B104" s="22">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="104" ht="144" spans="1:5">
+      <c r="A104" s="24"/>
+      <c r="B104" s="21">
         <v>5</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D104" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="E104" s="28" t="s">
-        <v>158</v>
+        <v>161</v>
+      </c>
+      <c r="E104" s="27" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="105" ht="155" customHeight="1" spans="1:5">
-      <c r="A105" s="25"/>
-      <c r="B105" s="22">
+      <c r="A105" s="24"/>
+      <c r="B105" s="21">
         <v>5</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="106" ht="56.25" spans="1:4">
-      <c r="A106" s="25"/>
-      <c r="B106" s="22">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="106" ht="40.5" spans="1:4">
+      <c r="A106" s="24"/>
+      <c r="B106" s="21">
         <v>5</v>
       </c>
       <c r="C106" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="D106" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="107" ht="40.5" spans="1:4">
+      <c r="A107" s="24"/>
+      <c r="B107" s="21">
+        <v>5</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="D107" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="108" ht="120.75" spans="1:4">
+      <c r="A108" s="24"/>
+      <c r="B108" s="21">
+        <v>5</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D108" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="109" ht="54" spans="1:4">
+      <c r="A109" s="24"/>
+      <c r="B109" s="21">
+        <v>5</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D109" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="110" ht="40.5" spans="1:4">
+      <c r="A110" s="24"/>
+      <c r="B110" s="21">
+        <v>5</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D110" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="111" ht="27" spans="1:4">
+      <c r="A111" s="24"/>
+      <c r="B111" s="21">
+        <v>5</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D111" s="11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="112" ht="25.5" spans="1:4">
+      <c r="A112" s="24"/>
+      <c r="B112" s="21">
+        <v>2</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D112" s="11"/>
+    </row>
+    <row r="113" ht="51" spans="1:4">
+      <c r="A113" s="24"/>
+      <c r="B113" s="21">
+        <v>2</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D113" s="11"/>
+    </row>
+    <row r="114" ht="38.25" spans="1:4">
+      <c r="A114" s="24"/>
+      <c r="B114" s="21">
+        <v>2</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D114" s="11"/>
+    </row>
+    <row r="115" ht="39" spans="1:4">
+      <c r="A115" s="24"/>
+      <c r="B115" s="21">
+        <v>2</v>
+      </c>
+      <c r="C115" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="D115" s="11"/>
+    </row>
+    <row r="116" ht="25.5" spans="1:4">
+      <c r="A116" s="24"/>
+      <c r="B116" s="21">
+        <v>2</v>
+      </c>
+      <c r="C116" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="D116" s="11"/>
+    </row>
+    <row r="117" ht="66.75" spans="1:4">
+      <c r="A117" s="24"/>
+      <c r="B117" s="21">
+        <v>5</v>
+      </c>
+      <c r="C117" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="D117" s="11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="118" ht="26.25" spans="1:4">
+      <c r="A118" s="24"/>
+      <c r="B118" s="21">
+        <v>2</v>
+      </c>
+      <c r="C118" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="D118" s="11"/>
+    </row>
+    <row r="119" ht="66.75" spans="1:4">
+      <c r="A119" s="24"/>
+      <c r="B119" s="21">
+        <v>5</v>
+      </c>
+      <c r="C119" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D119" s="11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="120" ht="38.25" spans="1:4">
+      <c r="A120" s="24"/>
+      <c r="B120" s="21">
+        <v>2</v>
+      </c>
+      <c r="C120" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="D120" s="25"/>
+    </row>
+    <row r="121" ht="78.75" spans="1:4">
+      <c r="A121" s="24"/>
+      <c r="B121" s="21">
+        <v>5</v>
+      </c>
+      <c r="C121" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="D121" s="25" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="122" ht="39.75" spans="1:4">
+      <c r="A122" s="24"/>
+      <c r="B122" s="21">
+        <v>5</v>
+      </c>
+      <c r="C122" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="D122" s="25"/>
+    </row>
+    <row r="123" ht="52.5" spans="1:4">
+      <c r="A123" s="24"/>
+      <c r="B123" s="21">
+        <v>2</v>
+      </c>
+      <c r="C123" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="D123" s="25"/>
+    </row>
+    <row r="124" ht="25.5" spans="1:4">
+      <c r="A124" s="24"/>
+      <c r="B124" s="21">
+        <v>2</v>
+      </c>
+      <c r="C124" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="D124" s="25"/>
+    </row>
+    <row r="125" ht="38.25" spans="1:4">
+      <c r="A125" s="24"/>
+      <c r="B125" s="21">
+        <v>5</v>
+      </c>
+      <c r="C125" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="D125" s="25"/>
+    </row>
+    <row r="126" ht="92.25" spans="1:4">
+      <c r="A126" s="24"/>
+      <c r="B126" s="21">
+        <v>5</v>
+      </c>
+      <c r="C126" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D126" s="25" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="127" ht="27" spans="1:4">
+      <c r="A127" s="24"/>
+      <c r="B127" s="21">
+        <v>5</v>
+      </c>
+      <c r="C127" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="D127" s="25" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="128" ht="38.25" spans="1:4">
+      <c r="A128" s="24"/>
+      <c r="B128" s="21">
+        <v>5</v>
+      </c>
+      <c r="C128" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D128" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="129" ht="53.25" spans="1:4">
+      <c r="A129" s="24"/>
+      <c r="B129" s="21">
+        <v>5</v>
+      </c>
+      <c r="C129" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="D129" s="11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="130" ht="105.75" spans="1:4">
+      <c r="A130" s="24"/>
+      <c r="B130" s="21">
+        <v>5</v>
+      </c>
+      <c r="C130" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="D130" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="131" ht="31" customHeight="1" spans="1:5">
+      <c r="A131" s="24"/>
+      <c r="B131" s="29">
+        <v>1</v>
+      </c>
+      <c r="C131" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D131" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="132" ht="39" spans="1:4">
+      <c r="A132" s="24"/>
+      <c r="B132" s="29">
+        <v>2</v>
+      </c>
+      <c r="C132" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D132" s="12"/>
+    </row>
+    <row r="133" ht="40.5" spans="1:4">
+      <c r="A133" s="24"/>
+      <c r="B133" s="29">
+        <v>5</v>
+      </c>
+      <c r="C133" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D133" s="12" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="134" ht="54" spans="1:4">
+      <c r="A134" s="24"/>
+      <c r="B134" s="29">
+        <v>5</v>
+      </c>
+      <c r="C134" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="D134" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="135" ht="51.75" spans="1:4">
+      <c r="A135" s="24"/>
+      <c r="B135" s="29">
+        <v>1</v>
+      </c>
+      <c r="C135" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="D135" s="12"/>
+    </row>
+    <row r="136" ht="25.5" spans="1:4">
+      <c r="A136" s="24"/>
+      <c r="B136" s="29">
+        <v>1</v>
+      </c>
+      <c r="C136" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="D136" s="12" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="137" ht="38.25" spans="1:4">
+      <c r="A137" s="24"/>
+      <c r="B137" s="29">
+        <v>1</v>
+      </c>
+      <c r="C137" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="D137" s="12"/>
+    </row>
+    <row r="138" ht="51" spans="1:4">
+      <c r="A138" s="24"/>
+      <c r="B138" s="29">
+        <v>1</v>
+      </c>
+      <c r="C138" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="D138" s="12"/>
+    </row>
+    <row r="139" ht="51" spans="1:4">
+      <c r="A139" s="24"/>
+      <c r="B139" s="29">
+        <v>1</v>
+      </c>
+      <c r="C139" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="D139" s="12"/>
+    </row>
+    <row r="140" ht="25.5" spans="1:4">
+      <c r="A140" s="24"/>
+      <c r="B140" s="29">
+        <v>1</v>
+      </c>
+      <c r="C140" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="D140" s="12"/>
+    </row>
+    <row r="141" ht="144.75" spans="1:5">
+      <c r="A141" s="24"/>
+      <c r="B141" s="29">
+        <v>5</v>
+      </c>
+      <c r="C141" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="D141" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="E141" t="s">
         <v>162</v>
       </c>
-      <c r="D106" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="107" ht="56.25" spans="1:4">
-      <c r="A107" s="25"/>
-      <c r="B107" s="22">
-        <v>5</v>
-      </c>
-      <c r="C107" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="D107" s="11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="108" ht="165.75" spans="1:4">
-      <c r="A108" s="25"/>
-      <c r="B108" s="22">
-        <v>5</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D108" s="11" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="109" ht="75" spans="1:4">
-      <c r="A109" s="25"/>
-      <c r="B109" s="22">
-        <v>5</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D109" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="110" ht="56.25" spans="1:4">
-      <c r="A110" s="25"/>
-      <c r="B110" s="22">
-        <v>5</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D110" s="11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="111" ht="37.5" spans="1:4">
-      <c r="A111" s="25"/>
-      <c r="B111" s="22">
-        <v>5</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D111" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="112" ht="31.5" spans="1:4">
-      <c r="A112" s="25"/>
-      <c r="B112" s="22">
-        <v>2</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D112" s="11"/>
-    </row>
-    <row r="113" ht="63" spans="1:4">
-      <c r="A113" s="25"/>
-      <c r="B113" s="22">
-        <v>2</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D113" s="11"/>
-    </row>
-    <row r="114" ht="47.25" spans="1:4">
-      <c r="A114" s="25"/>
-      <c r="B114" s="22">
-        <v>2</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D114" s="11"/>
-    </row>
-    <row r="115" ht="50.25" spans="1:4">
-      <c r="A115" s="25"/>
-      <c r="B115" s="22">
-        <v>2</v>
-      </c>
-      <c r="C115" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="D115" s="11"/>
-    </row>
-    <row r="116" ht="31.5" spans="1:4">
-      <c r="A116" s="25"/>
-      <c r="B116" s="22">
-        <v>2</v>
-      </c>
-      <c r="C116" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="D116" s="11"/>
-    </row>
-    <row r="117" ht="90.75" spans="1:4">
-      <c r="A117" s="25"/>
-      <c r="B117" s="22">
-        <v>5</v>
-      </c>
-      <c r="C117" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="D117" s="11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="118" ht="34.5" spans="1:4">
-      <c r="A118" s="25"/>
-      <c r="B118" s="22">
-        <v>2</v>
-      </c>
-      <c r="C118" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="D118" s="11"/>
-    </row>
-    <row r="119" ht="90.75" spans="1:4">
-      <c r="A119" s="25"/>
-      <c r="B119" s="22">
-        <v>5</v>
-      </c>
-      <c r="C119" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="D119" s="11" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="120" ht="47.25" spans="1:4">
-      <c r="A120" s="25"/>
-      <c r="B120" s="22">
-        <v>2</v>
-      </c>
-      <c r="C120" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="D120" s="26"/>
-    </row>
-    <row r="121" ht="103.5" spans="1:4">
-      <c r="A121" s="25"/>
-      <c r="B121" s="22">
-        <v>5</v>
-      </c>
-      <c r="C121" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="D121" s="26" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="122" ht="53.25" spans="1:4">
-      <c r="A122" s="25"/>
-      <c r="B122" s="22">
-        <v>5</v>
-      </c>
-      <c r="C122" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D122" s="26"/>
-    </row>
-    <row r="123" ht="69" spans="1:4">
-      <c r="A123" s="25"/>
-      <c r="B123" s="22">
-        <v>2</v>
-      </c>
-      <c r="C123" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="D123" s="26"/>
-    </row>
-    <row r="124" ht="31.5" spans="1:4">
-      <c r="A124" s="25"/>
-      <c r="B124" s="22">
-        <v>2</v>
-      </c>
-      <c r="C124" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="D124" s="26"/>
-    </row>
-    <row r="125" ht="47.25" spans="1:4">
-      <c r="A125" s="25"/>
-      <c r="B125" s="22">
-        <v>5</v>
-      </c>
-      <c r="C125" s="27" t="s">
-        <v>190</v>
-      </c>
-      <c r="D125" s="26"/>
-    </row>
-    <row r="126" ht="122.25" spans="1:4">
-      <c r="A126" s="25"/>
-      <c r="B126" s="22">
-        <v>5</v>
-      </c>
-      <c r="C126" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="D126" s="26" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="127" ht="37.5" spans="1:4">
-      <c r="A127" s="25"/>
-      <c r="B127" s="22">
-        <v>5</v>
-      </c>
-      <c r="C127" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="D127" s="26" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="128" ht="47.25" spans="1:4">
-      <c r="A128" s="25"/>
-      <c r="B128" s="22">
-        <v>5</v>
-      </c>
-      <c r="C128" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="D128" s="11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="129" ht="72" spans="1:4">
-      <c r="A129" s="25"/>
-      <c r="B129" s="22">
-        <v>5</v>
-      </c>
-      <c r="C129" s="29" t="s">
-        <v>197</v>
-      </c>
-      <c r="D129" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="130" ht="141" spans="1:4">
-      <c r="A130" s="25"/>
-      <c r="B130" s="22">
-        <v>5</v>
-      </c>
-      <c r="C130" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="D130" s="11" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="131" ht="31" customHeight="1" spans="1:5">
-      <c r="A131" s="25"/>
-      <c r="B131" s="30">
+    </row>
+    <row r="142" ht="38.25" spans="1:4">
+      <c r="A142" s="24"/>
+      <c r="B142" s="29">
         <v>1</v>
       </c>
-      <c r="C131" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="D131" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="E131" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="132" ht="50.25" spans="1:4">
-      <c r="A132" s="25"/>
-      <c r="B132" s="30">
-        <v>2</v>
-      </c>
-      <c r="C132" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="D132" s="12"/>
-    </row>
-    <row r="133" ht="56.25" spans="1:4">
-      <c r="A133" s="25"/>
-      <c r="B133" s="30">
-        <v>5</v>
-      </c>
-      <c r="C133" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="D133" s="12" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="134" ht="75" spans="1:4">
-      <c r="A134" s="25"/>
-      <c r="B134" s="30">
-        <v>5</v>
-      </c>
-      <c r="C134" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="D134" s="12" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="135" ht="66" spans="1:4">
-      <c r="A135" s="25"/>
-      <c r="B135" s="30">
+      <c r="C142" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D142" s="12"/>
+    </row>
+    <row r="143" ht="38.25" spans="1:4">
+      <c r="A143" s="24"/>
+      <c r="B143" s="29">
         <v>1</v>
       </c>
-      <c r="C135" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="D135" s="12"/>
-    </row>
-    <row r="136" ht="31.5" spans="1:4">
-      <c r="A136" s="25"/>
-      <c r="B136" s="30">
+      <c r="C143" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="D143" s="12"/>
+    </row>
+    <row r="144" ht="38.25" spans="1:5">
+      <c r="A144" s="24"/>
+      <c r="B144" s="17">
+        <v>5</v>
+      </c>
+      <c r="C144" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="D144" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="E144" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="145" ht="105.75" spans="1:5">
+      <c r="A145" s="24"/>
+      <c r="B145" s="29">
+        <v>5</v>
+      </c>
+      <c r="C145" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D145" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="E145" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="146" ht="25.5" spans="1:4">
+      <c r="A146" s="24"/>
+      <c r="B146" s="29">
         <v>1</v>
       </c>
-      <c r="C136" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="D136" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="137" ht="47.25" spans="1:4">
-      <c r="A137" s="25"/>
-      <c r="B137" s="30">
-        <v>1</v>
-      </c>
-      <c r="C137" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="D137" s="12"/>
-    </row>
-    <row r="138" ht="63" spans="1:4">
-      <c r="A138" s="25"/>
-      <c r="B138" s="30">
-        <v>1</v>
-      </c>
-      <c r="C138" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="D138" s="12"/>
-    </row>
-    <row r="139" ht="63" spans="1:4">
-      <c r="A139" s="25"/>
-      <c r="B139" s="30">
-        <v>1</v>
-      </c>
-      <c r="C139" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="D139" s="12"/>
-    </row>
-    <row r="140" ht="31.5" spans="1:4">
-      <c r="A140" s="25"/>
-      <c r="B140" s="30">
-        <v>1</v>
-      </c>
-      <c r="C140" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="D140" s="12"/>
-    </row>
-    <row r="141" ht="191.25" spans="1:5">
-      <c r="A141" s="25"/>
-      <c r="B141" s="30">
-        <v>5</v>
-      </c>
-      <c r="C141" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="D141" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="E141" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="142" ht="47.25" spans="1:4">
-      <c r="A142" s="25"/>
-      <c r="B142" s="30">
-        <v>1</v>
-      </c>
-      <c r="C142" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="D142" s="12"/>
-    </row>
-    <row r="143" ht="47.25" spans="1:4">
-      <c r="A143" s="25"/>
-      <c r="B143" s="30">
-        <v>1</v>
-      </c>
-      <c r="C143" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="D143" s="12"/>
-    </row>
-    <row r="144" ht="47.25" spans="1:5">
-      <c r="A144" s="25"/>
-      <c r="B144" s="17">
-        <v>5</v>
-      </c>
-      <c r="C144" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="D144" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="E144" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="145" ht="141" spans="1:5">
-      <c r="A145" s="25"/>
-      <c r="B145" s="30">
-        <v>5</v>
-      </c>
-      <c r="C145" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="D145" s="31" t="s">
-        <v>222</v>
-      </c>
-      <c r="E145" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="146" ht="31.5" spans="1:4">
-      <c r="A146" s="25"/>
-      <c r="B146" s="30">
-        <v>1</v>
-      </c>
       <c r="C146" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="D146" s="31"/>
+        <v>227</v>
+      </c>
+      <c r="D146" s="30"/>
     </row>
     <row r="147" ht="207" customHeight="1" spans="1:5">
-      <c r="A147" s="25"/>
-      <c r="B147" s="30">
+      <c r="A147" s="24"/>
+      <c r="B147" s="29">
         <v>5</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="D147" s="31" t="s">
-        <v>225</v>
+        <v>228</v>
+      </c>
+      <c r="D147" s="30" t="s">
+        <v>229</v>
       </c>
       <c r="E147" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="148" ht="47.25" spans="1:5">
-      <c r="A148" s="25"/>
-      <c r="B148" s="30">
+    <row r="148" ht="38.25" spans="1:5">
+      <c r="A148" s="24"/>
+      <c r="B148" s="29">
         <v>2</v>
       </c>
       <c r="C148" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="D148" s="31"/>
+        <v>230</v>
+      </c>
+      <c r="D148" s="30"/>
       <c r="E148" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="149" ht="159.75" spans="1:5">
-      <c r="A149" s="25"/>
-      <c r="B149" s="30">
+    <row r="149" ht="119.25" spans="1:5">
+      <c r="A149" s="24"/>
+      <c r="B149" s="29">
         <v>5</v>
       </c>
       <c r="C149" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D149" s="31" t="s">
-        <v>228</v>
+        <v>231</v>
+      </c>
+      <c r="D149" s="30" t="s">
+        <v>232</v>
       </c>
       <c r="E149" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="150" ht="31.5" spans="1:5">
-      <c r="A150" s="25"/>
-      <c r="B150" s="30">
+    <row r="150" ht="25.5" spans="1:5">
+      <c r="A150" s="24"/>
+      <c r="B150" s="29">
         <v>1</v>
       </c>
       <c r="C150" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="D150" s="31"/>
+        <v>233</v>
+      </c>
+      <c r="D150" s="30"/>
       <c r="E150" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="151" ht="87.75" spans="1:5">
-      <c r="A151" s="25"/>
-      <c r="B151" s="30">
+    <row r="151" ht="66" spans="1:5">
+      <c r="A151" s="24"/>
+      <c r="B151" s="29">
         <v>5</v>
       </c>
       <c r="C151" s="12" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="D151" s="11" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="E151" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="152" ht="81" customHeight="1" spans="1:4">
-      <c r="A152" s="25"/>
-      <c r="B152" s="30">
-        <v>5</v>
-      </c>
-      <c r="C152" s="32" t="s">
-        <v>232</v>
-      </c>
-      <c r="D152" s="31" t="s">
-        <v>233</v>
+      <c r="A152" s="24"/>
+      <c r="B152" s="29">
+        <v>5</v>
+      </c>
+      <c r="C152" s="31" t="s">
+        <v>236</v>
+      </c>
+      <c r="D152" s="30" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="153" ht="42" customHeight="1" spans="1:4">
-      <c r="A153" s="25"/>
-      <c r="B153" s="30"/>
-      <c r="C153" s="32" t="s">
-        <v>234</v>
-      </c>
-      <c r="D153" s="31" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="154" ht="31.5" spans="1:5">
-      <c r="A154" s="25"/>
-      <c r="B154" s="30"/>
+      <c r="A153" s="24"/>
+      <c r="B153" s="29"/>
+      <c r="C153" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="D153" s="30" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="154" ht="25.5" spans="1:5">
+      <c r="A154" s="24"/>
+      <c r="B154" s="29"/>
       <c r="C154" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="D154" s="31"/>
+        <v>240</v>
+      </c>
+      <c r="D154" s="30"/>
       <c r="E154" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="155" ht="47.25" spans="1:4">
-      <c r="A155" s="25"/>
-      <c r="B155" s="30"/>
+    <row r="155" ht="38.25" spans="1:4">
+      <c r="A155" s="24"/>
+      <c r="B155" s="29"/>
       <c r="C155" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="D155" s="31"/>
-    </row>
-    <row r="156" ht="47.25" spans="1:4">
-      <c r="A156" s="25"/>
-      <c r="B156" s="30"/>
+        <v>241</v>
+      </c>
+      <c r="D155" s="30"/>
+    </row>
+    <row r="156" ht="38.25" spans="1:4">
+      <c r="A156" s="24"/>
+      <c r="B156" s="29"/>
       <c r="C156" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="D156" s="31"/>
-    </row>
-    <row r="157" ht="47.25" spans="1:4">
-      <c r="A157" s="25"/>
-      <c r="B157" s="30"/>
+        <v>242</v>
+      </c>
+      <c r="D156" s="30"/>
+    </row>
+    <row r="157" ht="38.25" spans="1:4">
+      <c r="A157" s="24"/>
+      <c r="B157" s="29"/>
       <c r="C157" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="D157" s="31"/>
-    </row>
-    <row r="158" ht="47.25" spans="1:4">
-      <c r="A158" s="25"/>
-      <c r="B158" s="30"/>
+        <v>243</v>
+      </c>
+      <c r="D157" s="30"/>
+    </row>
+    <row r="158" ht="38.25" spans="1:4">
+      <c r="A158" s="24"/>
+      <c r="B158" s="29"/>
       <c r="C158" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="D158" s="31"/>
-    </row>
-    <row r="159" ht="75" spans="1:4">
-      <c r="A159" s="25"/>
-      <c r="B159" s="30">
-        <v>5</v>
-      </c>
-      <c r="C159" s="32" t="s">
-        <v>241</v>
-      </c>
-      <c r="D159" s="31" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="160" ht="47.25" spans="1:4">
-      <c r="A160" s="25"/>
-      <c r="B160" s="30"/>
+        <v>244</v>
+      </c>
+      <c r="D158" s="30"/>
+    </row>
+    <row r="159" ht="54" spans="1:4">
+      <c r="A159" s="24"/>
+      <c r="B159" s="29">
+        <v>5</v>
+      </c>
+      <c r="C159" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="D159" s="30" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="160" ht="38.25" spans="1:4">
+      <c r="A160" s="24"/>
+      <c r="B160" s="29"/>
       <c r="C160" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="D160" s="31"/>
-    </row>
-    <row r="161" ht="37.5" spans="1:5">
-      <c r="A161" s="25"/>
-      <c r="B161" s="30">
-        <v>5</v>
-      </c>
-      <c r="C161" s="32" t="s">
-        <v>244</v>
-      </c>
-      <c r="D161" s="31" t="s">
-        <v>245</v>
+        <v>247</v>
+      </c>
+      <c r="D160" s="30"/>
+    </row>
+    <row r="161" ht="27" spans="1:5">
+      <c r="A161" s="24"/>
+      <c r="B161" s="29">
+        <v>5</v>
+      </c>
+      <c r="C161" s="31" t="s">
+        <v>248</v>
+      </c>
+      <c r="D161" s="30" t="s">
+        <v>249</v>
       </c>
       <c r="E161" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="162" ht="47.25" spans="1:4">
-      <c r="A162" s="25"/>
-      <c r="B162" s="30"/>
+    <row r="162" ht="38.25" spans="1:4">
+      <c r="A162" s="24"/>
+      <c r="B162" s="29"/>
       <c r="C162" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="D162" s="31"/>
-    </row>
-    <row r="163" ht="93.75" spans="1:4">
-      <c r="A163" s="25"/>
-      <c r="B163" s="30">
+        <v>250</v>
+      </c>
+      <c r="D162" s="30"/>
+    </row>
+    <row r="163" ht="67.5" spans="1:4">
+      <c r="A163" s="24"/>
+      <c r="B163" s="29">
         <v>5</v>
       </c>
       <c r="C163" s="12" t="s">
-        <v>247</v>
-      </c>
-      <c r="D163" s="31" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="164" ht="222" spans="1:4">
-      <c r="A164" s="25"/>
-      <c r="B164" s="30">
+        <v>251</v>
+      </c>
+      <c r="D163" s="30" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="164" ht="161.25" spans="1:4">
+      <c r="A164" s="24"/>
+      <c r="B164" s="29">
         <v>5</v>
       </c>
       <c r="C164" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="D164" s="31" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="165" ht="168.75" spans="1:4">
-      <c r="A165" s="25"/>
-      <c r="B165" s="30">
+        <v>253</v>
+      </c>
+      <c r="D164" s="30" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="165" ht="121.5" spans="1:4">
+      <c r="A165" s="24"/>
+      <c r="B165" s="29">
         <v>5</v>
       </c>
       <c r="C165" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="D165" s="31" t="s">
-        <v>252</v>
+        <v>255</v>
+      </c>
+      <c r="D165" s="30" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="166" spans="1:4">
-      <c r="A166" s="25"/>
-      <c r="B166" s="30"/>
+      <c r="A166" s="24"/>
+      <c r="B166" s="29"/>
       <c r="C166" s="12"/>
-      <c r="D166" s="31"/>
+      <c r="D166" s="30"/>
     </row>
     <row r="167" spans="1:4">
-      <c r="A167" s="25"/>
-      <c r="B167" s="30"/>
+      <c r="A167" s="24"/>
+      <c r="B167" s="29"/>
       <c r="C167" s="12"/>
-      <c r="D167" s="31"/>
-    </row>
-    <row r="168" ht="144" spans="1:4">
-      <c r="A168" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="B168" s="30">
+      <c r="D167" s="30"/>
+    </row>
+    <row r="168" ht="106.5" spans="1:4">
+      <c r="A168" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="B168" s="29">
         <v>5</v>
       </c>
       <c r="C168" s="12" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="D168" s="11" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="169" ht="47.25" spans="1:4">
-      <c r="A169" s="33"/>
-      <c r="B169" s="30">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="169" ht="38.25" spans="1:4">
+      <c r="A169" s="32"/>
+      <c r="B169" s="29">
         <v>1</v>
       </c>
       <c r="C169" s="12" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="D169" s="11"/>
     </row>
-    <row r="170" ht="31.5" spans="1:4">
-      <c r="A170" s="33"/>
-      <c r="B170" s="30">
+    <row r="170" ht="25.5" spans="1:4">
+      <c r="A170" s="32"/>
+      <c r="B170" s="29">
         <v>1</v>
       </c>
       <c r="C170" s="12" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="D170" s="12"/>
     </row>
-    <row r="171" ht="31.5" spans="1:4">
-      <c r="A171" s="33"/>
-      <c r="B171" s="22">
+    <row r="171" ht="25.5" spans="1:4">
+      <c r="A171" s="32"/>
+      <c r="B171" s="21">
         <v>1</v>
       </c>
       <c r="C171" s="19" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D171" s="11"/>
     </row>
-    <row r="172" ht="56.25" spans="1:4">
-      <c r="A172" s="33"/>
-      <c r="B172" s="22">
+    <row r="172" ht="40.5" spans="1:4">
+      <c r="A172" s="32"/>
+      <c r="B172" s="21">
         <v>5</v>
       </c>
       <c r="C172" s="12" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="D172" s="8" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="173" ht="47.25" spans="1:4">
-      <c r="A173" s="33"/>
-      <c r="B173" s="22">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="173" ht="38.25" spans="1:4">
+      <c r="A173" s="32"/>
+      <c r="B173" s="21">
         <v>1</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="D173" s="11"/>
     </row>
-    <row r="174" ht="47.25" spans="1:4">
-      <c r="A174" s="33"/>
-      <c r="B174" s="22">
+    <row r="174" ht="38.25" spans="1:4">
+      <c r="A174" s="32"/>
+      <c r="B174" s="21">
         <v>1</v>
       </c>
       <c r="C174" s="12" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="D174" s="11"/>
     </row>
-    <row r="175" ht="53.25" spans="1:4">
-      <c r="A175" s="33"/>
-      <c r="B175" s="22">
+    <row r="175" ht="39.75" spans="1:4">
+      <c r="A175" s="32"/>
+      <c r="B175" s="21">
         <v>5</v>
       </c>
       <c r="C175" s="11" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D175" s="11" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="176" ht="235" customHeight="1" spans="1:4">
-      <c r="A176" s="33"/>
-      <c r="B176" s="22">
+      <c r="A176" s="32"/>
+      <c r="B176" s="21">
         <v>5</v>
       </c>
       <c r="C176" s="12" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D176" s="11" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="177" ht="208" customHeight="1" spans="1:5">
-      <c r="A177" s="33"/>
-      <c r="B177" s="22">
+      <c r="A177" s="32"/>
+      <c r="B177" s="21">
         <v>5</v>
       </c>
       <c r="C177" s="12" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="D177" s="11" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="E177" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="178" ht="38" customHeight="1" spans="1:3">
-      <c r="A178" s="33"/>
-      <c r="B178" s="22">
+      <c r="A178" s="32"/>
+      <c r="B178" s="21">
         <v>1</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="179" ht="38" customHeight="1" spans="1:4">
-      <c r="A179" s="33"/>
-      <c r="B179" s="22">
+      <c r="A179" s="32"/>
+      <c r="B179" s="21">
         <v>1</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="D179" s="11"/>
     </row>
     <row r="180" ht="51" customHeight="1" spans="1:4">
-      <c r="A180" s="33"/>
-      <c r="B180" s="22">
+      <c r="A180" s="32"/>
+      <c r="B180" s="21">
         <v>1</v>
       </c>
       <c r="C180" s="12" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="181" ht="28" customHeight="1" spans="1:4">
-      <c r="A181" s="33"/>
-      <c r="B181" s="22"/>
+      <c r="A181" s="32"/>
+      <c r="B181" s="21"/>
       <c r="C181" s="12"/>
       <c r="D181" s="11"/>
     </row>
     <row r="182" ht="34" customHeight="1" spans="1:4">
-      <c r="A182" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="B182" s="22">
+      <c r="A182" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="B182" s="21">
         <v>2</v>
       </c>
       <c r="C182" s="12" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="D182" s="11" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="183" ht="58" customHeight="1" spans="1:4">
-      <c r="A183" s="33"/>
-      <c r="B183" s="30">
+      <c r="A183" s="32"/>
+      <c r="B183" s="29">
         <v>1</v>
       </c>
       <c r="C183" s="12" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="D183" s="11"/>
     </row>
     <row r="184" ht="39" customHeight="1" spans="1:4">
-      <c r="A184" s="33"/>
-      <c r="B184" s="22">
+      <c r="A184" s="32"/>
+      <c r="B184" s="21">
         <v>2</v>
       </c>
       <c r="C184" s="12" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D184" s="11"/>
     </row>
     <row r="185" ht="28" customHeight="1" spans="1:4">
-      <c r="A185" s="33"/>
-      <c r="B185" s="22"/>
+      <c r="A185" s="32"/>
+      <c r="B185" s="21"/>
       <c r="C185" s="12"/>
       <c r="D185" s="11"/>
     </row>
     <row r="186" ht="28" customHeight="1" spans="1:4">
-      <c r="A186" s="33"/>
-      <c r="B186" s="22"/>
+      <c r="A186" s="32"/>
+      <c r="B186" s="21"/>
       <c r="C186" s="12"/>
       <c r="D186" s="11"/>
     </row>
     <row r="187" ht="28" customHeight="1" spans="1:4">
-      <c r="A187" s="33"/>
-      <c r="B187" s="22"/>
+      <c r="A187" s="32"/>
+      <c r="B187" s="21"/>
       <c r="C187" s="12"/>
       <c r="D187" s="11"/>
     </row>
     <row r="188" ht="28" customHeight="1" spans="1:4">
-      <c r="A188" s="33"/>
-      <c r="B188" s="22"/>
+      <c r="A188" s="32"/>
+      <c r="B188" s="21"/>
       <c r="C188" s="12"/>
       <c r="D188" s="11"/>
     </row>
     <row r="189" ht="28" customHeight="1" spans="1:4">
-      <c r="A189" s="33"/>
-      <c r="B189" s="22"/>
+      <c r="A189" s="32"/>
+      <c r="B189" s="21"/>
       <c r="C189" s="12"/>
       <c r="D189" s="11"/>
     </row>
     <row r="190" ht="28" customHeight="1" spans="1:4">
-      <c r="A190" s="33"/>
-      <c r="B190" s="22"/>
+      <c r="A190" s="32"/>
+      <c r="B190" s="21"/>
       <c r="C190" s="12"/>
       <c r="D190" s="11"/>
     </row>
     <row r="191" ht="28" customHeight="1" spans="1:4">
-      <c r="A191" s="33"/>
-      <c r="B191" s="22"/>
+      <c r="A191" s="32"/>
+      <c r="B191" s="21"/>
       <c r="C191" s="12"/>
       <c r="D191" s="11"/>
     </row>
     <row r="192" ht="28" customHeight="1" spans="1:4">
-      <c r="A192" s="33"/>
-      <c r="B192" s="22"/>
+      <c r="A192" s="32"/>
+      <c r="B192" s="21"/>
       <c r="C192" s="12"/>
       <c r="D192" s="11"/>
     </row>
-    <row r="193" ht="31.5" spans="1:4">
-      <c r="A193" s="33" t="s">
-        <v>278</v>
-      </c>
-      <c r="B193" s="22">
+    <row r="193" ht="25.5" spans="1:4">
+      <c r="A193" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="B193" s="21">
         <v>2</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="D193" s="11"/>
     </row>
-    <row r="194" ht="47.25" spans="1:4">
-      <c r="A194" s="33"/>
-      <c r="B194" s="22">
+    <row r="194" ht="38.25" spans="1:4">
+      <c r="A194" s="32"/>
+      <c r="B194" s="21">
         <v>1</v>
       </c>
       <c r="C194" s="12" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="D194" s="11"/>
     </row>
-    <row r="195" ht="31.5" spans="1:4">
-      <c r="A195" s="33"/>
-      <c r="B195" s="22">
+    <row r="195" ht="25.5" spans="1:4">
+      <c r="A195" s="32"/>
+      <c r="B195" s="21">
         <v>1</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D195" s="11"/>
     </row>
-    <row r="196" ht="31.5" spans="1:4">
-      <c r="A196" s="33"/>
-      <c r="B196" s="22">
+    <row r="196" ht="25.5" spans="1:4">
+      <c r="A196" s="32"/>
+      <c r="B196" s="21">
         <v>1</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="D196" s="11"/>
     </row>
-    <row r="197" ht="31.5" spans="1:4">
-      <c r="A197" s="33"/>
-      <c r="B197" s="22">
+    <row r="197" ht="25.5" spans="1:4">
+      <c r="A197" s="32"/>
+      <c r="B197" s="21">
         <v>1</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="D197" s="11"/>
     </row>
-    <row r="198" ht="31.5" spans="1:4">
-      <c r="A198" s="33"/>
-      <c r="B198" s="22">
+    <row r="198" ht="25.5" spans="1:4">
+      <c r="A198" s="32"/>
+      <c r="B198" s="21">
         <v>1</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D198" s="11"/>
     </row>
-    <row r="199" ht="31.5" spans="1:4">
-      <c r="A199" s="33"/>
-      <c r="B199" s="22">
+    <row r="199" ht="25.5" spans="1:4">
+      <c r="A199" s="32"/>
+      <c r="B199" s="21">
         <v>1</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="D199" s="11"/>
     </row>
-    <row r="200" ht="31.5" spans="1:4">
-      <c r="A200" s="33"/>
-      <c r="B200" s="22">
+    <row r="200" ht="25.5" spans="1:4">
+      <c r="A200" s="32"/>
+      <c r="B200" s="21">
         <v>1</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="D200" s="11"/>
     </row>
-    <row r="201" ht="47.25" spans="1:4">
-      <c r="A201" s="33"/>
-      <c r="B201" s="22">
+    <row r="201" ht="38.25" spans="1:4">
+      <c r="A201" s="32"/>
+      <c r="B201" s="21">
         <v>1</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="D201" s="11"/>
     </row>
-    <row r="202" ht="31.5" spans="1:4">
-      <c r="A202" s="33"/>
-      <c r="B202" s="22">
+    <row r="202" ht="25.5" spans="1:4">
+      <c r="A202" s="32"/>
+      <c r="B202" s="21">
         <v>1</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="D202" s="11"/>
     </row>
     <row r="203" spans="1:4">
-      <c r="A203" s="33"/>
-      <c r="B203" s="22">
+      <c r="A203" s="32"/>
+      <c r="B203" s="21">
         <v>1</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D203" s="11"/>
     </row>
-    <row r="204" ht="47.25" spans="1:4">
-      <c r="A204" s="33"/>
-      <c r="B204" s="22">
+    <row r="204" ht="38.25" spans="1:4">
+      <c r="A204" s="32"/>
+      <c r="B204" s="21">
         <v>1</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="D204" s="11"/>
     </row>
-    <row r="205" ht="47.25" spans="1:4">
-      <c r="A205" s="33"/>
-      <c r="B205" s="22">
+    <row r="205" ht="38.25" spans="1:4">
+      <c r="A205" s="32"/>
+      <c r="B205" s="21">
         <v>1</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D205" s="11"/>
     </row>
-    <row r="206" ht="112.5" spans="1:4">
-      <c r="A206" s="33"/>
-      <c r="B206" s="22">
+    <row r="206" ht="81" spans="1:4">
+      <c r="A206" s="32"/>
+      <c r="B206" s="21">
         <v>5</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="D206" s="11" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4">
-      <c r="A207" s="33"/>
-      <c r="B207" s="22"/>
-      <c r="D207" s="11"/>
-    </row>
-    <row r="208" ht="150" spans="1:4">
-      <c r="A208" s="33"/>
-      <c r="B208" s="22">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="207" ht="108" spans="1:4">
+      <c r="A207" s="32"/>
+      <c r="B207" s="21">
+        <v>5</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D207" s="11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="208" ht="66.75" spans="1:4">
+      <c r="A208" s="32"/>
+      <c r="B208" s="21">
         <v>5</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="D208" s="11" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="209" ht="90.75" spans="1:4">
-      <c r="A209" s="33"/>
-      <c r="B209" s="22">
-        <v>5</v>
-      </c>
-      <c r="C209" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D209" s="11" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="210" ht="197.25" spans="1:4">
-      <c r="A210" s="33"/>
-      <c r="B210" s="22">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="209" ht="146.25" spans="1:4">
+      <c r="A209" s="32"/>
+      <c r="B209" s="21">
+        <v>5</v>
+      </c>
+      <c r="C209" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="D209" s="33" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="210" ht="54" spans="1:4">
+      <c r="A210" s="32" t="s">
+        <v>304</v>
+      </c>
+      <c r="B210" s="21">
         <v>5</v>
       </c>
       <c r="C210" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="D210" s="34" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="211" ht="75" spans="1:4">
-      <c r="A211" s="33" t="s">
-        <v>300</v>
-      </c>
-      <c r="B211" s="22">
+        <v>305</v>
+      </c>
+      <c r="D210" s="33" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="211" ht="183" spans="1:4">
+      <c r="A211" s="32"/>
+      <c r="B211" s="21">
         <v>5</v>
       </c>
       <c r="C211" s="12" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
       <c r="D211" s="34" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="212" ht="238.5" spans="1:4">
-      <c r="A212" s="33"/>
-      <c r="B212" s="22">
-        <v>5</v>
-      </c>
-      <c r="C212" s="12" t="s">
-        <v>303</v>
-      </c>
-      <c r="D212" s="35" t="s">
-        <v>304</v>
-      </c>
+        <v>308</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
+      <c r="A212" s="32"/>
+      <c r="B212" s="21"/>
+      <c r="C212" s="12"/>
+      <c r="D212" s="33"/>
     </row>
     <row r="213" spans="1:4">
-      <c r="A213" s="33"/>
-      <c r="B213" s="22"/>
+      <c r="A213" s="32"/>
+      <c r="B213" s="21"/>
       <c r="C213" s="12"/>
-      <c r="D213" s="34"/>
+      <c r="D213" s="33"/>
     </row>
     <row r="214" spans="1:4">
-      <c r="A214" s="33"/>
-      <c r="B214" s="22"/>
+      <c r="A214" s="32"/>
+      <c r="B214" s="21"/>
       <c r="C214" s="12"/>
-      <c r="D214" s="34"/>
+      <c r="D214" s="33"/>
     </row>
     <row r="215" spans="1:4">
-      <c r="A215" s="33"/>
-      <c r="B215" s="22"/>
+      <c r="A215" s="32"/>
+      <c r="B215" s="21"/>
       <c r="C215" s="12"/>
-      <c r="D215" s="34"/>
+      <c r="D215" s="33"/>
     </row>
     <row r="216" spans="1:4">
-      <c r="A216" s="33"/>
-      <c r="B216" s="22"/>
+      <c r="A216" s="32"/>
+      <c r="B216" s="21"/>
       <c r="C216" s="12"/>
-      <c r="D216" s="34"/>
+      <c r="D216" s="33"/>
     </row>
     <row r="217" spans="1:4">
-      <c r="A217" s="33"/>
-      <c r="B217" s="22"/>
+      <c r="A217" s="32"/>
+      <c r="B217" s="21"/>
       <c r="C217" s="12"/>
-      <c r="D217" s="34"/>
-    </row>
-    <row r="218" spans="1:4">
-      <c r="A218" s="33"/>
-      <c r="B218" s="22"/>
-      <c r="C218" s="12"/>
-      <c r="D218" s="34"/>
-    </row>
-    <row r="219" ht="31.5" spans="1:4">
-      <c r="A219" s="33" t="s">
-        <v>305</v>
-      </c>
-      <c r="B219" s="22"/>
+      <c r="D217" s="33"/>
+    </row>
+    <row r="218" ht="25.5" spans="1:4">
+      <c r="A218" s="32" t="s">
+        <v>309</v>
+      </c>
+      <c r="B218" s="21"/>
+      <c r="C218" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="D218" s="33" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="219" ht="40.5" spans="1:4">
+      <c r="A219" s="32"/>
+      <c r="B219" s="21">
+        <v>5</v>
+      </c>
       <c r="C219" s="12" t="s">
-        <v>306</v>
-      </c>
-      <c r="D219" s="34" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="220" ht="56.25" spans="1:4">
-      <c r="A220" s="33"/>
-      <c r="B220" s="22">
+        <v>312</v>
+      </c>
+      <c r="D219" s="11" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="220" ht="38.25" spans="1:4">
+      <c r="A220" s="32"/>
+      <c r="B220" s="21">
         <v>5</v>
       </c>
       <c r="C220" s="12" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="D220" s="11" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="221" ht="47.25" spans="1:4">
-      <c r="A221" s="33"/>
-      <c r="B221" s="22">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="221" ht="109" customHeight="1" spans="1:4">
+      <c r="A221" s="32"/>
+      <c r="B221" s="21">
         <v>5</v>
       </c>
       <c r="C221" s="12" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="D221" s="11" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="222" spans="1:4">
-      <c r="A222" s="33"/>
-      <c r="B222" s="22">
-        <v>2</v>
-      </c>
-      <c r="C222" s="12" t="s">
-        <v>312</v>
-      </c>
-      <c r="D222" s="11"/>
-    </row>
-    <row r="223" ht="109" customHeight="1" spans="1:4">
-      <c r="A223" s="33"/>
-      <c r="B223" s="22">
-        <v>5</v>
-      </c>
-      <c r="C223" s="12" t="s">
-        <v>313</v>
-      </c>
-      <c r="D223" s="11" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="224" ht="42.75" spans="1:4">
-      <c r="A224" s="33"/>
-      <c r="B224" s="22">
-        <v>5</v>
-      </c>
-      <c r="C224" s="29" t="s">
-        <v>315</v>
-      </c>
-      <c r="D224" s="11" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="225" ht="56.25" spans="1:4">
-      <c r="A225" s="33" t="s">
         <v>317</v>
       </c>
-      <c r="B225" s="22">
-        <v>5</v>
-      </c>
-      <c r="C225" s="36" t="s">
+    </row>
+    <row r="222" ht="42.75" spans="1:4">
+      <c r="A222" s="32"/>
+      <c r="B222" s="21">
+        <v>5</v>
+      </c>
+      <c r="C222" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="D225" s="36" t="s">
+      <c r="D222" s="11" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="226" ht="67" customHeight="1" spans="1:4">
-      <c r="A226" s="33"/>
-      <c r="B226" s="22">
+    <row r="223" ht="40.5" spans="1:4">
+      <c r="A223" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="B223" s="21">
+        <v>5</v>
+      </c>
+      <c r="C223" s="35" t="s">
+        <v>321</v>
+      </c>
+      <c r="D223" s="35" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="224" ht="67" customHeight="1" spans="1:4">
+      <c r="A224" s="32"/>
+      <c r="B224" s="21">
+        <v>5</v>
+      </c>
+      <c r="C224" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="D224" s="12" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="225" ht="42" customHeight="1" spans="1:4">
+      <c r="A225" s="32"/>
+      <c r="B225" s="21">
+        <v>5</v>
+      </c>
+      <c r="C225" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="D225" s="12" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="226" ht="82" customHeight="1" spans="1:4">
+      <c r="A226" s="32"/>
+      <c r="B226" s="21">
         <v>5</v>
       </c>
       <c r="C226" s="12" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="D226" s="12" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="227" ht="42" customHeight="1" spans="1:4">
-      <c r="A227" s="33"/>
-      <c r="B227" s="22">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="227" ht="54" spans="1:4">
+      <c r="A227" s="32"/>
+      <c r="B227" s="29">
         <v>5</v>
       </c>
       <c r="C227" s="12" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="D227" s="12" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="228" ht="82" customHeight="1" spans="1:4">
-      <c r="A228" s="33"/>
-      <c r="B228" s="22">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="228" ht="25.5" spans="1:4">
+      <c r="A228" s="32"/>
+      <c r="B228" s="21">
         <v>5</v>
       </c>
       <c r="C228" s="12" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="D228" s="12" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="229" ht="75" spans="1:4">
-      <c r="A229" s="33"/>
-      <c r="B229" s="30">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="229" ht="220" customHeight="1" spans="1:4">
+      <c r="A229" s="32" t="s">
+        <v>333</v>
+      </c>
+      <c r="B229" s="21">
         <v>5</v>
       </c>
       <c r="C229" s="12" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="D229" s="12" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="230" ht="31.5" spans="1:4">
-      <c r="A230" s="33"/>
-      <c r="B230" s="22">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="230" ht="27" spans="1:4">
+      <c r="A230" s="32"/>
+      <c r="B230" s="21">
         <v>5</v>
       </c>
       <c r="C230" s="12" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="D230" s="12" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="231" ht="220" customHeight="1" spans="1:4">
-      <c r="A231" s="33" t="s">
-        <v>330</v>
-      </c>
-      <c r="B231" s="22">
-        <v>5</v>
-      </c>
-      <c r="C231" s="12" t="s">
-        <v>331</v>
-      </c>
-      <c r="D231" s="12" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="232" ht="37.5" spans="1:4">
-      <c r="A232" s="33"/>
-      <c r="B232" s="22">
-        <v>5</v>
-      </c>
-      <c r="C232" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="D232" s="12" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="233" ht="159.75" spans="1:4">
-      <c r="A233" s="33"/>
-      <c r="B233" s="22">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="231" ht="119.25" spans="1:4">
+      <c r="A231" s="32"/>
+      <c r="B231" s="21">
+        <v>5</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D231" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="232" ht="104.25" spans="1:4">
+      <c r="A232" s="32"/>
+      <c r="B232" s="21"/>
+      <c r="C232" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="D232" s="19" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="233" ht="64.5" spans="1:4">
+      <c r="A233" s="32"/>
+      <c r="B233" s="21">
         <v>5</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="234" ht="135" spans="1:4">
-      <c r="A234" s="33"/>
-      <c r="B234" s="22"/>
-      <c r="C234" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="D234" s="19" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="235" ht="81.75" spans="1:4">
-      <c r="A235" s="33"/>
-      <c r="B235" s="22">
-        <v>5</v>
-      </c>
-      <c r="C235" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="D235" s="2" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E235">
+  <autoFilter ref="E1:E233">
     <extLst/>
   </autoFilter>
   <mergeCells count="16">
@@ -5361,11 +5366,11 @@
     <mergeCell ref="A88:A167"/>
     <mergeCell ref="A168:A181"/>
     <mergeCell ref="A182:A192"/>
-    <mergeCell ref="A193:A210"/>
-    <mergeCell ref="A211:A218"/>
-    <mergeCell ref="A219:A224"/>
-    <mergeCell ref="A225:A230"/>
-    <mergeCell ref="A231:A235"/>
+    <mergeCell ref="A193:A209"/>
+    <mergeCell ref="A210:A217"/>
+    <mergeCell ref="A218:A222"/>
+    <mergeCell ref="A223:A228"/>
+    <mergeCell ref="A229:A233"/>
   </mergeCells>
   <conditionalFormatting sqref="B168">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
add frustum point net paper
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="13140" tabRatio="354"/>
+    <workbookView windowWidth="26970" windowHeight="12450" tabRatio="354"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$246</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$251</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="379">
   <si>
     <t>Scope</t>
   </si>
@@ -659,6 +659,33 @@
     <t>通过深度控制每个pixel上depthwise卷积的weights的大小和dilation-rate, 减轻图片上物体scale-variance的问题,  减轻了psudo-lidar方式对深度估计的依赖, 同时还能够有效利用RGB图片的语义信息;</t>
   </si>
   <si>
+    <t>(2017.11) Frustum PointNets for 3D Object Detection from RGB-D Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">用2D object detection产生框，结合深度产生截锥体， 截锥体内进行点云分割， 留下属于物体的点云， 最后在这一坨点云上进行3D-bbox估计；
+几个坐标系转换对结果影响比较大（figure 4,  table 8.0）：
+1. frustum rotation: 这样每个截锥体里面的点都有大致一样的点的分布， 后续好3d分割；
+2. mask centroid subtraction: 分割完以后的点都有较小的XYZ值，且都在（0, 0, 0）附近；
+3. T-Net: 估计一个bbox的中心，算是初加工吧； </t>
+  </si>
+  <si>
+    <t>(2019.03) Monocular 3D Object Detection with Pseudo-LiDAR Point Cloud</t>
+  </si>
+  <si>
+    <t>针对Pseudo-LiDAR点云比较noisy，提出了：a. 用bounding box consistance loss / bounding box consistency optimization 缓解local mis alignment； b. 用Instance-mask代替2d-bbox， 缓解long-tail的问题；
+算法的整体结构： 深度网络用了DORN, mask分支用了mask-rcnn,  3-d检测用了f-point-net
+note: it is difficult to learn the point cloud segmentation network without direct supervision</t>
+  </si>
+  <si>
+    <t>(2019.03) FVNet: 3D Front-View Proposal Generation for Real-Time Object Detection from Point Clouds</t>
+  </si>
+  <si>
+    <t>(2019.12) What You See is What You Get: Exploiting Visibility for 3D Object Detection</t>
+  </si>
+  <si>
+    <t>(2019.09)Object-Centric Stereo Matching for 3D Object Detection</t>
+  </si>
+  <si>
     <t>image semantic segmentation</t>
   </si>
   <si>
@@ -1760,10 +1787,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1822,24 +1849,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1853,23 +1864,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1880,6 +1898,30 @@
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1898,16 +1940,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1921,14 +1964,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -1936,31 +1971,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2000,19 +2027,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2024,25 +2057,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2066,13 +2093,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2084,31 +2129,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2126,25 +2159,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2162,13 +2189,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2180,19 +2201,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2248,8 +2275,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2265,6 +2292,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2299,6 +2335,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -2318,181 +2369,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2532,9 +2559,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2547,9 +2571,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2571,18 +2592,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2607,14 +2628,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2724,7 +2739,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="4C4C4C"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -2977,15 +2992,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G246"/>
+  <dimension ref="A1:G251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="12.75" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="15.75" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="13.4266666666667" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
@@ -3009,7 +3024,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="27" spans="1:4">
+    <row r="2" ht="33" spans="1:4">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -3021,7 +3036,7 @@
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" ht="13.5" spans="1:4">
+    <row r="3" ht="16.5" spans="1:4">
       <c r="A3" s="9"/>
       <c r="B3" s="10">
         <v>5</v>
@@ -3031,7 +3046,7 @@
       </c>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" ht="13.5" spans="1:4">
+    <row r="4" ht="16.5" spans="1:4">
       <c r="A4" s="9"/>
       <c r="B4" s="10">
         <v>5</v>
@@ -3041,7 +3056,7 @@
       </c>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" ht="13.5" spans="1:4">
+    <row r="5" ht="16.5" spans="1:4">
       <c r="A5" s="9"/>
       <c r="B5" s="10">
         <v>5</v>
@@ -3053,7 +3068,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="13.5" spans="1:4">
+    <row r="6" ht="16.5" spans="1:4">
       <c r="A6" s="9"/>
       <c r="B6" s="10"/>
       <c r="C6" s="12" t="s">
@@ -3061,8 +3076,8 @@
       </c>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" ht="25.5" spans="1:4">
-      <c r="A7" s="13" t="s">
+    <row r="7" ht="31.5" spans="1:4">
+      <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="10">
@@ -3073,16 +3088,16 @@
       </c>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" ht="25.5" spans="1:4">
-      <c r="A8" s="13"/>
+    <row r="8" ht="31.5" spans="1:4">
+      <c r="A8" s="9"/>
       <c r="B8" s="10"/>
       <c r="C8" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" ht="147" spans="1:4">
-      <c r="A9" s="13"/>
+    <row r="9" ht="180" spans="1:4">
+      <c r="A9" s="9"/>
       <c r="B9" s="10">
         <v>5</v>
       </c>
@@ -3093,7 +3108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" ht="51.75" spans="1:4">
+    <row r="10" ht="63.75" spans="1:4">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -3107,9 +3122,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" ht="13.5" spans="1:4">
+    <row r="11" ht="16.5" spans="1:4">
       <c r="A11" s="9"/>
-      <c r="B11" s="14">
+      <c r="B11" s="13">
         <v>5</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -3121,39 +3136,39 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="9"/>
-      <c r="B12" s="15">
-        <v>5</v>
-      </c>
-      <c r="C12" s="16" t="s">
+      <c r="B12" s="14">
+        <v>5</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="11"/>
     </row>
-    <row r="13" ht="25.5" spans="1:4">
+    <row r="13" ht="31.5" spans="1:4">
       <c r="A13" s="9"/>
       <c r="B13" s="10">
         <v>5</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" ht="67.5" spans="1:4">
+    <row r="14" ht="82.5" spans="1:4">
       <c r="A14" s="9"/>
       <c r="B14" s="10">
         <v>5</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" ht="66" spans="1:4">
+    <row r="15" ht="81" spans="1:4">
       <c r="A15" s="9" t="s">
         <v>26</v>
       </c>
@@ -3167,9 +3182,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" ht="27" spans="1:4">
+    <row r="16" ht="33" spans="1:4">
       <c r="A16" s="9"/>
-      <c r="B16" s="15">
+      <c r="B16" s="14">
         <v>5</v>
       </c>
       <c r="C16" s="11" t="s">
@@ -3193,7 +3208,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="9"/>
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <v>5</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -3206,9 +3221,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" ht="25.5" spans="1:4">
+    <row r="19" ht="31.5" spans="1:4">
       <c r="A19" s="9"/>
-      <c r="B19" s="15">
+      <c r="B19" s="14">
         <v>5</v>
       </c>
       <c r="C19" s="11" t="s">
@@ -3218,9 +3233,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" ht="66" spans="1:4">
+    <row r="20" ht="81" spans="1:4">
       <c r="A20" s="9"/>
-      <c r="B20" s="15">
+      <c r="B20" s="14">
         <v>5</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -3230,9 +3245,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" ht="27" spans="1:4">
+    <row r="21" ht="33" spans="1:4">
       <c r="A21" s="9"/>
-      <c r="B21" s="15">
+      <c r="B21" s="14">
         <v>5</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -3242,9 +3257,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" ht="38.25" spans="1:4">
+    <row r="22" ht="47.25" spans="1:4">
       <c r="A22" s="9"/>
-      <c r="B22" s="17">
+      <c r="B22" s="16">
         <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -3252,9 +3267,9 @@
       </c>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" ht="25.5" spans="1:4">
+    <row r="23" ht="31.5" spans="1:4">
       <c r="A23" s="9"/>
-      <c r="B23" s="15">
+      <c r="B23" s="14">
         <v>5</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -3262,9 +3277,9 @@
       </c>
       <c r="D23" s="11"/>
     </row>
-    <row r="24" ht="25.5" spans="1:4">
+    <row r="24" ht="31.5" spans="1:4">
       <c r="A24" s="9"/>
-      <c r="B24" s="15">
+      <c r="B24" s="14">
         <v>5</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -3272,9 +3287,9 @@
       </c>
       <c r="D24" s="11"/>
     </row>
-    <row r="25" ht="54" spans="1:4">
+    <row r="25" ht="66" spans="1:4">
       <c r="A25" s="9"/>
-      <c r="B25" s="15">
+      <c r="B25" s="14">
         <v>5</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -3284,9 +3299,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" ht="25.5" spans="1:4">
+    <row r="26" ht="31.5" spans="1:4">
       <c r="A26" s="9"/>
-      <c r="B26" s="15">
+      <c r="B26" s="14">
         <v>5</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -3296,12 +3311,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" ht="13.5" spans="1:5">
+    <row r="27" ht="16.5" spans="1:5">
       <c r="A27" s="9"/>
-      <c r="B27" s="15">
-        <v>5</v>
-      </c>
-      <c r="C27" s="18" t="s">
+      <c r="B27" s="14">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="11" t="s">
@@ -3311,9 +3326,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" ht="26.25" spans="1:4">
+    <row r="28" ht="32.25" spans="1:4">
       <c r="A28" s="9"/>
-      <c r="B28" s="15">
+      <c r="B28" s="14">
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -3323,9 +3338,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" ht="52.5" spans="1:4">
+    <row r="29" ht="64.5" spans="1:4">
       <c r="A29" s="9"/>
-      <c r="B29" s="15">
+      <c r="B29" s="14">
         <v>5</v>
       </c>
       <c r="C29" s="11" t="s">
@@ -3335,9 +3350,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" ht="25.5" spans="1:4">
+    <row r="30" ht="31.5" spans="1:4">
       <c r="A30" s="9"/>
-      <c r="B30" s="15">
+      <c r="B30" s="14">
         <v>5</v>
       </c>
       <c r="C30" s="12" t="s">
@@ -3347,9 +3362,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" ht="25.5" spans="1:4">
+    <row r="31" ht="31.5" spans="1:4">
       <c r="A31" s="9"/>
-      <c r="B31" s="15">
+      <c r="B31" s="14">
         <v>5</v>
       </c>
       <c r="C31" s="12" t="s">
@@ -3359,7 +3374,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="9"/>
-      <c r="B32" s="15">
+      <c r="B32" s="14">
         <v>5</v>
       </c>
       <c r="C32" s="12" t="s">
@@ -3369,7 +3384,7 @@
     </row>
     <row r="33" ht="53" customHeight="1" spans="1:4">
       <c r="A33" s="9"/>
-      <c r="B33" s="15">
+      <c r="B33" s="14">
         <v>5</v>
       </c>
       <c r="C33" s="12" t="s">
@@ -3381,7 +3396,7 @@
     </row>
     <row r="34" ht="53" customHeight="1" spans="1:4">
       <c r="A34" s="9"/>
-      <c r="B34" s="15">
+      <c r="B34" s="14">
         <v>5</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -3393,7 +3408,7 @@
     </row>
     <row r="35" ht="185" customHeight="1" spans="1:5">
       <c r="A35" s="9"/>
-      <c r="B35" s="15">
+      <c r="B35" s="14">
         <v>5</v>
       </c>
       <c r="C35" s="12" t="s">
@@ -3408,7 +3423,7 @@
     </row>
     <row r="36" ht="53" customHeight="1" spans="1:5">
       <c r="A36" s="9"/>
-      <c r="B36" s="15">
+      <c r="B36" s="14">
         <v>2</v>
       </c>
       <c r="C36" s="12" t="s">
@@ -3423,7 +3438,7 @@
     </row>
     <row r="37" ht="53" customHeight="1" spans="1:4">
       <c r="A37" s="9"/>
-      <c r="B37" s="17">
+      <c r="B37" s="16">
         <v>1</v>
       </c>
       <c r="C37" s="11" t="s">
@@ -3433,7 +3448,7 @@
     </row>
     <row r="38" ht="53" customHeight="1" spans="1:4">
       <c r="A38" s="9"/>
-      <c r="B38" s="17">
+      <c r="B38" s="16">
         <v>2</v>
       </c>
       <c r="C38" s="11" t="s">
@@ -3443,7 +3458,7 @@
     </row>
     <row r="39" ht="53" customHeight="1" spans="1:4">
       <c r="A39" s="9"/>
-      <c r="B39" s="17">
+      <c r="B39" s="16">
         <v>1</v>
       </c>
       <c r="C39" s="11" t="s">
@@ -3453,7 +3468,7 @@
     </row>
     <row r="40" ht="70" customHeight="1" spans="1:4">
       <c r="A40" s="9"/>
-      <c r="B40" s="17">
+      <c r="B40" s="16">
         <v>1</v>
       </c>
       <c r="C40" s="11" t="s">
@@ -3465,7 +3480,7 @@
     </row>
     <row r="41" ht="355" customHeight="1" spans="1:4">
       <c r="A41" s="9"/>
-      <c r="B41" s="15">
+      <c r="B41" s="14">
         <v>5</v>
       </c>
       <c r="C41" s="12" t="s">
@@ -3477,7 +3492,7 @@
     </row>
     <row r="42" ht="53" customHeight="1" spans="1:4">
       <c r="A42" s="9"/>
-      <c r="B42" s="15">
+      <c r="B42" s="14">
         <v>1</v>
       </c>
       <c r="C42" s="12" t="s">
@@ -3487,7 +3502,7 @@
     </row>
     <row r="43" ht="53" customHeight="1" spans="1:4">
       <c r="A43" s="9"/>
-      <c r="B43" s="15">
+      <c r="B43" s="14">
         <v>5</v>
       </c>
       <c r="C43" s="12" t="s">
@@ -3499,7 +3514,7 @@
     </row>
     <row r="44" ht="155" customHeight="1" spans="1:5">
       <c r="A44" s="9"/>
-      <c r="B44" s="19">
+      <c r="B44" s="17">
         <v>5</v>
       </c>
       <c r="C44" s="12" t="s">
@@ -3514,7 +3529,7 @@
     </row>
     <row r="45" ht="53" customHeight="1" spans="1:4">
       <c r="A45" s="9"/>
-      <c r="B45" s="19">
+      <c r="B45" s="17">
         <v>5</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -3526,7 +3541,7 @@
     </row>
     <row r="46" ht="53" customHeight="1" spans="1:4">
       <c r="A46" s="9"/>
-      <c r="B46" s="19">
+      <c r="B46" s="17">
         <v>5</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -3538,7 +3553,7 @@
     </row>
     <row r="47" ht="53" customHeight="1" spans="1:4">
       <c r="A47" s="9"/>
-      <c r="B47" s="19">
+      <c r="B47" s="17">
         <v>1</v>
       </c>
       <c r="C47" s="12" t="s">
@@ -3548,7 +3563,7 @@
     </row>
     <row r="48" ht="53" customHeight="1" spans="1:5">
       <c r="A48" s="9"/>
-      <c r="B48" s="19">
+      <c r="B48" s="17">
         <v>2</v>
       </c>
       <c r="C48" s="12" t="s">
@@ -3563,7 +3578,7 @@
     </row>
     <row r="49" ht="53" customHeight="1" spans="1:5">
       <c r="A49" s="9"/>
-      <c r="B49" s="19">
+      <c r="B49" s="17">
         <v>2</v>
       </c>
       <c r="C49" s="12" t="s">
@@ -3578,7 +3593,7 @@
     </row>
     <row r="50" ht="53" customHeight="1" spans="1:5">
       <c r="A50" s="9"/>
-      <c r="B50" s="19">
+      <c r="B50" s="17">
         <v>5</v>
       </c>
       <c r="C50" s="12" t="s">
@@ -3593,7 +3608,7 @@
     </row>
     <row r="51" ht="53" customHeight="1" spans="1:4">
       <c r="A51" s="9"/>
-      <c r="B51" s="19">
+      <c r="B51" s="17">
         <v>1</v>
       </c>
       <c r="C51" s="12" t="s">
@@ -3605,7 +3620,7 @@
     </row>
     <row r="52" ht="53" customHeight="1" spans="1:4">
       <c r="A52" s="9"/>
-      <c r="B52" s="19">
+      <c r="B52" s="17">
         <v>1</v>
       </c>
       <c r="C52" s="12" t="s">
@@ -3615,7 +3630,7 @@
     </row>
     <row r="53" ht="53" customHeight="1" spans="1:4">
       <c r="A53" s="9"/>
-      <c r="B53" s="19"/>
+      <c r="B53" s="17"/>
       <c r="C53" s="12" t="s">
         <v>93</v>
       </c>
@@ -3625,7 +3640,7 @@
     </row>
     <row r="54" ht="53" customHeight="1" spans="1:4">
       <c r="A54" s="9"/>
-      <c r="B54" s="19">
+      <c r="B54" s="17">
         <v>2</v>
       </c>
       <c r="C54" s="12" t="s">
@@ -3637,10 +3652,10 @@
       <c r="A55" s="9"/>
     </row>
     <row r="56" ht="183" customHeight="1" spans="1:4">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="B56" s="15">
+      <c r="B56" s="14">
         <v>5</v>
       </c>
       <c r="C56" s="2" t="s">
@@ -3651,28 +3666,28 @@
       </c>
     </row>
     <row r="57" ht="202" customHeight="1" spans="1:4">
-      <c r="A57" s="20"/>
-      <c r="B57" s="15">
+      <c r="A57" s="18"/>
+      <c r="B57" s="14">
         <v>5</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D57" s="21" t="s">
+      <c r="D57" s="19" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="58" ht="43" customHeight="1" spans="1:4">
-      <c r="A58" s="20"/>
-      <c r="B58" s="15"/>
+      <c r="A58" s="18"/>
+      <c r="B58" s="14"/>
       <c r="C58" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D58" s="21"/>
+      <c r="D58" s="19"/>
     </row>
     <row r="59" ht="69" customHeight="1" spans="1:3">
-      <c r="A59" s="20"/>
-      <c r="B59" s="15">
+      <c r="A59" s="18"/>
+      <c r="B59" s="14">
         <v>1</v>
       </c>
       <c r="C59" s="2" t="s">
@@ -3680,56 +3695,56 @@
       </c>
     </row>
     <row r="60" ht="56" customHeight="1" spans="1:3">
-      <c r="A60" s="20" t="s">
+      <c r="A60" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="15"/>
+      <c r="B60" s="14"/>
       <c r="C60" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="61" ht="30" customHeight="1" spans="1:3">
-      <c r="A61" s="20"/>
-      <c r="B61" s="15"/>
+      <c r="A61" s="18"/>
+      <c r="B61" s="14"/>
       <c r="C61" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="62" ht="29" customHeight="1" spans="1:3">
-      <c r="A62" s="20"/>
-      <c r="B62" s="15"/>
+      <c r="A62" s="18"/>
+      <c r="B62" s="14"/>
       <c r="C62" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="63" ht="69" customHeight="1" spans="1:3">
-      <c r="A63" s="20"/>
-      <c r="B63" s="15"/>
+      <c r="A63" s="18"/>
+      <c r="B63" s="14"/>
       <c r="C63" s="2" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="64" ht="69" customHeight="1" spans="1:2">
-      <c r="A64" s="20"/>
-      <c r="B64" s="15"/>
+      <c r="A64" s="18"/>
+      <c r="B64" s="14"/>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B65" s="15">
+      <c r="B65" s="14">
         <v>5</v>
       </c>
       <c r="C65" s="11" t="s">
         <v>109</v>
       </c>
       <c r="D65" s="11"/>
-      <c r="F65" s="28"/>
-      <c r="G65" s="28"/>
-    </row>
-    <row r="66" ht="51.75" spans="1:6">
+      <c r="F65" s="24"/>
+      <c r="G65" s="24"/>
+    </row>
+    <row r="66" ht="63.75" spans="1:6">
       <c r="A66" s="9"/>
-      <c r="B66" s="15">
+      <c r="B66" s="14">
         <v>5</v>
       </c>
       <c r="C66" s="11" t="s">
@@ -3740,7 +3755,7 @@
       </c>
       <c r="F66" s="1"/>
     </row>
-    <row r="67" ht="27" spans="1:4">
+    <row r="67" ht="33" spans="1:4">
       <c r="A67" s="9"/>
       <c r="B67" s="10">
         <v>5</v>
@@ -3752,7 +3767,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="68" ht="66.75" spans="1:4">
+    <row r="68" ht="81.75" spans="1:4">
       <c r="A68" s="9"/>
       <c r="B68" s="10">
         <v>5</v>
@@ -3764,9 +3779,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="69" ht="25.5" spans="1:4">
+    <row r="69" ht="31.5" spans="1:4">
       <c r="A69" s="9"/>
-      <c r="B69" s="22">
+      <c r="B69" s="20">
         <v>5</v>
       </c>
       <c r="C69" s="2" t="s">
@@ -3776,7 +3791,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="70" ht="27" spans="1:4">
+    <row r="70" ht="33" spans="1:4">
       <c r="A70" s="9"/>
       <c r="B70" s="10">
         <v>5</v>
@@ -3788,7 +3803,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="71" ht="25.5" spans="1:4">
+    <row r="71" ht="31.5" spans="1:4">
       <c r="A71" s="9"/>
       <c r="B71" s="10">
         <v>2</v>
@@ -3798,7 +3813,7 @@
       </c>
       <c r="D71" s="11"/>
     </row>
-    <row r="72" ht="65.25" spans="1:4">
+    <row r="72" ht="80.25" spans="1:4">
       <c r="A72" s="9"/>
       <c r="B72" s="10">
         <v>5</v>
@@ -3810,7 +3825,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="73" ht="40.5" spans="1:4">
+    <row r="73" ht="49.5" spans="1:4">
       <c r="A73" s="9"/>
       <c r="B73" s="10">
         <v>5</v>
@@ -3822,7 +3837,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="74" ht="38.25" spans="1:4">
+    <row r="74" ht="47.25" spans="1:4">
       <c r="A74" s="9"/>
       <c r="B74" s="10">
         <v>1</v>
@@ -3832,7 +3847,7 @@
       </c>
       <c r="D74" s="11"/>
     </row>
-    <row r="75" ht="25.5" spans="1:4">
+    <row r="75" ht="31.5" spans="1:4">
       <c r="A75" s="9"/>
       <c r="B75" s="10">
         <v>1</v>
@@ -3852,7 +3867,7 @@
       </c>
       <c r="D76" s="11"/>
     </row>
-    <row r="77" ht="25.5" spans="1:4">
+    <row r="77" ht="31.5" spans="1:4">
       <c r="A77" s="9"/>
       <c r="B77" s="10">
         <v>1</v>
@@ -3864,39 +3879,39 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="9"/>
-      <c r="B78" s="23"/>
+      <c r="B78" s="21"/>
       <c r="C78" s="12"/>
       <c r="D78" s="12"/>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="9"/>
-      <c r="B79" s="23"/>
+      <c r="B79" s="21"/>
       <c r="C79" s="12"/>
       <c r="D79" s="12"/>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="9"/>
-      <c r="B80" s="23"/>
+      <c r="B80" s="21"/>
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="9"/>
-      <c r="B81" s="23"/>
+      <c r="B81" s="21"/>
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="9"/>
-      <c r="B82" s="23"/>
+      <c r="B82" s="21"/>
       <c r="C82" s="12"/>
       <c r="D82" s="12"/>
     </row>
-    <row r="83" ht="67.5" spans="1:4">
-      <c r="A83" s="24" t="s">
+    <row r="83" ht="82.5" spans="1:4">
+      <c r="A83" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="B83" s="23">
+      <c r="B83" s="21">
         <v>5</v>
       </c>
       <c r="C83" s="12" t="s">
@@ -3906,9 +3921,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="84" ht="225.75" spans="1:4">
-      <c r="A84" s="24"/>
-      <c r="B84" s="23">
+    <row r="84" ht="276.75" spans="1:4">
+      <c r="A84" s="22"/>
+      <c r="B84" s="21">
         <v>5</v>
       </c>
       <c r="C84" s="12" t="s">
@@ -3918,9 +3933,9 @@
         <v>133</v>
       </c>
     </row>
-    <row r="85" ht="38.25" spans="1:4">
-      <c r="A85" s="24"/>
-      <c r="B85" s="23">
+    <row r="85" ht="47.25" spans="1:4">
+      <c r="A85" s="22"/>
+      <c r="B85" s="21">
         <v>5</v>
       </c>
       <c r="C85" s="12" t="s">
@@ -3930,9 +3945,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="86" ht="40.5" spans="1:4">
-      <c r="A86" s="24"/>
-      <c r="B86" s="23">
+    <row r="86" ht="49.5" spans="1:4">
+      <c r="A86" s="22"/>
+      <c r="B86" s="21">
         <v>5</v>
       </c>
       <c r="C86" s="12" t="s">
@@ -3942,9 +3957,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="87" ht="117" spans="1:4">
-      <c r="A87" s="24"/>
-      <c r="B87" s="23">
+    <row r="87" ht="144" spans="1:4">
+      <c r="A87" s="22"/>
+      <c r="B87" s="21">
         <v>5</v>
       </c>
       <c r="C87" s="12" t="s">
@@ -3954,17 +3969,19 @@
         <v>139</v>
       </c>
     </row>
-    <row r="88" ht="25.5" spans="1:4">
-      <c r="A88" s="24"/>
-      <c r="B88" s="23"/>
+    <row r="88" ht="31.5" spans="1:4">
+      <c r="A88" s="22"/>
+      <c r="B88" s="21"/>
       <c r="C88" s="12" t="s">
         <v>140</v>
       </c>
       <c r="D88" s="12"/>
     </row>
-    <row r="89" ht="27" spans="1:4">
-      <c r="A89" s="24"/>
-      <c r="B89" s="23"/>
+    <row r="89" ht="33" spans="1:4">
+      <c r="A89" s="22"/>
+      <c r="B89" s="21">
+        <v>5</v>
+      </c>
       <c r="C89" s="12" t="s">
         <v>141</v>
       </c>
@@ -3972,1067 +3989,1061 @@
         <v>142</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="24"/>
-      <c r="B90" s="23"/>
-      <c r="C90" s="12"/>
-      <c r="D90" s="12"/>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" s="24"/>
-    </row>
-    <row r="92" ht="39" spans="1:4">
-      <c r="A92" s="25" t="s">
+    <row r="90" ht="82.5" spans="1:4">
+      <c r="A90" s="22"/>
+      <c r="B90" s="21">
+        <v>5</v>
+      </c>
+      <c r="C90" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="B92" s="10">
-        <v>5</v>
-      </c>
-      <c r="C92" s="11" t="s">
+      <c r="D90" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D92" s="11"/>
-    </row>
-    <row r="93" ht="52.5" spans="1:4">
-      <c r="A93" s="25"/>
-      <c r="B93" s="10">
+    </row>
+    <row r="91" ht="65.25" spans="1:4">
+      <c r="A91" s="22"/>
+      <c r="B91" s="21">
+        <v>5</v>
+      </c>
+      <c r="C91" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="92" ht="47.25" spans="1:4">
+      <c r="A92" s="22"/>
+      <c r="B92" s="21"/>
+      <c r="C92" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D92" s="12"/>
+    </row>
+    <row r="93" ht="31.5" spans="1:4">
+      <c r="A93" s="22"/>
+      <c r="B93" s="21"/>
+      <c r="C93" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D93" s="12"/>
+    </row>
+    <row r="94" ht="31.5" spans="1:4">
+      <c r="A94" s="22"/>
+      <c r="B94" s="21"/>
+      <c r="C94" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D94" s="12"/>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="22"/>
+      <c r="B95" s="21"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12"/>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="22"/>
+    </row>
+    <row r="97" ht="48" spans="1:4">
+      <c r="A97" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="B97" s="10">
+        <v>5</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D97" s="11"/>
+    </row>
+    <row r="98" ht="64.5" spans="1:4">
+      <c r="A98" s="23"/>
+      <c r="B98" s="10">
         <v>6</v>
       </c>
-      <c r="C93" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="D93" s="11" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="94" ht="25.5" spans="1:4">
-      <c r="A94" s="25"/>
-      <c r="B94" s="22">
-        <v>5</v>
-      </c>
-      <c r="C94" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="D94" s="11" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="95" ht="25.5" spans="1:4">
-      <c r="A95" s="25"/>
-      <c r="B95" s="22">
-        <v>5</v>
-      </c>
-      <c r="C95" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="D95" s="11" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="96" ht="79.5" spans="1:4">
-      <c r="A96" s="25"/>
-      <c r="B96" s="22">
-        <v>5</v>
-      </c>
-      <c r="C96" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D96" s="11" t="s">
+      <c r="C98" s="11" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="97" ht="79.5" spans="1:4">
-      <c r="A97" s="25"/>
-      <c r="B97" s="22">
-        <v>5</v>
-      </c>
-      <c r="C97" s="11" t="s">
+      <c r="D98" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="D97" s="11" t="s">
+    </row>
+    <row r="99" ht="31.5" spans="1:4">
+      <c r="A99" s="23"/>
+      <c r="B99" s="20">
+        <v>5</v>
+      </c>
+      <c r="C99" s="11" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="98" ht="107.25" spans="1:4">
-      <c r="A98" s="25"/>
-      <c r="B98" s="22">
-        <v>5</v>
-      </c>
-      <c r="C98" s="11" t="s">
+      <c r="D99" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="D98" s="8" t="s">
+    </row>
+    <row r="100" ht="31.5" spans="1:4">
+      <c r="A100" s="23"/>
+      <c r="B100" s="20">
+        <v>5</v>
+      </c>
+      <c r="C100" s="11" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="99" ht="39.75" spans="1:4">
-      <c r="A99" s="25"/>
-      <c r="B99" s="22">
-        <v>5</v>
-      </c>
-      <c r="C99" s="11" t="s">
+      <c r="D100" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="D99" s="11" t="s">
+    </row>
+    <row r="101" ht="97.5" spans="1:4">
+      <c r="A101" s="23"/>
+      <c r="B101" s="20">
+        <v>5</v>
+      </c>
+      <c r="C101" s="11" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="100" ht="66" spans="1:4">
-      <c r="A100" s="25"/>
-      <c r="B100" s="22">
-        <v>5</v>
-      </c>
-      <c r="C100" s="11" t="s">
+      <c r="D101" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="D100" s="11" t="s">
+    </row>
+    <row r="102" ht="97.5" spans="1:4">
+      <c r="A102" s="23"/>
+      <c r="B102" s="20">
+        <v>5</v>
+      </c>
+      <c r="C102" s="11" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="101" ht="25.5" spans="1:4">
-      <c r="A101" s="25"/>
-      <c r="B101" s="22">
-        <v>5</v>
-      </c>
-      <c r="C101" s="11" t="s">
+      <c r="D102" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="D101" s="11"/>
-    </row>
-    <row r="102" ht="26.25" spans="1:4">
-      <c r="A102" s="25"/>
-      <c r="B102" s="22">
-        <v>5</v>
-      </c>
-      <c r="C102" s="11" t="s">
+    </row>
+    <row r="103" ht="131.25" spans="1:4">
+      <c r="A103" s="23"/>
+      <c r="B103" s="20">
+        <v>5</v>
+      </c>
+      <c r="C103" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="D102" s="11"/>
-    </row>
-    <row r="103" ht="25.5" spans="1:4">
-      <c r="A103" s="25"/>
-      <c r="B103" s="22">
+      <c r="D103" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="104" ht="48.75" spans="1:4">
+      <c r="A104" s="23"/>
+      <c r="B104" s="20">
+        <v>5</v>
+      </c>
+      <c r="C104" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D104" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="105" ht="81" spans="1:4">
+      <c r="A105" s="23"/>
+      <c r="B105" s="20">
+        <v>5</v>
+      </c>
+      <c r="C105" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="D105" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="106" ht="31.5" spans="1:4">
+      <c r="A106" s="23"/>
+      <c r="B106" s="20">
+        <v>5</v>
+      </c>
+      <c r="C106" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="D106" s="11"/>
+    </row>
+    <row r="107" ht="32.25" spans="1:4">
+      <c r="A107" s="23"/>
+      <c r="B107" s="20">
+        <v>5</v>
+      </c>
+      <c r="C107" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D107" s="11"/>
+    </row>
+    <row r="108" ht="31.5" spans="1:4">
+      <c r="A108" s="23"/>
+      <c r="B108" s="20">
         <v>2</v>
       </c>
-      <c r="C103" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="D103" s="11"/>
-    </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="25"/>
-      <c r="B104" s="22">
-        <v>5</v>
-      </c>
-      <c r="C104" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="D104" s="11"/>
-    </row>
-    <row r="105" ht="25.5" spans="1:4">
-      <c r="A105" s="25"/>
-      <c r="B105" s="22">
+      <c r="C108" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D108" s="11"/>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="23"/>
+      <c r="B109" s="20">
+        <v>5</v>
+      </c>
+      <c r="C109" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="D109" s="11"/>
+    </row>
+    <row r="110" ht="31.5" spans="1:4">
+      <c r="A110" s="23"/>
+      <c r="B110" s="20">
         <v>2</v>
       </c>
-      <c r="C105" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="D105" s="11"/>
-    </row>
-    <row r="106" ht="38.25" spans="1:4">
-      <c r="A106" s="25"/>
-      <c r="B106" s="22">
-        <v>5</v>
-      </c>
-      <c r="C106" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="D106" s="11" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="107" ht="38.25" spans="1:4">
-      <c r="A107" s="25"/>
-      <c r="B107" s="22">
-        <v>5</v>
-      </c>
-      <c r="C107" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="D107" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="108" ht="117" spans="1:5">
-      <c r="A108" s="25"/>
-      <c r="B108" s="22">
-        <v>5</v>
-      </c>
-      <c r="C108" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="D108" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="E108" s="29" t="s">
+      <c r="C110" s="12" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="109" ht="155" customHeight="1" spans="1:5">
-      <c r="A109" s="25"/>
-      <c r="B109" s="22">
-        <v>5</v>
-      </c>
-      <c r="C109" s="12" t="s">
+      <c r="D110" s="11"/>
+    </row>
+    <row r="111" ht="47.25" spans="1:4">
+      <c r="A111" s="23"/>
+      <c r="B111" s="20">
+        <v>5</v>
+      </c>
+      <c r="C111" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D109" s="11" t="s">
+      <c r="D111" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="E109" s="2" t="s">
+    </row>
+    <row r="112" ht="47.25" spans="1:4">
+      <c r="A112" s="23"/>
+      <c r="B112" s="20">
+        <v>5</v>
+      </c>
+      <c r="C112" s="12" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="110" ht="40.5" spans="1:4">
-      <c r="A110" s="25"/>
-      <c r="B110" s="22">
-        <v>5</v>
-      </c>
-      <c r="C110" s="12" t="s">
+      <c r="D112" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="D110" s="11" t="s">
+    </row>
+    <row r="113" ht="144" spans="1:5">
+      <c r="A113" s="23"/>
+      <c r="B113" s="20">
+        <v>5</v>
+      </c>
+      <c r="C113" s="12" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="111" ht="40.5" spans="1:4">
-      <c r="A111" s="25"/>
-      <c r="B111" s="22">
-        <v>5</v>
-      </c>
-      <c r="C111" s="12" t="s">
+      <c r="D113" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="D111" s="11" t="s">
+      <c r="E113" s="25" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
-      <c r="A112" s="25"/>
-    </row>
-    <row r="113" ht="54" spans="1:4">
-      <c r="A113" s="25"/>
-      <c r="B113" s="22">
-        <v>5</v>
-      </c>
-      <c r="C113" s="2" t="s">
+    <row r="114" ht="155" customHeight="1" spans="1:5">
+      <c r="A114" s="23"/>
+      <c r="B114" s="20">
+        <v>5</v>
+      </c>
+      <c r="C114" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="D113" s="11" t="s">
+      <c r="D114" s="11" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="114" ht="40.5" spans="1:4">
-      <c r="A114" s="25"/>
-      <c r="B114" s="22">
-        <v>5</v>
-      </c>
-      <c r="C114" s="2" t="s">
+      <c r="E114" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D114" s="11" t="s">
+    </row>
+    <row r="115" ht="49.5" spans="1:4">
+      <c r="A115" s="23"/>
+      <c r="B115" s="20">
+        <v>5</v>
+      </c>
+      <c r="C115" s="12" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="115" ht="25.5" spans="1:4">
-      <c r="A115" s="25"/>
-      <c r="B115" s="22">
-        <v>5</v>
-      </c>
-      <c r="C115" s="2" t="s">
+      <c r="D115" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="D115" s="11" t="s">
+    </row>
+    <row r="116" ht="49.5" spans="1:4">
+      <c r="A116" s="23"/>
+      <c r="B116" s="20">
+        <v>5</v>
+      </c>
+      <c r="C116" s="12" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="116" ht="25.5" spans="1:4">
-      <c r="A116" s="25"/>
-      <c r="B116" s="22">
+      <c r="D116" s="11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="23"/>
+    </row>
+    <row r="118" ht="66" spans="1:4">
+      <c r="A118" s="23"/>
+      <c r="B118" s="20">
+        <v>5</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D118" s="11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="119" ht="49.5" spans="1:4">
+      <c r="A119" s="23"/>
+      <c r="B119" s="20">
+        <v>5</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D119" s="11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="120" ht="31.5" spans="1:4">
+      <c r="A120" s="23"/>
+      <c r="B120" s="20">
+        <v>5</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D120" s="11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="121" ht="31.5" spans="1:4">
+      <c r="A121" s="23"/>
+      <c r="B121" s="20">
         <v>2</v>
       </c>
-      <c r="C116" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D116" s="11"/>
-    </row>
-    <row r="117" ht="38.25" spans="1:4">
-      <c r="A117" s="25"/>
-      <c r="B117" s="22">
+      <c r="C121" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D121" s="11"/>
+    </row>
+    <row r="122" ht="47.25" spans="1:4">
+      <c r="A122" s="23"/>
+      <c r="B122" s="20">
         <v>2</v>
       </c>
-      <c r="C117" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D117" s="11"/>
-    </row>
-    <row r="118" ht="25.5" spans="1:4">
-      <c r="A118" s="25"/>
-      <c r="B118" s="22">
+      <c r="C122" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D122" s="11"/>
+    </row>
+    <row r="123" ht="31.5" spans="1:4">
+      <c r="A123" s="23"/>
+      <c r="B123" s="20">
         <v>2</v>
       </c>
-      <c r="C118" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D118" s="11"/>
-    </row>
-    <row r="119" ht="39.75" spans="1:4">
-      <c r="A119" s="25"/>
-      <c r="B119" s="22">
-        <v>2</v>
-      </c>
-      <c r="C119" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="D119" s="11"/>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="A120" s="25"/>
-      <c r="B120" s="22">
-        <v>2</v>
-      </c>
-      <c r="C120" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D120" s="11"/>
-    </row>
-    <row r="121" ht="53.25" spans="1:4">
-      <c r="A121" s="25"/>
-      <c r="B121" s="22">
-        <v>5</v>
-      </c>
-      <c r="C121" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="D121" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="122" ht="26.25" spans="1:4">
-      <c r="A122" s="25"/>
-      <c r="B122" s="22">
-        <v>2</v>
-      </c>
-      <c r="C122" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="D122" s="11"/>
-    </row>
-    <row r="123" ht="39.75" spans="1:4">
-      <c r="A123" s="25"/>
-      <c r="B123" s="22">
-        <v>5</v>
-      </c>
-      <c r="C123" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D123" s="11" t="s">
+      <c r="C123" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="124" ht="25.5" spans="1:4">
-      <c r="A124" s="25"/>
-      <c r="B124" s="22">
+      <c r="D123" s="11"/>
+    </row>
+    <row r="124" ht="48.75" spans="1:4">
+      <c r="A124" s="23"/>
+      <c r="B124" s="20">
         <v>2</v>
       </c>
       <c r="C124" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="D124" s="26"/>
-    </row>
-    <row r="125" ht="66" spans="1:4">
-      <c r="A125" s="25"/>
-      <c r="B125" s="22">
-        <v>5</v>
+      <c r="D124" s="11"/>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="23"/>
+      <c r="B125" s="20">
+        <v>2</v>
       </c>
       <c r="C125" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="D125" s="26" t="s">
+      <c r="D125" s="11"/>
+    </row>
+    <row r="126" ht="65.25" spans="1:4">
+      <c r="A126" s="23"/>
+      <c r="B126" s="20">
+        <v>5</v>
+      </c>
+      <c r="C126" s="12" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="126" ht="26.25" spans="1:4">
-      <c r="A126" s="25"/>
-      <c r="B126" s="22">
-        <v>5</v>
-      </c>
-      <c r="C126" s="27" t="s">
+      <c r="D126" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="D126" s="26"/>
-    </row>
-    <row r="127" ht="39.75" spans="1:4">
-      <c r="A127" s="25"/>
-      <c r="B127" s="22">
+    </row>
+    <row r="127" ht="32.25" spans="1:4">
+      <c r="A127" s="23"/>
+      <c r="B127" s="20">
         <v>2</v>
       </c>
-      <c r="C127" s="27" t="s">
+      <c r="C127" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="D127" s="26"/>
-    </row>
-    <row r="128" ht="25.5" spans="1:4">
-      <c r="A128" s="25"/>
-      <c r="B128" s="22">
+      <c r="D127" s="11"/>
+    </row>
+    <row r="128" ht="48.75" spans="1:4">
+      <c r="A128" s="23"/>
+      <c r="B128" s="20">
+        <v>5</v>
+      </c>
+      <c r="C128" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="D128" s="11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="129" ht="31.5" spans="1:4">
+      <c r="A129" s="23"/>
+      <c r="B129" s="20">
         <v>2</v>
       </c>
-      <c r="C128" s="27" t="s">
-        <v>201</v>
-      </c>
-      <c r="D128" s="26"/>
-    </row>
-    <row r="129" ht="25.5" spans="1:4">
-      <c r="A129" s="25"/>
-      <c r="B129" s="22">
-        <v>5</v>
-      </c>
-      <c r="C129" s="27" t="s">
-        <v>202</v>
+      <c r="C129" s="12" t="s">
+        <v>203</v>
       </c>
       <c r="D129" s="26"/>
     </row>
-    <row r="130" ht="66" spans="1:4">
-      <c r="A130" s="25"/>
-      <c r="B130" s="22">
+    <row r="130" ht="81" spans="1:4">
+      <c r="A130" s="23"/>
+      <c r="B130" s="20">
         <v>5</v>
       </c>
       <c r="C130" s="12" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D130" s="26" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="131" ht="27" spans="1:4">
-      <c r="A131" s="25"/>
-      <c r="B131" s="22">
-        <v>5</v>
-      </c>
-      <c r="C131" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="D131" s="26" t="s">
+    </row>
+    <row r="131" ht="32.25" spans="1:4">
+      <c r="A131" s="23"/>
+      <c r="B131" s="20">
+        <v>5</v>
+      </c>
+      <c r="C131" s="27" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="132" ht="38.25" spans="1:4">
-      <c r="A132" s="25"/>
-      <c r="B132" s="22">
-        <v>5</v>
-      </c>
-      <c r="C132" s="12" t="s">
+      <c r="D131" s="26"/>
+    </row>
+    <row r="132" ht="48.75" spans="1:4">
+      <c r="A132" s="23"/>
+      <c r="B132" s="20">
+        <v>2</v>
+      </c>
+      <c r="C132" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="D132" s="11" t="s">
+      <c r="D132" s="26"/>
+    </row>
+    <row r="133" ht="31.5" spans="1:4">
+      <c r="A133" s="23"/>
+      <c r="B133" s="20">
+        <v>2</v>
+      </c>
+      <c r="C133" s="27" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="133" ht="39.75" spans="1:4">
-      <c r="A133" s="25"/>
-      <c r="B133" s="22">
-        <v>5</v>
-      </c>
-      <c r="C133" s="30" t="s">
+      <c r="D133" s="26"/>
+    </row>
+    <row r="134" ht="31.5" spans="1:4">
+      <c r="A134" s="23"/>
+      <c r="B134" s="20">
+        <v>5</v>
+      </c>
+      <c r="C134" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="D133" s="11" t="s">
+      <c r="D134" s="26"/>
+    </row>
+    <row r="135" ht="81" spans="1:4">
+      <c r="A135" s="23"/>
+      <c r="B135" s="20">
+        <v>5</v>
+      </c>
+      <c r="C135" s="12" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="134" ht="105.75" spans="1:4">
-      <c r="A134" s="25"/>
-      <c r="B134" s="22">
-        <v>5</v>
-      </c>
-      <c r="C134" s="11" t="s">
+      <c r="D135" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="D134" s="11" t="s">
+    </row>
+    <row r="136" ht="33" spans="1:4">
+      <c r="A136" s="23"/>
+      <c r="B136" s="20">
+        <v>5</v>
+      </c>
+      <c r="C136" s="12" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="135" ht="31" customHeight="1" spans="1:5">
-      <c r="A135" s="25"/>
-      <c r="B135" s="31">
+      <c r="D136" s="26" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="137" ht="47.25" spans="1:4">
+      <c r="A137" s="23"/>
+      <c r="B137" s="20">
+        <v>5</v>
+      </c>
+      <c r="C137" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="D137" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="138" ht="48.75" spans="1:4">
+      <c r="A138" s="23"/>
+      <c r="B138" s="20">
+        <v>5</v>
+      </c>
+      <c r="C138" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="D138" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="139" ht="129.75" spans="1:4">
+      <c r="A139" s="23"/>
+      <c r="B139" s="20">
+        <v>5</v>
+      </c>
+      <c r="C139" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D139" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="140" ht="31" customHeight="1" spans="1:5">
+      <c r="A140" s="23"/>
+      <c r="B140" s="29">
         <v>1</v>
       </c>
-      <c r="C135" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="D135" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="E135" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="136" ht="39" spans="1:4">
-      <c r="A136" s="25"/>
-      <c r="B136" s="31">
+      <c r="C140" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D140" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="141" ht="48" spans="1:4">
+      <c r="A141" s="23"/>
+      <c r="B141" s="29">
         <v>2</v>
       </c>
-      <c r="C136" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="D136" s="12"/>
-    </row>
-    <row r="137" ht="27" spans="1:4">
-      <c r="A137" s="25"/>
-      <c r="B137" s="31">
-        <v>5</v>
-      </c>
-      <c r="C137" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="D137" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="138" ht="40.5" spans="1:4">
-      <c r="A138" s="25"/>
-      <c r="B138" s="31">
-        <v>5</v>
-      </c>
-      <c r="C138" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="D138" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="139" ht="51.75" spans="1:4">
-      <c r="A139" s="25"/>
-      <c r="B139" s="31">
-        <v>1</v>
-      </c>
-      <c r="C139" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="D139" s="12"/>
-    </row>
-    <row r="140" ht="25.5" spans="1:4">
-      <c r="A140" s="25"/>
-      <c r="B140" s="31">
-        <v>1</v>
-      </c>
-      <c r="C140" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="D140" s="12" t="s">
+      <c r="C141" s="12" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="141" ht="38.25" spans="1:4">
-      <c r="A141" s="25"/>
-      <c r="B141" s="31">
-        <v>1</v>
-      </c>
-      <c r="C141" s="12" t="s">
+      <c r="D141" s="12"/>
+    </row>
+    <row r="142" ht="33" spans="1:4">
+      <c r="A142" s="23"/>
+      <c r="B142" s="29">
+        <v>5</v>
+      </c>
+      <c r="C142" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="D141" s="12"/>
-    </row>
-    <row r="142" ht="38.25" spans="1:4">
-      <c r="A142" s="25"/>
-      <c r="B142" s="31">
-        <v>1</v>
-      </c>
-      <c r="C142" s="12" t="s">
+      <c r="D142" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="D142" s="12"/>
-    </row>
-    <row r="143" ht="38.25" spans="1:4">
-      <c r="A143" s="25"/>
-      <c r="B143" s="31">
-        <v>1</v>
+    </row>
+    <row r="143" ht="49.5" spans="1:4">
+      <c r="A143" s="23"/>
+      <c r="B143" s="29">
+        <v>5</v>
       </c>
       <c r="C143" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="D143" s="12"/>
-    </row>
-    <row r="144" spans="1:4">
-      <c r="A144" s="25"/>
-      <c r="B144" s="31">
+      <c r="D143" s="12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="144" ht="63.75" spans="1:4">
+      <c r="A144" s="23"/>
+      <c r="B144" s="29">
         <v>1</v>
       </c>
       <c r="C144" s="12" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D144" s="12"/>
     </row>
-    <row r="145" ht="132" spans="1:5">
-      <c r="A145" s="25"/>
-      <c r="B145" s="31">
-        <v>5</v>
+    <row r="145" ht="31.5" spans="1:4">
+      <c r="A145" s="23"/>
+      <c r="B145" s="29">
+        <v>1</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D145" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="E145" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="146" ht="25.5" spans="1:4">
-      <c r="A146" s="25"/>
-      <c r="B146" s="31">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="146" ht="47.25" spans="1:4">
+      <c r="A146" s="23"/>
+      <c r="B146" s="29">
         <v>1</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D146" s="12"/>
     </row>
-    <row r="147" ht="25.5" spans="1:4">
-      <c r="A147" s="25"/>
-      <c r="B147" s="31">
+    <row r="147" ht="47.25" spans="1:4">
+      <c r="A147" s="23"/>
+      <c r="B147" s="29">
         <v>1</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D147" s="12"/>
     </row>
-    <row r="148" ht="27" spans="1:5">
-      <c r="A148" s="25"/>
-      <c r="B148" s="19">
-        <v>5</v>
+    <row r="148" ht="47.25" spans="1:4">
+      <c r="A148" s="23"/>
+      <c r="B148" s="29">
+        <v>1</v>
       </c>
       <c r="C148" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="D148" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="E148" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="149" ht="93" spans="1:5">
-      <c r="A149" s="25"/>
-      <c r="B149" s="31">
-        <v>5</v>
+      <c r="D148" s="12"/>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="23"/>
+      <c r="B149" s="29">
+        <v>1</v>
       </c>
       <c r="C149" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="D149" s="32" t="s">
+      <c r="D149" s="12"/>
+    </row>
+    <row r="150" ht="162" spans="1:5">
+      <c r="A150" s="23"/>
+      <c r="B150" s="29">
+        <v>5</v>
+      </c>
+      <c r="C150" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="E149" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="150" ht="25.5" spans="1:4">
-      <c r="A150" s="25"/>
-      <c r="B150" s="31">
+      <c r="D150" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="E150" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="151" ht="31.5" spans="1:4">
+      <c r="A151" s="23"/>
+      <c r="B151" s="29">
         <v>1</v>
-      </c>
-      <c r="C150" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="D150" s="32"/>
-    </row>
-    <row r="151" ht="207" customHeight="1" spans="1:5">
-      <c r="A151" s="25"/>
-      <c r="B151" s="31">
-        <v>5</v>
       </c>
       <c r="C151" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="D151" s="32" t="s">
+      <c r="D151" s="12"/>
+    </row>
+    <row r="152" ht="31.5" spans="1:4">
+      <c r="A152" s="23"/>
+      <c r="B152" s="29">
+        <v>1</v>
+      </c>
+      <c r="C152" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="E151" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="152" ht="25.5" spans="1:5">
-      <c r="A152" s="25"/>
-      <c r="B152" s="31">
-        <v>2</v>
-      </c>
-      <c r="C152" s="12" t="s">
+      <c r="D152" s="12"/>
+    </row>
+    <row r="153" ht="33" spans="1:5">
+      <c r="A153" s="23"/>
+      <c r="B153" s="17">
+        <v>5</v>
+      </c>
+      <c r="C153" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="D152" s="32"/>
-      <c r="E152" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="153" ht="119.25" spans="1:5">
-      <c r="A153" s="25"/>
-      <c r="B153" s="31">
-        <v>5</v>
-      </c>
-      <c r="C153" s="12" t="s">
+      <c r="D153" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="D153" s="32" t="s">
+      <c r="E153" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="154" ht="114" spans="1:5">
+      <c r="A154" s="23"/>
+      <c r="B154" s="29">
+        <v>5</v>
+      </c>
+      <c r="C154" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="E153" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="154" ht="25.5" spans="1:5">
-      <c r="A154" s="25"/>
-      <c r="B154" s="31">
+      <c r="D154" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="E154" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="155" ht="31.5" spans="1:4">
+      <c r="A155" s="23"/>
+      <c r="B155" s="29">
         <v>1</v>
-      </c>
-      <c r="C154" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="D154" s="32"/>
-      <c r="E154" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="155" ht="53.25" spans="1:5">
-      <c r="A155" s="25"/>
-      <c r="B155" s="31">
-        <v>5</v>
       </c>
       <c r="C155" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="D155" s="11" t="s">
+      <c r="D155" s="30"/>
+    </row>
+    <row r="156" ht="207" customHeight="1" spans="1:5">
+      <c r="A156" s="23"/>
+      <c r="B156" s="29">
+        <v>5</v>
+      </c>
+      <c r="C156" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="E155" t="s">
+      <c r="D156" s="30" t="s">
+        <v>244</v>
+      </c>
+      <c r="E156" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="156" ht="81" customHeight="1" spans="1:4">
-      <c r="A156" s="25"/>
-      <c r="B156" s="31">
-        <v>5</v>
-      </c>
-      <c r="C156" s="33" t="s">
-        <v>244</v>
-      </c>
-      <c r="D156" s="32" t="s">
+    <row r="157" ht="31.5" spans="1:5">
+      <c r="A157" s="23"/>
+      <c r="B157" s="29">
+        <v>2</v>
+      </c>
+      <c r="C157" s="12" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="157" ht="42" customHeight="1" spans="1:4">
-      <c r="A157" s="25"/>
-      <c r="B157" s="31"/>
-      <c r="C157" s="33" t="s">
+      <c r="D157" s="30"/>
+      <c r="E157" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="158" ht="146.25" spans="1:5">
+      <c r="A158" s="23"/>
+      <c r="B158" s="29">
+        <v>5</v>
+      </c>
+      <c r="C158" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="D157" s="32" t="s">
+      <c r="D158" s="30" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="158" ht="25.5" spans="1:5">
-      <c r="A158" s="25"/>
-      <c r="B158" s="31"/>
-      <c r="C158" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="D158" s="32"/>
       <c r="E158" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="159" ht="25.5" spans="1:4">
-      <c r="A159" s="25"/>
-      <c r="B159" s="31"/>
+    <row r="159" ht="31.5" spans="1:5">
+      <c r="A159" s="23"/>
+      <c r="B159" s="29">
+        <v>1</v>
+      </c>
       <c r="C159" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="D159" s="30"/>
+      <c r="E159" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="160" ht="65.25" spans="1:5">
+      <c r="A160" s="23"/>
+      <c r="B160" s="29">
+        <v>5</v>
+      </c>
+      <c r="C160" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="D159" s="32"/>
-    </row>
-    <row r="160" ht="25.5" spans="1:4">
-      <c r="A160" s="25"/>
-      <c r="B160" s="31"/>
-      <c r="C160" s="12" t="s">
+      <c r="D160" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="D160" s="32"/>
-    </row>
-    <row r="161" ht="25.5" spans="1:4">
-      <c r="A161" s="25"/>
-      <c r="B161" s="31"/>
-      <c r="C161" s="12" t="s">
+      <c r="E160" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="161" ht="81" customHeight="1" spans="1:4">
+      <c r="A161" s="23"/>
+      <c r="B161" s="29">
+        <v>5</v>
+      </c>
+      <c r="C161" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="D161" s="32"/>
-    </row>
-    <row r="162" ht="38.25" spans="1:4">
-      <c r="A162" s="25"/>
-      <c r="B162" s="31"/>
-      <c r="C162" s="12" t="s">
+      <c r="D161" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="D162" s="32"/>
-    </row>
-    <row r="163" ht="54" spans="1:4">
-      <c r="A163" s="25"/>
-      <c r="B163" s="31">
-        <v>5</v>
-      </c>
-      <c r="C163" s="33" t="s">
+    </row>
+    <row r="162" ht="42" customHeight="1" spans="1:4">
+      <c r="A162" s="23"/>
+      <c r="B162" s="29"/>
+      <c r="C162" s="31" t="s">
         <v>253</v>
       </c>
-      <c r="D163" s="32" t="s">
+      <c r="D162" s="30" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="164" ht="25.5" spans="1:4">
-      <c r="A164" s="25"/>
-      <c r="B164" s="31"/>
+    <row r="163" ht="31.5" spans="1:5">
+      <c r="A163" s="23"/>
+      <c r="B163" s="29"/>
+      <c r="C163" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="D163" s="30"/>
+      <c r="E163" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="164" ht="31.5" spans="1:4">
+      <c r="A164" s="23"/>
+      <c r="B164" s="29"/>
       <c r="C164" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="D164" s="32"/>
-    </row>
-    <row r="165" ht="25.5" spans="1:5">
-      <c r="A165" s="25"/>
-      <c r="B165" s="31">
-        <v>5</v>
-      </c>
-      <c r="C165" s="33" t="s">
         <v>256</v>
       </c>
-      <c r="D165" s="32" t="s">
+      <c r="D164" s="30"/>
+    </row>
+    <row r="165" ht="31.5" spans="1:4">
+      <c r="A165" s="23"/>
+      <c r="B165" s="29"/>
+      <c r="C165" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E165" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="166" ht="25.5" spans="1:4">
-      <c r="A166" s="25"/>
-      <c r="B166" s="31"/>
+      <c r="D165" s="30"/>
+    </row>
+    <row r="166" ht="31.5" spans="1:4">
+      <c r="A166" s="23"/>
+      <c r="B166" s="29"/>
       <c r="C166" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="D166" s="32"/>
-    </row>
-    <row r="167" ht="40.5" spans="1:4">
-      <c r="A167" s="25"/>
-      <c r="B167" s="31">
-        <v>5</v>
-      </c>
+      <c r="D166" s="30"/>
+    </row>
+    <row r="167" ht="47.25" spans="1:4">
+      <c r="A167" s="23"/>
+      <c r="B167" s="29"/>
       <c r="C167" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="D167" s="32" t="s">
+      <c r="D167" s="30"/>
+    </row>
+    <row r="168" ht="66" spans="1:4">
+      <c r="A168" s="23"/>
+      <c r="B168" s="29">
+        <v>5</v>
+      </c>
+      <c r="C168" s="31" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="168" ht="120.75" spans="1:4">
-      <c r="A168" s="25"/>
-      <c r="B168" s="31">
-        <v>5</v>
-      </c>
-      <c r="C168" s="12" t="s">
+      <c r="D168" s="30" t="s">
         <v>261</v>
       </c>
-      <c r="D168" s="32" t="s">
+    </row>
+    <row r="169" ht="31.5" spans="1:4">
+      <c r="A169" s="23"/>
+      <c r="B169" s="29"/>
+      <c r="C169" s="12" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="169" ht="108" spans="1:4">
-      <c r="A169" s="25"/>
-      <c r="B169" s="31">
-        <v>5</v>
-      </c>
-      <c r="C169" s="12" t="s">
+      <c r="D169" s="30"/>
+    </row>
+    <row r="170" ht="31.5" spans="1:5">
+      <c r="A170" s="23"/>
+      <c r="B170" s="29">
+        <v>5</v>
+      </c>
+      <c r="C170" s="31" t="s">
         <v>263</v>
       </c>
-      <c r="D169" s="32" t="s">
+      <c r="D170" s="30" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="170" spans="1:4">
-      <c r="A170" s="25"/>
-      <c r="B170" s="31"/>
-      <c r="C170" s="12"/>
-      <c r="D170" s="32"/>
-    </row>
-    <row r="171" spans="1:4">
-      <c r="A171" s="25"/>
-      <c r="B171" s="31"/>
-      <c r="C171" s="12"/>
-      <c r="D171" s="32"/>
-    </row>
-    <row r="172" ht="106.5" spans="1:4">
-      <c r="A172" s="34" t="s">
+      <c r="E170" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="171" ht="31.5" spans="1:4">
+      <c r="A171" s="23"/>
+      <c r="B171" s="29"/>
+      <c r="C171" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="B172" s="31">
+      <c r="D171" s="30"/>
+    </row>
+    <row r="172" ht="49.5" spans="1:4">
+      <c r="A172" s="23"/>
+      <c r="B172" s="29">
         <v>5</v>
       </c>
       <c r="C172" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="D172" s="11" t="s">
+      <c r="D172" s="30" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="173" ht="25.5" spans="1:4">
-      <c r="A173" s="34"/>
-      <c r="B173" s="31">
-        <v>1</v>
+    <row r="173" ht="147.75" spans="1:4">
+      <c r="A173" s="23"/>
+      <c r="B173" s="29">
+        <v>5</v>
       </c>
       <c r="C173" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="D173" s="11"/>
-    </row>
-    <row r="174" ht="25.5" spans="1:4">
-      <c r="A174" s="34"/>
-      <c r="B174" s="31">
-        <v>1</v>
+      <c r="D173" s="30" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="174" ht="132" spans="1:4">
+      <c r="A174" s="23"/>
+      <c r="B174" s="29">
+        <v>5</v>
       </c>
       <c r="C174" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="D174" s="12"/>
-    </row>
-    <row r="175" ht="25.5" spans="1:4">
-      <c r="A175" s="34"/>
-      <c r="B175" s="22">
-        <v>1</v>
-      </c>
-      <c r="C175" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="D175" s="11"/>
-    </row>
-    <row r="176" ht="27" spans="1:4">
-      <c r="A176" s="34"/>
-      <c r="B176" s="22">
-        <v>5</v>
-      </c>
-      <c r="C176" s="12" t="s">
+      <c r="D174" s="30" t="s">
         <v>271</v>
       </c>
-      <c r="D176" s="8" t="s">
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" s="23"/>
+      <c r="B175" s="29"/>
+      <c r="C175" s="12"/>
+      <c r="D175" s="30"/>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" s="23"/>
+      <c r="B176" s="29"/>
+      <c r="C176" s="12"/>
+      <c r="D176" s="30"/>
+    </row>
+    <row r="177" ht="130.5" spans="1:4">
+      <c r="A177" s="32" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="177" ht="25.5" spans="1:4">
-      <c r="A177" s="34"/>
-      <c r="B177" s="22">
-        <v>1</v>
+      <c r="B177" s="29">
+        <v>5</v>
       </c>
       <c r="C177" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="D177" s="11"/>
-    </row>
-    <row r="178" ht="25.5" spans="1:4">
-      <c r="A178" s="34"/>
-      <c r="B178" s="22">
+      <c r="D177" s="11" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="178" ht="31.5" spans="1:4">
+      <c r="A178" s="32"/>
+      <c r="B178" s="29">
         <v>1</v>
       </c>
       <c r="C178" s="12" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D178" s="11"/>
     </row>
-    <row r="179" ht="39.75" spans="1:4">
-      <c r="A179" s="34"/>
-      <c r="B179" s="22">
-        <v>5</v>
-      </c>
-      <c r="C179" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="D179" s="11" t="s">
+    <row r="179" ht="31.5" spans="1:4">
+      <c r="A179" s="32"/>
+      <c r="B179" s="29">
+        <v>1</v>
+      </c>
+      <c r="C179" s="12" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="180" ht="235" customHeight="1" spans="1:4">
-      <c r="A180" s="34"/>
-      <c r="B180" s="22">
-        <v>5</v>
-      </c>
-      <c r="C180" s="12" t="s">
+      <c r="D179" s="12"/>
+    </row>
+    <row r="180" ht="31.5" spans="1:4">
+      <c r="A180" s="32"/>
+      <c r="B180" s="20">
+        <v>1</v>
+      </c>
+      <c r="C180" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="D180" s="11" t="s">
+      <c r="D180" s="11"/>
+    </row>
+    <row r="181" ht="33" spans="1:4">
+      <c r="A181" s="32"/>
+      <c r="B181" s="20">
+        <v>5</v>
+      </c>
+      <c r="C181" s="12" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="181" ht="208" customHeight="1" spans="1:5">
-      <c r="A181" s="34"/>
-      <c r="B181" s="22">
-        <v>5</v>
-      </c>
-      <c r="C181" s="12" t="s">
+      <c r="D181" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="D181" s="11" t="s">
+    </row>
+    <row r="182" ht="31.5" spans="1:4">
+      <c r="A182" s="32"/>
+      <c r="B182" s="20">
+        <v>1</v>
+      </c>
+      <c r="C182" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="E181" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="182" ht="38" customHeight="1" spans="1:3">
-      <c r="A182" s="34"/>
-      <c r="B182" s="22">
+      <c r="D182" s="11"/>
+    </row>
+    <row r="183" ht="31.5" spans="1:4">
+      <c r="A183" s="32"/>
+      <c r="B183" s="20">
         <v>1</v>
       </c>
-      <c r="C182" s="2" t="s">
+      <c r="C183" s="12" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="183" ht="38" customHeight="1" spans="1:4">
-      <c r="A183" s="34"/>
-      <c r="B183" s="22">
-        <v>1</v>
-      </c>
-      <c r="C183" s="2" t="s">
+      <c r="D183" s="11"/>
+    </row>
+    <row r="184" ht="48.75" spans="1:4">
+      <c r="A184" s="32"/>
+      <c r="B184" s="20">
+        <v>5</v>
+      </c>
+      <c r="C184" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="D183" s="11"/>
-    </row>
-    <row r="184" ht="51" customHeight="1" spans="1:4">
-      <c r="A184" s="34"/>
-      <c r="B184" s="22">
-        <v>1</v>
-      </c>
-      <c r="C184" s="12" t="s">
+      <c r="D184" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="D184" s="2" t="s">
+    </row>
+    <row r="185" ht="235" customHeight="1" spans="1:4">
+      <c r="A185" s="32"/>
+      <c r="B185" s="20">
+        <v>5</v>
+      </c>
+      <c r="C185" s="12" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="185" ht="28" customHeight="1" spans="1:4">
-      <c r="A185" s="34"/>
-      <c r="B185" s="22"/>
-      <c r="C185" s="12"/>
-      <c r="D185" s="11"/>
-    </row>
-    <row r="186" ht="34" customHeight="1" spans="1:4">
-      <c r="A186" s="34" t="s">
+      <c r="D185" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="B186" s="22">
-        <v>2</v>
+    </row>
+    <row r="186" ht="208" customHeight="1" spans="1:5">
+      <c r="A186" s="32"/>
+      <c r="B186" s="20">
+        <v>5</v>
       </c>
       <c r="C186" s="12" t="s">
         <v>286</v>
@@ -5040,623 +5051,677 @@
       <c r="D186" s="11" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="187" ht="58" customHeight="1" spans="1:4">
-      <c r="A187" s="34"/>
-      <c r="B187" s="31">
+      <c r="E186" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="187" ht="38" customHeight="1" spans="1:3">
+      <c r="A187" s="32"/>
+      <c r="B187" s="20">
         <v>1</v>
       </c>
-      <c r="C187" s="12" t="s">
+      <c r="C187" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="D187" s="11"/>
-    </row>
-    <row r="188" ht="25.5" spans="1:4">
-      <c r="A188" s="34"/>
-      <c r="B188" s="22">
+    </row>
+    <row r="188" ht="38" customHeight="1" spans="1:4">
+      <c r="A188" s="32"/>
+      <c r="B188" s="20">
         <v>1</v>
       </c>
-      <c r="C188" s="12" t="s">
+      <c r="C188" s="2" t="s">
         <v>289</v>
       </c>
       <c r="D188" s="11"/>
     </row>
-    <row r="189" spans="1:4">
-      <c r="A189" s="34"/>
-      <c r="B189" s="22">
+    <row r="189" ht="51" customHeight="1" spans="1:4">
+      <c r="A189" s="32"/>
+      <c r="B189" s="20">
         <v>1</v>
       </c>
-      <c r="C189" s="2" t="s">
+      <c r="C189" s="12" t="s">
         <v>290</v>
       </c>
-      <c r="D189" s="11"/>
-    </row>
-    <row r="190" ht="25.5" spans="1:4">
-      <c r="A190" s="34"/>
-      <c r="B190" s="22">
+      <c r="D189" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="190" ht="28" customHeight="1" spans="1:4">
+      <c r="A190" s="32"/>
+      <c r="B190" s="20"/>
+      <c r="C190" s="12"/>
+      <c r="D190" s="11"/>
+    </row>
+    <row r="191" ht="34" customHeight="1" spans="1:4">
+      <c r="A191" s="32" t="s">
+        <v>292</v>
+      </c>
+      <c r="B191" s="20">
+        <v>2</v>
+      </c>
+      <c r="C191" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="D191" s="11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="192" ht="58" customHeight="1" spans="1:4">
+      <c r="A192" s="32"/>
+      <c r="B192" s="29">
         <v>1</v>
       </c>
-      <c r="C190" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="D190" s="11"/>
-    </row>
-    <row r="191" spans="1:4">
-      <c r="A191" s="34"/>
-      <c r="B191" s="22">
+      <c r="C192" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="D192" s="11"/>
+    </row>
+    <row r="193" ht="31.5" spans="1:4">
+      <c r="A193" s="32"/>
+      <c r="B193" s="20">
         <v>1</v>
       </c>
-      <c r="C191" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="D191" s="11"/>
-    </row>
-    <row r="192" ht="25.5" spans="1:4">
-      <c r="A192" s="34"/>
-      <c r="B192" s="22">
+      <c r="C193" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="D193" s="11"/>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" s="32"/>
+      <c r="B194" s="20">
         <v>1</v>
       </c>
-      <c r="C192" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="D192" s="11"/>
-    </row>
-    <row r="193" ht="25.5" spans="1:4">
-      <c r="A193" s="34"/>
-      <c r="B193" s="22">
+      <c r="C194" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D194" s="11"/>
+    </row>
+    <row r="195" ht="31.5" spans="1:4">
+      <c r="A195" s="32"/>
+      <c r="B195" s="20">
         <v>1</v>
       </c>
-      <c r="C193" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="D193" s="11"/>
-    </row>
-    <row r="194" ht="25.5" spans="1:4">
-      <c r="A194" s="34"/>
-      <c r="B194" s="22">
+      <c r="C195" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D195" s="11"/>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" s="32"/>
+      <c r="B196" s="20">
         <v>1</v>
       </c>
-      <c r="C194" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="D194" s="11"/>
-    </row>
-    <row r="195" ht="25.5" spans="1:4">
-      <c r="A195" s="34"/>
-      <c r="B195" s="22">
+      <c r="C196" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D196" s="11"/>
+    </row>
+    <row r="197" ht="31.5" spans="1:4">
+      <c r="A197" s="32"/>
+      <c r="B197" s="20">
         <v>1</v>
       </c>
-      <c r="C195" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D195" s="11"/>
-    </row>
-    <row r="196" ht="25.5" spans="1:4">
-      <c r="A196" s="34"/>
-      <c r="B196" s="22">
+      <c r="C197" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D197" s="11"/>
+    </row>
+    <row r="198" ht="31.5" spans="1:4">
+      <c r="A198" s="32"/>
+      <c r="B198" s="20">
         <v>1</v>
       </c>
-      <c r="C196" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D196" s="11"/>
-    </row>
-    <row r="197" spans="1:4">
-      <c r="A197" s="34"/>
-      <c r="B197" s="22">
+      <c r="C198" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D198" s="11"/>
+    </row>
+    <row r="199" ht="31.5" spans="1:4">
+      <c r="A199" s="32"/>
+      <c r="B199" s="20">
         <v>1</v>
       </c>
-      <c r="C197" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="D197" s="11"/>
-    </row>
-    <row r="198" ht="54" spans="1:4">
-      <c r="A198" s="34"/>
-      <c r="B198" s="22">
-        <v>5</v>
-      </c>
-      <c r="C198" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="D198" s="11" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="199" ht="38.25" spans="1:4">
-      <c r="A199" s="34"/>
-      <c r="B199" s="22">
+      <c r="C199" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D199" s="11"/>
+    </row>
+    <row r="200" ht="31.5" spans="1:4">
+      <c r="A200" s="32"/>
+      <c r="B200" s="20">
         <v>1</v>
       </c>
-      <c r="C199" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="D199" s="11"/>
-    </row>
-    <row r="200" ht="66.75" spans="1:4">
-      <c r="A200" s="34"/>
-      <c r="B200" s="22">
-        <v>5</v>
-      </c>
       <c r="C200" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="D200" s="11" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="201" ht="81" spans="1:4">
-      <c r="A201" s="34"/>
-      <c r="B201" s="22">
-        <v>5</v>
+      <c r="D200" s="11"/>
+    </row>
+    <row r="201" ht="31.5" spans="1:4">
+      <c r="A201" s="32"/>
+      <c r="B201" s="20">
+        <v>1</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="D201" s="11" t="s">
+      <c r="D201" s="11"/>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202" s="32"/>
+      <c r="B202" s="20">
+        <v>1</v>
+      </c>
+      <c r="C202" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="202" ht="53.25" spans="1:4">
-      <c r="A202" s="34"/>
-      <c r="B202" s="22">
-        <v>5</v>
-      </c>
-      <c r="C202" s="2" t="s">
+      <c r="D202" s="11"/>
+    </row>
+    <row r="203" ht="66" spans="1:4">
+      <c r="A203" s="32"/>
+      <c r="B203" s="20">
+        <v>5</v>
+      </c>
+      <c r="C203" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="D202" s="11" t="s">
+      <c r="D203" s="11" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="203" ht="93" spans="1:4">
-      <c r="A203" s="34"/>
-      <c r="B203" s="22">
-        <v>5</v>
-      </c>
-      <c r="C203" s="12" t="s">
+    <row r="204" ht="47.25" spans="1:4">
+      <c r="A204" s="32"/>
+      <c r="B204" s="20">
+        <v>1</v>
+      </c>
+      <c r="C204" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="D203" s="35" t="s">
+      <c r="D204" s="11"/>
+    </row>
+    <row r="205" ht="81.75" spans="1:4">
+      <c r="A205" s="32"/>
+      <c r="B205" s="20">
+        <v>5</v>
+      </c>
+      <c r="C205" s="2" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="204" ht="93.75" spans="1:4">
-      <c r="A204" s="34" t="s">
+      <c r="D205" s="11" t="s">
         <v>310</v>
       </c>
-      <c r="B204" s="22">
-        <v>5</v>
-      </c>
-      <c r="C204" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="D204" s="11" t="s">
+    </row>
+    <row r="206" ht="99" spans="1:4">
+      <c r="A206" s="32"/>
+      <c r="B206" s="20">
+        <v>5</v>
+      </c>
+      <c r="C206" s="2" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="205" ht="66.75" spans="1:4">
-      <c r="A205" s="34"/>
-      <c r="B205" s="22">
-        <v>5</v>
-      </c>
-      <c r="C205" s="12" t="s">
+      <c r="D206" s="11" t="s">
         <v>312</v>
       </c>
-      <c r="D205" s="35" t="s">
+    </row>
+    <row r="207" ht="65.25" spans="1:4">
+      <c r="A207" s="32"/>
+      <c r="B207" s="20">
+        <v>5</v>
+      </c>
+      <c r="C207" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="206" ht="94.5" spans="1:4">
-      <c r="A206" s="34"/>
-      <c r="B206" s="22">
-        <v>5</v>
-      </c>
-      <c r="C206" s="12" t="s">
+      <c r="D207" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="D206" s="35" t="s">
+    </row>
+    <row r="208" ht="114" spans="1:4">
+      <c r="A208" s="32"/>
+      <c r="B208" s="20">
+        <v>5</v>
+      </c>
+      <c r="C208" s="12" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="207" ht="27" spans="1:4">
-      <c r="A207" s="34"/>
-      <c r="B207" s="22">
-        <v>5</v>
-      </c>
-      <c r="C207" s="12" t="s">
+      <c r="D208" s="33" t="s">
         <v>316</v>
       </c>
-      <c r="D207" s="35" t="s">
+    </row>
+    <row r="209" ht="114.75" spans="1:4">
+      <c r="A209" s="32" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="208" ht="25.5" spans="1:4">
-      <c r="A208" s="34"/>
-      <c r="B208" s="22"/>
-      <c r="C208" s="12" t="s">
+      <c r="B209" s="20">
+        <v>5</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="D209" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="D208" s="35"/>
-    </row>
-    <row r="209" ht="27" spans="1:4">
-      <c r="A209" s="34"/>
-      <c r="B209" s="22"/>
-      <c r="C209" s="12" t="s">
+    </row>
+    <row r="210" ht="81.75" spans="1:4">
+      <c r="A210" s="32"/>
+      <c r="B210" s="20">
+        <v>5</v>
+      </c>
+      <c r="C210" s="12" t="s">
         <v>319</v>
       </c>
-      <c r="D209" s="35" t="s">
+      <c r="D210" s="33" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="210" spans="1:4">
-      <c r="A210" s="34"/>
-      <c r="B210" s="22"/>
-      <c r="C210" s="12"/>
-      <c r="D210" s="35"/>
-    </row>
-    <row r="211" spans="1:4">
-      <c r="A211" s="34"/>
-      <c r="B211" s="22"/>
-      <c r="C211" s="12"/>
-      <c r="D211" s="35"/>
-    </row>
-    <row r="212" spans="1:4">
-      <c r="A212" s="34"/>
-      <c r="B212" s="22"/>
-      <c r="C212" s="12"/>
-      <c r="D212" s="35"/>
-    </row>
-    <row r="213" ht="40.5" spans="1:4">
-      <c r="A213" s="34" t="s">
+    <row r="211" ht="115.5" spans="1:4">
+      <c r="A211" s="32"/>
+      <c r="B211" s="20">
+        <v>5</v>
+      </c>
+      <c r="C211" s="12" t="s">
         <v>321</v>
       </c>
-      <c r="B213" s="22">
-        <v>5</v>
-      </c>
+      <c r="D211" s="33" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="212" ht="33" spans="1:4">
+      <c r="A212" s="32"/>
+      <c r="B212" s="20">
+        <v>5</v>
+      </c>
+      <c r="C212" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="D212" s="33" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="213" ht="31.5" spans="1:4">
+      <c r="A213" s="32"/>
+      <c r="B213" s="20"/>
       <c r="C213" s="12" t="s">
-        <v>322</v>
-      </c>
-      <c r="D213" s="35" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="214" ht="144" spans="1:4">
-      <c r="A214" s="34"/>
-      <c r="B214" s="22">
-        <v>5</v>
-      </c>
+        <v>325</v>
+      </c>
+      <c r="D213" s="33"/>
+    </row>
+    <row r="214" ht="33" spans="1:4">
+      <c r="A214" s="32"/>
+      <c r="B214" s="20"/>
       <c r="C214" s="12" t="s">
-        <v>324</v>
-      </c>
-      <c r="D214" s="36" t="s">
-        <v>325</v>
+        <v>326</v>
+      </c>
+      <c r="D214" s="33" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="215" spans="1:4">
-      <c r="A215" s="34"/>
-      <c r="B215" s="22"/>
+      <c r="A215" s="32"/>
+      <c r="B215" s="20"/>
       <c r="C215" s="12"/>
-      <c r="D215" s="35"/>
+      <c r="D215" s="33"/>
     </row>
     <row r="216" spans="1:4">
-      <c r="A216" s="34"/>
-      <c r="B216" s="22"/>
+      <c r="A216" s="32"/>
+      <c r="B216" s="20"/>
       <c r="C216" s="12"/>
-      <c r="D216" s="35"/>
+      <c r="D216" s="33"/>
     </row>
     <row r="217" spans="1:4">
-      <c r="A217" s="34"/>
-      <c r="B217" s="22"/>
+      <c r="A217" s="32"/>
+      <c r="B217" s="20"/>
       <c r="C217" s="12"/>
-      <c r="D217" s="35"/>
-    </row>
-    <row r="218" spans="1:4">
-      <c r="A218" s="34"/>
-      <c r="B218" s="22"/>
-      <c r="C218" s="12"/>
-      <c r="D218" s="35"/>
-    </row>
-    <row r="219" spans="1:4">
-      <c r="A219" s="34"/>
-      <c r="B219" s="22"/>
-      <c r="C219" s="12"/>
-      <c r="D219" s="35"/>
+      <c r="D217" s="33"/>
+    </row>
+    <row r="218" ht="49.5" spans="1:4">
+      <c r="A218" s="32" t="s">
+        <v>328</v>
+      </c>
+      <c r="B218" s="20">
+        <v>5</v>
+      </c>
+      <c r="C218" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="D218" s="33" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="219" ht="177" spans="1:4">
+      <c r="A219" s="32"/>
+      <c r="B219" s="20">
+        <v>5</v>
+      </c>
+      <c r="C219" s="12" t="s">
+        <v>331</v>
+      </c>
+      <c r="D219" s="34" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="220" spans="1:4">
-      <c r="A220" s="34"/>
-      <c r="B220" s="22"/>
+      <c r="A220" s="32"/>
+      <c r="B220" s="20"/>
       <c r="C220" s="12"/>
-      <c r="D220" s="35"/>
-    </row>
-    <row r="221" ht="25.5" spans="1:4">
-      <c r="A221" s="34" t="s">
-        <v>326</v>
-      </c>
-      <c r="B221" s="22"/>
-      <c r="C221" s="12" t="s">
-        <v>327</v>
-      </c>
-      <c r="D221" s="35" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="222" ht="40.5" spans="1:4">
-      <c r="A222" s="34"/>
-      <c r="B222" s="22">
-        <v>5</v>
-      </c>
-      <c r="C222" s="12" t="s">
-        <v>329</v>
-      </c>
-      <c r="D222" s="11" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="223" ht="38.25" spans="1:4">
-      <c r="A223" s="34"/>
-      <c r="B223" s="22">
-        <v>5</v>
-      </c>
-      <c r="C223" s="12" t="s">
-        <v>331</v>
-      </c>
-      <c r="D223" s="11" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="224" ht="109" customHeight="1" spans="1:4">
-      <c r="A224" s="34"/>
-      <c r="B224" s="22">
-        <v>5</v>
-      </c>
-      <c r="C224" s="12" t="s">
+      <c r="D220" s="33"/>
+    </row>
+    <row r="221" spans="1:4">
+      <c r="A221" s="32"/>
+      <c r="B221" s="20"/>
+      <c r="C221" s="12"/>
+      <c r="D221" s="33"/>
+    </row>
+    <row r="222" spans="1:4">
+      <c r="A222" s="32"/>
+      <c r="B222" s="20"/>
+      <c r="C222" s="12"/>
+      <c r="D222" s="33"/>
+    </row>
+    <row r="223" spans="1:4">
+      <c r="A223" s="32"/>
+      <c r="B223" s="20"/>
+      <c r="C223" s="12"/>
+      <c r="D223" s="33"/>
+    </row>
+    <row r="224" spans="1:4">
+      <c r="A224" s="32"/>
+      <c r="B224" s="20"/>
+      <c r="C224" s="12"/>
+      <c r="D224" s="33"/>
+    </row>
+    <row r="225" spans="1:4">
+      <c r="A225" s="32"/>
+      <c r="B225" s="20"/>
+      <c r="C225" s="12"/>
+      <c r="D225" s="33"/>
+    </row>
+    <row r="226" ht="31.5" spans="1:4">
+      <c r="A226" s="32" t="s">
         <v>333</v>
       </c>
-      <c r="D224" s="11" t="s">
+      <c r="B226" s="20"/>
+      <c r="C226" s="12" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="225" ht="28.5" spans="1:4">
-      <c r="A225" s="34"/>
-      <c r="B225" s="22">
-        <v>5</v>
-      </c>
-      <c r="C225" s="30" t="s">
+      <c r="D226" s="33" t="s">
         <v>335</v>
       </c>
-      <c r="D225" s="11" t="s">
+    </row>
+    <row r="227" ht="49.5" spans="1:4">
+      <c r="A227" s="32"/>
+      <c r="B227" s="20">
+        <v>5</v>
+      </c>
+      <c r="C227" s="12" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="226" ht="27" spans="1:4">
-      <c r="A226" s="34" t="s">
+      <c r="D227" s="11" t="s">
         <v>337</v>
       </c>
-      <c r="B226" s="22">
-        <v>5</v>
-      </c>
-      <c r="C226" s="37" t="s">
+    </row>
+    <row r="228" ht="47.25" spans="1:4">
+      <c r="A228" s="32"/>
+      <c r="B228" s="20">
+        <v>5</v>
+      </c>
+      <c r="C228" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="D226" s="37" t="s">
+      <c r="D228" s="11" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="227" ht="67" customHeight="1" spans="1:4">
-      <c r="A227" s="34"/>
-      <c r="B227" s="22">
-        <v>5</v>
-      </c>
-      <c r="C227" s="12" t="s">
+    <row r="229" ht="109" customHeight="1" spans="1:4">
+      <c r="A229" s="32"/>
+      <c r="B229" s="20">
+        <v>5</v>
+      </c>
+      <c r="C229" s="12" t="s">
         <v>340</v>
       </c>
-      <c r="D227" s="12" t="s">
+      <c r="D229" s="11" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="228" ht="42" customHeight="1" spans="1:4">
-      <c r="A228" s="34"/>
-      <c r="B228" s="22">
-        <v>5</v>
-      </c>
-      <c r="C228" s="12" t="s">
+    <row r="230" ht="33" spans="1:4">
+      <c r="A230" s="32"/>
+      <c r="B230" s="20">
+        <v>5</v>
+      </c>
+      <c r="C230" s="28" t="s">
         <v>342</v>
       </c>
-      <c r="D228" s="12" t="s">
+      <c r="D230" s="11" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="229" ht="82" customHeight="1" spans="1:4">
-      <c r="A229" s="34"/>
-      <c r="B229" s="22">
-        <v>5</v>
-      </c>
-      <c r="C229" s="12" t="s">
+    <row r="231" ht="33" spans="1:4">
+      <c r="A231" s="32" t="s">
         <v>344</v>
       </c>
-      <c r="D229" s="12" t="s">
+      <c r="B231" s="20">
+        <v>5</v>
+      </c>
+      <c r="C231" s="35" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="230" ht="39.75" spans="1:4">
-      <c r="A230" s="34"/>
-      <c r="B230" s="31">
-        <v>5</v>
-      </c>
-      <c r="C230" s="12" t="s">
+      <c r="D231" s="35" t="s">
         <v>346</v>
       </c>
-      <c r="D230" s="12" t="s">
+    </row>
+    <row r="232" ht="67" customHeight="1" spans="1:4">
+      <c r="A232" s="32"/>
+      <c r="B232" s="20">
+        <v>5</v>
+      </c>
+      <c r="C232" s="12" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="231" ht="13.5" spans="1:4">
-      <c r="A231" s="34"/>
-      <c r="B231" s="22">
-        <v>5</v>
-      </c>
-      <c r="C231" s="12" t="s">
+      <c r="D232" s="12" t="s">
         <v>348</v>
       </c>
-      <c r="D231" s="12" t="s">
+    </row>
+    <row r="233" ht="42" customHeight="1" spans="1:4">
+      <c r="A233" s="32"/>
+      <c r="B233" s="20">
+        <v>5</v>
+      </c>
+      <c r="C233" s="12" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="232" ht="409.5" spans="1:4">
-      <c r="A232" s="34" t="s">
+      <c r="D233" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="B232" s="22">
-        <v>5</v>
-      </c>
-      <c r="C232" s="38" t="s">
+    </row>
+    <row r="234" ht="82" customHeight="1" spans="1:4">
+      <c r="A234" s="32"/>
+      <c r="B234" s="20">
+        <v>5</v>
+      </c>
+      <c r="C234" s="12" t="s">
         <v>351</v>
       </c>
-      <c r="D232" s="12" t="s">
+      <c r="D234" s="12" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="233" ht="40.5" spans="1:4">
-      <c r="A233" s="34"/>
-      <c r="B233" s="22">
-        <v>5</v>
-      </c>
-      <c r="C233" s="39" t="s">
+    <row r="235" ht="48.75" spans="1:4">
+      <c r="A235" s="32"/>
+      <c r="B235" s="29">
+        <v>5</v>
+      </c>
+      <c r="C235" s="12" t="s">
         <v>353</v>
       </c>
-      <c r="D233" s="12" t="s">
+      <c r="D235" s="12" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="234" ht="27" spans="1:4">
-      <c r="A234" s="34"/>
-      <c r="B234" s="22">
-        <v>5</v>
-      </c>
-      <c r="C234" s="40" t="s">
+    <row r="236" ht="16.5" spans="1:4">
+      <c r="A236" s="32"/>
+      <c r="B236" s="20">
+        <v>5</v>
+      </c>
+      <c r="C236" s="12" t="s">
         <v>355</v>
       </c>
-      <c r="D234" s="12" t="s">
+      <c r="D236" s="12" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="235" ht="13.5" spans="1:4">
-      <c r="A235" s="34"/>
-      <c r="B235" s="22">
-        <v>5</v>
-      </c>
-      <c r="C235" s="40" t="s">
+    <row r="237" ht="409.5" spans="1:4">
+      <c r="A237" s="32" t="s">
         <v>357</v>
       </c>
-      <c r="D235" s="12" t="s">
+      <c r="B237" s="20">
+        <v>5</v>
+      </c>
+      <c r="C237" s="19" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="236" ht="145.5" spans="1:4">
-      <c r="A236" s="34"/>
-      <c r="B236" s="22">
-        <v>5</v>
-      </c>
-      <c r="C236" s="40" t="s">
+      <c r="D237" s="12" t="s">
         <v>359</v>
       </c>
-      <c r="D236" s="12" t="s">
+    </row>
+    <row r="238" ht="49.5" spans="1:4">
+      <c r="A238" s="32"/>
+      <c r="B238" s="20">
+        <v>5</v>
+      </c>
+      <c r="C238" s="36" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="237" spans="1:4">
-      <c r="A237" s="34"/>
-      <c r="B237" s="22"/>
-      <c r="C237" s="40"/>
-      <c r="D237" s="12"/>
-    </row>
-    <row r="238" spans="1:4">
-      <c r="A238" s="34"/>
-      <c r="B238" s="22"/>
-      <c r="C238" s="40"/>
-      <c r="D238" s="12"/>
-    </row>
-    <row r="239" spans="1:4">
-      <c r="A239" s="34"/>
-      <c r="B239" s="22"/>
-      <c r="C239" s="40"/>
-      <c r="D239" s="12"/>
-    </row>
-    <row r="240" spans="1:4">
-      <c r="A240" s="34"/>
-      <c r="B240" s="22"/>
-      <c r="C240" s="40"/>
-      <c r="D240" s="12"/>
-    </row>
-    <row r="241" spans="1:4">
-      <c r="A241" s="34"/>
-      <c r="B241" s="22"/>
-      <c r="C241" s="40"/>
-      <c r="D241" s="12"/>
-    </row>
-    <row r="242" ht="220" customHeight="1" spans="1:4">
-      <c r="A242" s="34" t="s">
+      <c r="D238" s="12" t="s">
         <v>361</v>
       </c>
-      <c r="B242" s="22">
-        <v>5</v>
-      </c>
-      <c r="C242" s="12" t="s">
+    </row>
+    <row r="239" ht="33" spans="1:4">
+      <c r="A239" s="32"/>
+      <c r="B239" s="20">
+        <v>5</v>
+      </c>
+      <c r="C239" s="30" t="s">
         <v>362</v>
       </c>
-      <c r="D242" s="12" t="s">
+      <c r="D239" s="12" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="243" ht="25.5" spans="1:4">
-      <c r="A243" s="34"/>
-      <c r="B243" s="22">
-        <v>5</v>
-      </c>
-      <c r="C243" s="12" t="s">
+    <row r="240" ht="16.5" spans="1:4">
+      <c r="A240" s="32"/>
+      <c r="B240" s="20">
+        <v>5</v>
+      </c>
+      <c r="C240" s="30" t="s">
         <v>364</v>
       </c>
-      <c r="D243" s="12" t="s">
+      <c r="D240" s="12" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="244" ht="106.5" spans="1:4">
-      <c r="A244" s="34"/>
-      <c r="B244" s="22">
-        <v>5</v>
-      </c>
-      <c r="C244" s="2" t="s">
+    <row r="241" ht="178.5" spans="1:4">
+      <c r="A241" s="32"/>
+      <c r="B241" s="20">
+        <v>5</v>
+      </c>
+      <c r="C241" s="30" t="s">
         <v>366</v>
       </c>
-      <c r="D244" s="2" t="s">
+      <c r="D241" s="12" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="245" ht="104.25" spans="1:4">
-      <c r="A245" s="34"/>
-      <c r="B245" s="22"/>
-      <c r="C245" s="2" t="s">
+    <row r="242" spans="1:4">
+      <c r="A242" s="32"/>
+      <c r="B242" s="20"/>
+      <c r="C242" s="30"/>
+      <c r="D242" s="12"/>
+    </row>
+    <row r="243" spans="1:4">
+      <c r="A243" s="32"/>
+      <c r="B243" s="20"/>
+      <c r="C243" s="30"/>
+      <c r="D243" s="12"/>
+    </row>
+    <row r="244" spans="1:4">
+      <c r="A244" s="32"/>
+      <c r="B244" s="20"/>
+      <c r="C244" s="30"/>
+      <c r="D244" s="12"/>
+    </row>
+    <row r="245" spans="1:4">
+      <c r="A245" s="32"/>
+      <c r="B245" s="20"/>
+      <c r="C245" s="30"/>
+      <c r="D245" s="12"/>
+    </row>
+    <row r="246" spans="1:4">
+      <c r="A246" s="32"/>
+      <c r="B246" s="20"/>
+      <c r="C246" s="30"/>
+      <c r="D246" s="12"/>
+    </row>
+    <row r="247" ht="220" customHeight="1" spans="1:4">
+      <c r="A247" s="32" t="s">
         <v>368</v>
       </c>
-      <c r="D245" s="21" t="s">
+      <c r="B247" s="20">
+        <v>5</v>
+      </c>
+      <c r="C247" s="12" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="246" ht="39" spans="1:4">
-      <c r="A246" s="34"/>
-      <c r="B246" s="22">
-        <v>5</v>
-      </c>
-      <c r="C246" s="2" t="s">
+      <c r="D247" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="D246" s="2" t="s">
+    </row>
+    <row r="248" ht="31.5" spans="1:4">
+      <c r="A248" s="32"/>
+      <c r="B248" s="20">
+        <v>5</v>
+      </c>
+      <c r="C248" s="12" t="s">
         <v>371</v>
       </c>
+      <c r="D248" s="12" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="249" ht="130.5" spans="1:4">
+      <c r="A249" s="32"/>
+      <c r="B249" s="20">
+        <v>5</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="D249" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="250" ht="128.25" spans="1:4">
+      <c r="A250" s="32"/>
+      <c r="B250" s="20"/>
+      <c r="C250" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="D250" s="19" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="251" ht="48" spans="1:4">
+      <c r="A251" s="32"/>
+      <c r="B251" s="20">
+        <v>5</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="D251" s="2" t="s">
+        <v>378</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E246">
+  <autoFilter ref="E1:E251">
     <extLst/>
   </autoFilter>
   <mergeCells count="18">
@@ -5667,19 +5732,19 @@
     <mergeCell ref="A56:A59"/>
     <mergeCell ref="A60:A64"/>
     <mergeCell ref="A65:A82"/>
-    <mergeCell ref="A83:A91"/>
-    <mergeCell ref="A92:A171"/>
-    <mergeCell ref="A172:A185"/>
-    <mergeCell ref="A186:A187"/>
-    <mergeCell ref="A188:A203"/>
-    <mergeCell ref="A204:A212"/>
-    <mergeCell ref="A213:A220"/>
-    <mergeCell ref="A221:A225"/>
-    <mergeCell ref="A226:A231"/>
-    <mergeCell ref="A232:A241"/>
-    <mergeCell ref="A242:A246"/>
+    <mergeCell ref="A83:A96"/>
+    <mergeCell ref="A97:A176"/>
+    <mergeCell ref="A177:A190"/>
+    <mergeCell ref="A191:A192"/>
+    <mergeCell ref="A193:A208"/>
+    <mergeCell ref="A209:A217"/>
+    <mergeCell ref="A218:A225"/>
+    <mergeCell ref="A226:A230"/>
+    <mergeCell ref="A231:A236"/>
+    <mergeCell ref="A237:A246"/>
+    <mergeCell ref="A247:A251"/>
   </mergeCells>
-  <conditionalFormatting sqref="B172">
+  <conditionalFormatting sqref="B177">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -5690,7 +5755,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B54 B173:B1048576 B113:B171 B92:B111 B56:B90">
+  <conditionalFormatting sqref="B1:B54 B56:B95 B178:B1048576 B97:B116 B118:B176">
     <cfRule type="cellIs" dxfId="0" priority="4" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -5702,7 +5767,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C204" r:id="rId1" display="Panoptic Segmentation" tooltip="https://arxiv.org/abs/1801.00868"/>
+    <hyperlink ref="C209" r:id="rId1" display="Panoptic Segmentation" tooltip="https://arxiv.org/abs/1801.00868"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
add reading note 20200113
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$251</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$259</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="396">
   <si>
     <t>Scope</t>
   </si>
@@ -435,6 +435,21 @@
 of DNNs</t>
   </si>
   <si>
+    <t>Learning Affinity via Spatial Propagation Networks</t>
+  </si>
+  <si>
+    <t>SPN(Spatial Propagation Network): transform a two-dimensional map to a new one with desired properties(e.g. a new segmentation map with significatly refined details)
+通过弥散(diffusion)这种比较稀疏的方法提高每一点的receptive field, 3-way difusion能够使得每一个点都感受到整张图;
+3-way的计算量也比经典的non-local要小, 只有(NxNxCx3x4 &lt;&lt; NxNxCxNxN) 
+difussion和SGM的4/8/16 path 的cost aggregation是一样的;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Learning Depth with Convolutional Spatial Propagation Network</t>
+  </si>
+  <si>
+    <t>思想和SPN是一样的, 就是通过迭代, 慢慢扩大reciptive field(difussion)</t>
+  </si>
+  <si>
     <t>GAN
 and
 Style transfer</t>
@@ -684,6 +699,20 @@
   </si>
   <si>
     <t>(2019.09)Object-Centric Stereo Matching for 3D Object Detection</t>
+  </si>
+  <si>
+    <t>The performance gap between Lidar and pseudo-lidar is the streaking caused by ambiguity of depth valuers at object edge.
+贡献: 1. 提出了OC-stereo, 只估计fg object的深度, 缓解了在物体边界上深度估计不准确的问题, 提高了视差估计的速度; 2. 提出了一种缓解视差估计方法更"faver closer object"的方法;
+流程:.
+1. 左右图的2D bbox匹配: 高度和中心点disparity的对应关系筛选框 -&gt; 剩余的框都resize到同样的大小 -&gt; 用SSIM(Structure SIMilarity)算法匹配框; 
+2. object-centric Stereo Matching: 匹配的左右框中心点的视差为全局视差, 框内图片的视差为局部视差,  全局视差+局部视差为总视差; 训练的时候只取物体gt_mask里面的视差形成loss, 预测的时候只出mask覆盖的敌法的dipairty, 所以是object centric; 细节是把视差转换为深度再用L1 loss, 减轻了emphasis 在比较近的物体上;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RefinedMPL: Refined Monocular PseudoLiDAR for 3D Object Detection in Autonomous Driving</t>
+  </si>
+  <si>
+    <t>针对(单目)伪点云的点数多, bg/fg比例大, 质量不高的特点, 提出了一种unsupervise和一种supervise的方法, 对点云进行稀疏化和优化, 提高了基于pseudo-Lidar点云的算法的性能
+DSS: 距离分层采样, 越远的地方采样密度越高;</t>
   </si>
   <si>
     <t>image semantic segmentation</t>
@@ -1493,6 +1522,18 @@
   </si>
   <si>
     <t>针对全景分割中thing和stuff不重合的问题, 提出了thing and stuff consistency loss: thing head的每个ｏｂｊｅｃｔ拼成的ｍａｓｋ和语义分割 head属于stuff类别的channel拼成的mask做L2loss, 减小两个head之间的mismatch;</t>
+  </si>
+  <si>
+    <t>Panoptic-Deeplab: A Simple, Strong, and Fast Baseline for Bottom-Up Panoptic Segmentation</t>
+  </si>
+  <si>
+    <t>结构上用了DeeplabV3的的decoder做instance branch, instance mask预测每个instance的中心以及每个thing类别到中心的offset
+1. 语义分割: 结构和DeeplabV3一样
+2. 实例分割(class agnostic instance mask):  
+    instance中心预测: maxpool(stride=1) -&gt; 只保留pool前后值一样的点 -&gt; 过滤掉低阈值的点 -&gt; 只保留置信度最高的 top-k个点;
+    instance聚类: 对于thing-mask里面的点, 距离哪个中心最近, 就属于哪个instance;
+    instance的类别: 用这个instance罩住的semantic map的点做 majority-vote
+    instance的mask的置信度: 聚类中心的置信度与instance每个pixel对应的semantic score的均值的乘积: Score(Objectness) x Score(Class);</t>
   </si>
   <si>
     <t>车道线检测</t>
@@ -1647,6 +1688,51 @@
     <t>1. 用Enet做backbone，instance segmentation用了proposal free的方法</t>
   </si>
   <si>
+    <t xml:space="preserve"> Semantic Stereo Matching with Pyramid Cost Volumes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">两个点: 1. pyramid cost volumn; 2. 同时也做语义分割, 提高在不同类别边界处disparity的准确性; 
+这篇文章同时受segstereo的影响: SegStereo: Exploiting Semantic Information for Disparity Estimation:  https://github.com/yangguorun/SegStereo
+网络结构: 
+    a. 用Resnet50提取左右图的feature, 并用不同size的average pooling把feature变为1/4, 1/8, 1/16的尺寸;
+    b. 语义分割网络参考PSPNet, 左右图的feature都做输入 (不清楚的是, 最后只用一幅图feature出语义分割map, 还是左右图的psp之后的feature concate在一起出语义分割图)
+    c. yramid cost volume分为两部分: 1. sementic cost volumn: 用psp之后的feature构成3D cost volumn, 只在1/4这个level; 2. spatial cost volumn: 在1/4, 1/8, 1/16这几个level上构成3d cost volumn;
+    d. 3d-multi-cost aggregation: 其实也是一个Unet的结构, 3D hourglass 结构+3D attention模块, 见上面右图;
+Loss:
+    a. disparity用soft-argmax求出来;
+    b. Lbdry中, phi-x / phi-y是x/y 方向的intensity gradient(Lbdy可以解释为: 在类别的边界处, 视差也应该有大差异的, 因此可以使得网络对边缘的视差预测更好, 参考(2018.10, ACCV) Geometry meets semantics for semi-supervised monocular depth estimation, https://arxiv.org/pdf/1810.04093.pdf);
+</t>
+  </si>
+  <si>
+    <t>Look Deeper into Depth_Monocular Depth Estimation with Semantic Booster and Attention-Driven Loss</t>
+  </si>
+  <si>
+    <t>1. 设计了一个attention-driven loss, 减轻了网络对近处的pixel的bias, look deeper into the scene;
+        alpah_D: 和深度线性相关的loss weight;
+        lambda_D: 和学习过程有关，保证学习过程的稳定性；
+2. 设计了一个propagation stratagy, better incorporate semantics in depth estimation;
+3. 其实就是， 网络结构上， 深度和语义branch的信息相互shared； Loss上， 深度的梯度和语义的梯度相互制约；</t>
+  </si>
+  <si>
+    <t>SegStereo: Exploiting Semantic Information for Disparity Estimation</t>
+  </si>
+  <si>
+    <t>已经开源：  https://github.com/yangguorun/SegStereo
+同时训练深度和语义信息， unsupervise的方法比SGM效果好， supervise的方法在提交的时候是SOAT;
+没有用3D卷积；
+Lseg: 用disp把右图的seg feature warp到左图，再做softmax loss, 这样， Loss, 就能传递到预测视差的网络， Lseg是一直有监督的；</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SENSE: a Shared Encoder Network for Scene-flow Estimation
+</t>
+  </si>
+  <si>
+    <t>参考文献非常的详细；
+一个share encoder的多任务网络， 包含了scene-flow, 语义分割和disparity
+Loss是 supervised loss， Distilation Loss, Self-Supervised Loss的sum
+Self-Supervised Loss help a lot in sky region, 但是 Distilation Loss, Self-Supervised Loss的帮助其实并不多；</t>
+  </si>
+  <si>
     <t>stereo disparity estimation</t>
   </si>
   <si>
@@ -1787,10 +1873,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1849,6 +1935,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -1856,17 +1950,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1879,25 +1965,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1925,16 +1997,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1948,6 +2042,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1956,38 +2057,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2045,7 +2131,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2057,13 +2185,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2075,19 +2221,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2099,73 +2239,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2183,25 +2257,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2213,13 +2269,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2272,11 +2358,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2292,45 +2417,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2352,6 +2438,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -2360,162 +2455,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2992,12 +3078,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G251"/>
+  <dimension ref="A1:G259"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D92" sqref="D92"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="15.75" outlineLevelCol="6"/>
@@ -3648,252 +3734,264 @@
       </c>
       <c r="D54" s="12"/>
     </row>
-    <row r="55" ht="41" customHeight="1" spans="1:1">
+    <row r="55" ht="83" customHeight="1" spans="1:4">
       <c r="A55" s="9"/>
-    </row>
-    <row r="56" ht="183" customHeight="1" spans="1:4">
-      <c r="A56" s="18" t="s">
+      <c r="B55" s="17">
+        <v>5</v>
+      </c>
+      <c r="C55" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B56" s="14">
-        <v>5</v>
-      </c>
-      <c r="C56" s="2" t="s">
+      <c r="D55" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D56" s="2" t="s">
+    </row>
+    <row r="56" ht="53" customHeight="1" spans="1:4">
+      <c r="A56" s="9"/>
+      <c r="B56" s="17">
+        <v>5</v>
+      </c>
+      <c r="C56" s="12" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="57" ht="202" customHeight="1" spans="1:4">
-      <c r="A57" s="18"/>
-      <c r="B57" s="14">
-        <v>5</v>
-      </c>
-      <c r="C57" s="2" t="s">
+      <c r="D56" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D57" s="19" t="s">
+    </row>
+    <row r="57" ht="53" customHeight="1" spans="1:4">
+      <c r="A57" s="9"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+    </row>
+    <row r="58" ht="41" customHeight="1" spans="1:1">
+      <c r="A58" s="9"/>
+    </row>
+    <row r="59" ht="183" customHeight="1" spans="1:4">
+      <c r="A59" s="18" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="58" ht="43" customHeight="1" spans="1:4">
-      <c r="A58" s="18"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="2" t="s">
+      <c r="B59" s="14">
+        <v>5</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D58" s="19"/>
-    </row>
-    <row r="59" ht="69" customHeight="1" spans="1:3">
-      <c r="A59" s="18"/>
-      <c r="B59" s="14">
-        <v>1</v>
-      </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="60" ht="56" customHeight="1" spans="1:3">
-      <c r="A60" s="18" t="s">
+    <row r="60" ht="202" customHeight="1" spans="1:4">
+      <c r="A60" s="18"/>
+      <c r="B60" s="14">
+        <v>5</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="14"/>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="19" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="61" ht="30" customHeight="1" spans="1:3">
+    <row r="61" ht="43" customHeight="1" spans="1:4">
       <c r="A61" s="18"/>
       <c r="B61" s="14"/>
       <c r="C61" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="62" ht="29" customHeight="1" spans="1:3">
+      <c r="D61" s="19"/>
+    </row>
+    <row r="62" ht="69" customHeight="1" spans="1:3">
       <c r="A62" s="18"/>
-      <c r="B62" s="14"/>
+      <c r="B62" s="14">
+        <v>1</v>
+      </c>
       <c r="C62" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="63" ht="69" customHeight="1" spans="1:3">
-      <c r="A63" s="18"/>
+    <row r="63" ht="56" customHeight="1" spans="1:3">
+      <c r="A63" s="18" t="s">
+        <v>107</v>
+      </c>
       <c r="B63" s="14"/>
       <c r="C63" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="64" ht="69" customHeight="1" spans="1:2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="64" ht="30" customHeight="1" spans="1:3">
       <c r="A64" s="18"/>
       <c r="B64" s="14"/>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B65" s="14">
-        <v>5</v>
-      </c>
-      <c r="C65" s="11" t="s">
+      <c r="C64" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D65" s="11"/>
-      <c r="F65" s="24"/>
-      <c r="G65" s="24"/>
-    </row>
-    <row r="66" ht="63.75" spans="1:6">
-      <c r="A66" s="9"/>
-      <c r="B66" s="14">
-        <v>5</v>
-      </c>
-      <c r="C66" s="11" t="s">
+    </row>
+    <row r="65" ht="29" customHeight="1" spans="1:3">
+      <c r="A65" s="18"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D66" s="11" t="s">
+    </row>
+    <row r="66" ht="69" customHeight="1" spans="1:3">
+      <c r="A66" s="18"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F66" s="1"/>
-    </row>
-    <row r="67" ht="33" spans="1:4">
-      <c r="A67" s="9"/>
-      <c r="B67" s="10">
-        <v>5</v>
-      </c>
-      <c r="C67" s="11" t="s">
+    </row>
+    <row r="67" ht="69" customHeight="1" spans="1:2">
+      <c r="A67" s="18"/>
+      <c r="B67" s="14"/>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D67" s="11" t="s">
+      <c r="B68" s="14">
+        <v>5</v>
+      </c>
+      <c r="C68" s="11" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="68" ht="81.75" spans="1:4">
-      <c r="A68" s="9"/>
-      <c r="B68" s="10">
-        <v>5</v>
-      </c>
-      <c r="C68" s="11" t="s">
+      <c r="D68" s="11"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="24"/>
+    </row>
+    <row r="69" ht="63.75" spans="1:6">
+      <c r="A69" s="9"/>
+      <c r="B69" s="14">
+        <v>5</v>
+      </c>
+      <c r="C69" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D68" s="11" t="s">
+      <c r="D69" s="11" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="69" ht="31.5" spans="1:4">
-      <c r="A69" s="9"/>
-      <c r="B69" s="20">
-        <v>5</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D69" s="11" t="s">
-        <v>117</v>
-      </c>
+      <c r="F69" s="1"/>
     </row>
     <row r="70" ht="33" spans="1:4">
       <c r="A70" s="9"/>
       <c r="B70" s="10">
         <v>5</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>118</v>
+      <c r="C70" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="71" ht="31.5" spans="1:4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="71" ht="81.75" spans="1:4">
       <c r="A71" s="9"/>
       <c r="B71" s="10">
-        <v>2</v>
-      </c>
-      <c r="C71" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="72" ht="31.5" spans="1:4">
+      <c r="A72" s="9"/>
+      <c r="B72" s="20">
+        <v>5</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D71" s="11"/>
-    </row>
-    <row r="72" ht="80.25" spans="1:4">
-      <c r="A72" s="9"/>
-      <c r="B72" s="10">
-        <v>5</v>
-      </c>
-      <c r="C72" s="12" t="s">
+      <c r="D72" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="D72" s="11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="73" ht="49.5" spans="1:4">
+    </row>
+    <row r="73" ht="33" spans="1:4">
       <c r="A73" s="9"/>
       <c r="B73" s="10">
         <v>5</v>
       </c>
-      <c r="C73" s="12" t="s">
+      <c r="C73" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D73" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="D73" s="11" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="74" ht="47.25" spans="1:4">
+    </row>
+    <row r="74" ht="31.5" spans="1:4">
       <c r="A74" s="9"/>
       <c r="B74" s="10">
-        <v>1</v>
-      </c>
-      <c r="C74" s="12" t="s">
-        <v>125</v>
+        <v>2</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="D74" s="11"/>
     </row>
-    <row r="75" ht="31.5" spans="1:4">
+    <row r="75" ht="80.25" spans="1:4">
       <c r="A75" s="9"/>
       <c r="B75" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C75" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D75" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="D75" s="11"/>
-    </row>
-    <row r="76" spans="1:4">
+    </row>
+    <row r="76" ht="49.5" spans="1:4">
       <c r="A76" s="9"/>
       <c r="B76" s="10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C76" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="D76" s="11"/>
-    </row>
-    <row r="77" ht="31.5" spans="1:4">
+      <c r="D76" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="77" ht="47.25" spans="1:4">
       <c r="A77" s="9"/>
       <c r="B77" s="10">
         <v>1</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D77" s="11"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" ht="31.5" spans="1:4">
       <c r="A78" s="9"/>
-      <c r="B78" s="21"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
+      <c r="B78" s="10">
+        <v>1</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D78" s="11"/>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="9"/>
-      <c r="B79" s="21"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="B79" s="10">
+        <v>1</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D79" s="11"/>
+    </row>
+    <row r="80" ht="31.5" spans="1:4">
       <c r="A80" s="9"/>
-      <c r="B80" s="21"/>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
+      <c r="B80" s="10">
+        <v>1</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D80" s="11"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="9"/>
@@ -3907,343 +4005,332 @@
       <c r="C82" s="12"/>
       <c r="D82" s="12"/>
     </row>
-    <row r="83" ht="82.5" spans="1:4">
-      <c r="A83" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="B83" s="21">
-        <v>5</v>
-      </c>
-      <c r="C83" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="D83" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="84" ht="276.75" spans="1:4">
-      <c r="A84" s="22"/>
-      <c r="B84" s="21">
-        <v>5</v>
-      </c>
-      <c r="C84" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="D84" s="12" t="s">
+    <row r="83" spans="1:4">
+      <c r="A83" s="9"/>
+      <c r="B83" s="21"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="9"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="9"/>
+      <c r="B85" s="21"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+    </row>
+    <row r="86" ht="82.5" spans="1:4">
+      <c r="A86" s="22" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="85" ht="47.25" spans="1:4">
-      <c r="A85" s="22"/>
-      <c r="B85" s="21">
-        <v>5</v>
-      </c>
-      <c r="C85" s="12" t="s">
+      <c r="B86" s="21">
+        <v>5</v>
+      </c>
+      <c r="C86" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="D85" s="12" t="s">
+      <c r="D86" s="12" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="86" ht="49.5" spans="1:4">
-      <c r="A86" s="22"/>
-      <c r="B86" s="21">
-        <v>5</v>
-      </c>
-      <c r="C86" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="D86" s="12" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="87" ht="144" spans="1:4">
+    <row r="87" ht="276.75" spans="1:4">
       <c r="A87" s="22"/>
       <c r="B87" s="21">
         <v>5</v>
       </c>
       <c r="C87" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D87" s="12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="88" ht="47.25" spans="1:4">
+      <c r="A88" s="22"/>
+      <c r="B88" s="21">
+        <v>5</v>
+      </c>
+      <c r="C88" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="D87" s="12" t="s">
+      <c r="D88" s="12" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="88" ht="31.5" spans="1:4">
-      <c r="A88" s="22"/>
-      <c r="B88" s="21"/>
-      <c r="C88" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="D88" s="12"/>
-    </row>
-    <row r="89" ht="33" spans="1:4">
+    <row r="89" ht="49.5" spans="1:4">
       <c r="A89" s="22"/>
       <c r="B89" s="21">
         <v>5</v>
       </c>
       <c r="C89" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D89" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="D89" s="12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="90" ht="82.5" spans="1:4">
+    </row>
+    <row r="90" ht="144" spans="1:4">
       <c r="A90" s="22"/>
       <c r="B90" s="21">
         <v>5</v>
       </c>
       <c r="C90" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D90" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="D90" s="12" t="s">
+    </row>
+    <row r="91" ht="31.5" spans="1:4">
+      <c r="A91" s="22"/>
+      <c r="B91" s="21"/>
+      <c r="C91" s="12" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="91" ht="65.25" spans="1:4">
-      <c r="A91" s="22"/>
-      <c r="B91" s="21">
-        <v>5</v>
-      </c>
-      <c r="C91" s="12" t="s">
+      <c r="D91" s="12"/>
+    </row>
+    <row r="92" ht="33" spans="1:4">
+      <c r="A92" s="22"/>
+      <c r="B92" s="21">
+        <v>5</v>
+      </c>
+      <c r="C92" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="D91" s="12" t="s">
+      <c r="D92" s="12" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="92" ht="47.25" spans="1:4">
-      <c r="A92" s="22"/>
-      <c r="B92" s="21"/>
-      <c r="C92" s="12" t="s">
+    <row r="93" ht="82.5" spans="1:4">
+      <c r="A93" s="22"/>
+      <c r="B93" s="21">
+        <v>5</v>
+      </c>
+      <c r="C93" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="D92" s="12"/>
-    </row>
-    <row r="93" ht="31.5" spans="1:4">
-      <c r="A93" s="22"/>
-      <c r="B93" s="21"/>
-      <c r="C93" s="12" t="s">
+      <c r="D93" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="D93" s="12"/>
-    </row>
-    <row r="94" ht="31.5" spans="1:4">
+    </row>
+    <row r="94" ht="65.25" spans="1:4">
       <c r="A94" s="22"/>
-      <c r="B94" s="21"/>
+      <c r="B94" s="21">
+        <v>5</v>
+      </c>
       <c r="C94" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="D94" s="12"/>
-    </row>
-    <row r="95" spans="1:4">
+      <c r="D94" s="12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="95" ht="47.25" spans="1:4">
       <c r="A95" s="22"/>
       <c r="B95" s="21"/>
-      <c r="C95" s="12"/>
+      <c r="C95" s="12" t="s">
+        <v>151</v>
+      </c>
       <c r="D95" s="12"/>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" ht="31.5" spans="1:4">
       <c r="A96" s="22"/>
-    </row>
-    <row r="97" ht="48" spans="1:4">
-      <c r="A97" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="B97" s="10">
-        <v>5</v>
-      </c>
-      <c r="C97" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D97" s="11"/>
-    </row>
-    <row r="98" ht="64.5" spans="1:4">
-      <c r="A98" s="23"/>
-      <c r="B98" s="10">
+      <c r="B96" s="21"/>
+      <c r="C96" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D96" s="12"/>
+    </row>
+    <row r="97" ht="147" spans="1:4">
+      <c r="A97" s="22"/>
+      <c r="B97" s="21">
+        <v>5</v>
+      </c>
+      <c r="C97" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D97" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="98" ht="49.5" spans="1:4">
+      <c r="A98" s="22"/>
+      <c r="B98" s="21">
+        <v>5</v>
+      </c>
+      <c r="C98" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D98" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="22"/>
+    </row>
+    <row r="100" ht="48" spans="1:4">
+      <c r="A100" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="B100" s="10">
+        <v>5</v>
+      </c>
+      <c r="C100" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D100" s="11"/>
+    </row>
+    <row r="101" ht="64.5" spans="1:4">
+      <c r="A101" s="23"/>
+      <c r="B101" s="10">
         <v>6</v>
       </c>
-      <c r="C98" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D98" s="11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="99" ht="31.5" spans="1:4">
-      <c r="A99" s="23"/>
-      <c r="B99" s="20">
-        <v>5</v>
-      </c>
-      <c r="C99" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="D99" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="100" ht="31.5" spans="1:4">
-      <c r="A100" s="23"/>
-      <c r="B100" s="20">
-        <v>5</v>
-      </c>
-      <c r="C100" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="D100" s="11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="101" ht="97.5" spans="1:4">
-      <c r="A101" s="23"/>
-      <c r="B101" s="20">
-        <v>5</v>
-      </c>
       <c r="C101" s="11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="102" ht="97.5" spans="1:4">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="102" ht="31.5" spans="1:4">
       <c r="A102" s="23"/>
       <c r="B102" s="20">
         <v>5</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D102" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="103" ht="131.25" spans="1:4">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="103" ht="31.5" spans="1:4">
       <c r="A103" s="23"/>
       <c r="B103" s="20">
         <v>5</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="D103" s="8" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="104" ht="48.75" spans="1:4">
+      <c r="D103" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="104" ht="97.5" spans="1:4">
       <c r="A104" s="23"/>
       <c r="B104" s="20">
         <v>5</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="105" ht="81" spans="1:4">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="105" ht="97.5" spans="1:4">
       <c r="A105" s="23"/>
       <c r="B105" s="20">
         <v>5</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="106" ht="31.5" spans="1:4">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="106" ht="131.25" spans="1:4">
       <c r="A106" s="23"/>
       <c r="B106" s="20">
         <v>5</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="D106" s="11"/>
-    </row>
-    <row r="107" ht="32.25" spans="1:4">
+        <v>169</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="107" ht="48.75" spans="1:4">
       <c r="A107" s="23"/>
       <c r="B107" s="20">
         <v>5</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="D107" s="11"/>
-    </row>
-    <row r="108" ht="31.5" spans="1:4">
+        <v>171</v>
+      </c>
+      <c r="D107" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="108" ht="81" spans="1:4">
       <c r="A108" s="23"/>
       <c r="B108" s="20">
-        <v>2</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D108" s="11"/>
-    </row>
-    <row r="109" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D108" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="109" ht="31.5" spans="1:4">
       <c r="A109" s="23"/>
       <c r="B109" s="20">
         <v>5</v>
       </c>
-      <c r="C109" s="12" t="s">
-        <v>171</v>
+      <c r="C109" s="11" t="s">
+        <v>175</v>
       </c>
       <c r="D109" s="11"/>
     </row>
-    <row r="110" ht="31.5" spans="1:4">
+    <row r="110" ht="32.25" spans="1:4">
       <c r="A110" s="23"/>
       <c r="B110" s="20">
-        <v>2</v>
-      </c>
-      <c r="C110" s="12" t="s">
-        <v>172</v>
+        <v>5</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>176</v>
       </c>
       <c r="D110" s="11"/>
     </row>
-    <row r="111" ht="47.25" spans="1:4">
+    <row r="111" ht="31.5" spans="1:4">
       <c r="A111" s="23"/>
       <c r="B111" s="20">
-        <v>5</v>
-      </c>
-      <c r="C111" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="D111" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="112" ht="47.25" spans="1:4">
+        <v>2</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D111" s="11"/>
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112" s="23"/>
       <c r="B112" s="20">
         <v>5</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="D112" s="11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="113" ht="144" spans="1:5">
+        <v>178</v>
+      </c>
+      <c r="D112" s="11"/>
+    </row>
+    <row r="113" ht="31.5" spans="1:4">
       <c r="A113" s="23"/>
       <c r="B113" s="20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="D113" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="E113" s="25" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="114" ht="155" customHeight="1" spans="1:5">
+      <c r="D113" s="11"/>
+    </row>
+    <row r="114" ht="47.25" spans="1:4">
       <c r="A114" s="23"/>
       <c r="B114" s="20">
         <v>5</v>
@@ -4254,47 +4341,59 @@
       <c r="D114" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="E114" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="115" ht="49.5" spans="1:4">
+    </row>
+    <row r="115" ht="47.25" spans="1:4">
       <c r="A115" s="23"/>
       <c r="B115" s="20">
         <v>5</v>
       </c>
       <c r="C115" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="D115" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="D115" s="11" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="116" ht="49.5" spans="1:4">
+    </row>
+    <row r="116" ht="144" spans="1:5">
       <c r="A116" s="23"/>
       <c r="B116" s="20">
         <v>5</v>
       </c>
       <c r="C116" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="D116" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="D116" s="11" t="s">
+      <c r="E116" s="25" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" ht="155" customHeight="1" spans="1:5">
       <c r="A117" s="23"/>
-    </row>
-    <row r="118" ht="66" spans="1:4">
+      <c r="B117" s="20">
+        <v>5</v>
+      </c>
+      <c r="C117" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D117" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="118" ht="49.5" spans="1:4">
       <c r="A118" s="23"/>
       <c r="B118" s="20">
         <v>5</v>
       </c>
-      <c r="C118" s="2" t="s">
-        <v>187</v>
+      <c r="C118" s="12" t="s">
+        <v>190</v>
       </c>
       <c r="D118" s="11" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="119" ht="49.5" spans="1:4">
@@ -4302,406 +4401,393 @@
       <c r="B119" s="20">
         <v>5</v>
       </c>
-      <c r="C119" s="2" t="s">
-        <v>189</v>
+      <c r="C119" s="12" t="s">
+        <v>192</v>
       </c>
       <c r="D119" s="11" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="120" ht="31.5" spans="1:4">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
       <c r="A120" s="23"/>
-      <c r="B120" s="20">
-        <v>5</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D120" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="121" ht="31.5" spans="1:4">
+    </row>
+    <row r="121" ht="66" spans="1:4">
       <c r="A121" s="23"/>
       <c r="B121" s="20">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="D121" s="11"/>
-    </row>
-    <row r="122" ht="47.25" spans="1:4">
+        <v>194</v>
+      </c>
+      <c r="D121" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="122" ht="49.5" spans="1:4">
       <c r="A122" s="23"/>
       <c r="B122" s="20">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D122" s="11"/>
+        <v>196</v>
+      </c>
+      <c r="D122" s="11" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="123" ht="31.5" spans="1:4">
       <c r="A123" s="23"/>
       <c r="B123" s="20">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D123" s="11"/>
-    </row>
-    <row r="124" ht="48.75" spans="1:4">
+        <v>198</v>
+      </c>
+      <c r="D123" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="124" ht="31.5" spans="1:4">
       <c r="A124" s="23"/>
       <c r="B124" s="20">
         <v>2</v>
       </c>
-      <c r="C124" s="12" t="s">
-        <v>196</v>
+      <c r="C124" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="D124" s="11"/>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" ht="47.25" spans="1:4">
       <c r="A125" s="23"/>
       <c r="B125" s="20">
         <v>2</v>
       </c>
-      <c r="C125" s="12" t="s">
-        <v>197</v>
+      <c r="C125" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="D125" s="11"/>
     </row>
-    <row r="126" ht="65.25" spans="1:4">
+    <row r="126" ht="31.5" spans="1:4">
       <c r="A126" s="23"/>
       <c r="B126" s="20">
-        <v>5</v>
-      </c>
-      <c r="C126" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D126" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="127" ht="32.25" spans="1:4">
+        <v>2</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D126" s="11"/>
+    </row>
+    <row r="127" ht="48.75" spans="1:4">
       <c r="A127" s="23"/>
       <c r="B127" s="20">
         <v>2</v>
       </c>
       <c r="C127" s="12" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D127" s="11"/>
     </row>
-    <row r="128" ht="48.75" spans="1:4">
+    <row r="128" spans="1:4">
       <c r="A128" s="23"/>
       <c r="B128" s="20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C128" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="D128" s="11" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="129" ht="31.5" spans="1:4">
+        <v>204</v>
+      </c>
+      <c r="D128" s="11"/>
+    </row>
+    <row r="129" ht="65.25" spans="1:4">
       <c r="A129" s="23"/>
       <c r="B129" s="20">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C129" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="D129" s="26"/>
-    </row>
-    <row r="130" ht="81" spans="1:4">
+        <v>205</v>
+      </c>
+      <c r="D129" s="11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="130" ht="32.25" spans="1:4">
       <c r="A130" s="23"/>
       <c r="B130" s="20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C130" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="D130" s="26" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="131" ht="32.25" spans="1:4">
+        <v>207</v>
+      </c>
+      <c r="D130" s="11"/>
+    </row>
+    <row r="131" ht="48.75" spans="1:4">
       <c r="A131" s="23"/>
       <c r="B131" s="20">
         <v>5</v>
       </c>
-      <c r="C131" s="27" t="s">
-        <v>206</v>
-      </c>
-      <c r="D131" s="26"/>
-    </row>
-    <row r="132" ht="48.75" spans="1:4">
+      <c r="C131" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D131" s="11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="132" ht="31.5" spans="1:4">
       <c r="A132" s="23"/>
       <c r="B132" s="20">
         <v>2</v>
       </c>
-      <c r="C132" s="27" t="s">
-        <v>207</v>
+      <c r="C132" s="12" t="s">
+        <v>210</v>
       </c>
       <c r="D132" s="26"/>
     </row>
-    <row r="133" ht="31.5" spans="1:4">
+    <row r="133" ht="81" spans="1:4">
       <c r="A133" s="23"/>
       <c r="B133" s="20">
-        <v>2</v>
-      </c>
-      <c r="C133" s="27" t="s">
-        <v>208</v>
-      </c>
-      <c r="D133" s="26"/>
-    </row>
-    <row r="134" ht="31.5" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C133" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="D133" s="26" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="134" ht="32.25" spans="1:4">
       <c r="A134" s="23"/>
       <c r="B134" s="20">
         <v>5</v>
       </c>
       <c r="C134" s="27" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D134" s="26"/>
     </row>
-    <row r="135" ht="81" spans="1:4">
+    <row r="135" ht="48.75" spans="1:4">
       <c r="A135" s="23"/>
       <c r="B135" s="20">
-        <v>5</v>
-      </c>
-      <c r="C135" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="D135" s="26" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="136" ht="33" spans="1:4">
+        <v>2</v>
+      </c>
+      <c r="C135" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="D135" s="26"/>
+    </row>
+    <row r="136" ht="31.5" spans="1:4">
       <c r="A136" s="23"/>
       <c r="B136" s="20">
-        <v>5</v>
-      </c>
-      <c r="C136" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="D136" s="26" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="137" ht="47.25" spans="1:4">
+        <v>2</v>
+      </c>
+      <c r="C136" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="D136" s="26"/>
+    </row>
+    <row r="137" ht="31.5" spans="1:4">
       <c r="A137" s="23"/>
       <c r="B137" s="20">
         <v>5</v>
       </c>
-      <c r="C137" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="D137" s="11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="138" ht="48.75" spans="1:4">
+      <c r="C137" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="D137" s="26"/>
+    </row>
+    <row r="138" ht="81" spans="1:4">
       <c r="A138" s="23"/>
       <c r="B138" s="20">
         <v>5</v>
       </c>
-      <c r="C138" s="28" t="s">
-        <v>216</v>
-      </c>
-      <c r="D138" s="11" t="s">
+      <c r="C138" s="12" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="139" ht="129.75" spans="1:4">
+      <c r="D138" s="26" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="139" ht="33" spans="1:4">
       <c r="A139" s="23"/>
       <c r="B139" s="20">
         <v>5</v>
       </c>
-      <c r="C139" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="D139" s="11" t="s">
+      <c r="C139" s="12" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="140" ht="31" customHeight="1" spans="1:5">
+      <c r="D139" s="26" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="140" ht="47.25" spans="1:4">
       <c r="A140" s="23"/>
-      <c r="B140" s="29">
-        <v>1</v>
+      <c r="B140" s="20">
+        <v>5</v>
       </c>
       <c r="C140" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="D140" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="E140" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="141" ht="48" spans="1:4">
+      <c r="D140" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="141" ht="48.75" spans="1:4">
       <c r="A141" s="23"/>
-      <c r="B141" s="29">
-        <v>2</v>
-      </c>
-      <c r="C141" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="D141" s="12"/>
-    </row>
-    <row r="142" ht="33" spans="1:4">
+      <c r="B141" s="20">
+        <v>5</v>
+      </c>
+      <c r="C141" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="D141" s="11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="142" ht="129.75" spans="1:4">
       <c r="A142" s="23"/>
-      <c r="B142" s="29">
-        <v>5</v>
-      </c>
-      <c r="C142" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="D142" s="12" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="143" ht="49.5" spans="1:4">
+      <c r="B142" s="20">
+        <v>5</v>
+      </c>
+      <c r="C142" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="D142" s="11" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="143" ht="31" customHeight="1" spans="1:5">
       <c r="A143" s="23"/>
       <c r="B143" s="29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D143" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="144" ht="63.75" spans="1:4">
+        <v>228</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="144" ht="48" spans="1:4">
       <c r="A144" s="23"/>
       <c r="B144" s="29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C144" s="12" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D144" s="12"/>
     </row>
-    <row r="145" ht="31.5" spans="1:4">
+    <row r="145" ht="33" spans="1:4">
       <c r="A145" s="23"/>
       <c r="B145" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D145" s="12" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="146" ht="47.25" spans="1:4">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="146" ht="49.5" spans="1:4">
       <c r="A146" s="23"/>
       <c r="B146" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="D146" s="12"/>
-    </row>
-    <row r="147" ht="47.25" spans="1:4">
+        <v>232</v>
+      </c>
+      <c r="D146" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="147" ht="63.75" spans="1:4">
       <c r="A147" s="23"/>
       <c r="B147" s="29">
         <v>1</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D147" s="12"/>
     </row>
-    <row r="148" ht="47.25" spans="1:4">
+    <row r="148" ht="31.5" spans="1:4">
       <c r="A148" s="23"/>
       <c r="B148" s="29">
         <v>1</v>
       </c>
       <c r="C148" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="D148" s="12"/>
-    </row>
-    <row r="149" spans="1:4">
+        <v>235</v>
+      </c>
+      <c r="D148" s="12" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="149" ht="47.25" spans="1:4">
       <c r="A149" s="23"/>
       <c r="B149" s="29">
         <v>1</v>
       </c>
       <c r="C149" s="12" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D149" s="12"/>
     </row>
-    <row r="150" ht="162" spans="1:5">
+    <row r="150" ht="47.25" spans="1:4">
       <c r="A150" s="23"/>
       <c r="B150" s="29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C150" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="D150" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="E150" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="151" ht="31.5" spans="1:4">
+        <v>238</v>
+      </c>
+      <c r="D150" s="12"/>
+    </row>
+    <row r="151" ht="47.25" spans="1:4">
       <c r="A151" s="23"/>
       <c r="B151" s="29">
         <v>1</v>
       </c>
       <c r="C151" s="12" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D151" s="12"/>
     </row>
-    <row r="152" ht="31.5" spans="1:4">
+    <row r="152" spans="1:4">
       <c r="A152" s="23"/>
       <c r="B152" s="29">
         <v>1</v>
       </c>
       <c r="C152" s="12" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D152" s="12"/>
     </row>
-    <row r="153" ht="33" spans="1:5">
+    <row r="153" ht="162" spans="1:5">
       <c r="A153" s="23"/>
-      <c r="B153" s="17">
+      <c r="B153" s="29">
         <v>5</v>
       </c>
       <c r="C153" s="12" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D153" s="12" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="E153" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="154" ht="114" spans="1:5">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="154" ht="31.5" spans="1:4">
       <c r="A154" s="23"/>
       <c r="B154" s="29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C154" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="D154" s="30" t="s">
-        <v>241</v>
-      </c>
-      <c r="E154" t="s">
-        <v>179</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="D154" s="12"/>
     </row>
     <row r="155" ht="31.5" spans="1:4">
       <c r="A155" s="23"/>
@@ -4709,460 +4795,470 @@
         <v>1</v>
       </c>
       <c r="C155" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="D155" s="30"/>
-    </row>
-    <row r="156" ht="207" customHeight="1" spans="1:5">
+        <v>244</v>
+      </c>
+      <c r="D155" s="12"/>
+    </row>
+    <row r="156" ht="33" spans="1:5">
       <c r="A156" s="23"/>
-      <c r="B156" s="29">
+      <c r="B156" s="17">
         <v>5</v>
       </c>
       <c r="C156" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="D156" s="30" t="s">
-        <v>244</v>
+        <v>245</v>
+      </c>
+      <c r="D156" s="12" t="s">
+        <v>246</v>
       </c>
       <c r="E156" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="157" ht="31.5" spans="1:5">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="157" ht="114" spans="1:5">
       <c r="A157" s="23"/>
       <c r="B157" s="29">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C157" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="D157" s="30"/>
+        <v>247</v>
+      </c>
+      <c r="D157" s="30" t="s">
+        <v>248</v>
+      </c>
       <c r="E157" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="158" ht="146.25" spans="1:5">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="158" ht="31.5" spans="1:4">
       <c r="A158" s="23"/>
       <c r="B158" s="29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C158" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="D158" s="30" t="s">
-        <v>247</v>
-      </c>
-      <c r="E158" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="159" ht="31.5" spans="1:5">
+        <v>249</v>
+      </c>
+      <c r="D158" s="30"/>
+    </row>
+    <row r="159" ht="207" customHeight="1" spans="1:5">
       <c r="A159" s="23"/>
       <c r="B159" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C159" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="D159" s="30"/>
+        <v>250</v>
+      </c>
+      <c r="D159" s="30" t="s">
+        <v>251</v>
+      </c>
       <c r="E159" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="160" ht="65.25" spans="1:5">
+    <row r="160" ht="31.5" spans="1:5">
       <c r="A160" s="23"/>
       <c r="B160" s="29">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C160" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="D160" s="11" t="s">
-        <v>250</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="D160" s="30"/>
       <c r="E160" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="161" ht="81" customHeight="1" spans="1:4">
+    <row r="161" ht="146.25" spans="1:5">
       <c r="A161" s="23"/>
       <c r="B161" s="29">
         <v>5</v>
       </c>
-      <c r="C161" s="31" t="s">
-        <v>251</v>
+      <c r="C161" s="12" t="s">
+        <v>253</v>
       </c>
       <c r="D161" s="30" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="162" ht="42" customHeight="1" spans="1:4">
+        <v>254</v>
+      </c>
+      <c r="E161" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="162" ht="31.5" spans="1:5">
       <c r="A162" s="23"/>
-      <c r="B162" s="29"/>
-      <c r="C162" s="31" t="s">
-        <v>253</v>
-      </c>
-      <c r="D162" s="30" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="163" ht="31.5" spans="1:5">
+      <c r="B162" s="29">
+        <v>1</v>
+      </c>
+      <c r="C162" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="D162" s="30"/>
+      <c r="E162" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="163" ht="65.25" spans="1:5">
       <c r="A163" s="23"/>
-      <c r="B163" s="29"/>
+      <c r="B163" s="29">
+        <v>5</v>
+      </c>
       <c r="C163" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="D163" s="30"/>
+        <v>256</v>
+      </c>
+      <c r="D163" s="11" t="s">
+        <v>257</v>
+      </c>
       <c r="E163" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="164" ht="31.5" spans="1:4">
+    <row r="164" ht="81" customHeight="1" spans="1:4">
       <c r="A164" s="23"/>
-      <c r="B164" s="29"/>
-      <c r="C164" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="D164" s="30"/>
-    </row>
-    <row r="165" ht="31.5" spans="1:4">
+      <c r="B164" s="29">
+        <v>5</v>
+      </c>
+      <c r="C164" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="D164" s="30" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="165" ht="42" customHeight="1" spans="1:4">
       <c r="A165" s="23"/>
       <c r="B165" s="29"/>
-      <c r="C165" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="D165" s="30"/>
-    </row>
-    <row r="166" ht="31.5" spans="1:4">
+      <c r="C165" s="31" t="s">
+        <v>260</v>
+      </c>
+      <c r="D165" s="30" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="166" ht="31.5" spans="1:5">
       <c r="A166" s="23"/>
       <c r="B166" s="29"/>
       <c r="C166" s="12" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D166" s="30"/>
-    </row>
-    <row r="167" ht="47.25" spans="1:4">
+      <c r="E166" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="167" ht="31.5" spans="1:4">
       <c r="A167" s="23"/>
       <c r="B167" s="29"/>
       <c r="C167" s="12" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="D167" s="30"/>
     </row>
-    <row r="168" ht="66" spans="1:4">
+    <row r="168" ht="31.5" spans="1:4">
       <c r="A168" s="23"/>
-      <c r="B168" s="29">
-        <v>5</v>
-      </c>
-      <c r="C168" s="31" t="s">
-        <v>260</v>
-      </c>
-      <c r="D168" s="30" t="s">
-        <v>261</v>
-      </c>
+      <c r="B168" s="29"/>
+      <c r="C168" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D168" s="30"/>
     </row>
     <row r="169" ht="31.5" spans="1:4">
       <c r="A169" s="23"/>
       <c r="B169" s="29"/>
       <c r="C169" s="12" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D169" s="30"/>
     </row>
-    <row r="170" ht="31.5" spans="1:5">
+    <row r="170" ht="47.25" spans="1:4">
       <c r="A170" s="23"/>
-      <c r="B170" s="29">
-        <v>5</v>
-      </c>
-      <c r="C170" s="31" t="s">
-        <v>263</v>
-      </c>
-      <c r="D170" s="30" t="s">
-        <v>264</v>
-      </c>
-      <c r="E170" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="171" ht="31.5" spans="1:4">
+      <c r="B170" s="29"/>
+      <c r="C170" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="D170" s="30"/>
+    </row>
+    <row r="171" ht="66" spans="1:4">
       <c r="A171" s="23"/>
-      <c r="B171" s="29"/>
-      <c r="C171" s="12" t="s">
-        <v>265</v>
-      </c>
-      <c r="D171" s="30"/>
-    </row>
-    <row r="172" ht="49.5" spans="1:4">
+      <c r="B171" s="29">
+        <v>5</v>
+      </c>
+      <c r="C171" s="31" t="s">
+        <v>267</v>
+      </c>
+      <c r="D171" s="30" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="172" ht="31.5" spans="1:4">
       <c r="A172" s="23"/>
-      <c r="B172" s="29">
-        <v>5</v>
-      </c>
+      <c r="B172" s="29"/>
       <c r="C172" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="D172" s="30" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="173" ht="147.75" spans="1:4">
+        <v>269</v>
+      </c>
+      <c r="D172" s="30"/>
+    </row>
+    <row r="173" ht="31.5" spans="1:5">
       <c r="A173" s="23"/>
       <c r="B173" s="29">
         <v>5</v>
       </c>
-      <c r="C173" s="12" t="s">
-        <v>268</v>
+      <c r="C173" s="31" t="s">
+        <v>270</v>
       </c>
       <c r="D173" s="30" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="174" ht="132" spans="1:4">
+        <v>271</v>
+      </c>
+      <c r="E173" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="174" ht="31.5" spans="1:4">
       <c r="A174" s="23"/>
-      <c r="B174" s="29">
-        <v>5</v>
-      </c>
+      <c r="B174" s="29"/>
       <c r="C174" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="D174" s="30" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4">
+        <v>272</v>
+      </c>
+      <c r="D174" s="30"/>
+    </row>
+    <row r="175" ht="49.5" spans="1:4">
       <c r="A175" s="23"/>
-      <c r="B175" s="29"/>
-      <c r="C175" s="12"/>
-      <c r="D175" s="30"/>
-    </row>
-    <row r="176" spans="1:4">
+      <c r="B175" s="29">
+        <v>5</v>
+      </c>
+      <c r="C175" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="D175" s="30" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="176" ht="147.75" spans="1:4">
       <c r="A176" s="23"/>
-      <c r="B176" s="29"/>
-      <c r="C176" s="12"/>
-      <c r="D176" s="30"/>
-    </row>
-    <row r="177" ht="130.5" spans="1:4">
-      <c r="A177" s="32" t="s">
-        <v>272</v>
-      </c>
+      <c r="B176" s="29">
+        <v>5</v>
+      </c>
+      <c r="C176" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="D176" s="30" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="177" ht="132" spans="1:4">
+      <c r="A177" s="23"/>
       <c r="B177" s="29">
         <v>5</v>
       </c>
       <c r="C177" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="D177" s="11" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="178" ht="31.5" spans="1:4">
-      <c r="A178" s="32"/>
-      <c r="B178" s="29">
+        <v>277</v>
+      </c>
+      <c r="D177" s="30" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" s="23"/>
+      <c r="B178" s="29"/>
+      <c r="C178" s="12"/>
+      <c r="D178" s="30"/>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" s="23"/>
+      <c r="B179" s="29"/>
+      <c r="C179" s="12"/>
+      <c r="D179" s="30"/>
+    </row>
+    <row r="180" ht="130.5" spans="1:4">
+      <c r="A180" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="B180" s="29">
+        <v>5</v>
+      </c>
+      <c r="C180" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="D180" s="11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="181" ht="31.5" spans="1:4">
+      <c r="A181" s="32"/>
+      <c r="B181" s="29">
         <v>1</v>
       </c>
-      <c r="C178" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="D178" s="11"/>
-    </row>
-    <row r="179" ht="31.5" spans="1:4">
-      <c r="A179" s="32"/>
-      <c r="B179" s="29">
-        <v>1</v>
-      </c>
-      <c r="C179" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="D179" s="12"/>
-    </row>
-    <row r="180" ht="31.5" spans="1:4">
-      <c r="A180" s="32"/>
-      <c r="B180" s="20">
-        <v>1</v>
-      </c>
-      <c r="C180" s="19" t="s">
-        <v>277</v>
-      </c>
-      <c r="D180" s="11"/>
-    </row>
-    <row r="181" ht="33" spans="1:4">
-      <c r="A181" s="32"/>
-      <c r="B181" s="20">
-        <v>5</v>
-      </c>
       <c r="C181" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="D181" s="8" t="s">
-        <v>279</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="D181" s="11"/>
     </row>
     <row r="182" ht="31.5" spans="1:4">
       <c r="A182" s="32"/>
-      <c r="B182" s="20">
+      <c r="B182" s="29">
         <v>1</v>
       </c>
       <c r="C182" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="D182" s="11"/>
+        <v>283</v>
+      </c>
+      <c r="D182" s="12"/>
     </row>
     <row r="183" ht="31.5" spans="1:4">
       <c r="A183" s="32"/>
       <c r="B183" s="20">
         <v>1</v>
       </c>
-      <c r="C183" s="12" t="s">
-        <v>281</v>
+      <c r="C183" s="19" t="s">
+        <v>284</v>
       </c>
       <c r="D183" s="11"/>
     </row>
-    <row r="184" ht="48.75" spans="1:4">
+    <row r="184" ht="33" spans="1:4">
       <c r="A184" s="32"/>
       <c r="B184" s="20">
         <v>5</v>
       </c>
-      <c r="C184" s="11" t="s">
-        <v>282</v>
-      </c>
-      <c r="D184" s="11" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="185" ht="235" customHeight="1" spans="1:4">
+      <c r="C184" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="D184" s="8" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="185" ht="31.5" spans="1:4">
       <c r="A185" s="32"/>
       <c r="B185" s="20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C185" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="D185" s="11" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="186" ht="208" customHeight="1" spans="1:5">
+        <v>287</v>
+      </c>
+      <c r="D185" s="11"/>
+    </row>
+    <row r="186" ht="31.5" spans="1:4">
       <c r="A186" s="32"/>
       <c r="B186" s="20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C186" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="D186" s="11" t="s">
-        <v>287</v>
-      </c>
-      <c r="E186" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="187" ht="38" customHeight="1" spans="1:3">
+        <v>288</v>
+      </c>
+      <c r="D186" s="11"/>
+    </row>
+    <row r="187" ht="48.75" spans="1:4">
       <c r="A187" s="32"/>
       <c r="B187" s="20">
-        <v>1</v>
-      </c>
-      <c r="C187" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="188" ht="38" customHeight="1" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C187" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="D187" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="188" ht="235" customHeight="1" spans="1:4">
       <c r="A188" s="32"/>
       <c r="B188" s="20">
-        <v>1</v>
-      </c>
-      <c r="C188" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D188" s="11"/>
-    </row>
-    <row r="189" ht="51" customHeight="1" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C188" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="D188" s="11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="189" ht="208" customHeight="1" spans="1:5">
       <c r="A189" s="32"/>
       <c r="B189" s="20">
+        <v>5</v>
+      </c>
+      <c r="C189" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="D189" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="E189" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="190" ht="38" customHeight="1" spans="1:3">
+      <c r="A190" s="32"/>
+      <c r="B190" s="20">
         <v>1</v>
       </c>
-      <c r="C189" s="12" t="s">
-        <v>290</v>
-      </c>
-      <c r="D189" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="190" ht="28" customHeight="1" spans="1:4">
-      <c r="A190" s="32"/>
-      <c r="B190" s="20"/>
-      <c r="C190" s="12"/>
-      <c r="D190" s="11"/>
-    </row>
-    <row r="191" ht="34" customHeight="1" spans="1:4">
-      <c r="A191" s="32" t="s">
-        <v>292</v>
-      </c>
+      <c r="C190" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="191" ht="38" customHeight="1" spans="1:4">
+      <c r="A191" s="32"/>
       <c r="B191" s="20">
+        <v>1</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D191" s="11"/>
+    </row>
+    <row r="192" ht="51" customHeight="1" spans="1:4">
+      <c r="A192" s="32"/>
+      <c r="B192" s="20">
+        <v>1</v>
+      </c>
+      <c r="C192" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="193" ht="28" customHeight="1" spans="1:4">
+      <c r="A193" s="32"/>
+      <c r="B193" s="20"/>
+      <c r="C193" s="12"/>
+      <c r="D193" s="11"/>
+    </row>
+    <row r="194" ht="34" customHeight="1" spans="1:4">
+      <c r="A194" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="B194" s="20">
         <v>2</v>
       </c>
-      <c r="C191" s="12" t="s">
-        <v>293</v>
-      </c>
-      <c r="D191" s="11" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="192" ht="58" customHeight="1" spans="1:4">
-      <c r="A192" s="32"/>
-      <c r="B192" s="29">
+      <c r="C194" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="D194" s="11" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="195" ht="58" customHeight="1" spans="1:4">
+      <c r="A195" s="32"/>
+      <c r="B195" s="29">
         <v>1</v>
       </c>
-      <c r="C192" s="12" t="s">
-        <v>295</v>
-      </c>
-      <c r="D192" s="11"/>
-    </row>
-    <row r="193" ht="31.5" spans="1:4">
-      <c r="A193" s="32"/>
-      <c r="B193" s="20">
-        <v>1</v>
-      </c>
-      <c r="C193" s="12" t="s">
-        <v>296</v>
-      </c>
-      <c r="D193" s="11"/>
-    </row>
-    <row r="194" spans="1:4">
-      <c r="A194" s="32"/>
-      <c r="B194" s="20">
-        <v>1</v>
-      </c>
-      <c r="C194" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D194" s="11"/>
-    </row>
-    <row r="195" ht="31.5" spans="1:4">
-      <c r="A195" s="32"/>
-      <c r="B195" s="20">
-        <v>1</v>
-      </c>
-      <c r="C195" s="2" t="s">
-        <v>298</v>
+      <c r="C195" s="12" t="s">
+        <v>302</v>
       </c>
       <c r="D195" s="11"/>
     </row>
-    <row r="196" spans="1:4">
+    <row r="196" ht="31.5" spans="1:4">
       <c r="A196" s="32"/>
       <c r="B196" s="20">
         <v>1</v>
       </c>
-      <c r="C196" s="2" t="s">
-        <v>299</v>
+      <c r="C196" s="12" t="s">
+        <v>303</v>
       </c>
       <c r="D196" s="11"/>
     </row>
-    <row r="197" ht="31.5" spans="1:4">
+    <row r="197" spans="1:4">
       <c r="A197" s="32"/>
       <c r="B197" s="20">
         <v>1</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="D197" s="11"/>
     </row>
@@ -5172,17 +5268,17 @@
         <v>1</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="D198" s="11"/>
     </row>
-    <row r="199" ht="31.5" spans="1:4">
+    <row r="199" spans="1:4">
       <c r="A199" s="32"/>
       <c r="B199" s="20">
         <v>1</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D199" s="11"/>
     </row>
@@ -5192,7 +5288,7 @@
         <v>1</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D200" s="11"/>
     </row>
@@ -5202,201 +5298,207 @@
         <v>1</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="D201" s="11"/>
     </row>
-    <row r="202" spans="1:4">
+    <row r="202" ht="31.5" spans="1:4">
       <c r="A202" s="32"/>
       <c r="B202" s="20">
         <v>1</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="D202" s="11"/>
     </row>
-    <row r="203" ht="66" spans="1:4">
+    <row r="203" ht="31.5" spans="1:4">
       <c r="A203" s="32"/>
       <c r="B203" s="20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="D203" s="11" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="204" ht="47.25" spans="1:4">
+        <v>310</v>
+      </c>
+      <c r="D203" s="11"/>
+    </row>
+    <row r="204" ht="31.5" spans="1:4">
       <c r="A204" s="32"/>
       <c r="B204" s="20">
         <v>1</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="D204" s="11"/>
     </row>
-    <row r="205" ht="81.75" spans="1:4">
+    <row r="205" spans="1:4">
       <c r="A205" s="32"/>
       <c r="B205" s="20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="D205" s="11" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="206" ht="99" spans="1:4">
+        <v>312</v>
+      </c>
+      <c r="D205" s="11"/>
+    </row>
+    <row r="206" ht="66" spans="1:4">
       <c r="A206" s="32"/>
       <c r="B206" s="20">
         <v>5</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D206" s="11" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="207" ht="65.25" spans="1:4">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="207" ht="47.25" spans="1:4">
       <c r="A207" s="32"/>
       <c r="B207" s="20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D207" s="11" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="208" ht="114" spans="1:4">
+        <v>315</v>
+      </c>
+      <c r="D207" s="11"/>
+    </row>
+    <row r="208" ht="81.75" spans="1:4">
       <c r="A208" s="32"/>
       <c r="B208" s="20">
         <v>5</v>
       </c>
-      <c r="C208" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="D208" s="33" t="s">
+      <c r="C208" s="2" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="209" ht="114.75" spans="1:4">
-      <c r="A209" s="32" t="s">
+      <c r="D208" s="11" t="s">
         <v>317</v>
       </c>
+    </row>
+    <row r="209" ht="99" spans="1:4">
+      <c r="A209" s="32"/>
       <c r="B209" s="20">
         <v>5</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D209" s="11" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="210" ht="81.75" spans="1:4">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="210" ht="65.25" spans="1:4">
       <c r="A210" s="32"/>
       <c r="B210" s="20">
         <v>5</v>
       </c>
-      <c r="C210" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="D210" s="33" t="s">
+      <c r="C210" s="2" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="211" ht="115.5" spans="1:4">
+      <c r="D210" s="11" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="211" ht="114" spans="1:4">
       <c r="A211" s="32"/>
       <c r="B211" s="20">
         <v>5</v>
       </c>
       <c r="C211" s="12" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D211" s="33" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="212" ht="33" spans="1:4">
-      <c r="A212" s="32"/>
+        <v>323</v>
+      </c>
+    </row>
+    <row r="212" ht="114.75" spans="1:4">
+      <c r="A212" s="32" t="s">
+        <v>324</v>
+      </c>
       <c r="B212" s="20">
         <v>5</v>
       </c>
-      <c r="C212" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="D212" s="33" t="s">
+      <c r="C212" s="2" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="213" ht="31.5" spans="1:4">
+      <c r="D212" s="11" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="213" ht="81.75" spans="1:4">
       <c r="A213" s="32"/>
-      <c r="B213" s="20"/>
+      <c r="B213" s="20">
+        <v>5</v>
+      </c>
       <c r="C213" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="D213" s="33"/>
-    </row>
-    <row r="214" ht="33" spans="1:4">
+        <v>326</v>
+      </c>
+      <c r="D213" s="33" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="214" ht="115.5" spans="1:4">
       <c r="A214" s="32"/>
-      <c r="B214" s="20"/>
+      <c r="B214" s="20">
+        <v>5</v>
+      </c>
       <c r="C214" s="12" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D214" s="33" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="215" ht="33" spans="1:4">
       <c r="A215" s="32"/>
-      <c r="B215" s="20"/>
-      <c r="C215" s="12"/>
-      <c r="D215" s="33"/>
-    </row>
-    <row r="216" spans="1:4">
+      <c r="B215" s="20">
+        <v>5</v>
+      </c>
+      <c r="C215" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="D215" s="33" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="216" ht="31.5" spans="1:4">
       <c r="A216" s="32"/>
       <c r="B216" s="20"/>
-      <c r="C216" s="12"/>
+      <c r="C216" s="12" t="s">
+        <v>332</v>
+      </c>
       <c r="D216" s="33"/>
     </row>
-    <row r="217" spans="1:4">
+    <row r="217" ht="33" spans="1:4">
       <c r="A217" s="32"/>
-      <c r="B217" s="20"/>
-      <c r="C217" s="12"/>
-      <c r="D217" s="33"/>
-    </row>
-    <row r="218" ht="49.5" spans="1:4">
-      <c r="A218" s="32" t="s">
-        <v>328</v>
-      </c>
+      <c r="B217" s="20">
+        <v>5</v>
+      </c>
+      <c r="C217" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="D217" s="33" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="218" ht="115.5" spans="1:4">
+      <c r="A218" s="32"/>
       <c r="B218" s="20">
         <v>5</v>
       </c>
       <c r="C218" s="12" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="D218" s="33" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="219" ht="177" spans="1:4">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4">
       <c r="A219" s="32"/>
-      <c r="B219" s="20">
-        <v>5</v>
-      </c>
-      <c r="C219" s="12" t="s">
-        <v>331</v>
-      </c>
-      <c r="D219" s="34" t="s">
-        <v>332</v>
-      </c>
+      <c r="B219" s="20"/>
+      <c r="C219" s="12"/>
+      <c r="D219" s="33"/>
     </row>
     <row r="220" spans="1:4">
       <c r="A220" s="32"/>
@@ -5404,17 +5506,31 @@
       <c r="C220" s="12"/>
       <c r="D220" s="33"/>
     </row>
-    <row r="221" spans="1:4">
-      <c r="A221" s="32"/>
-      <c r="B221" s="20"/>
-      <c r="C221" s="12"/>
-      <c r="D221" s="33"/>
-    </row>
-    <row r="222" spans="1:4">
+    <row r="221" ht="49.5" spans="1:4">
+      <c r="A221" s="32" t="s">
+        <v>337</v>
+      </c>
+      <c r="B221" s="20">
+        <v>5</v>
+      </c>
+      <c r="C221" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="D221" s="33" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="222" ht="177" spans="1:4">
       <c r="A222" s="32"/>
-      <c r="B222" s="20"/>
-      <c r="C222" s="12"/>
-      <c r="D222" s="33"/>
+      <c r="B222" s="20">
+        <v>5</v>
+      </c>
+      <c r="C222" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="D222" s="34" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="223" spans="1:4">
       <c r="A223" s="32"/>
@@ -5434,317 +5550,400 @@
       <c r="C225" s="12"/>
       <c r="D225" s="33"/>
     </row>
-    <row r="226" ht="31.5" spans="1:4">
-      <c r="A226" s="32" t="s">
-        <v>333</v>
-      </c>
+    <row r="226" spans="1:4">
+      <c r="A226" s="32"/>
       <c r="B226" s="20"/>
-      <c r="C226" s="12" t="s">
-        <v>334</v>
-      </c>
-      <c r="D226" s="33" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="227" ht="49.5" spans="1:4">
+      <c r="C226" s="12"/>
+      <c r="D226" s="33"/>
+    </row>
+    <row r="227" spans="1:4">
       <c r="A227" s="32"/>
-      <c r="B227" s="20">
-        <v>5</v>
-      </c>
-      <c r="C227" s="12" t="s">
-        <v>336</v>
-      </c>
-      <c r="D227" s="11" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="228" ht="47.25" spans="1:4">
+      <c r="B227" s="20"/>
+      <c r="C227" s="12"/>
+      <c r="D227" s="33"/>
+    </row>
+    <row r="228" spans="1:4">
       <c r="A228" s="32"/>
-      <c r="B228" s="20">
-        <v>5</v>
-      </c>
-      <c r="C228" s="12" t="s">
-        <v>338</v>
-      </c>
-      <c r="D228" s="11" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="229" ht="109" customHeight="1" spans="1:4">
-      <c r="A229" s="32"/>
-      <c r="B229" s="20">
-        <v>5</v>
-      </c>
+      <c r="B228" s="20"/>
+      <c r="C228" s="12"/>
+      <c r="D228" s="33"/>
+    </row>
+    <row r="229" ht="31.5" spans="1:4">
+      <c r="A229" s="32" t="s">
+        <v>342</v>
+      </c>
+      <c r="B229" s="20"/>
       <c r="C229" s="12" t="s">
-        <v>340</v>
-      </c>
-      <c r="D229" s="11" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="230" ht="33" spans="1:4">
+        <v>343</v>
+      </c>
+      <c r="D229" s="33" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="230" ht="49.5" spans="1:4">
       <c r="A230" s="32"/>
       <c r="B230" s="20">
         <v>5</v>
       </c>
-      <c r="C230" s="28" t="s">
-        <v>342</v>
+      <c r="C230" s="12" t="s">
+        <v>345</v>
       </c>
       <c r="D230" s="11" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="231" ht="33" spans="1:4">
-      <c r="A231" s="32" t="s">
-        <v>344</v>
-      </c>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="231" ht="47.25" spans="1:4">
+      <c r="A231" s="32"/>
       <c r="B231" s="20">
         <v>5</v>
       </c>
-      <c r="C231" s="35" t="s">
-        <v>345</v>
-      </c>
-      <c r="D231" s="35" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="232" ht="67" customHeight="1" spans="1:4">
+      <c r="C231" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="D231" s="11" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="232" ht="109" customHeight="1" spans="1:4">
       <c r="A232" s="32"/>
       <c r="B232" s="20">
         <v>5</v>
       </c>
       <c r="C232" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="D232" s="12" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="233" ht="42" customHeight="1" spans="1:4">
+        <v>349</v>
+      </c>
+      <c r="D232" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="233" ht="33" spans="1:4">
       <c r="A233" s="32"/>
       <c r="B233" s="20">
         <v>5</v>
       </c>
-      <c r="C233" s="12" t="s">
-        <v>349</v>
-      </c>
-      <c r="D233" s="12" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="234" ht="82" customHeight="1" spans="1:4">
-      <c r="A234" s="32"/>
+      <c r="C233" s="28" t="s">
+        <v>351</v>
+      </c>
+      <c r="D233" s="11" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="234" ht="33" spans="1:4">
+      <c r="A234" s="32" t="s">
+        <v>353</v>
+      </c>
       <c r="B234" s="20">
         <v>5</v>
       </c>
-      <c r="C234" s="12" t="s">
-        <v>351</v>
-      </c>
-      <c r="D234" s="12" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="235" ht="48.75" spans="1:4">
+      <c r="C234" s="35" t="s">
+        <v>354</v>
+      </c>
+      <c r="D234" s="35" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="235" ht="67" customHeight="1" spans="1:4">
       <c r="A235" s="32"/>
-      <c r="B235" s="29">
+      <c r="B235" s="20">
         <v>5</v>
       </c>
       <c r="C235" s="12" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="D235" s="12" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="236" ht="16.5" spans="1:4">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="236" ht="42" customHeight="1" spans="1:4">
       <c r="A236" s="32"/>
       <c r="B236" s="20">
         <v>5</v>
       </c>
       <c r="C236" s="12" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="D236" s="12" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="237" ht="409.5" spans="1:4">
-      <c r="A237" s="32" t="s">
-        <v>357</v>
-      </c>
+        <v>359</v>
+      </c>
+    </row>
+    <row r="237" ht="82" customHeight="1" spans="1:4">
+      <c r="A237" s="32"/>
       <c r="B237" s="20">
         <v>5</v>
       </c>
-      <c r="C237" s="19" t="s">
-        <v>358</v>
+      <c r="C237" s="12" t="s">
+        <v>360</v>
       </c>
       <c r="D237" s="12" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="238" ht="49.5" spans="1:4">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="238" ht="48.75" spans="1:4">
       <c r="A238" s="32"/>
-      <c r="B238" s="20">
-        <v>5</v>
-      </c>
-      <c r="C238" s="36" t="s">
-        <v>360</v>
+      <c r="B238" s="29">
+        <v>5</v>
+      </c>
+      <c r="C238" s="12" t="s">
+        <v>362</v>
       </c>
       <c r="D238" s="12" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="239" ht="33" spans="1:4">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="239" ht="16.5" spans="1:4">
       <c r="A239" s="32"/>
       <c r="B239" s="20">
         <v>5</v>
       </c>
-      <c r="C239" s="30" t="s">
-        <v>362</v>
+      <c r="C239" s="12" t="s">
+        <v>364</v>
       </c>
       <c r="D239" s="12" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="240" ht="16.5" spans="1:4">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="240" ht="261" spans="1:4">
       <c r="A240" s="32"/>
       <c r="B240" s="20">
-        <v>5</v>
-      </c>
-      <c r="C240" s="30" t="s">
-        <v>364</v>
+        <v>6</v>
+      </c>
+      <c r="C240" s="12" t="s">
+        <v>366</v>
       </c>
       <c r="D240" s="12" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="241" ht="178.5" spans="1:4">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="241" ht="82.5" spans="1:4">
       <c r="A241" s="32"/>
       <c r="B241" s="20">
-        <v>5</v>
-      </c>
-      <c r="C241" s="30" t="s">
-        <v>366</v>
+        <v>7</v>
+      </c>
+      <c r="C241" s="12" t="s">
+        <v>368</v>
       </c>
       <c r="D241" s="12" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="242" ht="66" spans="1:4">
       <c r="A242" s="32"/>
-      <c r="B242" s="20"/>
-      <c r="C242" s="30"/>
-      <c r="D242" s="12"/>
-    </row>
-    <row r="243" spans="1:4">
+      <c r="B242" s="20">
+        <v>8</v>
+      </c>
+      <c r="C242" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="D242" s="12" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="243" ht="66" spans="1:4">
       <c r="A243" s="32"/>
-      <c r="B243" s="20"/>
-      <c r="C243" s="30"/>
-      <c r="D243" s="12"/>
+      <c r="B243" s="20">
+        <v>9</v>
+      </c>
+      <c r="C243" s="12" t="s">
+        <v>372</v>
+      </c>
+      <c r="D243" s="12" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="244" spans="1:4">
       <c r="A244" s="32"/>
       <c r="B244" s="20"/>
-      <c r="C244" s="30"/>
+      <c r="C244" s="12"/>
       <c r="D244" s="12"/>
     </row>
-    <row r="245" spans="1:4">
-      <c r="A245" s="32"/>
-      <c r="B245" s="20"/>
-      <c r="C245" s="30"/>
-      <c r="D245" s="12"/>
-    </row>
-    <row r="246" spans="1:4">
+    <row r="245" ht="409.5" spans="1:4">
+      <c r="A245" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="B245" s="20">
+        <v>5</v>
+      </c>
+      <c r="C245" s="19" t="s">
+        <v>375</v>
+      </c>
+      <c r="D245" s="12" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="246" ht="49.5" spans="1:4">
       <c r="A246" s="32"/>
-      <c r="B246" s="20"/>
-      <c r="C246" s="30"/>
-      <c r="D246" s="12"/>
-    </row>
-    <row r="247" ht="220" customHeight="1" spans="1:4">
-      <c r="A247" s="32" t="s">
-        <v>368</v>
-      </c>
+      <c r="B246" s="20">
+        <v>5</v>
+      </c>
+      <c r="C246" s="36" t="s">
+        <v>377</v>
+      </c>
+      <c r="D246" s="12" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="247" ht="33" spans="1:4">
+      <c r="A247" s="32"/>
       <c r="B247" s="20">
         <v>5</v>
       </c>
-      <c r="C247" s="12" t="s">
-        <v>369</v>
+      <c r="C247" s="30" t="s">
+        <v>379</v>
       </c>
       <c r="D247" s="12" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="248" ht="31.5" spans="1:4">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="248" ht="16.5" spans="1:4">
       <c r="A248" s="32"/>
       <c r="B248" s="20">
         <v>5</v>
       </c>
-      <c r="C248" s="12" t="s">
-        <v>371</v>
+      <c r="C248" s="30" t="s">
+        <v>381</v>
       </c>
       <c r="D248" s="12" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="249" ht="130.5" spans="1:4">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="249" ht="178.5" spans="1:4">
       <c r="A249" s="32"/>
       <c r="B249" s="20">
         <v>5</v>
       </c>
-      <c r="C249" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="D249" s="2" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="250" ht="128.25" spans="1:4">
+      <c r="C249" s="30" t="s">
+        <v>383</v>
+      </c>
+      <c r="D249" s="12" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4">
       <c r="A250" s="32"/>
       <c r="B250" s="20"/>
-      <c r="C250" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="D250" s="19" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="251" ht="48" spans="1:4">
+      <c r="C250" s="30"/>
+      <c r="D250" s="12"/>
+    </row>
+    <row r="251" spans="1:4">
       <c r="A251" s="32"/>
-      <c r="B251" s="20">
-        <v>5</v>
-      </c>
-      <c r="C251" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="D251" s="2" t="s">
-        <v>378</v>
+      <c r="B251" s="20"/>
+      <c r="C251" s="30"/>
+      <c r="D251" s="12"/>
+    </row>
+    <row r="252" spans="1:4">
+      <c r="A252" s="32"/>
+      <c r="B252" s="20"/>
+      <c r="C252" s="30"/>
+      <c r="D252" s="12"/>
+    </row>
+    <row r="253" spans="1:4">
+      <c r="A253" s="32"/>
+      <c r="B253" s="20"/>
+      <c r="C253" s="30"/>
+      <c r="D253" s="12"/>
+    </row>
+    <row r="254" spans="1:4">
+      <c r="A254" s="32"/>
+      <c r="B254" s="20"/>
+      <c r="C254" s="30"/>
+      <c r="D254" s="12"/>
+    </row>
+    <row r="255" ht="220" customHeight="1" spans="1:4">
+      <c r="A255" s="32" t="s">
+        <v>385</v>
+      </c>
+      <c r="B255" s="20">
+        <v>5</v>
+      </c>
+      <c r="C255" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="D255" s="12" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="256" ht="31.5" spans="1:4">
+      <c r="A256" s="32"/>
+      <c r="B256" s="20">
+        <v>5</v>
+      </c>
+      <c r="C256" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="D256" s="12" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="257" ht="130.5" spans="1:4">
+      <c r="A257" s="32"/>
+      <c r="B257" s="20">
+        <v>5</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D257" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="258" ht="128.25" spans="1:4">
+      <c r="A258" s="32"/>
+      <c r="B258" s="20"/>
+      <c r="C258" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="D258" s="19" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="259" ht="48" spans="1:4">
+      <c r="A259" s="32"/>
+      <c r="B259" s="20">
+        <v>5</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="D259" s="2" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E251">
+  <autoFilter ref="E1:E259">
     <extLst/>
   </autoFilter>
   <mergeCells count="18">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A15:A55"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="A60:A64"/>
-    <mergeCell ref="A65:A82"/>
-    <mergeCell ref="A83:A96"/>
-    <mergeCell ref="A97:A176"/>
-    <mergeCell ref="A177:A190"/>
-    <mergeCell ref="A191:A192"/>
-    <mergeCell ref="A193:A208"/>
-    <mergeCell ref="A209:A217"/>
-    <mergeCell ref="A218:A225"/>
-    <mergeCell ref="A226:A230"/>
-    <mergeCell ref="A231:A236"/>
-    <mergeCell ref="A237:A246"/>
-    <mergeCell ref="A247:A251"/>
+    <mergeCell ref="A15:A58"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A63:A67"/>
+    <mergeCell ref="A68:A85"/>
+    <mergeCell ref="A86:A99"/>
+    <mergeCell ref="A100:A179"/>
+    <mergeCell ref="A180:A193"/>
+    <mergeCell ref="A194:A195"/>
+    <mergeCell ref="A196:A211"/>
+    <mergeCell ref="A212:A220"/>
+    <mergeCell ref="A221:A228"/>
+    <mergeCell ref="A229:A233"/>
+    <mergeCell ref="A234:A244"/>
+    <mergeCell ref="A245:A254"/>
+    <mergeCell ref="A255:A259"/>
   </mergeCells>
-  <conditionalFormatting sqref="B177">
+  <conditionalFormatting sqref="B180">
+    <cfRule type="cellIs" dxfId="0" priority="4" stopIfTrue="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" stopIfTrue="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B239:B243">
     <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -5755,19 +5954,19 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B54 B56:B95 B178:B1048576 B97:B116 B118:B176">
-    <cfRule type="cellIs" dxfId="0" priority="4" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="B1:B57 B59:B98 B181:B238 B100:B119 B121:B179 B244:B1048576">
+    <cfRule type="cellIs" dxfId="0" priority="7" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="8" stopIfTrue="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="9" stopIfTrue="1" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C209" r:id="rId1" display="Panoptic Segmentation" tooltip="https://arxiv.org/abs/1801.00868"/>
+    <hyperlink ref="C212" r:id="rId1" display="Panoptic Segmentation" tooltip="https://arxiv.org/abs/1801.00868"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
add some reading note for panoptic segmentation
</commit_message>
<xml_diff>
--- a/reading_note.xlsx
+++ b/reading_note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14370" windowHeight="25455" tabRatio="354"/>
+    <workbookView windowWidth="27720" windowHeight="13140" tabRatio="354"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396">
   <si>
     <t>Scope</t>
   </si>
@@ -49,16 +49,10 @@
     <t>用FIFO使得读图, 预处理和训练流水线化, 提高训练效率</t>
   </si>
   <si>
-    <t>tensorflow, 多GPU训练</t>
-  </si>
-  <si>
     <t>数据集</t>
   </si>
   <si>
     <t>The Cityscapes Dataset for Semantic Urban Scene Understanding</t>
-  </si>
-  <si>
-    <t>FSS-1000: A 1000-Class Dataset for Few-Shot Segmentation</t>
   </si>
   <si>
     <t>(2019.06) DrivingStereo: A Large-Scale Dateset for Stereo Matching in Autonomous Driving Scenarios</t>
@@ -1405,45 +1399,12 @@
     <t>(2019 cvpr) Accel: A Corrective Fusion Network for Efficient Semantic Segmentation on Video</t>
   </si>
   <si>
-    <t>Pixel-level Encoding and Depth Layering for Instance-level Semantic Labeling</t>
-  </si>
-  <si>
-    <t>Recurrent Pixel Embedding for Instance Grouping</t>
-  </si>
-  <si>
-    <t>Semantic Instance Segmentation via Deep Metric Learning</t>
-  </si>
-  <si>
-    <t>Instancecut: from edges to instanes with multicut</t>
-  </si>
-  <si>
-    <t>Distance metric learning for large margin nearest neighbor classification</t>
-  </si>
-  <si>
-    <t>SGN_Sequential Grouping Networks for Instance Segmentation</t>
-  </si>
-  <si>
-    <t>Deep Watershed Transform for Instance Segmentation</t>
-  </si>
-  <si>
-    <t>Joint Graph Decomposition &amp; Node Labeling_Problem, Algorithms, Applications</t>
-  </si>
-  <si>
-    <t>Proposal-free instance segmentation with a clustering loss function</t>
-  </si>
-  <si>
-    <t>Segmentation is All You Need</t>
-  </si>
-  <si>
     <t>(2019, cvpr) instance segmentation by jointly optimizing spatial embeddings and clustering Bandwidth</t>
   </si>
   <si>
     <t>1. 针对之前的方法（比如Box2Pix）优化了：  a. 聚类的时候的不同物体的Margin可以需学习(且用 Lovase-hinge Loss 直接优化 IoU ); b. 学习seed map, 后处理的时候可以直接找出聚类中心；
 2. 后处理: seed map中概率最大的点作为聚类中心， 这个点对应位置的sigma map上sigma为聚类的sigma，这样可以提高聚类的速度；
 3.  cityscapes上， forward pass大概65ms， 后处理大概25ms</t>
-  </si>
-  <si>
-    <t>The Best of Both Modes: Separately Leverageing RGB and Depth for Unseen Object Instance Segmentation</t>
   </si>
   <si>
     <t>Instance Stixels: Segmenting and Grouping Stixels into Objects</t>
@@ -1480,6 +1441,12 @@
 弊端是，被遮挡的物体会被分成两个东西</t>
   </si>
   <si>
+    <t>(2019.04 ICCV) YOLACT_Real-time Instance Segmentation</t>
+  </si>
+  <si>
+    <t>(2019.12) YOLACT++_Better Real-time INstance Segmentation</t>
+  </si>
+  <si>
     <t>Panoptic Segmentation</t>
   </si>
   <si>
@@ -1507,6 +1474,18 @@
   </si>
   <si>
     <t>(2019 ICCV)AdaptIS: Adaptive Instance Selection Network</t>
+  </si>
+  <si>
+    <t>0. 这个方法的意义还在于, 可以用在交互式的instance分割上, 比如只想分割图片上的某几辆车, 可以就在这几辆车上点一下就行;
+1. 有mxnet和pytorch的实现: https://github.com/saic-vul/adaptis/tree/pytorch
+2. proposal-free的方法, 给出某个proposal的点, 就可以输出这个点所在的instance的mask(但是是class-agnostic的)
+3. 受风格迁移的启发, 把instance segmentation的问题转化为风格迁移的问题, 因此引入了AdaIN (adaptive instance normalization, https://arxiv.org/pdf/1703.06868.pdf )
+4. 结构:
+    a. Instance selection network: generates an object mask using features extracted by a backbone and a "characteristic" vector.
+    b. Point proposal network: 主要用在全景分割, 输出每个点可以产生好Query Points的概率; 这个网络在其它的网络都训练好了才训练, Ground Truth的做法为: 随机选N个点, 产生的Mask按照和训练集的IoU排序, top的20%作为positive example, 其余作为false example; 
+    c. controller network: 接受某个Query Point的feature, 产生控制AdaIn的参数;
+    d. relative coordiConv: 产生一个基于Query Point的相对位置map, concate到backbone提取的feature后面,输入Instance selection network;
+5. 更改了Focal Loss, 提出Normalized Focal Loss (NFL)解决Focal Loss的"gradient fade over time的问题":</t>
   </si>
   <si>
     <t>(2018.12) Learning to Fuse Things and Stuff</t>
@@ -1534,6 +1513,51 @@
 2. Train 和 Inference的过程一样；核心是一个可微的panoptic segmentation submodule;
 3. Dynamic pertential head用每个bbox(或者再加上mask)， 去这个bbox对应的semantic prob上“抠一块”下来， 放在(H/d)x(W/d)的图上； 属于stuff的class用一个global的框取抠；最后形成一个H/d)x(W/d)x(D+Nst)的大tensor, 算是一个初步的panoptic 结果;
 4. Instance affinity head: 用attention的方法精细化 H/d)x(W/d)x(D+Nst)的大tensor， 难点是如何减少计算量；</t>
+  </si>
+  <si>
+    <t>(2019.12) Real-Time Panoptic Segmentation from Dense Detections</t>
+  </si>
+  <si>
+    <t>这篇文章比较新的地方在于Dense Detection, 受了FCOS的启发: https://arxiv.org/pdf/1904.01355.pdf  FCOS: Fully Convolutional One-Stage Object Detection
+1. single-shot panoptic segmentation for real-time application
+2. a novel panoptic segmentation model that: 1) reuse dense bounding box proposals discarded by MNS to recover instance masks directly; 2) sharing computations across semantic segmentation and detection streams can significantly reduce the overal complexity.
+3. can work in  weakly supervised panoptic scenarios.
+4. 特点在于如何出instance-mask: a. 每个点预测一个bbox(包括这个bbox的四个点, 类别及类别的概率); b. NMS留下来的bbox作为query set; c. 对于query set里面每个bbox(Bj)里面的每个点, 计算M(x, y, j), M(x, y, j)为这个Bj的类别的概率(Psem)乘以这个点的bbox和Bj的IoU</t>
+  </si>
+  <si>
+    <t>(2019.11) single shot panoptic segmentation</t>
+  </si>
+  <si>
+    <t>主要用了inst.center来解决同一类不同bbox的semantic logic的重叠问题, 重叠部分, 看预测出来的offset离哪一个bbox中心近, 就属于哪一个instance; coco上大概25fps, 32PQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2019.06 ICCV) IMP_ Instance Mask Projection for High Accuracy Semantic Segmentation of Things
+</t>
+  </si>
+  <si>
+    <t>用mask-rcnn的instance的结果提高语义分割的方法, 把instance的mask 按照类别resize到semantic logits的大小, 并且和semantic logits concate在一起:</t>
+  </si>
+  <si>
+    <t>(2019.01 CVPR) UPSNet_ A Unified Panoptic Segmentation Network</t>
+  </si>
+  <si>
+    <t>1. 提出了一个可以参与训练的后处理网络, Panoptic segmentation head, 来出每个Pixel的ID (其实这个head对PQ只有0.4的涨幅);
+2. 已经开源: https://github.com/uber-research/UPSNet
+3. Panoptic segmentation head: 做出一个(1+N_inst + N_stuff) x H x W的tensor, 让后channel方向argmax决定每个pixel的ID, 如果ID在N_stuff的范围内, 则是stuff类别(ID_stuff = ClassID_stuff); 如果不在, 则是这个instance的ID, 设置一个unknow类别, 减少False Postive, 细节如下:
+    a. N_stuff: 直接把语义分割的stuff类别的logits复制过来;
+    b. N_thing: 每个channel放一个融合的instance mask, 这个mask是instance_branch的mask加上其bbox从semantic_branch对应类别的channnel上抠下来的logits;
+    c. unkonw: max(X_thing) - max(N_thing), 一个channel, 表示: 如果X_thing上有值的地方, 在N_thing上没有的话, 很可能就是漏掉的instance, 所以就放在unkown;</t>
+  </si>
+  <si>
+    <t>(2018.12 CVPR) Attention-guided Unified Network for Panoptic Segmentation</t>
+  </si>
+  <si>
+    <t>1. one observation: FG segmentation(like mask rcnn) is often more accurate.
+2. 为了使得thing branch的信息流动到stuff, 提出了PAM(proposal attention module)和MAM(Mask Attention Module):
+3. optimize a joint loss for both thing mask and stuff mask;
+4. PAM: RPN到stuff branch用了spatial attention, 注意Mi的activation是1-sigmoid, 这样可以把RPN强调fg的feature变为强调bg feature, spatial attention之后还加了channel Attention
+5. MAM: 用ROIUpsample把每个mask upsample回原尺寸, 在叠在一起做spatial attention(注意activation也是1-sigmoid), 然后也加了channel attention 
+6. 后融合还是采用了启发式的后融合;</t>
   </si>
   <si>
     <t>车道线检测</t>
@@ -1873,10 +1897,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1935,17 +1959,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1956,9 +1982,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1973,7 +2021,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1987,13 +2043,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -2002,9 +2051,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2017,32 +2066,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2056,26 +2096,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2125,13 +2149,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2143,19 +2197,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2167,13 +2215,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2191,25 +2293,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2221,73 +2317,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2299,13 +2329,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2358,32 +2382,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2414,20 +2441,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2441,17 +2465,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2460,148 +2484,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2825,7 +2849,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="4C4C4C"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -3081,12 +3105,12 @@
   <dimension ref="A1:G258"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A206" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C218" sqref="C218"/>
+      <selection pane="bottomLeft" activeCell="D196" sqref="D196"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="15.75" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.81333333333333" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="13.4266666666667" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
@@ -3110,7 +3134,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" ht="33" spans="1:4">
+    <row r="2" ht="27" spans="1:4">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -3122,7 +3146,7 @@
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" ht="16.5" spans="1:4">
+    <row r="3" ht="13.5" spans="1:4">
       <c r="A3" s="9"/>
       <c r="B3" s="10">
         <v>5</v>
@@ -3132,7 +3156,7 @@
       </c>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" ht="16.5" spans="1:4">
+    <row r="4" ht="13.5" spans="1:4">
       <c r="A4" s="9"/>
       <c r="B4" s="10">
         <v>5</v>
@@ -3142,7 +3166,7 @@
       </c>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" ht="16.5" spans="1:4">
+    <row r="5" ht="13.5" spans="1:4">
       <c r="A5" s="9"/>
       <c r="B5" s="10">
         <v>5</v>
@@ -3154,206 +3178,210 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="16.5" spans="1:4">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
+    <row r="6" ht="25.5" spans="1:4">
+      <c r="A6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="10">
+        <v>5</v>
+      </c>
       <c r="C6" s="12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" ht="31.5" spans="1:4">
-      <c r="A7" s="9" t="s">
-        <v>11</v>
-      </c>
+    <row r="7" ht="147" spans="1:4">
+      <c r="A7" s="9"/>
       <c r="B7" s="10">
         <v>5</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" ht="31.5" spans="1:4">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" ht="180" spans="1:4">
+    </row>
+    <row r="8" ht="51.75" spans="1:4">
+      <c r="A8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="10">
+        <v>5</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" ht="13.5" spans="1:4">
       <c r="A9" s="9"/>
-      <c r="B9" s="10">
-        <v>5</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>14</v>
+      <c r="B9" s="13">
+        <v>5</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>17</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" ht="63.75" spans="1:4">
-      <c r="A10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="10">
-        <v>5</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" ht="16.5" spans="1:4">
+    <row r="10" spans="1:4">
+      <c r="A10" s="9"/>
+      <c r="B10" s="14">
+        <v>5</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="11"/>
+    </row>
+    <row r="11" ht="25.5" spans="1:4">
       <c r="A11" s="9"/>
-      <c r="B11" s="13">
-        <v>5</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>19</v>
+      <c r="B11" s="10">
+        <v>5</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" ht="67.5" spans="1:4">
       <c r="A12" s="9"/>
-      <c r="B12" s="14">
+      <c r="B12" s="10">
         <v>5</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="11"/>
-    </row>
-    <row r="13" ht="31.5" spans="1:4">
-      <c r="A13" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" ht="66" spans="1:4">
+      <c r="A13" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="B13" s="10">
         <v>5</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>22</v>
+      <c r="C13" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" ht="82.5" spans="1:4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" ht="27" spans="1:4">
       <c r="A14" s="9"/>
-      <c r="B14" s="10">
-        <v>5</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>24</v>
+      <c r="B14" s="14">
+        <v>5</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>27</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" ht="81" spans="1:4">
-      <c r="A15" s="9" t="s">
-        <v>26</v>
-      </c>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" ht="37" customHeight="1" spans="1:4">
+      <c r="A15" s="9"/>
       <c r="B15" s="10">
         <v>5</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" ht="33" spans="1:4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="9"/>
       <c r="B16" s="14">
         <v>5</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" ht="37" customHeight="1" spans="1:4">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" ht="25.5" spans="1:4">
       <c r="A17" s="9"/>
-      <c r="B17" s="10">
+      <c r="B17" s="14">
         <v>5</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" ht="66" spans="1:4">
       <c r="A18" s="9"/>
       <c r="B18" s="14">
         <v>5</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>33</v>
+      <c r="C18" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" ht="31.5" spans="1:4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" ht="27" spans="1:4">
       <c r="A19" s="9"/>
       <c r="B19" s="14">
         <v>5</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>36</v>
+      <c r="C19" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" ht="81" spans="1:4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" ht="38.25" spans="1:4">
       <c r="A20" s="9"/>
-      <c r="B20" s="14">
-        <v>5</v>
+      <c r="B20" s="16">
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" ht="33" spans="1:4">
+        <v>40</v>
+      </c>
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" ht="25.5" spans="1:4">
       <c r="A21" s="9"/>
       <c r="B21" s="14">
         <v>5</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" ht="47.25" spans="1:4">
+      <c r="D21" s="11"/>
+    </row>
+    <row r="22" ht="25.5" spans="1:4">
       <c r="A22" s="9"/>
-      <c r="B22" s="16">
-        <v>1</v>
+      <c r="B22" s="14">
+        <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" ht="31.5" spans="1:4">
+    <row r="23" ht="54" spans="1:4">
       <c r="A23" s="9"/>
       <c r="B23" s="14">
         <v>5</v>
@@ -3361,94 +3389,94 @@
       <c r="C23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="11"/>
-    </row>
-    <row r="24" ht="31.5" spans="1:4">
+      <c r="D23" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" ht="25.5" spans="1:4">
       <c r="A24" s="9"/>
       <c r="B24" s="14">
         <v>5</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="11"/>
-    </row>
-    <row r="25" ht="66" spans="1:4">
+        <v>45</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" ht="13.5" spans="1:5">
       <c r="A25" s="9"/>
       <c r="B25" s="14">
         <v>5</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" ht="31.5" spans="1:4">
+        <v>48</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" ht="26.25" spans="1:4">
       <c r="A26" s="9"/>
       <c r="B26" s="14">
         <v>5</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" ht="16.5" spans="1:5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" ht="52.5" spans="1:4">
       <c r="A27" s="9"/>
       <c r="B27" s="14">
         <v>5</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>49</v>
+      <c r="C27" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" ht="32.25" spans="1:4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" ht="25.5" spans="1:4">
       <c r="A28" s="9"/>
       <c r="B28" s="14">
         <v>5</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>51</v>
+      <c r="C28" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" ht="64.5" spans="1:4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" ht="25.5" spans="1:4">
       <c r="A29" s="9"/>
       <c r="B29" s="14">
         <v>5</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" ht="31.5" spans="1:4">
+      <c r="C29" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="11"/>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="9"/>
       <c r="B30" s="14">
         <v>5</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="31" ht="31.5" spans="1:4">
+      <c r="D30" s="11"/>
+    </row>
+    <row r="31" ht="53" customHeight="1" spans="1:4">
       <c r="A31" s="9"/>
       <c r="B31" s="14">
         <v>5</v>
@@ -3456,71 +3484,71 @@
       <c r="C31" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="11"/>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="D31" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" ht="53" customHeight="1" spans="1:4">
       <c r="A32" s="9"/>
       <c r="B32" s="14">
         <v>5</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" s="11"/>
-    </row>
-    <row r="33" ht="53" customHeight="1" spans="1:4">
+      <c r="C32" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" ht="185" customHeight="1" spans="1:5">
       <c r="A33" s="9"/>
       <c r="B33" s="14">
         <v>5</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" ht="53" customHeight="1" spans="1:4">
+        <v>62</v>
+      </c>
+      <c r="E33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" ht="53" customHeight="1" spans="1:5">
       <c r="A34" s="9"/>
       <c r="B34" s="14">
-        <v>5</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>61</v>
+        <v>2</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>63</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" ht="185" customHeight="1" spans="1:5">
+        <v>64</v>
+      </c>
+      <c r="E34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" ht="53" customHeight="1" spans="1:4">
       <c r="A35" s="9"/>
-      <c r="B35" s="14">
-        <v>5</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" ht="53" customHeight="1" spans="1:5">
+      <c r="B35" s="16">
+        <v>1</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" ht="53" customHeight="1" spans="1:4">
       <c r="A36" s="9"/>
-      <c r="B36" s="14">
+      <c r="B36" s="16">
         <v>2</v>
       </c>
-      <c r="C36" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D36" s="11" t="s">
+      <c r="C36" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E36" t="s">
-        <v>35</v>
-      </c>
+      <c r="D36" s="11"/>
     </row>
     <row r="37" ht="53" customHeight="1" spans="1:4">
       <c r="A37" s="9"/>
@@ -3532,428 +3560,428 @@
       </c>
       <c r="D37" s="11"/>
     </row>
-    <row r="38" ht="53" customHeight="1" spans="1:4">
+    <row r="38" ht="70" customHeight="1" spans="1:4">
       <c r="A38" s="9"/>
       <c r="B38" s="16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D38" s="11"/>
-    </row>
-    <row r="39" ht="53" customHeight="1" spans="1:4">
+      <c r="D38" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" ht="355" customHeight="1" spans="1:4">
       <c r="A39" s="9"/>
-      <c r="B39" s="16">
+      <c r="B39" s="14">
+        <v>5</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" ht="53" customHeight="1" spans="1:4">
+      <c r="A40" s="9"/>
+      <c r="B40" s="14">
         <v>1</v>
       </c>
-      <c r="C39" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" s="11"/>
-    </row>
-    <row r="40" ht="70" customHeight="1" spans="1:4">
-      <c r="A40" s="9"/>
-      <c r="B40" s="16">
-        <v>1</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" ht="355" customHeight="1" spans="1:4">
+      <c r="C40" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" ht="53" customHeight="1" spans="1:4">
       <c r="A41" s="9"/>
       <c r="B41" s="14">
         <v>5</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="42" ht="53" customHeight="1" spans="1:4">
+      <c r="D41" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" ht="155" customHeight="1" spans="1:5">
       <c r="A42" s="9"/>
-      <c r="B42" s="14">
-        <v>1</v>
+      <c r="B42" s="17">
+        <v>5</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D42" s="11"/>
+        <v>75</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E42" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="43" ht="53" customHeight="1" spans="1:4">
       <c r="A43" s="9"/>
-      <c r="B43" s="14">
-        <v>5</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" ht="155" customHeight="1" spans="1:5">
+      <c r="B43" s="17">
+        <v>5</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" ht="53" customHeight="1" spans="1:4">
       <c r="A44" s="9"/>
       <c r="B44" s="17">
         <v>5</v>
       </c>
-      <c r="C44" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E44" t="s">
-        <v>35</v>
+      <c r="C44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="45" ht="53" customHeight="1" spans="1:4">
       <c r="A45" s="9"/>
       <c r="B45" s="17">
-        <v>5</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="46" ht="53" customHeight="1" spans="1:4">
+        <v>1</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" s="12"/>
+    </row>
+    <row r="46" ht="53" customHeight="1" spans="1:5">
       <c r="A46" s="9"/>
       <c r="B46" s="17">
-        <v>5</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="12" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="47" ht="53" customHeight="1" spans="1:4">
+      <c r="D46" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" ht="53" customHeight="1" spans="1:5">
       <c r="A47" s="9"/>
       <c r="B47" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="D47" s="12"/>
+        <v>84</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="48" ht="53" customHeight="1" spans="1:5">
       <c r="A48" s="9"/>
       <c r="B48" s="17">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E48" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="49" ht="53" customHeight="1" spans="1:5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" ht="53" customHeight="1" spans="1:4">
       <c r="A49" s="9"/>
       <c r="B49" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="E49" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="50" ht="53" customHeight="1" spans="1:5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" ht="53" customHeight="1" spans="1:4">
       <c r="A50" s="9"/>
       <c r="B50" s="17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E50" t="s">
-        <v>35</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D50" s="12"/>
     </row>
     <row r="51" ht="53" customHeight="1" spans="1:4">
       <c r="A51" s="9"/>
-      <c r="B51" s="17">
-        <v>1</v>
-      </c>
+      <c r="B51" s="17"/>
       <c r="C51" s="12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" ht="53" customHeight="1" spans="1:4">
       <c r="A52" s="9"/>
       <c r="B52" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D52" s="12"/>
     </row>
-    <row r="53" ht="53" customHeight="1" spans="1:4">
+    <row r="53" ht="83" customHeight="1" spans="1:4">
       <c r="A53" s="9"/>
-      <c r="B53" s="17"/>
+      <c r="B53" s="17">
+        <v>5</v>
+      </c>
       <c r="C53" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" ht="53" customHeight="1" spans="1:4">
       <c r="A54" s="9"/>
       <c r="B54" s="17">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D54" s="12"/>
-    </row>
-    <row r="55" ht="83" customHeight="1" spans="1:4">
+        <v>96</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="55" ht="53" customHeight="1" spans="1:4">
       <c r="A55" s="9"/>
-      <c r="B55" s="17">
-        <v>5</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="56" ht="53" customHeight="1" spans="1:4">
+      <c r="B55" s="17"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+    </row>
+    <row r="56" ht="41" customHeight="1" spans="1:1">
       <c r="A56" s="9"/>
-      <c r="B56" s="17">
-        <v>5</v>
-      </c>
-      <c r="C56" s="12" t="s">
+    </row>
+    <row r="57" ht="183" customHeight="1" spans="1:4">
+      <c r="A57" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="D56" s="12" t="s">
+      <c r="B57" s="14">
+        <v>5</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="57" ht="53" customHeight="1" spans="1:4">
-      <c r="A57" s="9"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-    </row>
-    <row r="58" ht="41" customHeight="1" spans="1:1">
-      <c r="A58" s="9"/>
-    </row>
-    <row r="59" ht="183" customHeight="1" spans="1:4">
-      <c r="A59" s="18" t="s">
+      <c r="D57" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B59" s="14">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="58" ht="202" customHeight="1" spans="1:4">
+      <c r="A58" s="18"/>
+      <c r="B58" s="14">
+        <v>5</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" ht="43" customHeight="1" spans="1:4">
+      <c r="A59" s="18"/>
+      <c r="B59" s="14"/>
       <c r="C59" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="60" ht="202" customHeight="1" spans="1:4">
+        <v>103</v>
+      </c>
+      <c r="D59" s="19"/>
+    </row>
+    <row r="60" ht="69" customHeight="1" spans="1:3">
       <c r="A60" s="18"/>
       <c r="B60" s="14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D60" s="19" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="61" ht="43" customHeight="1" spans="1:4">
-      <c r="A61" s="18"/>
+    <row r="61" ht="56" customHeight="1" spans="1:3">
+      <c r="A61" s="18" t="s">
+        <v>105</v>
+      </c>
       <c r="B61" s="14"/>
       <c r="C61" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D61" s="19"/>
-    </row>
-    <row r="62" ht="69" customHeight="1" spans="1:3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="62" ht="30" customHeight="1" spans="1:3">
       <c r="A62" s="18"/>
-      <c r="B62" s="14">
-        <v>1</v>
-      </c>
+      <c r="B62" s="14"/>
       <c r="C62" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="63" ht="56" customHeight="1" spans="1:3">
-      <c r="A63" s="18" t="s">
         <v>107</v>
       </c>
+    </row>
+    <row r="63" ht="29" customHeight="1" spans="1:3">
+      <c r="A63" s="18"/>
       <c r="B63" s="14"/>
       <c r="C63" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="64" ht="30" customHeight="1" spans="1:3">
+    <row r="64" ht="69" customHeight="1" spans="1:3">
       <c r="A64" s="18"/>
       <c r="B64" s="14"/>
       <c r="C64" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="65" ht="29" customHeight="1" spans="1:3">
+    <row r="65" ht="69" customHeight="1" spans="1:2">
       <c r="A65" s="18"/>
       <c r="B65" s="14"/>
-      <c r="C65" s="2" t="s">
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="9" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="66" ht="69" customHeight="1" spans="1:3">
-      <c r="A66" s="18"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="2" t="s">
+      <c r="B66" s="14">
+        <v>5</v>
+      </c>
+      <c r="C66" s="11" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="67" ht="69" customHeight="1" spans="1:2">
-      <c r="A67" s="18"/>
-      <c r="B67" s="14"/>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="9" t="s">
+      <c r="D66" s="11"/>
+      <c r="F66" s="24"/>
+      <c r="G66" s="24"/>
+    </row>
+    <row r="67" ht="51.75" spans="1:6">
+      <c r="A67" s="9"/>
+      <c r="B67" s="14">
+        <v>5</v>
+      </c>
+      <c r="C67" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="B68" s="14">
+      <c r="D67" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F67" s="1"/>
+    </row>
+    <row r="68" ht="27" spans="1:4">
+      <c r="A68" s="9"/>
+      <c r="B68" s="10">
         <v>5</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="D68" s="11"/>
-      <c r="F68" s="24"/>
-      <c r="G68" s="24"/>
-    </row>
-    <row r="69" ht="63.75" spans="1:6">
+        <v>114</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="69" ht="66.75" spans="1:4">
       <c r="A69" s="9"/>
-      <c r="B69" s="14">
+      <c r="B69" s="10">
         <v>5</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="F69" s="1"/>
-    </row>
-    <row r="70" ht="33" spans="1:4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" ht="25.5" spans="1:4">
       <c r="A70" s="9"/>
-      <c r="B70" s="10">
-        <v>5</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>116</v>
+      <c r="B70" s="20">
+        <v>5</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="71" ht="81.75" spans="1:4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="71" ht="27" spans="1:4">
       <c r="A71" s="9"/>
       <c r="B71" s="10">
         <v>5</v>
       </c>
-      <c r="C71" s="11" t="s">
-        <v>118</v>
+      <c r="C71" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="72" ht="31.5" spans="1:4">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" ht="25.5" spans="1:4">
       <c r="A72" s="9"/>
-      <c r="B72" s="20">
-        <v>5</v>
+      <c r="B72" s="10">
+        <v>2</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="73" ht="33" spans="1:4">
+        <v>122</v>
+      </c>
+      <c r="D72" s="11"/>
+    </row>
+    <row r="73" ht="65.25" spans="1:4">
       <c r="A73" s="9"/>
       <c r="B73" s="10">
         <v>5</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>122</v>
+      <c r="C73" s="12" t="s">
+        <v>123</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="74" ht="31.5" spans="1:4">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="74" ht="40.5" spans="1:4">
       <c r="A74" s="9"/>
       <c r="B74" s="10">
-        <v>2</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D74" s="11"/>
-    </row>
-    <row r="75" ht="80.25" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75" ht="38.25" spans="1:4">
       <c r="A75" s="9"/>
       <c r="B75" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="D75" s="11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="76" ht="49.5" spans="1:4">
+        <v>127</v>
+      </c>
+      <c r="D75" s="11"/>
+    </row>
+    <row r="76" ht="25.5" spans="1:4">
       <c r="A76" s="9"/>
       <c r="B76" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="D76" s="11" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="77" ht="47.25" spans="1:4">
+      <c r="D76" s="11"/>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" s="9"/>
       <c r="B77" s="10">
         <v>1</v>
@@ -3963,7 +3991,7 @@
       </c>
       <c r="D77" s="11"/>
     </row>
-    <row r="78" ht="31.5" spans="1:4">
+    <row r="78" ht="25.5" spans="1:4">
       <c r="A78" s="9"/>
       <c r="B78" s="10">
         <v>1</v>
@@ -3975,23 +4003,15 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="9"/>
-      <c r="B79" s="10">
-        <v>1</v>
-      </c>
-      <c r="C79" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="D79" s="11"/>
-    </row>
-    <row r="80" ht="31.5" spans="1:4">
+      <c r="B79" s="21"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="9"/>
-      <c r="B80" s="10">
-        <v>1</v>
-      </c>
-      <c r="C80" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="D80" s="11"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="9"/>
@@ -4011,306 +4031,314 @@
       <c r="C83" s="12"/>
       <c r="D83" s="12"/>
     </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="9"/>
-      <c r="B84" s="21"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="9"/>
-      <c r="B85" s="21"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
-    </row>
-    <row r="86" ht="82.5" spans="1:4">
-      <c r="A86" s="22" t="s">
+    <row r="84" ht="67.5" spans="1:4">
+      <c r="A84" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B84" s="21">
+        <v>5</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D84" s="12" t="s">
         <v>133</v>
       </c>
+    </row>
+    <row r="85" ht="225.75" spans="1:4">
+      <c r="A85" s="22"/>
+      <c r="B85" s="21">
+        <v>5</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="86" ht="38.25" spans="1:4">
+      <c r="A86" s="22"/>
       <c r="B86" s="21">
         <v>5</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="87" ht="276.75" spans="1:4">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="87" ht="40.5" spans="1:4">
       <c r="A87" s="22"/>
       <c r="B87" s="21">
         <v>5</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="88" ht="47.25" spans="1:4">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="88" ht="117" spans="1:4">
       <c r="A88" s="22"/>
       <c r="B88" s="21">
         <v>5</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D88" s="12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="89" ht="49.5" spans="1:4">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="89" ht="25.5" spans="1:4">
       <c r="A89" s="22"/>
-      <c r="B89" s="21">
-        <v>5</v>
-      </c>
+      <c r="B89" s="21"/>
       <c r="C89" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="D89" s="12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="90" ht="144" spans="1:4">
+        <v>142</v>
+      </c>
+      <c r="D89" s="12"/>
+    </row>
+    <row r="90" ht="27" spans="1:4">
       <c r="A90" s="22"/>
       <c r="B90" s="21">
         <v>5</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="91" ht="31.5" spans="1:4">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="91" ht="67.5" spans="1:4">
       <c r="A91" s="22"/>
-      <c r="B91" s="21"/>
+      <c r="B91" s="21">
+        <v>5</v>
+      </c>
       <c r="C91" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="D91" s="12"/>
-    </row>
-    <row r="92" ht="33" spans="1:4">
+        <v>145</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="92" ht="53.25" spans="1:4">
       <c r="A92" s="22"/>
       <c r="B92" s="21">
         <v>5</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D92" s="12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="93" ht="82.5" spans="1:4">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="93" ht="38.25" spans="1:4">
       <c r="A93" s="22"/>
-      <c r="B93" s="21">
-        <v>5</v>
-      </c>
+      <c r="B93" s="21"/>
       <c r="C93" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="D93" s="12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="94" ht="65.25" spans="1:4">
+        <v>149</v>
+      </c>
+      <c r="D93" s="12"/>
+    </row>
+    <row r="94" ht="25.5" spans="1:4">
       <c r="A94" s="22"/>
-      <c r="B94" s="21">
-        <v>5</v>
-      </c>
+      <c r="B94" s="21"/>
       <c r="C94" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="D94" s="12" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="95" ht="47.25" spans="1:4">
+      <c r="D94" s="12"/>
+    </row>
+    <row r="95" ht="120" spans="1:4">
       <c r="A95" s="22"/>
-      <c r="B95" s="21"/>
+      <c r="B95" s="21">
+        <v>5</v>
+      </c>
       <c r="C95" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="D95" s="12"/>
-    </row>
-    <row r="96" ht="31.5" spans="1:4">
+      <c r="D95" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="96" ht="40.5" spans="1:4">
       <c r="A96" s="22"/>
-      <c r="B96" s="21"/>
+      <c r="B96" s="21">
+        <v>5</v>
+      </c>
       <c r="C96" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="D96" s="12"/>
-    </row>
-    <row r="97" ht="147" spans="1:4">
+        <v>153</v>
+      </c>
+      <c r="D96" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
       <c r="A97" s="22"/>
-      <c r="B97" s="21">
-        <v>5</v>
-      </c>
-      <c r="C97" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="D97" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="98" ht="49.5" spans="1:4">
-      <c r="A98" s="22"/>
-      <c r="B98" s="21">
-        <v>5</v>
-      </c>
-      <c r="C98" s="12" t="s">
+    </row>
+    <row r="98" ht="39" spans="1:4">
+      <c r="A98" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="D98" s="12" t="s">
+      <c r="B98" s="10">
+        <v>5</v>
+      </c>
+      <c r="C98" s="11" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="99" spans="1:1">
-      <c r="A99" s="22"/>
-    </row>
-    <row r="100" ht="48" spans="1:4">
-      <c r="A100" s="23" t="s">
+      <c r="D98" s="11"/>
+    </row>
+    <row r="99" ht="52.5" spans="1:4">
+      <c r="A99" s="23"/>
+      <c r="B99" s="10">
+        <v>6</v>
+      </c>
+      <c r="C99" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="B100" s="10">
+      <c r="D99" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="100" ht="25.5" spans="1:4">
+      <c r="A100" s="23"/>
+      <c r="B100" s="20">
         <v>5</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="D100" s="11"/>
-    </row>
-    <row r="101" ht="64.5" spans="1:4">
+        <v>159</v>
+      </c>
+      <c r="D100" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="101" ht="25.5" spans="1:4">
       <c r="A101" s="23"/>
-      <c r="B101" s="10">
-        <v>6</v>
+      <c r="B101" s="20">
+        <v>5</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="102" ht="31.5" spans="1:4">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="102" ht="79.5" spans="1:4">
       <c r="A102" s="23"/>
       <c r="B102" s="20">
         <v>5</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D102" s="11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="103" ht="31.5" spans="1:4">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="103" ht="79.5" spans="1:4">
       <c r="A103" s="23"/>
       <c r="B103" s="20">
         <v>5</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D103" s="11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="104" ht="97.5" spans="1:4">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="104" ht="107.25" spans="1:4">
       <c r="A104" s="23"/>
       <c r="B104" s="20">
         <v>5</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="D104" s="11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="105" ht="97.5" spans="1:4">
+        <v>167</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="105" ht="39.75" spans="1:4">
       <c r="A105" s="23"/>
       <c r="B105" s="20">
         <v>5</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="106" ht="131.25" spans="1:4">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="106" ht="66" spans="1:4">
       <c r="A106" s="23"/>
       <c r="B106" s="20">
         <v>5</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="D106" s="8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="107" ht="48.75" spans="1:4">
+        <v>171</v>
+      </c>
+      <c r="D106" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="107" ht="25.5" spans="1:4">
       <c r="A107" s="23"/>
       <c r="B107" s="20">
         <v>5</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="D107" s="11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="108" ht="81" spans="1:4">
+        <v>173</v>
+      </c>
+      <c r="D107" s="11"/>
+    </row>
+    <row r="108" ht="26.25" spans="1:4">
       <c r="A108" s="23"/>
       <c r="B108" s="20">
         <v>5</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="D108" s="11" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="109" ht="31.5" spans="1:4">
+      <c r="D108" s="11"/>
+    </row>
+    <row r="109" ht="25.5" spans="1:4">
       <c r="A109" s="23"/>
       <c r="B109" s="20">
-        <v>5</v>
-      </c>
-      <c r="C109" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C109" s="2" t="s">
         <v>175</v>
       </c>
       <c r="D109" s="11"/>
     </row>
-    <row r="110" ht="32.25" spans="1:4">
+    <row r="110" spans="1:4">
       <c r="A110" s="23"/>
       <c r="B110" s="20">
         <v>5</v>
       </c>
-      <c r="C110" s="11" t="s">
+      <c r="C110" s="12" t="s">
         <v>176</v>
       </c>
       <c r="D110" s="11"/>
     </row>
-    <row r="111" ht="31.5" spans="1:4">
+    <row r="111" ht="25.5" spans="1:4">
       <c r="A111" s="23"/>
       <c r="B111" s="20">
         <v>2</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C111" s="12" t="s">
         <v>177</v>
       </c>
       <c r="D111" s="11"/>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" ht="38.25" spans="1:4">
       <c r="A112" s="23"/>
       <c r="B112" s="20">
         <v>5</v>
@@ -4318,136 +4346,136 @@
       <c r="C112" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="D112" s="11"/>
-    </row>
-    <row r="113" ht="31.5" spans="1:4">
+      <c r="D112" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="113" ht="38.25" spans="1:4">
       <c r="A113" s="23"/>
       <c r="B113" s="20">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="D113" s="11"/>
-    </row>
-    <row r="114" ht="47.25" spans="1:4">
+        <v>180</v>
+      </c>
+      <c r="D113" s="11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="114" ht="117" spans="1:5">
       <c r="A114" s="23"/>
       <c r="B114" s="20">
         <v>5</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="D114" s="11" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="115" ht="47.25" spans="1:4">
+        <v>182</v>
+      </c>
+      <c r="D114" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="E114" s="25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="115" ht="155" customHeight="1" spans="1:5">
       <c r="A115" s="23"/>
       <c r="B115" s="20">
         <v>5</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D115" s="11" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="116" ht="144" spans="1:5">
+        <v>186</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="116" ht="40.5" spans="1:4">
       <c r="A116" s="23"/>
       <c r="B116" s="20">
         <v>5</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="D116" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="E116" s="25" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="117" ht="155" customHeight="1" spans="1:5">
+        <v>188</v>
+      </c>
+      <c r="D116" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="117" ht="40.5" spans="1:4">
       <c r="A117" s="23"/>
       <c r="B117" s="20">
         <v>5</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D117" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="118" ht="49.5" spans="1:4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
       <c r="A118" s="23"/>
-      <c r="B118" s="20">
-        <v>5</v>
-      </c>
-      <c r="C118" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="D118" s="11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="119" ht="49.5" spans="1:4">
+    </row>
+    <row r="119" ht="54" spans="1:4">
       <c r="A119" s="23"/>
       <c r="B119" s="20">
         <v>5</v>
       </c>
-      <c r="C119" s="12" t="s">
+      <c r="C119" s="2" t="s">
         <v>192</v>
       </c>
       <c r="D119" s="11" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" ht="40.5" spans="1:4">
       <c r="A120" s="23"/>
-    </row>
-    <row r="121" ht="66" spans="1:4">
+      <c r="B120" s="20">
+        <v>5</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D120" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="121" ht="25.5" spans="1:4">
       <c r="A121" s="23"/>
       <c r="B121" s="20">
         <v>5</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D121" s="11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="122" ht="49.5" spans="1:4">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="122" ht="25.5" spans="1:4">
       <c r="A122" s="23"/>
       <c r="B122" s="20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D122" s="11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="123" ht="31.5" spans="1:4">
+        <v>198</v>
+      </c>
+      <c r="D122" s="11"/>
+    </row>
+    <row r="123" ht="38.25" spans="1:4">
       <c r="A123" s="23"/>
       <c r="B123" s="20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D123" s="11" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="124" ht="31.5" spans="1:4">
+      <c r="D123" s="11"/>
+    </row>
+    <row r="124" ht="25.5" spans="1:4">
       <c r="A124" s="23"/>
       <c r="B124" s="20">
         <v>2</v>
@@ -4457,274 +4485,274 @@
       </c>
       <c r="D124" s="11"/>
     </row>
-    <row r="125" ht="47.25" spans="1:4">
+    <row r="125" ht="39.75" spans="1:4">
       <c r="A125" s="23"/>
       <c r="B125" s="20">
         <v>2</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="C125" s="12" t="s">
         <v>201</v>
       </c>
       <c r="D125" s="11"/>
     </row>
-    <row r="126" ht="31.5" spans="1:4">
+    <row r="126" spans="1:4">
       <c r="A126" s="23"/>
       <c r="B126" s="20">
         <v>2</v>
       </c>
-      <c r="C126" s="2" t="s">
+      <c r="C126" s="12" t="s">
         <v>202</v>
       </c>
       <c r="D126" s="11"/>
     </row>
-    <row r="127" ht="48.75" spans="1:4">
+    <row r="127" ht="53.25" spans="1:4">
       <c r="A127" s="23"/>
       <c r="B127" s="20">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C127" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="D127" s="11"/>
-    </row>
-    <row r="128" spans="1:4">
+      <c r="D127" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="128" ht="26.25" spans="1:4">
       <c r="A128" s="23"/>
       <c r="B128" s="20">
         <v>2</v>
       </c>
       <c r="C128" s="12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D128" s="11"/>
     </row>
-    <row r="129" ht="65.25" spans="1:4">
+    <row r="129" ht="39.75" spans="1:4">
       <c r="A129" s="23"/>
       <c r="B129" s="20">
         <v>5</v>
       </c>
       <c r="C129" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D129" s="11" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="130" ht="32.25" spans="1:4">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="130" ht="25.5" spans="1:4">
       <c r="A130" s="23"/>
       <c r="B130" s="20">
         <v>2</v>
       </c>
       <c r="C130" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="D130" s="11"/>
-    </row>
-    <row r="131" ht="48.75" spans="1:4">
+        <v>208</v>
+      </c>
+      <c r="D130" s="26"/>
+    </row>
+    <row r="131" ht="66" spans="1:4">
       <c r="A131" s="23"/>
       <c r="B131" s="20">
         <v>5</v>
       </c>
       <c r="C131" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="D131" s="11" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="132" ht="31.5" spans="1:4">
+      <c r="D131" s="26" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="132" ht="26.25" spans="1:4">
       <c r="A132" s="23"/>
       <c r="B132" s="20">
-        <v>2</v>
-      </c>
-      <c r="C132" s="12" t="s">
-        <v>210</v>
+        <v>5</v>
+      </c>
+      <c r="C132" s="27" t="s">
+        <v>211</v>
       </c>
       <c r="D132" s="26"/>
     </row>
-    <row r="133" ht="81" spans="1:4">
+    <row r="133" ht="39.75" spans="1:4">
       <c r="A133" s="23"/>
       <c r="B133" s="20">
-        <v>5</v>
-      </c>
-      <c r="C133" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="D133" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C133" s="27" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="134" ht="32.25" spans="1:4">
+      <c r="D133" s="26"/>
+    </row>
+    <row r="134" ht="25.5" spans="1:4">
       <c r="A134" s="23"/>
       <c r="B134" s="20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C134" s="27" t="s">
         <v>213</v>
       </c>
       <c r="D134" s="26"/>
     </row>
-    <row r="135" ht="48.75" spans="1:4">
+    <row r="135" ht="25.5" spans="1:4">
       <c r="A135" s="23"/>
       <c r="B135" s="20">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C135" s="27" t="s">
         <v>214</v>
       </c>
       <c r="D135" s="26"/>
     </row>
-    <row r="136" ht="31.5" spans="1:4">
+    <row r="136" ht="66" spans="1:4">
       <c r="A136" s="23"/>
       <c r="B136" s="20">
-        <v>2</v>
-      </c>
-      <c r="C136" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C136" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="D136" s="26"/>
-    </row>
-    <row r="137" ht="31.5" spans="1:4">
+      <c r="D136" s="26" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="137" ht="27" spans="1:4">
       <c r="A137" s="23"/>
       <c r="B137" s="20">
         <v>5</v>
       </c>
-      <c r="C137" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="D137" s="26"/>
-    </row>
-    <row r="138" ht="81" spans="1:4">
+      <c r="C137" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="D137" s="26" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="138" ht="38.25" spans="1:4">
       <c r="A138" s="23"/>
       <c r="B138" s="20">
         <v>5</v>
       </c>
       <c r="C138" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="D138" s="26" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="139" ht="33" spans="1:4">
+        <v>219</v>
+      </c>
+      <c r="D138" s="11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="139" ht="39.75" spans="1:4">
       <c r="A139" s="23"/>
       <c r="B139" s="20">
         <v>5</v>
       </c>
-      <c r="C139" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="D139" s="26" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="140" ht="47.25" spans="1:4">
+      <c r="C139" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="D139" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="140" ht="105.75" spans="1:4">
       <c r="A140" s="23"/>
       <c r="B140" s="20">
         <v>5</v>
       </c>
-      <c r="C140" s="12" t="s">
-        <v>221</v>
+      <c r="C140" s="11" t="s">
+        <v>223</v>
       </c>
       <c r="D140" s="11" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="141" ht="48.75" spans="1:4">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="141" ht="31" customHeight="1" spans="1:5">
       <c r="A141" s="23"/>
-      <c r="B141" s="20">
-        <v>5</v>
-      </c>
-      <c r="C141" s="28" t="s">
-        <v>223</v>
-      </c>
-      <c r="D141" s="11" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="142" ht="129.75" spans="1:4">
+      <c r="B141" s="29">
+        <v>1</v>
+      </c>
+      <c r="C141" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D141" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="142" ht="39" spans="1:4">
       <c r="A142" s="23"/>
-      <c r="B142" s="20">
-        <v>5</v>
-      </c>
-      <c r="C142" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="D142" s="11" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="143" ht="31" customHeight="1" spans="1:5">
+      <c r="B142" s="29">
+        <v>2</v>
+      </c>
+      <c r="C142" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D142" s="12"/>
+    </row>
+    <row r="143" ht="27" spans="1:4">
       <c r="A143" s="23"/>
       <c r="B143" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D143" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="E143" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="144" ht="48" spans="1:4">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="144" ht="40.5" spans="1:4">
       <c r="A144" s="23"/>
       <c r="B144" s="29">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C144" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="D144" s="12"/>
-    </row>
-    <row r="145" ht="33" spans="1:4">
+        <v>230</v>
+      </c>
+      <c r="D144" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="145" ht="51.75" spans="1:4">
       <c r="A145" s="23"/>
       <c r="B145" s="29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="D145" s="12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="146" ht="49.5" spans="1:4">
+        <v>232</v>
+      </c>
+      <c r="D145" s="12"/>
+    </row>
+    <row r="146" ht="25.5" spans="1:4">
       <c r="A146" s="23"/>
       <c r="B146" s="29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D146" s="12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="147" ht="63.75" spans="1:4">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="147" ht="38.25" spans="1:4">
       <c r="A147" s="23"/>
       <c r="B147" s="29">
         <v>1</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D147" s="12"/>
     </row>
-    <row r="148" ht="31.5" spans="1:4">
+    <row r="148" ht="38.25" spans="1:4">
       <c r="A148" s="23"/>
       <c r="B148" s="29">
         <v>1</v>
       </c>
       <c r="C148" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="D148" s="12" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="149" ht="47.25" spans="1:4">
+      <c r="D148" s="12"/>
+    </row>
+    <row r="149" ht="38.25" spans="1:4">
       <c r="A149" s="23"/>
       <c r="B149" s="29">
         <v>1</v>
@@ -4734,7 +4762,7 @@
       </c>
       <c r="D149" s="12"/>
     </row>
-    <row r="150" ht="47.25" spans="1:4">
+    <row r="150" spans="1:4">
       <c r="A150" s="23"/>
       <c r="B150" s="29">
         <v>1</v>
@@ -4744,206 +4772,202 @@
       </c>
       <c r="D150" s="12"/>
     </row>
-    <row r="151" ht="47.25" spans="1:4">
+    <row r="151" ht="132" spans="1:5">
       <c r="A151" s="23"/>
       <c r="B151" s="29">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C151" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="D151" s="12"/>
-    </row>
-    <row r="152" spans="1:4">
+      <c r="D151" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="E151" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="152" ht="25.5" spans="1:4">
       <c r="A152" s="23"/>
       <c r="B152" s="29">
         <v>1</v>
       </c>
       <c r="C152" s="12" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D152" s="12"/>
     </row>
-    <row r="153" ht="162" spans="1:5">
+    <row r="153" ht="25.5" spans="1:4">
       <c r="A153" s="23"/>
       <c r="B153" s="29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C153" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="D153" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="E153" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="154" ht="31.5" spans="1:4">
+      <c r="D153" s="12"/>
+    </row>
+    <row r="154" ht="27" spans="1:5">
       <c r="A154" s="23"/>
-      <c r="B154" s="29">
-        <v>1</v>
+      <c r="B154" s="17">
+        <v>5</v>
       </c>
       <c r="C154" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="D154" s="12"/>
-    </row>
-    <row r="155" ht="31.5" spans="1:4">
+      <c r="D154" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="E154" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="155" ht="93" spans="1:5">
       <c r="A155" s="23"/>
       <c r="B155" s="29">
+        <v>5</v>
+      </c>
+      <c r="C155" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="D155" s="30" t="s">
+        <v>246</v>
+      </c>
+      <c r="E155" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="156" ht="25.5" spans="1:4">
+      <c r="A156" s="23"/>
+      <c r="B156" s="29">
         <v>1</v>
       </c>
-      <c r="C155" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="D155" s="12"/>
-    </row>
-    <row r="156" ht="33" spans="1:5">
-      <c r="A156" s="23"/>
-      <c r="B156" s="17">
-        <v>5</v>
-      </c>
       <c r="C156" s="12" t="s">
-        <v>245</v>
-      </c>
-      <c r="D156" s="12" t="s">
-        <v>246</v>
-      </c>
-      <c r="E156" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="157" ht="114" spans="1:5">
+        <v>247</v>
+      </c>
+      <c r="D156" s="30"/>
+    </row>
+    <row r="157" ht="207" customHeight="1" spans="1:5">
       <c r="A157" s="23"/>
       <c r="B157" s="29">
         <v>5</v>
       </c>
       <c r="C157" s="12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D157" s="30" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E157" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="158" ht="31.5" spans="1:4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="158" ht="25.5" spans="1:5">
       <c r="A158" s="23"/>
       <c r="B158" s="29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C158" s="12" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D158" s="30"/>
-    </row>
-    <row r="159" ht="207" customHeight="1" spans="1:5">
+      <c r="E158" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="159" ht="119.25" spans="1:5">
       <c r="A159" s="23"/>
       <c r="B159" s="29">
         <v>5</v>
       </c>
       <c r="C159" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D159" s="30" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E159" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="160" ht="31.5" spans="1:5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="160" ht="25.5" spans="1:5">
       <c r="A160" s="23"/>
       <c r="B160" s="29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C160" s="12" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D160" s="30"/>
       <c r="E160" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="161" ht="146.25" spans="1:5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="161" ht="53.25" spans="1:5">
       <c r="A161" s="23"/>
       <c r="B161" s="29">
         <v>5</v>
       </c>
       <c r="C161" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="D161" s="30" t="s">
         <v>254</v>
       </c>
+      <c r="D161" s="11" t="s">
+        <v>255</v>
+      </c>
       <c r="E161" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="162" ht="31.5" spans="1:5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="162" ht="81" customHeight="1" spans="1:4">
       <c r="A162" s="23"/>
       <c r="B162" s="29">
-        <v>1</v>
-      </c>
-      <c r="C162" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="D162" s="30"/>
-      <c r="E162" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="163" ht="65.25" spans="1:5">
+        <v>5</v>
+      </c>
+      <c r="C162" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="D162" s="30" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="163" ht="42" customHeight="1" spans="1:4">
       <c r="A163" s="23"/>
-      <c r="B163" s="29">
-        <v>5</v>
-      </c>
-      <c r="C163" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="D163" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="E163" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="164" ht="81" customHeight="1" spans="1:4">
+      <c r="B163" s="29"/>
+      <c r="C163" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="D163" s="30" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="164" ht="25.5" spans="1:5">
       <c r="A164" s="23"/>
-      <c r="B164" s="29">
-        <v>5</v>
-      </c>
-      <c r="C164" s="31" t="s">
-        <v>258</v>
-      </c>
-      <c r="D164" s="30" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="165" ht="42" customHeight="1" spans="1:4">
+      <c r="B164" s="29"/>
+      <c r="C164" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="D164" s="30"/>
+      <c r="E164" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="165" ht="25.5" spans="1:4">
       <c r="A165" s="23"/>
       <c r="B165" s="29"/>
-      <c r="C165" s="31" t="s">
-        <v>260</v>
-      </c>
-      <c r="D165" s="30" t="s">
+      <c r="C165" s="12" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="166" ht="31.5" spans="1:5">
+      <c r="D165" s="30"/>
+    </row>
+    <row r="166" ht="25.5" spans="1:4">
       <c r="A166" s="23"/>
       <c r="B166" s="29"/>
       <c r="C166" s="12" t="s">
         <v>262</v>
       </c>
       <c r="D166" s="30"/>
-      <c r="E166" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="167" ht="31.5" spans="1:4">
+    </row>
+    <row r="167" ht="25.5" spans="1:4">
       <c r="A167" s="23"/>
       <c r="B167" s="29"/>
       <c r="C167" s="12" t="s">
@@ -4951,7 +4975,7 @@
       </c>
       <c r="D167" s="30"/>
     </row>
-    <row r="168" ht="31.5" spans="1:4">
+    <row r="168" ht="38.25" spans="1:4">
       <c r="A168" s="23"/>
       <c r="B168" s="29"/>
       <c r="C168" s="12" t="s">
@@ -4959,540 +4983,525 @@
       </c>
       <c r="D168" s="30"/>
     </row>
-    <row r="169" ht="31.5" spans="1:4">
+    <row r="169" ht="54" spans="1:4">
       <c r="A169" s="23"/>
-      <c r="B169" s="29"/>
-      <c r="C169" s="12" t="s">
+      <c r="B169" s="29">
+        <v>5</v>
+      </c>
+      <c r="C169" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="D169" s="30"/>
-    </row>
-    <row r="170" ht="47.25" spans="1:4">
+      <c r="D169" s="30" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="170" ht="25.5" spans="1:4">
       <c r="A170" s="23"/>
       <c r="B170" s="29"/>
       <c r="C170" s="12" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D170" s="30"/>
     </row>
-    <row r="171" ht="66" spans="1:4">
+    <row r="171" ht="25.5" spans="1:5">
       <c r="A171" s="23"/>
       <c r="B171" s="29">
         <v>5</v>
       </c>
       <c r="C171" s="31" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D171" s="30" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="172" ht="31.5" spans="1:4">
+        <v>269</v>
+      </c>
+      <c r="E171" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="172" ht="25.5" spans="1:4">
       <c r="A172" s="23"/>
       <c r="B172" s="29"/>
       <c r="C172" s="12" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D172" s="30"/>
     </row>
-    <row r="173" ht="31.5" spans="1:5">
+    <row r="173" ht="40.5" spans="1:4">
       <c r="A173" s="23"/>
       <c r="B173" s="29">
         <v>5</v>
       </c>
-      <c r="C173" s="31" t="s">
-        <v>270</v>
+      <c r="C173" s="12" t="s">
+        <v>271</v>
       </c>
       <c r="D173" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="E173" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="174" ht="31.5" spans="1:4">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="174" ht="120.75" spans="1:4">
       <c r="A174" s="23"/>
-      <c r="B174" s="29"/>
+      <c r="B174" s="29">
+        <v>5</v>
+      </c>
       <c r="C174" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="D174" s="30"/>
-    </row>
-    <row r="175" ht="49.5" spans="1:4">
+        <v>273</v>
+      </c>
+      <c r="D174" s="30" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="175" ht="108" spans="1:4">
       <c r="A175" s="23"/>
       <c r="B175" s="29">
         <v>5</v>
       </c>
       <c r="C175" s="12" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D175" s="30" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="176" ht="147.75" spans="1:4">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
       <c r="A176" s="23"/>
-      <c r="B176" s="29">
-        <v>5</v>
-      </c>
-      <c r="C176" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="D176" s="30" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="177" ht="132" spans="1:4">
+      <c r="B176" s="29"/>
+      <c r="C176" s="12"/>
+      <c r="D176" s="30"/>
+    </row>
+    <row r="177" spans="1:4">
       <c r="A177" s="23"/>
-      <c r="B177" s="29">
-        <v>5</v>
-      </c>
-      <c r="C177" s="12" t="s">
+      <c r="B177" s="29"/>
+      <c r="C177" s="12"/>
+      <c r="D177" s="30"/>
+    </row>
+    <row r="178" ht="106.5" spans="1:4">
+      <c r="A178" s="32" t="s">
         <v>277</v>
       </c>
-      <c r="D177" s="30" t="s">
+      <c r="B178" s="29">
+        <v>5</v>
+      </c>
+      <c r="C178" s="12" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="178" spans="1:4">
-      <c r="A178" s="23"/>
-      <c r="B178" s="29"/>
-      <c r="C178" s="12"/>
-      <c r="D178" s="30"/>
-    </row>
-    <row r="179" spans="1:4">
-      <c r="A179" s="23"/>
-      <c r="B179" s="29"/>
-      <c r="C179" s="12"/>
-      <c r="D179" s="30"/>
-    </row>
-    <row r="180" ht="130.5" spans="1:4">
-      <c r="A180" s="32" t="s">
+      <c r="D178" s="11" t="s">
         <v>279</v>
       </c>
+    </row>
+    <row r="179" ht="25.5" spans="1:4">
+      <c r="A179" s="32"/>
+      <c r="B179" s="29">
+        <v>1</v>
+      </c>
+      <c r="C179" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="D179" s="11"/>
+    </row>
+    <row r="180" ht="25.5" spans="1:4">
+      <c r="A180" s="32"/>
       <c r="B180" s="29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C180" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="D180" s="11" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="181" ht="31.5" spans="1:4">
+      <c r="D180" s="12"/>
+    </row>
+    <row r="181" ht="25.5" spans="1:4">
       <c r="A181" s="32"/>
-      <c r="B181" s="29">
+      <c r="B181" s="20">
         <v>1</v>
       </c>
-      <c r="C181" s="12" t="s">
+      <c r="C181" s="19" t="s">
         <v>282</v>
       </c>
       <c r="D181" s="11"/>
     </row>
-    <row r="182" ht="31.5" spans="1:4">
+    <row r="182" ht="27" spans="1:4">
       <c r="A182" s="32"/>
-      <c r="B182" s="29">
-        <v>1</v>
+      <c r="B182" s="20">
+        <v>5</v>
       </c>
       <c r="C182" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="D182" s="12"/>
-    </row>
-    <row r="183" ht="31.5" spans="1:4">
+      <c r="D182" s="8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="183" ht="25.5" spans="1:4">
       <c r="A183" s="32"/>
       <c r="B183" s="20">
         <v>1</v>
       </c>
-      <c r="C183" s="19" t="s">
-        <v>284</v>
+      <c r="C183" s="12" t="s">
+        <v>285</v>
       </c>
       <c r="D183" s="11"/>
     </row>
-    <row r="184" ht="33" spans="1:4">
+    <row r="184" ht="25.5" spans="1:4">
       <c r="A184" s="32"/>
       <c r="B184" s="20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C184" s="12" t="s">
-        <v>285</v>
-      </c>
-      <c r="D184" s="8" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="185" ht="31.5" spans="1:4">
+      <c r="D184" s="11"/>
+    </row>
+    <row r="185" ht="39.75" spans="1:4">
       <c r="A185" s="32"/>
       <c r="B185" s="20">
-        <v>1</v>
-      </c>
-      <c r="C185" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C185" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="D185" s="11"/>
-    </row>
-    <row r="186" ht="31.5" spans="1:4">
+      <c r="D185" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="186" ht="235" customHeight="1" spans="1:4">
       <c r="A186" s="32"/>
       <c r="B186" s="20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C186" s="12" t="s">
-        <v>288</v>
-      </c>
-      <c r="D186" s="11"/>
-    </row>
-    <row r="187" ht="48.75" spans="1:4">
+        <v>289</v>
+      </c>
+      <c r="D186" s="11" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="187" ht="208" customHeight="1" spans="1:5">
       <c r="A187" s="32"/>
       <c r="B187" s="20">
         <v>5</v>
       </c>
-      <c r="C187" s="11" t="s">
-        <v>289</v>
+      <c r="C187" s="12" t="s">
+        <v>291</v>
       </c>
       <c r="D187" s="11" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="188" ht="235" customHeight="1" spans="1:4">
+        <v>292</v>
+      </c>
+      <c r="E187" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="188" ht="38" customHeight="1" spans="1:3">
       <c r="A188" s="32"/>
       <c r="B188" s="20">
-        <v>5</v>
-      </c>
-      <c r="C188" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="D188" s="11" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="189" ht="208" customHeight="1" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="189" ht="38" customHeight="1" spans="1:4">
       <c r="A189" s="32"/>
       <c r="B189" s="20">
-        <v>5</v>
-      </c>
-      <c r="C189" s="12" t="s">
-        <v>293</v>
-      </c>
-      <c r="D189" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C189" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E189" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="190" ht="38" customHeight="1" spans="1:3">
+      <c r="D189" s="11"/>
+    </row>
+    <row r="190" ht="51" customHeight="1" spans="1:4">
       <c r="A190" s="32"/>
       <c r="B190" s="20">
         <v>1</v>
       </c>
-      <c r="C190" s="2" t="s">
+      <c r="C190" s="12" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="191" ht="38" customHeight="1" spans="1:4">
+      <c r="D190" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="191" ht="28" customHeight="1" spans="1:4">
       <c r="A191" s="32"/>
-      <c r="B191" s="20">
+      <c r="B191" s="20"/>
+      <c r="C191" s="12"/>
+      <c r="D191" s="11"/>
+    </row>
+    <row r="192" ht="34" customHeight="1" spans="1:4">
+      <c r="A192" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="B192" s="20">
+        <v>2</v>
+      </c>
+      <c r="C192" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="D192" s="11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="193" ht="58" customHeight="1" spans="1:4">
+      <c r="A193" s="32"/>
+      <c r="B193" s="29">
         <v>1</v>
       </c>
-      <c r="C191" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D191" s="11"/>
-    </row>
-    <row r="192" ht="51" customHeight="1" spans="1:4">
-      <c r="A192" s="32"/>
-      <c r="B192" s="20">
-        <v>1</v>
-      </c>
-      <c r="C192" s="12" t="s">
-        <v>297</v>
-      </c>
-      <c r="D192" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="193" ht="28" customHeight="1" spans="1:4">
-      <c r="A193" s="32"/>
-      <c r="B193" s="20"/>
-      <c r="C193" s="12"/>
+      <c r="C193" s="12" t="s">
+        <v>300</v>
+      </c>
       <c r="D193" s="11"/>
     </row>
-    <row r="194" ht="34" customHeight="1" spans="1:4">
-      <c r="A194" s="32" t="s">
-        <v>299</v>
-      </c>
+    <row r="194" ht="54" spans="1:4">
+      <c r="A194" s="32"/>
       <c r="B194" s="20">
-        <v>2</v>
-      </c>
-      <c r="C194" s="12" t="s">
-        <v>300</v>
+        <v>5</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>301</v>
       </c>
       <c r="D194" s="11" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="195" ht="58" customHeight="1" spans="1:4">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="195" ht="66.75" spans="1:4">
       <c r="A195" s="32"/>
-      <c r="B195" s="29">
-        <v>1</v>
-      </c>
-      <c r="C195" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="D195" s="11"/>
-    </row>
-    <row r="196" ht="31.5" spans="1:4">
+      <c r="B195" s="20">
+        <v>5</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D195" s="11" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="196" ht="81" spans="1:4">
       <c r="A196" s="32"/>
       <c r="B196" s="20">
-        <v>1</v>
-      </c>
-      <c r="C196" s="12" t="s">
-        <v>303</v>
-      </c>
-      <c r="D196" s="11"/>
-    </row>
-    <row r="197" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D196" s="11" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="197" ht="53.25" spans="1:4">
       <c r="A197" s="32"/>
       <c r="B197" s="20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="D197" s="11"/>
-    </row>
-    <row r="198" ht="31.5" spans="1:4">
+        <v>307</v>
+      </c>
+      <c r="D197" s="11" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="198" ht="93" spans="1:4">
       <c r="A198" s="32"/>
       <c r="B198" s="20">
-        <v>1</v>
-      </c>
-      <c r="C198" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="D198" s="11"/>
-    </row>
-    <row r="199" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C198" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="D198" s="33" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="199" ht="25.5" spans="1:4">
       <c r="A199" s="32"/>
-      <c r="B199" s="20">
-        <v>1</v>
-      </c>
+      <c r="B199" s="20"/>
       <c r="C199" s="2" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="D199" s="11"/>
     </row>
-    <row r="200" ht="31.5" spans="1:4">
+    <row r="200" ht="25.5" spans="1:4">
       <c r="A200" s="32"/>
-      <c r="B200" s="20">
-        <v>1</v>
-      </c>
+      <c r="B200" s="20"/>
       <c r="C200" s="2" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="D200" s="11"/>
     </row>
-    <row r="201" ht="31.5" spans="1:4">
+    <row r="201" spans="1:4">
       <c r="A201" s="32"/>
-      <c r="B201" s="20">
-        <v>1</v>
-      </c>
-      <c r="C201" s="2" t="s">
-        <v>308</v>
-      </c>
+      <c r="B201" s="20"/>
       <c r="D201" s="11"/>
     </row>
-    <row r="202" ht="31.5" spans="1:4">
+    <row r="202" spans="1:4">
       <c r="A202" s="32"/>
-      <c r="B202" s="20">
-        <v>1</v>
-      </c>
-      <c r="C202" s="2" t="s">
-        <v>309</v>
-      </c>
+      <c r="B202" s="20"/>
       <c r="D202" s="11"/>
     </row>
-    <row r="203" ht="31.5" spans="1:4">
+    <row r="203" spans="1:1">
       <c r="A203" s="32"/>
-      <c r="B203" s="20">
-        <v>1</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="D203" s="11"/>
-    </row>
-    <row r="204" ht="31.5" spans="1:4">
-      <c r="A204" s="32"/>
+    </row>
+    <row r="204" ht="93.75" spans="1:4">
+      <c r="A204" s="32" t="s">
+        <v>313</v>
+      </c>
       <c r="B204" s="20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="D204" s="11"/>
-    </row>
-    <row r="205" spans="1:4">
+        <v>313</v>
+      </c>
+      <c r="D204" s="11" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="205" ht="94.5" spans="1:4">
       <c r="A205" s="32"/>
       <c r="B205" s="20">
-        <v>1</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="D205" s="11"/>
-    </row>
-    <row r="206" ht="66" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C205" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="D205" s="33" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="206" ht="27" spans="1:4">
       <c r="A206" s="32"/>
       <c r="B206" s="20">
         <v>5</v>
       </c>
-      <c r="C206" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D206" s="11" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="207" ht="47.25" spans="1:4">
+      <c r="C206" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="D206" s="33" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="207" ht="160.5" spans="1:4">
       <c r="A207" s="32"/>
       <c r="B207" s="20">
-        <v>1</v>
-      </c>
-      <c r="C207" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D207" s="11"/>
-    </row>
-    <row r="208" ht="81.75" spans="1:4">
+        <v>5</v>
+      </c>
+      <c r="C207" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="D207" s="33" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="208" ht="27" spans="1:4">
       <c r="A208" s="32"/>
       <c r="B208" s="20">
         <v>5</v>
       </c>
-      <c r="C208" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="D208" s="11" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="209" ht="99" spans="1:4">
+      <c r="C208" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="D208" s="33" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="209" ht="94.5" spans="1:4">
       <c r="A209" s="32"/>
       <c r="B209" s="20">
         <v>5</v>
       </c>
-      <c r="C209" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="D209" s="11" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="210" ht="65.25" spans="1:4">
+      <c r="C209" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="D209" s="33" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="210" ht="67.5" spans="1:4">
       <c r="A210" s="32"/>
       <c r="B210" s="20">
         <v>5</v>
       </c>
-      <c r="C210" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="D210" s="11" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="211" ht="114" spans="1:4">
+      <c r="C210" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="D210" s="33" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="211" ht="117" spans="1:4">
       <c r="A211" s="32"/>
       <c r="B211" s="20">
         <v>5</v>
       </c>
       <c r="C211" s="12" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="D211" s="33" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="212" ht="114.75" spans="1:4">
-      <c r="A212" s="32" t="s">
-        <v>324</v>
-      </c>
+        <v>328</v>
+      </c>
+    </row>
+    <row r="212" ht="27" spans="1:4">
+      <c r="A212" s="32"/>
       <c r="B212" s="20">
         <v>5</v>
       </c>
-      <c r="C212" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="D212" s="11" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="213" ht="115.5" spans="1:4">
+      <c r="C212" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="D212" s="33" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="213" ht="38.25" spans="1:4">
       <c r="A213" s="32"/>
       <c r="B213" s="20">
         <v>5</v>
       </c>
       <c r="C213" s="12" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="D213" s="33" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="214" ht="33" spans="1:4">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="214" ht="121.5" spans="1:4">
       <c r="A214" s="32"/>
       <c r="B214" s="20">
         <v>5</v>
       </c>
       <c r="C214" s="12" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="D214" s="33" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="215" ht="31.5" spans="1:4">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="215" ht="105.75" spans="1:4">
       <c r="A215" s="32"/>
-      <c r="B215" s="20"/>
+      <c r="B215" s="20">
+        <v>5</v>
+      </c>
       <c r="C215" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="D215" s="33"/>
-    </row>
-    <row r="216" ht="33" spans="1:4">
+        <v>335</v>
+      </c>
+      <c r="D215" s="33" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4">
       <c r="A216" s="32"/>
-      <c r="B216" s="20">
-        <v>5</v>
-      </c>
-      <c r="C216" s="12" t="s">
-        <v>331</v>
-      </c>
-      <c r="D216" s="33" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="217" ht="115.5" spans="1:4">
+      <c r="B216" s="20"/>
+      <c r="C216" s="12"/>
+      <c r="D216" s="33"/>
+    </row>
+    <row r="217" spans="1:4">
       <c r="A217" s="32"/>
-      <c r="B217" s="20">
-        <v>5</v>
-      </c>
-      <c r="C217" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="D217" s="33" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="218" ht="82.5" spans="1:4">
+      <c r="B217" s="20"/>
+      <c r="C217" s="12"/>
+      <c r="D217" s="33"/>
+    </row>
+    <row r="218" spans="1:4">
       <c r="A218" s="32"/>
-      <c r="B218" s="20">
-        <v>5</v>
-      </c>
-      <c r="C218" s="12" t="s">
-        <v>335</v>
-      </c>
-      <c r="D218" s="33" t="s">
-        <v>336</v>
-      </c>
+      <c r="B218" s="20"/>
+      <c r="C218" s="12"/>
+      <c r="D218" s="33"/>
     </row>
     <row r="219" spans="1:4">
       <c r="A219" s="32"/>
@@ -5500,7 +5509,7 @@
       <c r="C219" s="12"/>
       <c r="D219" s="33"/>
     </row>
-    <row r="220" ht="49.5" spans="1:4">
+    <row r="220" ht="40.5" spans="1:4">
       <c r="A220" s="32" t="s">
         <v>337</v>
       </c>
@@ -5514,7 +5523,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="221" ht="177" spans="1:4">
+    <row r="221" ht="144" spans="1:4">
       <c r="A221" s="32"/>
       <c r="B221" s="20">
         <v>5</v>
@@ -5562,7 +5571,7 @@
       <c r="C227" s="12"/>
       <c r="D227" s="33"/>
     </row>
-    <row r="228" ht="31.5" spans="1:4">
+    <row r="228" ht="25.5" spans="1:4">
       <c r="A228" s="32" t="s">
         <v>342</v>
       </c>
@@ -5574,7 +5583,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="229" ht="49.5" spans="1:4">
+    <row r="229" ht="40.5" spans="1:4">
       <c r="A229" s="32"/>
       <c r="B229" s="20">
         <v>5</v>
@@ -5586,7 +5595,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="230" ht="47.25" spans="1:4">
+    <row r="230" ht="38.25" spans="1:4">
       <c r="A230" s="32"/>
       <c r="B230" s="20">
         <v>5</v>
@@ -5610,7 +5619,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="232" ht="33" spans="1:4">
+    <row r="232" ht="28.5" spans="1:4">
       <c r="A232" s="32"/>
       <c r="B232" s="20">
         <v>5</v>
@@ -5622,7 +5631,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="233" ht="33" spans="1:4">
+    <row r="233" ht="27" spans="1:4">
       <c r="A233" s="32" t="s">
         <v>353</v>
       </c>
@@ -5672,7 +5681,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="237" ht="48.75" spans="1:4">
+    <row r="237" ht="39.75" spans="1:4">
       <c r="A237" s="32"/>
       <c r="B237" s="29">
         <v>5</v>
@@ -5684,7 +5693,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="238" ht="16.5" spans="1:4">
+    <row r="238" ht="13.5" spans="1:4">
       <c r="A238" s="32"/>
       <c r="B238" s="20">
         <v>5</v>
@@ -5696,7 +5705,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="239" ht="261" spans="1:4">
+    <row r="239" ht="213" spans="1:4">
       <c r="A239" s="32"/>
       <c r="B239" s="20">
         <v>6</v>
@@ -5708,7 +5717,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="240" ht="82.5" spans="1:4">
+    <row r="240" ht="67.5" spans="1:4">
       <c r="A240" s="32"/>
       <c r="B240" s="20">
         <v>7</v>
@@ -5720,7 +5729,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="241" ht="66" spans="1:4">
+    <row r="241" ht="54" spans="1:4">
       <c r="A241" s="32"/>
       <c r="B241" s="20">
         <v>8</v>
@@ -5732,7 +5741,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="242" ht="66" spans="1:4">
+    <row r="242" ht="54" spans="1:4">
       <c r="A242" s="32"/>
       <c r="B242" s="20">
         <v>9</v>
@@ -5764,7 +5773,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="245" ht="49.5" spans="1:4">
+    <row r="245" ht="40.5" spans="1:4">
       <c r="A245" s="32"/>
       <c r="B245" s="20">
         <v>5</v>
@@ -5776,7 +5785,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="246" ht="33" spans="1:4">
+    <row r="246" ht="27" spans="1:4">
       <c r="A246" s="32"/>
       <c r="B246" s="20">
         <v>5</v>
@@ -5788,7 +5797,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="247" ht="16.5" spans="1:4">
+    <row r="247" ht="13.5" spans="1:4">
       <c r="A247" s="32"/>
       <c r="B247" s="20">
         <v>5</v>
@@ -5800,7 +5809,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="248" ht="178.5" spans="1:4">
+    <row r="248" ht="145.5" spans="1:4">
       <c r="A248" s="32"/>
       <c r="B248" s="20">
         <v>5</v>
@@ -5856,7 +5865,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="255" ht="31.5" spans="1:4">
+    <row r="255" ht="25.5" spans="1:4">
       <c r="A255" s="32"/>
       <c r="B255" s="20">
         <v>5</v>
@@ -5868,7 +5877,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="256" ht="130.5" spans="1:4">
+    <row r="256" ht="106.5" spans="1:4">
       <c r="A256" s="32"/>
       <c r="B256" s="20">
         <v>5</v>
@@ -5880,7 +5889,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="257" ht="128.25" spans="1:4">
+    <row r="257" ht="104.25" spans="1:4">
       <c r="A257" s="32"/>
       <c r="B257" s="20"/>
       <c r="C257" s="2" t="s">
@@ -5890,7 +5899,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="258" ht="48" spans="1:4">
+    <row r="258" ht="39" spans="1:4">
       <c r="A258" s="32"/>
       <c r="B258" s="20">
         <v>5</v>
@@ -5907,26 +5916,26 @@
     <extLst/>
   </autoFilter>
   <mergeCells count="18">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A15:A58"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A63:A67"/>
-    <mergeCell ref="A68:A85"/>
-    <mergeCell ref="A86:A99"/>
-    <mergeCell ref="A100:A179"/>
-    <mergeCell ref="A180:A193"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="A196:A211"/>
-    <mergeCell ref="A212:A219"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A61:A65"/>
+    <mergeCell ref="A66:A83"/>
+    <mergeCell ref="A84:A97"/>
+    <mergeCell ref="A98:A177"/>
+    <mergeCell ref="A178:A191"/>
+    <mergeCell ref="A192:A193"/>
+    <mergeCell ref="A194:A203"/>
+    <mergeCell ref="A204:A219"/>
     <mergeCell ref="A220:A227"/>
     <mergeCell ref="A228:A232"/>
     <mergeCell ref="A233:A243"/>
     <mergeCell ref="A244:A253"/>
     <mergeCell ref="A254:A258"/>
   </mergeCells>
-  <conditionalFormatting sqref="B180">
+  <conditionalFormatting sqref="B178">
     <cfRule type="cellIs" dxfId="0" priority="4" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -5948,7 +5957,7 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B57 B59:B98 B181:B237 B121:B179 B100:B119 B243:B1048576">
+  <conditionalFormatting sqref="B1:B55 B57:B96 B179:B202 B98:B117 B204:B237 B243:B1048576 B119:B177">
     <cfRule type="cellIs" dxfId="0" priority="7" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -5960,7 +5969,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C212" r:id="rId1" display="Panoptic Segmentation" tooltip="https://arxiv.org/abs/1801.00868"/>
+    <hyperlink ref="C204" r:id="rId1" display="Panoptic Segmentation" tooltip="https://arxiv.org/abs/1801.00868"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>